<commit_message>
PRELIM - Added weighted waypoints and processing routines
Added weighted waypoint type defs and processing routines.  This will allow easier and more consistent implementation of splines similar to what Pathweaver does with it's custom code, without custom code.   Also removed several unused type defs (x_y_heading, and waypoints)
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2764" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2767" uniqueCount="681">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -2051,6 +2051,12 @@
   </si>
   <si>
     <t xml:space="preserve">UTIL_WAYPOINT.ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTIL_WEIGHTED_WAYPOINT.ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New V1.5</t>
   </si>
   <si>
     <t xml:space="preserve">WAYPOINTS.CTL</t>
@@ -2462,14 +2468,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I596"/>
+  <dimension ref="A1:I605"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B595" activeCellId="0" sqref="B595"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2560,28 +2566,28 @@
         <v>11</v>
       </c>
       <c r="B9" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B931,"X")</f>
-        <v>380</v>
+        <f aca="false">COUNTIF(B18:B932,"X")</f>
+        <v>378</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C18:C931,"X")</f>
+        <f aca="false">COUNTIF(C18:C932,"X")</f>
         <v>368</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D18:D931,"X")</f>
-        <v>132</v>
+        <f aca="false">COUNTIF(D18:D932,"X")</f>
+        <v>130</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E18:E931,"X")</f>
+        <f aca="false">COUNTIF(E18:E932,"X")</f>
         <v>352</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F18:F931,"S")+COUNTIF(F18:F931,"I")+COUNTIF(F18:F931,"X")+COUNTIF(F18:F931,"SI")+COUNTIF(F18:F931,"IS")+COUNTIF(F18:F931,"N/A")</f>
+        <f aca="false">COUNTIF(F18:F932,"S")+COUNTIF(F18:F932,"I")+COUNTIF(F18:F932,"X")+COUNTIF(F18:F932,"SI")+COUNTIF(F18:F932,"IS")+COUNTIF(F18:F932,"N/A")</f>
         <v>180</v>
       </c>
       <c r="G9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.968421052631579</v>
+        <v>0.973544973544973</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,7 +2598,7 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.473684210526316</v>
+        <v>0.476190476190476</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13851,33 +13857,29 @@
     </row>
     <row r="595" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A595" s="9"/>
-      <c r="B595" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C595" s="25"/>
-      <c r="D595" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E595" s="25"/>
-      <c r="F595" s="25" t="s">
-        <v>591</v>
-      </c>
-      <c r="G595" s="26" t="s">
+      <c r="B595" s="22"/>
+      <c r="C595" s="22"/>
+      <c r="D595" s="22"/>
+      <c r="E595" s="22"/>
+      <c r="F595" s="22" t="s">
+        <v>674</v>
+      </c>
+      <c r="G595" s="23" t="s">
         <v>676</v>
       </c>
-      <c r="H595" s="26"/>
-      <c r="I595" s="26" t="s">
+      <c r="H595" s="23"/>
+      <c r="I595" s="23" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="596" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="596" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A596" s="9"/>
       <c r="B596" s="25" t="s">
-        <v>21</v>
+        <v>591</v>
       </c>
       <c r="C596" s="25"/>
       <c r="D596" s="25" t="s">
-        <v>21</v>
+        <v>591</v>
       </c>
       <c r="E596" s="25"/>
       <c r="F596" s="25" t="s">
@@ -13888,8 +13890,32 @@
       </c>
       <c r="H596" s="26"/>
       <c r="I596" s="26" t="s">
-        <v>677</v>
-      </c>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="597" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A597" s="9"/>
+      <c r="B597" s="25" t="s">
+        <v>591</v>
+      </c>
+      <c r="C597" s="25"/>
+      <c r="D597" s="25" t="s">
+        <v>591</v>
+      </c>
+      <c r="E597" s="25"/>
+      <c r="F597" s="25" t="s">
+        <v>591</v>
+      </c>
+      <c r="G597" s="26" t="s">
+        <v>680</v>
+      </c>
+      <c r="H597" s="26"/>
+      <c r="I597" s="26" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="605" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F605" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Update menus to add new and missing functions
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2848" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2874" uniqueCount="707">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -2552,8 +2552,8 @@
   </sheetPr>
   <dimension ref="A1:I629"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A588" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E623" activeCellId="0" sqref="E623"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2653,15 +2653,15 @@
       </c>
       <c r="D9" s="13" t="n">
         <f aca="false">COUNTIF(D18:D956,"X")</f>
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E9" s="13" t="n">
         <f aca="false">COUNTIF(E18:E956,"X")</f>
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="F9" s="13" t="n">
         <f aca="false">COUNTIF(F18:F956,"S")+COUNTIF(F18:F956,"I")+COUNTIF(F18:F956,"X")+COUNTIF(F18:F956,"SI")+COUNTIF(F18:F956,"IS")+COUNTIF(F18:F956,"N/A")</f>
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G9" s="14" t="n">
         <f aca="false">C9/B9</f>
@@ -2676,7 +2676,7 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.477386934673367</v>
+        <v>0.487437185929648</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,7 +4536,9 @@
       <c r="D113" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E113" s="25"/>
+      <c r="E113" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F113" s="22" t="s">
         <v>22</v>
       </c>
@@ -4555,7 +4557,9 @@
       <c r="D114" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E114" s="25"/>
+      <c r="E114" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F114" s="22" t="s">
         <v>22</v>
       </c>
@@ -4574,7 +4578,9 @@
       <c r="D115" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E115" s="25"/>
+      <c r="E115" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F115" s="22" t="s">
         <v>22</v>
       </c>
@@ -4593,7 +4599,9 @@
       <c r="D116" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E116" s="25"/>
+      <c r="E116" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F116" s="22" t="s">
         <v>22</v>
       </c>
@@ -4612,7 +4620,9 @@
       <c r="D117" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E117" s="25"/>
+      <c r="E117" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F117" s="22" t="s">
         <v>22</v>
       </c>
@@ -6233,8 +6243,12 @@
       <c r="D198" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E198" s="25"/>
-      <c r="F198" s="22"/>
+      <c r="E198" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F198" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="G198" s="23" t="s">
         <v>220</v>
       </c>
@@ -6250,8 +6264,12 @@
       <c r="D199" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E199" s="25"/>
-      <c r="F199" s="22"/>
+      <c r="E199" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F199" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="G199" s="23" t="s">
         <v>221</v>
       </c>
@@ -6939,8 +6957,12 @@
       <c r="D230" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E230" s="25"/>
-      <c r="F230" s="22"/>
+      <c r="E230" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F230" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="G230" s="23" t="s">
         <v>275</v>
       </c>
@@ -6956,8 +6978,12 @@
       <c r="D231" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E231" s="25"/>
-      <c r="F231" s="22"/>
+      <c r="E231" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F231" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="G231" s="23" t="s">
         <v>276</v>
       </c>
@@ -9438,7 +9464,9 @@
       <c r="D360" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E360" s="25"/>
+      <c r="E360" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F360" s="22"/>
       <c r="G360" s="23" t="s">
         <v>433</v>
@@ -9476,7 +9504,9 @@
       <c r="D362" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E362" s="25"/>
+      <c r="E362" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F362" s="22"/>
       <c r="G362" s="23" t="s">
         <v>436</v>
@@ -11173,14 +11203,16 @@
       </c>
       <c r="I450" s="23"/>
     </row>
-    <row r="451" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="451" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="19"/>
       <c r="B451" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C451" s="25"/>
       <c r="D451" s="22"/>
-      <c r="E451" s="25"/>
+      <c r="E451" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F451" s="22"/>
       <c r="G451" s="23" t="s">
         <v>547</v>
@@ -12356,7 +12388,7 @@
       <c r="H517" s="23"/>
       <c r="I517" s="23"/>
     </row>
-    <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="518" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="9"/>
       <c r="B518" s="22" t="s">
         <v>21</v>
@@ -12365,7 +12397,9 @@
       <c r="D518" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E518" s="25"/>
+      <c r="E518" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F518" s="22"/>
       <c r="G518" s="23" t="s">
         <v>615</v>
@@ -13511,14 +13545,18 @@
       <c r="H581" s="23"/>
       <c r="I581" s="23"/>
     </row>
-    <row r="582" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="582" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="9"/>
       <c r="B582" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C582" s="22"/>
-      <c r="D582" s="22"/>
-      <c r="E582" s="22"/>
+      <c r="C582" s="25"/>
+      <c r="D582" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E582" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F582" s="22" t="s">
         <v>610</v>
       </c>
@@ -13528,14 +13566,18 @@
       <c r="H582" s="23"/>
       <c r="I582" s="23"/>
     </row>
-    <row r="583" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="583" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="9"/>
       <c r="B583" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C583" s="22"/>
-      <c r="D583" s="22"/>
-      <c r="E583" s="22"/>
+      <c r="C583" s="25"/>
+      <c r="D583" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E583" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F583" s="22" t="s">
         <v>610</v>
       </c>
@@ -13569,11 +13611,13 @@
       <c r="B585" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C585" s="22"/>
+      <c r="C585" s="25"/>
       <c r="D585" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E585" s="22"/>
+      <c r="E585" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F585" s="22" t="s">
         <v>610</v>
       </c>
@@ -13588,11 +13632,13 @@
       <c r="B586" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C586" s="22"/>
+      <c r="C586" s="25"/>
       <c r="D586" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E586" s="22"/>
+      <c r="E586" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F586" s="22" t="s">
         <v>610</v>
       </c>
@@ -13607,11 +13653,13 @@
       <c r="B587" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C587" s="22"/>
+      <c r="C587" s="25"/>
       <c r="D587" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E587" s="22"/>
+      <c r="E587" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F587" s="22" t="s">
         <v>610</v>
       </c>
@@ -14296,7 +14344,9 @@
       <c r="D618" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E618" s="25"/>
+      <c r="E618" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F618" s="22" t="s">
         <v>699</v>
       </c>
@@ -14350,7 +14400,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="621" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="621" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B621" s="22" t="s">
         <v>21</v>
       </c>
@@ -14358,7 +14408,9 @@
       <c r="D621" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E621" s="25"/>
+      <c r="E621" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F621" s="22" t="s">
         <v>699</v>
       </c>

</xml_diff>

<commit_message>
Added Rotation Degrees create/get funtions, on windows prompt to replace traj files, updated menus
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,12 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2973" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2980" uniqueCount="736">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
   <si>
-    <t xml:space="preserve">Revision 1.X    1/26/2021 – Added Holonomic Drive Control.  Added a rotation convience function.</t>
+    <t xml:space="preserve">Revision 1.X    2/11/2021 – Added menu items..</t>
   </si>
   <si>
     <t xml:space="preserve">This documents which Java/C++ WPILIB routines have been </t>
@@ -782,6 +782,9 @@
   </si>
   <si>
     <t xml:space="preserve"> rotation2d new( double x, double y )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation_CreateAngleDegrees.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> rotation2d fromDegrees( double degrees )</t>
@@ -2650,8 +2653,8 @@
   </sheetPr>
   <dimension ref="A1:I655"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A146" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B175" activeCellId="0" sqref="B175"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2743,11 +2746,11 @@
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">COUNTIF(B18:B982,"X")</f>
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">COUNTIF(C18:C982,"X")</f>
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D9" s="13" t="n">
         <f aca="false">COUNTIF(D18:D982,"X")</f>
@@ -2755,15 +2758,15 @@
       </c>
       <c r="E9" s="13" t="n">
         <f aca="false">COUNTIF(E18:E982,"X")</f>
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="F9" s="13" t="n">
         <f aca="false">COUNTIF(F18:F982,"S")+COUNTIF(F18:F982,"I")+COUNTIF(F18:F982,"X")+COUNTIF(F18:F982,"SI")+COUNTIF(F18:F982,"IS")+COUNTIF(F18:F982,"N/A")</f>
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.894865525672372</v>
+        <v>0.891041162227603</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2774,7 +2777,7 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.491442542787286</v>
+        <v>0.491525423728814</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4817,14 +4820,16 @@
       <c r="H123" s="23"/>
       <c r="I123" s="23"/>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="19"/>
       <c r="B124" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C124" s="25"/>
       <c r="D124" s="22"/>
-      <c r="E124" s="25"/>
+      <c r="E124" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F124" s="22"/>
       <c r="G124" s="23" t="s">
         <v>126</v>
@@ -6830,27 +6835,29 @@
       </c>
       <c r="I223" s="23"/>
     </row>
-    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="19"/>
-      <c r="B224" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="C224" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="D224" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="E224" s="29"/>
-      <c r="F224" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="G224" s="30"/>
+      <c r="B224" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C224" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D224" s="22"/>
+      <c r="E224" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F224" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G224" s="23" t="s">
+        <v>253</v>
+      </c>
       <c r="H224" s="23" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I224" s="23" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6869,10 +6876,10 @@
         <v>22</v>
       </c>
       <c r="G225" s="23" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H225" s="23" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I225" s="23"/>
     </row>
@@ -6892,10 +6899,10 @@
         <v>22</v>
       </c>
       <c r="G226" s="23" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H226" s="23" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I226" s="23"/>
     </row>
@@ -6915,10 +6922,10 @@
         <v>22</v>
       </c>
       <c r="G227" s="23" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H227" s="23" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I227" s="23"/>
     </row>
@@ -6938,10 +6945,10 @@
         <v>22</v>
       </c>
       <c r="G228" s="23" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H228" s="23" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I228" s="23"/>
     </row>
@@ -6961,10 +6968,10 @@
         <v>22</v>
       </c>
       <c r="G229" s="23" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H229" s="23" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I229" s="23"/>
     </row>
@@ -6984,11 +6991,11 @@
         <v>22</v>
       </c>
       <c r="G230" s="23" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H230" s="23"/>
       <c r="I230" s="23" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7007,36 +7014,36 @@
         <v>22</v>
       </c>
       <c r="G231" s="23" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H231" s="23" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="I231" s="23" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="232" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="19"/>
-      <c r="B232" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="C232" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="D232" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="E232" s="29"/>
-      <c r="F232" s="29" t="s">
-        <v>202</v>
+      <c r="B232" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C232" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D232" s="22"/>
+      <c r="E232" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F232" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="G232" s="30"/>
       <c r="H232" s="23" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I232" s="23" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7055,13 +7062,13 @@
         <v>22</v>
       </c>
       <c r="G233" s="23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H233" s="23" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="I233" s="23" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7080,13 +7087,13 @@
         <v>22</v>
       </c>
       <c r="G234" s="23" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H234" s="23" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="I234" s="23" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7105,13 +7112,13 @@
         <v>22</v>
       </c>
       <c r="G235" s="23" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H235" s="23" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I235" s="23" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7129,10 +7136,10 @@
         <v>22</v>
       </c>
       <c r="G236" s="23" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H236" s="23" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I236" s="23"/>
     </row>
@@ -7168,7 +7175,7 @@
     </row>
     <row r="239" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="21" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B239" s="22" t="s">
         <v>21</v>
@@ -7184,10 +7191,10 @@
         <v>22</v>
       </c>
       <c r="G239" s="23" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H239" s="23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I239" s="23"/>
     </row>
@@ -7207,10 +7214,10 @@
         <v>22</v>
       </c>
       <c r="G240" s="23" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H240" s="23" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I240" s="23"/>
     </row>
@@ -7231,7 +7238,7 @@
       </c>
       <c r="G241" s="30"/>
       <c r="H241" s="23" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I241" s="23" t="s">
         <v>221</v>
@@ -7253,10 +7260,10 @@
         <v>22</v>
       </c>
       <c r="G242" s="23" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H242" s="23" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I242" s="23"/>
     </row>
@@ -7276,13 +7283,13 @@
         <v>22</v>
       </c>
       <c r="G243" s="23" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H243" s="23" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I243" s="23" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7301,13 +7308,13 @@
         <v>22</v>
       </c>
       <c r="G244" s="23" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H244" s="23" t="s">
         <v>234</v>
       </c>
       <c r="I244" s="23" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7326,7 +7333,7 @@
         <v>22</v>
       </c>
       <c r="G245" s="23" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H245" s="23"/>
       <c r="I245" s="23"/>
@@ -7347,7 +7354,7 @@
         <v>22</v>
       </c>
       <c r="G246" s="23" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H246" s="23"/>
       <c r="I246" s="23"/>
@@ -7368,13 +7375,13 @@
         <v>22</v>
       </c>
       <c r="G247" s="23" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H247" s="23" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="I247" s="23" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7392,10 +7399,10 @@
         <v>22</v>
       </c>
       <c r="G248" s="23" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H248" s="23" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="I248" s="23"/>
     </row>
@@ -7431,7 +7438,7 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="21" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B251" s="29" t="s">
         <v>202</v>
@@ -7448,7 +7455,7 @@
       </c>
       <c r="G251" s="30"/>
       <c r="H251" s="23" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I251" s="23" t="s">
         <v>221</v>
@@ -7470,26 +7477,28 @@
         <v>22</v>
       </c>
       <c r="G252" s="23" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H252" s="23" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="I252" s="23"/>
     </row>
-    <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="19"/>
       <c r="B253" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C253" s="25"/>
       <c r="D253" s="22"/>
-      <c r="E253" s="25"/>
+      <c r="E253" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F253" s="22" t="s">
         <v>22</v>
       </c>
       <c r="G253" s="23" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H253" s="23"/>
       <c r="I253" s="23"/>
@@ -7510,10 +7519,10 @@
         <v>22</v>
       </c>
       <c r="G254" s="23" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H254" s="23" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I254" s="23"/>
     </row>
@@ -7533,13 +7542,13 @@
         <v>22</v>
       </c>
       <c r="G255" s="23" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H255" s="23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I255" s="23" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7558,13 +7567,13 @@
         <v>22</v>
       </c>
       <c r="G256" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="H256" s="23" t="s">
+        <v>311</v>
+      </c>
+      <c r="I256" s="23" t="s">
         <v>309</v>
-      </c>
-      <c r="H256" s="23" t="s">
-        <v>310</v>
-      </c>
-      <c r="I256" s="23" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7585,7 +7594,7 @@
         <v>22</v>
       </c>
       <c r="G257" s="23" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H257" s="23"/>
       <c r="I257" s="23"/>
@@ -7606,13 +7615,13 @@
         <v>22</v>
       </c>
       <c r="G258" s="23" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H258" s="23" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I258" s="23" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7631,10 +7640,10 @@
         <v>22</v>
       </c>
       <c r="G259" s="23" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H259" s="23" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="I259" s="23"/>
     </row>
@@ -7654,10 +7663,10 @@
         <v>22</v>
       </c>
       <c r="G260" s="23" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H260" s="23" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="I260" s="23"/>
     </row>
@@ -7677,10 +7686,10 @@
         <v>22</v>
       </c>
       <c r="G261" s="23" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H261" s="23" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="I261" s="23"/>
     </row>
@@ -7700,10 +7709,10 @@
         <v>22</v>
       </c>
       <c r="G262" s="23" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H262" s="23" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="I262" s="23"/>
     </row>
@@ -7723,10 +7732,10 @@
         <v>22</v>
       </c>
       <c r="G263" s="23" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H263" s="23" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I263" s="23"/>
     </row>
@@ -7747,10 +7756,10 @@
       </c>
       <c r="G264" s="30"/>
       <c r="H264" s="23" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="I264" s="23" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7768,10 +7777,10 @@
         <v>22</v>
       </c>
       <c r="G265" s="23" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H265" s="23" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="I265" s="23"/>
     </row>
@@ -7807,7 +7816,7 @@
     </row>
     <row r="268" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="21" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B268" s="22" t="s">
         <v>21</v>
@@ -7823,10 +7832,10 @@
         <v>22</v>
       </c>
       <c r="G268" s="23" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H268" s="23" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="I268" s="23"/>
     </row>
@@ -7846,10 +7855,10 @@
         <v>22</v>
       </c>
       <c r="G269" s="23" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H269" s="23" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="I269" s="23"/>
     </row>
@@ -7870,7 +7879,7 @@
         <v>22</v>
       </c>
       <c r="G270" s="23" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H270" s="23"/>
       <c r="I270" s="23"/>
@@ -7890,7 +7899,7 @@
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="16" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B273" s="32"/>
       <c r="C273" s="18"/>
@@ -7937,7 +7946,7 @@
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="21" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B276" s="29" t="s">
         <v>202</v>
@@ -7954,7 +7963,7 @@
       </c>
       <c r="G276" s="30"/>
       <c r="H276" s="23" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="I276" s="23" t="s">
         <v>221</v>
@@ -7976,10 +7985,10 @@
         <v>22</v>
       </c>
       <c r="G277" s="23" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H277" s="23" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="I277" s="23"/>
     </row>
@@ -7998,10 +8007,10 @@
         <v>22</v>
       </c>
       <c r="G278" s="23" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H278" s="23" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I278" s="23"/>
     </row>
@@ -8037,7 +8046,7 @@
     </row>
     <row r="281" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="21" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B281" s="22" t="s">
         <v>21</v>
@@ -8053,10 +8062,10 @@
         <v>25</v>
       </c>
       <c r="G281" s="23" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="H281" s="23" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="I281" s="23"/>
     </row>
@@ -8076,10 +8085,10 @@
         <v>21</v>
       </c>
       <c r="G282" s="23" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H282" s="23" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="I282" s="23"/>
     </row>
@@ -8098,10 +8107,10 @@
         <v>22</v>
       </c>
       <c r="G283" s="23" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="H283" s="23" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="I283" s="23"/>
     </row>
@@ -8137,7 +8146,7 @@
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="21" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B286" s="29" t="s">
         <v>202</v>
@@ -8154,7 +8163,7 @@
       </c>
       <c r="G286" s="30"/>
       <c r="H286" s="23" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="I286" s="23"/>
     </row>
@@ -8175,7 +8184,7 @@
       </c>
       <c r="G287" s="30"/>
       <c r="H287" s="23" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="I287" s="23"/>
     </row>
@@ -8196,10 +8205,10 @@
       </c>
       <c r="G288" s="30"/>
       <c r="H288" s="23" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="I288" s="23" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8219,7 +8228,7 @@
       </c>
       <c r="G289" s="30"/>
       <c r="H289" s="23" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="I289" s="23"/>
     </row>
@@ -8238,13 +8247,13 @@
         <v>21</v>
       </c>
       <c r="G290" s="23" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H290" s="23" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I290" s="23" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8279,7 +8288,7 @@
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="21" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B293" s="33" t="s">
         <v>202</v>
@@ -8290,7 +8299,7 @@
       <c r="F293" s="22"/>
       <c r="G293" s="30"/>
       <c r="H293" s="23" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="I293" s="23"/>
     </row>
@@ -8305,7 +8314,7 @@
       <c r="F294" s="22"/>
       <c r="G294" s="30"/>
       <c r="H294" s="23" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="I294" s="23"/>
     </row>
@@ -8324,10 +8333,10 @@
         <v>21</v>
       </c>
       <c r="G295" s="23" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="H295" s="23" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="I295" s="23"/>
     </row>
@@ -8363,7 +8372,7 @@
     </row>
     <row r="298" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="21" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B298" s="22" t="s">
         <v>21</v>
@@ -8379,7 +8388,7 @@
         <v>25</v>
       </c>
       <c r="G298" s="23" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H298" s="23"/>
       <c r="I298" s="23"/>
@@ -8400,7 +8409,7 @@
         <v>21</v>
       </c>
       <c r="G299" s="23" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H299" s="23"/>
       <c r="I299" s="23"/>
@@ -8421,7 +8430,7 @@
         <v>21</v>
       </c>
       <c r="G300" s="23" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H300" s="23"/>
       <c r="I300" s="23"/>
@@ -8442,7 +8451,7 @@
         <v>21</v>
       </c>
       <c r="G301" s="23" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="H301" s="23"/>
       <c r="I301" s="23"/>
@@ -8462,7 +8471,7 @@
         <v>21</v>
       </c>
       <c r="G302" s="23" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="H302" s="23"/>
       <c r="I302" s="23"/>
@@ -8499,7 +8508,7 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="21" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B305" s="22"/>
       <c r="C305" s="22"/>
@@ -8513,7 +8522,7 @@
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="34"/>
       <c r="B306" s="35" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C306" s="35"/>
     </row>
@@ -8549,7 +8558,7 @@
     </row>
     <row r="309" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="21" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B309" s="22" t="s">
         <v>21</v>
@@ -8563,7 +8572,7 @@
       </c>
       <c r="F309" s="22"/>
       <c r="G309" s="23" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H309" s="23"/>
       <c r="I309" s="23"/>
@@ -8582,7 +8591,7 @@
       </c>
       <c r="F310" s="22"/>
       <c r="G310" s="23" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H310" s="23"/>
       <c r="I310" s="23"/>
@@ -8601,7 +8610,7 @@
       </c>
       <c r="F311" s="22"/>
       <c r="G311" s="23" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H311" s="23"/>
       <c r="I311" s="23"/>
@@ -8620,7 +8629,7 @@
       </c>
       <c r="F312" s="22"/>
       <c r="G312" s="23" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H312" s="23"/>
       <c r="I312" s="23"/>
@@ -8639,7 +8648,7 @@
       </c>
       <c r="F313" s="22"/>
       <c r="G313" s="23" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H313" s="23"/>
       <c r="I313" s="23"/>
@@ -8657,7 +8666,7 @@
       </c>
       <c r="F314" s="22"/>
       <c r="G314" s="23" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H314" s="23"/>
       <c r="I314" s="23"/>
@@ -8694,7 +8703,7 @@
     </row>
     <row r="317" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="21" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B317" s="22" t="s">
         <v>21</v>
@@ -8710,10 +8719,10 @@
         <v>22</v>
       </c>
       <c r="G317" s="23" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H317" s="23" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I317" s="23"/>
     </row>
@@ -8732,10 +8741,10 @@
         <v>21</v>
       </c>
       <c r="G318" s="23" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H318" s="23" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I318" s="23"/>
     </row>
@@ -8771,7 +8780,7 @@
     </row>
     <row r="321" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="21" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B321" s="29" t="s">
         <v>202</v>
@@ -8788,10 +8797,10 @@
       </c>
       <c r="G321" s="23"/>
       <c r="H321" s="23" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="I321" s="23" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8810,11 +8819,11 @@
       </c>
       <c r="F322" s="22"/>
       <c r="G322" s="23" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="H322" s="23"/>
       <c r="I322" s="23" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8833,11 +8842,11 @@
       </c>
       <c r="F323" s="22"/>
       <c r="G323" s="23" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H323" s="23"/>
       <c r="I323" s="23" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8854,10 +8863,10 @@
       </c>
       <c r="F324" s="22"/>
       <c r="G324" s="23" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="H324" s="23" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="I324" s="23"/>
     </row>
@@ -8875,10 +8884,10 @@
       </c>
       <c r="F325" s="22"/>
       <c r="G325" s="23" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H325" s="23" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I325" s="23"/>
     </row>
@@ -8899,10 +8908,10 @@
       </c>
       <c r="G326" s="23"/>
       <c r="H326" s="23" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="I326" s="23" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8921,11 +8930,11 @@
       </c>
       <c r="F327" s="22"/>
       <c r="G327" s="23" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H327" s="23"/>
       <c r="I327" s="23" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8944,11 +8953,11 @@
       </c>
       <c r="F328" s="22"/>
       <c r="G328" s="23" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="H328" s="23"/>
       <c r="I328" s="23" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8966,10 +8975,10 @@
       </c>
       <c r="F329" s="22"/>
       <c r="G329" s="23" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H329" s="23" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I329" s="23"/>
     </row>
@@ -9005,7 +9014,7 @@
     </row>
     <row r="332" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="21" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B332" s="22" t="s">
         <v>21</v>
@@ -9019,10 +9028,10 @@
       </c>
       <c r="F332" s="22"/>
       <c r="G332" s="23" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H332" s="23" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="I332" s="23"/>
     </row>
@@ -9040,10 +9049,10 @@
       </c>
       <c r="F333" s="22"/>
       <c r="G333" s="23" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="H333" s="23" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I333" s="23"/>
     </row>
@@ -9061,10 +9070,10 @@
       </c>
       <c r="F334" s="22"/>
       <c r="G334" s="23" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="H334" s="23" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="I334" s="23"/>
     </row>
@@ -9082,10 +9091,10 @@
       </c>
       <c r="F335" s="22"/>
       <c r="G335" s="23" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H335" s="23" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="I335" s="23"/>
     </row>
@@ -9106,10 +9115,10 @@
       </c>
       <c r="G336" s="23"/>
       <c r="H336" s="23" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="I336" s="23" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9128,11 +9137,11 @@
       </c>
       <c r="F337" s="22"/>
       <c r="G337" s="23" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="H337" s="23"/>
       <c r="I337" s="23" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9151,11 +9160,11 @@
       </c>
       <c r="F338" s="22"/>
       <c r="G338" s="23" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="H338" s="23"/>
       <c r="I338" s="23" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9175,10 +9184,10 @@
       </c>
       <c r="G339" s="23"/>
       <c r="H339" s="23" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="I339" s="23" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9197,11 +9206,11 @@
       </c>
       <c r="F340" s="22"/>
       <c r="G340" s="23" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="H340" s="23"/>
       <c r="I340" s="23" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9219,11 +9228,11 @@
       </c>
       <c r="F341" s="22"/>
       <c r="G341" s="23" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H341" s="23"/>
       <c r="I341" s="23" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9258,7 +9267,7 @@
     </row>
     <row r="344" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="21" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B344" s="22" t="s">
         <v>21</v>
@@ -9274,10 +9283,10 @@
         <v>22</v>
       </c>
       <c r="G344" s="23" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="H344" s="23" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I344" s="23"/>
     </row>
@@ -9296,28 +9305,30 @@
         <v>22</v>
       </c>
       <c r="G345" s="23" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="H345" s="23" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="I345" s="23"/>
     </row>
-    <row r="346" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B346" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C346" s="25"/>
       <c r="D346" s="22"/>
-      <c r="E346" s="25"/>
+      <c r="E346" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F346" s="22" t="s">
         <v>22</v>
       </c>
       <c r="G346" s="23" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H346" s="23" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="I346" s="23"/>
     </row>
@@ -9336,7 +9347,7 @@
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="16" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B349" s="17"/>
       <c r="C349" s="18"/>
@@ -9383,7 +9394,7 @@
     </row>
     <row r="352" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="21" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B352" s="22" t="s">
         <v>21</v>
@@ -9397,10 +9408,10 @@
       </c>
       <c r="F352" s="22"/>
       <c r="G352" s="23" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H352" s="23" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="I352" s="23"/>
     </row>
@@ -9417,10 +9428,10 @@
         <v>16</v>
       </c>
       <c r="H353" s="23" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="I353" s="23" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9437,10 +9448,10 @@
       </c>
       <c r="F354" s="22"/>
       <c r="G354" s="23" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="H354" s="23" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="I354" s="23"/>
     </row>
@@ -9457,10 +9468,10 @@
       </c>
       <c r="F355" s="22"/>
       <c r="G355" s="23" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H355" s="23" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="I355" s="23"/>
     </row>
@@ -9496,7 +9507,7 @@
     </row>
     <row r="358" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="21" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B358" s="22" t="s">
         <v>21</v>
@@ -9512,10 +9523,10 @@
         <v>22</v>
       </c>
       <c r="G358" s="23" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H358" s="23" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="I358" s="23"/>
     </row>
@@ -9536,7 +9547,7 @@
       </c>
       <c r="G359" s="30"/>
       <c r="H359" s="23" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="I359" s="23" t="s">
         <v>221</v>
@@ -9553,10 +9564,10 @@
       <c r="F360" s="22"/>
       <c r="G360" s="30"/>
       <c r="H360" s="23" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="I360" s="23" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9569,10 +9580,10 @@
       <c r="F361" s="22"/>
       <c r="G361" s="30"/>
       <c r="H361" s="23" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="I361" s="23" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9607,7 +9618,7 @@
     </row>
     <row r="364" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="21" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B364" s="22" t="s">
         <v>21</v>
@@ -9621,10 +9632,10 @@
       </c>
       <c r="F364" s="22"/>
       <c r="G364" s="23" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H364" s="23" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="I364" s="23"/>
     </row>
@@ -9639,10 +9650,10 @@
       <c r="F365" s="22"/>
       <c r="G365" s="23"/>
       <c r="H365" s="23" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="I365" s="23" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9659,10 +9670,10 @@
       </c>
       <c r="F366" s="22"/>
       <c r="G366" s="23" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H366" s="23" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="I366" s="23"/>
     </row>
@@ -9679,10 +9690,10 @@
       </c>
       <c r="F367" s="22"/>
       <c r="G367" s="23" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H367" s="23" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="I367" s="23"/>
     </row>
@@ -9718,7 +9729,7 @@
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="21" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B370" s="29" t="s">
         <v>202</v>
@@ -9735,13 +9746,13 @@
       </c>
       <c r="G370" s="30"/>
       <c r="H370" s="23" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="I370" s="23"/>
     </row>
     <row r="371" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="19" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B371" s="22" t="s">
         <v>21</v>
@@ -9755,10 +9766,10 @@
       </c>
       <c r="F371" s="22"/>
       <c r="G371" s="23" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="H371" s="23" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="I371" s="23"/>
     </row>
@@ -9779,7 +9790,7 @@
       </c>
       <c r="G372" s="30"/>
       <c r="H372" s="23" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="I372" s="23"/>
     </row>
@@ -9793,10 +9804,10 @@
       <c r="F373" s="22"/>
       <c r="G373" s="30"/>
       <c r="H373" s="23" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="I373" s="23" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9831,7 +9842,7 @@
     </row>
     <row r="376" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="21" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B376" s="22" t="s">
         <v>21</v>
@@ -9845,10 +9856,10 @@
       </c>
       <c r="F376" s="22"/>
       <c r="G376" s="23" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="H376" s="23" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="I376" s="23"/>
     </row>
@@ -9866,7 +9877,7 @@
       </c>
       <c r="F377" s="22"/>
       <c r="G377" s="23" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="H377" s="23"/>
       <c r="I377" s="23"/>
@@ -9885,10 +9896,10 @@
       </c>
       <c r="F378" s="22"/>
       <c r="G378" s="23" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="H378" s="23" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="I378" s="23"/>
     </row>
@@ -9906,7 +9917,7 @@
       </c>
       <c r="F379" s="22"/>
       <c r="G379" s="23" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H379" s="23"/>
       <c r="I379" s="23"/>
@@ -9925,10 +9936,10 @@
       </c>
       <c r="F380" s="22"/>
       <c r="G380" s="23" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="H380" s="23" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="I380" s="23"/>
     </row>
@@ -9948,7 +9959,7 @@
       </c>
       <c r="F381" s="22"/>
       <c r="G381" s="23" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H381" s="23"/>
       <c r="I381" s="23" t="s">
@@ -9971,7 +9982,7 @@
       </c>
       <c r="F382" s="22"/>
       <c r="G382" s="23" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="H382" s="23"/>
       <c r="I382" s="23" t="s">
@@ -9994,7 +10005,7 @@
       </c>
       <c r="F383" s="22"/>
       <c r="G383" s="23" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="H383" s="23"/>
       <c r="I383" s="23" t="s">
@@ -10015,10 +10026,10 @@
       </c>
       <c r="F384" s="22"/>
       <c r="G384" s="23" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="H384" s="23" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="I384" s="23"/>
     </row>
@@ -10036,10 +10047,10 @@
       </c>
       <c r="F385" s="22"/>
       <c r="G385" s="23" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="H385" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="I385" s="23" t="s">
         <v>196</v>
@@ -10061,10 +10072,10 @@
         <v>22</v>
       </c>
       <c r="G386" s="23" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="H386" s="23" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="I386" s="23"/>
     </row>
@@ -10083,10 +10094,10 @@
         <v>22</v>
       </c>
       <c r="G387" s="23" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="H387" s="23" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="I387" s="23"/>
     </row>
@@ -10122,7 +10133,7 @@
     </row>
     <row r="390" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="21" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B390" s="22" t="s">
         <v>21</v>
@@ -10136,10 +10147,10 @@
       </c>
       <c r="F390" s="22"/>
       <c r="G390" s="23" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="H390" s="23" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="I390" s="23"/>
     </row>
@@ -10157,10 +10168,10 @@
       </c>
       <c r="F391" s="22"/>
       <c r="G391" s="23" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="H391" s="23" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="I391" s="23"/>
     </row>
@@ -10180,7 +10191,7 @@
       </c>
       <c r="F392" s="22"/>
       <c r="G392" s="23" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="H392" s="23"/>
       <c r="I392" s="23" t="s">
@@ -10203,7 +10214,7 @@
       </c>
       <c r="F393" s="22"/>
       <c r="G393" s="23" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H393" s="23"/>
       <c r="I393" s="23" t="s">
@@ -10225,7 +10236,7 @@
       </c>
       <c r="F394" s="22"/>
       <c r="G394" s="23" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="H394" s="23"/>
       <c r="I394" s="23" t="s">
@@ -10247,7 +10258,7 @@
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="16" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B397" s="17"/>
       <c r="C397" s="18"/>
@@ -10294,7 +10305,7 @@
     </row>
     <row r="400" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="21" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B400" s="22" t="s">
         <v>21</v>
@@ -10310,26 +10321,28 @@
         <v>22</v>
       </c>
       <c r="G400" s="23" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="H400" s="23" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="I400" s="23"/>
     </row>
-    <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="401" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="21"/>
       <c r="B401" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C401" s="25"/>
       <c r="D401" s="22"/>
-      <c r="E401" s="25"/>
+      <c r="E401" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F401" s="22" t="s">
         <v>22</v>
       </c>
       <c r="G401" s="23" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="H401" s="23"/>
       <c r="I401" s="23"/>
@@ -10345,10 +10358,10 @@
       <c r="F402" s="22"/>
       <c r="G402" s="30"/>
       <c r="H402" s="23" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="I402" s="23" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10362,10 +10375,10 @@
       <c r="F403" s="22"/>
       <c r="G403" s="30"/>
       <c r="H403" s="23" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="I403" s="23" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10379,10 +10392,10 @@
       <c r="F404" s="22"/>
       <c r="G404" s="30"/>
       <c r="H404" s="23" t="s">
+        <v>487</v>
+      </c>
+      <c r="I404" s="23" t="s">
         <v>486</v>
-      </c>
-      <c r="I404" s="23" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10399,10 +10412,10 @@
       </c>
       <c r="F405" s="22"/>
       <c r="G405" s="23" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="H405" s="23" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="I405" s="23"/>
     </row>
@@ -10422,11 +10435,11 @@
       </c>
       <c r="F406" s="22"/>
       <c r="G406" s="23" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="H406" s="23"/>
       <c r="I406" s="23" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10443,10 +10456,10 @@
       </c>
       <c r="F407" s="22"/>
       <c r="G407" s="23" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="H407" s="23" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="I407" s="23"/>
     </row>
@@ -10464,28 +10477,30 @@
       </c>
       <c r="F408" s="22"/>
       <c r="G408" s="23" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="H408" s="23" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="I408" s="23"/>
     </row>
-    <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="409" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="19"/>
-      <c r="B409" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="C409" s="22"/>
+      <c r="B409" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C409" s="25"/>
       <c r="D409" s="22"/>
-      <c r="E409" s="22"/>
+      <c r="E409" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F409" s="22"/>
       <c r="G409" s="23"/>
       <c r="H409" s="23" t="s">
         <v>246</v>
       </c>
       <c r="I409" s="23" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10504,10 +10519,10 @@
         <v>22</v>
       </c>
       <c r="G410" s="23" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="H410" s="23" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="I410" s="23" t="s">
         <v>196</v>
@@ -10528,10 +10543,10 @@
         <v>22</v>
       </c>
       <c r="G411" s="23" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H411" s="23" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="I411" s="23" t="s">
         <v>196</v>
@@ -10569,7 +10584,7 @@
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="21" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B414" s="29" t="s">
         <v>202</v>
@@ -10586,7 +10601,7 @@
       </c>
       <c r="G414" s="30"/>
       <c r="H414" s="23" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="I414" s="23"/>
     </row>
@@ -10606,10 +10621,10 @@
         <v>22</v>
       </c>
       <c r="G415" s="23" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H415" s="23" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="I415" s="23"/>
     </row>
@@ -10626,28 +10641,30 @@
       </c>
       <c r="F416" s="22"/>
       <c r="G416" s="23" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="H416" s="23" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="I416" s="23"/>
     </row>
-    <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="417" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="19"/>
-      <c r="B417" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="C417" s="22"/>
+      <c r="B417" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C417" s="25"/>
       <c r="D417" s="22"/>
-      <c r="E417" s="22"/>
+      <c r="E417" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="F417" s="22"/>
       <c r="G417" s="23"/>
       <c r="H417" s="23" t="s">
         <v>246</v>
       </c>
       <c r="I417" s="23" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10685,7 +10702,7 @@
     </row>
     <row r="421" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="21" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B421" s="22" t="s">
         <v>21</v>
@@ -10701,10 +10718,10 @@
         <v>22</v>
       </c>
       <c r="G421" s="23" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="H421" s="23" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="I421" s="23"/>
     </row>
@@ -10725,10 +10742,10 @@
       </c>
       <c r="G422" s="30"/>
       <c r="H422" s="23" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="I422" s="23" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10748,10 +10765,10 @@
       </c>
       <c r="G423" s="30"/>
       <c r="H423" s="23" t="s">
+        <v>512</v>
+      </c>
+      <c r="I423" s="23" t="s">
         <v>511</v>
-      </c>
-      <c r="I423" s="23" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10770,10 +10787,10 @@
         <v>22</v>
       </c>
       <c r="G424" s="23" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="H424" s="23" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="I424" s="23"/>
     </row>
@@ -10793,10 +10810,10 @@
         <v>22</v>
       </c>
       <c r="G425" s="23" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="H425" s="23" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="I425" s="23"/>
     </row>
@@ -10816,10 +10833,10 @@
         <v>22</v>
       </c>
       <c r="G426" s="23" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="H426" s="23" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="I426" s="23"/>
     </row>
@@ -10834,10 +10851,10 @@
       <c r="F427" s="22"/>
       <c r="G427" s="30"/>
       <c r="H427" s="23" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="I427" s="23" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10851,7 +10868,7 @@
       <c r="F428" s="22"/>
       <c r="G428" s="30"/>
       <c r="H428" s="23" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="I428" s="23"/>
     </row>
@@ -10866,10 +10883,10 @@
       <c r="F429" s="22"/>
       <c r="G429" s="30"/>
       <c r="H429" s="23" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="I429" s="23" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10883,7 +10900,7 @@
       <c r="F430" s="22"/>
       <c r="G430" s="30"/>
       <c r="H430" s="23" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="I430" s="23"/>
     </row>
@@ -10898,10 +10915,10 @@
       <c r="F431" s="22"/>
       <c r="G431" s="30"/>
       <c r="H431" s="23" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="I431" s="23" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10915,10 +10932,10 @@
       <c r="F432" s="22"/>
       <c r="G432" s="30"/>
       <c r="H432" s="23" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="I432" s="23" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10938,10 +10955,10 @@
       </c>
       <c r="G433" s="30"/>
       <c r="H433" s="23" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="I433" s="23" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10955,10 +10972,10 @@
       <c r="F434" s="22"/>
       <c r="G434" s="30"/>
       <c r="H434" s="23" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="I434" s="23" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10977,10 +10994,10 @@
         <v>22</v>
       </c>
       <c r="G435" s="23" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="H435" s="23" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="I435" s="23"/>
     </row>
@@ -11002,7 +11019,7 @@
         <v>22</v>
       </c>
       <c r="G436" s="23" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="H436" s="23"/>
       <c r="I436" s="23"/>
@@ -11024,7 +11041,7 @@
         <v>22</v>
       </c>
       <c r="G437" s="23" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="H437" s="23"/>
       <c r="I437" s="23"/>
@@ -11032,7 +11049,7 @@
     <row r="438" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="19"/>
       <c r="H438" s="36" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11067,7 +11084,7 @@
     </row>
     <row r="441" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="21" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B441" s="22" t="s">
         <v>21</v>
@@ -11081,13 +11098,13 @@
       </c>
       <c r="F441" s="22"/>
       <c r="G441" s="23" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="H441" s="23" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="I441" s="23" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11104,13 +11121,13 @@
       </c>
       <c r="F442" s="22"/>
       <c r="G442" s="23" t="s">
+        <v>536</v>
+      </c>
+      <c r="H442" s="23" t="s">
+        <v>537</v>
+      </c>
+      <c r="I442" s="23" t="s">
         <v>535</v>
-      </c>
-      <c r="H442" s="23" t="s">
-        <v>536</v>
-      </c>
-      <c r="I442" s="23" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11127,13 +11144,13 @@
       </c>
       <c r="F443" s="22"/>
       <c r="G443" s="23" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="H443" s="23" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="I443" s="23" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11150,13 +11167,13 @@
       </c>
       <c r="F444" s="22"/>
       <c r="G444" s="23" t="s">
+        <v>541</v>
+      </c>
+      <c r="H444" s="23" t="s">
+        <v>542</v>
+      </c>
+      <c r="I444" s="23" t="s">
         <v>540</v>
-      </c>
-      <c r="H444" s="23" t="s">
-        <v>541</v>
-      </c>
-      <c r="I444" s="23" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11172,10 +11189,10 @@
       </c>
       <c r="F445" s="22"/>
       <c r="G445" s="23" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="H445" s="23" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="I445" s="23"/>
     </row>
@@ -11211,7 +11228,7 @@
     </row>
     <row r="448" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="37" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B448" s="29" t="s">
         <v>202</v>
@@ -11228,10 +11245,10 @@
       </c>
       <c r="G448" s="30"/>
       <c r="H448" s="23" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="I448" s="23" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11251,10 +11268,10 @@
       </c>
       <c r="G449" s="30"/>
       <c r="H449" s="23" t="s">
+        <v>548</v>
+      </c>
+      <c r="I449" s="23" t="s">
         <v>547</v>
-      </c>
-      <c r="I449" s="23" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11274,10 +11291,10 @@
       </c>
       <c r="G450" s="30"/>
       <c r="H450" s="23" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="I450" s="23" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11315,7 +11332,7 @@
     </row>
     <row r="454" customFormat="false" ht="96.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="37" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B454" s="22" t="s">
         <v>21</v>
@@ -11329,10 +11346,10 @@
       </c>
       <c r="F454" s="22"/>
       <c r="G454" s="23" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="H454" s="23" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="I454" s="23"/>
     </row>
@@ -11350,13 +11367,13 @@
       </c>
       <c r="F455" s="22"/>
       <c r="G455" s="23" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="H455" s="23" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="I455" s="38" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11375,7 +11392,7 @@
       </c>
       <c r="F456" s="22"/>
       <c r="G456" s="23" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="H456" s="23"/>
       <c r="I456" s="23"/>
@@ -11396,7 +11413,7 @@
       </c>
       <c r="F457" s="22"/>
       <c r="G457" s="23" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="H457" s="23"/>
       <c r="I457" s="23"/>
@@ -11416,11 +11433,11 @@
       </c>
       <c r="F458" s="22"/>
       <c r="G458" s="23" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="H458" s="23"/>
       <c r="I458" s="38" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11455,7 +11472,7 @@
     </row>
     <row r="461" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="37" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B461" s="22" t="s">
         <v>21</v>
@@ -11469,10 +11486,10 @@
       </c>
       <c r="F461" s="22"/>
       <c r="G461" s="23" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="H461" s="23" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="I461" s="23"/>
     </row>
@@ -11493,7 +11510,7 @@
       </c>
       <c r="G462" s="30"/>
       <c r="H462" s="23" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="I462" s="23"/>
     </row>
@@ -11513,7 +11530,7 @@
       </c>
       <c r="F463" s="22"/>
       <c r="G463" s="23" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="H463" s="23"/>
       <c r="I463" s="23"/>
@@ -11534,7 +11551,7 @@
       </c>
       <c r="F464" s="22"/>
       <c r="G464" s="23" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="H464" s="23"/>
       <c r="I464" s="23"/>
@@ -11555,7 +11572,7 @@
       </c>
       <c r="F465" s="22"/>
       <c r="G465" s="23" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="H465" s="23"/>
       <c r="I465" s="23"/>
@@ -11575,7 +11592,7 @@
       </c>
       <c r="F466" s="22"/>
       <c r="G466" s="23" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="H466" s="23"/>
       <c r="I466" s="23"/>
@@ -11615,7 +11632,7 @@
     </row>
     <row r="469" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="21" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B469" s="22" t="s">
         <v>21</v>
@@ -11629,10 +11646,10 @@
       </c>
       <c r="F469" s="22"/>
       <c r="G469" s="23" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="H469" s="23" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="I469" s="23"/>
     </row>
@@ -11648,10 +11665,10 @@
       </c>
       <c r="F470" s="22"/>
       <c r="G470" s="23" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="H470" s="23" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="I470" s="23"/>
     </row>
@@ -11672,7 +11689,7 @@
       </c>
       <c r="G471" s="23"/>
       <c r="H471" s="23" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="I471" s="23"/>
     </row>
@@ -11692,7 +11709,7 @@
       </c>
       <c r="G472" s="23"/>
       <c r="H472" s="23" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="I472" s="23"/>
     </row>
@@ -11728,7 +11745,7 @@
     </row>
     <row r="475" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="21" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B475" s="22" t="s">
         <v>21</v>
@@ -11742,7 +11759,7 @@
       </c>
       <c r="F475" s="22"/>
       <c r="G475" s="23" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="H475" s="23"/>
       <c r="I475" s="23"/>
@@ -11761,7 +11778,7 @@
       </c>
       <c r="F476" s="22"/>
       <c r="G476" s="23" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="H476" s="23"/>
       <c r="I476" s="23"/>
@@ -11780,11 +11797,11 @@
       </c>
       <c r="F477" s="22"/>
       <c r="G477" s="23" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="H477" s="23"/>
       <c r="I477" s="23" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11803,7 +11820,7 @@
       </c>
       <c r="F478" s="22"/>
       <c r="G478" s="23" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="H478" s="23"/>
       <c r="I478" s="23"/>
@@ -11822,7 +11839,7 @@
       </c>
       <c r="F479" s="22"/>
       <c r="G479" s="23" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="H479" s="23"/>
       <c r="I479" s="23"/>
@@ -11841,7 +11858,7 @@
       </c>
       <c r="F480" s="22"/>
       <c r="G480" s="23" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="H480" s="23"/>
       <c r="I480" s="23"/>
@@ -11860,7 +11877,7 @@
       </c>
       <c r="F481" s="22"/>
       <c r="G481" s="23" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="H481" s="23"/>
       <c r="I481" s="23"/>
@@ -11879,11 +11896,11 @@
       </c>
       <c r="F482" s="22"/>
       <c r="G482" s="23" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="H482" s="23"/>
       <c r="I482" s="23" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11900,7 +11917,7 @@
       </c>
       <c r="F483" s="22"/>
       <c r="G483" s="23" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H483" s="23"/>
       <c r="I483" s="23"/>
@@ -11919,7 +11936,7 @@
       </c>
       <c r="F484" s="22"/>
       <c r="G484" s="23" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="H484" s="23"/>
       <c r="I484" s="23"/>
@@ -11938,7 +11955,7 @@
       </c>
       <c r="F485" s="22"/>
       <c r="G485" s="23" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="H485" s="23"/>
       <c r="I485" s="23"/>
@@ -11956,7 +11973,7 @@
       </c>
       <c r="F486" s="22"/>
       <c r="G486" s="23" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="H486" s="23"/>
       <c r="I486" s="23"/>
@@ -11976,7 +11993,7 @@
     </row>
     <row r="489" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="16" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B489" s="17"/>
       <c r="C489" s="18"/>
@@ -12023,7 +12040,7 @@
     </row>
     <row r="492" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="37" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B492" s="22" t="s">
         <v>21</v>
@@ -12037,10 +12054,10 @@
       </c>
       <c r="F492" s="22"/>
       <c r="G492" s="23" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H492" s="23" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="I492" s="23"/>
     </row>
@@ -12058,10 +12075,10 @@
       </c>
       <c r="F493" s="22"/>
       <c r="G493" s="23" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="H493" s="23" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="I493" s="23"/>
     </row>
@@ -12080,13 +12097,13 @@
         <v>22</v>
       </c>
       <c r="G494" s="23" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="H494" s="23" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="I494" s="23" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12121,7 +12138,7 @@
     </row>
     <row r="497" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="21" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B497" s="22" t="s">
         <v>21</v>
@@ -12135,10 +12152,10 @@
       </c>
       <c r="F497" s="22"/>
       <c r="G497" s="23" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="H497" s="23" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="I497" s="23"/>
     </row>
@@ -12156,10 +12173,10 @@
       </c>
       <c r="F498" s="22"/>
       <c r="G498" s="23" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="H498" s="23" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="I498" s="23"/>
     </row>
@@ -12178,10 +12195,10 @@
         <v>22</v>
       </c>
       <c r="G499" s="23" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="H499" s="23" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="I499" s="23"/>
     </row>
@@ -12217,7 +12234,7 @@
     </row>
     <row r="502" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="21" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B502" s="22" t="s">
         <v>21</v>
@@ -12231,10 +12248,10 @@
       </c>
       <c r="F502" s="22"/>
       <c r="G502" s="23" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="H502" s="23" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="I502" s="23"/>
     </row>
@@ -12252,13 +12269,13 @@
       </c>
       <c r="F503" s="22"/>
       <c r="G503" s="23" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="H503" s="23" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="I503" s="23" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12276,13 +12293,13 @@
         <v>22</v>
       </c>
       <c r="G504" s="23" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="H504" s="23" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="I504" s="23" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12317,7 +12334,7 @@
     </row>
     <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="21" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B507" s="33" t="s">
         <v>202</v>
@@ -12329,11 +12346,11 @@
       <c r="E507" s="25"/>
       <c r="F507" s="22"/>
       <c r="G507" s="23" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="H507" s="23"/>
       <c r="I507" s="39" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12348,11 +12365,11 @@
       <c r="E508" s="25"/>
       <c r="F508" s="22"/>
       <c r="G508" s="23" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="H508" s="23"/>
       <c r="I508" s="39" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12368,11 +12385,11 @@
         <v>22</v>
       </c>
       <c r="G509" s="23" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="H509" s="23"/>
       <c r="I509" s="39" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12407,7 +12424,7 @@
     </row>
     <row r="512" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="37" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B512" s="22" t="s">
         <v>21</v>
@@ -12423,7 +12440,7 @@
         <v>22</v>
       </c>
       <c r="G512" s="23" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="H512" s="23"/>
       <c r="I512" s="23"/>
@@ -12442,7 +12459,7 @@
       </c>
       <c r="F513" s="22"/>
       <c r="G513" s="23" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="H513" s="23"/>
       <c r="I513" s="23"/>
@@ -12460,7 +12477,7 @@
       </c>
       <c r="F514" s="22"/>
       <c r="G514" s="23" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="H514" s="23"/>
       <c r="I514" s="23"/>
@@ -12497,7 +12514,7 @@
     </row>
     <row r="517" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="37" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B517" s="22" t="s">
         <v>21</v>
@@ -12511,10 +12528,10 @@
       </c>
       <c r="F517" s="22"/>
       <c r="G517" s="23" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="H517" s="23" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="I517" s="23"/>
     </row>
@@ -12532,10 +12549,10 @@
       </c>
       <c r="F518" s="22"/>
       <c r="G518" s="23" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="H518" s="23" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="I518" s="23"/>
     </row>
@@ -12554,13 +12571,13 @@
         <v>22</v>
       </c>
       <c r="G519" s="23" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H519" s="23" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="I519" s="23" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12568,13 +12585,13 @@
     </row>
     <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="21" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="40"/>
       <c r="B522" s="41" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C522" s="41"/>
       <c r="D522" s="41"/>
@@ -12614,7 +12631,7 @@
     </row>
     <row r="525" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="21" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B525" s="22" t="s">
         <v>21</v>
@@ -12630,10 +12647,10 @@
         <v>22</v>
       </c>
       <c r="G525" s="23" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="H525" s="23" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="I525" s="23"/>
     </row>
@@ -12652,10 +12669,10 @@
         <v>22</v>
       </c>
       <c r="G526" s="23" t="s">
+        <v>626</v>
+      </c>
+      <c r="H526" s="23" t="s">
         <v>625</v>
-      </c>
-      <c r="H526" s="23" t="s">
-        <v>624</v>
       </c>
       <c r="I526" s="23"/>
     </row>
@@ -12674,7 +12691,7 @@
     </row>
     <row r="529" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="16" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B529" s="17"/>
       <c r="C529" s="18"/>
@@ -12694,12 +12711,12 @@
     </row>
     <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="9" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="9" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12731,7 +12748,7 @@
     </row>
     <row r="534" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="21" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B534" s="22" t="s">
         <v>21</v>
@@ -12747,7 +12764,7 @@
       </c>
       <c r="F534" s="22"/>
       <c r="G534" s="23" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="H534" s="23"/>
       <c r="I534" s="23"/>
@@ -12770,7 +12787,7 @@
         <v>22</v>
       </c>
       <c r="G535" s="23" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="H535" s="23"/>
       <c r="I535" s="23"/>
@@ -12793,7 +12810,7 @@
         <v>22</v>
       </c>
       <c r="G536" s="23" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="H536" s="23"/>
       <c r="I536" s="23"/>
@@ -12816,7 +12833,7 @@
         <v>22</v>
       </c>
       <c r="G537" s="23" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="H537" s="23"/>
       <c r="I537" s="23"/>
@@ -12837,11 +12854,11 @@
       </c>
       <c r="F538" s="25"/>
       <c r="G538" s="23" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="H538" s="23"/>
       <c r="I538" s="23" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12859,14 +12876,14 @@
         <v>59</v>
       </c>
       <c r="F539" s="25" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G539" s="23" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="H539" s="23"/>
       <c r="I539" s="23" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12885,7 +12902,7 @@
       </c>
       <c r="F540" s="22"/>
       <c r="G540" s="23" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="H540" s="23"/>
       <c r="I540" s="23"/>
@@ -12906,7 +12923,7 @@
       </c>
       <c r="F541" s="22"/>
       <c r="G541" s="23" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H541" s="23"/>
       <c r="I541" s="23"/>
@@ -12925,7 +12942,7 @@
       </c>
       <c r="F542" s="22"/>
       <c r="G542" s="23" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="H542" s="23"/>
       <c r="I542" s="23"/>
@@ -12946,7 +12963,7 @@
       </c>
       <c r="F543" s="22"/>
       <c r="G543" s="23" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="H543" s="23"/>
       <c r="I543" s="23"/>
@@ -12967,7 +12984,7 @@
       </c>
       <c r="F544" s="22"/>
       <c r="G544" s="23" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="H544" s="23"/>
       <c r="I544" s="23" t="s">
@@ -12990,7 +13007,7 @@
       </c>
       <c r="F545" s="22"/>
       <c r="G545" s="23" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="H545" s="23"/>
       <c r="I545" s="23" t="s">
@@ -13013,7 +13030,7 @@
       </c>
       <c r="F546" s="22"/>
       <c r="G546" s="23" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="H546" s="23"/>
       <c r="I546" s="23"/>
@@ -13034,7 +13051,7 @@
       </c>
       <c r="F547" s="22"/>
       <c r="G547" s="23" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="H547" s="23"/>
       <c r="I547" s="23" t="s">
@@ -13057,7 +13074,7 @@
       </c>
       <c r="F548" s="22"/>
       <c r="G548" s="23" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="H548" s="23"/>
       <c r="I548" s="23"/>
@@ -13078,7 +13095,7 @@
       </c>
       <c r="F549" s="22"/>
       <c r="G549" s="23" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="H549" s="23"/>
       <c r="I549" s="23" t="s">
@@ -13101,7 +13118,7 @@
       </c>
       <c r="F550" s="22"/>
       <c r="G550" s="23" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="H550" s="23"/>
       <c r="I550" s="23" t="s">
@@ -13124,7 +13141,7 @@
       </c>
       <c r="F551" s="22"/>
       <c r="G551" s="23" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="H551" s="23"/>
       <c r="I551" s="23"/>
@@ -13145,7 +13162,7 @@
       </c>
       <c r="F552" s="22"/>
       <c r="G552" s="23" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H552" s="23"/>
       <c r="I552" s="23"/>
@@ -13166,7 +13183,7 @@
       </c>
       <c r="F553" s="22"/>
       <c r="G553" s="23" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="H553" s="23"/>
       <c r="I553" s="23"/>
@@ -13187,7 +13204,7 @@
       </c>
       <c r="F554" s="22"/>
       <c r="G554" s="23" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="H554" s="23"/>
       <c r="I554" s="23"/>
@@ -13207,7 +13224,7 @@
       </c>
       <c r="F555" s="22"/>
       <c r="G555" s="23" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="H555" s="23"/>
       <c r="I555" s="23"/>
@@ -13231,7 +13248,7 @@
     </row>
     <row r="559" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="16" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B559" s="17"/>
       <c r="C559" s="18"/>
@@ -13251,12 +13268,12 @@
     </row>
     <row r="561" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="9" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="9" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13288,7 +13305,7 @@
     </row>
     <row r="564" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="21" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B564" s="22" t="s">
         <v>21</v>
@@ -13306,7 +13323,7 @@
         <v>22</v>
       </c>
       <c r="G564" s="23" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H564" s="23"/>
       <c r="I564" s="23"/>
@@ -13329,7 +13346,7 @@
         <v>22</v>
       </c>
       <c r="G565" s="23" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="H565" s="23"/>
       <c r="I565" s="23"/>
@@ -13352,7 +13369,7 @@
         <v>22</v>
       </c>
       <c r="G566" s="23" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="H566" s="23"/>
       <c r="I566" s="23"/>
@@ -13375,7 +13392,7 @@
         <v>22</v>
       </c>
       <c r="G567" s="23" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="H567" s="23"/>
       <c r="I567" s="23"/>
@@ -13398,7 +13415,7 @@
         <v>22</v>
       </c>
       <c r="G568" s="23" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H568" s="23"/>
       <c r="I568" s="23"/>
@@ -13421,7 +13438,7 @@
         <v>22</v>
       </c>
       <c r="G569" s="23" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="H569" s="23"/>
       <c r="I569" s="23"/>
@@ -13444,7 +13461,7 @@
         <v>22</v>
       </c>
       <c r="G570" s="23" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="H570" s="23"/>
       <c r="I570" s="23"/>
@@ -13467,7 +13484,7 @@
         <v>22</v>
       </c>
       <c r="G571" s="23" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="H571" s="23"/>
       <c r="I571" s="23"/>
@@ -13490,7 +13507,7 @@
         <v>22</v>
       </c>
       <c r="G572" s="23" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="H572" s="23"/>
       <c r="I572" s="23"/>
@@ -13513,7 +13530,7 @@
         <v>22</v>
       </c>
       <c r="G573" s="23" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="H573" s="23"/>
       <c r="I573" s="23"/>
@@ -13536,7 +13553,7 @@
         <v>22</v>
       </c>
       <c r="G574" s="23" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="H574" s="23"/>
       <c r="I574" s="23"/>
@@ -13559,7 +13576,7 @@
         <v>22</v>
       </c>
       <c r="G575" s="23" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="H575" s="23"/>
       <c r="I575" s="23"/>
@@ -13581,7 +13598,7 @@
         <v>22</v>
       </c>
       <c r="G576" s="23" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="H576" s="23"/>
       <c r="I576" s="23"/>
@@ -13604,7 +13621,7 @@
     </row>
     <row r="580" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="16" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B580" s="17"/>
       <c r="C580" s="18"/>
@@ -13624,12 +13641,12 @@
     </row>
     <row r="582" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="9" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="583" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="9" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="584" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13661,7 +13678,7 @@
     </row>
     <row r="585" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="21" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B585" s="22" t="s">
         <v>21</v>
@@ -13677,7 +13694,7 @@
       </c>
       <c r="F585" s="22"/>
       <c r="G585" s="23" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="H585" s="23"/>
       <c r="I585" s="23"/>
@@ -13698,7 +13715,7 @@
       </c>
       <c r="F586" s="22"/>
       <c r="G586" s="23" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="H586" s="23"/>
       <c r="I586" s="23"/>
@@ -13719,7 +13736,7 @@
       </c>
       <c r="F587" s="22"/>
       <c r="G587" s="23" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="H587" s="23"/>
       <c r="I587" s="23"/>
@@ -13739,7 +13756,7 @@
       </c>
       <c r="F588" s="22"/>
       <c r="G588" s="23" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="H588" s="23"/>
       <c r="I588" s="23"/>
@@ -13759,7 +13776,7 @@
     </row>
     <row r="591" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="16" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B591" s="17"/>
       <c r="C591" s="18"/>
@@ -13806,7 +13823,7 @@
     </row>
     <row r="594" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="21" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B594" s="22" t="s">
         <v>21</v>
@@ -13817,10 +13834,10 @@
         <v>21</v>
       </c>
       <c r="F594" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G594" s="23" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="H594" s="23"/>
       <c r="I594" s="23"/>
@@ -13840,10 +13857,10 @@
         <v>21</v>
       </c>
       <c r="F595" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G595" s="23" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="H595" s="23"/>
       <c r="I595" s="23"/>
@@ -13863,10 +13880,10 @@
         <v>21</v>
       </c>
       <c r="F596" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G596" s="23" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H596" s="23"/>
       <c r="I596" s="23"/>
@@ -13886,10 +13903,10 @@
         <v>21</v>
       </c>
       <c r="F597" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G597" s="23" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H597" s="23"/>
       <c r="I597" s="23"/>
@@ -13905,10 +13922,10 @@
         <v>21</v>
       </c>
       <c r="F598" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G598" s="23" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="H598" s="23"/>
       <c r="I598" s="23"/>
@@ -13922,14 +13939,14 @@
       <c r="D599" s="22"/>
       <c r="E599" s="25"/>
       <c r="F599" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G599" s="23" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="H599" s="23"/>
       <c r="I599" s="23" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="600" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13945,10 +13962,10 @@
         <v>21</v>
       </c>
       <c r="F600" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G600" s="23" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="H600" s="23"/>
       <c r="I600" s="23"/>
@@ -13968,10 +13985,10 @@
         <v>21</v>
       </c>
       <c r="F601" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G601" s="23" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="H601" s="23"/>
       <c r="I601" s="23"/>
@@ -13991,10 +14008,10 @@
         <v>21</v>
       </c>
       <c r="F602" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G602" s="23" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="H602" s="23"/>
       <c r="I602" s="23"/>
@@ -14014,10 +14031,10 @@
         <v>21</v>
       </c>
       <c r="F603" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G603" s="23" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="H603" s="23"/>
       <c r="I603" s="23"/>
@@ -14033,10 +14050,10 @@
         <v>21</v>
       </c>
       <c r="F604" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G604" s="23" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="H604" s="23"/>
       <c r="I604" s="23"/>
@@ -14056,10 +14073,10 @@
         <v>21</v>
       </c>
       <c r="F605" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G605" s="23" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="H605" s="23"/>
       <c r="I605" s="23"/>
@@ -14079,10 +14096,10 @@
         <v>21</v>
       </c>
       <c r="F606" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G606" s="23" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H606" s="23"/>
       <c r="I606" s="23"/>
@@ -14100,10 +14117,10 @@
         <v>21</v>
       </c>
       <c r="F607" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G607" s="23" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="H607" s="23"/>
       <c r="I607" s="23"/>
@@ -14121,10 +14138,10 @@
         <v>21</v>
       </c>
       <c r="F608" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G608" s="23" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="H608" s="23"/>
       <c r="I608" s="23"/>
@@ -14140,10 +14157,10 @@
         <v>21</v>
       </c>
       <c r="F609" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G609" s="23" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="H609" s="23"/>
       <c r="I609" s="23"/>
@@ -14161,10 +14178,10 @@
         <v>21</v>
       </c>
       <c r="F610" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G610" s="23" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="H610" s="23"/>
       <c r="I610" s="23"/>
@@ -14182,10 +14199,10 @@
         <v>21</v>
       </c>
       <c r="F611" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G611" s="23" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="H611" s="23"/>
       <c r="I611" s="23"/>
@@ -14203,10 +14220,10 @@
         <v>21</v>
       </c>
       <c r="F612" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G612" s="23" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="H612" s="23"/>
       <c r="I612" s="23"/>
@@ -14226,10 +14243,10 @@
         <v>21</v>
       </c>
       <c r="F613" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G613" s="23" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="H613" s="23"/>
       <c r="I613" s="23"/>
@@ -14249,10 +14266,10 @@
         <v>21</v>
       </c>
       <c r="F614" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G614" s="23" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="H614" s="23"/>
       <c r="I614" s="23"/>
@@ -14268,10 +14285,10 @@
         <v>21</v>
       </c>
       <c r="F615" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G615" s="23" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="H615" s="23"/>
       <c r="I615" s="23"/>
@@ -14291,10 +14308,10 @@
         <v>21</v>
       </c>
       <c r="F616" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G616" s="23" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="H616" s="23"/>
       <c r="I616" s="23"/>
@@ -14314,10 +14331,10 @@
         <v>21</v>
       </c>
       <c r="F617" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G617" s="23" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="H617" s="23"/>
       <c r="I617" s="23"/>
@@ -14337,10 +14354,10 @@
         <v>21</v>
       </c>
       <c r="F618" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G618" s="23" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="H618" s="23"/>
       <c r="I618" s="23"/>
@@ -14356,10 +14373,10 @@
         <v>21</v>
       </c>
       <c r="F619" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G619" s="23" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="H619" s="23"/>
       <c r="I619" s="23"/>
@@ -14379,10 +14396,10 @@
         <v>21</v>
       </c>
       <c r="F620" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G620" s="23" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="H620" s="23"/>
       <c r="I620" s="23"/>
@@ -14402,10 +14419,10 @@
         <v>21</v>
       </c>
       <c r="F621" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G621" s="23" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="H621" s="23"/>
       <c r="I621" s="23"/>
@@ -14425,10 +14442,10 @@
         <v>21</v>
       </c>
       <c r="F622" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G622" s="23" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H622" s="23"/>
       <c r="I622" s="23"/>
@@ -14448,10 +14465,10 @@
         <v>21</v>
       </c>
       <c r="F623" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G623" s="23" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H623" s="23"/>
       <c r="I623" s="23"/>
@@ -14471,10 +14488,10 @@
         <v>21</v>
       </c>
       <c r="F624" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G624" s="23" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="H624" s="23"/>
       <c r="I624" s="23"/>
@@ -14490,10 +14507,10 @@
         <v>21</v>
       </c>
       <c r="F625" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G625" s="23" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="H625" s="23"/>
       <c r="I625" s="23"/>
@@ -14513,10 +14530,10 @@
         <v>21</v>
       </c>
       <c r="F626" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G626" s="23" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="H626" s="23"/>
       <c r="I626" s="23"/>
@@ -14536,10 +14553,10 @@
         <v>21</v>
       </c>
       <c r="F627" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G627" s="23" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="H627" s="23"/>
       <c r="I627" s="23"/>
@@ -14559,10 +14576,10 @@
         <v>21</v>
       </c>
       <c r="F628" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G628" s="23" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="H628" s="23"/>
       <c r="I628" s="23"/>
@@ -14582,10 +14599,10 @@
         <v>21</v>
       </c>
       <c r="F629" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G629" s="23" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="H629" s="23"/>
       <c r="I629" s="23"/>
@@ -14599,10 +14616,10 @@
       </c>
       <c r="E630" s="25"/>
       <c r="F630" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G630" s="23" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="H630" s="23"/>
       <c r="I630" s="23"/>
@@ -14622,10 +14639,10 @@
         <v>21</v>
       </c>
       <c r="F631" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G631" s="23" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="H631" s="23"/>
       <c r="I631" s="23"/>
@@ -14645,10 +14662,10 @@
         <v>21</v>
       </c>
       <c r="F632" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G632" s="23" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="H632" s="23"/>
       <c r="I632" s="23"/>
@@ -14668,10 +14685,10 @@
         <v>21</v>
       </c>
       <c r="F633" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G633" s="23" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="H633" s="23"/>
       <c r="I633" s="23"/>
@@ -14691,10 +14708,10 @@
         <v>21</v>
       </c>
       <c r="F634" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G634" s="23" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="H634" s="23"/>
       <c r="I634" s="23"/>
@@ -14714,10 +14731,10 @@
         <v>21</v>
       </c>
       <c r="F635" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G635" s="23" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="H635" s="23"/>
       <c r="I635" s="23"/>
@@ -14737,10 +14754,10 @@
         <v>21</v>
       </c>
       <c r="F636" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G636" s="23" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="H636" s="23"/>
       <c r="I636" s="23"/>
@@ -14760,10 +14777,10 @@
         <v>21</v>
       </c>
       <c r="F637" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G637" s="23" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="H637" s="23"/>
       <c r="I637" s="23"/>
@@ -14779,10 +14796,10 @@
         <v>21</v>
       </c>
       <c r="F638" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G638" s="23" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="H638" s="23"/>
       <c r="I638" s="23"/>
@@ -14798,10 +14815,10 @@
         <v>21</v>
       </c>
       <c r="F639" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G639" s="23" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="H639" s="23"/>
       <c r="I639" s="23"/>
@@ -14817,10 +14834,10 @@
         <v>21</v>
       </c>
       <c r="F640" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G640" s="23" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="H640" s="23"/>
       <c r="I640" s="23"/>
@@ -14840,10 +14857,10 @@
         <v>21</v>
       </c>
       <c r="F641" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G641" s="23" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="H641" s="23"/>
       <c r="I641" s="23"/>
@@ -14863,10 +14880,10 @@
         <v>21</v>
       </c>
       <c r="F642" s="22" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G642" s="23" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="H642" s="23"/>
       <c r="I642" s="23"/>
@@ -14886,10 +14903,10 @@
         <v>21</v>
       </c>
       <c r="F643" s="22" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G643" s="23" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="H643" s="23"/>
       <c r="I643" s="23"/>
@@ -14907,56 +14924,56 @@
         <v>21</v>
       </c>
       <c r="F644" s="22" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G644" s="23" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="H644" s="23"/>
       <c r="I644" s="23" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="645" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="9"/>
       <c r="B645" s="27" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C645" s="27"/>
       <c r="D645" s="27" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E645" s="27"/>
       <c r="F645" s="27" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G645" s="28" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="H645" s="28"/>
       <c r="I645" s="28" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="646" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="9"/>
       <c r="B646" s="27" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C646" s="27"/>
       <c r="D646" s="27" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E646" s="27"/>
       <c r="F646" s="27" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G646" s="28" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="H646" s="28"/>
       <c r="I646" s="28" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="647" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14971,14 +14988,14 @@
         <v>21</v>
       </c>
       <c r="F647" s="22" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G647" s="23" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="H647" s="23"/>
       <c r="I647" s="23" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="655" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Misc state space updates -- Dont use yet !
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3627" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="928">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -2554,6 +2554,15 @@
     <t xml:space="preserve">STATE SPACE HELPER</t>
   </si>
   <si>
+    <t xml:space="preserve">MAT BUILDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MatBuilder_Fill.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MatBuilder_Create.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">MATRIX HELPER</t>
   </si>
   <si>
@@ -2563,9 +2572,6 @@
     <t xml:space="preserve">MatrixHelper_CooerceSize.vi</t>
   </si>
   <si>
-    <t xml:space="preserve">MatrixHelper_Create.vi</t>
-  </si>
-  <si>
     <t xml:space="preserve">VECTOR BUILDER</t>
   </si>
   <si>
@@ -2597,6 +2603,9 @@
   </si>
   <si>
     <t xml:space="preserve">VecBuilder_10x1Fill.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VecBuilder_ArrayBy1Fill.vi</t>
   </si>
   <si>
     <t xml:space="preserve">TYPE DEFINITIONS</t>
@@ -3256,8 +3265,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A570" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C570" activeCellId="0" sqref="C570"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A776" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B786" activeCellId="0" sqref="B786"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3348,28 +3357,28 @@
         <v>11</v>
       </c>
       <c r="B9" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1196,"X")</f>
-        <v>540</v>
+        <f aca="false">COUNTIF(B18:B1200,"X")</f>
+        <v>544</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C18:C1196,"X")</f>
+        <f aca="false">COUNTIF(C18:C1200,"X")</f>
         <v>368</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D18:D1196,"X")</f>
+        <f aca="false">COUNTIF(D18:D1200,"X")</f>
         <v>166</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E18:E1196,"X")</f>
-        <v>508</v>
+        <f aca="false">COUNTIF(E18:E1200,"X")</f>
+        <v>511</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F18:F1196,"S")+COUNTIF(F18:F1196,"I")+COUNTIF(F18:F1196,"X")+COUNTIF(F18:F1196,"SI")+COUNTIF(F18:F1196,"IS")+COUNTIF(F18:F1196,"N/A")</f>
+        <f aca="false">COUNTIF(F18:F1200,"S")+COUNTIF(F18:F1200,"I")+COUNTIF(F18:F1200,"X")+COUNTIF(F18:F1200,"SI")+COUNTIF(F18:F1200,"IS")+COUNTIF(F18:F1200,"N/A")</f>
         <v>211</v>
       </c>
       <c r="G9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.681481481481481</v>
+        <v>0.676470588235294</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3377,7 +3386,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="13" t="n">
-        <f aca="false">COUNTIF(B19:B1197,"/")</f>
+        <f aca="false">COUNTIF(B19:B1201,"/")</f>
         <v>8</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -3387,7 +3396,7 @@
     <row r="11" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.390740740740741</v>
+        <v>0.387867647058823</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18112,78 +18121,80 @@
     </row>
     <row r="782" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A782" s="19"/>
-      <c r="B782" s="44"/>
-      <c r="C782" s="4"/>
-      <c r="D782" s="4"/>
-      <c r="E782" s="4"/>
-      <c r="F782" s="4"/>
-    </row>
-    <row r="783" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B783" s="46"/>
-      <c r="C783" s="1"/>
-      <c r="D783" s="1"/>
-      <c r="E783" s="1"/>
-      <c r="F783" s="1"/>
-      <c r="G783" s="1"/>
-      <c r="H783" s="1"/>
-      <c r="I783" s="1"/>
-      <c r="J783" s="1"/>
-      <c r="K783" s="1"/>
-      <c r="L783" s="1"/>
-    </row>
-    <row r="784" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A784" s="19"/>
-      <c r="B784" s="11" t="s">
+      <c r="B782" s="19"/>
+      <c r="C782" s="19"/>
+      <c r="D782" s="19"/>
+      <c r="E782" s="19"/>
+      <c r="F782" s="19"/>
+    </row>
+    <row r="783" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A783" s="19"/>
+      <c r="B783" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C784" s="11" t="s">
+      <c r="C783" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D784" s="11" t="s">
+      <c r="D783" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E784" s="11" t="s">
+      <c r="E783" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F784" s="11" t="s">
+      <c r="F783" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G784" s="20" t="s">
+      <c r="G783" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H784" s="20" t="s">
+      <c r="H783" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I784" s="20" t="s">
+      <c r="I783" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J784" s="11" t="s">
+      <c r="J783" s="11" t="s">
         <v>690</v>
       </c>
-      <c r="K784" s="11" t="s">
+      <c r="K783" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="L784" s="11" t="s">
+      <c r="L783" s="11" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="785" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A785" s="21" t="s">
+    <row r="784" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A784" s="21" t="s">
         <v>843</v>
       </c>
+      <c r="B784" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C784" s="25"/>
+      <c r="D784" s="22"/>
+      <c r="E784" s="25"/>
+      <c r="F784" s="25"/>
+      <c r="G784" s="23" t="s">
+        <v>844</v>
+      </c>
+      <c r="H784" s="23"/>
+      <c r="I784" s="23"/>
+      <c r="J784" s="22"/>
+      <c r="K784" s="22"/>
+      <c r="L784" s="22"/>
+    </row>
+    <row r="785" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B785" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C785" s="25"/>
-      <c r="D785" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D785" s="22"/>
       <c r="E785" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F785" s="25"/>
       <c r="G785" s="23" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H785" s="23"/>
       <c r="I785" s="23"/>
@@ -18191,176 +18202,187 @@
       <c r="K785" s="22"/>
       <c r="L785" s="22"/>
     </row>
-    <row r="786" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B786" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C786" s="25"/>
-      <c r="D786" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E786" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F786" s="25"/>
-      <c r="G786" s="23" t="s">
-        <v>845</v>
-      </c>
-      <c r="H786" s="23"/>
-      <c r="I786" s="23"/>
-      <c r="J786" s="22"/>
-      <c r="K786" s="22"/>
-      <c r="L786" s="22"/>
-    </row>
-    <row r="787" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B787" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C787" s="25"/>
-      <c r="D787" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E787" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F787" s="25"/>
-      <c r="G787" s="23" t="s">
+    <row r="786" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A786" s="19"/>
+      <c r="B786" s="44"/>
+      <c r="C786" s="4"/>
+      <c r="D786" s="4"/>
+      <c r="E786" s="4"/>
+      <c r="F786" s="4"/>
+    </row>
+    <row r="787" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B787" s="46"/>
+      <c r="C787" s="1"/>
+      <c r="D787" s="1"/>
+      <c r="E787" s="1"/>
+      <c r="F787" s="1"/>
+      <c r="G787" s="1"/>
+      <c r="H787" s="1"/>
+      <c r="I787" s="1"/>
+      <c r="J787" s="1"/>
+      <c r="K787" s="1"/>
+      <c r="L787" s="1"/>
+    </row>
+    <row r="788" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A788" s="19"/>
+      <c r="B788" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C788" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D788" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E788" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F788" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G788" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H788" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I788" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J788" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K788" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L788" s="11" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="789" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A789" s="21" t="s">
         <v>846</v>
       </c>
-      <c r="H787" s="23"/>
-      <c r="I787" s="23"/>
-      <c r="J787" s="22"/>
-      <c r="K787" s="22"/>
-      <c r="L787" s="22"/>
-    </row>
-    <row r="788" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B788" s="1"/>
-      <c r="C788" s="1"/>
-      <c r="D788" s="1"/>
-      <c r="E788" s="1"/>
-      <c r="F788" s="1"/>
-      <c r="G788" s="1"/>
-      <c r="H788" s="1"/>
-      <c r="I788" s="1"/>
-      <c r="J788" s="1"/>
-      <c r="K788" s="1"/>
-      <c r="L788" s="1"/>
-      <c r="M788" s="1"/>
-      <c r="N788" s="1"/>
-    </row>
-    <row r="789" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B789" s="46"/>
-      <c r="C789" s="1"/>
-      <c r="D789" s="1"/>
-      <c r="E789" s="1"/>
-      <c r="F789" s="1"/>
-      <c r="G789" s="1"/>
-      <c r="H789" s="1"/>
-      <c r="I789" s="1"/>
-      <c r="J789" s="1"/>
-      <c r="K789" s="1"/>
-      <c r="L789" s="1"/>
-    </row>
-    <row r="790" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A790" s="19"/>
-      <c r="B790" s="11" t="s">
+      <c r="B789" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C789" s="25"/>
+      <c r="D789" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E789" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F789" s="25"/>
+      <c r="G789" s="23" t="s">
+        <v>847</v>
+      </c>
+      <c r="H789" s="23"/>
+      <c r="I789" s="23"/>
+      <c r="J789" s="22"/>
+      <c r="K789" s="22"/>
+      <c r="L789" s="22"/>
+    </row>
+    <row r="790" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B790" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C790" s="25"/>
+      <c r="D790" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E790" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F790" s="25"/>
+      <c r="G790" s="23" t="s">
+        <v>848</v>
+      </c>
+      <c r="H790" s="23"/>
+      <c r="I790" s="23"/>
+      <c r="J790" s="22"/>
+      <c r="K790" s="22"/>
+      <c r="L790" s="22"/>
+    </row>
+    <row r="791" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B791" s="1"/>
+      <c r="C791" s="1"/>
+      <c r="D791" s="1"/>
+      <c r="E791" s="1"/>
+      <c r="F791" s="1"/>
+      <c r="G791" s="1"/>
+      <c r="H791" s="1"/>
+      <c r="I791" s="1"/>
+      <c r="J791" s="1"/>
+      <c r="K791" s="1"/>
+      <c r="L791" s="1"/>
+      <c r="M791" s="1"/>
+      <c r="N791" s="1"/>
+    </row>
+    <row r="792" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B792" s="46"/>
+      <c r="C792" s="1"/>
+      <c r="D792" s="1"/>
+      <c r="E792" s="1"/>
+      <c r="F792" s="1"/>
+      <c r="G792" s="1"/>
+      <c r="H792" s="1"/>
+      <c r="I792" s="1"/>
+      <c r="J792" s="1"/>
+      <c r="K792" s="1"/>
+      <c r="L792" s="1"/>
+    </row>
+    <row r="793" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A793" s="19"/>
+      <c r="B793" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C790" s="11" t="s">
+      <c r="C793" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D790" s="11" t="s">
+      <c r="D793" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E790" s="11" t="s">
+      <c r="E793" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F790" s="11" t="s">
+      <c r="F793" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G790" s="20" t="s">
+      <c r="G793" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H790" s="20" t="s">
+      <c r="H793" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I790" s="20" t="s">
+      <c r="I793" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J790" s="11" t="s">
+      <c r="J793" s="11" t="s">
         <v>690</v>
       </c>
-      <c r="K790" s="11" t="s">
+      <c r="K793" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="L790" s="11" t="s">
+      <c r="L793" s="11" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="791" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A791" s="21" t="s">
-        <v>847</v>
-      </c>
-      <c r="B791" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C791" s="25"/>
-      <c r="D791" s="22"/>
-      <c r="E791" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F791" s="25"/>
-      <c r="G791" s="23" t="s">
-        <v>848</v>
-      </c>
-      <c r="H791" s="23"/>
-      <c r="I791" s="23"/>
-      <c r="J791" s="22"/>
-      <c r="K791" s="22"/>
-      <c r="L791" s="22"/>
-    </row>
-    <row r="792" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B792" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C792" s="25"/>
-      <c r="D792" s="22"/>
-      <c r="E792" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F792" s="25"/>
-      <c r="G792" s="23" t="s">
+    <row r="794" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A794" s="21" t="s">
         <v>849</v>
       </c>
-      <c r="H792" s="23"/>
-      <c r="I792" s="23"/>
-      <c r="J792" s="22"/>
-      <c r="K792" s="22"/>
-      <c r="L792" s="22"/>
-    </row>
-    <row r="793" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B793" s="25"/>
-      <c r="C793" s="25"/>
-      <c r="D793" s="22"/>
-      <c r="E793" s="22"/>
-      <c r="F793" s="25"/>
-      <c r="G793" s="23" t="s">
-        <v>850</v>
-      </c>
-      <c r="H793" s="23"/>
-      <c r="I793" s="23"/>
-      <c r="J793" s="22"/>
-      <c r="K793" s="22"/>
-      <c r="L793" s="22"/>
-    </row>
-    <row r="794" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B794" s="25"/>
+      <c r="B794" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C794" s="25"/>
       <c r="D794" s="22"/>
-      <c r="E794" s="22"/>
+      <c r="E794" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F794" s="25"/>
       <c r="G794" s="23" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H794" s="23"/>
       <c r="I794" s="23"/>
@@ -18369,13 +18391,17 @@
       <c r="L794" s="22"/>
     </row>
     <row r="795" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B795" s="25"/>
+      <c r="B795" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C795" s="25"/>
       <c r="D795" s="22"/>
-      <c r="E795" s="22"/>
+      <c r="E795" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F795" s="25"/>
       <c r="G795" s="23" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="H795" s="23"/>
       <c r="I795" s="23"/>
@@ -18384,13 +18410,17 @@
       <c r="L795" s="22"/>
     </row>
     <row r="796" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B796" s="25"/>
+      <c r="B796" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C796" s="25"/>
       <c r="D796" s="22"/>
-      <c r="E796" s="22"/>
+      <c r="E796" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F796" s="25"/>
       <c r="G796" s="23" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="H796" s="23"/>
       <c r="I796" s="23"/>
@@ -18399,13 +18429,17 @@
       <c r="L796" s="22"/>
     </row>
     <row r="797" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B797" s="25"/>
+      <c r="B797" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C797" s="25"/>
       <c r="D797" s="22"/>
-      <c r="E797" s="22"/>
+      <c r="E797" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F797" s="25"/>
       <c r="G797" s="23" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H797" s="23"/>
       <c r="I797" s="23"/>
@@ -18420,7 +18454,7 @@
       <c r="E798" s="22"/>
       <c r="F798" s="25"/>
       <c r="G798" s="23" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H798" s="23"/>
       <c r="I798" s="23"/>
@@ -18435,7 +18469,7 @@
       <c r="E799" s="22"/>
       <c r="F799" s="25"/>
       <c r="G799" s="23" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="H799" s="23"/>
       <c r="I799" s="23"/>
@@ -18450,7 +18484,7 @@
       <c r="E800" s="22"/>
       <c r="F800" s="25"/>
       <c r="G800" s="23" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="H800" s="23"/>
       <c r="I800" s="23"/>
@@ -18458,192 +18492,170 @@
       <c r="K800" s="22"/>
       <c r="L800" s="22"/>
     </row>
-    <row r="801" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B801" s="22"/>
-      <c r="C801" s="22"/>
+    <row r="801" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B801" s="25"/>
+      <c r="C801" s="25"/>
       <c r="D801" s="22"/>
       <c r="E801" s="22"/>
-      <c r="F801" s="22"/>
-      <c r="G801" s="23"/>
+      <c r="F801" s="25"/>
+      <c r="G801" s="23" t="s">
+        <v>857</v>
+      </c>
       <c r="H801" s="23"/>
       <c r="I801" s="23"/>
       <c r="J801" s="22"/>
       <c r="K801" s="22"/>
       <c r="L801" s="22"/>
     </row>
-    <row r="802" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B802" s="1"/>
-      <c r="C802" s="1"/>
-      <c r="D802" s="1"/>
-      <c r="E802" s="1"/>
-      <c r="F802" s="1"/>
-      <c r="G802" s="1"/>
-      <c r="H802" s="1"/>
-      <c r="I802" s="1"/>
-      <c r="J802" s="1"/>
-      <c r="K802" s="1"/>
-      <c r="L802" s="1"/>
-      <c r="M802" s="1"/>
-      <c r="N802" s="1"/>
-      <c r="O802" s="1"/>
-    </row>
-    <row r="803" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A803" s="9"/>
+    <row r="802" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B802" s="25"/>
+      <c r="C802" s="25"/>
+      <c r="D802" s="22"/>
+      <c r="E802" s="22"/>
+      <c r="F802" s="25"/>
+      <c r="G802" s="23" t="s">
+        <v>858</v>
+      </c>
+      <c r="H802" s="23"/>
+      <c r="I802" s="23"/>
+      <c r="J802" s="22"/>
+      <c r="K802" s="22"/>
+      <c r="L802" s="22"/>
+    </row>
+    <row r="803" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B803" s="25"/>
+      <c r="C803" s="25"/>
+      <c r="D803" s="22"/>
+      <c r="E803" s="22"/>
+      <c r="F803" s="25"/>
+      <c r="G803" s="23" t="s">
+        <v>859</v>
+      </c>
+      <c r="H803" s="23"/>
+      <c r="I803" s="23"/>
+      <c r="J803" s="22"/>
+      <c r="K803" s="22"/>
+      <c r="L803" s="22"/>
     </row>
     <row r="804" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A804" s="16" t="s">
+      <c r="B804" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C804" s="25"/>
+      <c r="D804" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E804" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F804" s="25"/>
+      <c r="G804" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="H804" s="23"/>
+      <c r="I804" s="23"/>
+      <c r="J804" s="22"/>
+      <c r="K804" s="22"/>
+      <c r="L804" s="22"/>
+    </row>
+    <row r="805" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B805" s="22"/>
+      <c r="C805" s="22"/>
+      <c r="D805" s="22"/>
+      <c r="E805" s="22"/>
+      <c r="F805" s="22"/>
+      <c r="G805" s="23"/>
+      <c r="H805" s="23"/>
+      <c r="I805" s="23"/>
+      <c r="J805" s="22"/>
+      <c r="K805" s="22"/>
+      <c r="L805" s="22"/>
+    </row>
+    <row r="806" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B806" s="1"/>
+      <c r="C806" s="1"/>
+      <c r="D806" s="1"/>
+      <c r="E806" s="1"/>
+      <c r="F806" s="1"/>
+      <c r="G806" s="1"/>
+      <c r="H806" s="1"/>
+      <c r="I806" s="1"/>
+      <c r="J806" s="1"/>
+      <c r="K806" s="1"/>
+      <c r="L806" s="1"/>
+      <c r="M806" s="1"/>
+      <c r="N806" s="1"/>
+      <c r="O806" s="1"/>
+    </row>
+    <row r="807" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A807" s="9"/>
+    </row>
+    <row r="808" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A808" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B804" s="17"/>
-      <c r="C804" s="18"/>
-      <c r="D804" s="18"/>
-      <c r="E804" s="18"/>
-      <c r="F804" s="18"/>
-    </row>
-    <row r="805" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A805" s="16" t="s">
-        <v>858</v>
-      </c>
-      <c r="B805" s="17"/>
-      <c r="C805" s="18"/>
-      <c r="D805" s="18"/>
-      <c r="E805" s="18"/>
-      <c r="F805" s="18"/>
-    </row>
-    <row r="806" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A806" s="16" t="s">
+      <c r="B808" s="17"/>
+      <c r="C808" s="18"/>
+      <c r="D808" s="18"/>
+      <c r="E808" s="18"/>
+      <c r="F808" s="18"/>
+    </row>
+    <row r="809" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A809" s="16" t="s">
+        <v>861</v>
+      </c>
+      <c r="B809" s="17"/>
+      <c r="C809" s="18"/>
+      <c r="D809" s="18"/>
+      <c r="E809" s="18"/>
+      <c r="F809" s="18"/>
+    </row>
+    <row r="810" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A810" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B806" s="17"/>
-      <c r="C806" s="18"/>
-      <c r="D806" s="18"/>
-      <c r="E806" s="18"/>
-      <c r="F806" s="18"/>
-    </row>
-    <row r="807" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A807" s="9"/>
-      <c r="B807" s="11" t="s">
+      <c r="B810" s="17"/>
+      <c r="C810" s="18"/>
+      <c r="D810" s="18"/>
+      <c r="E810" s="18"/>
+      <c r="F810" s="18"/>
+    </row>
+    <row r="811" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A811" s="9"/>
+      <c r="B811" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C807" s="11" t="s">
+      <c r="C811" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D807" s="11" t="s">
+      <c r="D811" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E807" s="11" t="s">
+      <c r="E811" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F807" s="11" t="s">
+      <c r="F811" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G807" s="20" t="s">
+      <c r="G811" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H807" s="20" t="s">
+      <c r="H811" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I807" s="20" t="s">
+      <c r="I811" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="808" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A808" s="21" t="s">
-        <v>859</v>
-      </c>
-      <c r="B808" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C808" s="25"/>
-      <c r="D808" s="22"/>
-      <c r="E808" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F808" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G808" s="23" t="s">
-        <v>860</v>
-      </c>
-      <c r="H808" s="23"/>
-      <c r="I808" s="23"/>
-    </row>
-    <row r="809" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A809" s="21"/>
-      <c r="B809" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C809" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D809" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E809" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F809" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G809" s="23" t="s">
-        <v>861</v>
-      </c>
-      <c r="H809" s="23"/>
-      <c r="I809" s="23"/>
-    </row>
-    <row r="810" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A810" s="9"/>
-      <c r="B810" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C810" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D810" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E810" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F810" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G810" s="23" t="s">
+    <row r="812" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A812" s="21" t="s">
         <v>862</v>
       </c>
-      <c r="H810" s="23"/>
-      <c r="I810" s="23"/>
-    </row>
-    <row r="811" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A811" s="9"/>
-      <c r="B811" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C811" s="25"/>
-      <c r="D811" s="22"/>
-      <c r="E811" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F811" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G811" s="45" t="s">
-        <v>863</v>
-      </c>
-      <c r="H811" s="23"/>
-      <c r="I811" s="23"/>
-    </row>
-    <row r="812" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A812" s="9"/>
       <c r="B812" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C812" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D812" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C812" s="25"/>
+      <c r="D812" s="22"/>
       <c r="E812" s="22" t="s">
         <v>22</v>
       </c>
@@ -18651,18 +18663,22 @@
         <v>640</v>
       </c>
       <c r="G812" s="23" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H812" s="23"/>
       <c r="I812" s="23"/>
     </row>
     <row r="813" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A813" s="9"/>
+      <c r="A813" s="21"/>
       <c r="B813" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C813" s="25"/>
-      <c r="D813" s="22"/>
+      <c r="C813" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D813" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E813" s="22" t="s">
         <v>22</v>
       </c>
@@ -18670,7 +18686,7 @@
         <v>640</v>
       </c>
       <c r="G813" s="23" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H813" s="23"/>
       <c r="I813" s="23"/>
@@ -18680,8 +18696,12 @@
       <c r="B814" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C814" s="25"/>
-      <c r="D814" s="22"/>
+      <c r="C814" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D814" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E814" s="22" t="s">
         <v>22</v>
       </c>
@@ -18689,12 +18709,12 @@
         <v>640</v>
       </c>
       <c r="G814" s="23" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="H814" s="23"/>
       <c r="I814" s="23"/>
     </row>
-    <row r="815" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="815" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A815" s="9"/>
       <c r="B815" s="22" t="s">
         <v>22</v>
@@ -18707,21 +18727,23 @@
       <c r="F815" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="G815" s="23" t="s">
-        <v>867</v>
+      <c r="G815" s="45" t="s">
+        <v>866</v>
       </c>
       <c r="H815" s="23"/>
-      <c r="I815" s="23" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="816" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I815" s="23"/>
+    </row>
+    <row r="816" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A816" s="9"/>
       <c r="B816" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C816" s="25"/>
-      <c r="D816" s="22"/>
+      <c r="C816" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D816" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E816" s="22" t="s">
         <v>22</v>
       </c>
@@ -18729,7 +18751,7 @@
         <v>640</v>
       </c>
       <c r="G816" s="23" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H816" s="23"/>
       <c r="I816" s="23"/>
@@ -18739,9 +18761,7 @@
       <c r="B817" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C817" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C817" s="25"/>
       <c r="D817" s="22"/>
       <c r="E817" s="22" t="s">
         <v>22</v>
@@ -18750,12 +18770,12 @@
         <v>640</v>
       </c>
       <c r="G817" s="23" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="H817" s="23"/>
       <c r="I817" s="23"/>
     </row>
-    <row r="818" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="818" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A818" s="9"/>
       <c r="B818" s="22" t="s">
         <v>22</v>
@@ -18769,7 +18789,7 @@
         <v>640</v>
       </c>
       <c r="G818" s="23" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="H818" s="23"/>
       <c r="I818" s="23"/>
@@ -18788,10 +18808,12 @@
         <v>640</v>
       </c>
       <c r="G819" s="23" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="H819" s="23"/>
-      <c r="I819" s="23"/>
+      <c r="I819" s="23" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="820" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A820" s="9"/>
@@ -18807,17 +18829,19 @@
         <v>640</v>
       </c>
       <c r="G820" s="23" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="H820" s="23"/>
       <c r="I820" s="23"/>
     </row>
-    <row r="821" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="821" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A821" s="9"/>
       <c r="B821" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C821" s="25"/>
+      <c r="C821" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D821" s="22"/>
       <c r="E821" s="22" t="s">
         <v>22</v>
@@ -18826,7 +18850,7 @@
         <v>640</v>
       </c>
       <c r="G821" s="23" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H821" s="23"/>
       <c r="I821" s="23"/>
@@ -18837,9 +18861,7 @@
         <v>22</v>
       </c>
       <c r="C822" s="25"/>
-      <c r="D822" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D822" s="22"/>
       <c r="E822" s="22" t="s">
         <v>22</v>
       </c>
@@ -18847,22 +18869,18 @@
         <v>640</v>
       </c>
       <c r="G822" s="23" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H822" s="23"/>
       <c r="I822" s="23"/>
     </row>
-    <row r="823" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="823" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A823" s="9"/>
       <c r="B823" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C823" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D823" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C823" s="25"/>
+      <c r="D823" s="22"/>
       <c r="E823" s="22" t="s">
         <v>22</v>
       </c>
@@ -18870,22 +18888,18 @@
         <v>640</v>
       </c>
       <c r="G823" s="23" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="H823" s="23"/>
       <c r="I823" s="23"/>
     </row>
-    <row r="824" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="824" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A824" s="9"/>
       <c r="B824" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C824" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D824" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C824" s="25"/>
+      <c r="D824" s="22"/>
       <c r="E824" s="22" t="s">
         <v>22</v>
       </c>
@@ -18893,22 +18907,18 @@
         <v>640</v>
       </c>
       <c r="G824" s="23" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H824" s="23"/>
       <c r="I824" s="23"/>
     </row>
-    <row r="825" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="825" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A825" s="9"/>
       <c r="B825" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C825" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D825" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C825" s="25"/>
+      <c r="D825" s="22"/>
       <c r="E825" s="22" t="s">
         <v>22</v>
       </c>
@@ -18916,18 +18926,20 @@
         <v>640</v>
       </c>
       <c r="G825" s="23" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="H825" s="23"/>
       <c r="I825" s="23"/>
     </row>
-    <row r="826" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="826" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A826" s="9"/>
       <c r="B826" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C826" s="25"/>
-      <c r="D826" s="22"/>
+      <c r="D826" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E826" s="22" t="s">
         <v>22</v>
       </c>
@@ -18935,7 +18947,7 @@
         <v>640</v>
       </c>
       <c r="G826" s="23" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H826" s="23"/>
       <c r="I826" s="23"/>
@@ -18958,7 +18970,7 @@
         <v>640</v>
       </c>
       <c r="G827" s="23" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H827" s="23"/>
       <c r="I827" s="23"/>
@@ -18981,7 +18993,7 @@
         <v>640</v>
       </c>
       <c r="G828" s="23" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H828" s="23"/>
       <c r="I828" s="23"/>
@@ -18991,7 +19003,9 @@
       <c r="B829" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C829" s="25"/>
+      <c r="C829" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D829" s="22" t="s">
         <v>22</v>
       </c>
@@ -19002,7 +19016,7 @@
         <v>640</v>
       </c>
       <c r="G829" s="23" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="H829" s="23"/>
       <c r="I829" s="23"/>
@@ -19013,9 +19027,7 @@
         <v>22</v>
       </c>
       <c r="C830" s="25"/>
-      <c r="D830" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D830" s="22"/>
       <c r="E830" s="22" t="s">
         <v>22</v>
       </c>
@@ -19023,18 +19035,22 @@
         <v>640</v>
       </c>
       <c r="G830" s="23" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H830" s="23"/>
       <c r="I830" s="23"/>
     </row>
-    <row r="831" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="831" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A831" s="9"/>
       <c r="B831" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C831" s="25"/>
-      <c r="D831" s="22"/>
+      <c r="C831" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D831" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E831" s="22" t="s">
         <v>22</v>
       </c>
@@ -19042,7 +19058,7 @@
         <v>640</v>
       </c>
       <c r="G831" s="23" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H831" s="23"/>
       <c r="I831" s="23"/>
@@ -19052,7 +19068,9 @@
       <c r="B832" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C832" s="25"/>
+      <c r="C832" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D832" s="22" t="s">
         <v>22</v>
       </c>
@@ -19063,7 +19081,7 @@
         <v>640</v>
       </c>
       <c r="G832" s="23" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="H832" s="23"/>
       <c r="I832" s="23"/>
@@ -19084,7 +19102,7 @@
         <v>640</v>
       </c>
       <c r="G833" s="23" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="H833" s="23"/>
       <c r="I833" s="23"/>
@@ -19105,22 +19123,18 @@
         <v>640</v>
       </c>
       <c r="G834" s="23" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="H834" s="23"/>
       <c r="I834" s="23"/>
     </row>
-    <row r="835" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="835" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A835" s="9"/>
       <c r="B835" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C835" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D835" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C835" s="25"/>
+      <c r="D835" s="22"/>
       <c r="E835" s="22" t="s">
         <v>22</v>
       </c>
@@ -19128,7 +19142,7 @@
         <v>640</v>
       </c>
       <c r="G835" s="23" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="H835" s="23"/>
       <c r="I835" s="23"/>
@@ -19138,9 +19152,7 @@
       <c r="B836" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C836" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C836" s="25"/>
       <c r="D836" s="22" t="s">
         <v>22</v>
       </c>
@@ -19151,7 +19163,7 @@
         <v>640</v>
       </c>
       <c r="G836" s="23" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="H836" s="23"/>
       <c r="I836" s="23"/>
@@ -19162,7 +19174,9 @@
         <v>22</v>
       </c>
       <c r="C837" s="25"/>
-      <c r="D837" s="22"/>
+      <c r="D837" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E837" s="22" t="s">
         <v>22</v>
       </c>
@@ -19170,7 +19184,7 @@
         <v>640</v>
       </c>
       <c r="G837" s="23" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="H837" s="23"/>
       <c r="I837" s="23"/>
@@ -19180,9 +19194,7 @@
       <c r="B838" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C838" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C838" s="25"/>
       <c r="D838" s="22" t="s">
         <v>22</v>
       </c>
@@ -19193,7 +19205,7 @@
         <v>640</v>
       </c>
       <c r="G838" s="23" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="H838" s="23"/>
       <c r="I838" s="23"/>
@@ -19216,7 +19228,7 @@
         <v>640</v>
       </c>
       <c r="G839" s="23" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="H839" s="23"/>
       <c r="I839" s="23"/>
@@ -19239,7 +19251,7 @@
         <v>640</v>
       </c>
       <c r="G840" s="23" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H840" s="23"/>
       <c r="I840" s="23"/>
@@ -19258,7 +19270,7 @@
         <v>640</v>
       </c>
       <c r="G841" s="23" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H841" s="23"/>
       <c r="I841" s="23"/>
@@ -19281,7 +19293,7 @@
         <v>640</v>
       </c>
       <c r="G842" s="23" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H842" s="23"/>
       <c r="I842" s="23"/>
@@ -19304,7 +19316,7 @@
         <v>640</v>
       </c>
       <c r="G843" s="23" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="H843" s="23"/>
       <c r="I843" s="23"/>
@@ -19327,7 +19339,7 @@
         <v>640</v>
       </c>
       <c r="G844" s="23" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="H844" s="23"/>
       <c r="I844" s="23"/>
@@ -19337,12 +19349,8 @@
       <c r="B845" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C845" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D845" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C845" s="25"/>
+      <c r="D845" s="22"/>
       <c r="E845" s="22" t="s">
         <v>22</v>
       </c>
@@ -19350,7 +19358,7 @@
         <v>640</v>
       </c>
       <c r="G845" s="23" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H845" s="23"/>
       <c r="I845" s="23"/>
@@ -19373,7 +19381,7 @@
         <v>640</v>
       </c>
       <c r="G846" s="23" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="H846" s="23"/>
       <c r="I846" s="23"/>
@@ -19383,8 +19391,12 @@
       <c r="B847" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C847" s="25"/>
-      <c r="D847" s="22"/>
+      <c r="C847" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D847" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E847" s="22" t="s">
         <v>22</v>
       </c>
@@ -19392,7 +19404,7 @@
         <v>640</v>
       </c>
       <c r="G847" s="23" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="H847" s="23"/>
       <c r="I847" s="23"/>
@@ -19415,7 +19427,7 @@
         <v>640</v>
       </c>
       <c r="G848" s="23" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="H848" s="23"/>
       <c r="I848" s="23"/>
@@ -19438,7 +19450,7 @@
         <v>640</v>
       </c>
       <c r="G849" s="23" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="H849" s="23"/>
       <c r="I849" s="23"/>
@@ -19461,7 +19473,7 @@
         <v>640</v>
       </c>
       <c r="G850" s="23" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="H850" s="23"/>
       <c r="I850" s="23"/>
@@ -19471,12 +19483,8 @@
       <c r="B851" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C851" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D851" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C851" s="25"/>
+      <c r="D851" s="22"/>
       <c r="E851" s="22" t="s">
         <v>22</v>
       </c>
@@ -19484,31 +19492,33 @@
         <v>640</v>
       </c>
       <c r="G851" s="23" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="H851" s="23"/>
       <c r="I851" s="23"/>
     </row>
-    <row r="852" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="852" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A852" s="9"/>
-      <c r="B852" s="25" t="s">
-        <v>611</v>
-      </c>
-      <c r="C852" s="25"/>
+      <c r="B852" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C852" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D852" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E852" s="25"/>
+      <c r="E852" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F852" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G852" s="23" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="H852" s="23"/>
-      <c r="I852" s="23" t="s">
-        <v>613</v>
-      </c>
+      <c r="I852" s="23"/>
     </row>
     <row r="853" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A853" s="9"/>
@@ -19528,7 +19538,7 @@
         <v>640</v>
       </c>
       <c r="G853" s="23" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H853" s="23"/>
       <c r="I853" s="23"/>
@@ -19551,7 +19561,7 @@
         <v>640</v>
       </c>
       <c r="G854" s="23" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="H854" s="23"/>
       <c r="I854" s="23"/>
@@ -19574,33 +19584,31 @@
         <v>640</v>
       </c>
       <c r="G855" s="23" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="H855" s="23"/>
       <c r="I855" s="23"/>
     </row>
-    <row r="856" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="856" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A856" s="9"/>
-      <c r="B856" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C856" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B856" s="25" t="s">
+        <v>611</v>
+      </c>
+      <c r="C856" s="25"/>
       <c r="D856" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E856" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E856" s="25"/>
       <c r="F856" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G856" s="23" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="H856" s="23"/>
-      <c r="I856" s="23"/>
+      <c r="I856" s="23" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="857" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A857" s="9"/>
@@ -19620,7 +19628,7 @@
         <v>640</v>
       </c>
       <c r="G857" s="23" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="H857" s="23"/>
       <c r="I857" s="23"/>
@@ -19643,7 +19651,7 @@
         <v>640</v>
       </c>
       <c r="G858" s="23" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="H858" s="23"/>
       <c r="I858" s="23"/>
@@ -19666,7 +19674,7 @@
         <v>640</v>
       </c>
       <c r="G859" s="23" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H859" s="23"/>
       <c r="I859" s="23"/>
@@ -19676,8 +19684,12 @@
       <c r="B860" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C860" s="25"/>
-      <c r="D860" s="22"/>
+      <c r="C860" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D860" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E860" s="22" t="s">
         <v>22</v>
       </c>
@@ -19685,17 +19697,22 @@
         <v>640</v>
       </c>
       <c r="G860" s="23" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="H860" s="23"/>
       <c r="I860" s="23"/>
     </row>
     <row r="861" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A861" s="9"/>
       <c r="B861" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C861" s="25"/>
-      <c r="D861" s="22"/>
+      <c r="C861" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D861" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E861" s="22" t="s">
         <v>22</v>
       </c>
@@ -19703,17 +19720,22 @@
         <v>640</v>
       </c>
       <c r="G861" s="23" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="H861" s="23"/>
       <c r="I861" s="23"/>
     </row>
     <row r="862" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A862" s="9"/>
       <c r="B862" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C862" s="25"/>
-      <c r="D862" s="22"/>
+      <c r="C862" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D862" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E862" s="22" t="s">
         <v>22</v>
       </c>
@@ -19721,12 +19743,13 @@
         <v>640</v>
       </c>
       <c r="G862" s="23" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H862" s="23"/>
       <c r="I862" s="23"/>
     </row>
     <row r="863" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A863" s="9"/>
       <c r="B863" s="22" t="s">
         <v>22</v>
       </c>
@@ -19743,21 +19766,18 @@
         <v>640</v>
       </c>
       <c r="G863" s="23" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H863" s="23"/>
       <c r="I863" s="23"/>
     </row>
     <row r="864" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A864" s="9"/>
       <c r="B864" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C864" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D864" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C864" s="25"/>
+      <c r="D864" s="22"/>
       <c r="E864" s="22" t="s">
         <v>22</v>
       </c>
@@ -19765,7 +19785,7 @@
         <v>640</v>
       </c>
       <c r="G864" s="23" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H864" s="23"/>
       <c r="I864" s="23"/>
@@ -19774,20 +19794,16 @@
       <c r="B865" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C865" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D865" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C865" s="25"/>
+      <c r="D865" s="22"/>
       <c r="E865" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F865" s="22" t="s">
-        <v>917</v>
+        <v>640</v>
       </c>
       <c r="G865" s="23" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="H865" s="23"/>
       <c r="I865" s="23"/>
@@ -19797,48 +19813,48 @@
         <v>22</v>
       </c>
       <c r="C866" s="25"/>
-      <c r="D866" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D866" s="22"/>
       <c r="E866" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F866" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G866" s="23" t="s">
         <v>917</v>
       </c>
-      <c r="G866" s="23" t="s">
-        <v>919</v>
-      </c>
       <c r="H866" s="23"/>
-      <c r="I866" s="23" t="s">
-        <v>920</v>
-      </c>
+      <c r="I866" s="23"/>
     </row>
     <row r="867" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B867" s="27" t="s">
+      <c r="B867" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C867" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D867" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E867" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F867" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="C867" s="27"/>
-      <c r="D867" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="E867" s="27"/>
-      <c r="F867" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="G867" s="28" t="s">
-        <v>921</v>
-      </c>
-      <c r="H867" s="28"/>
-      <c r="I867" s="28" t="s">
-        <v>922</v>
-      </c>
+      <c r="G867" s="23" t="s">
+        <v>918</v>
+      </c>
+      <c r="H867" s="23"/>
+      <c r="I867" s="23"/>
     </row>
     <row r="868" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B868" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C868" s="25"/>
+      <c r="C868" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D868" s="22" t="s">
         <v>22</v>
       </c>
@@ -19846,40 +19862,120 @@
         <v>22</v>
       </c>
       <c r="F868" s="22" t="s">
-        <v>917</v>
+        <v>640</v>
       </c>
       <c r="G868" s="23" t="s">
+        <v>919</v>
+      </c>
+      <c r="H868" s="23"/>
+      <c r="I868" s="23"/>
+    </row>
+    <row r="869" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B869" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C869" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D869" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E869" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F869" s="22" t="s">
+        <v>920</v>
+      </c>
+      <c r="G869" s="23" t="s">
+        <v>921</v>
+      </c>
+      <c r="H869" s="23"/>
+      <c r="I869" s="23"/>
+    </row>
+    <row r="870" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B870" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C870" s="25"/>
+      <c r="D870" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E870" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F870" s="22" t="s">
+        <v>920</v>
+      </c>
+      <c r="G870" s="23" t="s">
+        <v>922</v>
+      </c>
+      <c r="H870" s="23"/>
+      <c r="I870" s="23" t="s">
         <v>923</v>
       </c>
-      <c r="H868" s="23"/>
-      <c r="I868" s="23" t="s">
+    </row>
+    <row r="871" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B871" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="C871" s="27"/>
+      <c r="D871" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="E871" s="27"/>
+      <c r="F871" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="G871" s="28" t="s">
+        <v>924</v>
+      </c>
+      <c r="H871" s="28"/>
+      <c r="I871" s="28" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="872" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B872" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C872" s="25"/>
+      <c r="D872" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E872" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F872" s="22" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="869" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B869" s="27" t="s">
+      <c r="G872" s="23" t="s">
+        <v>926</v>
+      </c>
+      <c r="H872" s="23"/>
+      <c r="I872" s="23" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="873" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B873" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="C869" s="27"/>
-      <c r="D869" s="27" t="s">
+      <c r="C873" s="27"/>
+      <c r="D873" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="E869" s="27"/>
-      <c r="F869" s="27" t="s">
+      <c r="E873" s="27"/>
+      <c r="F873" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="G869" s="28" t="s">
-        <v>924</v>
-      </c>
-      <c r="H869" s="28"/>
-      <c r="I869" s="28" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G873" s="28" t="s">
+        <v>927</v>
+      </c>
+      <c r="H873" s="28"/>
+      <c r="I873" s="28" t="s">
+        <v>925</v>
+      </c>
+    </row>
     <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Fixed state space discAB issue.  Added additional routines and menus
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3743" uniqueCount="959">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -2479,6 +2479,54 @@
     <t xml:space="preserve">BatterySim_CalculateLoadedVoltage.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">ELEVATOR SIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_New.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_GetCurrentDraw.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_GetPositionMeters.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_GetVelocityMetersPerSecond.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_SetInputVoltage.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_UpdateX.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_WouldHitLowerLimit.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_WouldHitUpperLimit.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_Update.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Needed because this doesn’t extend.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_HasHitLowerLimit.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_HasHitUpperLimit.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_New_NoNoise.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_New_LinSys.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElevatorSim_New_LinSys_NoNoise.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLYWHEEL SIM</t>
   </si>
   <si>
@@ -2533,6 +2581,9 @@
     <t xml:space="preserve">LinearSystemSim_UpdateX.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">LinearSystemSim_UpdateY.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">LinearSystemSim_New_NoNoise.vi</t>
   </si>
   <si>
@@ -2548,6 +2599,9 @@
     <t xml:space="preserve">LinearSystemSim_GetCurrentDrawAmps.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">DONT IMPLEMENT…</t>
+  </si>
+  <si>
     <t xml:space="preserve">LinearSystemSim_ClampInput.vi</t>
   </si>
   <si>
@@ -2608,6 +2662,42 @@
     <t xml:space="preserve">VecBuilder_ArrayBy1Fill.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">MATH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUMERICAL INTEGRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Func_Ax_Bu_K.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Func_Bs.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Func_Ch.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Func_Ct.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Rk4_Dbl.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Rk4_K_Dbl.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Rkf45_Ax_Bu_K.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Rkf45Impl_Ax_Bu_K.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Trap_Dbl.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Trap_Mat.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">TYPE DEFINITIONS</t>
   </si>
   <si>
@@ -2627,6 +2717,9 @@
   </si>
   <si>
     <t xml:space="preserve">DIFF_DRIVE_KINEMATICS.CTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELEVATOR_SIM.CTL</t>
   </si>
   <si>
     <t xml:space="preserve">ELEV_FF.CTL</t>
@@ -3265,8 +3358,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A776" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B786" activeCellId="0" sqref="B786"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A768" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G779" activeCellId="0" sqref="G779"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3357,28 +3450,28 @@
         <v>11</v>
       </c>
       <c r="B9" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1200,"X")</f>
-        <v>544</v>
+        <f aca="false">COUNTIF(B18:B1244,"X")</f>
+        <v>566</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C18:C1200,"X")</f>
+        <f aca="false">COUNTIF(C18:C1244,"X")</f>
         <v>368</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D18:D1200,"X")</f>
-        <v>166</v>
+        <f aca="false">COUNTIF(D18:D1244,"X")</f>
+        <v>168</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E18:E1200,"X")</f>
-        <v>511</v>
+        <f aca="false">COUNTIF(E18:E1244,"X")</f>
+        <v>524</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F18:F1200,"S")+COUNTIF(F18:F1200,"I")+COUNTIF(F18:F1200,"X")+COUNTIF(F18:F1200,"SI")+COUNTIF(F18:F1200,"IS")+COUNTIF(F18:F1200,"N/A")</f>
-        <v>211</v>
+        <f aca="false">COUNTIF(F18:F1244,"S")+COUNTIF(F18:F1244,"I")+COUNTIF(F18:F1244,"X")+COUNTIF(F18:F1244,"SI")+COUNTIF(F18:F1244,"IS")+COUNTIF(F18:F1244,"N/A")</f>
+        <v>212</v>
       </c>
       <c r="G9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.676470588235294</v>
+        <v>0.65017667844523</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3386,8 +3479,8 @@
         <v>12</v>
       </c>
       <c r="B10" s="13" t="n">
-        <f aca="false">COUNTIF(B19:B1201,"/")</f>
-        <v>8</v>
+        <f aca="false">COUNTIF(B19:B1245,"/")</f>
+        <v>10</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>13</v>
@@ -3396,7 +3489,7 @@
     <row r="11" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.387867647058823</v>
+        <v>0.374558303886926</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15785,7 +15878,7 @@
       <c r="L662" s="22"/>
     </row>
     <row r="663" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B663" s="25" t="s">
+      <c r="B663" s="27" t="s">
         <v>611</v>
       </c>
       <c r="C663" s="25"/>
@@ -17564,7 +17657,6 @@
       <c r="O753" s="1"/>
     </row>
     <row r="754" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A754" s="21"/>
       <c r="B754" s="22" t="s">
         <v>22</v>
       </c>
@@ -17587,7 +17679,6 @@
       <c r="O754" s="1"/>
     </row>
     <row r="755" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A755" s="21"/>
       <c r="B755" s="22" t="s">
         <v>22</v>
       </c>
@@ -17610,7 +17701,6 @@
       <c r="O755" s="1"/>
     </row>
     <row r="756" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A756" s="21"/>
       <c r="B756" s="22" t="s">
         <v>22</v>
       </c>
@@ -17633,7 +17723,6 @@
       <c r="O756" s="1"/>
     </row>
     <row r="757" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A757" s="21"/>
       <c r="B757" s="22" t="s">
         <v>22</v>
       </c>
@@ -17656,19 +17745,20 @@
       <c r="O757" s="1"/>
     </row>
     <row r="758" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A758" s="21"/>
-      <c r="B758" s="25"/>
+      <c r="B758" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C758" s="25"/>
       <c r="D758" s="22"/>
-      <c r="E758" s="22"/>
+      <c r="E758" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F758" s="25"/>
       <c r="G758" s="23" t="s">
         <v>825</v>
       </c>
       <c r="H758" s="23"/>
-      <c r="I758" s="23" t="s">
-        <v>103</v>
-      </c>
+      <c r="I758" s="23"/>
       <c r="J758" s="22"/>
       <c r="K758" s="22"/>
       <c r="L758" s="22"/>
@@ -17677,19 +17767,20 @@
       <c r="O758" s="1"/>
     </row>
     <row r="759" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A759" s="21"/>
-      <c r="B759" s="25"/>
+      <c r="B759" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C759" s="25"/>
       <c r="D759" s="22"/>
-      <c r="E759" s="22"/>
+      <c r="E759" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F759" s="25"/>
       <c r="G759" s="23" t="s">
         <v>826</v>
       </c>
       <c r="H759" s="23"/>
-      <c r="I759" s="23" t="s">
-        <v>103</v>
-      </c>
+      <c r="I759" s="23"/>
       <c r="J759" s="22"/>
       <c r="K759" s="22"/>
       <c r="L759" s="22"/>
@@ -17697,19 +17788,24 @@
       <c r="N759" s="1"/>
       <c r="O759" s="1"/>
     </row>
-    <row r="760" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A760" s="21"/>
-      <c r="B760" s="25"/>
+    <row r="760" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B760" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C760" s="25"/>
-      <c r="D760" s="22"/>
-      <c r="E760" s="22"/>
+      <c r="D760" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E760" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F760" s="25"/>
       <c r="G760" s="23" t="s">
         <v>827</v>
       </c>
       <c r="H760" s="23"/>
       <c r="I760" s="23" t="s">
-        <v>103</v>
+        <v>828</v>
       </c>
       <c r="J760" s="22"/>
       <c r="K760" s="22"/>
@@ -17718,14 +17814,19 @@
       <c r="N760" s="1"/>
       <c r="O760" s="1"/>
     </row>
-    <row r="761" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A761" s="21"/>
-      <c r="B761" s="22"/>
-      <c r="C761" s="22"/>
+    <row r="761" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B761" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C761" s="25"/>
       <c r="D761" s="22"/>
-      <c r="E761" s="22"/>
-      <c r="F761" s="22"/>
-      <c r="G761" s="23"/>
+      <c r="E761" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F761" s="25"/>
+      <c r="G761" s="23" t="s">
+        <v>829</v>
+      </c>
       <c r="H761" s="23"/>
       <c r="I761" s="23"/>
       <c r="J761" s="22"/>
@@ -17735,76 +17836,54 @@
       <c r="N761" s="1"/>
       <c r="O761" s="1"/>
     </row>
-    <row r="762" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B762" s="46"/>
-      <c r="C762" s="1"/>
-      <c r="D762" s="1"/>
-      <c r="E762" s="1"/>
-      <c r="F762" s="1"/>
-      <c r="G762" s="1"/>
-      <c r="H762" s="1"/>
-      <c r="I762" s="1"/>
-      <c r="J762" s="1"/>
-      <c r="K762" s="1"/>
-      <c r="L762" s="1"/>
+    <row r="762" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B762" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C762" s="25"/>
+      <c r="D762" s="22"/>
+      <c r="E762" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F762" s="25"/>
+      <c r="G762" s="23" t="s">
+        <v>830</v>
+      </c>
+      <c r="H762" s="23"/>
+      <c r="I762" s="23"/>
+      <c r="J762" s="22"/>
+      <c r="K762" s="22"/>
+      <c r="L762" s="22"/>
       <c r="M762" s="1"/>
       <c r="N762" s="1"/>
       <c r="O762" s="1"/>
     </row>
-    <row r="763" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A763" s="19"/>
-      <c r="B763" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C763" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D763" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E763" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F763" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G763" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H763" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I763" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J763" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="K763" s="11" t="s">
-        <v>691</v>
-      </c>
-      <c r="L763" s="11" t="s">
-        <v>692</v>
-      </c>
+    <row r="763" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B763" s="25"/>
+      <c r="C763" s="25"/>
+      <c r="D763" s="22"/>
+      <c r="E763" s="25"/>
+      <c r="F763" s="25"/>
+      <c r="G763" s="23" t="s">
+        <v>831</v>
+      </c>
+      <c r="H763" s="23"/>
+      <c r="I763" s="23"/>
+      <c r="J763" s="22"/>
+      <c r="K763" s="22"/>
+      <c r="L763" s="22"/>
       <c r="M763" s="1"/>
       <c r="N763" s="1"/>
       <c r="O763" s="1"/>
     </row>
     <row r="764" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A764" s="21" t="s">
-        <v>828</v>
-      </c>
-      <c r="B764" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B764" s="25"/>
       <c r="C764" s="25"/>
       <c r="D764" s="22"/>
-      <c r="E764" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E764" s="25"/>
       <c r="F764" s="25"/>
       <c r="G764" s="23" t="s">
-        <v>829</v>
+        <v>832</v>
       </c>
       <c r="H764" s="23"/>
       <c r="I764" s="23"/>
@@ -17816,18 +17895,13 @@
       <c r="O764" s="1"/>
     </row>
     <row r="765" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A765" s="21"/>
-      <c r="B765" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B765" s="25"/>
       <c r="C765" s="25"/>
       <c r="D765" s="22"/>
-      <c r="E765" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E765" s="25"/>
       <c r="F765" s="25"/>
       <c r="G765" s="23" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="H765" s="23"/>
       <c r="I765" s="23"/>
@@ -17838,56 +17912,65 @@
       <c r="N765" s="1"/>
       <c r="O765" s="1"/>
     </row>
-    <row r="766" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A766" s="21"/>
-      <c r="B766" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C766" s="25"/>
-      <c r="D766" s="22"/>
-      <c r="E766" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F766" s="25"/>
-      <c r="G766" s="23" t="s">
-        <v>831</v>
-      </c>
-      <c r="H766" s="23"/>
-      <c r="I766" s="23"/>
-      <c r="J766" s="22"/>
-      <c r="K766" s="22"/>
-      <c r="L766" s="22"/>
+    <row r="766" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B766" s="46"/>
+      <c r="C766" s="1"/>
+      <c r="D766" s="1"/>
+      <c r="E766" s="1"/>
+      <c r="F766" s="1"/>
+      <c r="G766" s="1"/>
+      <c r="H766" s="1"/>
+      <c r="I766" s="1"/>
+      <c r="J766" s="1"/>
+      <c r="K766" s="1"/>
+      <c r="L766" s="1"/>
       <c r="M766" s="1"/>
       <c r="N766" s="1"/>
       <c r="O766" s="1"/>
     </row>
-    <row r="767" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A767" s="21"/>
-      <c r="B767" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C767" s="25"/>
-      <c r="D767" s="22"/>
-      <c r="E767" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F767" s="25"/>
-      <c r="G767" s="23" t="s">
-        <v>832</v>
-      </c>
-      <c r="H767" s="23"/>
-      <c r="I767" s="23" t="s">
-        <v>833</v>
-      </c>
-      <c r="J767" s="22"/>
-      <c r="K767" s="22"/>
-      <c r="L767" s="22"/>
+    <row r="767" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A767" s="19"/>
+      <c r="B767" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C767" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D767" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E767" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F767" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G767" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H767" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I767" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J767" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K767" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L767" s="11" t="s">
+        <v>692</v>
+      </c>
       <c r="M767" s="1"/>
       <c r="N767" s="1"/>
       <c r="O767" s="1"/>
     </row>
     <row r="768" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A768" s="21"/>
+      <c r="A768" s="21" t="s">
+        <v>834</v>
+      </c>
       <c r="B768" s="22" t="s">
         <v>22</v>
       </c>
@@ -17898,7 +17981,7 @@
       </c>
       <c r="F768" s="25"/>
       <c r="G768" s="23" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="H768" s="23"/>
       <c r="I768" s="23"/>
@@ -17916,10 +17999,12 @@
       </c>
       <c r="C769" s="25"/>
       <c r="D769" s="22"/>
-      <c r="E769" s="22"/>
+      <c r="E769" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F769" s="25"/>
       <c r="G769" s="23" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="H769" s="23"/>
       <c r="I769" s="23"/>
@@ -17932,13 +18017,17 @@
     </row>
     <row r="770" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A770" s="21"/>
-      <c r="B770" s="25"/>
+      <c r="B770" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C770" s="25"/>
       <c r="D770" s="22"/>
-      <c r="E770" s="22"/>
+      <c r="E770" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F770" s="25"/>
       <c r="G770" s="23" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="H770" s="23"/>
       <c r="I770" s="23"/>
@@ -17951,13 +18040,17 @@
     </row>
     <row r="771" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A771" s="21"/>
-      <c r="B771" s="25"/>
+      <c r="B771" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C771" s="25"/>
       <c r="D771" s="22"/>
-      <c r="E771" s="22"/>
+      <c r="E771" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F771" s="25"/>
       <c r="G771" s="23" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="H771" s="23"/>
       <c r="I771" s="23"/>
@@ -17970,13 +18063,17 @@
     </row>
     <row r="772" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A772" s="21"/>
-      <c r="B772" s="25"/>
+      <c r="B772" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C772" s="25"/>
       <c r="D772" s="22"/>
-      <c r="E772" s="22"/>
+      <c r="E772" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F772" s="25"/>
       <c r="G772" s="23" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="H772" s="23"/>
       <c r="I772" s="23"/>
@@ -17989,13 +18086,17 @@
     </row>
     <row r="773" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A773" s="21"/>
-      <c r="B773" s="25"/>
+      <c r="B773" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C773" s="25"/>
       <c r="D773" s="22"/>
-      <c r="E773" s="22"/>
+      <c r="E773" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F773" s="25"/>
       <c r="G773" s="23" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="H773" s="23"/>
       <c r="I773" s="23"/>
@@ -18014,10 +18115,12 @@
       <c r="E774" s="22"/>
       <c r="F774" s="25"/>
       <c r="G774" s="23" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="H774" s="23"/>
-      <c r="I774" s="23"/>
+      <c r="I774" s="23" t="s">
+        <v>103</v>
+      </c>
       <c r="J774" s="22"/>
       <c r="K774" s="22"/>
       <c r="L774" s="22"/>
@@ -18027,16 +18130,18 @@
     </row>
     <row r="775" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A775" s="21"/>
-      <c r="B775" s="48"/>
+      <c r="B775" s="25"/>
       <c r="C775" s="25"/>
       <c r="D775" s="22"/>
       <c r="E775" s="22"/>
       <c r="F775" s="25"/>
       <c r="G775" s="23" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="H775" s="23"/>
-      <c r="I775" s="23"/>
+      <c r="I775" s="23" t="s">
+        <v>103</v>
+      </c>
       <c r="J775" s="22"/>
       <c r="K775" s="22"/>
       <c r="L775" s="22"/>
@@ -18044,16 +18149,20 @@
       <c r="N775" s="1"/>
       <c r="O775" s="1"/>
     </row>
-    <row r="776" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="776" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A776" s="21"/>
-      <c r="B776" s="22"/>
-      <c r="C776" s="22"/>
+      <c r="B776" s="25"/>
+      <c r="C776" s="25"/>
       <c r="D776" s="22"/>
       <c r="E776" s="22"/>
-      <c r="F776" s="22"/>
-      <c r="G776" s="23"/>
+      <c r="F776" s="25"/>
+      <c r="G776" s="23" t="s">
+        <v>843</v>
+      </c>
       <c r="H776" s="23"/>
-      <c r="I776" s="23"/>
+      <c r="I776" s="23" t="s">
+        <v>103</v>
+      </c>
       <c r="J776" s="22"/>
       <c r="K776" s="22"/>
       <c r="L776" s="22"/>
@@ -18062,444 +18171,496 @@
       <c r="O776" s="1"/>
     </row>
     <row r="777" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A777" s="19"/>
-      <c r="B777" s="19"/>
-      <c r="C777" s="19"/>
-      <c r="D777" s="19"/>
-      <c r="E777" s="19"/>
-      <c r="F777" s="19"/>
-      <c r="G777" s="1"/>
-      <c r="H777" s="1"/>
-      <c r="I777" s="1"/>
-      <c r="J777" s="1"/>
-      <c r="K777" s="1"/>
-      <c r="L777" s="1"/>
+      <c r="A777" s="21"/>
+      <c r="B777" s="22"/>
+      <c r="C777" s="22"/>
+      <c r="D777" s="22"/>
+      <c r="E777" s="22"/>
+      <c r="F777" s="22"/>
+      <c r="G777" s="23"/>
+      <c r="H777" s="23"/>
+      <c r="I777" s="23"/>
+      <c r="J777" s="22"/>
+      <c r="K777" s="22"/>
+      <c r="L777" s="22"/>
       <c r="M777" s="1"/>
       <c r="N777" s="1"/>
       <c r="O777" s="1"/>
     </row>
     <row r="778" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A778" s="19"/>
-      <c r="B778" s="44"/>
-      <c r="C778" s="4"/>
-      <c r="D778" s="4"/>
-      <c r="E778" s="4"/>
-      <c r="F778" s="4"/>
-    </row>
-    <row r="779" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A779" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B779" s="43"/>
-      <c r="C779" s="18"/>
-      <c r="D779" s="18"/>
-      <c r="E779" s="18"/>
-      <c r="F779" s="18"/>
-    </row>
-    <row r="780" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A780" s="16" t="s">
-        <v>842</v>
-      </c>
-      <c r="B780" s="43"/>
-      <c r="C780" s="18"/>
-      <c r="D780" s="18"/>
-      <c r="E780" s="18"/>
-      <c r="F780" s="18"/>
+      <c r="B778" s="46"/>
+      <c r="C778" s="1"/>
+      <c r="D778" s="1"/>
+      <c r="E778" s="1"/>
+      <c r="F778" s="1"/>
+      <c r="G778" s="1"/>
+      <c r="H778" s="1"/>
+      <c r="I778" s="1"/>
+      <c r="J778" s="1"/>
+      <c r="K778" s="1"/>
+      <c r="L778" s="1"/>
+      <c r="M778" s="1"/>
+      <c r="N778" s="1"/>
+      <c r="O778" s="1"/>
+    </row>
+    <row r="779" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A779" s="19"/>
+      <c r="B779" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C779" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D779" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E779" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F779" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G779" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H779" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I779" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J779" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K779" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L779" s="11" t="s">
+        <v>692</v>
+      </c>
+      <c r="M779" s="1"/>
+      <c r="N779" s="1"/>
+      <c r="O779" s="1"/>
+    </row>
+    <row r="780" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A780" s="21" t="s">
+        <v>844</v>
+      </c>
+      <c r="B780" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C780" s="25"/>
+      <c r="D780" s="22"/>
+      <c r="E780" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F780" s="25"/>
+      <c r="G780" s="23" t="s">
+        <v>845</v>
+      </c>
+      <c r="H780" s="23"/>
+      <c r="I780" s="23"/>
+      <c r="J780" s="22"/>
+      <c r="K780" s="22"/>
+      <c r="L780" s="22"/>
+      <c r="M780" s="1"/>
+      <c r="N780" s="1"/>
+      <c r="O780" s="1"/>
     </row>
     <row r="781" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A781" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B781" s="43"/>
-      <c r="C781" s="18"/>
-      <c r="D781" s="18"/>
-      <c r="E781" s="18"/>
-      <c r="F781" s="18"/>
-      <c r="H781" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="782" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A782" s="19"/>
-      <c r="B782" s="19"/>
-      <c r="C782" s="19"/>
-      <c r="D782" s="19"/>
-      <c r="E782" s="19"/>
-      <c r="F782" s="19"/>
-    </row>
-    <row r="783" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A783" s="19"/>
-      <c r="B783" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C783" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D783" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E783" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F783" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G783" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H783" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I783" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J783" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="K783" s="11" t="s">
-        <v>691</v>
-      </c>
-      <c r="L783" s="11" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="784" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A784" s="21" t="s">
-        <v>843</v>
-      </c>
+      <c r="A781" s="21"/>
+      <c r="B781" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C781" s="25"/>
+      <c r="D781" s="22"/>
+      <c r="E781" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F781" s="25"/>
+      <c r="G781" s="23" t="s">
+        <v>846</v>
+      </c>
+      <c r="H781" s="23"/>
+      <c r="I781" s="23"/>
+      <c r="J781" s="22"/>
+      <c r="K781" s="22"/>
+      <c r="L781" s="22"/>
+      <c r="M781" s="1"/>
+      <c r="N781" s="1"/>
+      <c r="O781" s="1"/>
+    </row>
+    <row r="782" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A782" s="21"/>
+      <c r="B782" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C782" s="25"/>
+      <c r="D782" s="22"/>
+      <c r="E782" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F782" s="25"/>
+      <c r="G782" s="23" t="s">
+        <v>847</v>
+      </c>
+      <c r="H782" s="23"/>
+      <c r="I782" s="23"/>
+      <c r="J782" s="22"/>
+      <c r="K782" s="22"/>
+      <c r="L782" s="22"/>
+      <c r="M782" s="1"/>
+      <c r="N782" s="1"/>
+      <c r="O782" s="1"/>
+    </row>
+    <row r="783" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A783" s="21"/>
+      <c r="B783" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C783" s="25"/>
+      <c r="D783" s="22"/>
+      <c r="E783" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F783" s="25"/>
+      <c r="G783" s="23" t="s">
+        <v>848</v>
+      </c>
+      <c r="H783" s="23"/>
+      <c r="I783" s="23" t="s">
+        <v>849</v>
+      </c>
+      <c r="J783" s="22"/>
+      <c r="K783" s="22"/>
+      <c r="L783" s="22"/>
+      <c r="M783" s="1"/>
+      <c r="N783" s="1"/>
+      <c r="O783" s="1"/>
+    </row>
+    <row r="784" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A784" s="21"/>
       <c r="B784" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C784" s="25"/>
       <c r="D784" s="22"/>
-      <c r="E784" s="25"/>
+      <c r="E784" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F784" s="25"/>
       <c r="G784" s="23" t="s">
-        <v>844</v>
+        <v>850</v>
       </c>
       <c r="H784" s="23"/>
       <c r="I784" s="23"/>
       <c r="J784" s="22"/>
       <c r="K784" s="22"/>
       <c r="L784" s="22"/>
-    </row>
-    <row r="785" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M784" s="1"/>
+      <c r="N784" s="1"/>
+      <c r="O784" s="1"/>
+    </row>
+    <row r="785" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A785" s="21"/>
       <c r="B785" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C785" s="25"/>
       <c r="D785" s="22"/>
-      <c r="E785" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E785" s="22"/>
       <c r="F785" s="25"/>
       <c r="G785" s="23" t="s">
-        <v>845</v>
+        <v>851</v>
       </c>
       <c r="H785" s="23"/>
       <c r="I785" s="23"/>
       <c r="J785" s="22"/>
       <c r="K785" s="22"/>
       <c r="L785" s="22"/>
+      <c r="M785" s="1"/>
+      <c r="N785" s="1"/>
+      <c r="O785" s="1"/>
     </row>
     <row r="786" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A786" s="19"/>
-      <c r="B786" s="44"/>
-      <c r="C786" s="4"/>
-      <c r="D786" s="4"/>
-      <c r="E786" s="4"/>
-      <c r="F786" s="4"/>
-    </row>
-    <row r="787" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B787" s="46"/>
-      <c r="C787" s="1"/>
-      <c r="D787" s="1"/>
-      <c r="E787" s="1"/>
-      <c r="F787" s="1"/>
-      <c r="G787" s="1"/>
-      <c r="H787" s="1"/>
-      <c r="I787" s="1"/>
-      <c r="J787" s="1"/>
-      <c r="K787" s="1"/>
-      <c r="L787" s="1"/>
-    </row>
-    <row r="788" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A788" s="19"/>
-      <c r="B788" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C788" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D788" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E788" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F788" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G788" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H788" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I788" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J788" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="K788" s="11" t="s">
-        <v>691</v>
-      </c>
-      <c r="L788" s="11" t="s">
-        <v>692</v>
-      </c>
+      <c r="A786" s="21"/>
+      <c r="B786" s="27" t="s">
+        <v>611</v>
+      </c>
+      <c r="C786" s="25"/>
+      <c r="D786" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E786" s="22"/>
+      <c r="F786" s="25"/>
+      <c r="G786" s="23" t="s">
+        <v>852</v>
+      </c>
+      <c r="H786" s="23"/>
+      <c r="I786" s="23"/>
+      <c r="J786" s="22"/>
+      <c r="K786" s="22"/>
+      <c r="L786" s="22"/>
+      <c r="M786" s="1"/>
+      <c r="N786" s="1"/>
+      <c r="O786" s="1"/>
+    </row>
+    <row r="787" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A787" s="21"/>
+      <c r="B787" s="25"/>
+      <c r="C787" s="25"/>
+      <c r="D787" s="22"/>
+      <c r="E787" s="22"/>
+      <c r="F787" s="25"/>
+      <c r="G787" s="23" t="s">
+        <v>853</v>
+      </c>
+      <c r="H787" s="23"/>
+      <c r="I787" s="23"/>
+      <c r="J787" s="22"/>
+      <c r="K787" s="22"/>
+      <c r="L787" s="22"/>
+      <c r="M787" s="1"/>
+      <c r="N787" s="1"/>
+      <c r="O787" s="1"/>
+    </row>
+    <row r="788" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A788" s="21"/>
+      <c r="B788" s="27" t="s">
+        <v>611</v>
+      </c>
+      <c r="C788" s="25"/>
+      <c r="D788" s="22"/>
+      <c r="E788" s="25"/>
+      <c r="F788" s="25"/>
+      <c r="G788" s="23" t="s">
+        <v>854</v>
+      </c>
+      <c r="H788" s="23"/>
+      <c r="I788" s="23"/>
+      <c r="J788" s="22"/>
+      <c r="K788" s="22"/>
+      <c r="L788" s="22"/>
+      <c r="M788" s="1"/>
+      <c r="N788" s="1"/>
+      <c r="O788" s="1"/>
     </row>
     <row r="789" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A789" s="21" t="s">
-        <v>846</v>
-      </c>
+      <c r="A789" s="21"/>
       <c r="B789" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C789" s="25"/>
-      <c r="D789" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E789" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D789" s="22"/>
+      <c r="E789" s="22"/>
       <c r="F789" s="25"/>
       <c r="G789" s="23" t="s">
-        <v>847</v>
+        <v>855</v>
       </c>
       <c r="H789" s="23"/>
       <c r="I789" s="23"/>
       <c r="J789" s="22"/>
       <c r="K789" s="22"/>
       <c r="L789" s="22"/>
+      <c r="M789" s="1"/>
+      <c r="N789" s="1"/>
+      <c r="O789" s="1"/>
     </row>
     <row r="790" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A790" s="21"/>
       <c r="B790" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C790" s="25"/>
-      <c r="D790" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E790" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D790" s="22"/>
+      <c r="E790" s="25"/>
       <c r="F790" s="25"/>
       <c r="G790" s="23" t="s">
-        <v>848</v>
+        <v>856</v>
       </c>
       <c r="H790" s="23"/>
       <c r="I790" s="23"/>
       <c r="J790" s="22"/>
       <c r="K790" s="22"/>
       <c r="L790" s="22"/>
+      <c r="M790" s="1"/>
+      <c r="N790" s="1"/>
+      <c r="O790" s="1"/>
     </row>
     <row r="791" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B791" s="1"/>
-      <c r="C791" s="1"/>
-      <c r="D791" s="1"/>
-      <c r="E791" s="1"/>
-      <c r="F791" s="1"/>
-      <c r="G791" s="1"/>
-      <c r="H791" s="1"/>
-      <c r="I791" s="1"/>
-      <c r="J791" s="1"/>
-      <c r="K791" s="1"/>
-      <c r="L791" s="1"/>
+      <c r="A791" s="21"/>
+      <c r="B791" s="25"/>
+      <c r="C791" s="25"/>
+      <c r="D791" s="22"/>
+      <c r="E791" s="22"/>
+      <c r="F791" s="25"/>
+      <c r="G791" s="23" t="s">
+        <v>857</v>
+      </c>
+      <c r="H791" s="23"/>
+      <c r="I791" s="23" t="s">
+        <v>858</v>
+      </c>
+      <c r="J791" s="22"/>
+      <c r="K791" s="22"/>
+      <c r="L791" s="22"/>
       <c r="M791" s="1"/>
       <c r="N791" s="1"/>
-    </row>
-    <row r="792" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B792" s="46"/>
-      <c r="C792" s="1"/>
-      <c r="D792" s="1"/>
-      <c r="E792" s="1"/>
-      <c r="F792" s="1"/>
-      <c r="G792" s="1"/>
-      <c r="H792" s="1"/>
-      <c r="I792" s="1"/>
-      <c r="J792" s="1"/>
-      <c r="K792" s="1"/>
-      <c r="L792" s="1"/>
-    </row>
-    <row r="793" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A793" s="19"/>
-      <c r="B793" s="11" t="s">
+      <c r="O791" s="1"/>
+    </row>
+    <row r="792" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A792" s="21"/>
+      <c r="B792" s="48"/>
+      <c r="C792" s="25"/>
+      <c r="D792" s="22"/>
+      <c r="E792" s="22"/>
+      <c r="F792" s="25"/>
+      <c r="G792" s="23" t="s">
+        <v>859</v>
+      </c>
+      <c r="H792" s="23"/>
+      <c r="I792" s="23"/>
+      <c r="J792" s="22"/>
+      <c r="K792" s="22"/>
+      <c r="L792" s="22"/>
+      <c r="M792" s="1"/>
+      <c r="N792" s="1"/>
+      <c r="O792" s="1"/>
+    </row>
+    <row r="793" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A793" s="21"/>
+      <c r="B793" s="22"/>
+      <c r="C793" s="22"/>
+      <c r="D793" s="22"/>
+      <c r="E793" s="22"/>
+      <c r="F793" s="22"/>
+      <c r="G793" s="23"/>
+      <c r="H793" s="23"/>
+      <c r="I793" s="23"/>
+      <c r="J793" s="22"/>
+      <c r="K793" s="22"/>
+      <c r="L793" s="22"/>
+      <c r="M793" s="1"/>
+      <c r="N793" s="1"/>
+      <c r="O793" s="1"/>
+    </row>
+    <row r="794" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A794" s="19"/>
+      <c r="B794" s="19"/>
+      <c r="C794" s="19"/>
+      <c r="D794" s="19"/>
+      <c r="E794" s="19"/>
+      <c r="F794" s="19"/>
+      <c r="G794" s="1"/>
+      <c r="H794" s="1"/>
+      <c r="I794" s="1"/>
+      <c r="J794" s="1"/>
+      <c r="K794" s="1"/>
+      <c r="L794" s="1"/>
+      <c r="M794" s="1"/>
+      <c r="N794" s="1"/>
+      <c r="O794" s="1"/>
+    </row>
+    <row r="795" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A795" s="19"/>
+      <c r="B795" s="44"/>
+      <c r="C795" s="4"/>
+      <c r="D795" s="4"/>
+      <c r="E795" s="4"/>
+      <c r="F795" s="4"/>
+    </row>
+    <row r="796" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A796" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B796" s="43"/>
+      <c r="C796" s="18"/>
+      <c r="D796" s="18"/>
+      <c r="E796" s="18"/>
+      <c r="F796" s="18"/>
+    </row>
+    <row r="797" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A797" s="16" t="s">
+        <v>860</v>
+      </c>
+      <c r="B797" s="43"/>
+      <c r="C797" s="18"/>
+      <c r="D797" s="18"/>
+      <c r="E797" s="18"/>
+      <c r="F797" s="18"/>
+    </row>
+    <row r="798" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A798" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B798" s="43"/>
+      <c r="C798" s="18"/>
+      <c r="D798" s="18"/>
+      <c r="E798" s="18"/>
+      <c r="F798" s="18"/>
+      <c r="H798" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="799" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A799" s="19"/>
+      <c r="B799" s="19"/>
+      <c r="C799" s="19"/>
+      <c r="D799" s="19"/>
+      <c r="E799" s="19"/>
+      <c r="F799" s="19"/>
+    </row>
+    <row r="800" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A800" s="19"/>
+      <c r="B800" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C793" s="11" t="s">
+      <c r="C800" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D793" s="11" t="s">
+      <c r="D800" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E793" s="11" t="s">
+      <c r="E800" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F793" s="11" t="s">
+      <c r="F800" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G793" s="20" t="s">
+      <c r="G800" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H793" s="20" t="s">
+      <c r="H800" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I793" s="20" t="s">
+      <c r="I800" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J793" s="11" t="s">
+      <c r="J800" s="11" t="s">
         <v>690</v>
       </c>
-      <c r="K793" s="11" t="s">
+      <c r="K800" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="L793" s="11" t="s">
+      <c r="L800" s="11" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="794" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A794" s="21" t="s">
-        <v>849</v>
-      </c>
-      <c r="B794" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C794" s="25"/>
-      <c r="D794" s="22"/>
-      <c r="E794" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F794" s="25"/>
-      <c r="G794" s="23" t="s">
-        <v>850</v>
-      </c>
-      <c r="H794" s="23"/>
-      <c r="I794" s="23"/>
-      <c r="J794" s="22"/>
-      <c r="K794" s="22"/>
-      <c r="L794" s="22"/>
-    </row>
-    <row r="795" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B795" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C795" s="25"/>
-      <c r="D795" s="22"/>
-      <c r="E795" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F795" s="25"/>
-      <c r="G795" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="H795" s="23"/>
-      <c r="I795" s="23"/>
-      <c r="J795" s="22"/>
-      <c r="K795" s="22"/>
-      <c r="L795" s="22"/>
-    </row>
-    <row r="796" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B796" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C796" s="25"/>
-      <c r="D796" s="22"/>
-      <c r="E796" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F796" s="25"/>
-      <c r="G796" s="23" t="s">
-        <v>852</v>
-      </c>
-      <c r="H796" s="23"/>
-      <c r="I796" s="23"/>
-      <c r="J796" s="22"/>
-      <c r="K796" s="22"/>
-      <c r="L796" s="22"/>
-    </row>
-    <row r="797" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B797" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C797" s="25"/>
-      <c r="D797" s="22"/>
-      <c r="E797" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F797" s="25"/>
-      <c r="G797" s="23" t="s">
-        <v>853</v>
-      </c>
-      <c r="H797" s="23"/>
-      <c r="I797" s="23"/>
-      <c r="J797" s="22"/>
-      <c r="K797" s="22"/>
-      <c r="L797" s="22"/>
-    </row>
-    <row r="798" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B798" s="25"/>
-      <c r="C798" s="25"/>
-      <c r="D798" s="22"/>
-      <c r="E798" s="22"/>
-      <c r="F798" s="25"/>
-      <c r="G798" s="23" t="s">
-        <v>854</v>
-      </c>
-      <c r="H798" s="23"/>
-      <c r="I798" s="23"/>
-      <c r="J798" s="22"/>
-      <c r="K798" s="22"/>
-      <c r="L798" s="22"/>
-    </row>
-    <row r="799" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B799" s="25"/>
-      <c r="C799" s="25"/>
-      <c r="D799" s="22"/>
-      <c r="E799" s="22"/>
-      <c r="F799" s="25"/>
-      <c r="G799" s="23" t="s">
-        <v>855</v>
-      </c>
-      <c r="H799" s="23"/>
-      <c r="I799" s="23"/>
-      <c r="J799" s="22"/>
-      <c r="K799" s="22"/>
-      <c r="L799" s="22"/>
-    </row>
-    <row r="800" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B800" s="25"/>
-      <c r="C800" s="25"/>
-      <c r="D800" s="22"/>
-      <c r="E800" s="22"/>
-      <c r="F800" s="25"/>
-      <c r="G800" s="23" t="s">
-        <v>856</v>
-      </c>
-      <c r="H800" s="23"/>
-      <c r="I800" s="23"/>
-      <c r="J800" s="22"/>
-      <c r="K800" s="22"/>
-      <c r="L800" s="22"/>
-    </row>
     <row r="801" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B801" s="25"/>
+      <c r="A801" s="21" t="s">
+        <v>861</v>
+      </c>
+      <c r="B801" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C801" s="25"/>
       <c r="D801" s="22"/>
-      <c r="E801" s="22"/>
+      <c r="E801" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F801" s="25"/>
       <c r="G801" s="23" t="s">
-        <v>857</v>
+        <v>862</v>
       </c>
       <c r="H801" s="23"/>
       <c r="I801" s="23"/>
@@ -18507,14 +18668,18 @@
       <c r="K801" s="22"/>
       <c r="L801" s="22"/>
     </row>
-    <row r="802" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B802" s="25"/>
+    <row r="802" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B802" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C802" s="25"/>
       <c r="D802" s="22"/>
-      <c r="E802" s="22"/>
+      <c r="E802" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F802" s="25"/>
       <c r="G802" s="23" t="s">
-        <v>858</v>
+        <v>863</v>
       </c>
       <c r="H802" s="23"/>
       <c r="I802" s="23"/>
@@ -18522,135 +18687,195 @@
       <c r="K802" s="22"/>
       <c r="L802" s="22"/>
     </row>
-    <row r="803" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B803" s="25"/>
-      <c r="C803" s="25"/>
-      <c r="D803" s="22"/>
-      <c r="E803" s="22"/>
-      <c r="F803" s="25"/>
-      <c r="G803" s="23" t="s">
-        <v>859</v>
-      </c>
-      <c r="H803" s="23"/>
-      <c r="I803" s="23"/>
-      <c r="J803" s="22"/>
-      <c r="K803" s="22"/>
-      <c r="L803" s="22"/>
+    <row r="803" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A803" s="19"/>
+      <c r="B803" s="44"/>
+      <c r="C803" s="4"/>
+      <c r="D803" s="4"/>
+      <c r="E803" s="4"/>
+      <c r="F803" s="4"/>
     </row>
     <row r="804" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B804" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C804" s="25"/>
-      <c r="D804" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E804" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F804" s="25"/>
-      <c r="G804" s="23" t="s">
-        <v>860</v>
-      </c>
-      <c r="H804" s="23"/>
-      <c r="I804" s="23"/>
-      <c r="J804" s="22"/>
-      <c r="K804" s="22"/>
-      <c r="L804" s="22"/>
-    </row>
-    <row r="805" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B805" s="22"/>
-      <c r="C805" s="22"/>
-      <c r="D805" s="22"/>
-      <c r="E805" s="22"/>
-      <c r="F805" s="22"/>
-      <c r="G805" s="23"/>
-      <c r="H805" s="23"/>
-      <c r="I805" s="23"/>
-      <c r="J805" s="22"/>
-      <c r="K805" s="22"/>
-      <c r="L805" s="22"/>
-    </row>
-    <row r="806" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B806" s="1"/>
-      <c r="C806" s="1"/>
-      <c r="D806" s="1"/>
-      <c r="E806" s="1"/>
-      <c r="F806" s="1"/>
-      <c r="G806" s="1"/>
-      <c r="H806" s="1"/>
-      <c r="I806" s="1"/>
-      <c r="J806" s="1"/>
-      <c r="K806" s="1"/>
-      <c r="L806" s="1"/>
-      <c r="M806" s="1"/>
-      <c r="N806" s="1"/>
-      <c r="O806" s="1"/>
-    </row>
-    <row r="807" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A807" s="9"/>
+      <c r="B804" s="46"/>
+      <c r="C804" s="1"/>
+      <c r="D804" s="1"/>
+      <c r="E804" s="1"/>
+      <c r="F804" s="1"/>
+      <c r="G804" s="1"/>
+      <c r="H804" s="1"/>
+      <c r="I804" s="1"/>
+      <c r="J804" s="1"/>
+      <c r="K804" s="1"/>
+      <c r="L804" s="1"/>
+    </row>
+    <row r="805" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A805" s="19"/>
+      <c r="B805" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C805" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D805" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E805" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F805" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G805" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H805" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I805" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J805" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K805" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L805" s="11" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="806" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A806" s="21" t="s">
+        <v>864</v>
+      </c>
+      <c r="B806" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C806" s="25"/>
+      <c r="D806" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E806" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F806" s="25"/>
+      <c r="G806" s="23" t="s">
+        <v>865</v>
+      </c>
+      <c r="H806" s="23"/>
+      <c r="I806" s="23"/>
+      <c r="J806" s="22"/>
+      <c r="K806" s="22"/>
+      <c r="L806" s="22"/>
+    </row>
+    <row r="807" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B807" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C807" s="25"/>
+      <c r="D807" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E807" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F807" s="25"/>
+      <c r="G807" s="23" t="s">
+        <v>866</v>
+      </c>
+      <c r="H807" s="23"/>
+      <c r="I807" s="23"/>
+      <c r="J807" s="22"/>
+      <c r="K807" s="22"/>
+      <c r="L807" s="22"/>
     </row>
     <row r="808" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A808" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B808" s="17"/>
-      <c r="C808" s="18"/>
-      <c r="D808" s="18"/>
-      <c r="E808" s="18"/>
-      <c r="F808" s="18"/>
+      <c r="B808" s="1"/>
+      <c r="C808" s="1"/>
+      <c r="D808" s="1"/>
+      <c r="E808" s="1"/>
+      <c r="F808" s="1"/>
+      <c r="G808" s="1"/>
+      <c r="H808" s="1"/>
+      <c r="I808" s="1"/>
+      <c r="J808" s="1"/>
+      <c r="K808" s="1"/>
+      <c r="L808" s="1"/>
+      <c r="M808" s="1"/>
+      <c r="N808" s="1"/>
     </row>
     <row r="809" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A809" s="16" t="s">
-        <v>861</v>
-      </c>
-      <c r="B809" s="17"/>
-      <c r="C809" s="18"/>
-      <c r="D809" s="18"/>
-      <c r="E809" s="18"/>
-      <c r="F809" s="18"/>
-    </row>
-    <row r="810" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A810" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B810" s="17"/>
-      <c r="C810" s="18"/>
-      <c r="D810" s="18"/>
-      <c r="E810" s="18"/>
-      <c r="F810" s="18"/>
-    </row>
-    <row r="811" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A811" s="9"/>
-      <c r="B811" s="11" t="s">
+      <c r="B809" s="46"/>
+      <c r="C809" s="1"/>
+      <c r="D809" s="1"/>
+      <c r="E809" s="1"/>
+      <c r="F809" s="1"/>
+      <c r="G809" s="1"/>
+      <c r="H809" s="1"/>
+      <c r="I809" s="1"/>
+      <c r="J809" s="1"/>
+      <c r="K809" s="1"/>
+      <c r="L809" s="1"/>
+    </row>
+    <row r="810" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A810" s="19"/>
+      <c r="B810" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C811" s="11" t="s">
+      <c r="C810" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D811" s="11" t="s">
+      <c r="D810" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E811" s="11" t="s">
+      <c r="E810" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F811" s="11" t="s">
+      <c r="F810" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G811" s="20" t="s">
+      <c r="G810" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H811" s="20" t="s">
+      <c r="H810" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I811" s="20" t="s">
+      <c r="I810" s="20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="812" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A812" s="21" t="s">
-        <v>862</v>
-      </c>
+      <c r="J810" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K810" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L810" s="11" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="811" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A811" s="21" t="s">
+        <v>867</v>
+      </c>
+      <c r="B811" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C811" s="25"/>
+      <c r="D811" s="22"/>
+      <c r="E811" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F811" s="25"/>
+      <c r="G811" s="23" t="s">
+        <v>868</v>
+      </c>
+      <c r="H811" s="23"/>
+      <c r="I811" s="23"/>
+      <c r="J811" s="22"/>
+      <c r="K811" s="22"/>
+      <c r="L811" s="22"/>
+    </row>
+    <row r="812" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B812" s="22" t="s">
         <v>22</v>
       </c>
@@ -18659,924 +18884,694 @@
       <c r="E812" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F812" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="F812" s="25"/>
       <c r="G812" s="23" t="s">
-        <v>863</v>
+        <v>869</v>
       </c>
       <c r="H812" s="23"/>
       <c r="I812" s="23"/>
-    </row>
-    <row r="813" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A813" s="21"/>
+      <c r="J812" s="22"/>
+      <c r="K812" s="22"/>
+      <c r="L812" s="22"/>
+    </row>
+    <row r="813" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B813" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C813" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D813" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C813" s="25"/>
+      <c r="D813" s="22"/>
       <c r="E813" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F813" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="F813" s="25"/>
       <c r="G813" s="23" t="s">
-        <v>864</v>
+        <v>870</v>
       </c>
       <c r="H813" s="23"/>
       <c r="I813" s="23"/>
-    </row>
-    <row r="814" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A814" s="9"/>
+      <c r="J813" s="22"/>
+      <c r="K813" s="22"/>
+      <c r="L813" s="22"/>
+    </row>
+    <row r="814" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B814" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C814" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D814" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C814" s="25"/>
+      <c r="D814" s="22"/>
       <c r="E814" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F814" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="F814" s="25"/>
       <c r="G814" s="23" t="s">
-        <v>865</v>
+        <v>871</v>
       </c>
       <c r="H814" s="23"/>
       <c r="I814" s="23"/>
-    </row>
-    <row r="815" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A815" s="9"/>
-      <c r="B815" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="J814" s="22"/>
+      <c r="K814" s="22"/>
+      <c r="L814" s="22"/>
+    </row>
+    <row r="815" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B815" s="25"/>
       <c r="C815" s="25"/>
       <c r="D815" s="22"/>
-      <c r="E815" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F815" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G815" s="45" t="s">
-        <v>866</v>
+      <c r="E815" s="22"/>
+      <c r="F815" s="25"/>
+      <c r="G815" s="23" t="s">
+        <v>872</v>
       </c>
       <c r="H815" s="23"/>
       <c r="I815" s="23"/>
-    </row>
-    <row r="816" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A816" s="9"/>
-      <c r="B816" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C816" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D816" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E816" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F816" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="J815" s="22"/>
+      <c r="K815" s="22"/>
+      <c r="L815" s="22"/>
+    </row>
+    <row r="816" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B816" s="25"/>
+      <c r="C816" s="25"/>
+      <c r="D816" s="22"/>
+      <c r="E816" s="22"/>
+      <c r="F816" s="25"/>
       <c r="G816" s="23" t="s">
-        <v>867</v>
+        <v>873</v>
       </c>
       <c r="H816" s="23"/>
       <c r="I816" s="23"/>
-    </row>
-    <row r="817" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A817" s="9"/>
-      <c r="B817" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="J816" s="22"/>
+      <c r="K816" s="22"/>
+      <c r="L816" s="22"/>
+    </row>
+    <row r="817" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B817" s="25"/>
       <c r="C817" s="25"/>
       <c r="D817" s="22"/>
-      <c r="E817" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F817" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="E817" s="22"/>
+      <c r="F817" s="25"/>
       <c r="G817" s="23" t="s">
-        <v>868</v>
+        <v>874</v>
       </c>
       <c r="H817" s="23"/>
       <c r="I817" s="23"/>
-    </row>
-    <row r="818" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A818" s="9"/>
-      <c r="B818" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="J817" s="22"/>
+      <c r="K817" s="22"/>
+      <c r="L817" s="22"/>
+    </row>
+    <row r="818" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B818" s="25"/>
       <c r="C818" s="25"/>
       <c r="D818" s="22"/>
-      <c r="E818" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F818" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="E818" s="22"/>
+      <c r="F818" s="25"/>
       <c r="G818" s="23" t="s">
-        <v>869</v>
+        <v>875</v>
       </c>
       <c r="H818" s="23"/>
       <c r="I818" s="23"/>
+      <c r="J818" s="22"/>
+      <c r="K818" s="22"/>
+      <c r="L818" s="22"/>
     </row>
     <row r="819" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A819" s="9"/>
-      <c r="B819" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B819" s="25"/>
       <c r="C819" s="25"/>
       <c r="D819" s="22"/>
-      <c r="E819" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F819" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="E819" s="22"/>
+      <c r="F819" s="25"/>
       <c r="G819" s="23" t="s">
-        <v>870</v>
+        <v>876</v>
       </c>
       <c r="H819" s="23"/>
-      <c r="I819" s="23" t="s">
-        <v>268</v>
-      </c>
+      <c r="I819" s="23"/>
+      <c r="J819" s="22"/>
+      <c r="K819" s="22"/>
+      <c r="L819" s="22"/>
     </row>
     <row r="820" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A820" s="9"/>
-      <c r="B820" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B820" s="25"/>
       <c r="C820" s="25"/>
       <c r="D820" s="22"/>
-      <c r="E820" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F820" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="E820" s="22"/>
+      <c r="F820" s="25"/>
       <c r="G820" s="23" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="H820" s="23"/>
       <c r="I820" s="23"/>
+      <c r="J820" s="22"/>
+      <c r="K820" s="22"/>
+      <c r="L820" s="22"/>
     </row>
     <row r="821" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A821" s="9"/>
       <c r="B821" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C821" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D821" s="22"/>
+      <c r="C821" s="25"/>
+      <c r="D821" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E821" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F821" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="F821" s="25"/>
       <c r="G821" s="23" t="s">
-        <v>872</v>
+        <v>878</v>
       </c>
       <c r="H821" s="23"/>
       <c r="I821" s="23"/>
-    </row>
-    <row r="822" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A822" s="9"/>
-      <c r="B822" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C822" s="25"/>
+      <c r="J821" s="22"/>
+      <c r="K821" s="22"/>
+      <c r="L821" s="22"/>
+    </row>
+    <row r="822" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B822" s="22"/>
+      <c r="C822" s="22"/>
       <c r="D822" s="22"/>
-      <c r="E822" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F822" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G822" s="23" t="s">
-        <v>873</v>
-      </c>
+      <c r="E822" s="22"/>
+      <c r="F822" s="22"/>
+      <c r="G822" s="23"/>
       <c r="H822" s="23"/>
       <c r="I822" s="23"/>
-    </row>
-    <row r="823" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A823" s="9"/>
-      <c r="B823" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C823" s="25"/>
-      <c r="D823" s="22"/>
-      <c r="E823" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F823" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G823" s="23" t="s">
-        <v>874</v>
-      </c>
-      <c r="H823" s="23"/>
-      <c r="I823" s="23"/>
-    </row>
-    <row r="824" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A824" s="9"/>
-      <c r="B824" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C824" s="25"/>
-      <c r="D824" s="22"/>
-      <c r="E824" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F824" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G824" s="23" t="s">
-        <v>875</v>
-      </c>
-      <c r="H824" s="23"/>
-      <c r="I824" s="23"/>
-    </row>
-    <row r="825" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A825" s="9"/>
-      <c r="B825" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C825" s="25"/>
-      <c r="D825" s="22"/>
-      <c r="E825" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F825" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G825" s="23" t="s">
-        <v>876</v>
-      </c>
-      <c r="H825" s="23"/>
-      <c r="I825" s="23"/>
-    </row>
-    <row r="826" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A826" s="9"/>
-      <c r="B826" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C826" s="25"/>
-      <c r="D826" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E826" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F826" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G826" s="23" t="s">
-        <v>877</v>
-      </c>
-      <c r="H826" s="23"/>
-      <c r="I826" s="23"/>
+      <c r="J822" s="22"/>
+      <c r="K822" s="22"/>
+      <c r="L822" s="22"/>
+    </row>
+    <row r="823" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B823" s="1"/>
+      <c r="C823" s="1"/>
+      <c r="D823" s="1"/>
+      <c r="E823" s="1"/>
+      <c r="F823" s="1"/>
+      <c r="G823" s="1"/>
+      <c r="H823" s="1"/>
+      <c r="I823" s="1"/>
+      <c r="J823" s="1"/>
+      <c r="K823" s="1"/>
+      <c r="L823" s="1"/>
+      <c r="M823" s="1"/>
+      <c r="N823" s="1"/>
+    </row>
+    <row r="824" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A824" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B824" s="17"/>
+      <c r="C824" s="18"/>
+      <c r="D824" s="18"/>
+      <c r="E824" s="18"/>
+      <c r="F824" s="18"/>
+      <c r="G824" s="1"/>
+      <c r="H824" s="1"/>
+      <c r="I824" s="1"/>
+      <c r="J824" s="1"/>
+      <c r="K824" s="1"/>
+      <c r="L824" s="1"/>
+      <c r="M824" s="1"/>
+      <c r="N824" s="1"/>
+    </row>
+    <row r="825" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A825" s="16" t="s">
+        <v>879</v>
+      </c>
+      <c r="B825" s="17"/>
+      <c r="C825" s="18"/>
+      <c r="D825" s="18"/>
+      <c r="E825" s="18"/>
+      <c r="F825" s="18"/>
+      <c r="G825" s="1"/>
+      <c r="H825" s="1"/>
+      <c r="I825" s="1"/>
+      <c r="J825" s="1"/>
+      <c r="K825" s="1"/>
+      <c r="L825" s="1"/>
+      <c r="M825" s="1"/>
+      <c r="N825" s="1"/>
+    </row>
+    <row r="826" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A826" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B826" s="17"/>
+      <c r="C826" s="18"/>
+      <c r="D826" s="18"/>
+      <c r="E826" s="18"/>
+      <c r="F826" s="18"/>
+      <c r="G826" s="1"/>
+      <c r="H826" s="1"/>
+      <c r="I826" s="1"/>
+      <c r="J826" s="1"/>
+      <c r="K826" s="1"/>
+      <c r="L826" s="1"/>
+      <c r="M826" s="1"/>
+      <c r="N826" s="1"/>
     </row>
     <row r="827" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A827" s="9"/>
-      <c r="B827" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C827" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D827" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E827" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F827" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G827" s="23" t="s">
-        <v>878</v>
-      </c>
-      <c r="H827" s="23"/>
-      <c r="I827" s="23"/>
+      <c r="B827" s="1"/>
+      <c r="C827" s="1"/>
+      <c r="D827" s="1"/>
+      <c r="E827" s="1"/>
+      <c r="F827" s="1"/>
+      <c r="G827" s="1"/>
+      <c r="H827" s="1"/>
+      <c r="I827" s="1"/>
+      <c r="J827" s="1"/>
+      <c r="K827" s="1"/>
+      <c r="L827" s="1"/>
+      <c r="M827" s="1"/>
+      <c r="N827" s="1"/>
     </row>
     <row r="828" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A828" s="9"/>
-      <c r="B828" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C828" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D828" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E828" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F828" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G828" s="23" t="s">
-        <v>879</v>
-      </c>
-      <c r="H828" s="23"/>
-      <c r="I828" s="23"/>
-    </row>
-    <row r="829" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A829" s="9"/>
-      <c r="B829" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C829" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D829" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E829" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F829" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G829" s="23" t="s">
+      <c r="B828" s="46"/>
+      <c r="C828" s="1"/>
+      <c r="D828" s="1"/>
+      <c r="E828" s="1"/>
+      <c r="F828" s="1"/>
+      <c r="G828" s="1"/>
+      <c r="H828" s="1"/>
+      <c r="I828" s="1"/>
+      <c r="J828" s="1"/>
+      <c r="K828" s="1"/>
+      <c r="L828" s="1"/>
+    </row>
+    <row r="829" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A829" s="19"/>
+      <c r="B829" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C829" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D829" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E829" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F829" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G829" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H829" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I829" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J829" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K829" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L829" s="11" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="830" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A830" s="21" t="s">
         <v>880</v>
       </c>
-      <c r="H829" s="23"/>
-      <c r="I829" s="23"/>
-    </row>
-    <row r="830" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A830" s="9"/>
       <c r="B830" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C830" s="25"/>
       <c r="D830" s="22"/>
-      <c r="E830" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F830" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="E830" s="22"/>
+      <c r="F830" s="25"/>
       <c r="G830" s="23" t="s">
         <v>881</v>
       </c>
       <c r="H830" s="23"/>
       <c r="I830" s="23"/>
-    </row>
-    <row r="831" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A831" s="9"/>
+      <c r="J830" s="22"/>
+      <c r="K830" s="22"/>
+      <c r="L830" s="22"/>
+    </row>
+    <row r="831" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B831" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C831" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D831" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E831" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F831" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="C831" s="25"/>
+      <c r="D831" s="22"/>
+      <c r="E831" s="22"/>
+      <c r="F831" s="25"/>
       <c r="G831" s="23" t="s">
         <v>882</v>
       </c>
       <c r="H831" s="23"/>
       <c r="I831" s="23"/>
-    </row>
-    <row r="832" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A832" s="9"/>
+      <c r="J831" s="22"/>
+      <c r="K831" s="22"/>
+      <c r="L831" s="22"/>
+    </row>
+    <row r="832" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B832" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C832" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D832" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E832" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F832" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="C832" s="25"/>
+      <c r="D832" s="22"/>
+      <c r="E832" s="22"/>
+      <c r="F832" s="25"/>
       <c r="G832" s="23" t="s">
         <v>883</v>
       </c>
       <c r="H832" s="23"/>
       <c r="I832" s="23"/>
-    </row>
-    <row r="833" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A833" s="9"/>
+      <c r="J832" s="22"/>
+      <c r="K832" s="22"/>
+      <c r="L832" s="22"/>
+    </row>
+    <row r="833" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B833" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C833" s="25"/>
-      <c r="D833" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E833" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F833" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="D833" s="22"/>
+      <c r="E833" s="22"/>
+      <c r="F833" s="25"/>
       <c r="G833" s="23" t="s">
         <v>884</v>
       </c>
       <c r="H833" s="23"/>
       <c r="I833" s="23"/>
-    </row>
-    <row r="834" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A834" s="9"/>
-      <c r="B834" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="J833" s="22"/>
+      <c r="K833" s="22"/>
+      <c r="L833" s="22"/>
+    </row>
+    <row r="834" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B834" s="25"/>
       <c r="C834" s="25"/>
-      <c r="D834" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E834" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F834" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="D834" s="22"/>
+      <c r="E834" s="22"/>
+      <c r="F834" s="25"/>
       <c r="G834" s="23" t="s">
         <v>885</v>
       </c>
       <c r="H834" s="23"/>
       <c r="I834" s="23"/>
+      <c r="J834" s="22"/>
+      <c r="K834" s="22"/>
+      <c r="L834" s="22"/>
     </row>
     <row r="835" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A835" s="9"/>
-      <c r="B835" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B835" s="25"/>
       <c r="C835" s="25"/>
       <c r="D835" s="22"/>
-      <c r="E835" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F835" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="E835" s="22"/>
+      <c r="F835" s="25"/>
       <c r="G835" s="23" t="s">
         <v>886</v>
       </c>
       <c r="H835" s="23"/>
       <c r="I835" s="23"/>
-    </row>
-    <row r="836" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A836" s="9"/>
+      <c r="J835" s="22"/>
+      <c r="K835" s="22"/>
+      <c r="L835" s="22"/>
+    </row>
+    <row r="836" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B836" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C836" s="25"/>
-      <c r="D836" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E836" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F836" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="D836" s="22"/>
+      <c r="E836" s="22"/>
+      <c r="F836" s="25"/>
       <c r="G836" s="23" t="s">
         <v>887</v>
       </c>
       <c r="H836" s="23"/>
       <c r="I836" s="23"/>
-    </row>
-    <row r="837" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A837" s="9"/>
+      <c r="J836" s="22"/>
+      <c r="K836" s="22"/>
+      <c r="L836" s="22"/>
+    </row>
+    <row r="837" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B837" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C837" s="25"/>
-      <c r="D837" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E837" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F837" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="D837" s="22"/>
+      <c r="E837" s="22"/>
+      <c r="F837" s="25"/>
       <c r="G837" s="23" t="s">
         <v>888</v>
       </c>
       <c r="H837" s="23"/>
       <c r="I837" s="23"/>
-    </row>
-    <row r="838" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A838" s="9"/>
+      <c r="J837" s="22"/>
+      <c r="K837" s="22"/>
+      <c r="L837" s="22"/>
+    </row>
+    <row r="838" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B838" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C838" s="25"/>
-      <c r="D838" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E838" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F838" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="D838" s="22"/>
+      <c r="E838" s="22"/>
+      <c r="F838" s="25"/>
       <c r="G838" s="23" t="s">
         <v>889</v>
       </c>
       <c r="H838" s="23"/>
       <c r="I838" s="23"/>
-    </row>
-    <row r="839" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A839" s="9"/>
+      <c r="J838" s="22"/>
+      <c r="K838" s="22"/>
+      <c r="L838" s="22"/>
+    </row>
+    <row r="839" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B839" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C839" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D839" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E839" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F839" s="22" t="s">
-        <v>640</v>
-      </c>
+      <c r="C839" s="25"/>
+      <c r="D839" s="22"/>
+      <c r="E839" s="22"/>
+      <c r="F839" s="25"/>
       <c r="G839" s="23" t="s">
         <v>890</v>
       </c>
       <c r="H839" s="23"/>
       <c r="I839" s="23"/>
+      <c r="J839" s="22"/>
+      <c r="K839" s="22"/>
+      <c r="L839" s="22"/>
     </row>
     <row r="840" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A840" s="9"/>
-      <c r="B840" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C840" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D840" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E840" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F840" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G840" s="23" t="s">
-        <v>891</v>
-      </c>
+      <c r="B840" s="22"/>
+      <c r="C840" s="22"/>
+      <c r="D840" s="22"/>
+      <c r="E840" s="22"/>
+      <c r="F840" s="22"/>
+      <c r="G840" s="23"/>
       <c r="H840" s="23"/>
       <c r="I840" s="23"/>
+      <c r="J840" s="22"/>
+      <c r="K840" s="22"/>
+      <c r="L840" s="22"/>
     </row>
     <row r="841" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A841" s="9"/>
-      <c r="B841" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C841" s="25"/>
+      <c r="B841" s="22"/>
+      <c r="C841" s="22"/>
       <c r="D841" s="22"/>
-      <c r="E841" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F841" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G841" s="23" t="s">
-        <v>892</v>
-      </c>
+      <c r="E841" s="22"/>
+      <c r="F841" s="22"/>
+      <c r="G841" s="23"/>
       <c r="H841" s="23"/>
       <c r="I841" s="23"/>
+      <c r="J841" s="22"/>
+      <c r="K841" s="22"/>
+      <c r="L841" s="22"/>
     </row>
     <row r="842" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A842" s="9"/>
-      <c r="B842" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C842" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D842" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E842" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F842" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G842" s="23" t="s">
-        <v>893</v>
-      </c>
+      <c r="B842" s="22"/>
+      <c r="C842" s="22"/>
+      <c r="D842" s="22"/>
+      <c r="E842" s="22"/>
+      <c r="F842" s="22"/>
+      <c r="G842" s="23"/>
       <c r="H842" s="23"/>
       <c r="I842" s="23"/>
+      <c r="J842" s="22"/>
+      <c r="K842" s="22"/>
+      <c r="L842" s="22"/>
     </row>
     <row r="843" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A843" s="9"/>
-      <c r="B843" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C843" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D843" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E843" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F843" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G843" s="23" t="s">
-        <v>894</v>
-      </c>
-      <c r="H843" s="23"/>
-      <c r="I843" s="23"/>
+      <c r="B843" s="1"/>
+      <c r="C843" s="1"/>
+      <c r="D843" s="1"/>
+      <c r="E843" s="1"/>
+      <c r="F843" s="1"/>
+      <c r="G843" s="1"/>
+      <c r="H843" s="1"/>
+      <c r="I843" s="1"/>
+      <c r="J843" s="1"/>
+      <c r="K843" s="1"/>
+      <c r="L843" s="1"/>
+      <c r="M843" s="1"/>
+      <c r="N843" s="1"/>
     </row>
     <row r="844" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A844" s="9"/>
-      <c r="B844" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C844" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D844" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E844" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F844" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G844" s="23" t="s">
-        <v>895</v>
-      </c>
-      <c r="H844" s="23"/>
-      <c r="I844" s="23"/>
+      <c r="B844" s="1"/>
+      <c r="C844" s="1"/>
+      <c r="D844" s="1"/>
+      <c r="E844" s="1"/>
+      <c r="F844" s="1"/>
+      <c r="G844" s="1"/>
+      <c r="H844" s="1"/>
+      <c r="I844" s="1"/>
+      <c r="J844" s="1"/>
+      <c r="K844" s="1"/>
+      <c r="L844" s="1"/>
+      <c r="M844" s="1"/>
+      <c r="N844" s="1"/>
     </row>
     <row r="845" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A845" s="9"/>
-      <c r="B845" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C845" s="25"/>
-      <c r="D845" s="22"/>
-      <c r="E845" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F845" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G845" s="23" t="s">
-        <v>896</v>
-      </c>
-      <c r="H845" s="23"/>
-      <c r="I845" s="23"/>
+      <c r="B845" s="1"/>
+      <c r="C845" s="1"/>
+      <c r="D845" s="1"/>
+      <c r="E845" s="1"/>
+      <c r="F845" s="1"/>
+      <c r="G845" s="1"/>
+      <c r="H845" s="1"/>
+      <c r="I845" s="1"/>
+      <c r="J845" s="1"/>
+      <c r="K845" s="1"/>
+      <c r="L845" s="1"/>
+      <c r="M845" s="1"/>
+      <c r="N845" s="1"/>
     </row>
     <row r="846" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A846" s="9"/>
-      <c r="B846" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C846" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D846" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E846" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F846" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G846" s="23" t="s">
-        <v>897</v>
-      </c>
-      <c r="H846" s="23"/>
-      <c r="I846" s="23"/>
+      <c r="B846" s="1"/>
+      <c r="C846" s="1"/>
+      <c r="D846" s="1"/>
+      <c r="E846" s="1"/>
+      <c r="F846" s="1"/>
+      <c r="G846" s="1"/>
+      <c r="H846" s="1"/>
+      <c r="I846" s="1"/>
+      <c r="J846" s="1"/>
+      <c r="K846" s="1"/>
+      <c r="L846" s="1"/>
+      <c r="M846" s="1"/>
+      <c r="N846" s="1"/>
     </row>
     <row r="847" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A847" s="9"/>
-      <c r="B847" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C847" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D847" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E847" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F847" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G847" s="23" t="s">
-        <v>898</v>
-      </c>
-      <c r="H847" s="23"/>
-      <c r="I847" s="23"/>
+      <c r="B847" s="1"/>
+      <c r="C847" s="1"/>
+      <c r="D847" s="1"/>
+      <c r="E847" s="1"/>
+      <c r="F847" s="1"/>
+      <c r="G847" s="1"/>
+      <c r="H847" s="1"/>
+      <c r="I847" s="1"/>
+      <c r="J847" s="1"/>
+      <c r="K847" s="1"/>
+      <c r="L847" s="1"/>
+      <c r="M847" s="1"/>
+      <c r="N847" s="1"/>
     </row>
     <row r="848" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A848" s="9"/>
-      <c r="B848" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C848" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D848" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E848" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F848" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G848" s="23" t="s">
-        <v>899</v>
-      </c>
-      <c r="H848" s="23"/>
-      <c r="I848" s="23"/>
+      <c r="B848" s="1"/>
+      <c r="C848" s="1"/>
+      <c r="D848" s="1"/>
+      <c r="E848" s="1"/>
+      <c r="F848" s="1"/>
+      <c r="G848" s="1"/>
+      <c r="H848" s="1"/>
+      <c r="I848" s="1"/>
+      <c r="J848" s="1"/>
+      <c r="K848" s="1"/>
+      <c r="L848" s="1"/>
+      <c r="M848" s="1"/>
+      <c r="N848" s="1"/>
     </row>
     <row r="849" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A849" s="9"/>
-      <c r="B849" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C849" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D849" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E849" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F849" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G849" s="23" t="s">
-        <v>900</v>
-      </c>
-      <c r="H849" s="23"/>
-      <c r="I849" s="23"/>
+      <c r="B849" s="1"/>
+      <c r="C849" s="1"/>
+      <c r="D849" s="1"/>
+      <c r="E849" s="1"/>
+      <c r="F849" s="1"/>
+      <c r="G849" s="1"/>
+      <c r="H849" s="1"/>
+      <c r="I849" s="1"/>
+      <c r="J849" s="1"/>
+      <c r="K849" s="1"/>
+      <c r="L849" s="1"/>
+      <c r="M849" s="1"/>
+      <c r="N849" s="1"/>
+      <c r="O849" s="1"/>
     </row>
     <row r="850" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A850" s="9"/>
-      <c r="B850" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C850" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D850" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E850" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F850" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G850" s="23" t="s">
-        <v>901</v>
-      </c>
-      <c r="H850" s="23"/>
-      <c r="I850" s="23"/>
     </row>
     <row r="851" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A851" s="9"/>
-      <c r="B851" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C851" s="25"/>
-      <c r="D851" s="22"/>
-      <c r="E851" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F851" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G851" s="23" t="s">
-        <v>902</v>
-      </c>
-      <c r="H851" s="23"/>
-      <c r="I851" s="23"/>
+      <c r="A851" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B851" s="17"/>
+      <c r="C851" s="18"/>
+      <c r="D851" s="18"/>
+      <c r="E851" s="18"/>
+      <c r="F851" s="18"/>
     </row>
     <row r="852" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A852" s="9"/>
-      <c r="B852" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C852" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D852" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E852" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F852" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G852" s="23" t="s">
-        <v>903</v>
-      </c>
-      <c r="H852" s="23"/>
-      <c r="I852" s="23"/>
+      <c r="A852" s="16" t="s">
+        <v>891</v>
+      </c>
+      <c r="B852" s="17"/>
+      <c r="C852" s="18"/>
+      <c r="D852" s="18"/>
+      <c r="E852" s="18"/>
+      <c r="F852" s="18"/>
     </row>
     <row r="853" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A853" s="9"/>
-      <c r="B853" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C853" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D853" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E853" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F853" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G853" s="23" t="s">
-        <v>904</v>
-      </c>
-      <c r="H853" s="23"/>
-      <c r="I853" s="23"/>
-    </row>
-    <row r="854" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A853" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B853" s="17"/>
+      <c r="C853" s="18"/>
+      <c r="D853" s="18"/>
+      <c r="E853" s="18"/>
+      <c r="F853" s="18"/>
+    </row>
+    <row r="854" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A854" s="9"/>
-      <c r="B854" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C854" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D854" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E854" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F854" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G854" s="23" t="s">
-        <v>905</v>
-      </c>
-      <c r="H854" s="23"/>
-      <c r="I854" s="23"/>
+      <c r="B854" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C854" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D854" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E854" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F854" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G854" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H854" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I854" s="20" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="855" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A855" s="9"/>
+      <c r="A855" s="21" t="s">
+        <v>892</v>
+      </c>
       <c r="B855" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C855" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D855" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C855" s="25"/>
+      <c r="D855" s="22"/>
       <c r="E855" s="22" t="s">
         <v>22</v>
       </c>
@@ -19584,31 +19579,33 @@
         <v>640</v>
       </c>
       <c r="G855" s="23" t="s">
-        <v>906</v>
+        <v>893</v>
       </c>
       <c r="H855" s="23"/>
       <c r="I855" s="23"/>
     </row>
-    <row r="856" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A856" s="9"/>
-      <c r="B856" s="25" t="s">
-        <v>611</v>
-      </c>
-      <c r="C856" s="25"/>
+    <row r="856" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A856" s="21"/>
+      <c r="B856" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C856" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D856" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E856" s="25"/>
+      <c r="E856" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F856" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G856" s="23" t="s">
-        <v>907</v>
+        <v>894</v>
       </c>
       <c r="H856" s="23"/>
-      <c r="I856" s="23" t="s">
-        <v>613</v>
-      </c>
+      <c r="I856" s="23"/>
     </row>
     <row r="857" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A857" s="9"/>
@@ -19628,7 +19625,7 @@
         <v>640</v>
       </c>
       <c r="G857" s="23" t="s">
-        <v>908</v>
+        <v>895</v>
       </c>
       <c r="H857" s="23"/>
       <c r="I857" s="23"/>
@@ -19638,20 +19635,16 @@
       <c r="B858" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C858" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D858" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C858" s="25"/>
+      <c r="D858" s="22"/>
       <c r="E858" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F858" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="G858" s="23" t="s">
-        <v>909</v>
+      <c r="G858" s="45" t="s">
+        <v>896</v>
       </c>
       <c r="H858" s="23"/>
       <c r="I858" s="23"/>
@@ -19674,7 +19667,7 @@
         <v>640</v>
       </c>
       <c r="G859" s="23" t="s">
-        <v>910</v>
+        <v>897</v>
       </c>
       <c r="H859" s="23"/>
       <c r="I859" s="23"/>
@@ -19684,12 +19677,8 @@
       <c r="B860" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C860" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D860" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C860" s="25"/>
+      <c r="D860" s="22"/>
       <c r="E860" s="22" t="s">
         <v>22</v>
       </c>
@@ -19697,7 +19686,7 @@
         <v>640</v>
       </c>
       <c r="G860" s="23" t="s">
-        <v>911</v>
+        <v>898</v>
       </c>
       <c r="H860" s="23"/>
       <c r="I860" s="23"/>
@@ -19707,12 +19696,8 @@
       <c r="B861" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C861" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D861" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C861" s="25"/>
+      <c r="D861" s="22"/>
       <c r="E861" s="22" t="s">
         <v>22</v>
       </c>
@@ -19720,7 +19705,7 @@
         <v>640</v>
       </c>
       <c r="G861" s="23" t="s">
-        <v>912</v>
+        <v>899</v>
       </c>
       <c r="H861" s="23"/>
       <c r="I861" s="23"/>
@@ -19730,12 +19715,8 @@
       <c r="B862" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C862" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D862" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C862" s="25"/>
+      <c r="D862" s="22"/>
       <c r="E862" s="22" t="s">
         <v>22</v>
       </c>
@@ -19743,22 +19724,18 @@
         <v>640</v>
       </c>
       <c r="G862" s="23" t="s">
-        <v>913</v>
+        <v>900</v>
       </c>
       <c r="H862" s="23"/>
       <c r="I862" s="23"/>
     </row>
-    <row r="863" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="863" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A863" s="9"/>
       <c r="B863" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C863" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D863" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C863" s="25"/>
+      <c r="D863" s="22"/>
       <c r="E863" s="22" t="s">
         <v>22</v>
       </c>
@@ -19766,12 +19743,14 @@
         <v>640</v>
       </c>
       <c r="G863" s="23" t="s">
-        <v>914</v>
+        <v>901</v>
       </c>
       <c r="H863" s="23"/>
-      <c r="I863" s="23"/>
-    </row>
-    <row r="864" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I863" s="23" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="864" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A864" s="9"/>
       <c r="B864" s="22" t="s">
         <v>22</v>
@@ -19785,16 +19764,19 @@
         <v>640</v>
       </c>
       <c r="G864" s="23" t="s">
-        <v>915</v>
+        <v>902</v>
       </c>
       <c r="H864" s="23"/>
       <c r="I864" s="23"/>
     </row>
     <row r="865" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A865" s="9"/>
       <c r="B865" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C865" s="25"/>
+      <c r="C865" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D865" s="22"/>
       <c r="E865" s="22" t="s">
         <v>22</v>
@@ -19803,12 +19785,13 @@
         <v>640</v>
       </c>
       <c r="G865" s="23" t="s">
-        <v>916</v>
+        <v>903</v>
       </c>
       <c r="H865" s="23"/>
       <c r="I865" s="23"/>
     </row>
-    <row r="866" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="866" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A866" s="9"/>
       <c r="B866" s="22" t="s">
         <v>22</v>
       </c>
@@ -19821,21 +19804,18 @@
         <v>640</v>
       </c>
       <c r="G866" s="23" t="s">
-        <v>917</v>
+        <v>904</v>
       </c>
       <c r="H866" s="23"/>
       <c r="I866" s="23"/>
     </row>
-    <row r="867" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="867" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A867" s="9"/>
       <c r="B867" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C867" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D867" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C867" s="25"/>
+      <c r="D867" s="22"/>
       <c r="E867" s="22" t="s">
         <v>22</v>
       </c>
@@ -19843,21 +19823,18 @@
         <v>640</v>
       </c>
       <c r="G867" s="23" t="s">
-        <v>918</v>
+        <v>905</v>
       </c>
       <c r="H867" s="23"/>
       <c r="I867" s="23"/>
     </row>
-    <row r="868" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="868" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A868" s="9"/>
       <c r="B868" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C868" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D868" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C868" s="25"/>
+      <c r="D868" s="22"/>
       <c r="E868" s="22" t="s">
         <v>22</v>
       </c>
@@ -19865,34 +19842,32 @@
         <v>640</v>
       </c>
       <c r="G868" s="23" t="s">
-        <v>919</v>
+        <v>906</v>
       </c>
       <c r="H868" s="23"/>
       <c r="I868" s="23"/>
     </row>
-    <row r="869" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="869" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A869" s="9"/>
       <c r="B869" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C869" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D869" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C869" s="25"/>
+      <c r="D869" s="22"/>
       <c r="E869" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F869" s="22" t="s">
-        <v>920</v>
+        <v>640</v>
       </c>
       <c r="G869" s="23" t="s">
-        <v>921</v>
+        <v>907</v>
       </c>
       <c r="H869" s="23"/>
       <c r="I869" s="23"/>
     </row>
-    <row r="870" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="870" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A870" s="9"/>
       <c r="B870" s="22" t="s">
         <v>22</v>
       </c>
@@ -19904,122 +19879,1038 @@
         <v>22</v>
       </c>
       <c r="F870" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G870" s="23" t="s">
+        <v>908</v>
+      </c>
+      <c r="H870" s="23"/>
+      <c r="I870" s="23"/>
+    </row>
+    <row r="871" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A871" s="9"/>
+      <c r="B871" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C871" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D871" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E871" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F871" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G871" s="23" t="s">
+        <v>909</v>
+      </c>
+      <c r="H871" s="23"/>
+      <c r="I871" s="23"/>
+    </row>
+    <row r="872" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A872" s="9"/>
+      <c r="B872" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C872" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D872" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E872" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F872" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G872" s="23" t="s">
+        <v>910</v>
+      </c>
+      <c r="H872" s="23"/>
+      <c r="I872" s="23"/>
+    </row>
+    <row r="873" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A873" s="9"/>
+      <c r="B873" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C873" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D873" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E873" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F873" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G873" s="23" t="s">
+        <v>911</v>
+      </c>
+      <c r="H873" s="23"/>
+      <c r="I873" s="23"/>
+    </row>
+    <row r="874" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A874" s="9"/>
+      <c r="B874" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C874" s="25"/>
+      <c r="D874" s="22"/>
+      <c r="E874" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F874" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G874" s="23" t="s">
+        <v>912</v>
+      </c>
+      <c r="H874" s="23"/>
+      <c r="I874" s="23"/>
+    </row>
+    <row r="875" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A875" s="9"/>
+      <c r="B875" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C875" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D875" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E875" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F875" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G875" s="23" t="s">
+        <v>913</v>
+      </c>
+      <c r="H875" s="23"/>
+      <c r="I875" s="23"/>
+    </row>
+    <row r="876" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A876" s="9"/>
+      <c r="B876" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C876" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D876" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E876" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F876" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G876" s="23" t="s">
+        <v>914</v>
+      </c>
+      <c r="H876" s="23"/>
+      <c r="I876" s="23"/>
+    </row>
+    <row r="877" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A877" s="9"/>
+      <c r="B877" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C877" s="25"/>
+      <c r="D877" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E877" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F877" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G877" s="23" t="s">
+        <v>915</v>
+      </c>
+      <c r="H877" s="23"/>
+      <c r="I877" s="23"/>
+    </row>
+    <row r="878" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A878" s="9"/>
+      <c r="B878" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C878" s="25"/>
+      <c r="D878" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E878" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F878" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G878" s="23" t="s">
+        <v>916</v>
+      </c>
+      <c r="H878" s="23"/>
+      <c r="I878" s="23"/>
+    </row>
+    <row r="879" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A879" s="9"/>
+      <c r="B879" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C879" s="25"/>
+      <c r="D879" s="22"/>
+      <c r="E879" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F879" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G879" s="23" t="s">
+        <v>917</v>
+      </c>
+      <c r="H879" s="23"/>
+      <c r="I879" s="23"/>
+    </row>
+    <row r="880" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A880" s="9"/>
+      <c r="B880" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C880" s="25"/>
+      <c r="D880" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E880" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F880" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G880" s="23" t="s">
+        <v>918</v>
+      </c>
+      <c r="H880" s="23"/>
+      <c r="I880" s="23"/>
+    </row>
+    <row r="881" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A881" s="9"/>
+      <c r="B881" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C881" s="25"/>
+      <c r="D881" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E881" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F881" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G881" s="23" t="s">
+        <v>919</v>
+      </c>
+      <c r="H881" s="23"/>
+      <c r="I881" s="23"/>
+    </row>
+    <row r="882" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A882" s="9"/>
+      <c r="B882" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C882" s="25"/>
+      <c r="D882" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E882" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F882" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G882" s="23" t="s">
         <v>920</v>
       </c>
-      <c r="G870" s="23" t="s">
+      <c r="H882" s="23"/>
+      <c r="I882" s="23"/>
+    </row>
+    <row r="883" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A883" s="9"/>
+      <c r="B883" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C883" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D883" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E883" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F883" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G883" s="23" t="s">
+        <v>921</v>
+      </c>
+      <c r="H883" s="23"/>
+      <c r="I883" s="23"/>
+    </row>
+    <row r="884" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A884" s="9"/>
+      <c r="B884" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C884" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D884" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E884" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F884" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G884" s="23" t="s">
         <v>922</v>
       </c>
-      <c r="H870" s="23"/>
-      <c r="I870" s="23" t="s">
+      <c r="H884" s="23"/>
+      <c r="I884" s="23"/>
+    </row>
+    <row r="885" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A885" s="9"/>
+      <c r="B885" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C885" s="25"/>
+      <c r="D885" s="22"/>
+      <c r="E885" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F885" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G885" s="23" t="s">
         <v>923</v>
       </c>
-    </row>
-    <row r="871" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B871" s="27" t="s">
+      <c r="H885" s="23"/>
+      <c r="I885" s="23"/>
+    </row>
+    <row r="886" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A886" s="9"/>
+      <c r="B886" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C886" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D886" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E886" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F886" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="C871" s="27"/>
-      <c r="D871" s="27" t="s">
+      <c r="G886" s="23" t="s">
+        <v>924</v>
+      </c>
+      <c r="H886" s="23"/>
+      <c r="I886" s="23"/>
+    </row>
+    <row r="887" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A887" s="9"/>
+      <c r="B887" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C887" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D887" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E887" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F887" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="E871" s="27"/>
-      <c r="F871" s="27" t="s">
+      <c r="G887" s="23" t="s">
+        <v>925</v>
+      </c>
+      <c r="H887" s="23"/>
+      <c r="I887" s="23"/>
+    </row>
+    <row r="888" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A888" s="9"/>
+      <c r="B888" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C888" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D888" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E888" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F888" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="G871" s="28" t="s">
-        <v>924</v>
-      </c>
-      <c r="H871" s="28"/>
-      <c r="I871" s="28" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="872" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B872" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C872" s="25"/>
-      <c r="D872" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E872" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F872" s="22" t="s">
-        <v>920</v>
-      </c>
-      <c r="G872" s="23" t="s">
+      <c r="G888" s="23" t="s">
         <v>926</v>
       </c>
-      <c r="H872" s="23"/>
-      <c r="I872" s="23" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="873" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B873" s="27" t="s">
+      <c r="H888" s="23"/>
+      <c r="I888" s="23"/>
+    </row>
+    <row r="889" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A889" s="9"/>
+      <c r="B889" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C889" s="25"/>
+      <c r="D889" s="22"/>
+      <c r="E889" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F889" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="C873" s="27"/>
-      <c r="D873" s="27" t="s">
+      <c r="G889" s="23" t="s">
+        <v>927</v>
+      </c>
+      <c r="H889" s="23"/>
+      <c r="I889" s="23"/>
+    </row>
+    <row r="890" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A890" s="9"/>
+      <c r="B890" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C890" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D890" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E890" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F890" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="E873" s="27"/>
-      <c r="F873" s="27" t="s">
+      <c r="G890" s="23" t="s">
+        <v>928</v>
+      </c>
+      <c r="H890" s="23"/>
+      <c r="I890" s="23"/>
+    </row>
+    <row r="891" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A891" s="9"/>
+      <c r="B891" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C891" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D891" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E891" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F891" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="G873" s="28" t="s">
-        <v>927</v>
-      </c>
-      <c r="H873" s="28"/>
-      <c r="I873" s="28" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G891" s="23" t="s">
+        <v>929</v>
+      </c>
+      <c r="H891" s="23"/>
+      <c r="I891" s="23"/>
+    </row>
+    <row r="892" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A892" s="9"/>
+      <c r="B892" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C892" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D892" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E892" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F892" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G892" s="23" t="s">
+        <v>930</v>
+      </c>
+      <c r="H892" s="23"/>
+      <c r="I892" s="23"/>
+    </row>
+    <row r="893" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A893" s="9"/>
+      <c r="B893" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C893" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D893" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E893" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F893" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G893" s="23" t="s">
+        <v>931</v>
+      </c>
+      <c r="H893" s="23"/>
+      <c r="I893" s="23"/>
+    </row>
+    <row r="894" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A894" s="9"/>
+      <c r="B894" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C894" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D894" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E894" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F894" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G894" s="23" t="s">
+        <v>932</v>
+      </c>
+      <c r="H894" s="23"/>
+      <c r="I894" s="23"/>
+    </row>
+    <row r="895" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A895" s="9"/>
+      <c r="B895" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C895" s="25"/>
+      <c r="D895" s="22"/>
+      <c r="E895" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F895" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G895" s="23" t="s">
+        <v>933</v>
+      </c>
+      <c r="H895" s="23"/>
+      <c r="I895" s="23"/>
+    </row>
+    <row r="896" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A896" s="9"/>
+      <c r="B896" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C896" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D896" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E896" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F896" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G896" s="23" t="s">
+        <v>934</v>
+      </c>
+      <c r="H896" s="23"/>
+      <c r="I896" s="23"/>
+    </row>
+    <row r="897" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A897" s="9"/>
+      <c r="B897" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C897" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D897" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E897" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F897" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G897" s="23" t="s">
+        <v>935</v>
+      </c>
+      <c r="H897" s="23"/>
+      <c r="I897" s="23"/>
+    </row>
+    <row r="898" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A898" s="9"/>
+      <c r="B898" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C898" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D898" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E898" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F898" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G898" s="23" t="s">
+        <v>936</v>
+      </c>
+      <c r="H898" s="23"/>
+      <c r="I898" s="23"/>
+    </row>
+    <row r="899" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A899" s="9"/>
+      <c r="B899" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C899" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D899" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E899" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F899" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G899" s="23" t="s">
+        <v>937</v>
+      </c>
+      <c r="H899" s="23"/>
+      <c r="I899" s="23"/>
+    </row>
+    <row r="900" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A900" s="9"/>
+      <c r="B900" s="25" t="s">
+        <v>611</v>
+      </c>
+      <c r="C900" s="25"/>
+      <c r="D900" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E900" s="25"/>
+      <c r="F900" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G900" s="23" t="s">
+        <v>938</v>
+      </c>
+      <c r="H900" s="23"/>
+      <c r="I900" s="23" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="901" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A901" s="9"/>
+      <c r="B901" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C901" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D901" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E901" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F901" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G901" s="23" t="s">
+        <v>939</v>
+      </c>
+      <c r="H901" s="23"/>
+      <c r="I901" s="23"/>
+    </row>
+    <row r="902" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A902" s="9"/>
+      <c r="B902" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C902" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D902" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E902" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F902" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G902" s="23" t="s">
+        <v>940</v>
+      </c>
+      <c r="H902" s="23"/>
+      <c r="I902" s="23"/>
+    </row>
+    <row r="903" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A903" s="9"/>
+      <c r="B903" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C903" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D903" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E903" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F903" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G903" s="23" t="s">
+        <v>941</v>
+      </c>
+      <c r="H903" s="23"/>
+      <c r="I903" s="23"/>
+    </row>
+    <row r="904" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A904" s="9"/>
+      <c r="B904" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C904" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D904" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E904" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F904" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G904" s="23" t="s">
+        <v>942</v>
+      </c>
+      <c r="H904" s="23"/>
+      <c r="I904" s="23"/>
+    </row>
+    <row r="905" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A905" s="9"/>
+      <c r="B905" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C905" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D905" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E905" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F905" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G905" s="23" t="s">
+        <v>943</v>
+      </c>
+      <c r="H905" s="23"/>
+      <c r="I905" s="23"/>
+    </row>
+    <row r="906" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A906" s="9"/>
+      <c r="B906" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C906" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D906" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E906" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F906" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G906" s="23" t="s">
+        <v>944</v>
+      </c>
+      <c r="H906" s="23"/>
+      <c r="I906" s="23"/>
+    </row>
+    <row r="907" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A907" s="9"/>
+      <c r="B907" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C907" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D907" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E907" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F907" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G907" s="23" t="s">
+        <v>945</v>
+      </c>
+      <c r="H907" s="23"/>
+      <c r="I907" s="23"/>
+    </row>
+    <row r="908" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A908" s="9"/>
+      <c r="B908" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C908" s="25"/>
+      <c r="D908" s="22"/>
+      <c r="E908" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F908" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G908" s="23" t="s">
+        <v>946</v>
+      </c>
+      <c r="H908" s="23"/>
+      <c r="I908" s="23"/>
+    </row>
+    <row r="909" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B909" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C909" s="25"/>
+      <c r="D909" s="22"/>
+      <c r="E909" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F909" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G909" s="23" t="s">
+        <v>947</v>
+      </c>
+      <c r="H909" s="23"/>
+      <c r="I909" s="23"/>
+    </row>
+    <row r="910" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B910" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C910" s="25"/>
+      <c r="D910" s="22"/>
+      <c r="E910" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F910" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G910" s="23" t="s">
+        <v>948</v>
+      </c>
+      <c r="H910" s="23"/>
+      <c r="I910" s="23"/>
+    </row>
+    <row r="911" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B911" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C911" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D911" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E911" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F911" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G911" s="23" t="s">
+        <v>949</v>
+      </c>
+      <c r="H911" s="23"/>
+      <c r="I911" s="23"/>
+    </row>
+    <row r="912" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B912" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C912" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D912" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E912" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F912" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G912" s="23" t="s">
+        <v>950</v>
+      </c>
+      <c r="H912" s="23"/>
+      <c r="I912" s="23"/>
+    </row>
+    <row r="913" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B913" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C913" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D913" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E913" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F913" s="22" t="s">
+        <v>951</v>
+      </c>
+      <c r="G913" s="23" t="s">
+        <v>952</v>
+      </c>
+      <c r="H913" s="23"/>
+      <c r="I913" s="23"/>
+    </row>
+    <row r="914" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B914" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C914" s="25"/>
+      <c r="D914" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E914" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F914" s="22" t="s">
+        <v>951</v>
+      </c>
+      <c r="G914" s="23" t="s">
+        <v>953</v>
+      </c>
+      <c r="H914" s="23"/>
+      <c r="I914" s="23" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="915" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B915" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="C915" s="27"/>
+      <c r="D915" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="E915" s="27"/>
+      <c r="F915" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="G915" s="28" t="s">
+        <v>955</v>
+      </c>
+      <c r="H915" s="28"/>
+      <c r="I915" s="28" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="916" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B916" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C916" s="25"/>
+      <c r="D916" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E916" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F916" s="22" t="s">
+        <v>951</v>
+      </c>
+      <c r="G916" s="23" t="s">
+        <v>957</v>
+      </c>
+      <c r="H916" s="23"/>
+      <c r="I916" s="23" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="917" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B917" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="C917" s="27"/>
+      <c r="D917" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="E917" s="27"/>
+      <c r="F917" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="G917" s="28" t="s">
+        <v>958</v>
+      </c>
+      <c r="H917" s="28"/>
+      <c r="I917" s="28" t="s">
+        <v>956</v>
+      </c>
+    </row>
     <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
update menu items.  Added noise to simulation
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,12 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3743" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3824" uniqueCount="973">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
   <si>
-    <t xml:space="preserve">Revision 2.X    2/19/2021 – State Space Items – (This list is missing one VI….)</t>
+    <t xml:space="preserve">Revision 2.X    2/23/2021 – State Space Items – (This list is missing one VI….)</t>
   </si>
   <si>
     <t xml:space="preserve">This documents which Java/C++ WPILIB routines have been </t>
@@ -2605,6 +2605,45 @@
     <t xml:space="preserve">LinearSystemSim_ClampInput.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">SINGLE JOINT ARM SIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_EsitmateMOI.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_GetAngleRads.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_GetCurrentDraw.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_GetVelocityRadsPerSec.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_HasHitLowerLimit.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_HasHitUpperLimit.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_New.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_SetInputVoltage.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_Update.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_UpdateX.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_WouldHitLowerLimit.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SngJntArmSim_WouldHitUpperLimit.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">STATE SPACE HELPER</t>
   </si>
   <si>
@@ -2801,6 +2840,9 @@
   </si>
   <si>
     <t xml:space="preserve">ROTATION2D.CTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINGLE_JOINT_ARM_SIM.CTL</t>
   </si>
   <si>
     <t xml:space="preserve">SIMPLE_MOTOR_FF.CTL</t>
@@ -2960,7 +3002,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3023,12 +3065,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9999"/>
-        <bgColor rgb="FFFF8080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF3333"/>
         <bgColor rgb="FFFF0000"/>
       </patternFill>
@@ -3082,7 +3118,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3275,10 +3311,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3327,7 +3359,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF9999"/>
+      <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
@@ -3358,8 +3390,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A768" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G779" activeCellId="0" sqref="G779"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3450,28 +3482,28 @@
         <v>11</v>
       </c>
       <c r="B9" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1244,"X")</f>
-        <v>566</v>
+        <f aca="false">COUNTIF(B18:B1260,"X")</f>
+        <v>584</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C18:C1244,"X")</f>
+        <f aca="false">COUNTIF(C18:C1260,"X")</f>
         <v>368</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D18:D1244,"X")</f>
+        <f aca="false">COUNTIF(D18:D1260,"X")</f>
         <v>168</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E18:E1244,"X")</f>
-        <v>524</v>
+        <f aca="false">COUNTIF(E18:E1260,"X")</f>
+        <v>555</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F18:F1244,"S")+COUNTIF(F18:F1244,"I")+COUNTIF(F18:F1244,"X")+COUNTIF(F18:F1244,"SI")+COUNTIF(F18:F1244,"IS")+COUNTIF(F18:F1244,"N/A")</f>
-        <v>212</v>
+        <f aca="false">COUNTIF(F18:F1260,"S")+COUNTIF(F18:F1260,"I")+COUNTIF(F18:F1260,"X")+COUNTIF(F18:F1260,"SI")+COUNTIF(F18:F1260,"IS")+COUNTIF(F18:F1260,"N/A")</f>
+        <v>213</v>
       </c>
       <c r="G9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.65017667844523</v>
+        <v>0.63013698630137</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3479,8 +3511,8 @@
         <v>12</v>
       </c>
       <c r="B10" s="13" t="n">
-        <f aca="false">COUNTIF(B19:B1245,"/")</f>
-        <v>10</v>
+        <f aca="false">COUNTIF(B19:B1261,"/")</f>
+        <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>13</v>
@@ -3489,7 +3521,7 @@
     <row r="11" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.374558303886926</v>
+        <v>0.36472602739726</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4777,7 +4809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="21" t="s">
         <v>84</v>
       </c>
@@ -4786,7 +4818,9 @@
       </c>
       <c r="C84" s="25"/>
       <c r="D84" s="22"/>
-      <c r="E84" s="25"/>
+      <c r="E84" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F84" s="22"/>
       <c r="G84" s="23" t="s">
         <v>85</v>
@@ -14359,7 +14393,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="579" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="579" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="21" t="s">
         <v>674</v>
       </c>
@@ -14368,7 +14402,9 @@
       </c>
       <c r="C579" s="25"/>
       <c r="D579" s="22"/>
-      <c r="E579" s="25"/>
+      <c r="E579" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F579" s="25"/>
       <c r="G579" s="23" t="s">
         <v>675</v>
@@ -14382,7 +14418,9 @@
       </c>
       <c r="C580" s="25"/>
       <c r="D580" s="22"/>
-      <c r="E580" s="25"/>
+      <c r="E580" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F580" s="25"/>
       <c r="G580" s="23" t="s">
         <v>676</v>
@@ -14396,7 +14434,9 @@
       </c>
       <c r="C581" s="25"/>
       <c r="D581" s="22"/>
-      <c r="E581" s="25"/>
+      <c r="E581" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F581" s="25"/>
       <c r="G581" s="23" t="s">
         <v>677</v>
@@ -14410,7 +14450,9 @@
       </c>
       <c r="C582" s="25"/>
       <c r="D582" s="22"/>
-      <c r="E582" s="25"/>
+      <c r="E582" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F582" s="25"/>
       <c r="G582" s="23" t="s">
         <v>678</v>
@@ -14424,7 +14466,9 @@
       </c>
       <c r="C583" s="25"/>
       <c r="D583" s="22"/>
-      <c r="E583" s="25"/>
+      <c r="E583" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F583" s="25"/>
       <c r="G583" s="23" t="s">
         <v>679</v>
@@ -14438,7 +14482,9 @@
       </c>
       <c r="C584" s="25"/>
       <c r="D584" s="22"/>
-      <c r="E584" s="25"/>
+      <c r="E584" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F584" s="25"/>
       <c r="G584" s="23" t="s">
         <v>680</v>
@@ -14452,7 +14498,9 @@
       </c>
       <c r="C585" s="25"/>
       <c r="D585" s="22"/>
-      <c r="E585" s="25"/>
+      <c r="E585" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F585" s="25"/>
       <c r="G585" s="23" t="s">
         <v>681</v>
@@ -14466,7 +14514,9 @@
       </c>
       <c r="C586" s="25"/>
       <c r="D586" s="22"/>
-      <c r="E586" s="25"/>
+      <c r="E586" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F586" s="25"/>
       <c r="G586" s="23" t="s">
         <v>682</v>
@@ -17255,10 +17305,14 @@
       <c r="L733" s="22"/>
     </row>
     <row r="734" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B734" s="25"/>
+      <c r="B734" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C734" s="25"/>
       <c r="D734" s="22"/>
-      <c r="E734" s="22"/>
+      <c r="E734" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F734" s="25"/>
       <c r="G734" s="23" t="s">
         <v>807</v>
@@ -17285,10 +17339,14 @@
       <c r="L735" s="22"/>
     </row>
     <row r="736" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B736" s="25"/>
+      <c r="B736" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C736" s="25"/>
       <c r="D736" s="22"/>
-      <c r="E736" s="22"/>
+      <c r="E736" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F736" s="25"/>
       <c r="G736" s="23" t="s">
         <v>809</v>
@@ -17300,8 +17358,8 @@
       <c r="L736" s="22"/>
     </row>
     <row r="737" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B737" s="47" t="s">
-        <v>611</v>
+      <c r="B737" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="C737" s="25"/>
       <c r="D737" s="22"/>
@@ -17340,10 +17398,14 @@
       <c r="L738" s="22"/>
     </row>
     <row r="739" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B739" s="25"/>
+      <c r="B739" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C739" s="25"/>
       <c r="D739" s="22"/>
-      <c r="E739" s="22"/>
+      <c r="E739" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F739" s="25"/>
       <c r="G739" s="23" t="s">
         <v>812</v>
@@ -17355,10 +17417,14 @@
       <c r="L739" s="22"/>
     </row>
     <row r="740" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B740" s="25"/>
+      <c r="B740" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C740" s="25"/>
       <c r="D740" s="22"/>
-      <c r="E740" s="22"/>
+      <c r="E740" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F740" s="25"/>
       <c r="G740" s="23" t="s">
         <v>813</v>
@@ -18368,7 +18434,9 @@
       </c>
       <c r="C785" s="25"/>
       <c r="D785" s="22"/>
-      <c r="E785" s="22"/>
+      <c r="E785" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="F785" s="25"/>
       <c r="G785" s="23" t="s">
         <v>851</v>
@@ -18391,7 +18459,9 @@
       <c r="D786" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E786" s="22"/>
+      <c r="E786" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="F786" s="25"/>
       <c r="G786" s="23" t="s">
         <v>852</v>
@@ -18452,7 +18522,9 @@
       </c>
       <c r="C789" s="25"/>
       <c r="D789" s="22"/>
-      <c r="E789" s="22"/>
+      <c r="E789" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F789" s="25"/>
       <c r="G789" s="23" t="s">
         <v>855</v>
@@ -18473,7 +18545,9 @@
       </c>
       <c r="C790" s="25"/>
       <c r="D790" s="22"/>
-      <c r="E790" s="25"/>
+      <c r="E790" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F790" s="25"/>
       <c r="G790" s="23" t="s">
         <v>856</v>
@@ -18510,7 +18584,7 @@
     </row>
     <row r="792" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A792" s="21"/>
-      <c r="B792" s="48"/>
+      <c r="B792" s="47"/>
       <c r="C792" s="25"/>
       <c r="D792" s="22"/>
       <c r="E792" s="22"/>
@@ -18529,127 +18603,202 @@
     </row>
     <row r="793" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A793" s="21"/>
-      <c r="B793" s="22"/>
-      <c r="C793" s="22"/>
-      <c r="D793" s="22"/>
-      <c r="E793" s="22"/>
-      <c r="F793" s="22"/>
-      <c r="G793" s="23"/>
-      <c r="H793" s="23"/>
-      <c r="I793" s="23"/>
-      <c r="J793" s="22"/>
-      <c r="K793" s="22"/>
-      <c r="L793" s="22"/>
-      <c r="M793" s="1"/>
+      <c r="B793" s="21"/>
+      <c r="C793" s="21"/>
+      <c r="D793" s="21"/>
+      <c r="E793" s="21"/>
+      <c r="F793" s="21"/>
+      <c r="G793" s="21"/>
+      <c r="H793" s="21"/>
+      <c r="I793" s="21"/>
+      <c r="J793" s="21"/>
+      <c r="K793" s="21"/>
+      <c r="L793" s="21"/>
+      <c r="M793" s="21"/>
       <c r="N793" s="1"/>
       <c r="O793" s="1"/>
     </row>
-    <row r="794" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="794" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A794" s="19"/>
-      <c r="B794" s="19"/>
-      <c r="C794" s="19"/>
-      <c r="D794" s="19"/>
-      <c r="E794" s="19"/>
-      <c r="F794" s="19"/>
-      <c r="G794" s="1"/>
-      <c r="H794" s="1"/>
-      <c r="I794" s="1"/>
-      <c r="J794" s="1"/>
-      <c r="K794" s="1"/>
-      <c r="L794" s="1"/>
+      <c r="B794" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C794" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D794" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E794" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F794" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G794" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H794" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I794" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J794" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K794" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L794" s="11" t="s">
+        <v>692</v>
+      </c>
       <c r="M794" s="1"/>
       <c r="N794" s="1"/>
       <c r="O794" s="1"/>
     </row>
     <row r="795" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A795" s="19"/>
-      <c r="B795" s="44"/>
-      <c r="C795" s="4"/>
-      <c r="D795" s="4"/>
-      <c r="E795" s="4"/>
-      <c r="F795" s="4"/>
-    </row>
-    <row r="796" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A796" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B796" s="43"/>
-      <c r="C796" s="18"/>
-      <c r="D796" s="18"/>
-      <c r="E796" s="18"/>
-      <c r="F796" s="18"/>
-    </row>
-    <row r="797" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A797" s="16" t="s">
+      <c r="A795" s="21" t="s">
         <v>860</v>
       </c>
-      <c r="B797" s="43"/>
-      <c r="C797" s="18"/>
-      <c r="D797" s="18"/>
-      <c r="E797" s="18"/>
-      <c r="F797" s="18"/>
+      <c r="B795" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C795" s="25"/>
+      <c r="D795" s="22"/>
+      <c r="E795" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F795" s="25"/>
+      <c r="G795" s="23" t="s">
+        <v>861</v>
+      </c>
+      <c r="H795" s="23"/>
+      <c r="I795" s="23"/>
+      <c r="J795" s="22"/>
+      <c r="K795" s="22"/>
+      <c r="L795" s="22"/>
+      <c r="M795" s="1"/>
+      <c r="N795" s="1"/>
+      <c r="O795" s="1"/>
+    </row>
+    <row r="796" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A796" s="21"/>
+      <c r="B796" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C796" s="25"/>
+      <c r="D796" s="22"/>
+      <c r="E796" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F796" s="25"/>
+      <c r="G796" s="23" t="s">
+        <v>862</v>
+      </c>
+      <c r="H796" s="23"/>
+      <c r="I796" s="23"/>
+      <c r="J796" s="22"/>
+      <c r="K796" s="22"/>
+      <c r="L796" s="22"/>
+      <c r="M796" s="1"/>
+      <c r="N796" s="1"/>
+      <c r="O796" s="1"/>
+    </row>
+    <row r="797" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A797" s="21"/>
+      <c r="B797" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C797" s="25"/>
+      <c r="D797" s="22"/>
+      <c r="E797" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F797" s="25"/>
+      <c r="G797" s="23" t="s">
+        <v>863</v>
+      </c>
+      <c r="H797" s="23"/>
+      <c r="I797" s="23"/>
+      <c r="J797" s="22"/>
+      <c r="K797" s="22"/>
+      <c r="L797" s="22"/>
+      <c r="M797" s="1"/>
+      <c r="N797" s="1"/>
+      <c r="O797" s="1"/>
     </row>
     <row r="798" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A798" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B798" s="43"/>
-      <c r="C798" s="18"/>
-      <c r="D798" s="18"/>
-      <c r="E798" s="18"/>
-      <c r="F798" s="18"/>
-      <c r="H798" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="799" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A799" s="19"/>
-      <c r="B799" s="19"/>
-      <c r="C799" s="19"/>
-      <c r="D799" s="19"/>
-      <c r="E799" s="19"/>
-      <c r="F799" s="19"/>
-    </row>
-    <row r="800" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A800" s="19"/>
-      <c r="B800" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C800" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D800" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E800" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F800" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G800" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H800" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I800" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J800" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="K800" s="11" t="s">
-        <v>691</v>
-      </c>
-      <c r="L800" s="11" t="s">
-        <v>692</v>
-      </c>
+      <c r="A798" s="21"/>
+      <c r="B798" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C798" s="25"/>
+      <c r="D798" s="22"/>
+      <c r="E798" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F798" s="25"/>
+      <c r="G798" s="23" t="s">
+        <v>864</v>
+      </c>
+      <c r="H798" s="23"/>
+      <c r="I798" s="23"/>
+      <c r="J798" s="22"/>
+      <c r="K798" s="22"/>
+      <c r="L798" s="22"/>
+      <c r="M798" s="1"/>
+      <c r="N798" s="1"/>
+      <c r="O798" s="1"/>
+    </row>
+    <row r="799" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A799" s="21"/>
+      <c r="B799" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C799" s="25"/>
+      <c r="D799" s="22"/>
+      <c r="E799" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F799" s="25"/>
+      <c r="G799" s="23" t="s">
+        <v>865</v>
+      </c>
+      <c r="H799" s="23"/>
+      <c r="I799" s="23"/>
+      <c r="J799" s="22"/>
+      <c r="K799" s="22"/>
+      <c r="L799" s="22"/>
+      <c r="M799" s="1"/>
+      <c r="N799" s="1"/>
+      <c r="O799" s="1"/>
+    </row>
+    <row r="800" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A800" s="21"/>
+      <c r="B800" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C800" s="25"/>
+      <c r="D800" s="22"/>
+      <c r="E800" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F800" s="25"/>
+      <c r="G800" s="23" t="s">
+        <v>866</v>
+      </c>
+      <c r="H800" s="23"/>
+      <c r="I800" s="23"/>
+      <c r="J800" s="22"/>
+      <c r="K800" s="22"/>
+      <c r="L800" s="22"/>
+      <c r="M800" s="1"/>
+      <c r="N800" s="1"/>
+      <c r="O800" s="1"/>
     </row>
     <row r="801" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A801" s="21" t="s">
-        <v>861</v>
-      </c>
+      <c r="A801" s="21"/>
       <c r="B801" s="22" t="s">
         <v>22</v>
       </c>
@@ -18660,15 +18809,19 @@
       </c>
       <c r="F801" s="25"/>
       <c r="G801" s="23" t="s">
-        <v>862</v>
+        <v>867</v>
       </c>
       <c r="H801" s="23"/>
       <c r="I801" s="23"/>
       <c r="J801" s="22"/>
       <c r="K801" s="22"/>
       <c r="L801" s="22"/>
-    </row>
-    <row r="802" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M801" s="1"/>
+      <c r="N801" s="1"/>
+      <c r="O801" s="1"/>
+    </row>
+    <row r="802" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A802" s="21"/>
       <c r="B802" s="22" t="s">
         <v>22</v>
       </c>
@@ -18679,282 +18832,260 @@
       </c>
       <c r="F802" s="25"/>
       <c r="G802" s="23" t="s">
-        <v>863</v>
+        <v>868</v>
       </c>
       <c r="H802" s="23"/>
       <c r="I802" s="23"/>
       <c r="J802" s="22"/>
       <c r="K802" s="22"/>
       <c r="L802" s="22"/>
-    </row>
-    <row r="803" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A803" s="19"/>
-      <c r="B803" s="44"/>
-      <c r="C803" s="4"/>
-      <c r="D803" s="4"/>
-      <c r="E803" s="4"/>
-      <c r="F803" s="4"/>
-    </row>
-    <row r="804" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B804" s="46"/>
-      <c r="C804" s="1"/>
-      <c r="D804" s="1"/>
-      <c r="E804" s="1"/>
-      <c r="F804" s="1"/>
-      <c r="G804" s="1"/>
-      <c r="H804" s="1"/>
-      <c r="I804" s="1"/>
-      <c r="J804" s="1"/>
-      <c r="K804" s="1"/>
-      <c r="L804" s="1"/>
-    </row>
-    <row r="805" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A805" s="19"/>
-      <c r="B805" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C805" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D805" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E805" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F805" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G805" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H805" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I805" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J805" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="K805" s="11" t="s">
-        <v>691</v>
-      </c>
-      <c r="L805" s="11" t="s">
-        <v>692</v>
-      </c>
+      <c r="M802" s="1"/>
+      <c r="N802" s="1"/>
+      <c r="O802" s="1"/>
+    </row>
+    <row r="803" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A803" s="21"/>
+      <c r="B803" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C803" s="25"/>
+      <c r="D803" s="22"/>
+      <c r="E803" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F803" s="25"/>
+      <c r="G803" s="23" t="s">
+        <v>869</v>
+      </c>
+      <c r="H803" s="23"/>
+      <c r="I803" s="23"/>
+      <c r="J803" s="22"/>
+      <c r="K803" s="22"/>
+      <c r="L803" s="22"/>
+      <c r="M803" s="1"/>
+      <c r="N803" s="1"/>
+      <c r="O803" s="1"/>
+    </row>
+    <row r="804" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A804" s="21"/>
+      <c r="B804" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C804" s="25"/>
+      <c r="D804" s="22"/>
+      <c r="E804" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F804" s="25"/>
+      <c r="G804" s="23" t="s">
+        <v>870</v>
+      </c>
+      <c r="H804" s="23"/>
+      <c r="I804" s="23"/>
+      <c r="J804" s="22"/>
+      <c r="K804" s="22"/>
+      <c r="L804" s="22"/>
+      <c r="M804" s="1"/>
+      <c r="N804" s="1"/>
+      <c r="O804" s="1"/>
+    </row>
+    <row r="805" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A805" s="21"/>
+      <c r="B805" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C805" s="25"/>
+      <c r="D805" s="22"/>
+      <c r="E805" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F805" s="25"/>
+      <c r="G805" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="H805" s="23"/>
+      <c r="I805" s="23"/>
+      <c r="J805" s="22"/>
+      <c r="K805" s="22"/>
+      <c r="L805" s="22"/>
+      <c r="M805" s="1"/>
+      <c r="N805" s="1"/>
+      <c r="O805" s="1"/>
     </row>
     <row r="806" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A806" s="21" t="s">
-        <v>864</v>
-      </c>
+      <c r="A806" s="21"/>
       <c r="B806" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C806" s="25"/>
-      <c r="D806" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D806" s="22"/>
       <c r="E806" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F806" s="25"/>
       <c r="G806" s="23" t="s">
-        <v>865</v>
+        <v>872</v>
       </c>
       <c r="H806" s="23"/>
       <c r="I806" s="23"/>
       <c r="J806" s="22"/>
       <c r="K806" s="22"/>
       <c r="L806" s="22"/>
-    </row>
-    <row r="807" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B807" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C807" s="25"/>
-      <c r="D807" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E807" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F807" s="25"/>
-      <c r="G807" s="23" t="s">
-        <v>866</v>
-      </c>
+      <c r="M806" s="1"/>
+      <c r="N806" s="1"/>
+      <c r="O806" s="1"/>
+    </row>
+    <row r="807" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A807" s="21"/>
+      <c r="B807" s="22"/>
+      <c r="C807" s="22"/>
+      <c r="D807" s="22"/>
+      <c r="E807" s="22"/>
+      <c r="F807" s="22"/>
+      <c r="G807" s="23"/>
       <c r="H807" s="23"/>
       <c r="I807" s="23"/>
       <c r="J807" s="22"/>
       <c r="K807" s="22"/>
       <c r="L807" s="22"/>
+      <c r="M807" s="1"/>
+      <c r="N807" s="1"/>
+      <c r="O807" s="1"/>
     </row>
     <row r="808" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B808" s="1"/>
-      <c r="C808" s="1"/>
-      <c r="D808" s="1"/>
-      <c r="E808" s="1"/>
-      <c r="F808" s="1"/>
-      <c r="G808" s="1"/>
-      <c r="H808" s="1"/>
-      <c r="I808" s="1"/>
-      <c r="J808" s="1"/>
-      <c r="K808" s="1"/>
-      <c r="L808" s="1"/>
+      <c r="A808" s="21"/>
+      <c r="B808" s="22"/>
+      <c r="C808" s="22"/>
+      <c r="D808" s="22"/>
+      <c r="E808" s="22"/>
+      <c r="F808" s="22"/>
+      <c r="G808" s="23"/>
+      <c r="H808" s="23"/>
+      <c r="I808" s="23"/>
+      <c r="J808" s="22"/>
+      <c r="K808" s="22"/>
+      <c r="L808" s="22"/>
       <c r="M808" s="1"/>
       <c r="N808" s="1"/>
+      <c r="O808" s="1"/>
     </row>
     <row r="809" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B809" s="46"/>
-      <c r="C809" s="1"/>
-      <c r="D809" s="1"/>
-      <c r="E809" s="1"/>
-      <c r="F809" s="1"/>
+      <c r="A809" s="19"/>
+      <c r="B809" s="19"/>
+      <c r="C809" s="19"/>
+      <c r="D809" s="19"/>
+      <c r="E809" s="19"/>
+      <c r="F809" s="19"/>
       <c r="G809" s="1"/>
       <c r="H809" s="1"/>
       <c r="I809" s="1"/>
       <c r="J809" s="1"/>
       <c r="K809" s="1"/>
       <c r="L809" s="1"/>
-    </row>
-    <row r="810" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M809" s="1"/>
+      <c r="N809" s="1"/>
+      <c r="O809" s="1"/>
+    </row>
+    <row r="810" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A810" s="19"/>
-      <c r="B810" s="11" t="s">
+      <c r="B810" s="44"/>
+      <c r="C810" s="4"/>
+      <c r="D810" s="4"/>
+      <c r="E810" s="4"/>
+      <c r="F810" s="4"/>
+    </row>
+    <row r="811" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A811" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B811" s="43"/>
+      <c r="C811" s="18"/>
+      <c r="D811" s="18"/>
+      <c r="E811" s="18"/>
+      <c r="F811" s="18"/>
+    </row>
+    <row r="812" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A812" s="16" t="s">
+        <v>873</v>
+      </c>
+      <c r="B812" s="43"/>
+      <c r="C812" s="18"/>
+      <c r="D812" s="18"/>
+      <c r="E812" s="18"/>
+      <c r="F812" s="18"/>
+    </row>
+    <row r="813" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A813" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B813" s="43"/>
+      <c r="C813" s="18"/>
+      <c r="D813" s="18"/>
+      <c r="E813" s="18"/>
+      <c r="F813" s="18"/>
+      <c r="H813" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="814" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A814" s="19"/>
+      <c r="B814" s="19"/>
+      <c r="C814" s="19"/>
+      <c r="D814" s="19"/>
+      <c r="E814" s="19"/>
+      <c r="F814" s="19"/>
+    </row>
+    <row r="815" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A815" s="19"/>
+      <c r="B815" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C810" s="11" t="s">
+      <c r="C815" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D810" s="11" t="s">
+      <c r="D815" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E810" s="11" t="s">
+      <c r="E815" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F810" s="11" t="s">
+      <c r="F815" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G810" s="20" t="s">
+      <c r="G815" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H810" s="20" t="s">
+      <c r="H815" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I810" s="20" t="s">
+      <c r="I815" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J810" s="11" t="s">
+      <c r="J815" s="11" t="s">
         <v>690</v>
       </c>
-      <c r="K810" s="11" t="s">
+      <c r="K815" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="L810" s="11" t="s">
+      <c r="L815" s="11" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="811" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A811" s="21" t="s">
-        <v>867</v>
-      </c>
-      <c r="B811" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C811" s="25"/>
-      <c r="D811" s="22"/>
-      <c r="E811" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F811" s="25"/>
-      <c r="G811" s="23" t="s">
-        <v>868</v>
-      </c>
-      <c r="H811" s="23"/>
-      <c r="I811" s="23"/>
-      <c r="J811" s="22"/>
-      <c r="K811" s="22"/>
-      <c r="L811" s="22"/>
-    </row>
-    <row r="812" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B812" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C812" s="25"/>
-      <c r="D812" s="22"/>
-      <c r="E812" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F812" s="25"/>
-      <c r="G812" s="23" t="s">
-        <v>869</v>
-      </c>
-      <c r="H812" s="23"/>
-      <c r="I812" s="23"/>
-      <c r="J812" s="22"/>
-      <c r="K812" s="22"/>
-      <c r="L812" s="22"/>
-    </row>
-    <row r="813" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B813" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C813" s="25"/>
-      <c r="D813" s="22"/>
-      <c r="E813" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F813" s="25"/>
-      <c r="G813" s="23" t="s">
-        <v>870</v>
-      </c>
-      <c r="H813" s="23"/>
-      <c r="I813" s="23"/>
-      <c r="J813" s="22"/>
-      <c r="K813" s="22"/>
-      <c r="L813" s="22"/>
-    </row>
-    <row r="814" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B814" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C814" s="25"/>
-      <c r="D814" s="22"/>
-      <c r="E814" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F814" s="25"/>
-      <c r="G814" s="23" t="s">
-        <v>871</v>
-      </c>
-      <c r="H814" s="23"/>
-      <c r="I814" s="23"/>
-      <c r="J814" s="22"/>
-      <c r="K814" s="22"/>
-      <c r="L814" s="22"/>
-    </row>
-    <row r="815" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B815" s="25"/>
-      <c r="C815" s="25"/>
-      <c r="D815" s="22"/>
-      <c r="E815" s="22"/>
-      <c r="F815" s="25"/>
-      <c r="G815" s="23" t="s">
-        <v>872</v>
-      </c>
-      <c r="H815" s="23"/>
-      <c r="I815" s="23"/>
-      <c r="J815" s="22"/>
-      <c r="K815" s="22"/>
-      <c r="L815" s="22"/>
-    </row>
     <row r="816" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B816" s="25"/>
+      <c r="A816" s="21" t="s">
+        <v>874</v>
+      </c>
+      <c r="B816" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C816" s="25"/>
       <c r="D816" s="22"/>
-      <c r="E816" s="22"/>
+      <c r="E816" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F816" s="25"/>
       <c r="G816" s="23" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="H816" s="23"/>
       <c r="I816" s="23"/>
@@ -18962,14 +19093,18 @@
       <c r="K816" s="22"/>
       <c r="L816" s="22"/>
     </row>
-    <row r="817" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B817" s="25"/>
+    <row r="817" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B817" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C817" s="25"/>
       <c r="D817" s="22"/>
-      <c r="E817" s="22"/>
+      <c r="E817" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F817" s="25"/>
       <c r="G817" s="23" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="H817" s="23"/>
       <c r="I817" s="23"/>
@@ -18977,52 +19112,67 @@
       <c r="K817" s="22"/>
       <c r="L817" s="22"/>
     </row>
-    <row r="818" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B818" s="25"/>
-      <c r="C818" s="25"/>
-      <c r="D818" s="22"/>
-      <c r="E818" s="22"/>
-      <c r="F818" s="25"/>
-      <c r="G818" s="23" t="s">
-        <v>875</v>
-      </c>
-      <c r="H818" s="23"/>
-      <c r="I818" s="23"/>
-      <c r="J818" s="22"/>
-      <c r="K818" s="22"/>
-      <c r="L818" s="22"/>
-    </row>
-    <row r="819" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B819" s="25"/>
-      <c r="C819" s="25"/>
-      <c r="D819" s="22"/>
-      <c r="E819" s="22"/>
-      <c r="F819" s="25"/>
-      <c r="G819" s="23" t="s">
-        <v>876</v>
-      </c>
-      <c r="H819" s="23"/>
-      <c r="I819" s="23"/>
-      <c r="J819" s="22"/>
-      <c r="K819" s="22"/>
-      <c r="L819" s="22"/>
-    </row>
-    <row r="820" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B820" s="25"/>
-      <c r="C820" s="25"/>
-      <c r="D820" s="22"/>
-      <c r="E820" s="22"/>
-      <c r="F820" s="25"/>
-      <c r="G820" s="23" t="s">
+    <row r="818" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A818" s="19"/>
+      <c r="B818" s="44"/>
+      <c r="C818" s="4"/>
+      <c r="D818" s="4"/>
+      <c r="E818" s="4"/>
+      <c r="F818" s="4"/>
+    </row>
+    <row r="819" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B819" s="46"/>
+      <c r="C819" s="1"/>
+      <c r="D819" s="1"/>
+      <c r="E819" s="1"/>
+      <c r="F819" s="1"/>
+      <c r="G819" s="1"/>
+      <c r="H819" s="1"/>
+      <c r="I819" s="1"/>
+      <c r="J819" s="1"/>
+      <c r="K819" s="1"/>
+      <c r="L819" s="1"/>
+    </row>
+    <row r="820" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A820" s="19"/>
+      <c r="B820" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C820" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D820" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E820" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F820" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G820" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H820" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I820" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J820" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K820" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L820" s="11" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="821" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A821" s="21" t="s">
         <v>877</v>
       </c>
-      <c r="H820" s="23"/>
-      <c r="I820" s="23"/>
-      <c r="J820" s="22"/>
-      <c r="K820" s="22"/>
-      <c r="L820" s="22"/>
-    </row>
-    <row r="821" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B821" s="22" t="s">
         <v>22</v>
       </c>
@@ -19043,13 +19193,21 @@
       <c r="K821" s="22"/>
       <c r="L821" s="22"/>
     </row>
-    <row r="822" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B822" s="22"/>
-      <c r="C822" s="22"/>
-      <c r="D822" s="22"/>
-      <c r="E822" s="22"/>
-      <c r="F822" s="22"/>
-      <c r="G822" s="23"/>
+    <row r="822" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B822" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C822" s="25"/>
+      <c r="D822" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E822" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F822" s="25"/>
+      <c r="G822" s="23" t="s">
+        <v>879</v>
+      </c>
       <c r="H822" s="23"/>
       <c r="I822" s="23"/>
       <c r="J822" s="22"/>
@@ -19072,136 +19230,141 @@
       <c r="N823" s="1"/>
     </row>
     <row r="824" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A824" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B824" s="17"/>
-      <c r="C824" s="18"/>
-      <c r="D824" s="18"/>
-      <c r="E824" s="18"/>
-      <c r="F824" s="18"/>
+      <c r="B824" s="46"/>
+      <c r="C824" s="1"/>
+      <c r="D824" s="1"/>
+      <c r="E824" s="1"/>
+      <c r="F824" s="1"/>
       <c r="G824" s="1"/>
       <c r="H824" s="1"/>
       <c r="I824" s="1"/>
       <c r="J824" s="1"/>
       <c r="K824" s="1"/>
       <c r="L824" s="1"/>
-      <c r="M824" s="1"/>
-      <c r="N824" s="1"/>
-    </row>
-    <row r="825" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A825" s="16" t="s">
-        <v>879</v>
-      </c>
-      <c r="B825" s="17"/>
-      <c r="C825" s="18"/>
-      <c r="D825" s="18"/>
-      <c r="E825" s="18"/>
-      <c r="F825" s="18"/>
-      <c r="G825" s="1"/>
-      <c r="H825" s="1"/>
-      <c r="I825" s="1"/>
-      <c r="J825" s="1"/>
-      <c r="K825" s="1"/>
-      <c r="L825" s="1"/>
-      <c r="M825" s="1"/>
-      <c r="N825" s="1"/>
-    </row>
-    <row r="826" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A826" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B826" s="17"/>
-      <c r="C826" s="18"/>
-      <c r="D826" s="18"/>
-      <c r="E826" s="18"/>
-      <c r="F826" s="18"/>
-      <c r="G826" s="1"/>
-      <c r="H826" s="1"/>
-      <c r="I826" s="1"/>
-      <c r="J826" s="1"/>
-      <c r="K826" s="1"/>
-      <c r="L826" s="1"/>
-      <c r="M826" s="1"/>
-      <c r="N826" s="1"/>
-    </row>
-    <row r="827" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B827" s="1"/>
-      <c r="C827" s="1"/>
-      <c r="D827" s="1"/>
-      <c r="E827" s="1"/>
-      <c r="F827" s="1"/>
-      <c r="G827" s="1"/>
-      <c r="H827" s="1"/>
-      <c r="I827" s="1"/>
-      <c r="J827" s="1"/>
-      <c r="K827" s="1"/>
-      <c r="L827" s="1"/>
-      <c r="M827" s="1"/>
-      <c r="N827" s="1"/>
-    </row>
-    <row r="828" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B828" s="46"/>
-      <c r="C828" s="1"/>
-      <c r="D828" s="1"/>
-      <c r="E828" s="1"/>
-      <c r="F828" s="1"/>
-      <c r="G828" s="1"/>
-      <c r="H828" s="1"/>
-      <c r="I828" s="1"/>
-      <c r="J828" s="1"/>
-      <c r="K828" s="1"/>
-      <c r="L828" s="1"/>
-    </row>
-    <row r="829" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A829" s="19"/>
-      <c r="B829" s="11" t="s">
+    </row>
+    <row r="825" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A825" s="19"/>
+      <c r="B825" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C829" s="11" t="s">
+      <c r="C825" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D829" s="11" t="s">
+      <c r="D825" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E829" s="11" t="s">
+      <c r="E825" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F829" s="11" t="s">
+      <c r="F825" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G829" s="20" t="s">
+      <c r="G825" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H829" s="20" t="s">
+      <c r="H825" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I829" s="20" t="s">
+      <c r="I825" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J829" s="11" t="s">
+      <c r="J825" s="11" t="s">
         <v>690</v>
       </c>
-      <c r="K829" s="11" t="s">
+      <c r="K825" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="L829" s="11" t="s">
+      <c r="L825" s="11" t="s">
         <v>692</v>
       </c>
     </row>
+    <row r="826" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A826" s="21" t="s">
+        <v>880</v>
+      </c>
+      <c r="B826" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C826" s="25"/>
+      <c r="D826" s="22"/>
+      <c r="E826" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F826" s="25"/>
+      <c r="G826" s="23" t="s">
+        <v>881</v>
+      </c>
+      <c r="H826" s="23"/>
+      <c r="I826" s="23"/>
+      <c r="J826" s="22"/>
+      <c r="K826" s="22"/>
+      <c r="L826" s="22"/>
+    </row>
+    <row r="827" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B827" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C827" s="25"/>
+      <c r="D827" s="22"/>
+      <c r="E827" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F827" s="25"/>
+      <c r="G827" s="23" t="s">
+        <v>882</v>
+      </c>
+      <c r="H827" s="23"/>
+      <c r="I827" s="23"/>
+      <c r="J827" s="22"/>
+      <c r="K827" s="22"/>
+      <c r="L827" s="22"/>
+    </row>
+    <row r="828" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B828" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C828" s="25"/>
+      <c r="D828" s="22"/>
+      <c r="E828" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F828" s="25"/>
+      <c r="G828" s="23" t="s">
+        <v>883</v>
+      </c>
+      <c r="H828" s="23"/>
+      <c r="I828" s="23"/>
+      <c r="J828" s="22"/>
+      <c r="K828" s="22"/>
+      <c r="L828" s="22"/>
+    </row>
+    <row r="829" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B829" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C829" s="25"/>
+      <c r="D829" s="22"/>
+      <c r="E829" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F829" s="25"/>
+      <c r="G829" s="23" t="s">
+        <v>884</v>
+      </c>
+      <c r="H829" s="23"/>
+      <c r="I829" s="23"/>
+      <c r="J829" s="22"/>
+      <c r="K829" s="22"/>
+      <c r="L829" s="22"/>
+    </row>
     <row r="830" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A830" s="21" t="s">
-        <v>880</v>
-      </c>
-      <c r="B830" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B830" s="25"/>
       <c r="C830" s="25"/>
       <c r="D830" s="22"/>
       <c r="E830" s="22"/>
       <c r="F830" s="25"/>
       <c r="G830" s="23" t="s">
-        <v>881</v>
+        <v>885</v>
       </c>
       <c r="H830" s="23"/>
       <c r="I830" s="23"/>
@@ -19210,15 +19373,13 @@
       <c r="L830" s="22"/>
     </row>
     <row r="831" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B831" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B831" s="25"/>
       <c r="C831" s="25"/>
       <c r="D831" s="22"/>
       <c r="E831" s="22"/>
       <c r="F831" s="25"/>
       <c r="G831" s="23" t="s">
-        <v>882</v>
+        <v>886</v>
       </c>
       <c r="H831" s="23"/>
       <c r="I831" s="23"/>
@@ -19227,15 +19388,13 @@
       <c r="L831" s="22"/>
     </row>
     <row r="832" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B832" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B832" s="25"/>
       <c r="C832" s="25"/>
       <c r="D832" s="22"/>
       <c r="E832" s="22"/>
       <c r="F832" s="25"/>
       <c r="G832" s="23" t="s">
-        <v>883</v>
+        <v>887</v>
       </c>
       <c r="H832" s="23"/>
       <c r="I832" s="23"/>
@@ -19244,15 +19403,13 @@
       <c r="L832" s="22"/>
     </row>
     <row r="833" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B833" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B833" s="25"/>
       <c r="C833" s="25"/>
       <c r="D833" s="22"/>
       <c r="E833" s="22"/>
       <c r="F833" s="25"/>
       <c r="G833" s="23" t="s">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="H833" s="23"/>
       <c r="I833" s="23"/>
@@ -19267,7 +19424,7 @@
       <c r="E834" s="22"/>
       <c r="F834" s="25"/>
       <c r="G834" s="23" t="s">
-        <v>885</v>
+        <v>889</v>
       </c>
       <c r="H834" s="23"/>
       <c r="I834" s="23"/>
@@ -19282,7 +19439,7 @@
       <c r="E835" s="22"/>
       <c r="F835" s="25"/>
       <c r="G835" s="23" t="s">
-        <v>886</v>
+        <v>890</v>
       </c>
       <c r="H835" s="23"/>
       <c r="I835" s="23"/>
@@ -19290,16 +19447,20 @@
       <c r="K835" s="22"/>
       <c r="L835" s="22"/>
     </row>
-    <row r="836" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="836" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B836" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C836" s="25"/>
-      <c r="D836" s="22"/>
-      <c r="E836" s="22"/>
+      <c r="D836" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E836" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F836" s="25"/>
       <c r="G836" s="23" t="s">
-        <v>887</v>
+        <v>891</v>
       </c>
       <c r="H836" s="23"/>
       <c r="I836" s="23"/>
@@ -19307,98 +19468,105 @@
       <c r="K836" s="22"/>
       <c r="L836" s="22"/>
     </row>
-    <row r="837" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B837" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C837" s="25"/>
+    <row r="837" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B837" s="22"/>
+      <c r="C837" s="22"/>
       <c r="D837" s="22"/>
       <c r="E837" s="22"/>
-      <c r="F837" s="25"/>
-      <c r="G837" s="23" t="s">
-        <v>888</v>
-      </c>
+      <c r="F837" s="22"/>
+      <c r="G837" s="23"/>
       <c r="H837" s="23"/>
       <c r="I837" s="23"/>
       <c r="J837" s="22"/>
       <c r="K837" s="22"/>
       <c r="L837" s="22"/>
     </row>
-    <row r="838" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B838" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C838" s="25"/>
-      <c r="D838" s="22"/>
-      <c r="E838" s="22"/>
-      <c r="F838" s="25"/>
-      <c r="G838" s="23" t="s">
-        <v>889</v>
-      </c>
-      <c r="H838" s="23"/>
-      <c r="I838" s="23"/>
-      <c r="J838" s="22"/>
-      <c r="K838" s="22"/>
-      <c r="L838" s="22"/>
-    </row>
-    <row r="839" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B839" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C839" s="25"/>
-      <c r="D839" s="22"/>
-      <c r="E839" s="22"/>
-      <c r="F839" s="25"/>
-      <c r="G839" s="23" t="s">
-        <v>890</v>
-      </c>
-      <c r="H839" s="23"/>
-      <c r="I839" s="23"/>
-      <c r="J839" s="22"/>
-      <c r="K839" s="22"/>
-      <c r="L839" s="22"/>
+    <row r="838" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B838" s="1"/>
+      <c r="C838" s="1"/>
+      <c r="D838" s="1"/>
+      <c r="E838" s="1"/>
+      <c r="F838" s="1"/>
+      <c r="G838" s="1"/>
+      <c r="H838" s="1"/>
+      <c r="I838" s="1"/>
+      <c r="J838" s="1"/>
+      <c r="K838" s="1"/>
+      <c r="L838" s="1"/>
+      <c r="M838" s="1"/>
+      <c r="N838" s="1"/>
+    </row>
+    <row r="839" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A839" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B839" s="17"/>
+      <c r="C839" s="18"/>
+      <c r="D839" s="18"/>
+      <c r="E839" s="18"/>
+      <c r="F839" s="18"/>
+      <c r="G839" s="1"/>
+      <c r="H839" s="1"/>
+      <c r="I839" s="1"/>
+      <c r="J839" s="1"/>
+      <c r="K839" s="1"/>
+      <c r="L839" s="1"/>
+      <c r="M839" s="1"/>
+      <c r="N839" s="1"/>
     </row>
     <row r="840" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B840" s="22"/>
-      <c r="C840" s="22"/>
-      <c r="D840" s="22"/>
-      <c r="E840" s="22"/>
-      <c r="F840" s="22"/>
-      <c r="G840" s="23"/>
-      <c r="H840" s="23"/>
-      <c r="I840" s="23"/>
-      <c r="J840" s="22"/>
-      <c r="K840" s="22"/>
-      <c r="L840" s="22"/>
+      <c r="A840" s="16" t="s">
+        <v>892</v>
+      </c>
+      <c r="B840" s="17"/>
+      <c r="C840" s="18"/>
+      <c r="D840" s="18"/>
+      <c r="E840" s="18"/>
+      <c r="F840" s="18"/>
+      <c r="G840" s="1"/>
+      <c r="H840" s="1"/>
+      <c r="I840" s="1"/>
+      <c r="J840" s="1"/>
+      <c r="K840" s="1"/>
+      <c r="L840" s="1"/>
+      <c r="M840" s="1"/>
+      <c r="N840" s="1"/>
     </row>
     <row r="841" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B841" s="22"/>
-      <c r="C841" s="22"/>
-      <c r="D841" s="22"/>
-      <c r="E841" s="22"/>
-      <c r="F841" s="22"/>
-      <c r="G841" s="23"/>
-      <c r="H841" s="23"/>
-      <c r="I841" s="23"/>
-      <c r="J841" s="22"/>
-      <c r="K841" s="22"/>
-      <c r="L841" s="22"/>
+      <c r="A841" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B841" s="17"/>
+      <c r="C841" s="18"/>
+      <c r="D841" s="18"/>
+      <c r="E841" s="18"/>
+      <c r="F841" s="18"/>
+      <c r="G841" s="1"/>
+      <c r="H841" s="1"/>
+      <c r="I841" s="1"/>
+      <c r="J841" s="1"/>
+      <c r="K841" s="1"/>
+      <c r="L841" s="1"/>
+      <c r="M841" s="1"/>
+      <c r="N841" s="1"/>
     </row>
     <row r="842" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B842" s="22"/>
-      <c r="C842" s="22"/>
-      <c r="D842" s="22"/>
-      <c r="E842" s="22"/>
-      <c r="F842" s="22"/>
-      <c r="G842" s="23"/>
-      <c r="H842" s="23"/>
-      <c r="I842" s="23"/>
-      <c r="J842" s="22"/>
-      <c r="K842" s="22"/>
-      <c r="L842" s="22"/>
+      <c r="B842" s="1"/>
+      <c r="C842" s="1"/>
+      <c r="D842" s="1"/>
+      <c r="E842" s="1"/>
+      <c r="F842" s="1"/>
+      <c r="G842" s="1"/>
+      <c r="H842" s="1"/>
+      <c r="I842" s="1"/>
+      <c r="J842" s="1"/>
+      <c r="K842" s="1"/>
+      <c r="L842" s="1"/>
+      <c r="M842" s="1"/>
+      <c r="N842" s="1"/>
     </row>
     <row r="843" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B843" s="1"/>
+      <c r="B843" s="46"/>
       <c r="C843" s="1"/>
       <c r="D843" s="1"/>
       <c r="E843" s="1"/>
@@ -19409,472 +19577,442 @@
       <c r="J843" s="1"/>
       <c r="K843" s="1"/>
       <c r="L843" s="1"/>
-      <c r="M843" s="1"/>
-      <c r="N843" s="1"/>
-    </row>
-    <row r="844" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B844" s="1"/>
-      <c r="C844" s="1"/>
-      <c r="D844" s="1"/>
-      <c r="E844" s="1"/>
-      <c r="F844" s="1"/>
-      <c r="G844" s="1"/>
-      <c r="H844" s="1"/>
-      <c r="I844" s="1"/>
-      <c r="J844" s="1"/>
-      <c r="K844" s="1"/>
-      <c r="L844" s="1"/>
-      <c r="M844" s="1"/>
-      <c r="N844" s="1"/>
-    </row>
-    <row r="845" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B845" s="1"/>
-      <c r="C845" s="1"/>
-      <c r="D845" s="1"/>
-      <c r="E845" s="1"/>
-      <c r="F845" s="1"/>
-      <c r="G845" s="1"/>
-      <c r="H845" s="1"/>
-      <c r="I845" s="1"/>
-      <c r="J845" s="1"/>
-      <c r="K845" s="1"/>
-      <c r="L845" s="1"/>
-      <c r="M845" s="1"/>
-      <c r="N845" s="1"/>
-    </row>
-    <row r="846" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B846" s="1"/>
-      <c r="C846" s="1"/>
-      <c r="D846" s="1"/>
-      <c r="E846" s="1"/>
-      <c r="F846" s="1"/>
-      <c r="G846" s="1"/>
-      <c r="H846" s="1"/>
-      <c r="I846" s="1"/>
-      <c r="J846" s="1"/>
-      <c r="K846" s="1"/>
-      <c r="L846" s="1"/>
-      <c r="M846" s="1"/>
-      <c r="N846" s="1"/>
-    </row>
-    <row r="847" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B847" s="1"/>
-      <c r="C847" s="1"/>
-      <c r="D847" s="1"/>
-      <c r="E847" s="1"/>
-      <c r="F847" s="1"/>
-      <c r="G847" s="1"/>
-      <c r="H847" s="1"/>
-      <c r="I847" s="1"/>
-      <c r="J847" s="1"/>
-      <c r="K847" s="1"/>
-      <c r="L847" s="1"/>
-      <c r="M847" s="1"/>
-      <c r="N847" s="1"/>
-    </row>
-    <row r="848" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B848" s="1"/>
-      <c r="C848" s="1"/>
-      <c r="D848" s="1"/>
-      <c r="E848" s="1"/>
-      <c r="F848" s="1"/>
-      <c r="G848" s="1"/>
-      <c r="H848" s="1"/>
-      <c r="I848" s="1"/>
-      <c r="J848" s="1"/>
-      <c r="K848" s="1"/>
-      <c r="L848" s="1"/>
-      <c r="M848" s="1"/>
-      <c r="N848" s="1"/>
-    </row>
-    <row r="849" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B849" s="1"/>
-      <c r="C849" s="1"/>
-      <c r="D849" s="1"/>
-      <c r="E849" s="1"/>
-      <c r="F849" s="1"/>
-      <c r="G849" s="1"/>
-      <c r="H849" s="1"/>
-      <c r="I849" s="1"/>
-      <c r="J849" s="1"/>
-      <c r="K849" s="1"/>
-      <c r="L849" s="1"/>
-      <c r="M849" s="1"/>
-      <c r="N849" s="1"/>
-      <c r="O849" s="1"/>
-    </row>
-    <row r="850" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A850" s="9"/>
-    </row>
-    <row r="851" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A851" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B851" s="17"/>
-      <c r="C851" s="18"/>
-      <c r="D851" s="18"/>
-      <c r="E851" s="18"/>
-      <c r="F851" s="18"/>
-    </row>
-    <row r="852" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A852" s="16" t="s">
-        <v>891</v>
-      </c>
-      <c r="B852" s="17"/>
-      <c r="C852" s="18"/>
-      <c r="D852" s="18"/>
-      <c r="E852" s="18"/>
-      <c r="F852" s="18"/>
-    </row>
-    <row r="853" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A853" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B853" s="17"/>
-      <c r="C853" s="18"/>
-      <c r="D853" s="18"/>
-      <c r="E853" s="18"/>
-      <c r="F853" s="18"/>
-    </row>
-    <row r="854" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A854" s="9"/>
-      <c r="B854" s="11" t="s">
+    </row>
+    <row r="844" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A844" s="19"/>
+      <c r="B844" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C854" s="11" t="s">
+      <c r="C844" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D854" s="11" t="s">
+      <c r="D844" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E854" s="11" t="s">
+      <c r="E844" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F854" s="11" t="s">
+      <c r="F844" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G854" s="20" t="s">
+      <c r="G844" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H854" s="20" t="s">
+      <c r="H844" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I854" s="20" t="s">
+      <c r="I844" s="20" t="s">
         <v>20</v>
       </c>
+      <c r="J844" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K844" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L844" s="11" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="845" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A845" s="21" t="s">
+        <v>893</v>
+      </c>
+      <c r="B845" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C845" s="25"/>
+      <c r="D845" s="22"/>
+      <c r="E845" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F845" s="25"/>
+      <c r="G845" s="23" t="s">
+        <v>894</v>
+      </c>
+      <c r="H845" s="23"/>
+      <c r="I845" s="23"/>
+      <c r="J845" s="22"/>
+      <c r="K845" s="22"/>
+      <c r="L845" s="22"/>
+    </row>
+    <row r="846" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B846" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C846" s="25"/>
+      <c r="D846" s="22"/>
+      <c r="E846" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F846" s="25"/>
+      <c r="G846" s="23" t="s">
+        <v>895</v>
+      </c>
+      <c r="H846" s="23"/>
+      <c r="I846" s="23"/>
+      <c r="J846" s="22"/>
+      <c r="K846" s="22"/>
+      <c r="L846" s="22"/>
+    </row>
+    <row r="847" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B847" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C847" s="25"/>
+      <c r="D847" s="22"/>
+      <c r="E847" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F847" s="25"/>
+      <c r="G847" s="23" t="s">
+        <v>896</v>
+      </c>
+      <c r="H847" s="23"/>
+      <c r="I847" s="23"/>
+      <c r="J847" s="22"/>
+      <c r="K847" s="22"/>
+      <c r="L847" s="22"/>
+    </row>
+    <row r="848" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B848" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C848" s="25"/>
+      <c r="D848" s="22"/>
+      <c r="E848" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F848" s="25"/>
+      <c r="G848" s="23" t="s">
+        <v>897</v>
+      </c>
+      <c r="H848" s="23"/>
+      <c r="I848" s="23"/>
+      <c r="J848" s="22"/>
+      <c r="K848" s="22"/>
+      <c r="L848" s="22"/>
+    </row>
+    <row r="849" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B849" s="25"/>
+      <c r="C849" s="25"/>
+      <c r="D849" s="22"/>
+      <c r="E849" s="22"/>
+      <c r="F849" s="25"/>
+      <c r="G849" s="23" t="s">
+        <v>898</v>
+      </c>
+      <c r="H849" s="23"/>
+      <c r="I849" s="23"/>
+      <c r="J849" s="22"/>
+      <c r="K849" s="22"/>
+      <c r="L849" s="22"/>
+    </row>
+    <row r="850" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B850" s="25"/>
+      <c r="C850" s="25"/>
+      <c r="D850" s="22"/>
+      <c r="E850" s="22"/>
+      <c r="F850" s="25"/>
+      <c r="G850" s="23" t="s">
+        <v>899</v>
+      </c>
+      <c r="H850" s="23"/>
+      <c r="I850" s="23"/>
+      <c r="J850" s="22"/>
+      <c r="K850" s="22"/>
+      <c r="L850" s="22"/>
+    </row>
+    <row r="851" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B851" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C851" s="25"/>
+      <c r="D851" s="22"/>
+      <c r="E851" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F851" s="25"/>
+      <c r="G851" s="23" t="s">
+        <v>900</v>
+      </c>
+      <c r="H851" s="23"/>
+      <c r="I851" s="23"/>
+      <c r="J851" s="22"/>
+      <c r="K851" s="22"/>
+      <c r="L851" s="22"/>
+    </row>
+    <row r="852" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B852" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C852" s="25"/>
+      <c r="D852" s="22"/>
+      <c r="E852" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F852" s="25"/>
+      <c r="G852" s="23" t="s">
+        <v>901</v>
+      </c>
+      <c r="H852" s="23"/>
+      <c r="I852" s="23"/>
+      <c r="J852" s="22"/>
+      <c r="K852" s="22"/>
+      <c r="L852" s="22"/>
+    </row>
+    <row r="853" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B853" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C853" s="25"/>
+      <c r="D853" s="22"/>
+      <c r="E853" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F853" s="25"/>
+      <c r="G853" s="23" t="s">
+        <v>902</v>
+      </c>
+      <c r="H853" s="23"/>
+      <c r="I853" s="23"/>
+      <c r="J853" s="22"/>
+      <c r="K853" s="22"/>
+      <c r="L853" s="22"/>
+    </row>
+    <row r="854" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B854" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C854" s="25"/>
+      <c r="D854" s="22"/>
+      <c r="E854" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F854" s="25"/>
+      <c r="G854" s="23" t="s">
+        <v>903</v>
+      </c>
+      <c r="H854" s="23"/>
+      <c r="I854" s="23"/>
+      <c r="J854" s="22"/>
+      <c r="K854" s="22"/>
+      <c r="L854" s="22"/>
     </row>
     <row r="855" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A855" s="21" t="s">
-        <v>892</v>
-      </c>
-      <c r="B855" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C855" s="25"/>
+      <c r="B855" s="22"/>
+      <c r="C855" s="22"/>
       <c r="D855" s="22"/>
-      <c r="E855" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F855" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G855" s="23" t="s">
-        <v>893</v>
-      </c>
+      <c r="E855" s="22"/>
+      <c r="F855" s="22"/>
+      <c r="G855" s="23"/>
       <c r="H855" s="23"/>
       <c r="I855" s="23"/>
+      <c r="J855" s="22"/>
+      <c r="K855" s="22"/>
+      <c r="L855" s="22"/>
     </row>
     <row r="856" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A856" s="21"/>
-      <c r="B856" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C856" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D856" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E856" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F856" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G856" s="23" t="s">
-        <v>894</v>
-      </c>
+      <c r="B856" s="22"/>
+      <c r="C856" s="22"/>
+      <c r="D856" s="22"/>
+      <c r="E856" s="22"/>
+      <c r="F856" s="22"/>
+      <c r="G856" s="23"/>
       <c r="H856" s="23"/>
       <c r="I856" s="23"/>
+      <c r="J856" s="22"/>
+      <c r="K856" s="22"/>
+      <c r="L856" s="22"/>
     </row>
     <row r="857" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A857" s="9"/>
-      <c r="B857" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C857" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D857" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E857" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F857" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G857" s="23" t="s">
-        <v>895</v>
-      </c>
+      <c r="B857" s="22"/>
+      <c r="C857" s="22"/>
+      <c r="D857" s="22"/>
+      <c r="E857" s="22"/>
+      <c r="F857" s="22"/>
+      <c r="G857" s="23"/>
       <c r="H857" s="23"/>
       <c r="I857" s="23"/>
+      <c r="J857" s="22"/>
+      <c r="K857" s="22"/>
+      <c r="L857" s="22"/>
     </row>
     <row r="858" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A858" s="9"/>
-      <c r="B858" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C858" s="25"/>
-      <c r="D858" s="22"/>
-      <c r="E858" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F858" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G858" s="45" t="s">
-        <v>896</v>
-      </c>
-      <c r="H858" s="23"/>
-      <c r="I858" s="23"/>
+      <c r="B858" s="1"/>
+      <c r="C858" s="1"/>
+      <c r="D858" s="1"/>
+      <c r="E858" s="1"/>
+      <c r="F858" s="1"/>
+      <c r="G858" s="1"/>
+      <c r="H858" s="1"/>
+      <c r="I858" s="1"/>
+      <c r="J858" s="1"/>
+      <c r="K858" s="1"/>
+      <c r="L858" s="1"/>
+      <c r="M858" s="1"/>
+      <c r="N858" s="1"/>
     </row>
     <row r="859" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A859" s="9"/>
-      <c r="B859" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C859" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D859" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E859" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F859" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G859" s="23" t="s">
-        <v>897</v>
-      </c>
-      <c r="H859" s="23"/>
-      <c r="I859" s="23"/>
+      <c r="B859" s="1"/>
+      <c r="C859" s="1"/>
+      <c r="D859" s="1"/>
+      <c r="E859" s="1"/>
+      <c r="F859" s="1"/>
+      <c r="G859" s="1"/>
+      <c r="H859" s="1"/>
+      <c r="I859" s="1"/>
+      <c r="J859" s="1"/>
+      <c r="K859" s="1"/>
+      <c r="L859" s="1"/>
+      <c r="M859" s="1"/>
+      <c r="N859" s="1"/>
     </row>
     <row r="860" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A860" s="9"/>
-      <c r="B860" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C860" s="25"/>
-      <c r="D860" s="22"/>
-      <c r="E860" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F860" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G860" s="23" t="s">
-        <v>898</v>
-      </c>
-      <c r="H860" s="23"/>
-      <c r="I860" s="23"/>
+      <c r="B860" s="1"/>
+      <c r="C860" s="1"/>
+      <c r="D860" s="1"/>
+      <c r="E860" s="1"/>
+      <c r="F860" s="1"/>
+      <c r="G860" s="1"/>
+      <c r="H860" s="1"/>
+      <c r="I860" s="1"/>
+      <c r="J860" s="1"/>
+      <c r="K860" s="1"/>
+      <c r="L860" s="1"/>
+      <c r="M860" s="1"/>
+      <c r="N860" s="1"/>
     </row>
     <row r="861" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A861" s="9"/>
-      <c r="B861" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C861" s="25"/>
-      <c r="D861" s="22"/>
-      <c r="E861" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F861" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G861" s="23" t="s">
-        <v>899</v>
-      </c>
-      <c r="H861" s="23"/>
-      <c r="I861" s="23"/>
+      <c r="B861" s="1"/>
+      <c r="C861" s="1"/>
+      <c r="D861" s="1"/>
+      <c r="E861" s="1"/>
+      <c r="F861" s="1"/>
+      <c r="G861" s="1"/>
+      <c r="H861" s="1"/>
+      <c r="I861" s="1"/>
+      <c r="J861" s="1"/>
+      <c r="K861" s="1"/>
+      <c r="L861" s="1"/>
+      <c r="M861" s="1"/>
+      <c r="N861" s="1"/>
     </row>
     <row r="862" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A862" s="9"/>
-      <c r="B862" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C862" s="25"/>
-      <c r="D862" s="22"/>
-      <c r="E862" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F862" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G862" s="23" t="s">
-        <v>900</v>
-      </c>
-      <c r="H862" s="23"/>
-      <c r="I862" s="23"/>
-    </row>
-    <row r="863" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A863" s="9"/>
-      <c r="B863" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C863" s="25"/>
-      <c r="D863" s="22"/>
-      <c r="E863" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F863" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G863" s="23" t="s">
-        <v>901</v>
-      </c>
-      <c r="H863" s="23"/>
-      <c r="I863" s="23" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="864" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A864" s="9"/>
-      <c r="B864" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C864" s="25"/>
-      <c r="D864" s="22"/>
-      <c r="E864" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F864" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G864" s="23" t="s">
-        <v>902</v>
-      </c>
-      <c r="H864" s="23"/>
-      <c r="I864" s="23"/>
+      <c r="B862" s="1"/>
+      <c r="C862" s="1"/>
+      <c r="D862" s="1"/>
+      <c r="E862" s="1"/>
+      <c r="F862" s="1"/>
+      <c r="G862" s="1"/>
+      <c r="H862" s="1"/>
+      <c r="I862" s="1"/>
+      <c r="J862" s="1"/>
+      <c r="K862" s="1"/>
+      <c r="L862" s="1"/>
+      <c r="M862" s="1"/>
+      <c r="N862" s="1"/>
+    </row>
+    <row r="863" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B863" s="1"/>
+      <c r="C863" s="1"/>
+      <c r="D863" s="1"/>
+      <c r="E863" s="1"/>
+      <c r="F863" s="1"/>
+      <c r="G863" s="1"/>
+      <c r="H863" s="1"/>
+      <c r="I863" s="1"/>
+      <c r="J863" s="1"/>
+      <c r="K863" s="1"/>
+      <c r="L863" s="1"/>
+      <c r="M863" s="1"/>
+      <c r="N863" s="1"/>
+    </row>
+    <row r="864" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B864" s="1"/>
+      <c r="C864" s="1"/>
+      <c r="D864" s="1"/>
+      <c r="E864" s="1"/>
+      <c r="F864" s="1"/>
+      <c r="G864" s="1"/>
+      <c r="H864" s="1"/>
+      <c r="I864" s="1"/>
+      <c r="J864" s="1"/>
+      <c r="K864" s="1"/>
+      <c r="L864" s="1"/>
+      <c r="M864" s="1"/>
+      <c r="N864" s="1"/>
+      <c r="O864" s="1"/>
     </row>
     <row r="865" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A865" s="9"/>
-      <c r="B865" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C865" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D865" s="22"/>
-      <c r="E865" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F865" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G865" s="23" t="s">
-        <v>903</v>
-      </c>
-      <c r="H865" s="23"/>
-      <c r="I865" s="23"/>
-    </row>
-    <row r="866" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A866" s="9"/>
-      <c r="B866" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C866" s="25"/>
-      <c r="D866" s="22"/>
-      <c r="E866" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F866" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G866" s="23" t="s">
+    </row>
+    <row r="866" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A866" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B866" s="17"/>
+      <c r="C866" s="18"/>
+      <c r="D866" s="18"/>
+      <c r="E866" s="18"/>
+      <c r="F866" s="18"/>
+    </row>
+    <row r="867" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A867" s="16" t="s">
         <v>904</v>
       </c>
-      <c r="H866" s="23"/>
-      <c r="I866" s="23"/>
-    </row>
-    <row r="867" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A867" s="9"/>
-      <c r="B867" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C867" s="25"/>
-      <c r="D867" s="22"/>
-      <c r="E867" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F867" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G867" s="23" t="s">
+      <c r="B867" s="17"/>
+      <c r="C867" s="18"/>
+      <c r="D867" s="18"/>
+      <c r="E867" s="18"/>
+      <c r="F867" s="18"/>
+    </row>
+    <row r="868" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A868" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B868" s="17"/>
+      <c r="C868" s="18"/>
+      <c r="D868" s="18"/>
+      <c r="E868" s="18"/>
+      <c r="F868" s="18"/>
+    </row>
+    <row r="869" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A869" s="9"/>
+      <c r="B869" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C869" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D869" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E869" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F869" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G869" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H869" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I869" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="870" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A870" s="21" t="s">
         <v>905</v>
       </c>
-      <c r="H867" s="23"/>
-      <c r="I867" s="23"/>
-    </row>
-    <row r="868" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A868" s="9"/>
-      <c r="B868" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C868" s="25"/>
-      <c r="D868" s="22"/>
-      <c r="E868" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F868" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G868" s="23" t="s">
-        <v>906</v>
-      </c>
-      <c r="H868" s="23"/>
-      <c r="I868" s="23"/>
-    </row>
-    <row r="869" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A869" s="9"/>
-      <c r="B869" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C869" s="25"/>
-      <c r="D869" s="22"/>
-      <c r="E869" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F869" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G869" s="23" t="s">
-        <v>907</v>
-      </c>
-      <c r="H869" s="23"/>
-      <c r="I869" s="23"/>
-    </row>
-    <row r="870" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A870" s="9"/>
       <c r="B870" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C870" s="25"/>
-      <c r="D870" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D870" s="22"/>
       <c r="E870" s="22" t="s">
         <v>22</v>
       </c>
@@ -19882,13 +20020,13 @@
         <v>640</v>
       </c>
       <c r="G870" s="23" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="H870" s="23"/>
       <c r="I870" s="23"/>
     </row>
     <row r="871" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A871" s="9"/>
+      <c r="A871" s="21"/>
       <c r="B871" s="22" t="s">
         <v>22</v>
       </c>
@@ -19905,7 +20043,7 @@
         <v>640</v>
       </c>
       <c r="G871" s="23" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="H871" s="23"/>
       <c r="I871" s="23"/>
@@ -19928,7 +20066,7 @@
         <v>640</v>
       </c>
       <c r="G872" s="23" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="H872" s="23"/>
       <c r="I872" s="23"/>
@@ -19938,20 +20076,16 @@
       <c r="B873" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C873" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D873" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C873" s="25"/>
+      <c r="D873" s="22"/>
       <c r="E873" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F873" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="G873" s="23" t="s">
-        <v>911</v>
+      <c r="G873" s="45" t="s">
+        <v>909</v>
       </c>
       <c r="H873" s="23"/>
       <c r="I873" s="23"/>
@@ -19961,8 +20095,12 @@
       <c r="B874" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C874" s="25"/>
-      <c r="D874" s="22"/>
+      <c r="C874" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D874" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E874" s="22" t="s">
         <v>22</v>
       </c>
@@ -19970,7 +20108,7 @@
         <v>640</v>
       </c>
       <c r="G874" s="23" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="H874" s="23"/>
       <c r="I874" s="23"/>
@@ -19980,12 +20118,8 @@
       <c r="B875" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C875" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D875" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C875" s="25"/>
+      <c r="D875" s="22"/>
       <c r="E875" s="22" t="s">
         <v>22</v>
       </c>
@@ -19993,7 +20127,7 @@
         <v>640</v>
       </c>
       <c r="G875" s="23" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="H875" s="23"/>
       <c r="I875" s="23"/>
@@ -20003,12 +20137,8 @@
       <c r="B876" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C876" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D876" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C876" s="25"/>
+      <c r="D876" s="22"/>
       <c r="E876" s="22" t="s">
         <v>22</v>
       </c>
@@ -20016,7 +20146,7 @@
         <v>640</v>
       </c>
       <c r="G876" s="23" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="H876" s="23"/>
       <c r="I876" s="23"/>
@@ -20027,9 +20157,7 @@
         <v>22</v>
       </c>
       <c r="C877" s="25"/>
-      <c r="D877" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D877" s="22"/>
       <c r="E877" s="22" t="s">
         <v>22</v>
       </c>
@@ -20037,20 +20165,18 @@
         <v>640</v>
       </c>
       <c r="G877" s="23" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="H877" s="23"/>
       <c r="I877" s="23"/>
     </row>
-    <row r="878" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="878" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A878" s="9"/>
       <c r="B878" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C878" s="25"/>
-      <c r="D878" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D878" s="22"/>
       <c r="E878" s="22" t="s">
         <v>22</v>
       </c>
@@ -20058,10 +20184,12 @@
         <v>640</v>
       </c>
       <c r="G878" s="23" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="H878" s="23"/>
-      <c r="I878" s="23"/>
+      <c r="I878" s="23" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="879" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A879" s="9"/>
@@ -20077,7 +20205,7 @@
         <v>640</v>
       </c>
       <c r="G879" s="23" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="H879" s="23"/>
       <c r="I879" s="23"/>
@@ -20087,10 +20215,10 @@
       <c r="B880" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C880" s="25"/>
-      <c r="D880" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C880" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D880" s="22"/>
       <c r="E880" s="22" t="s">
         <v>22</v>
       </c>
@@ -20098,20 +20226,18 @@
         <v>640</v>
       </c>
       <c r="G880" s="23" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="H880" s="23"/>
       <c r="I880" s="23"/>
     </row>
-    <row r="881" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="881" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A881" s="9"/>
       <c r="B881" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C881" s="25"/>
-      <c r="D881" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D881" s="22"/>
       <c r="E881" s="22" t="s">
         <v>22</v>
       </c>
@@ -20119,20 +20245,18 @@
         <v>640</v>
       </c>
       <c r="G881" s="23" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="H881" s="23"/>
       <c r="I881" s="23"/>
     </row>
-    <row r="882" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="882" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A882" s="9"/>
       <c r="B882" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C882" s="25"/>
-      <c r="D882" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D882" s="22"/>
       <c r="E882" s="22" t="s">
         <v>22</v>
       </c>
@@ -20140,22 +20264,18 @@
         <v>640</v>
       </c>
       <c r="G882" s="23" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="H882" s="23"/>
       <c r="I882" s="23"/>
     </row>
-    <row r="883" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="883" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A883" s="9"/>
       <c r="B883" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C883" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D883" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C883" s="25"/>
+      <c r="D883" s="22"/>
       <c r="E883" s="22" t="s">
         <v>22</v>
       </c>
@@ -20163,22 +20283,18 @@
         <v>640</v>
       </c>
       <c r="G883" s="23" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="H883" s="23"/>
       <c r="I883" s="23"/>
     </row>
-    <row r="884" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="884" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A884" s="9"/>
       <c r="B884" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C884" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D884" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C884" s="25"/>
+      <c r="D884" s="22"/>
       <c r="E884" s="22" t="s">
         <v>22</v>
       </c>
@@ -20186,18 +20302,20 @@
         <v>640</v>
       </c>
       <c r="G884" s="23" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="H884" s="23"/>
       <c r="I884" s="23"/>
     </row>
-    <row r="885" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="885" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A885" s="9"/>
       <c r="B885" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C885" s="25"/>
-      <c r="D885" s="22"/>
+      <c r="D885" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E885" s="22" t="s">
         <v>22</v>
       </c>
@@ -20205,7 +20323,7 @@
         <v>640</v>
       </c>
       <c r="G885" s="23" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="H885" s="23"/>
       <c r="I885" s="23"/>
@@ -20228,7 +20346,7 @@
         <v>640</v>
       </c>
       <c r="G886" s="23" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="H886" s="23"/>
       <c r="I886" s="23"/>
@@ -20251,7 +20369,7 @@
         <v>640</v>
       </c>
       <c r="G887" s="23" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="H887" s="23"/>
       <c r="I887" s="23"/>
@@ -20274,7 +20392,7 @@
         <v>640</v>
       </c>
       <c r="G888" s="23" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="H888" s="23"/>
       <c r="I888" s="23"/>
@@ -20293,7 +20411,7 @@
         <v>640</v>
       </c>
       <c r="G889" s="23" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="H889" s="23"/>
       <c r="I889" s="23"/>
@@ -20316,7 +20434,7 @@
         <v>640</v>
       </c>
       <c r="G890" s="23" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="H890" s="23"/>
       <c r="I890" s="23"/>
@@ -20339,7 +20457,7 @@
         <v>640</v>
       </c>
       <c r="G891" s="23" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="H891" s="23"/>
       <c r="I891" s="23"/>
@@ -20349,9 +20467,7 @@
       <c r="B892" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C892" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C892" s="25"/>
       <c r="D892" s="22" t="s">
         <v>22</v>
       </c>
@@ -20362,7 +20478,7 @@
         <v>640</v>
       </c>
       <c r="G892" s="23" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="H892" s="23"/>
       <c r="I892" s="23"/>
@@ -20372,9 +20488,7 @@
       <c r="B893" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C893" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C893" s="25"/>
       <c r="D893" s="22" t="s">
         <v>22</v>
       </c>
@@ -20385,22 +20499,18 @@
         <v>640</v>
       </c>
       <c r="G893" s="23" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="H893" s="23"/>
       <c r="I893" s="23"/>
     </row>
-    <row r="894" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="894" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A894" s="9"/>
       <c r="B894" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C894" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D894" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C894" s="25"/>
+      <c r="D894" s="22"/>
       <c r="E894" s="22" t="s">
         <v>22</v>
       </c>
@@ -20408,7 +20518,7 @@
         <v>640</v>
       </c>
       <c r="G894" s="23" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="H894" s="23"/>
       <c r="I894" s="23"/>
@@ -20419,7 +20529,9 @@
         <v>22</v>
       </c>
       <c r="C895" s="25"/>
-      <c r="D895" s="22"/>
+      <c r="D895" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E895" s="22" t="s">
         <v>22</v>
       </c>
@@ -20427,7 +20539,7 @@
         <v>640</v>
       </c>
       <c r="G895" s="23" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="H895" s="23"/>
       <c r="I895" s="23"/>
@@ -20437,9 +20549,7 @@
       <c r="B896" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C896" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C896" s="25"/>
       <c r="D896" s="22" t="s">
         <v>22</v>
       </c>
@@ -20450,7 +20560,7 @@
         <v>640</v>
       </c>
       <c r="G896" s="23" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="H896" s="23"/>
       <c r="I896" s="23"/>
@@ -20460,9 +20570,7 @@
       <c r="B897" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C897" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C897" s="25"/>
       <c r="D897" s="22" t="s">
         <v>22</v>
       </c>
@@ -20473,7 +20581,7 @@
         <v>640</v>
       </c>
       <c r="G897" s="23" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="H897" s="23"/>
       <c r="I897" s="23"/>
@@ -20496,7 +20604,7 @@
         <v>640</v>
       </c>
       <c r="G898" s="23" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="H898" s="23"/>
       <c r="I898" s="23"/>
@@ -20519,31 +20627,29 @@
         <v>640</v>
       </c>
       <c r="G899" s="23" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="H899" s="23"/>
       <c r="I899" s="23"/>
     </row>
-    <row r="900" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="900" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A900" s="9"/>
-      <c r="B900" s="25" t="s">
-        <v>611</v>
+      <c r="B900" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="C900" s="25"/>
-      <c r="D900" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E900" s="25"/>
+      <c r="D900" s="22"/>
+      <c r="E900" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F900" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G900" s="23" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="H900" s="23"/>
-      <c r="I900" s="23" t="s">
-        <v>613</v>
-      </c>
+      <c r="I900" s="23"/>
     </row>
     <row r="901" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A901" s="9"/>
@@ -20563,7 +20669,7 @@
         <v>640</v>
       </c>
       <c r="G901" s="23" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="H901" s="23"/>
       <c r="I901" s="23"/>
@@ -20586,7 +20692,7 @@
         <v>640</v>
       </c>
       <c r="G902" s="23" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="H902" s="23"/>
       <c r="I902" s="23"/>
@@ -20596,12 +20702,8 @@
       <c r="B903" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C903" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D903" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C903" s="25"/>
+      <c r="D903" s="22"/>
       <c r="E903" s="22" t="s">
         <v>22</v>
       </c>
@@ -20609,7 +20711,7 @@
         <v>640</v>
       </c>
       <c r="G903" s="23" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="H903" s="23"/>
       <c r="I903" s="23"/>
@@ -20632,7 +20734,7 @@
         <v>640</v>
       </c>
       <c r="G904" s="23" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="H904" s="23"/>
       <c r="I904" s="23"/>
@@ -20642,12 +20744,8 @@
       <c r="B905" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C905" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D905" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C905" s="25"/>
+      <c r="D905" s="22"/>
       <c r="E905" s="22" t="s">
         <v>22</v>
       </c>
@@ -20655,7 +20753,7 @@
         <v>640</v>
       </c>
       <c r="G905" s="23" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="H905" s="23"/>
       <c r="I905" s="23"/>
@@ -20678,7 +20776,7 @@
         <v>640</v>
       </c>
       <c r="G906" s="23" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="H906" s="23"/>
       <c r="I906" s="23"/>
@@ -20701,7 +20799,7 @@
         <v>640</v>
       </c>
       <c r="G907" s="23" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="H907" s="23"/>
       <c r="I907" s="23"/>
@@ -20711,8 +20809,12 @@
       <c r="B908" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C908" s="25"/>
-      <c r="D908" s="22"/>
+      <c r="C908" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D908" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E908" s="22" t="s">
         <v>22</v>
       </c>
@@ -20720,17 +20822,22 @@
         <v>640</v>
       </c>
       <c r="G908" s="23" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H908" s="23"/>
       <c r="I908" s="23"/>
     </row>
     <row r="909" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A909" s="9"/>
       <c r="B909" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C909" s="25"/>
-      <c r="D909" s="22"/>
+      <c r="C909" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D909" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E909" s="22" t="s">
         <v>22</v>
       </c>
@@ -20738,17 +20845,22 @@
         <v>640</v>
       </c>
       <c r="G909" s="23" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="H909" s="23"/>
       <c r="I909" s="23"/>
     </row>
     <row r="910" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A910" s="9"/>
       <c r="B910" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C910" s="25"/>
-      <c r="D910" s="22"/>
+      <c r="C910" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D910" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E910" s="22" t="s">
         <v>22</v>
       </c>
@@ -20756,21 +20868,18 @@
         <v>640</v>
       </c>
       <c r="G910" s="23" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="H910" s="23"/>
       <c r="I910" s="23"/>
     </row>
     <row r="911" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A911" s="9"/>
       <c r="B911" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C911" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D911" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C911" s="25"/>
+      <c r="D911" s="22"/>
       <c r="E911" s="22" t="s">
         <v>22</v>
       </c>
@@ -20778,12 +20887,13 @@
         <v>640</v>
       </c>
       <c r="G911" s="23" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="H911" s="23"/>
       <c r="I911" s="23"/>
     </row>
     <row r="912" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A912" s="9"/>
       <c r="B912" s="22" t="s">
         <v>22</v>
       </c>
@@ -20800,12 +20910,13 @@
         <v>640</v>
       </c>
       <c r="G912" s="23" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="H912" s="23"/>
       <c r="I912" s="23"/>
     </row>
     <row r="913" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A913" s="9"/>
       <c r="B913" s="22" t="s">
         <v>22</v>
       </c>
@@ -20819,19 +20930,22 @@
         <v>22</v>
       </c>
       <c r="F913" s="22" t="s">
-        <v>951</v>
+        <v>640</v>
       </c>
       <c r="G913" s="23" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="H913" s="23"/>
       <c r="I913" s="23"/>
     </row>
     <row r="914" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A914" s="9"/>
       <c r="B914" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C914" s="25"/>
+      <c r="C914" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D914" s="22" t="s">
         <v>22</v>
       </c>
@@ -20839,94 +20953,424 @@
         <v>22</v>
       </c>
       <c r="F914" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G914" s="23" t="s">
+        <v>950</v>
+      </c>
+      <c r="H914" s="23"/>
+      <c r="I914" s="23"/>
+    </row>
+    <row r="915" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A915" s="9"/>
+      <c r="B915" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C915" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D915" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E915" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F915" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G915" s="23" t="s">
         <v>951</v>
       </c>
-      <c r="G914" s="23" t="s">
-        <v>953</v>
-      </c>
-      <c r="H914" s="23"/>
-      <c r="I914" s="23" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="915" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B915" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="C915" s="27"/>
-      <c r="D915" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="E915" s="27"/>
-      <c r="F915" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="G915" s="28" t="s">
-        <v>955</v>
-      </c>
-      <c r="H915" s="28"/>
-      <c r="I915" s="28" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="916" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B916" s="22" t="s">
-        <v>22</v>
+      <c r="H915" s="23"/>
+      <c r="I915" s="23"/>
+    </row>
+    <row r="916" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A916" s="9"/>
+      <c r="B916" s="25" t="s">
+        <v>611</v>
       </c>
       <c r="C916" s="25"/>
       <c r="D916" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E916" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E916" s="25"/>
       <c r="F916" s="22" t="s">
-        <v>951</v>
+        <v>640</v>
       </c>
       <c r="G916" s="23" t="s">
-        <v>957</v>
+        <v>952</v>
       </c>
       <c r="H916" s="23"/>
       <c r="I916" s="23" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="917" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A917" s="9"/>
+      <c r="B917" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C917" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D917" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E917" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F917" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G917" s="23" t="s">
+        <v>953</v>
+      </c>
+      <c r="H917" s="23"/>
+      <c r="I917" s="23"/>
+    </row>
+    <row r="918" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A918" s="9"/>
+      <c r="B918" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C918" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D918" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E918" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F918" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G918" s="23" t="s">
         <v>954</v>
       </c>
-    </row>
-    <row r="917" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B917" s="27" t="s">
+      <c r="H918" s="23"/>
+      <c r="I918" s="23"/>
+    </row>
+    <row r="919" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A919" s="9"/>
+      <c r="B919" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C919" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D919" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E919" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F919" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="C917" s="27"/>
-      <c r="D917" s="27" t="s">
+      <c r="G919" s="23" t="s">
+        <v>955</v>
+      </c>
+      <c r="H919" s="23"/>
+      <c r="I919" s="23"/>
+    </row>
+    <row r="920" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A920" s="9"/>
+      <c r="B920" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C920" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D920" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E920" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F920" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="E917" s="27"/>
-      <c r="F917" s="27" t="s">
+      <c r="G920" s="23" t="s">
+        <v>956</v>
+      </c>
+      <c r="H920" s="23"/>
+      <c r="I920" s="23"/>
+    </row>
+    <row r="921" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A921" s="9"/>
+      <c r="B921" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C921" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D921" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E921" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F921" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="G917" s="28" t="s">
+      <c r="G921" s="23" t="s">
+        <v>957</v>
+      </c>
+      <c r="H921" s="23"/>
+      <c r="I921" s="23"/>
+    </row>
+    <row r="922" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A922" s="9"/>
+      <c r="B922" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C922" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D922" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E922" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F922" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G922" s="23" t="s">
         <v>958</v>
       </c>
-      <c r="H917" s="28"/>
-      <c r="I917" s="28" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H922" s="23"/>
+      <c r="I922" s="23"/>
+    </row>
+    <row r="923" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A923" s="9"/>
+      <c r="B923" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C923" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D923" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E923" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F923" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G923" s="23" t="s">
+        <v>959</v>
+      </c>
+      <c r="H923" s="23"/>
+      <c r="I923" s="23"/>
+    </row>
+    <row r="924" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A924" s="9"/>
+      <c r="B924" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C924" s="25"/>
+      <c r="D924" s="22"/>
+      <c r="E924" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F924" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G924" s="23" t="s">
+        <v>960</v>
+      </c>
+      <c r="H924" s="23"/>
+      <c r="I924" s="23"/>
+    </row>
+    <row r="925" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B925" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C925" s="25"/>
+      <c r="D925" s="22"/>
+      <c r="E925" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F925" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G925" s="23" t="s">
+        <v>961</v>
+      </c>
+      <c r="H925" s="23"/>
+      <c r="I925" s="23"/>
+    </row>
+    <row r="926" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B926" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C926" s="25"/>
+      <c r="D926" s="22"/>
+      <c r="E926" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F926" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G926" s="23" t="s">
+        <v>962</v>
+      </c>
+      <c r="H926" s="23"/>
+      <c r="I926" s="23"/>
+    </row>
+    <row r="927" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B927" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C927" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D927" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E927" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F927" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G927" s="23" t="s">
+        <v>963</v>
+      </c>
+      <c r="H927" s="23"/>
+      <c r="I927" s="23"/>
+    </row>
+    <row r="928" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B928" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C928" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D928" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E928" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F928" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G928" s="23" t="s">
+        <v>964</v>
+      </c>
+      <c r="H928" s="23"/>
+      <c r="I928" s="23"/>
+    </row>
+    <row r="929" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B929" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C929" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D929" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E929" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F929" s="22" t="s">
+        <v>965</v>
+      </c>
+      <c r="G929" s="23" t="s">
+        <v>966</v>
+      </c>
+      <c r="H929" s="23"/>
+      <c r="I929" s="23"/>
+    </row>
+    <row r="930" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B930" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C930" s="25"/>
+      <c r="D930" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E930" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F930" s="22" t="s">
+        <v>965</v>
+      </c>
+      <c r="G930" s="23" t="s">
+        <v>967</v>
+      </c>
+      <c r="H930" s="23"/>
+      <c r="I930" s="23" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="931" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B931" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="C931" s="27"/>
+      <c r="D931" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="E931" s="27"/>
+      <c r="F931" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="G931" s="28" t="s">
+        <v>969</v>
+      </c>
+      <c r="H931" s="28"/>
+      <c r="I931" s="28" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="932" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B932" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C932" s="25"/>
+      <c r="D932" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E932" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F932" s="22" t="s">
+        <v>965</v>
+      </c>
+      <c r="G932" s="23" t="s">
+        <v>971</v>
+      </c>
+      <c r="H932" s="23"/>
+      <c r="I932" s="23" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="933" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B933" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="C933" s="27"/>
+      <c r="D933" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="E933" s="27"/>
+      <c r="F933" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="G933" s="28" t="s">
+        <v>972</v>
+      </c>
+      <c r="H933" s="28"/>
+      <c r="I933" s="28" t="s">
+        <v>970</v>
+      </c>
+    </row>
     <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Updated vi spreadsheet and rebuilt
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3824" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3838" uniqueCount="978">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -2518,6 +2518,9 @@
     <t xml:space="preserve">ElevatorSim_HasHitUpperLimit.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">ElevatorSim_RKF45_Func.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">ElevatorSim_New_NoNoise.vi</t>
   </si>
   <si>
@@ -2629,6 +2632,9 @@
     <t xml:space="preserve">SngJntArmSim_New.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">SngJntArmSim_Rkf45_Func.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">SngJntArmSim_SetInputVoltage.vi</t>
   </si>
   <si>
@@ -2725,9 +2731,15 @@
     <t xml:space="preserve">NumIntegrate_Rk4_K_Dbl.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">NumIntegrate_Rkf45.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">NumIntegrate_Rkf45_Ax_Bu_K.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">NumIntegrate_Rkf45Impl.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">NumIntegrate_Rkf45Impl_Ax_Bu_K.vi</t>
   </si>
   <si>
@@ -2801,6 +2813,9 @@
   </si>
   <si>
     <t xml:space="preserve">MEDIAN_FILTER.CTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_RKF45_FUNC_TYPE.ctl</t>
   </si>
   <si>
     <t xml:space="preserve">PARAM_STACK_ITEM.CTL</t>
@@ -3390,8 +3405,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A781" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G804" activeCellId="0" sqref="G804"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3482,28 +3497,28 @@
         <v>11</v>
       </c>
       <c r="B9" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1260,"X")</f>
-        <v>584</v>
+        <f aca="false">COUNTIF(B18:B1265,"X")</f>
+        <v>589</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C18:C1260,"X")</f>
+        <f aca="false">COUNTIF(C18:C1265,"X")</f>
         <v>368</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D18:D1260,"X")</f>
-        <v>168</v>
+        <f aca="false">COUNTIF(D18:D1265,"X")</f>
+        <v>170</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E18:E1260,"X")</f>
+        <f aca="false">COUNTIF(E18:E1265,"X")</f>
         <v>555</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F18:F1260,"S")+COUNTIF(F18:F1260,"I")+COUNTIF(F18:F1260,"X")+COUNTIF(F18:F1260,"SI")+COUNTIF(F18:F1260,"IS")+COUNTIF(F18:F1260,"N/A")</f>
-        <v>213</v>
+        <f aca="false">COUNTIF(F18:F1265,"S")+COUNTIF(F18:F1265,"I")+COUNTIF(F18:F1265,"X")+COUNTIF(F18:F1265,"SI")+COUNTIF(F18:F1265,"IS")+COUNTIF(F18:F1265,"N/A")</f>
+        <v>214</v>
       </c>
       <c r="G9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.63013698630137</v>
+        <v>0.624787775891341</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3511,7 +3526,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="13" t="n">
-        <f aca="false">COUNTIF(B19:B1261,"/")</f>
+        <f aca="false">COUNTIF(B19:B1266,"/")</f>
         <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -3521,7 +3536,7 @@
     <row r="11" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.36472602739726</v>
+        <v>0.363327674023769</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17924,10 +17939,14 @@
       <c r="N762" s="1"/>
       <c r="O762" s="1"/>
     </row>
-    <row r="763" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B763" s="25"/>
+    <row r="763" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B763" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C763" s="25"/>
-      <c r="D763" s="22"/>
+      <c r="D763" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E763" s="25"/>
       <c r="F763" s="25"/>
       <c r="G763" s="23" t="s">
@@ -17978,88 +17997,83 @@
       <c r="N765" s="1"/>
       <c r="O765" s="1"/>
     </row>
-    <row r="766" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B766" s="46"/>
-      <c r="C766" s="1"/>
-      <c r="D766" s="1"/>
-      <c r="E766" s="1"/>
-      <c r="F766" s="1"/>
-      <c r="G766" s="1"/>
-      <c r="H766" s="1"/>
-      <c r="I766" s="1"/>
-      <c r="J766" s="1"/>
-      <c r="K766" s="1"/>
-      <c r="L766" s="1"/>
+    <row r="766" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B766" s="25"/>
+      <c r="C766" s="25"/>
+      <c r="D766" s="22"/>
+      <c r="E766" s="25"/>
+      <c r="F766" s="25"/>
+      <c r="G766" s="23" t="s">
+        <v>834</v>
+      </c>
+      <c r="H766" s="23"/>
+      <c r="I766" s="23"/>
+      <c r="J766" s="22"/>
+      <c r="K766" s="22"/>
+      <c r="L766" s="22"/>
       <c r="M766" s="1"/>
       <c r="N766" s="1"/>
       <c r="O766" s="1"/>
     </row>
-    <row r="767" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A767" s="19"/>
-      <c r="B767" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C767" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D767" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E767" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F767" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G767" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H767" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I767" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J767" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="K767" s="11" t="s">
-        <v>691</v>
-      </c>
-      <c r="L767" s="11" t="s">
-        <v>692</v>
-      </c>
+    <row r="767" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B767" s="46"/>
+      <c r="C767" s="1"/>
+      <c r="D767" s="1"/>
+      <c r="E767" s="1"/>
+      <c r="F767" s="1"/>
+      <c r="G767" s="1"/>
+      <c r="H767" s="1"/>
+      <c r="I767" s="1"/>
+      <c r="J767" s="1"/>
+      <c r="K767" s="1"/>
+      <c r="L767" s="1"/>
       <c r="M767" s="1"/>
       <c r="N767" s="1"/>
       <c r="O767" s="1"/>
     </row>
-    <row r="768" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A768" s="21" t="s">
-        <v>834</v>
-      </c>
-      <c r="B768" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C768" s="25"/>
-      <c r="D768" s="22"/>
-      <c r="E768" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F768" s="25"/>
-      <c r="G768" s="23" t="s">
-        <v>835</v>
-      </c>
-      <c r="H768" s="23"/>
-      <c r="I768" s="23"/>
-      <c r="J768" s="22"/>
-      <c r="K768" s="22"/>
-      <c r="L768" s="22"/>
+    <row r="768" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A768" s="19"/>
+      <c r="B768" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C768" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D768" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E768" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F768" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G768" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H768" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I768" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J768" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K768" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L768" s="11" t="s">
+        <v>692</v>
+      </c>
       <c r="M768" s="1"/>
       <c r="N768" s="1"/>
       <c r="O768" s="1"/>
     </row>
     <row r="769" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A769" s="21"/>
+      <c r="A769" s="21" t="s">
+        <v>835</v>
+      </c>
       <c r="B769" s="22" t="s">
         <v>22</v>
       </c>
@@ -18175,18 +18189,20 @@
     </row>
     <row r="774" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A774" s="21"/>
-      <c r="B774" s="25"/>
+      <c r="B774" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C774" s="25"/>
       <c r="D774" s="22"/>
-      <c r="E774" s="22"/>
+      <c r="E774" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F774" s="25"/>
       <c r="G774" s="23" t="s">
         <v>841</v>
       </c>
       <c r="H774" s="23"/>
-      <c r="I774" s="23" t="s">
-        <v>103</v>
-      </c>
+      <c r="I774" s="23"/>
       <c r="J774" s="22"/>
       <c r="K774" s="22"/>
       <c r="L774" s="22"/>
@@ -18236,16 +18252,20 @@
       <c r="N776" s="1"/>
       <c r="O776" s="1"/>
     </row>
-    <row r="777" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="777" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A777" s="21"/>
-      <c r="B777" s="22"/>
-      <c r="C777" s="22"/>
+      <c r="B777" s="25"/>
+      <c r="C777" s="25"/>
       <c r="D777" s="22"/>
       <c r="E777" s="22"/>
-      <c r="F777" s="22"/>
-      <c r="G777" s="23"/>
+      <c r="F777" s="25"/>
+      <c r="G777" s="23" t="s">
+        <v>844</v>
+      </c>
       <c r="H777" s="23"/>
-      <c r="I777" s="23"/>
+      <c r="I777" s="23" t="s">
+        <v>103</v>
+      </c>
       <c r="J777" s="22"/>
       <c r="K777" s="22"/>
       <c r="L777" s="22"/>
@@ -18254,87 +18274,81 @@
       <c r="O777" s="1"/>
     </row>
     <row r="778" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B778" s="46"/>
-      <c r="C778" s="1"/>
-      <c r="D778" s="1"/>
-      <c r="E778" s="1"/>
-      <c r="F778" s="1"/>
-      <c r="G778" s="1"/>
-      <c r="H778" s="1"/>
-      <c r="I778" s="1"/>
-      <c r="J778" s="1"/>
-      <c r="K778" s="1"/>
-      <c r="L778" s="1"/>
+      <c r="A778" s="21"/>
+      <c r="B778" s="22"/>
+      <c r="C778" s="22"/>
+      <c r="D778" s="22"/>
+      <c r="E778" s="22"/>
+      <c r="F778" s="22"/>
+      <c r="G778" s="23"/>
+      <c r="H778" s="23"/>
+      <c r="I778" s="23"/>
+      <c r="J778" s="22"/>
+      <c r="K778" s="22"/>
+      <c r="L778" s="22"/>
       <c r="M778" s="1"/>
       <c r="N778" s="1"/>
       <c r="O778" s="1"/>
     </row>
-    <row r="779" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A779" s="19"/>
-      <c r="B779" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C779" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D779" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E779" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F779" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G779" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H779" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I779" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J779" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="K779" s="11" t="s">
-        <v>691</v>
-      </c>
-      <c r="L779" s="11" t="s">
-        <v>692</v>
-      </c>
+    <row r="779" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B779" s="46"/>
+      <c r="C779" s="1"/>
+      <c r="D779" s="1"/>
+      <c r="E779" s="1"/>
+      <c r="F779" s="1"/>
+      <c r="G779" s="1"/>
+      <c r="H779" s="1"/>
+      <c r="I779" s="1"/>
+      <c r="J779" s="1"/>
+      <c r="K779" s="1"/>
+      <c r="L779" s="1"/>
       <c r="M779" s="1"/>
       <c r="N779" s="1"/>
       <c r="O779" s="1"/>
     </row>
-    <row r="780" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A780" s="21" t="s">
-        <v>844</v>
-      </c>
-      <c r="B780" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C780" s="25"/>
-      <c r="D780" s="22"/>
-      <c r="E780" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F780" s="25"/>
-      <c r="G780" s="23" t="s">
-        <v>845</v>
-      </c>
-      <c r="H780" s="23"/>
-      <c r="I780" s="23"/>
-      <c r="J780" s="22"/>
-      <c r="K780" s="22"/>
-      <c r="L780" s="22"/>
+    <row r="780" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A780" s="19"/>
+      <c r="B780" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C780" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D780" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E780" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F780" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G780" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H780" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I780" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J780" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K780" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L780" s="11" t="s">
+        <v>692</v>
+      </c>
       <c r="M780" s="1"/>
       <c r="N780" s="1"/>
       <c r="O780" s="1"/>
     </row>
     <row r="781" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A781" s="21"/>
+      <c r="A781" s="21" t="s">
+        <v>845</v>
+      </c>
       <c r="B781" s="22" t="s">
         <v>22</v>
       </c>
@@ -18394,9 +18408,7 @@
         <v>848</v>
       </c>
       <c r="H783" s="23"/>
-      <c r="I783" s="23" t="s">
-        <v>849</v>
-      </c>
+      <c r="I783" s="23"/>
       <c r="J783" s="22"/>
       <c r="K783" s="22"/>
       <c r="L783" s="22"/>
@@ -18416,10 +18428,12 @@
       </c>
       <c r="F784" s="25"/>
       <c r="G784" s="23" t="s">
+        <v>849</v>
+      </c>
+      <c r="H784" s="23"/>
+      <c r="I784" s="23" t="s">
         <v>850</v>
       </c>
-      <c r="H784" s="23"/>
-      <c r="I784" s="23"/>
       <c r="J784" s="22"/>
       <c r="K784" s="22"/>
       <c r="L784" s="22"/>
@@ -18435,7 +18449,7 @@
       <c r="C785" s="25"/>
       <c r="D785" s="22"/>
       <c r="E785" s="22" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="F785" s="25"/>
       <c r="G785" s="23" t="s">
@@ -18450,15 +18464,13 @@
       <c r="N785" s="1"/>
       <c r="O785" s="1"/>
     </row>
-    <row r="786" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="786" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A786" s="21"/>
-      <c r="B786" s="27" t="s">
-        <v>611</v>
+      <c r="B786" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="C786" s="25"/>
-      <c r="D786" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D786" s="22"/>
       <c r="E786" s="22" t="s">
         <v>60</v>
       </c>
@@ -18475,12 +18487,18 @@
       <c r="N786" s="1"/>
       <c r="O786" s="1"/>
     </row>
-    <row r="787" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="787" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A787" s="21"/>
-      <c r="B787" s="25"/>
+      <c r="B787" s="27" t="s">
+        <v>611</v>
+      </c>
       <c r="C787" s="25"/>
-      <c r="D787" s="22"/>
-      <c r="E787" s="22"/>
+      <c r="D787" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E787" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="F787" s="25"/>
       <c r="G787" s="23" t="s">
         <v>853</v>
@@ -18496,12 +18514,10 @@
     </row>
     <row r="788" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A788" s="21"/>
-      <c r="B788" s="27" t="s">
-        <v>611</v>
-      </c>
+      <c r="B788" s="25"/>
       <c r="C788" s="25"/>
       <c r="D788" s="22"/>
-      <c r="E788" s="25"/>
+      <c r="E788" s="22"/>
       <c r="F788" s="25"/>
       <c r="G788" s="23" t="s">
         <v>854</v>
@@ -18517,14 +18533,12 @@
     </row>
     <row r="789" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A789" s="21"/>
-      <c r="B789" s="22" t="s">
-        <v>22</v>
+      <c r="B789" s="27" t="s">
+        <v>611</v>
       </c>
       <c r="C789" s="25"/>
       <c r="D789" s="22"/>
-      <c r="E789" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E789" s="25"/>
       <c r="F789" s="25"/>
       <c r="G789" s="23" t="s">
         <v>855</v>
@@ -18561,20 +18575,22 @@
       <c r="N790" s="1"/>
       <c r="O790" s="1"/>
     </row>
-    <row r="791" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="791" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A791" s="21"/>
-      <c r="B791" s="25"/>
+      <c r="B791" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C791" s="25"/>
       <c r="D791" s="22"/>
-      <c r="E791" s="22"/>
+      <c r="E791" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F791" s="25"/>
       <c r="G791" s="23" t="s">
         <v>857</v>
       </c>
       <c r="H791" s="23"/>
-      <c r="I791" s="23" t="s">
-        <v>858</v>
-      </c>
+      <c r="I791" s="23"/>
       <c r="J791" s="22"/>
       <c r="K791" s="22"/>
       <c r="L791" s="22"/>
@@ -18582,18 +18598,20 @@
       <c r="N791" s="1"/>
       <c r="O791" s="1"/>
     </row>
-    <row r="792" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="792" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A792" s="21"/>
-      <c r="B792" s="47"/>
+      <c r="B792" s="25"/>
       <c r="C792" s="25"/>
       <c r="D792" s="22"/>
       <c r="E792" s="22"/>
       <c r="F792" s="25"/>
       <c r="G792" s="23" t="s">
+        <v>858</v>
+      </c>
+      <c r="H792" s="23"/>
+      <c r="I792" s="23" t="s">
         <v>859</v>
       </c>
-      <c r="H792" s="23"/>
-      <c r="I792" s="23"/>
       <c r="J792" s="22"/>
       <c r="K792" s="22"/>
       <c r="L792" s="22"/>
@@ -18601,89 +18619,85 @@
       <c r="N792" s="1"/>
       <c r="O792" s="1"/>
     </row>
-    <row r="793" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="793" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A793" s="21"/>
-      <c r="B793" s="21"/>
-      <c r="C793" s="21"/>
-      <c r="D793" s="21"/>
-      <c r="E793" s="21"/>
-      <c r="F793" s="21"/>
-      <c r="G793" s="21"/>
-      <c r="H793" s="21"/>
-      <c r="I793" s="21"/>
-      <c r="J793" s="21"/>
-      <c r="K793" s="21"/>
-      <c r="L793" s="21"/>
-      <c r="M793" s="21"/>
+      <c r="B793" s="47"/>
+      <c r="C793" s="25"/>
+      <c r="D793" s="22"/>
+      <c r="E793" s="22"/>
+      <c r="F793" s="25"/>
+      <c r="G793" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="H793" s="23"/>
+      <c r="I793" s="23"/>
+      <c r="J793" s="22"/>
+      <c r="K793" s="22"/>
+      <c r="L793" s="22"/>
+      <c r="M793" s="1"/>
       <c r="N793" s="1"/>
       <c r="O793" s="1"/>
     </row>
-    <row r="794" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A794" s="19"/>
-      <c r="B794" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C794" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D794" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E794" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F794" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G794" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H794" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I794" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J794" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="K794" s="11" t="s">
-        <v>691</v>
-      </c>
-      <c r="L794" s="11" t="s">
-        <v>692</v>
-      </c>
-      <c r="M794" s="1"/>
+    <row r="794" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A794" s="21"/>
+      <c r="B794" s="21"/>
+      <c r="C794" s="21"/>
+      <c r="D794" s="21"/>
+      <c r="E794" s="21"/>
+      <c r="F794" s="21"/>
+      <c r="G794" s="21"/>
+      <c r="H794" s="21"/>
+      <c r="I794" s="21"/>
+      <c r="J794" s="21"/>
+      <c r="K794" s="21"/>
+      <c r="L794" s="21"/>
+      <c r="M794" s="21"/>
       <c r="N794" s="1"/>
       <c r="O794" s="1"/>
     </row>
-    <row r="795" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A795" s="21" t="s">
-        <v>860</v>
-      </c>
-      <c r="B795" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C795" s="25"/>
-      <c r="D795" s="22"/>
-      <c r="E795" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F795" s="25"/>
-      <c r="G795" s="23" t="s">
-        <v>861</v>
-      </c>
-      <c r="H795" s="23"/>
-      <c r="I795" s="23"/>
-      <c r="J795" s="22"/>
-      <c r="K795" s="22"/>
-      <c r="L795" s="22"/>
+    <row r="795" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A795" s="19"/>
+      <c r="B795" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C795" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D795" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E795" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F795" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G795" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H795" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I795" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J795" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="K795" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="L795" s="11" t="s">
+        <v>692</v>
+      </c>
       <c r="M795" s="1"/>
       <c r="N795" s="1"/>
       <c r="O795" s="1"/>
     </row>
-    <row r="796" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A796" s="21"/>
+    <row r="796" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A796" s="21" t="s">
+        <v>861</v>
+      </c>
       <c r="B796" s="22" t="s">
         <v>22</v>
       </c>
@@ -18843,16 +18857,14 @@
       <c r="N802" s="1"/>
       <c r="O802" s="1"/>
     </row>
-    <row r="803" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="803" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A803" s="21"/>
       <c r="B803" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C803" s="25"/>
       <c r="D803" s="22"/>
-      <c r="E803" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E803" s="25"/>
       <c r="F803" s="25"/>
       <c r="G803" s="23" t="s">
         <v>869</v>
@@ -18935,14 +18947,20 @@
       <c r="N806" s="1"/>
       <c r="O806" s="1"/>
     </row>
-    <row r="807" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="807" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A807" s="21"/>
-      <c r="B807" s="22"/>
-      <c r="C807" s="22"/>
+      <c r="B807" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C807" s="25"/>
       <c r="D807" s="22"/>
-      <c r="E807" s="22"/>
-      <c r="F807" s="22"/>
-      <c r="G807" s="23"/>
+      <c r="E807" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F807" s="25"/>
+      <c r="G807" s="23" t="s">
+        <v>873</v>
+      </c>
       <c r="H807" s="23"/>
       <c r="I807" s="23"/>
       <c r="J807" s="22"/>
@@ -18952,14 +18970,20 @@
       <c r="N807" s="1"/>
       <c r="O807" s="1"/>
     </row>
-    <row r="808" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="808" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A808" s="21"/>
-      <c r="B808" s="22"/>
-      <c r="C808" s="22"/>
+      <c r="B808" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C808" s="25"/>
       <c r="D808" s="22"/>
-      <c r="E808" s="22"/>
-      <c r="F808" s="22"/>
-      <c r="G808" s="23"/>
+      <c r="E808" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F808" s="25"/>
+      <c r="G808" s="23" t="s">
+        <v>874</v>
+      </c>
       <c r="H808" s="23"/>
       <c r="I808" s="23"/>
       <c r="J808" s="22"/>
@@ -18970,51 +18994,65 @@
       <c r="O808" s="1"/>
     </row>
     <row r="809" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A809" s="19"/>
-      <c r="B809" s="19"/>
-      <c r="C809" s="19"/>
-      <c r="D809" s="19"/>
-      <c r="E809" s="19"/>
-      <c r="F809" s="19"/>
-      <c r="G809" s="1"/>
-      <c r="H809" s="1"/>
-      <c r="I809" s="1"/>
-      <c r="J809" s="1"/>
-      <c r="K809" s="1"/>
-      <c r="L809" s="1"/>
+      <c r="A809" s="21"/>
+      <c r="B809" s="22"/>
+      <c r="C809" s="22"/>
+      <c r="D809" s="22"/>
+      <c r="E809" s="22"/>
+      <c r="F809" s="22"/>
+      <c r="G809" s="23"/>
+      <c r="H809" s="23"/>
+      <c r="I809" s="23"/>
+      <c r="J809" s="22"/>
+      <c r="K809" s="22"/>
+      <c r="L809" s="22"/>
       <c r="M809" s="1"/>
       <c r="N809" s="1"/>
       <c r="O809" s="1"/>
     </row>
     <row r="810" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A810" s="19"/>
-      <c r="B810" s="44"/>
-      <c r="C810" s="4"/>
-      <c r="D810" s="4"/>
-      <c r="E810" s="4"/>
-      <c r="F810" s="4"/>
+      <c r="A810" s="21"/>
+      <c r="B810" s="22"/>
+      <c r="C810" s="22"/>
+      <c r="D810" s="22"/>
+      <c r="E810" s="22"/>
+      <c r="F810" s="22"/>
+      <c r="G810" s="23"/>
+      <c r="H810" s="23"/>
+      <c r="I810" s="23"/>
+      <c r="J810" s="22"/>
+      <c r="K810" s="22"/>
+      <c r="L810" s="22"/>
+      <c r="M810" s="1"/>
+      <c r="N810" s="1"/>
+      <c r="O810" s="1"/>
     </row>
     <row r="811" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A811" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B811" s="43"/>
-      <c r="C811" s="18"/>
-      <c r="D811" s="18"/>
-      <c r="E811" s="18"/>
-      <c r="F811" s="18"/>
+      <c r="A811" s="19"/>
+      <c r="B811" s="19"/>
+      <c r="C811" s="19"/>
+      <c r="D811" s="19"/>
+      <c r="E811" s="19"/>
+      <c r="F811" s="19"/>
+      <c r="G811" s="1"/>
+      <c r="H811" s="1"/>
+      <c r="I811" s="1"/>
+      <c r="J811" s="1"/>
+      <c r="K811" s="1"/>
+      <c r="L811" s="1"/>
+      <c r="M811" s="1"/>
+      <c r="N811" s="1"/>
+      <c r="O811" s="1"/>
     </row>
     <row r="812" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A812" s="16" t="s">
-        <v>873</v>
-      </c>
-      <c r="B812" s="43"/>
-      <c r="C812" s="18"/>
-      <c r="D812" s="18"/>
-      <c r="E812" s="18"/>
-      <c r="F812" s="18"/>
-    </row>
-    <row r="813" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A812" s="19"/>
+      <c r="B812" s="44"/>
+      <c r="C812" s="4"/>
+      <c r="D812" s="4"/>
+      <c r="E812" s="4"/>
+      <c r="F812" s="4"/>
+    </row>
+    <row r="813" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A813" s="16" t="s">
         <v>15</v>
       </c>
@@ -19023,303 +19061,285 @@
       <c r="D813" s="18"/>
       <c r="E813" s="18"/>
       <c r="F813" s="18"/>
-      <c r="H813" s="4" t="s">
+    </row>
+    <row r="814" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A814" s="16" t="s">
+        <v>875</v>
+      </c>
+      <c r="B814" s="43"/>
+      <c r="C814" s="18"/>
+      <c r="D814" s="18"/>
+      <c r="E814" s="18"/>
+      <c r="F814" s="18"/>
+    </row>
+    <row r="815" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A815" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B815" s="43"/>
+      <c r="C815" s="18"/>
+      <c r="D815" s="18"/>
+      <c r="E815" s="18"/>
+      <c r="F815" s="18"/>
+      <c r="H815" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="814" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A814" s="19"/>
-      <c r="B814" s="19"/>
-      <c r="C814" s="19"/>
-      <c r="D814" s="19"/>
-      <c r="E814" s="19"/>
-      <c r="F814" s="19"/>
-    </row>
-    <row r="815" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A815" s="19"/>
-      <c r="B815" s="11" t="s">
+    <row r="816" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A816" s="19"/>
+      <c r="B816" s="19"/>
+      <c r="C816" s="19"/>
+      <c r="D816" s="19"/>
+      <c r="E816" s="19"/>
+      <c r="F816" s="19"/>
+    </row>
+    <row r="817" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A817" s="19"/>
+      <c r="B817" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C815" s="11" t="s">
+      <c r="C817" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D815" s="11" t="s">
+      <c r="D817" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E815" s="11" t="s">
+      <c r="E817" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F815" s="11" t="s">
+      <c r="F817" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G815" s="20" t="s">
+      <c r="G817" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H815" s="20" t="s">
+      <c r="H817" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I815" s="20" t="s">
+      <c r="I817" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J815" s="11" t="s">
+      <c r="J817" s="11" t="s">
         <v>690</v>
       </c>
-      <c r="K815" s="11" t="s">
+      <c r="K817" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="L815" s="11" t="s">
+      <c r="L817" s="11" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="816" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A816" s="21" t="s">
-        <v>874</v>
-      </c>
-      <c r="B816" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C816" s="25"/>
-      <c r="D816" s="22"/>
-      <c r="E816" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F816" s="25"/>
-      <c r="G816" s="23" t="s">
-        <v>875</v>
-      </c>
-      <c r="H816" s="23"/>
-      <c r="I816" s="23"/>
-      <c r="J816" s="22"/>
-      <c r="K816" s="22"/>
-      <c r="L816" s="22"/>
-    </row>
-    <row r="817" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B817" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C817" s="25"/>
-      <c r="D817" s="22"/>
-      <c r="E817" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F817" s="25"/>
-      <c r="G817" s="23" t="s">
+    <row r="818" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A818" s="21" t="s">
         <v>876</v>
       </c>
-      <c r="H817" s="23"/>
-      <c r="I817" s="23"/>
-      <c r="J817" s="22"/>
-      <c r="K817" s="22"/>
-      <c r="L817" s="22"/>
-    </row>
-    <row r="818" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A818" s="19"/>
-      <c r="B818" s="44"/>
-      <c r="C818" s="4"/>
-      <c r="D818" s="4"/>
-      <c r="E818" s="4"/>
-      <c r="F818" s="4"/>
+      <c r="B818" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C818" s="25"/>
+      <c r="D818" s="22"/>
+      <c r="E818" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F818" s="25"/>
+      <c r="G818" s="23" t="s">
+        <v>877</v>
+      </c>
+      <c r="H818" s="23"/>
+      <c r="I818" s="23"/>
+      <c r="J818" s="22"/>
+      <c r="K818" s="22"/>
+      <c r="L818" s="22"/>
     </row>
     <row r="819" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B819" s="46"/>
-      <c r="C819" s="1"/>
-      <c r="D819" s="1"/>
-      <c r="E819" s="1"/>
-      <c r="F819" s="1"/>
-      <c r="G819" s="1"/>
-      <c r="H819" s="1"/>
-      <c r="I819" s="1"/>
-      <c r="J819" s="1"/>
-      <c r="K819" s="1"/>
-      <c r="L819" s="1"/>
-    </row>
-    <row r="820" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B819" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C819" s="25"/>
+      <c r="D819" s="22"/>
+      <c r="E819" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F819" s="25"/>
+      <c r="G819" s="23" t="s">
+        <v>878</v>
+      </c>
+      <c r="H819" s="23"/>
+      <c r="I819" s="23"/>
+      <c r="J819" s="22"/>
+      <c r="K819" s="22"/>
+      <c r="L819" s="22"/>
+    </row>
+    <row r="820" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A820" s="19"/>
-      <c r="B820" s="11" t="s">
+      <c r="B820" s="44"/>
+      <c r="C820" s="4"/>
+      <c r="D820" s="4"/>
+      <c r="E820" s="4"/>
+      <c r="F820" s="4"/>
+    </row>
+    <row r="821" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B821" s="46"/>
+      <c r="C821" s="1"/>
+      <c r="D821" s="1"/>
+      <c r="E821" s="1"/>
+      <c r="F821" s="1"/>
+      <c r="G821" s="1"/>
+      <c r="H821" s="1"/>
+      <c r="I821" s="1"/>
+      <c r="J821" s="1"/>
+      <c r="K821" s="1"/>
+      <c r="L821" s="1"/>
+    </row>
+    <row r="822" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A822" s="19"/>
+      <c r="B822" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C820" s="11" t="s">
+      <c r="C822" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D820" s="11" t="s">
+      <c r="D822" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E820" s="11" t="s">
+      <c r="E822" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F820" s="11" t="s">
+      <c r="F822" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G820" s="20" t="s">
+      <c r="G822" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H820" s="20" t="s">
+      <c r="H822" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I820" s="20" t="s">
+      <c r="I822" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J820" s="11" t="s">
+      <c r="J822" s="11" t="s">
         <v>690</v>
       </c>
-      <c r="K820" s="11" t="s">
+      <c r="K822" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="L820" s="11" t="s">
+      <c r="L822" s="11" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="821" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A821" s="21" t="s">
-        <v>877</v>
-      </c>
-      <c r="B821" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C821" s="25"/>
-      <c r="D821" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E821" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F821" s="25"/>
-      <c r="G821" s="23" t="s">
-        <v>878</v>
-      </c>
-      <c r="H821" s="23"/>
-      <c r="I821" s="23"/>
-      <c r="J821" s="22"/>
-      <c r="K821" s="22"/>
-      <c r="L821" s="22"/>
-    </row>
-    <row r="822" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B822" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C822" s="25"/>
-      <c r="D822" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E822" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F822" s="25"/>
-      <c r="G822" s="23" t="s">
+    <row r="823" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A823" s="21" t="s">
         <v>879</v>
       </c>
-      <c r="H822" s="23"/>
-      <c r="I822" s="23"/>
-      <c r="J822" s="22"/>
-      <c r="K822" s="22"/>
-      <c r="L822" s="22"/>
-    </row>
-    <row r="823" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B823" s="1"/>
-      <c r="C823" s="1"/>
-      <c r="D823" s="1"/>
-      <c r="E823" s="1"/>
-      <c r="F823" s="1"/>
-      <c r="G823" s="1"/>
-      <c r="H823" s="1"/>
-      <c r="I823" s="1"/>
-      <c r="J823" s="1"/>
-      <c r="K823" s="1"/>
-      <c r="L823" s="1"/>
-      <c r="M823" s="1"/>
-      <c r="N823" s="1"/>
-    </row>
-    <row r="824" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B824" s="46"/>
-      <c r="C824" s="1"/>
-      <c r="D824" s="1"/>
-      <c r="E824" s="1"/>
-      <c r="F824" s="1"/>
-      <c r="G824" s="1"/>
-      <c r="H824" s="1"/>
-      <c r="I824" s="1"/>
-      <c r="J824" s="1"/>
-      <c r="K824" s="1"/>
-      <c r="L824" s="1"/>
-    </row>
-    <row r="825" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A825" s="19"/>
-      <c r="B825" s="11" t="s">
+      <c r="B823" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C823" s="25"/>
+      <c r="D823" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E823" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F823" s="25"/>
+      <c r="G823" s="23" t="s">
+        <v>880</v>
+      </c>
+      <c r="H823" s="23"/>
+      <c r="I823" s="23"/>
+      <c r="J823" s="22"/>
+      <c r="K823" s="22"/>
+      <c r="L823" s="22"/>
+    </row>
+    <row r="824" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B824" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C824" s="25"/>
+      <c r="D824" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E824" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F824" s="25"/>
+      <c r="G824" s="23" t="s">
+        <v>881</v>
+      </c>
+      <c r="H824" s="23"/>
+      <c r="I824" s="23"/>
+      <c r="J824" s="22"/>
+      <c r="K824" s="22"/>
+      <c r="L824" s="22"/>
+    </row>
+    <row r="825" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B825" s="1"/>
+      <c r="C825" s="1"/>
+      <c r="D825" s="1"/>
+      <c r="E825" s="1"/>
+      <c r="F825" s="1"/>
+      <c r="G825" s="1"/>
+      <c r="H825" s="1"/>
+      <c r="I825" s="1"/>
+      <c r="J825" s="1"/>
+      <c r="K825" s="1"/>
+      <c r="L825" s="1"/>
+      <c r="M825" s="1"/>
+      <c r="N825" s="1"/>
+    </row>
+    <row r="826" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B826" s="46"/>
+      <c r="C826" s="1"/>
+      <c r="D826" s="1"/>
+      <c r="E826" s="1"/>
+      <c r="F826" s="1"/>
+      <c r="G826" s="1"/>
+      <c r="H826" s="1"/>
+      <c r="I826" s="1"/>
+      <c r="J826" s="1"/>
+      <c r="K826" s="1"/>
+      <c r="L826" s="1"/>
+    </row>
+    <row r="827" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A827" s="19"/>
+      <c r="B827" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C825" s="11" t="s">
+      <c r="C827" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D825" s="11" t="s">
+      <c r="D827" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E825" s="11" t="s">
+      <c r="E827" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F825" s="11" t="s">
+      <c r="F827" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G825" s="20" t="s">
+      <c r="G827" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H825" s="20" t="s">
+      <c r="H827" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I825" s="20" t="s">
+      <c r="I827" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J825" s="11" t="s">
+      <c r="J827" s="11" t="s">
         <v>690</v>
       </c>
-      <c r="K825" s="11" t="s">
+      <c r="K827" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="L825" s="11" t="s">
+      <c r="L827" s="11" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="826" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A826" s="21" t="s">
-        <v>880</v>
-      </c>
-      <c r="B826" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C826" s="25"/>
-      <c r="D826" s="22"/>
-      <c r="E826" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F826" s="25"/>
-      <c r="G826" s="23" t="s">
-        <v>881</v>
-      </c>
-      <c r="H826" s="23"/>
-      <c r="I826" s="23"/>
-      <c r="J826" s="22"/>
-      <c r="K826" s="22"/>
-      <c r="L826" s="22"/>
-    </row>
-    <row r="827" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B827" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C827" s="25"/>
-      <c r="D827" s="22"/>
-      <c r="E827" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F827" s="25"/>
-      <c r="G827" s="23" t="s">
+    <row r="828" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A828" s="21" t="s">
         <v>882</v>
       </c>
-      <c r="H827" s="23"/>
-      <c r="I827" s="23"/>
-      <c r="J827" s="22"/>
-      <c r="K827" s="22"/>
-      <c r="L827" s="22"/>
-    </row>
-    <row r="828" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B828" s="22" t="s">
         <v>22</v>
       </c>
@@ -19358,10 +19378,14 @@
       <c r="L829" s="22"/>
     </row>
     <row r="830" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B830" s="25"/>
+      <c r="B830" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C830" s="25"/>
       <c r="D830" s="22"/>
-      <c r="E830" s="22"/>
+      <c r="E830" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F830" s="25"/>
       <c r="G830" s="23" t="s">
         <v>885</v>
@@ -19373,10 +19397,14 @@
       <c r="L830" s="22"/>
     </row>
     <row r="831" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B831" s="25"/>
+      <c r="B831" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C831" s="25"/>
       <c r="D831" s="22"/>
-      <c r="E831" s="22"/>
+      <c r="E831" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F831" s="25"/>
       <c r="G831" s="23" t="s">
         <v>886</v>
@@ -19447,17 +19475,11 @@
       <c r="K835" s="22"/>
       <c r="L835" s="22"/>
     </row>
-    <row r="836" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B836" s="22" t="s">
-        <v>22</v>
-      </c>
+    <row r="836" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B836" s="25"/>
       <c r="C836" s="25"/>
-      <c r="D836" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E836" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D836" s="22"/>
+      <c r="E836" s="22"/>
       <c r="F836" s="25"/>
       <c r="G836" s="23" t="s">
         <v>891</v>
@@ -19468,13 +19490,15 @@
       <c r="K836" s="22"/>
       <c r="L836" s="22"/>
     </row>
-    <row r="837" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B837" s="22"/>
-      <c r="C837" s="22"/>
+    <row r="837" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B837" s="25"/>
+      <c r="C837" s="25"/>
       <c r="D837" s="22"/>
       <c r="E837" s="22"/>
-      <c r="F837" s="22"/>
-      <c r="G837" s="23"/>
+      <c r="F837" s="25"/>
+      <c r="G837" s="23" t="s">
+        <v>892</v>
+      </c>
       <c r="H837" s="23"/>
       <c r="I837" s="23"/>
       <c r="J837" s="22"/>
@@ -19482,47 +19506,45 @@
       <c r="L837" s="22"/>
     </row>
     <row r="838" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B838" s="1"/>
-      <c r="C838" s="1"/>
-      <c r="D838" s="1"/>
-      <c r="E838" s="1"/>
-      <c r="F838" s="1"/>
-      <c r="G838" s="1"/>
-      <c r="H838" s="1"/>
-      <c r="I838" s="1"/>
-      <c r="J838" s="1"/>
-      <c r="K838" s="1"/>
-      <c r="L838" s="1"/>
-      <c r="M838" s="1"/>
-      <c r="N838" s="1"/>
+      <c r="B838" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C838" s="25"/>
+      <c r="D838" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E838" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F838" s="25"/>
+      <c r="G838" s="23" t="s">
+        <v>893</v>
+      </c>
+      <c r="H838" s="23"/>
+      <c r="I838" s="23"/>
+      <c r="J838" s="22"/>
+      <c r="K838" s="22"/>
+      <c r="L838" s="22"/>
     </row>
     <row r="839" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A839" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B839" s="17"/>
-      <c r="C839" s="18"/>
-      <c r="D839" s="18"/>
-      <c r="E839" s="18"/>
-      <c r="F839" s="18"/>
-      <c r="G839" s="1"/>
-      <c r="H839" s="1"/>
-      <c r="I839" s="1"/>
-      <c r="J839" s="1"/>
-      <c r="K839" s="1"/>
-      <c r="L839" s="1"/>
-      <c r="M839" s="1"/>
-      <c r="N839" s="1"/>
+      <c r="B839" s="22"/>
+      <c r="C839" s="22"/>
+      <c r="D839" s="22"/>
+      <c r="E839" s="22"/>
+      <c r="F839" s="22"/>
+      <c r="G839" s="23"/>
+      <c r="H839" s="23"/>
+      <c r="I839" s="23"/>
+      <c r="J839" s="22"/>
+      <c r="K839" s="22"/>
+      <c r="L839" s="22"/>
     </row>
     <row r="840" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A840" s="16" t="s">
-        <v>892</v>
-      </c>
-      <c r="B840" s="17"/>
-      <c r="C840" s="18"/>
-      <c r="D840" s="18"/>
-      <c r="E840" s="18"/>
-      <c r="F840" s="18"/>
+      <c r="B840" s="1"/>
+      <c r="C840" s="1"/>
+      <c r="D840" s="1"/>
+      <c r="E840" s="1"/>
+      <c r="F840" s="1"/>
       <c r="G840" s="1"/>
       <c r="H840" s="1"/>
       <c r="I840" s="1"/>
@@ -19551,11 +19573,14 @@
       <c r="N841" s="1"/>
     </row>
     <row r="842" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B842" s="1"/>
-      <c r="C842" s="1"/>
-      <c r="D842" s="1"/>
-      <c r="E842" s="1"/>
-      <c r="F842" s="1"/>
+      <c r="A842" s="16" t="s">
+        <v>894</v>
+      </c>
+      <c r="B842" s="17"/>
+      <c r="C842" s="18"/>
+      <c r="D842" s="18"/>
+      <c r="E842" s="18"/>
+      <c r="F842" s="18"/>
       <c r="G842" s="1"/>
       <c r="H842" s="1"/>
       <c r="I842" s="1"/>
@@ -19566,96 +19591,91 @@
       <c r="N842" s="1"/>
     </row>
     <row r="843" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B843" s="46"/>
-      <c r="C843" s="1"/>
-      <c r="D843" s="1"/>
-      <c r="E843" s="1"/>
-      <c r="F843" s="1"/>
+      <c r="A843" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B843" s="17"/>
+      <c r="C843" s="18"/>
+      <c r="D843" s="18"/>
+      <c r="E843" s="18"/>
+      <c r="F843" s="18"/>
       <c r="G843" s="1"/>
       <c r="H843" s="1"/>
       <c r="I843" s="1"/>
       <c r="J843" s="1"/>
       <c r="K843" s="1"/>
       <c r="L843" s="1"/>
-    </row>
-    <row r="844" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A844" s="19"/>
-      <c r="B844" s="11" t="s">
+      <c r="M843" s="1"/>
+      <c r="N843" s="1"/>
+    </row>
+    <row r="844" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B844" s="1"/>
+      <c r="C844" s="1"/>
+      <c r="D844" s="1"/>
+      <c r="E844" s="1"/>
+      <c r="F844" s="1"/>
+      <c r="G844" s="1"/>
+      <c r="H844" s="1"/>
+      <c r="I844" s="1"/>
+      <c r="J844" s="1"/>
+      <c r="K844" s="1"/>
+      <c r="L844" s="1"/>
+      <c r="M844" s="1"/>
+      <c r="N844" s="1"/>
+    </row>
+    <row r="845" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B845" s="46"/>
+      <c r="C845" s="1"/>
+      <c r="D845" s="1"/>
+      <c r="E845" s="1"/>
+      <c r="F845" s="1"/>
+      <c r="G845" s="1"/>
+      <c r="H845" s="1"/>
+      <c r="I845" s="1"/>
+      <c r="J845" s="1"/>
+      <c r="K845" s="1"/>
+      <c r="L845" s="1"/>
+    </row>
+    <row r="846" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A846" s="19"/>
+      <c r="B846" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C844" s="11" t="s">
+      <c r="C846" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D844" s="11" t="s">
+      <c r="D846" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E844" s="11" t="s">
+      <c r="E846" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F844" s="11" t="s">
+      <c r="F846" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G844" s="20" t="s">
+      <c r="G846" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H844" s="20" t="s">
+      <c r="H846" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I844" s="20" t="s">
+      <c r="I846" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J844" s="11" t="s">
+      <c r="J846" s="11" t="s">
         <v>690</v>
       </c>
-      <c r="K844" s="11" t="s">
+      <c r="K846" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="L844" s="11" t="s">
+      <c r="L846" s="11" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="845" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A845" s="21" t="s">
-        <v>893</v>
-      </c>
-      <c r="B845" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C845" s="25"/>
-      <c r="D845" s="22"/>
-      <c r="E845" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F845" s="25"/>
-      <c r="G845" s="23" t="s">
-        <v>894</v>
-      </c>
-      <c r="H845" s="23"/>
-      <c r="I845" s="23"/>
-      <c r="J845" s="22"/>
-      <c r="K845" s="22"/>
-      <c r="L845" s="22"/>
-    </row>
-    <row r="846" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B846" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C846" s="25"/>
-      <c r="D846" s="22"/>
-      <c r="E846" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F846" s="25"/>
-      <c r="G846" s="23" t="s">
+    <row r="847" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A847" s="21" t="s">
         <v>895</v>
       </c>
-      <c r="H846" s="23"/>
-      <c r="I846" s="23"/>
-      <c r="J846" s="22"/>
-      <c r="K846" s="22"/>
-      <c r="L846" s="22"/>
-    </row>
-    <row r="847" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B847" s="22" t="s">
         <v>22</v>
       </c>
@@ -19694,10 +19714,14 @@
       <c r="L848" s="22"/>
     </row>
     <row r="849" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B849" s="25"/>
+      <c r="B849" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C849" s="25"/>
       <c r="D849" s="22"/>
-      <c r="E849" s="22"/>
+      <c r="E849" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="F849" s="25"/>
       <c r="G849" s="23" t="s">
         <v>898</v>
@@ -19709,10 +19733,14 @@
       <c r="L849" s="22"/>
     </row>
     <row r="850" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B850" s="25"/>
+      <c r="B850" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C850" s="25"/>
       <c r="D850" s="22"/>
-      <c r="E850" s="22"/>
+      <c r="E850" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="F850" s="25"/>
       <c r="G850" s="23" t="s">
         <v>899</v>
@@ -19724,14 +19752,10 @@
       <c r="L850" s="22"/>
     </row>
     <row r="851" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B851" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B851" s="25"/>
       <c r="C851" s="25"/>
       <c r="D851" s="22"/>
-      <c r="E851" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E851" s="22"/>
       <c r="F851" s="25"/>
       <c r="G851" s="23" t="s">
         <v>900</v>
@@ -19743,14 +19767,10 @@
       <c r="L851" s="22"/>
     </row>
     <row r="852" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B852" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B852" s="25"/>
       <c r="C852" s="25"/>
       <c r="D852" s="22"/>
-      <c r="E852" s="22" t="s">
-        <v>60</v>
-      </c>
+      <c r="E852" s="22"/>
       <c r="F852" s="25"/>
       <c r="G852" s="23" t="s">
         <v>901</v>
@@ -19767,9 +19787,7 @@
       </c>
       <c r="C853" s="25"/>
       <c r="D853" s="22"/>
-      <c r="E853" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E853" s="25"/>
       <c r="F853" s="25"/>
       <c r="G853" s="23" t="s">
         <v>902</v>
@@ -19800,103 +19818,119 @@
       <c r="L854" s="22"/>
     </row>
     <row r="855" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B855" s="22"/>
-      <c r="C855" s="22"/>
+      <c r="B855" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C855" s="25"/>
       <c r="D855" s="22"/>
-      <c r="E855" s="22"/>
-      <c r="F855" s="22"/>
-      <c r="G855" s="23"/>
+      <c r="E855" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F855" s="25"/>
+      <c r="G855" s="23" t="s">
+        <v>904</v>
+      </c>
       <c r="H855" s="23"/>
       <c r="I855" s="23"/>
       <c r="J855" s="22"/>
       <c r="K855" s="22"/>
       <c r="L855" s="22"/>
     </row>
-    <row r="856" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B856" s="22"/>
-      <c r="C856" s="22"/>
+    <row r="856" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B856" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C856" s="25"/>
       <c r="D856" s="22"/>
-      <c r="E856" s="22"/>
-      <c r="F856" s="22"/>
-      <c r="G856" s="23"/>
+      <c r="E856" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F856" s="25"/>
+      <c r="G856" s="23" t="s">
+        <v>905</v>
+      </c>
       <c r="H856" s="23"/>
       <c r="I856" s="23"/>
       <c r="J856" s="22"/>
       <c r="K856" s="22"/>
       <c r="L856" s="22"/>
     </row>
-    <row r="857" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B857" s="22"/>
-      <c r="C857" s="22"/>
+    <row r="857" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B857" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C857" s="25"/>
       <c r="D857" s="22"/>
-      <c r="E857" s="22"/>
-      <c r="F857" s="22"/>
-      <c r="G857" s="23"/>
+      <c r="E857" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F857" s="25"/>
+      <c r="G857" s="23" t="s">
+        <v>906</v>
+      </c>
       <c r="H857" s="23"/>
       <c r="I857" s="23"/>
       <c r="J857" s="22"/>
       <c r="K857" s="22"/>
       <c r="L857" s="22"/>
     </row>
-    <row r="858" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B858" s="1"/>
-      <c r="C858" s="1"/>
-      <c r="D858" s="1"/>
-      <c r="E858" s="1"/>
-      <c r="F858" s="1"/>
-      <c r="G858" s="1"/>
-      <c r="H858" s="1"/>
-      <c r="I858" s="1"/>
-      <c r="J858" s="1"/>
-      <c r="K858" s="1"/>
-      <c r="L858" s="1"/>
-      <c r="M858" s="1"/>
-      <c r="N858" s="1"/>
+    <row r="858" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B858" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C858" s="25"/>
+      <c r="D858" s="22"/>
+      <c r="E858" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F858" s="25"/>
+      <c r="G858" s="23" t="s">
+        <v>907</v>
+      </c>
+      <c r="H858" s="23"/>
+      <c r="I858" s="23"/>
+      <c r="J858" s="22"/>
+      <c r="K858" s="22"/>
+      <c r="L858" s="22"/>
     </row>
     <row r="859" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B859" s="1"/>
-      <c r="C859" s="1"/>
-      <c r="D859" s="1"/>
-      <c r="E859" s="1"/>
-      <c r="F859" s="1"/>
-      <c r="G859" s="1"/>
-      <c r="H859" s="1"/>
-      <c r="I859" s="1"/>
-      <c r="J859" s="1"/>
-      <c r="K859" s="1"/>
-      <c r="L859" s="1"/>
-      <c r="M859" s="1"/>
-      <c r="N859" s="1"/>
+      <c r="B859" s="22"/>
+      <c r="C859" s="22"/>
+      <c r="D859" s="22"/>
+      <c r="E859" s="22"/>
+      <c r="F859" s="22"/>
+      <c r="G859" s="23"/>
+      <c r="H859" s="23"/>
+      <c r="I859" s="23"/>
+      <c r="J859" s="22"/>
+      <c r="K859" s="22"/>
+      <c r="L859" s="22"/>
     </row>
     <row r="860" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B860" s="1"/>
-      <c r="C860" s="1"/>
-      <c r="D860" s="1"/>
-      <c r="E860" s="1"/>
-      <c r="F860" s="1"/>
-      <c r="G860" s="1"/>
-      <c r="H860" s="1"/>
-      <c r="I860" s="1"/>
-      <c r="J860" s="1"/>
-      <c r="K860" s="1"/>
-      <c r="L860" s="1"/>
-      <c r="M860" s="1"/>
-      <c r="N860" s="1"/>
+      <c r="B860" s="22"/>
+      <c r="C860" s="22"/>
+      <c r="D860" s="22"/>
+      <c r="E860" s="22"/>
+      <c r="F860" s="22"/>
+      <c r="G860" s="23"/>
+      <c r="H860" s="23"/>
+      <c r="I860" s="23"/>
+      <c r="J860" s="22"/>
+      <c r="K860" s="22"/>
+      <c r="L860" s="22"/>
     </row>
     <row r="861" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B861" s="1"/>
-      <c r="C861" s="1"/>
-      <c r="D861" s="1"/>
-      <c r="E861" s="1"/>
-      <c r="F861" s="1"/>
-      <c r="G861" s="1"/>
-      <c r="H861" s="1"/>
-      <c r="I861" s="1"/>
-      <c r="J861" s="1"/>
-      <c r="K861" s="1"/>
-      <c r="L861" s="1"/>
-      <c r="M861" s="1"/>
-      <c r="N861" s="1"/>
+      <c r="B861" s="22"/>
+      <c r="C861" s="22"/>
+      <c r="D861" s="22"/>
+      <c r="E861" s="22"/>
+      <c r="F861" s="22"/>
+      <c r="G861" s="23"/>
+      <c r="H861" s="23"/>
+      <c r="I861" s="23"/>
+      <c r="J861" s="22"/>
+      <c r="K861" s="22"/>
+      <c r="L861" s="22"/>
     </row>
     <row r="862" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B862" s="1"/>
@@ -19942,165 +19976,137 @@
       <c r="L864" s="1"/>
       <c r="M864" s="1"/>
       <c r="N864" s="1"/>
-      <c r="O864" s="1"/>
     </row>
     <row r="865" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A865" s="9"/>
+      <c r="B865" s="1"/>
+      <c r="C865" s="1"/>
+      <c r="D865" s="1"/>
+      <c r="E865" s="1"/>
+      <c r="F865" s="1"/>
+      <c r="G865" s="1"/>
+      <c r="H865" s="1"/>
+      <c r="I865" s="1"/>
+      <c r="J865" s="1"/>
+      <c r="K865" s="1"/>
+      <c r="L865" s="1"/>
+      <c r="M865" s="1"/>
+      <c r="N865" s="1"/>
     </row>
     <row r="866" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A866" s="16" t="s">
+      <c r="B866" s="1"/>
+      <c r="C866" s="1"/>
+      <c r="D866" s="1"/>
+      <c r="E866" s="1"/>
+      <c r="F866" s="1"/>
+      <c r="G866" s="1"/>
+      <c r="H866" s="1"/>
+      <c r="I866" s="1"/>
+      <c r="J866" s="1"/>
+      <c r="K866" s="1"/>
+      <c r="L866" s="1"/>
+      <c r="M866" s="1"/>
+      <c r="N866" s="1"/>
+    </row>
+    <row r="867" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B867" s="1"/>
+      <c r="C867" s="1"/>
+      <c r="D867" s="1"/>
+      <c r="E867" s="1"/>
+      <c r="F867" s="1"/>
+      <c r="G867" s="1"/>
+      <c r="H867" s="1"/>
+      <c r="I867" s="1"/>
+      <c r="J867" s="1"/>
+      <c r="K867" s="1"/>
+      <c r="L867" s="1"/>
+      <c r="M867" s="1"/>
+      <c r="N867" s="1"/>
+    </row>
+    <row r="868" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B868" s="1"/>
+      <c r="C868" s="1"/>
+      <c r="D868" s="1"/>
+      <c r="E868" s="1"/>
+      <c r="F868" s="1"/>
+      <c r="G868" s="1"/>
+      <c r="H868" s="1"/>
+      <c r="I868" s="1"/>
+      <c r="J868" s="1"/>
+      <c r="K868" s="1"/>
+      <c r="L868" s="1"/>
+      <c r="M868" s="1"/>
+      <c r="N868" s="1"/>
+      <c r="O868" s="1"/>
+    </row>
+    <row r="869" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A869" s="9"/>
+    </row>
+    <row r="870" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A870" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B866" s="17"/>
-      <c r="C866" s="18"/>
-      <c r="D866" s="18"/>
-      <c r="E866" s="18"/>
-      <c r="F866" s="18"/>
-    </row>
-    <row r="867" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A867" s="16" t="s">
-        <v>904</v>
-      </c>
-      <c r="B867" s="17"/>
-      <c r="C867" s="18"/>
-      <c r="D867" s="18"/>
-      <c r="E867" s="18"/>
-      <c r="F867" s="18"/>
-    </row>
-    <row r="868" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A868" s="16" t="s">
+      <c r="B870" s="17"/>
+      <c r="C870" s="18"/>
+      <c r="D870" s="18"/>
+      <c r="E870" s="18"/>
+      <c r="F870" s="18"/>
+    </row>
+    <row r="871" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A871" s="16" t="s">
+        <v>908</v>
+      </c>
+      <c r="B871" s="17"/>
+      <c r="C871" s="18"/>
+      <c r="D871" s="18"/>
+      <c r="E871" s="18"/>
+      <c r="F871" s="18"/>
+    </row>
+    <row r="872" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A872" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B868" s="17"/>
-      <c r="C868" s="18"/>
-      <c r="D868" s="18"/>
-      <c r="E868" s="18"/>
-      <c r="F868" s="18"/>
-    </row>
-    <row r="869" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A869" s="9"/>
-      <c r="B869" s="11" t="s">
+      <c r="B872" s="17"/>
+      <c r="C872" s="18"/>
+      <c r="D872" s="18"/>
+      <c r="E872" s="18"/>
+      <c r="F872" s="18"/>
+    </row>
+    <row r="873" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A873" s="9"/>
+      <c r="B873" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C869" s="11" t="s">
+      <c r="C873" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D869" s="11" t="s">
+      <c r="D873" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E869" s="11" t="s">
+      <c r="E873" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F869" s="11" t="s">
+      <c r="F873" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G869" s="20" t="s">
+      <c r="G873" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H869" s="20" t="s">
+      <c r="H873" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I869" s="20" t="s">
+      <c r="I873" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="870" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A870" s="21" t="s">
-        <v>905</v>
-      </c>
-      <c r="B870" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C870" s="25"/>
-      <c r="D870" s="22"/>
-      <c r="E870" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F870" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G870" s="23" t="s">
-        <v>906</v>
-      </c>
-      <c r="H870" s="23"/>
-      <c r="I870" s="23"/>
-    </row>
-    <row r="871" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A871" s="21"/>
-      <c r="B871" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C871" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D871" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E871" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F871" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G871" s="23" t="s">
-        <v>907</v>
-      </c>
-      <c r="H871" s="23"/>
-      <c r="I871" s="23"/>
-    </row>
-    <row r="872" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A872" s="9"/>
-      <c r="B872" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C872" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D872" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E872" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F872" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G872" s="23" t="s">
-        <v>908</v>
-      </c>
-      <c r="H872" s="23"/>
-      <c r="I872" s="23"/>
-    </row>
-    <row r="873" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A873" s="9"/>
-      <c r="B873" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C873" s="25"/>
-      <c r="D873" s="22"/>
-      <c r="E873" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F873" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G873" s="45" t="s">
+    <row r="874" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A874" s="21" t="s">
         <v>909</v>
       </c>
-      <c r="H873" s="23"/>
-      <c r="I873" s="23"/>
-    </row>
-    <row r="874" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A874" s="9"/>
       <c r="B874" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C874" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D874" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C874" s="25"/>
+      <c r="D874" s="22"/>
       <c r="E874" s="22" t="s">
         <v>22</v>
       </c>
@@ -20114,12 +20120,16 @@
       <c r="I874" s="23"/>
     </row>
     <row r="875" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A875" s="9"/>
+      <c r="A875" s="21"/>
       <c r="B875" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C875" s="25"/>
-      <c r="D875" s="22"/>
+      <c r="C875" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D875" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E875" s="22" t="s">
         <v>22</v>
       </c>
@@ -20137,8 +20147,12 @@
       <c r="B876" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C876" s="25"/>
-      <c r="D876" s="22"/>
+      <c r="C876" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D876" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E876" s="22" t="s">
         <v>22</v>
       </c>
@@ -20164,19 +20178,23 @@
       <c r="F877" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="G877" s="23" t="s">
+      <c r="G877" s="45" t="s">
         <v>913</v>
       </c>
       <c r="H877" s="23"/>
       <c r="I877" s="23"/>
     </row>
-    <row r="878" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="878" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A878" s="9"/>
       <c r="B878" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C878" s="25"/>
-      <c r="D878" s="22"/>
+      <c r="C878" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D878" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E878" s="22" t="s">
         <v>22</v>
       </c>
@@ -20187,11 +20205,9 @@
         <v>914</v>
       </c>
       <c r="H878" s="23"/>
-      <c r="I878" s="23" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="879" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I878" s="23"/>
+    </row>
+    <row r="879" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A879" s="9"/>
       <c r="B879" s="22" t="s">
         <v>22</v>
@@ -20215,9 +20231,7 @@
       <c r="B880" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C880" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C880" s="25"/>
       <c r="D880" s="22"/>
       <c r="E880" s="22" t="s">
         <v>22</v>
@@ -20231,7 +20245,7 @@
       <c r="H880" s="23"/>
       <c r="I880" s="23"/>
     </row>
-    <row r="881" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="881" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A881" s="9"/>
       <c r="B881" s="22" t="s">
         <v>22</v>
@@ -20267,7 +20281,9 @@
         <v>918</v>
       </c>
       <c r="H882" s="23"/>
-      <c r="I882" s="23"/>
+      <c r="I882" s="23" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="883" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A883" s="9"/>
@@ -20288,12 +20304,14 @@
       <c r="H883" s="23"/>
       <c r="I883" s="23"/>
     </row>
-    <row r="884" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="884" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A884" s="9"/>
       <c r="B884" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C884" s="25"/>
+      <c r="C884" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D884" s="22"/>
       <c r="E884" s="22" t="s">
         <v>22</v>
@@ -20313,9 +20331,7 @@
         <v>22</v>
       </c>
       <c r="C885" s="25"/>
-      <c r="D885" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D885" s="22"/>
       <c r="E885" s="22" t="s">
         <v>22</v>
       </c>
@@ -20328,17 +20344,13 @@
       <c r="H885" s="23"/>
       <c r="I885" s="23"/>
     </row>
-    <row r="886" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="886" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A886" s="9"/>
       <c r="B886" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C886" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D886" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C886" s="25"/>
+      <c r="D886" s="22"/>
       <c r="E886" s="22" t="s">
         <v>22</v>
       </c>
@@ -20351,17 +20363,13 @@
       <c r="H886" s="23"/>
       <c r="I886" s="23"/>
     </row>
-    <row r="887" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="887" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A887" s="9"/>
       <c r="B887" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C887" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D887" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C887" s="25"/>
+      <c r="D887" s="22"/>
       <c r="E887" s="22" t="s">
         <v>22</v>
       </c>
@@ -20374,17 +20382,13 @@
       <c r="H887" s="23"/>
       <c r="I887" s="23"/>
     </row>
-    <row r="888" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="888" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A888" s="9"/>
       <c r="B888" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C888" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D888" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C888" s="25"/>
+      <c r="D888" s="22"/>
       <c r="E888" s="22" t="s">
         <v>22</v>
       </c>
@@ -20397,13 +20401,15 @@
       <c r="H888" s="23"/>
       <c r="I888" s="23"/>
     </row>
-    <row r="889" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="889" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A889" s="9"/>
       <c r="B889" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C889" s="25"/>
-      <c r="D889" s="22"/>
+      <c r="D889" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E889" s="22" t="s">
         <v>22</v>
       </c>
@@ -20467,7 +20473,9 @@
       <c r="B892" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C892" s="25"/>
+      <c r="C892" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D892" s="22" t="s">
         <v>22</v>
       </c>
@@ -20489,9 +20497,7 @@
         <v>22</v>
       </c>
       <c r="C893" s="25"/>
-      <c r="D893" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D893" s="22"/>
       <c r="E893" s="22" t="s">
         <v>22</v>
       </c>
@@ -20504,16 +20510,16 @@
       <c r="H893" s="23"/>
       <c r="I893" s="23"/>
     </row>
-    <row r="894" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="894" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A894" s="9"/>
       <c r="B894" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C894" s="25"/>
-      <c r="D894" s="22"/>
-      <c r="E894" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D894" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E894" s="22"/>
       <c r="F894" s="22" t="s">
         <v>640</v>
       </c>
@@ -20528,7 +20534,9 @@
       <c r="B895" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C895" s="25"/>
+      <c r="C895" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D895" s="22" t="s">
         <v>22</v>
       </c>
@@ -20549,7 +20557,9 @@
       <c r="B896" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C896" s="25"/>
+      <c r="C896" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D896" s="22" t="s">
         <v>22</v>
       </c>
@@ -20591,9 +20601,7 @@
       <c r="B898" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C898" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C898" s="25"/>
       <c r="D898" s="22" t="s">
         <v>22</v>
       </c>
@@ -20609,17 +20617,13 @@
       <c r="H898" s="23"/>
       <c r="I898" s="23"/>
     </row>
-    <row r="899" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="899" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A899" s="9"/>
       <c r="B899" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C899" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D899" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C899" s="25"/>
+      <c r="D899" s="22"/>
       <c r="E899" s="22" t="s">
         <v>22</v>
       </c>
@@ -20638,7 +20642,9 @@
         <v>22</v>
       </c>
       <c r="C900" s="25"/>
-      <c r="D900" s="22"/>
+      <c r="D900" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E900" s="22" t="s">
         <v>22</v>
       </c>
@@ -20656,9 +20662,7 @@
       <c r="B901" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C901" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C901" s="25"/>
       <c r="D901" s="22" t="s">
         <v>22</v>
       </c>
@@ -20679,9 +20683,7 @@
       <c r="B902" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C902" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C902" s="25"/>
       <c r="D902" s="22" t="s">
         <v>22</v>
       </c>
@@ -20702,8 +20704,12 @@
       <c r="B903" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C903" s="25"/>
-      <c r="D903" s="22"/>
+      <c r="C903" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D903" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E903" s="22" t="s">
         <v>22</v>
       </c>
@@ -20809,12 +20815,8 @@
       <c r="B908" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C908" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D908" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C908" s="25"/>
+      <c r="D908" s="22"/>
       <c r="E908" s="22" t="s">
         <v>22</v>
       </c>
@@ -20855,12 +20857,8 @@
       <c r="B910" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C910" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D910" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C910" s="25"/>
+      <c r="D910" s="22"/>
       <c r="E910" s="22" t="s">
         <v>22</v>
       </c>
@@ -20878,8 +20876,12 @@
       <c r="B911" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C911" s="25"/>
-      <c r="D911" s="22"/>
+      <c r="C911" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D911" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E911" s="22" t="s">
         <v>22</v>
       </c>
@@ -20984,16 +20986,16 @@
       <c r="H915" s="23"/>
       <c r="I915" s="23"/>
     </row>
-    <row r="916" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="916" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A916" s="9"/>
-      <c r="B916" s="25" t="s">
-        <v>611</v>
+      <c r="B916" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="C916" s="25"/>
-      <c r="D916" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E916" s="25"/>
+      <c r="D916" s="22"/>
+      <c r="E916" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F916" s="22" t="s">
         <v>640</v>
       </c>
@@ -21001,9 +21003,7 @@
         <v>952</v>
       </c>
       <c r="H916" s="23"/>
-      <c r="I916" s="23" t="s">
-        <v>613</v>
-      </c>
+      <c r="I916" s="23"/>
     </row>
     <row r="917" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A917" s="9"/>
@@ -21097,20 +21097,16 @@
       <c r="H920" s="23"/>
       <c r="I920" s="23"/>
     </row>
-    <row r="921" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="921" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A921" s="9"/>
-      <c r="B921" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C921" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B921" s="25" t="s">
+        <v>611</v>
+      </c>
+      <c r="C921" s="25"/>
       <c r="D921" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E921" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E921" s="25"/>
       <c r="F921" s="22" t="s">
         <v>640</v>
       </c>
@@ -21118,7 +21114,9 @@
         <v>957</v>
       </c>
       <c r="H921" s="23"/>
-      <c r="I921" s="23"/>
+      <c r="I921" s="23" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="922" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A922" s="9"/>
@@ -21171,8 +21169,12 @@
       <c r="B924" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C924" s="25"/>
-      <c r="D924" s="22"/>
+      <c r="C924" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D924" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E924" s="22" t="s">
         <v>22</v>
       </c>
@@ -21186,11 +21188,16 @@
       <c r="I924" s="23"/>
     </row>
     <row r="925" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A925" s="9"/>
       <c r="B925" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C925" s="25"/>
-      <c r="D925" s="22"/>
+      <c r="C925" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D925" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E925" s="22" t="s">
         <v>22</v>
       </c>
@@ -21204,11 +21211,16 @@
       <c r="I925" s="23"/>
     </row>
     <row r="926" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A926" s="9"/>
       <c r="B926" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C926" s="25"/>
-      <c r="D926" s="22"/>
+      <c r="C926" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D926" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E926" s="22" t="s">
         <v>22</v>
       </c>
@@ -21222,6 +21234,7 @@
       <c r="I926" s="23"/>
     </row>
     <row r="927" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A927" s="9"/>
       <c r="B927" s="22" t="s">
         <v>22</v>
       </c>
@@ -21244,6 +21257,7 @@
       <c r="I927" s="23"/>
     </row>
     <row r="928" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A928" s="9"/>
       <c r="B928" s="22" t="s">
         <v>22</v>
       </c>
@@ -21266,23 +21280,20 @@
       <c r="I928" s="23"/>
     </row>
     <row r="929" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A929" s="9"/>
       <c r="B929" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C929" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D929" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C929" s="25"/>
+      <c r="D929" s="22"/>
       <c r="E929" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F929" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G929" s="23" t="s">
         <v>965</v>
-      </c>
-      <c r="G929" s="23" t="s">
-        <v>966</v>
       </c>
       <c r="H929" s="23"/>
       <c r="I929" s="23"/>
@@ -21292,48 +21303,44 @@
         <v>22</v>
       </c>
       <c r="C930" s="25"/>
-      <c r="D930" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D930" s="22"/>
       <c r="E930" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F930" s="22" t="s">
-        <v>965</v>
+        <v>640</v>
       </c>
       <c r="G930" s="23" t="s">
+        <v>966</v>
+      </c>
+      <c r="H930" s="23"/>
+      <c r="I930" s="23"/>
+    </row>
+    <row r="931" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B931" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C931" s="25"/>
+      <c r="D931" s="22"/>
+      <c r="E931" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F931" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G931" s="23" t="s">
         <v>967</v>
       </c>
-      <c r="H930" s="23"/>
-      <c r="I930" s="23" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="931" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B931" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="C931" s="27"/>
-      <c r="D931" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="E931" s="27"/>
-      <c r="F931" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="G931" s="28" t="s">
-        <v>969</v>
-      </c>
-      <c r="H931" s="28"/>
-      <c r="I931" s="28" t="s">
-        <v>970</v>
-      </c>
+      <c r="H931" s="23"/>
+      <c r="I931" s="23"/>
     </row>
     <row r="932" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B932" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C932" s="25"/>
+      <c r="C932" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D932" s="22" t="s">
         <v>22</v>
       </c>
@@ -21341,41 +21348,142 @@
         <v>22</v>
       </c>
       <c r="F932" s="22" t="s">
-        <v>965</v>
+        <v>640</v>
       </c>
       <c r="G932" s="23" t="s">
+        <v>968</v>
+      </c>
+      <c r="H932" s="23"/>
+      <c r="I932" s="23"/>
+    </row>
+    <row r="933" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B933" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C933" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D933" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E933" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F933" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="G933" s="23" t="s">
+        <v>969</v>
+      </c>
+      <c r="H933" s="23"/>
+      <c r="I933" s="23"/>
+    </row>
+    <row r="934" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B934" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C934" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D934" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E934" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F934" s="22" t="s">
+        <v>970</v>
+      </c>
+      <c r="G934" s="23" t="s">
         <v>971</v>
       </c>
-      <c r="H932" s="23"/>
-      <c r="I932" s="23" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="933" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B933" s="27" t="s">
+      <c r="H934" s="23"/>
+      <c r="I934" s="23"/>
+    </row>
+    <row r="935" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B935" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C935" s="25"/>
+      <c r="D935" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E935" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F935" s="22" t="s">
+        <v>970</v>
+      </c>
+      <c r="G935" s="23" t="s">
+        <v>972</v>
+      </c>
+      <c r="H935" s="23"/>
+      <c r="I935" s="23" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="936" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B936" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="C933" s="27"/>
-      <c r="D933" s="27" t="s">
+      <c r="C936" s="27"/>
+      <c r="D936" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="E933" s="27"/>
-      <c r="F933" s="27" t="s">
+      <c r="E936" s="27"/>
+      <c r="F936" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="G933" s="28" t="s">
-        <v>972</v>
-      </c>
-      <c r="H933" s="28"/>
-      <c r="I933" s="28" t="s">
+      <c r="G936" s="28" t="s">
+        <v>974</v>
+      </c>
+      <c r="H936" s="28"/>
+      <c r="I936" s="28" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="937" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B937" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C937" s="25"/>
+      <c r="D937" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E937" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F937" s="22" t="s">
         <v>970</v>
       </c>
-    </row>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G937" s="23" t="s">
+        <v>976</v>
+      </c>
+      <c r="H937" s="23"/>
+      <c r="I937" s="23" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="938" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B938" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="C938" s="27"/>
+      <c r="D938" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="E938" s="27"/>
+      <c r="F938" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="G938" s="28" t="s">
+        <v>977</v>
+      </c>
+      <c r="H938" s="28"/>
+      <c r="I938" s="28" t="s">
+        <v>975</v>
+      </c>
+    </row>
     <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Misc state space updates
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4004" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4010" uniqueCount="1039">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -2281,6 +2281,9 @@
     <t xml:space="preserve">LinearQuadraticRegulator_LatencyCompensate.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">Routine exists, but it only has interger raise matrix to power.</t>
+  </si>
+  <si>
     <t xml:space="preserve">LinearQuadraticRegulator_New_ELMS.vi</t>
   </si>
   <si>
@@ -2656,9 +2659,6 @@
     <t xml:space="preserve">LinearSystemSim_SetInput_Single.vi</t>
   </si>
   <si>
-    <t xml:space="preserve">NEED TO CLAMP !!</t>
-  </si>
-  <si>
     <t xml:space="preserve">LinearSystemSim_Update.vi</t>
   </si>
   <si>
@@ -2677,6 +2677,9 @@
     <t xml:space="preserve">LinearSystemSim_SetInput_Array.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">Doesn’t use clamp ?</t>
+  </si>
+  <si>
     <t xml:space="preserve">LinearSystemSim_Setstate.vi</t>
   </si>
   <si>
@@ -2759,6 +2762,12 @@
   </si>
   <si>
     <t xml:space="preserve">Matrix_SetColumn.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matrix_Pow.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This uses the NI matrix routine which only raises to integer values.</t>
   </si>
   <si>
     <t xml:space="preserve">MATRIX HELPER</t>
@@ -3191,7 +3200,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3231,7 +3240,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF3333"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -3250,12 +3259,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFEEEEEE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3333"/>
-        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -3496,8 +3499,8 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3556,7 +3559,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -3580,7 +3583,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3671,28 +3674,28 @@
         <v>11</v>
       </c>
       <c r="B9" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1342,"X")</f>
-        <v>650</v>
+        <f aca="false">COUNTIF(B18:B1343,"X")</f>
+        <v>654</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C18:C1342,"X")</f>
+        <f aca="false">COUNTIF(C18:C1343,"X")</f>
         <v>368</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D18:D1342,"X")</f>
+        <f aca="false">COUNTIF(D18:D1343,"X")</f>
         <v>172</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E18:E1342,"X")</f>
+        <f aca="false">COUNTIF(E18:E1343,"X")</f>
         <v>555</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F18:F1342,"S")+COUNTIF(F18:F1342,"I")+COUNTIF(F18:F1342,"X")+COUNTIF(F18:F1342,"SI")+COUNTIF(F18:F1342,"IS")+COUNTIF(F18:F1342,"N/A")</f>
+        <f aca="false">COUNTIF(F18:F1343,"S")+COUNTIF(F18:F1343,"I")+COUNTIF(F18:F1343,"X")+COUNTIF(F18:F1343,"SI")+COUNTIF(F18:F1343,"IS")+COUNTIF(F18:F1343,"N/A")</f>
         <v>221</v>
       </c>
       <c r="G9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.566153846153846</v>
+        <v>0.562691131498471</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3700,7 +3703,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="13" t="n">
-        <f aca="false">COUNTIF(B19:B1343,"/")</f>
+        <f aca="false">COUNTIF(B19:B1344,"/")</f>
         <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -3710,7 +3713,7 @@
     <row r="11" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.34</v>
+        <v>0.337920489296636</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16266,7 +16269,7 @@
       <c r="K671" s="22"/>
       <c r="L671" s="22"/>
     </row>
-    <row r="672" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="672" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B672" s="27" t="s">
         <v>611</v>
       </c>
@@ -16281,7 +16284,7 @@
       </c>
       <c r="H672" s="23"/>
       <c r="I672" s="23" t="s">
-        <v>613</v>
+        <v>752</v>
       </c>
       <c r="J672" s="22"/>
       <c r="K672" s="22"/>
@@ -16298,7 +16301,7 @@
       </c>
       <c r="F673" s="25"/>
       <c r="G673" s="23" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="H673" s="23"/>
       <c r="I673" s="23"/>
@@ -16313,7 +16316,7 @@
       <c r="E674" s="25"/>
       <c r="F674" s="25"/>
       <c r="G674" s="23" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="H674" s="23"/>
       <c r="I674" s="23"/>
@@ -16332,7 +16335,7 @@
       </c>
       <c r="F675" s="25"/>
       <c r="G675" s="23" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="H675" s="23"/>
       <c r="I675" s="23"/>
@@ -16351,7 +16354,7 @@
       </c>
       <c r="F676" s="25"/>
       <c r="G676" s="23" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="H676" s="23"/>
       <c r="I676" s="23"/>
@@ -16370,7 +16373,7 @@
       </c>
       <c r="F677" s="25"/>
       <c r="G677" s="23" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="H677" s="23"/>
       <c r="I677" s="23"/>
@@ -16442,7 +16445,7 @@
     </row>
     <row r="681" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="21" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B681" s="22" t="s">
         <v>22</v>
@@ -16454,7 +16457,7 @@
       </c>
       <c r="F681" s="25"/>
       <c r="G681" s="23" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="H681" s="23"/>
       <c r="I681" s="23"/>
@@ -16473,7 +16476,7 @@
       </c>
       <c r="F682" s="25"/>
       <c r="G682" s="23" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="H682" s="23"/>
       <c r="I682" s="23"/>
@@ -16492,7 +16495,7 @@
       </c>
       <c r="F683" s="25"/>
       <c r="G683" s="23" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="H683" s="23"/>
       <c r="I683" s="23"/>
@@ -16511,7 +16514,7 @@
       </c>
       <c r="F684" s="25"/>
       <c r="G684" s="23" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="H684" s="23"/>
       <c r="I684" s="23"/>
@@ -16530,7 +16533,7 @@
       </c>
       <c r="F685" s="25"/>
       <c r="G685" s="23" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="H685" s="23"/>
       <c r="I685" s="23"/>
@@ -16549,7 +16552,7 @@
       </c>
       <c r="F686" s="25"/>
       <c r="G686" s="23" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="H686" s="23"/>
       <c r="I686" s="23"/>
@@ -16568,7 +16571,7 @@
       </c>
       <c r="F687" s="25"/>
       <c r="G687" s="23" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="H687" s="23"/>
       <c r="I687" s="23"/>
@@ -16587,7 +16590,7 @@
       </c>
       <c r="F688" s="25"/>
       <c r="G688" s="23" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="H688" s="23"/>
       <c r="I688" s="23"/>
@@ -16606,7 +16609,7 @@
       </c>
       <c r="F689" s="25"/>
       <c r="G689" s="23" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H689" s="23"/>
       <c r="I689" s="23"/>
@@ -16625,7 +16628,7 @@
       </c>
       <c r="F690" s="25"/>
       <c r="G690" s="23" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="H690" s="23"/>
       <c r="I690" s="23"/>
@@ -16644,7 +16647,7 @@
       </c>
       <c r="F691" s="25"/>
       <c r="G691" s="23" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="H691" s="23"/>
       <c r="I691" s="23"/>
@@ -16729,7 +16732,7 @@
     </row>
     <row r="696" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="21" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B696" s="22" t="s">
         <v>22</v>
@@ -16741,7 +16744,7 @@
       </c>
       <c r="F696" s="25"/>
       <c r="G696" s="23" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H696" s="23"/>
       <c r="I696" s="23"/>
@@ -16760,7 +16763,7 @@
       </c>
       <c r="F697" s="25"/>
       <c r="G697" s="23" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H697" s="23"/>
       <c r="I697" s="23"/>
@@ -16775,7 +16778,7 @@
       <c r="E698" s="25"/>
       <c r="F698" s="25"/>
       <c r="G698" s="23" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="H698" s="23"/>
       <c r="I698" s="23"/>
@@ -16794,7 +16797,7 @@
       </c>
       <c r="F699" s="25"/>
       <c r="G699" s="23" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="H699" s="23"/>
       <c r="I699" s="23"/>
@@ -16813,7 +16816,7 @@
       </c>
       <c r="F700" s="25"/>
       <c r="G700" s="23" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="H700" s="23"/>
       <c r="I700" s="23"/>
@@ -16832,7 +16835,7 @@
       </c>
       <c r="F701" s="25"/>
       <c r="G701" s="23" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="H701" s="23"/>
       <c r="I701" s="23"/>
@@ -16851,7 +16854,7 @@
       </c>
       <c r="F702" s="25"/>
       <c r="G702" s="23" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="H702" s="23"/>
       <c r="I702" s="23"/>
@@ -16870,7 +16873,7 @@
       </c>
       <c r="F703" s="25"/>
       <c r="G703" s="23" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="H703" s="23"/>
       <c r="I703" s="23"/>
@@ -16889,7 +16892,7 @@
       </c>
       <c r="F704" s="25"/>
       <c r="G704" s="23" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="H704" s="23"/>
       <c r="I704" s="23"/>
@@ -16908,7 +16911,7 @@
       </c>
       <c r="F705" s="25"/>
       <c r="G705" s="23" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="H705" s="23"/>
       <c r="I705" s="23"/>
@@ -16927,7 +16930,7 @@
       </c>
       <c r="F706" s="25"/>
       <c r="G706" s="23" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="H706" s="23"/>
       <c r="I706" s="23"/>
@@ -16946,7 +16949,7 @@
       </c>
       <c r="F707" s="25"/>
       <c r="G707" s="23" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="H707" s="23"/>
       <c r="I707" s="23"/>
@@ -16965,7 +16968,7 @@
       </c>
       <c r="F708" s="25"/>
       <c r="G708" s="23" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="H708" s="23"/>
       <c r="I708" s="23"/>
@@ -16984,7 +16987,7 @@
       </c>
       <c r="F709" s="25"/>
       <c r="G709" s="23" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="H709" s="23"/>
       <c r="I709" s="23"/>
@@ -16999,7 +17002,7 @@
       <c r="E710" s="22"/>
       <c r="F710" s="25"/>
       <c r="G710" s="23" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="H710" s="23"/>
       <c r="I710" s="23"/>
@@ -17008,13 +17011,13 @@
       <c r="L710" s="22"/>
     </row>
     <row r="711" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B711" s="25"/>
+      <c r="B711" s="27"/>
       <c r="C711" s="25"/>
       <c r="D711" s="22"/>
       <c r="E711" s="22"/>
       <c r="F711" s="25"/>
       <c r="G711" s="23" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="H711" s="23"/>
       <c r="I711" s="23"/>
@@ -17033,7 +17036,7 @@
       </c>
       <c r="F712" s="25"/>
       <c r="G712" s="23" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="H712" s="23"/>
       <c r="I712" s="23"/>
@@ -17052,7 +17055,7 @@
       </c>
       <c r="F713" s="25"/>
       <c r="G713" s="23" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="H713" s="23"/>
       <c r="I713" s="23"/>
@@ -17071,7 +17074,7 @@
       </c>
       <c r="F714" s="25"/>
       <c r="G714" s="23" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="H714" s="23"/>
       <c r="I714" s="23"/>
@@ -17090,7 +17093,7 @@
       </c>
       <c r="F715" s="25"/>
       <c r="G715" s="23" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="H715" s="23"/>
       <c r="I715" s="23"/>
@@ -17099,13 +17102,13 @@
       <c r="L715" s="22"/>
     </row>
     <row r="716" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B716" s="25"/>
+      <c r="B716" s="27"/>
       <c r="C716" s="25"/>
       <c r="D716" s="22"/>
       <c r="E716" s="22"/>
       <c r="F716" s="25"/>
       <c r="G716" s="23" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="H716" s="23"/>
       <c r="I716" s="23"/>
@@ -17114,13 +17117,13 @@
       <c r="L716" s="22"/>
     </row>
     <row r="717" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B717" s="25"/>
+      <c r="B717" s="27"/>
       <c r="C717" s="25"/>
       <c r="D717" s="22"/>
       <c r="E717" s="22"/>
       <c r="F717" s="25"/>
       <c r="G717" s="23" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="H717" s="23"/>
       <c r="I717" s="23"/>
@@ -17139,7 +17142,7 @@
       </c>
       <c r="F718" s="25"/>
       <c r="G718" s="23" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="H718" s="23"/>
       <c r="I718" s="23"/>
@@ -17154,7 +17157,7 @@
       <c r="E719" s="22"/>
       <c r="F719" s="25"/>
       <c r="G719" s="23" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="H719" s="23"/>
       <c r="I719" s="23"/>
@@ -17169,7 +17172,7 @@
       <c r="E720" s="22"/>
       <c r="F720" s="25"/>
       <c r="G720" s="23" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="H720" s="23"/>
       <c r="I720" s="23"/>
@@ -17221,7 +17224,7 @@
     </row>
     <row r="724" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A724" s="16" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B724" s="43"/>
       <c r="C724" s="18"/>
@@ -17302,7 +17305,7 @@
     </row>
     <row r="728" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A728" s="21" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B728" s="22" t="s">
         <v>22</v>
@@ -17314,7 +17317,7 @@
       </c>
       <c r="F728" s="25"/>
       <c r="G728" s="23" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="H728" s="23"/>
       <c r="I728" s="23"/>
@@ -17334,7 +17337,7 @@
       </c>
       <c r="F729" s="25"/>
       <c r="G729" s="23" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="H729" s="23"/>
       <c r="I729" s="23"/>
@@ -17354,7 +17357,7 @@
       </c>
       <c r="F730" s="25"/>
       <c r="G730" s="23" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="H730" s="23"/>
       <c r="I730" s="23"/>
@@ -17374,7 +17377,7 @@
       </c>
       <c r="F731" s="25"/>
       <c r="G731" s="23" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="H731" s="23"/>
       <c r="I731" s="23"/>
@@ -17394,7 +17397,7 @@
       </c>
       <c r="F732" s="25"/>
       <c r="G732" s="23" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H732" s="23"/>
       <c r="I732" s="23"/>
@@ -17467,7 +17470,7 @@
     </row>
     <row r="736" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A736" s="21" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B736" s="22" t="s">
         <v>22</v>
@@ -17479,7 +17482,7 @@
       </c>
       <c r="F736" s="25"/>
       <c r="G736" s="23" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="H736" s="23"/>
       <c r="I736" s="23"/>
@@ -17498,7 +17501,7 @@
       </c>
       <c r="F737" s="25"/>
       <c r="G737" s="23" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="H737" s="23"/>
       <c r="I737" s="23"/>
@@ -17517,7 +17520,7 @@
       </c>
       <c r="F738" s="25"/>
       <c r="G738" s="23" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="H738" s="23"/>
       <c r="I738" s="23"/>
@@ -17526,13 +17529,15 @@
       <c r="L738" s="22"/>
     </row>
     <row r="739" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B739" s="25"/>
+      <c r="B739" s="27" t="s">
+        <v>611</v>
+      </c>
       <c r="C739" s="25"/>
       <c r="D739" s="22"/>
       <c r="E739" s="22"/>
       <c r="F739" s="25"/>
       <c r="G739" s="23" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="H739" s="23"/>
       <c r="I739" s="23"/>
@@ -17551,7 +17556,7 @@
       </c>
       <c r="F740" s="25"/>
       <c r="G740" s="23" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="H740" s="23"/>
       <c r="I740" s="23"/>
@@ -17570,7 +17575,7 @@
       </c>
       <c r="F741" s="25"/>
       <c r="G741" s="23" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="H741" s="23"/>
       <c r="I741" s="23" t="s">
@@ -17591,7 +17596,7 @@
       </c>
       <c r="F742" s="25"/>
       <c r="G742" s="23" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="H742" s="23"/>
       <c r="I742" s="23"/>
@@ -17610,7 +17615,7 @@
       </c>
       <c r="F743" s="25"/>
       <c r="G743" s="23" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="H743" s="23"/>
       <c r="I743" s="23"/>
@@ -17629,7 +17634,7 @@
       </c>
       <c r="F744" s="25"/>
       <c r="G744" s="23" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="H744" s="23"/>
       <c r="I744" s="23"/>
@@ -17682,7 +17687,7 @@
     </row>
     <row r="748" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A748" s="16" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="B748" s="43"/>
       <c r="C748" s="18"/>
@@ -17775,7 +17780,7 @@
     </row>
     <row r="752" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A752" s="21" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B752" s="22" t="s">
         <v>22</v>
@@ -17787,7 +17792,7 @@
       </c>
       <c r="F752" s="25"/>
       <c r="G752" s="23" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="H752" s="23"/>
       <c r="I752" s="23"/>
@@ -17810,7 +17815,7 @@
       </c>
       <c r="F753" s="25"/>
       <c r="G753" s="23" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="H753" s="23"/>
       <c r="I753" s="23"/>
@@ -17878,7 +17883,7 @@
     </row>
     <row r="756" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A756" s="21" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B756" s="22" t="s">
         <v>22</v>
@@ -17888,7 +17893,7 @@
       <c r="E756" s="25"/>
       <c r="F756" s="25"/>
       <c r="G756" s="23" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="H756" s="23"/>
       <c r="I756" s="23"/>
@@ -17909,7 +17914,7 @@
       <c r="E757" s="25"/>
       <c r="F757" s="25"/>
       <c r="G757" s="23" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="H757" s="23"/>
       <c r="I757" s="23"/>
@@ -17930,7 +17935,7 @@
       <c r="E758" s="25"/>
       <c r="F758" s="25"/>
       <c r="G758" s="23" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="H758" s="23"/>
       <c r="I758" s="23"/>
@@ -17951,7 +17956,7 @@
       <c r="E759" s="25"/>
       <c r="F759" s="25"/>
       <c r="G759" s="23" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="H759" s="23"/>
       <c r="I759" s="23"/>
@@ -17972,7 +17977,7 @@
       <c r="E760" s="25"/>
       <c r="F760" s="25"/>
       <c r="G760" s="23" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="H760" s="23"/>
       <c r="I760" s="23"/>
@@ -17993,7 +17998,7 @@
       <c r="E761" s="25"/>
       <c r="F761" s="25"/>
       <c r="G761" s="23" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="H761" s="23"/>
       <c r="I761" s="23"/>
@@ -18014,7 +18019,7 @@
       <c r="E762" s="25"/>
       <c r="F762" s="25"/>
       <c r="G762" s="23" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="H762" s="23"/>
       <c r="I762" s="23"/>
@@ -18035,7 +18040,7 @@
       <c r="E763" s="25"/>
       <c r="F763" s="25"/>
       <c r="G763" s="23" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="H763" s="23"/>
       <c r="I763" s="23"/>
@@ -18056,7 +18061,7 @@
       <c r="E764" s="25"/>
       <c r="F764" s="25"/>
       <c r="G764" s="23" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="H764" s="23"/>
       <c r="I764" s="23"/>
@@ -18077,7 +18082,7 @@
       <c r="E765" s="25"/>
       <c r="F765" s="25"/>
       <c r="G765" s="23" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="H765" s="23"/>
       <c r="I765" s="23"/>
@@ -18098,7 +18103,7 @@
       <c r="E766" s="25"/>
       <c r="F766" s="25"/>
       <c r="G766" s="23" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="H766" s="23"/>
       <c r="I766" s="23"/>
@@ -18119,7 +18124,7 @@
       <c r="E767" s="25"/>
       <c r="F767" s="25"/>
       <c r="G767" s="23" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H767" s="23"/>
       <c r="I767" s="23"/>
@@ -18140,7 +18145,7 @@
       <c r="E768" s="25"/>
       <c r="F768" s="25"/>
       <c r="G768" s="23" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="H768" s="23"/>
       <c r="I768" s="23"/>
@@ -18161,7 +18166,7 @@
       <c r="E769" s="25"/>
       <c r="F769" s="25"/>
       <c r="G769" s="23" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="H769" s="23"/>
       <c r="I769" s="23"/>
@@ -18182,7 +18187,7 @@
       <c r="E770" s="25"/>
       <c r="F770" s="25"/>
       <c r="G770" s="23" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="H770" s="23"/>
       <c r="I770" s="23"/>
@@ -18203,7 +18208,7 @@
       <c r="E771" s="25"/>
       <c r="F771" s="25"/>
       <c r="G771" s="23" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="H771" s="23"/>
       <c r="I771" s="23"/>
@@ -18224,7 +18229,7 @@
       <c r="E772" s="25"/>
       <c r="F772" s="25"/>
       <c r="G772" s="23" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="H772" s="23"/>
       <c r="I772" s="23"/>
@@ -18245,7 +18250,7 @@
       <c r="E773" s="25"/>
       <c r="F773" s="25"/>
       <c r="G773" s="23" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="H773" s="23"/>
       <c r="I773" s="23"/>
@@ -18266,7 +18271,7 @@
       <c r="E774" s="25"/>
       <c r="F774" s="25"/>
       <c r="G774" s="23" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="H774" s="23"/>
       <c r="I774" s="23"/>
@@ -18287,7 +18292,7 @@
       <c r="E775" s="25"/>
       <c r="F775" s="25"/>
       <c r="G775" s="23" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="H775" s="23"/>
       <c r="I775" s="23"/>
@@ -18308,7 +18313,7 @@
       <c r="E776" s="25"/>
       <c r="F776" s="25"/>
       <c r="G776" s="23" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="H776" s="23"/>
       <c r="I776" s="23"/>
@@ -18329,7 +18334,7 @@
       <c r="E777" s="25"/>
       <c r="F777" s="25"/>
       <c r="G777" s="23" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="H777" s="23"/>
       <c r="I777" s="23"/>
@@ -18350,7 +18355,7 @@
       <c r="E778" s="25"/>
       <c r="F778" s="25"/>
       <c r="G778" s="23" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="H778" s="23"/>
       <c r="I778" s="23"/>
@@ -18371,7 +18376,7 @@
       <c r="E779" s="25"/>
       <c r="F779" s="25"/>
       <c r="G779" s="23" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="H779" s="23"/>
       <c r="I779" s="23"/>
@@ -18392,7 +18397,7 @@
       <c r="E780" s="25"/>
       <c r="F780" s="25"/>
       <c r="G780" s="23" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="H780" s="23"/>
       <c r="I780" s="23"/>
@@ -18413,7 +18418,7 @@
       <c r="E781" s="25"/>
       <c r="F781" s="25"/>
       <c r="G781" s="23" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="H781" s="23"/>
       <c r="I781" s="23"/>
@@ -18434,7 +18439,7 @@
       <c r="E782" s="25"/>
       <c r="F782" s="25"/>
       <c r="G782" s="23" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="H782" s="23"/>
       <c r="I782" s="23"/>
@@ -18455,7 +18460,7 @@
       <c r="E783" s="25"/>
       <c r="F783" s="25"/>
       <c r="G783" s="23" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H783" s="23"/>
       <c r="I783" s="23"/>
@@ -18542,7 +18547,7 @@
     </row>
     <row r="787" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A787" s="21" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B787" s="22" t="s">
         <v>22</v>
@@ -18554,7 +18559,7 @@
       </c>
       <c r="F787" s="25"/>
       <c r="G787" s="23" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="H787" s="23"/>
       <c r="I787" s="23"/>
@@ -18577,7 +18582,7 @@
       </c>
       <c r="F788" s="25"/>
       <c r="G788" s="23" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="H788" s="23"/>
       <c r="I788" s="23"/>
@@ -18599,7 +18604,7 @@
       </c>
       <c r="F789" s="25"/>
       <c r="G789" s="23" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="H789" s="23"/>
       <c r="I789" s="23"/>
@@ -18621,7 +18626,7 @@
       </c>
       <c r="F790" s="25"/>
       <c r="G790" s="23" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="H790" s="23"/>
       <c r="I790" s="23"/>
@@ -18643,7 +18648,7 @@
       </c>
       <c r="F791" s="25"/>
       <c r="G791" s="23" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="H791" s="23"/>
       <c r="I791" s="23"/>
@@ -18665,7 +18670,7 @@
       </c>
       <c r="F792" s="25"/>
       <c r="G792" s="23" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="H792" s="23"/>
       <c r="I792" s="23"/>
@@ -18687,7 +18692,7 @@
       </c>
       <c r="F793" s="25"/>
       <c r="G793" s="23" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="H793" s="23"/>
       <c r="I793" s="23"/>
@@ -18709,7 +18714,7 @@
       </c>
       <c r="F794" s="25"/>
       <c r="G794" s="23" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="H794" s="23"/>
       <c r="I794" s="23"/>
@@ -18733,11 +18738,11 @@
       </c>
       <c r="F795" s="25"/>
       <c r="G795" s="23" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="H795" s="23"/>
       <c r="I795" s="23" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="J795" s="22"/>
       <c r="K795" s="22"/>
@@ -18757,7 +18762,7 @@
       </c>
       <c r="F796" s="25"/>
       <c r="G796" s="23" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="H796" s="23"/>
       <c r="I796" s="23"/>
@@ -18779,7 +18784,7 @@
       </c>
       <c r="F797" s="25"/>
       <c r="G797" s="23" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H797" s="23"/>
       <c r="I797" s="23"/>
@@ -18801,7 +18806,7 @@
       <c r="E798" s="25"/>
       <c r="F798" s="25"/>
       <c r="G798" s="23" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H798" s="23"/>
       <c r="I798" s="23"/>
@@ -18819,7 +18824,7 @@
       <c r="E799" s="25"/>
       <c r="F799" s="25"/>
       <c r="G799" s="23" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="H799" s="23"/>
       <c r="I799" s="23"/>
@@ -18837,7 +18842,7 @@
       <c r="E800" s="25"/>
       <c r="F800" s="25"/>
       <c r="G800" s="23" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="H800" s="23"/>
       <c r="I800" s="23"/>
@@ -18855,7 +18860,7 @@
       <c r="E801" s="25"/>
       <c r="F801" s="25"/>
       <c r="G801" s="23" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="H801" s="23"/>
       <c r="I801" s="23"/>
@@ -18923,7 +18928,7 @@
     </row>
     <row r="804" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A804" s="21" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B804" s="22" t="s">
         <v>22</v>
@@ -18935,7 +18940,7 @@
       </c>
       <c r="F804" s="25"/>
       <c r="G804" s="23" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="H804" s="23"/>
       <c r="I804" s="23"/>
@@ -18958,7 +18963,7 @@
       </c>
       <c r="F805" s="25"/>
       <c r="G805" s="23" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="H805" s="23"/>
       <c r="I805" s="23"/>
@@ -18981,7 +18986,7 @@
       </c>
       <c r="F806" s="25"/>
       <c r="G806" s="23" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="H806" s="23"/>
       <c r="I806" s="23"/>
@@ -19004,7 +19009,7 @@
       </c>
       <c r="F807" s="25"/>
       <c r="G807" s="23" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H807" s="23"/>
       <c r="I807" s="23"/>
@@ -19027,7 +19032,7 @@
       </c>
       <c r="F808" s="25"/>
       <c r="G808" s="23" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="H808" s="23"/>
       <c r="I808" s="23"/>
@@ -19050,7 +19055,7 @@
       </c>
       <c r="F809" s="25"/>
       <c r="G809" s="23" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="H809" s="23"/>
       <c r="I809" s="23"/>
@@ -19069,7 +19074,7 @@
       <c r="E810" s="22"/>
       <c r="F810" s="25"/>
       <c r="G810" s="23" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="H810" s="23"/>
       <c r="I810" s="23" t="s">
@@ -19090,7 +19095,7 @@
       <c r="E811" s="22"/>
       <c r="F811" s="25"/>
       <c r="G811" s="23" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="H811" s="23"/>
       <c r="I811" s="23" t="s">
@@ -19111,7 +19116,7 @@
       <c r="E812" s="22"/>
       <c r="F812" s="25"/>
       <c r="G812" s="23" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="H812" s="23"/>
       <c r="I812" s="23" t="s">
@@ -19198,7 +19203,7 @@
     </row>
     <row r="816" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A816" s="21" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B816" s="22" t="s">
         <v>22</v>
@@ -19210,7 +19215,7 @@
       </c>
       <c r="F816" s="25"/>
       <c r="G816" s="23" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H816" s="23"/>
       <c r="I816" s="23"/>
@@ -19233,7 +19238,7 @@
       </c>
       <c r="F817" s="25"/>
       <c r="G817" s="23" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="H817" s="23"/>
       <c r="I817" s="23"/>
@@ -19256,7 +19261,7 @@
       </c>
       <c r="F818" s="25"/>
       <c r="G818" s="23" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="H818" s="23"/>
       <c r="I818" s="23"/>
@@ -19267,7 +19272,7 @@
       <c r="N818" s="1"/>
       <c r="O818" s="1"/>
     </row>
-    <row r="819" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="819" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A819" s="21"/>
       <c r="B819" s="22" t="s">
         <v>22</v>
@@ -19279,12 +19284,10 @@
       </c>
       <c r="F819" s="25"/>
       <c r="G819" s="23" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="H819" s="23"/>
-      <c r="I819" s="23" t="s">
-        <v>877</v>
-      </c>
+      <c r="I819" s="23"/>
       <c r="J819" s="22"/>
       <c r="K819" s="22"/>
       <c r="L819" s="22"/>
@@ -19403,7 +19406,7 @@
       <c r="N824" s="1"/>
       <c r="O824" s="1"/>
     </row>
-    <row r="825" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="825" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A825" s="21"/>
       <c r="B825" s="22" t="s">
         <v>22</v>
@@ -19418,7 +19421,9 @@
         <v>883</v>
       </c>
       <c r="H825" s="23"/>
-      <c r="I825" s="23"/>
+      <c r="I825" s="23" t="s">
+        <v>884</v>
+      </c>
       <c r="J825" s="22"/>
       <c r="K825" s="22"/>
       <c r="L825" s="22"/>
@@ -19438,7 +19443,7 @@
       </c>
       <c r="F826" s="25"/>
       <c r="G826" s="23" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="H826" s="23"/>
       <c r="I826" s="23"/>
@@ -19457,11 +19462,11 @@
       <c r="E827" s="22"/>
       <c r="F827" s="25"/>
       <c r="G827" s="23" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="H827" s="23"/>
       <c r="I827" s="23" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="J827" s="22"/>
       <c r="K827" s="22"/>
@@ -19470,15 +19475,17 @@
       <c r="N827" s="1"/>
       <c r="O827" s="1"/>
     </row>
-    <row r="828" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="828" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A828" s="21"/>
-      <c r="B828" s="47"/>
+      <c r="B828" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C828" s="25"/>
       <c r="D828" s="22"/>
       <c r="E828" s="22"/>
       <c r="F828" s="25"/>
       <c r="G828" s="23" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="H828" s="23"/>
       <c r="I828" s="23"/>
@@ -19547,7 +19554,7 @@
     </row>
     <row r="831" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A831" s="21" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B831" s="22" t="s">
         <v>22</v>
@@ -19559,7 +19566,7 @@
       </c>
       <c r="F831" s="25"/>
       <c r="G831" s="23" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="H831" s="23"/>
       <c r="I831" s="23"/>
@@ -19582,7 +19589,7 @@
       </c>
       <c r="F832" s="25"/>
       <c r="G832" s="23" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="H832" s="23"/>
       <c r="I832" s="23"/>
@@ -19605,7 +19612,7 @@
       </c>
       <c r="F833" s="25"/>
       <c r="G833" s="23" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="H833" s="23"/>
       <c r="I833" s="23"/>
@@ -19628,7 +19635,7 @@
       </c>
       <c r="F834" s="25"/>
       <c r="G834" s="23" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="H834" s="23"/>
       <c r="I834" s="23"/>
@@ -19651,7 +19658,7 @@
       </c>
       <c r="F835" s="25"/>
       <c r="G835" s="23" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="H835" s="23"/>
       <c r="I835" s="23"/>
@@ -19674,7 +19681,7 @@
       </c>
       <c r="F836" s="25"/>
       <c r="G836" s="23" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="H836" s="23"/>
       <c r="I836" s="23"/>
@@ -19697,7 +19704,7 @@
       </c>
       <c r="F837" s="25"/>
       <c r="G837" s="23" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="H837" s="23"/>
       <c r="I837" s="23"/>
@@ -19718,7 +19725,7 @@
       <c r="E838" s="25"/>
       <c r="F838" s="25"/>
       <c r="G838" s="23" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="H838" s="23"/>
       <c r="I838" s="23"/>
@@ -19741,7 +19748,7 @@
       </c>
       <c r="F839" s="25"/>
       <c r="G839" s="23" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="H839" s="23"/>
       <c r="I839" s="23"/>
@@ -19764,7 +19771,7 @@
       </c>
       <c r="F840" s="25"/>
       <c r="G840" s="23" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="H840" s="23"/>
       <c r="I840" s="23"/>
@@ -19787,7 +19794,7 @@
       </c>
       <c r="F841" s="25"/>
       <c r="G841" s="23" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="H841" s="23"/>
       <c r="I841" s="23"/>
@@ -19810,7 +19817,7 @@
       </c>
       <c r="F842" s="25"/>
       <c r="G842" s="23" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="H842" s="23"/>
       <c r="I842" s="23"/>
@@ -19833,7 +19840,7 @@
       </c>
       <c r="F843" s="25"/>
       <c r="G843" s="23" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="H843" s="23"/>
       <c r="I843" s="23"/>
@@ -19915,7 +19922,7 @@
     </row>
     <row r="849" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A849" s="16" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B849" s="43"/>
       <c r="C849" s="18"/>
@@ -19982,7 +19989,7 @@
     </row>
     <row r="853" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A853" s="21" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B853" s="22" t="s">
         <v>22</v>
@@ -19994,7 +20001,7 @@
       </c>
       <c r="F853" s="25"/>
       <c r="G853" s="23" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="H853" s="23"/>
       <c r="I853" s="23"/>
@@ -20013,7 +20020,7 @@
       </c>
       <c r="F854" s="25"/>
       <c r="G854" s="23" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="H854" s="23"/>
       <c r="I854" s="23"/>
@@ -20067,7 +20074,7 @@
     </row>
     <row r="857" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A857" s="21" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B857" s="22" t="s">
         <v>22</v>
@@ -20077,7 +20084,7 @@
       <c r="E857" s="25"/>
       <c r="F857" s="25"/>
       <c r="G857" s="23" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="H857" s="23"/>
       <c r="I857" s="23"/>
@@ -20094,7 +20101,7 @@
       <c r="E858" s="25"/>
       <c r="F858" s="25"/>
       <c r="G858" s="23" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="H858" s="23"/>
       <c r="I858" s="23"/>
@@ -20111,7 +20118,7 @@
       <c r="E859" s="25"/>
       <c r="F859" s="25"/>
       <c r="G859" s="23" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="H859" s="23"/>
       <c r="I859" s="23"/>
@@ -20128,7 +20135,7 @@
       <c r="E860" s="25"/>
       <c r="F860" s="25"/>
       <c r="G860" s="23" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="H860" s="23"/>
       <c r="I860" s="23"/>
@@ -20145,7 +20152,7 @@
       <c r="E861" s="25"/>
       <c r="F861" s="25"/>
       <c r="G861" s="23" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="H861" s="23"/>
       <c r="I861" s="23"/>
@@ -20162,7 +20169,7 @@
       <c r="E862" s="25"/>
       <c r="F862" s="25"/>
       <c r="G862" s="23" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="H862" s="23"/>
       <c r="I862" s="23"/>
@@ -20170,26 +20177,36 @@
       <c r="K862" s="22"/>
       <c r="L862" s="22"/>
     </row>
-    <row r="863" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B863" s="22"/>
-      <c r="C863" s="22"/>
+    <row r="863" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B863" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C863" s="25"/>
       <c r="D863" s="22"/>
-      <c r="E863" s="22"/>
-      <c r="F863" s="22"/>
-      <c r="G863" s="23"/>
+      <c r="E863" s="25"/>
+      <c r="F863" s="25"/>
+      <c r="G863" s="23" t="s">
+        <v>913</v>
+      </c>
       <c r="H863" s="23"/>
-      <c r="I863" s="23"/>
+      <c r="I863" s="47" t="s">
+        <v>914</v>
+      </c>
       <c r="J863" s="22"/>
       <c r="K863" s="22"/>
       <c r="L863" s="22"/>
     </row>
-    <row r="864" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B864" s="22"/>
-      <c r="C864" s="22"/>
+    <row r="864" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B864" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C864" s="25"/>
       <c r="D864" s="22"/>
-      <c r="E864" s="22"/>
-      <c r="F864" s="22"/>
-      <c r="G864" s="23"/>
+      <c r="E864" s="25"/>
+      <c r="F864" s="25"/>
+      <c r="G864" s="23" t="s">
+        <v>913</v>
+      </c>
       <c r="H864" s="23"/>
       <c r="I864" s="23"/>
       <c r="J864" s="22"/>
@@ -20197,87 +20214,79 @@
       <c r="L864" s="22"/>
     </row>
     <row r="865" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A865" s="19"/>
-      <c r="B865" s="44"/>
-      <c r="C865" s="4"/>
-      <c r="D865" s="4"/>
-      <c r="E865" s="4"/>
-      <c r="F865" s="4"/>
+      <c r="B865" s="22"/>
+      <c r="C865" s="22"/>
+      <c r="D865" s="22"/>
+      <c r="E865" s="22"/>
+      <c r="F865" s="22"/>
+      <c r="G865" s="23"/>
+      <c r="H865" s="23"/>
+      <c r="I865" s="23"/>
+      <c r="J865" s="22"/>
+      <c r="K865" s="22"/>
+      <c r="L865" s="22"/>
     </row>
     <row r="866" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B866" s="46"/>
-      <c r="C866" s="1"/>
-      <c r="D866" s="1"/>
-      <c r="E866" s="1"/>
-      <c r="F866" s="1"/>
-      <c r="G866" s="1"/>
-      <c r="H866" s="1"/>
-      <c r="I866" s="1"/>
-      <c r="J866" s="1"/>
-      <c r="K866" s="1"/>
-      <c r="L866" s="1"/>
-    </row>
-    <row r="867" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A867" s="19"/>
-      <c r="B867" s="11" t="s">
+      <c r="A866" s="19"/>
+      <c r="B866" s="44"/>
+      <c r="C866" s="4"/>
+      <c r="D866" s="4"/>
+      <c r="E866" s="4"/>
+      <c r="F866" s="4"/>
+    </row>
+    <row r="867" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B867" s="46"/>
+      <c r="C867" s="1"/>
+      <c r="D867" s="1"/>
+      <c r="E867" s="1"/>
+      <c r="F867" s="1"/>
+      <c r="G867" s="1"/>
+      <c r="H867" s="1"/>
+      <c r="I867" s="1"/>
+      <c r="J867" s="1"/>
+      <c r="K867" s="1"/>
+      <c r="L867" s="1"/>
+    </row>
+    <row r="868" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A868" s="19"/>
+      <c r="B868" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C867" s="11" t="s">
+      <c r="C868" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D867" s="11" t="s">
+      <c r="D868" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E867" s="11" t="s">
+      <c r="E868" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F867" s="11" t="s">
+      <c r="F868" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G867" s="20" t="s">
+      <c r="G868" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H867" s="20" t="s">
+      <c r="H868" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I867" s="20" t="s">
+      <c r="I868" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J867" s="11" t="s">
+      <c r="J868" s="11" t="s">
         <v>692</v>
       </c>
-      <c r="K867" s="11" t="s">
+      <c r="K868" s="11" t="s">
         <v>693</v>
       </c>
-      <c r="L867" s="11" t="s">
+      <c r="L868" s="11" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="868" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A868" s="21" t="s">
-        <v>912</v>
-      </c>
-      <c r="B868" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C868" s="25"/>
-      <c r="D868" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E868" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F868" s="25"/>
-      <c r="G868" s="23" t="s">
-        <v>913</v>
-      </c>
-      <c r="H868" s="23"/>
-      <c r="I868" s="23"/>
-      <c r="J868" s="22"/>
-      <c r="K868" s="22"/>
-      <c r="L868" s="22"/>
-    </row>
     <row r="869" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A869" s="21" t="s">
+        <v>915</v>
+      </c>
       <c r="B869" s="22" t="s">
         <v>22</v>
       </c>
@@ -20290,7 +20299,7 @@
       </c>
       <c r="F869" s="25"/>
       <c r="G869" s="23" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="H869" s="23"/>
       <c r="I869" s="23"/>
@@ -20298,23 +20307,29 @@
       <c r="K869" s="22"/>
       <c r="L869" s="22"/>
     </row>
-    <row r="870" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B870" s="1"/>
-      <c r="C870" s="1"/>
-      <c r="D870" s="1"/>
-      <c r="E870" s="1"/>
-      <c r="F870" s="1"/>
-      <c r="G870" s="1"/>
-      <c r="H870" s="1"/>
-      <c r="I870" s="1"/>
-      <c r="J870" s="1"/>
-      <c r="K870" s="1"/>
-      <c r="L870" s="1"/>
-      <c r="M870" s="1"/>
-      <c r="N870" s="1"/>
+    <row r="870" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B870" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C870" s="25"/>
+      <c r="D870" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E870" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F870" s="25"/>
+      <c r="G870" s="23" t="s">
+        <v>917</v>
+      </c>
+      <c r="H870" s="23"/>
+      <c r="I870" s="23"/>
+      <c r="J870" s="22"/>
+      <c r="K870" s="22"/>
+      <c r="L870" s="22"/>
     </row>
     <row r="871" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B871" s="46"/>
+      <c r="B871" s="1"/>
       <c r="C871" s="1"/>
       <c r="D871" s="1"/>
       <c r="E871" s="1"/>
@@ -20325,66 +20340,62 @@
       <c r="J871" s="1"/>
       <c r="K871" s="1"/>
       <c r="L871" s="1"/>
-    </row>
-    <row r="872" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A872" s="19"/>
-      <c r="B872" s="11" t="s">
+      <c r="M871" s="1"/>
+      <c r="N871" s="1"/>
+    </row>
+    <row r="872" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B872" s="46"/>
+      <c r="C872" s="1"/>
+      <c r="D872" s="1"/>
+      <c r="E872" s="1"/>
+      <c r="F872" s="1"/>
+      <c r="G872" s="1"/>
+      <c r="H872" s="1"/>
+      <c r="I872" s="1"/>
+      <c r="J872" s="1"/>
+      <c r="K872" s="1"/>
+      <c r="L872" s="1"/>
+    </row>
+    <row r="873" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A873" s="19"/>
+      <c r="B873" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C872" s="11" t="s">
+      <c r="C873" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D872" s="11" t="s">
+      <c r="D873" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E872" s="11" t="s">
+      <c r="E873" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F872" s="11" t="s">
+      <c r="F873" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G872" s="20" t="s">
+      <c r="G873" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H872" s="20" t="s">
+      <c r="H873" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I872" s="20" t="s">
+      <c r="I873" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J872" s="11" t="s">
+      <c r="J873" s="11" t="s">
         <v>692</v>
       </c>
-      <c r="K872" s="11" t="s">
+      <c r="K873" s="11" t="s">
         <v>693</v>
       </c>
-      <c r="L872" s="11" t="s">
+      <c r="L873" s="11" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="873" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A873" s="21" t="s">
-        <v>915</v>
-      </c>
-      <c r="B873" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C873" s="25"/>
-      <c r="D873" s="22"/>
-      <c r="E873" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F873" s="25"/>
-      <c r="G873" s="23" t="s">
-        <v>916</v>
-      </c>
-      <c r="H873" s="23"/>
-      <c r="I873" s="23"/>
-      <c r="J873" s="22"/>
-      <c r="K873" s="22"/>
-      <c r="L873" s="22"/>
-    </row>
     <row r="874" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A874" s="21" t="s">
+        <v>918</v>
+      </c>
       <c r="B874" s="22" t="s">
         <v>22</v>
       </c>
@@ -20395,7 +20406,7 @@
       </c>
       <c r="F874" s="25"/>
       <c r="G874" s="23" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="H874" s="23"/>
       <c r="I874" s="23"/>
@@ -20414,7 +20425,7 @@
       </c>
       <c r="F875" s="25"/>
       <c r="G875" s="23" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="H875" s="23"/>
       <c r="I875" s="23"/>
@@ -20433,7 +20444,7 @@
       </c>
       <c r="F876" s="25"/>
       <c r="G876" s="23" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="H876" s="23"/>
       <c r="I876" s="23"/>
@@ -20447,10 +20458,12 @@
       </c>
       <c r="C877" s="25"/>
       <c r="D877" s="22"/>
-      <c r="E877" s="25"/>
+      <c r="E877" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F877" s="25"/>
       <c r="G877" s="23" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="H877" s="23"/>
       <c r="I877" s="23"/>
@@ -20467,7 +20480,7 @@
       <c r="E878" s="25"/>
       <c r="F878" s="25"/>
       <c r="G878" s="23" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="H878" s="23"/>
       <c r="I878" s="23"/>
@@ -20484,7 +20497,7 @@
       <c r="E879" s="25"/>
       <c r="F879" s="25"/>
       <c r="G879" s="23" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="H879" s="23"/>
       <c r="I879" s="23"/>
@@ -20501,7 +20514,7 @@
       <c r="E880" s="25"/>
       <c r="F880" s="25"/>
       <c r="G880" s="23" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="H880" s="23"/>
       <c r="I880" s="23"/>
@@ -20510,13 +20523,15 @@
       <c r="L880" s="22"/>
     </row>
     <row r="881" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B881" s="25"/>
+      <c r="B881" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="C881" s="25"/>
       <c r="D881" s="22"/>
-      <c r="E881" s="22"/>
+      <c r="E881" s="25"/>
       <c r="F881" s="25"/>
       <c r="G881" s="23" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="H881" s="23"/>
       <c r="I881" s="23"/>
@@ -20531,7 +20546,7 @@
       <c r="E882" s="22"/>
       <c r="F882" s="25"/>
       <c r="G882" s="23" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="H882" s="23"/>
       <c r="I882" s="23"/>
@@ -20539,20 +20554,14 @@
       <c r="K882" s="22"/>
       <c r="L882" s="22"/>
     </row>
-    <row r="883" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B883" s="22" t="s">
-        <v>22</v>
-      </c>
+    <row r="883" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B883" s="25"/>
       <c r="C883" s="25"/>
-      <c r="D883" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E883" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D883" s="22"/>
+      <c r="E883" s="22"/>
       <c r="F883" s="25"/>
       <c r="G883" s="23" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="H883" s="23"/>
       <c r="I883" s="23"/>
@@ -20561,12 +20570,20 @@
       <c r="L883" s="22"/>
     </row>
     <row r="884" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B884" s="22"/>
-      <c r="C884" s="22"/>
-      <c r="D884" s="22"/>
-      <c r="E884" s="22"/>
-      <c r="F884" s="22"/>
-      <c r="G884" s="23"/>
+      <c r="B884" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C884" s="25"/>
+      <c r="D884" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E884" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F884" s="25"/>
+      <c r="G884" s="23" t="s">
+        <v>929</v>
+      </c>
       <c r="H884" s="23"/>
       <c r="I884" s="23"/>
       <c r="J884" s="22"/>
@@ -20574,29 +20591,24 @@
       <c r="L884" s="22"/>
     </row>
     <row r="885" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B885" s="1"/>
-      <c r="C885" s="1"/>
-      <c r="D885" s="1"/>
-      <c r="E885" s="1"/>
-      <c r="F885" s="1"/>
-      <c r="G885" s="1"/>
-      <c r="H885" s="1"/>
-      <c r="I885" s="1"/>
-      <c r="J885" s="1"/>
-      <c r="K885" s="1"/>
-      <c r="L885" s="1"/>
-      <c r="M885" s="1"/>
-      <c r="N885" s="1"/>
+      <c r="B885" s="22"/>
+      <c r="C885" s="22"/>
+      <c r="D885" s="22"/>
+      <c r="E885" s="22"/>
+      <c r="F885" s="22"/>
+      <c r="G885" s="23"/>
+      <c r="H885" s="23"/>
+      <c r="I885" s="23"/>
+      <c r="J885" s="22"/>
+      <c r="K885" s="22"/>
+      <c r="L885" s="22"/>
     </row>
     <row r="886" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A886" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B886" s="17"/>
-      <c r="C886" s="18"/>
-      <c r="D886" s="18"/>
-      <c r="E886" s="18"/>
-      <c r="F886" s="18"/>
+      <c r="B886" s="1"/>
+      <c r="C886" s="1"/>
+      <c r="D886" s="1"/>
+      <c r="E886" s="1"/>
+      <c r="F886" s="1"/>
       <c r="G886" s="1"/>
       <c r="H886" s="1"/>
       <c r="I886" s="1"/>
@@ -20608,7 +20620,7 @@
     </row>
     <row r="887" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A887" s="16" t="s">
-        <v>927</v>
+        <v>15</v>
       </c>
       <c r="B887" s="17"/>
       <c r="C887" s="18"/>
@@ -20626,7 +20638,7 @@
     </row>
     <row r="888" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A888" s="16" t="s">
-        <v>15</v>
+        <v>930</v>
       </c>
       <c r="B888" s="17"/>
       <c r="C888" s="18"/>
@@ -20643,11 +20655,14 @@
       <c r="N888" s="1"/>
     </row>
     <row r="889" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B889" s="1"/>
-      <c r="C889" s="1"/>
-      <c r="D889" s="1"/>
-      <c r="E889" s="1"/>
-      <c r="F889" s="1"/>
+      <c r="A889" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B889" s="17"/>
+      <c r="C889" s="18"/>
+      <c r="D889" s="18"/>
+      <c r="E889" s="18"/>
+      <c r="F889" s="18"/>
       <c r="G889" s="1"/>
       <c r="H889" s="1"/>
       <c r="I889" s="1"/>
@@ -20658,7 +20673,7 @@
       <c r="N889" s="1"/>
     </row>
     <row r="890" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B890" s="46"/>
+      <c r="B890" s="1"/>
       <c r="C890" s="1"/>
       <c r="D890" s="1"/>
       <c r="E890" s="1"/>
@@ -20669,64 +20684,62 @@
       <c r="J890" s="1"/>
       <c r="K890" s="1"/>
       <c r="L890" s="1"/>
-    </row>
-    <row r="891" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A891" s="19"/>
-      <c r="B891" s="11" t="s">
+      <c r="M890" s="1"/>
+      <c r="N890" s="1"/>
+    </row>
+    <row r="891" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B891" s="46"/>
+      <c r="C891" s="1"/>
+      <c r="D891" s="1"/>
+      <c r="E891" s="1"/>
+      <c r="F891" s="1"/>
+      <c r="G891" s="1"/>
+      <c r="H891" s="1"/>
+      <c r="I891" s="1"/>
+      <c r="J891" s="1"/>
+      <c r="K891" s="1"/>
+      <c r="L891" s="1"/>
+    </row>
+    <row r="892" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A892" s="19"/>
+      <c r="B892" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C891" s="11" t="s">
+      <c r="C892" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D891" s="11" t="s">
+      <c r="D892" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E891" s="11" t="s">
+      <c r="E892" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F891" s="11" t="s">
+      <c r="F892" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G891" s="20" t="s">
+      <c r="G892" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H891" s="20" t="s">
+      <c r="H892" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I891" s="20" t="s">
+      <c r="I892" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J891" s="11" t="s">
+      <c r="J892" s="11" t="s">
         <v>692</v>
       </c>
-      <c r="K891" s="11" t="s">
+      <c r="K892" s="11" t="s">
         <v>693</v>
       </c>
-      <c r="L891" s="11" t="s">
+      <c r="L892" s="11" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="892" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A892" s="21" t="s">
-        <v>928</v>
-      </c>
-      <c r="B892" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C892" s="25"/>
-      <c r="D892" s="22"/>
-      <c r="E892" s="25"/>
-      <c r="F892" s="25"/>
-      <c r="G892" s="23" t="s">
-        <v>929</v>
-      </c>
-      <c r="H892" s="23"/>
-      <c r="I892" s="23"/>
-      <c r="J892" s="22"/>
-      <c r="K892" s="22"/>
-      <c r="L892" s="22"/>
-    </row>
     <row r="893" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A893" s="21" t="s">
+        <v>931</v>
+      </c>
       <c r="B893" s="22" t="s">
         <v>22</v>
       </c>
@@ -20735,7 +20748,7 @@
       <c r="E893" s="25"/>
       <c r="F893" s="25"/>
       <c r="G893" s="23" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="H893" s="23"/>
       <c r="I893" s="23"/>
@@ -20752,7 +20765,7 @@
       <c r="E894" s="25"/>
       <c r="F894" s="25"/>
       <c r="G894" s="23" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="H894" s="23"/>
       <c r="I894" s="23"/>
@@ -20769,7 +20782,7 @@
       <c r="E895" s="25"/>
       <c r="F895" s="25"/>
       <c r="G895" s="23" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="H895" s="23"/>
       <c r="I895" s="23"/>
@@ -20786,7 +20799,7 @@
       <c r="E896" s="25"/>
       <c r="F896" s="25"/>
       <c r="G896" s="23" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="H896" s="23"/>
       <c r="I896" s="23"/>
@@ -20803,7 +20816,7 @@
       <c r="E897" s="25"/>
       <c r="F897" s="25"/>
       <c r="G897" s="23" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="H897" s="23"/>
       <c r="I897" s="23"/>
@@ -20820,7 +20833,7 @@
       <c r="E898" s="25"/>
       <c r="F898" s="25"/>
       <c r="G898" s="23" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="H898" s="23"/>
       <c r="I898" s="23"/>
@@ -20837,7 +20850,7 @@
       <c r="E899" s="25"/>
       <c r="F899" s="25"/>
       <c r="G899" s="23" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="H899" s="23"/>
       <c r="I899" s="23"/>
@@ -20854,7 +20867,7 @@
       <c r="E900" s="25"/>
       <c r="F900" s="25"/>
       <c r="G900" s="23" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="H900" s="23"/>
       <c r="I900" s="23"/>
@@ -20863,12 +20876,16 @@
       <c r="L900" s="22"/>
     </row>
     <row r="901" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B901" s="22"/>
-      <c r="C901" s="22"/>
+      <c r="B901" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C901" s="25"/>
       <c r="D901" s="22"/>
-      <c r="E901" s="22"/>
-      <c r="F901" s="22"/>
-      <c r="G901" s="23"/>
+      <c r="E901" s="25"/>
+      <c r="F901" s="25"/>
+      <c r="G901" s="23" t="s">
+        <v>940</v>
+      </c>
       <c r="H901" s="23"/>
       <c r="I901" s="23"/>
       <c r="J901" s="22"/>
@@ -20876,77 +20893,71 @@
       <c r="L901" s="22"/>
     </row>
     <row r="902" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B902" s="46"/>
-      <c r="C902" s="1"/>
-      <c r="D902" s="1"/>
-      <c r="E902" s="1"/>
-      <c r="F902" s="1"/>
-      <c r="G902" s="1"/>
-      <c r="H902" s="1"/>
-      <c r="I902" s="1"/>
-      <c r="J902" s="1"/>
-      <c r="K902" s="1"/>
-      <c r="L902" s="1"/>
-    </row>
-    <row r="903" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A903" s="19"/>
-      <c r="B903" s="11" t="s">
+      <c r="B902" s="22"/>
+      <c r="C902" s="22"/>
+      <c r="D902" s="22"/>
+      <c r="E902" s="22"/>
+      <c r="F902" s="22"/>
+      <c r="G902" s="23"/>
+      <c r="H902" s="23"/>
+      <c r="I902" s="23"/>
+      <c r="J902" s="22"/>
+      <c r="K902" s="22"/>
+      <c r="L902" s="22"/>
+    </row>
+    <row r="903" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B903" s="46"/>
+      <c r="C903" s="1"/>
+      <c r="D903" s="1"/>
+      <c r="E903" s="1"/>
+      <c r="F903" s="1"/>
+      <c r="G903" s="1"/>
+      <c r="H903" s="1"/>
+      <c r="I903" s="1"/>
+      <c r="J903" s="1"/>
+      <c r="K903" s="1"/>
+      <c r="L903" s="1"/>
+    </row>
+    <row r="904" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A904" s="19"/>
+      <c r="B904" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C903" s="11" t="s">
+      <c r="C904" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D903" s="11" t="s">
+      <c r="D904" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E903" s="11" t="s">
+      <c r="E904" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F903" s="11" t="s">
+      <c r="F904" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G903" s="20" t="s">
+      <c r="G904" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H903" s="20" t="s">
+      <c r="H904" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I903" s="20" t="s">
+      <c r="I904" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J903" s="11" t="s">
+      <c r="J904" s="11" t="s">
         <v>692</v>
       </c>
-      <c r="K903" s="11" t="s">
+      <c r="K904" s="11" t="s">
         <v>693</v>
       </c>
-      <c r="L903" s="11" t="s">
+      <c r="L904" s="11" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="904" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A904" s="21" t="s">
-        <v>938</v>
-      </c>
-      <c r="B904" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C904" s="25"/>
-      <c r="D904" s="22"/>
-      <c r="E904" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F904" s="25"/>
-      <c r="G904" s="23" t="s">
-        <v>939</v>
-      </c>
-      <c r="H904" s="23"/>
-      <c r="I904" s="23"/>
-      <c r="J904" s="22"/>
-      <c r="K904" s="22"/>
-      <c r="L904" s="22"/>
-    </row>
     <row r="905" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A905" s="21" t="s">
+        <v>941</v>
+      </c>
       <c r="B905" s="22" t="s">
         <v>22</v>
       </c>
@@ -20957,7 +20968,7 @@
       </c>
       <c r="F905" s="25"/>
       <c r="G905" s="23" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="H905" s="23"/>
       <c r="I905" s="23"/>
@@ -20976,7 +20987,7 @@
       </c>
       <c r="F906" s="25"/>
       <c r="G906" s="23" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="H906" s="23"/>
       <c r="I906" s="23"/>
@@ -20995,7 +21006,7 @@
       </c>
       <c r="F907" s="25"/>
       <c r="G907" s="23" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="H907" s="23"/>
       <c r="I907" s="23"/>
@@ -21004,15 +21015,17 @@
       <c r="L907" s="22"/>
     </row>
     <row r="908" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B908" s="25" t="s">
-        <v>611</v>
+      <c r="B908" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="C908" s="25"/>
       <c r="D908" s="22"/>
-      <c r="E908" s="22"/>
+      <c r="E908" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="F908" s="25"/>
       <c r="G908" s="23" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="H908" s="23"/>
       <c r="I908" s="23"/>
@@ -21029,7 +21042,7 @@
       <c r="E909" s="22"/>
       <c r="F909" s="25"/>
       <c r="G909" s="23" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="H909" s="23"/>
       <c r="I909" s="23"/>
@@ -21037,16 +21050,16 @@
       <c r="K909" s="22"/>
       <c r="L909" s="22"/>
     </row>
-    <row r="910" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B910" s="22" t="s">
-        <v>22</v>
+    <row r="910" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B910" s="25" t="s">
+        <v>611</v>
       </c>
       <c r="C910" s="25"/>
       <c r="D910" s="22"/>
-      <c r="E910" s="25"/>
+      <c r="E910" s="22"/>
       <c r="F910" s="25"/>
       <c r="G910" s="23" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="H910" s="23"/>
       <c r="I910" s="23"/>
@@ -21063,7 +21076,7 @@
       <c r="E911" s="25"/>
       <c r="F911" s="25"/>
       <c r="G911" s="23" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="H911" s="23"/>
       <c r="I911" s="23"/>
@@ -21071,7 +21084,7 @@
       <c r="K911" s="22"/>
       <c r="L911" s="22"/>
     </row>
-    <row r="912" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="912" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B912" s="22" t="s">
         <v>22</v>
       </c>
@@ -21080,7 +21093,7 @@
       <c r="E912" s="25"/>
       <c r="F912" s="25"/>
       <c r="G912" s="23" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="H912" s="23"/>
       <c r="I912" s="23"/>
@@ -21094,12 +21107,10 @@
       </c>
       <c r="C913" s="25"/>
       <c r="D913" s="22"/>
-      <c r="E913" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E913" s="25"/>
       <c r="F913" s="25"/>
       <c r="G913" s="23" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="H913" s="23"/>
       <c r="I913" s="23"/>
@@ -21107,18 +21118,18 @@
       <c r="K913" s="22"/>
       <c r="L913" s="22"/>
     </row>
-    <row r="914" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="914" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B914" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C914" s="25"/>
       <c r="D914" s="22"/>
       <c r="E914" s="22" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="F914" s="25"/>
       <c r="G914" s="23" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="H914" s="23"/>
       <c r="I914" s="23"/>
@@ -21126,7 +21137,7 @@
       <c r="K914" s="22"/>
       <c r="L914" s="22"/>
     </row>
-    <row r="915" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="915" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B915" s="22" t="s">
         <v>22</v>
       </c>
@@ -21137,7 +21148,7 @@
       </c>
       <c r="F915" s="25"/>
       <c r="G915" s="23" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="H915" s="23"/>
       <c r="I915" s="23"/>
@@ -21152,11 +21163,11 @@
       <c r="C916" s="25"/>
       <c r="D916" s="22"/>
       <c r="E916" s="22" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="F916" s="25"/>
       <c r="G916" s="23" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="H916" s="23"/>
       <c r="I916" s="23"/>
@@ -21175,7 +21186,7 @@
       </c>
       <c r="F917" s="25"/>
       <c r="G917" s="23" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="H917" s="23"/>
       <c r="I917" s="23"/>
@@ -21183,13 +21194,19 @@
       <c r="K917" s="22"/>
       <c r="L917" s="22"/>
     </row>
-    <row r="918" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B918" s="22"/>
-      <c r="C918" s="22"/>
+    <row r="918" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B918" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C918" s="25"/>
       <c r="D918" s="22"/>
-      <c r="E918" s="22"/>
-      <c r="F918" s="22"/>
-      <c r="G918" s="23"/>
+      <c r="E918" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F918" s="25"/>
+      <c r="G918" s="23" t="s">
+        <v>955</v>
+      </c>
       <c r="H918" s="23"/>
       <c r="I918" s="23"/>
       <c r="J918" s="22"/>
@@ -21223,82 +21240,74 @@
       <c r="L920" s="22"/>
     </row>
     <row r="921" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B921" s="1"/>
-      <c r="C921" s="1"/>
-      <c r="D921" s="1"/>
-      <c r="E921" s="1"/>
-      <c r="F921" s="1"/>
-      <c r="G921" s="1"/>
-      <c r="H921" s="1"/>
-      <c r="I921" s="1"/>
-      <c r="J921" s="1"/>
-      <c r="K921" s="1"/>
-      <c r="L921" s="1"/>
-      <c r="M921" s="1"/>
-      <c r="N921" s="1"/>
-    </row>
-    <row r="922" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A922" s="19"/>
-      <c r="B922" s="11" t="s">
+      <c r="B921" s="22"/>
+      <c r="C921" s="22"/>
+      <c r="D921" s="22"/>
+      <c r="E921" s="22"/>
+      <c r="F921" s="22"/>
+      <c r="G921" s="23"/>
+      <c r="H921" s="23"/>
+      <c r="I921" s="23"/>
+      <c r="J921" s="22"/>
+      <c r="K921" s="22"/>
+      <c r="L921" s="22"/>
+    </row>
+    <row r="922" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B922" s="1"/>
+      <c r="C922" s="1"/>
+      <c r="D922" s="1"/>
+      <c r="E922" s="1"/>
+      <c r="F922" s="1"/>
+      <c r="G922" s="1"/>
+      <c r="H922" s="1"/>
+      <c r="I922" s="1"/>
+      <c r="J922" s="1"/>
+      <c r="K922" s="1"/>
+      <c r="L922" s="1"/>
+      <c r="M922" s="1"/>
+      <c r="N922" s="1"/>
+    </row>
+    <row r="923" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A923" s="19"/>
+      <c r="B923" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C922" s="11" t="s">
+      <c r="C923" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D922" s="11" t="s">
+      <c r="D923" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E922" s="11" t="s">
+      <c r="E923" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F922" s="11" t="s">
+      <c r="F923" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G922" s="20" t="s">
+      <c r="G923" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H922" s="20" t="s">
+      <c r="H923" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I922" s="20" t="s">
+      <c r="I923" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J922" s="11" t="s">
+      <c r="J923" s="11" t="s">
         <v>692</v>
       </c>
-      <c r="K922" s="11" t="s">
+      <c r="K923" s="11" t="s">
         <v>693</v>
       </c>
-      <c r="L922" s="11" t="s">
+      <c r="L923" s="11" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="923" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A923" s="21" t="s">
-        <v>953</v>
-      </c>
-      <c r="B923" s="25" t="s">
-        <v>611</v>
-      </c>
-      <c r="C923" s="25"/>
-      <c r="D923" s="22"/>
-      <c r="E923" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F923" s="25"/>
-      <c r="G923" s="23" t="s">
-        <v>954</v>
-      </c>
-      <c r="H923" s="23"/>
-      <c r="I923" s="23" t="s">
-        <v>613</v>
-      </c>
-      <c r="J923" s="22"/>
-      <c r="K923" s="22"/>
-      <c r="L923" s="22"/>
-    </row>
     <row r="924" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B924" s="25" t="s">
+      <c r="A924" s="21" t="s">
+        <v>956</v>
+      </c>
+      <c r="B924" s="27" t="s">
         <v>611</v>
       </c>
       <c r="C924" s="25"/>
@@ -21308,7 +21317,7 @@
       </c>
       <c r="F924" s="25"/>
       <c r="G924" s="23" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="H924" s="23"/>
       <c r="I924" s="23" t="s">
@@ -21318,7 +21327,7 @@
       <c r="K924" s="22"/>
       <c r="L924" s="22"/>
     </row>
-    <row r="925" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="925" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B925" s="22" t="s">
         <v>22</v>
       </c>
@@ -21329,7 +21338,7 @@
       </c>
       <c r="F925" s="25"/>
       <c r="G925" s="23" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="H925" s="23"/>
       <c r="I925" s="23"/>
@@ -21348,7 +21357,7 @@
       </c>
       <c r="F926" s="25"/>
       <c r="G926" s="23" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="H926" s="23"/>
       <c r="I926" s="23"/>
@@ -21367,7 +21376,7 @@
       </c>
       <c r="F927" s="25"/>
       <c r="G927" s="23" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="H927" s="23"/>
       <c r="I927" s="23"/>
@@ -21375,13 +21384,19 @@
       <c r="K927" s="22"/>
       <c r="L927" s="22"/>
     </row>
-    <row r="928" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B928" s="22"/>
-      <c r="C928" s="22"/>
+    <row r="928" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B928" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C928" s="25"/>
       <c r="D928" s="22"/>
-      <c r="E928" s="22"/>
-      <c r="F928" s="22"/>
-      <c r="G928" s="23"/>
+      <c r="E928" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F928" s="25"/>
+      <c r="G928" s="23" t="s">
+        <v>961</v>
+      </c>
       <c r="H928" s="23"/>
       <c r="I928" s="23"/>
       <c r="J928" s="22"/>
@@ -21389,20 +21404,20 @@
       <c r="L928" s="22"/>
     </row>
     <row r="929" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B929" s="46"/>
-      <c r="C929" s="1"/>
-      <c r="D929" s="1"/>
-      <c r="E929" s="1"/>
-      <c r="F929" s="1"/>
-      <c r="G929" s="1"/>
-      <c r="H929" s="1"/>
-      <c r="I929" s="1"/>
-      <c r="J929" s="1"/>
-      <c r="K929" s="1"/>
-      <c r="L929" s="1"/>
+      <c r="B929" s="22"/>
+      <c r="C929" s="22"/>
+      <c r="D929" s="22"/>
+      <c r="E929" s="22"/>
+      <c r="F929" s="22"/>
+      <c r="G929" s="23"/>
+      <c r="H929" s="23"/>
+      <c r="I929" s="23"/>
+      <c r="J929" s="22"/>
+      <c r="K929" s="22"/>
+      <c r="L929" s="22"/>
     </row>
     <row r="930" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B930" s="1"/>
+      <c r="B930" s="46"/>
       <c r="C930" s="1"/>
       <c r="D930" s="1"/>
       <c r="E930" s="1"/>
@@ -21413,8 +21428,6 @@
       <c r="J930" s="1"/>
       <c r="K930" s="1"/>
       <c r="L930" s="1"/>
-      <c r="M930" s="1"/>
-      <c r="N930" s="1"/>
     </row>
     <row r="931" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B931" s="1"/>
@@ -21535,24 +21548,29 @@
       <c r="L938" s="1"/>
       <c r="M938" s="1"/>
       <c r="N938" s="1"/>
-      <c r="O938" s="1"/>
     </row>
     <row r="939" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A939" s="9"/>
+      <c r="B939" s="1"/>
+      <c r="C939" s="1"/>
+      <c r="D939" s="1"/>
+      <c r="E939" s="1"/>
+      <c r="F939" s="1"/>
+      <c r="G939" s="1"/>
+      <c r="H939" s="1"/>
+      <c r="I939" s="1"/>
+      <c r="J939" s="1"/>
+      <c r="K939" s="1"/>
+      <c r="L939" s="1"/>
+      <c r="M939" s="1"/>
+      <c r="N939" s="1"/>
+      <c r="O939" s="1"/>
     </row>
     <row r="940" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A940" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B940" s="17"/>
-      <c r="C940" s="18"/>
-      <c r="D940" s="18"/>
-      <c r="E940" s="18"/>
-      <c r="F940" s="18"/>
+      <c r="A940" s="9"/>
     </row>
     <row r="941" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A941" s="16" t="s">
-        <v>959</v>
+        <v>15</v>
       </c>
       <c r="B941" s="17"/>
       <c r="C941" s="18"/>
@@ -21562,7 +21580,7 @@
     </row>
     <row r="942" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A942" s="16" t="s">
-        <v>15</v>
+        <v>962</v>
       </c>
       <c r="B942" s="17"/>
       <c r="C942" s="18"/>
@@ -21570,65 +21588,52 @@
       <c r="E942" s="18"/>
       <c r="F942" s="18"/>
     </row>
-    <row r="943" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A943" s="9"/>
-      <c r="B943" s="11" t="s">
+    <row r="943" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A943" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B943" s="17"/>
+      <c r="C943" s="18"/>
+      <c r="D943" s="18"/>
+      <c r="E943" s="18"/>
+      <c r="F943" s="18"/>
+    </row>
+    <row r="944" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A944" s="9"/>
+      <c r="B944" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C943" s="11" t="s">
+      <c r="C944" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D943" s="11" t="s">
+      <c r="D944" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E943" s="11" t="s">
+      <c r="E944" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F943" s="11" t="s">
+      <c r="F944" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G943" s="20" t="s">
+      <c r="G944" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H943" s="20" t="s">
+      <c r="H944" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I943" s="20" t="s">
+      <c r="I944" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="944" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A944" s="21" t="s">
-        <v>960</v>
-      </c>
-      <c r="B944" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C944" s="25"/>
-      <c r="D944" s="22"/>
-      <c r="E944" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F944" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="G944" s="23" t="s">
-        <v>961</v>
-      </c>
-      <c r="H944" s="23"/>
-      <c r="I944" s="23"/>
-    </row>
     <row r="945" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A945" s="21"/>
+      <c r="A945" s="21" t="s">
+        <v>963</v>
+      </c>
       <c r="B945" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C945" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D945" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C945" s="25"/>
+      <c r="D945" s="22"/>
       <c r="E945" s="22" t="s">
         <v>22</v>
       </c>
@@ -21636,13 +21641,13 @@
         <v>640</v>
       </c>
       <c r="G945" s="23" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="H945" s="23"/>
       <c r="I945" s="23"/>
     </row>
     <row r="946" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A946" s="9"/>
+      <c r="A946" s="21"/>
       <c r="B946" s="22" t="s">
         <v>22</v>
       </c>
@@ -21659,7 +21664,7 @@
         <v>640</v>
       </c>
       <c r="G946" s="23" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="H946" s="23"/>
       <c r="I946" s="23"/>
@@ -21669,16 +21674,20 @@
       <c r="B947" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C947" s="25"/>
-      <c r="D947" s="22"/>
+      <c r="C947" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D947" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E947" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F947" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="G947" s="45" t="s">
-        <v>964</v>
+      <c r="G947" s="23" t="s">
+        <v>966</v>
       </c>
       <c r="H947" s="23"/>
       <c r="I947" s="23"/>
@@ -21688,20 +21697,16 @@
       <c r="B948" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C948" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D948" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C948" s="25"/>
+      <c r="D948" s="22"/>
       <c r="E948" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F948" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="G948" s="23" t="s">
-        <v>965</v>
+      <c r="G948" s="45" t="s">
+        <v>967</v>
       </c>
       <c r="H948" s="23"/>
       <c r="I948" s="23"/>
@@ -21711,14 +21716,20 @@
       <c r="B949" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C949" s="25"/>
-      <c r="D949" s="22"/>
-      <c r="E949" s="25"/>
+      <c r="C949" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D949" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E949" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F949" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G949" s="23" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="H949" s="23"/>
       <c r="I949" s="23"/>
@@ -21735,7 +21746,7 @@
         <v>640</v>
       </c>
       <c r="G950" s="23" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="H950" s="23"/>
       <c r="I950" s="23"/>
@@ -21752,7 +21763,7 @@
         <v>640</v>
       </c>
       <c r="G951" s="23" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="H951" s="23"/>
       <c r="I951" s="23"/>
@@ -21769,7 +21780,7 @@
         <v>640</v>
       </c>
       <c r="G952" s="23" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="H952" s="23"/>
       <c r="I952" s="23"/>
@@ -21786,7 +21797,7 @@
         <v>640</v>
       </c>
       <c r="G953" s="23" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="H953" s="23"/>
       <c r="I953" s="23"/>
@@ -21798,14 +21809,12 @@
       </c>
       <c r="C954" s="25"/>
       <c r="D954" s="22"/>
-      <c r="E954" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E954" s="25"/>
       <c r="F954" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G954" s="23" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="H954" s="23"/>
       <c r="I954" s="23"/>
@@ -21824,7 +21833,7 @@
         <v>640</v>
       </c>
       <c r="G955" s="23" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="H955" s="23"/>
       <c r="I955" s="23"/>
@@ -21843,12 +21852,12 @@
         <v>640</v>
       </c>
       <c r="G956" s="23" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="H956" s="23"/>
       <c r="I956" s="23"/>
     </row>
-    <row r="957" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="957" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A957" s="9"/>
       <c r="B957" s="22" t="s">
         <v>22</v>
@@ -21862,12 +21871,10 @@
         <v>640</v>
       </c>
       <c r="G957" s="23" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="H957" s="23"/>
-      <c r="I957" s="23" t="s">
-        <v>268</v>
-      </c>
+      <c r="I957" s="23"/>
     </row>
     <row r="958" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A958" s="9"/>
@@ -21883,19 +21890,19 @@
         <v>640</v>
       </c>
       <c r="G958" s="23" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="H958" s="23"/>
-      <c r="I958" s="23"/>
-    </row>
-    <row r="959" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I958" s="23" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="959" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A959" s="9"/>
       <c r="B959" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C959" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C959" s="25"/>
       <c r="D959" s="22"/>
       <c r="E959" s="22" t="s">
         <v>22</v>
@@ -21904,17 +21911,19 @@
         <v>640</v>
       </c>
       <c r="G959" s="23" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="H959" s="23"/>
       <c r="I959" s="23"/>
     </row>
-    <row r="960" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="960" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A960" s="9"/>
       <c r="B960" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C960" s="25"/>
+      <c r="C960" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D960" s="22"/>
       <c r="E960" s="22" t="s">
         <v>22</v>
@@ -21923,7 +21932,7 @@
         <v>640</v>
       </c>
       <c r="G960" s="23" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="H960" s="23"/>
       <c r="I960" s="23"/>
@@ -21942,7 +21951,7 @@
         <v>640</v>
       </c>
       <c r="G961" s="23" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="H961" s="23"/>
       <c r="I961" s="23"/>
@@ -21961,7 +21970,7 @@
         <v>640</v>
       </c>
       <c r="G962" s="23" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="H962" s="23"/>
       <c r="I962" s="23"/>
@@ -21980,7 +21989,7 @@
         <v>640</v>
       </c>
       <c r="G963" s="23" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="H963" s="23"/>
       <c r="I963" s="23"/>
@@ -21991,9 +22000,7 @@
         <v>22</v>
       </c>
       <c r="C964" s="25"/>
-      <c r="D964" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D964" s="22"/>
       <c r="E964" s="22" t="s">
         <v>22</v>
       </c>
@@ -22001,19 +22008,17 @@
         <v>640</v>
       </c>
       <c r="G964" s="23" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="H964" s="23"/>
       <c r="I964" s="23"/>
     </row>
-    <row r="965" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="965" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A965" s="9"/>
       <c r="B965" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C965" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C965" s="25"/>
       <c r="D965" s="22" t="s">
         <v>22</v>
       </c>
@@ -22024,7 +22029,7 @@
         <v>640</v>
       </c>
       <c r="G965" s="23" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="H965" s="23"/>
       <c r="I965" s="23"/>
@@ -22047,7 +22052,7 @@
         <v>640</v>
       </c>
       <c r="G966" s="23" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="H966" s="23"/>
       <c r="I966" s="23"/>
@@ -22070,7 +22075,7 @@
         <v>640</v>
       </c>
       <c r="G967" s="23" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="H967" s="23"/>
       <c r="I967" s="23"/>
@@ -22080,8 +22085,12 @@
       <c r="B968" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C968" s="25"/>
-      <c r="D968" s="22"/>
+      <c r="C968" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D968" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E968" s="22" t="s">
         <v>22</v>
       </c>
@@ -22089,7 +22098,7 @@
         <v>640</v>
       </c>
       <c r="G968" s="23" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="H968" s="23"/>
       <c r="I968" s="23"/>
@@ -22101,54 +22110,50 @@
       </c>
       <c r="C969" s="25"/>
       <c r="D969" s="22"/>
-      <c r="E969" s="25"/>
+      <c r="E969" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F969" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G969" s="23" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="H969" s="23"/>
       <c r="I969" s="23"/>
     </row>
-    <row r="970" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="970" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A970" s="9"/>
       <c r="B970" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C970" s="25"/>
-      <c r="D970" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D970" s="22"/>
       <c r="E970" s="25"/>
       <c r="F970" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G970" s="23" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="H970" s="23"/>
       <c r="I970" s="23"/>
     </row>
-    <row r="971" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="971" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A971" s="9"/>
       <c r="B971" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C971" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C971" s="25"/>
       <c r="D971" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E971" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E971" s="25"/>
       <c r="F971" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G971" s="23" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="H971" s="23"/>
       <c r="I971" s="23"/>
@@ -22171,7 +22176,7 @@
         <v>640</v>
       </c>
       <c r="G972" s="23" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="H972" s="23"/>
       <c r="I972" s="23"/>
@@ -22181,7 +22186,9 @@
       <c r="B973" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C973" s="25"/>
+      <c r="C973" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D973" s="22" t="s">
         <v>22</v>
       </c>
@@ -22192,7 +22199,7 @@
         <v>640</v>
       </c>
       <c r="G973" s="23" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="H973" s="23"/>
       <c r="I973" s="23"/>
@@ -22213,18 +22220,20 @@
         <v>640</v>
       </c>
       <c r="G974" s="23" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="H974" s="23"/>
       <c r="I974" s="23"/>
     </row>
-    <row r="975" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="975" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A975" s="9"/>
       <c r="B975" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C975" s="25"/>
-      <c r="D975" s="22"/>
+      <c r="D975" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E975" s="22" t="s">
         <v>22</v>
       </c>
@@ -22232,20 +22241,18 @@
         <v>640</v>
       </c>
       <c r="G975" s="23" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="H975" s="23"/>
       <c r="I975" s="23"/>
     </row>
-    <row r="976" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="976" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A976" s="9"/>
       <c r="B976" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C976" s="25"/>
-      <c r="D976" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="D976" s="22"/>
       <c r="E976" s="22" t="s">
         <v>22</v>
       </c>
@@ -22253,7 +22260,7 @@
         <v>640</v>
       </c>
       <c r="G976" s="23" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="H976" s="23"/>
       <c r="I976" s="23"/>
@@ -22274,7 +22281,7 @@
         <v>640</v>
       </c>
       <c r="G977" s="23" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="H977" s="23"/>
       <c r="I977" s="23"/>
@@ -22295,7 +22302,7 @@
         <v>640</v>
       </c>
       <c r="G978" s="23" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="H978" s="23"/>
       <c r="I978" s="23"/>
@@ -22305,9 +22312,7 @@
       <c r="B979" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C979" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C979" s="25"/>
       <c r="D979" s="22" t="s">
         <v>22</v>
       </c>
@@ -22318,7 +22323,7 @@
         <v>640</v>
       </c>
       <c r="G979" s="23" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="H979" s="23"/>
       <c r="I979" s="23"/>
@@ -22341,7 +22346,7 @@
         <v>640</v>
       </c>
       <c r="G980" s="23" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="H980" s="23"/>
       <c r="I980" s="23"/>
@@ -22351,8 +22356,12 @@
       <c r="B981" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C981" s="25"/>
-      <c r="D981" s="22"/>
+      <c r="C981" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D981" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E981" s="22" t="s">
         <v>22</v>
       </c>
@@ -22360,7 +22369,7 @@
         <v>640</v>
       </c>
       <c r="G981" s="23" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="H981" s="23"/>
       <c r="I981" s="23"/>
@@ -22370,12 +22379,8 @@
       <c r="B982" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C982" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D982" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C982" s="25"/>
+      <c r="D982" s="22"/>
       <c r="E982" s="22" t="s">
         <v>22</v>
       </c>
@@ -22383,7 +22388,7 @@
         <v>640</v>
       </c>
       <c r="G982" s="23" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="H982" s="23"/>
       <c r="I982" s="23"/>
@@ -22406,7 +22411,7 @@
         <v>640</v>
       </c>
       <c r="G983" s="23" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="H983" s="23"/>
       <c r="I983" s="23"/>
@@ -22416,8 +22421,12 @@
       <c r="B984" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C984" s="25"/>
-      <c r="D984" s="22"/>
+      <c r="C984" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D984" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E984" s="22" t="s">
         <v>22</v>
       </c>
@@ -22425,7 +22434,7 @@
         <v>640</v>
       </c>
       <c r="G984" s="23" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="H984" s="23"/>
       <c r="I984" s="23"/>
@@ -22435,12 +22444,8 @@
       <c r="B985" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C985" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D985" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C985" s="25"/>
+      <c r="D985" s="22"/>
       <c r="E985" s="22" t="s">
         <v>22</v>
       </c>
@@ -22448,7 +22453,7 @@
         <v>640</v>
       </c>
       <c r="G985" s="23" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="H985" s="23"/>
       <c r="I985" s="23"/>
@@ -22458,8 +22463,12 @@
       <c r="B986" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C986" s="25"/>
-      <c r="D986" s="22"/>
+      <c r="C986" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D986" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E986" s="22" t="s">
         <v>22</v>
       </c>
@@ -22467,7 +22476,7 @@
         <v>640</v>
       </c>
       <c r="G986" s="23" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="H986" s="23"/>
       <c r="I986" s="23"/>
@@ -22477,12 +22486,8 @@
       <c r="B987" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C987" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D987" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C987" s="25"/>
+      <c r="D987" s="22"/>
       <c r="E987" s="22" t="s">
         <v>22</v>
       </c>
@@ -22490,7 +22495,7 @@
         <v>640</v>
       </c>
       <c r="G987" s="23" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="H987" s="23"/>
       <c r="I987" s="23"/>
@@ -22513,7 +22518,7 @@
         <v>640</v>
       </c>
       <c r="G988" s="23" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="H988" s="23"/>
       <c r="I988" s="23"/>
@@ -22536,7 +22541,7 @@
         <v>640</v>
       </c>
       <c r="G989" s="23" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="H989" s="23"/>
       <c r="I989" s="23"/>
@@ -22559,7 +22564,7 @@
         <v>640</v>
       </c>
       <c r="G990" s="23" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="H990" s="23"/>
       <c r="I990" s="23"/>
@@ -22582,7 +22587,7 @@
         <v>640</v>
       </c>
       <c r="G991" s="23" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="H991" s="23"/>
       <c r="I991" s="23"/>
@@ -22592,8 +22597,12 @@
       <c r="B992" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C992" s="25"/>
-      <c r="D992" s="22"/>
+      <c r="C992" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D992" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E992" s="22" t="s">
         <v>22</v>
       </c>
@@ -22601,7 +22610,7 @@
         <v>640</v>
       </c>
       <c r="G992" s="23" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="H992" s="23"/>
       <c r="I992" s="23"/>
@@ -22611,12 +22620,8 @@
       <c r="B993" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C993" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D993" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C993" s="25"/>
+      <c r="D993" s="22"/>
       <c r="E993" s="22" t="s">
         <v>22</v>
       </c>
@@ -22624,7 +22629,7 @@
         <v>640</v>
       </c>
       <c r="G993" s="23" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="H993" s="23"/>
       <c r="I993" s="23"/>
@@ -22647,7 +22652,7 @@
         <v>640</v>
       </c>
       <c r="G994" s="23" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="H994" s="23"/>
       <c r="I994" s="23"/>
@@ -22670,7 +22675,7 @@
         <v>640</v>
       </c>
       <c r="G995" s="23" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="H995" s="23"/>
       <c r="I995" s="23"/>
@@ -22693,54 +22698,54 @@
         <v>640</v>
       </c>
       <c r="G996" s="23" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="H996" s="23"/>
       <c r="I996" s="23"/>
     </row>
-    <row r="997" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="997" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A997" s="9"/>
-      <c r="B997" s="25" t="s">
-        <v>611</v>
-      </c>
-      <c r="C997" s="25"/>
+      <c r="B997" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C997" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D997" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E997" s="25"/>
+      <c r="E997" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F997" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G997" s="23" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="H997" s="23"/>
-      <c r="I997" s="23" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="998" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I997" s="23"/>
+    </row>
+    <row r="998" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A998" s="9"/>
-      <c r="B998" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C998" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B998" s="25" t="s">
+        <v>611</v>
+      </c>
+      <c r="C998" s="25"/>
       <c r="D998" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E998" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="E998" s="25"/>
       <c r="F998" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G998" s="23" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="H998" s="23"/>
-      <c r="I998" s="23"/>
+      <c r="I998" s="23" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="999" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A999" s="9"/>
@@ -22760,7 +22765,7 @@
         <v>640</v>
       </c>
       <c r="G999" s="23" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="H999" s="23"/>
       <c r="I999" s="23"/>
@@ -22783,7 +22788,7 @@
         <v>640</v>
       </c>
       <c r="G1000" s="23" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="H1000" s="23"/>
       <c r="I1000" s="23"/>
@@ -22806,7 +22811,7 @@
         <v>640</v>
       </c>
       <c r="G1001" s="23" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="H1001" s="23"/>
       <c r="I1001" s="23"/>
@@ -22829,7 +22834,7 @@
         <v>640</v>
       </c>
       <c r="G1002" s="23" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="H1002" s="23"/>
       <c r="I1002" s="23"/>
@@ -22852,7 +22857,7 @@
         <v>640</v>
       </c>
       <c r="G1003" s="23" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="H1003" s="23"/>
       <c r="I1003" s="23"/>
@@ -22875,7 +22880,7 @@
         <v>640</v>
       </c>
       <c r="G1004" s="23" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="H1004" s="23"/>
       <c r="I1004" s="23"/>
@@ -22885,8 +22890,12 @@
       <c r="B1005" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C1005" s="25"/>
-      <c r="D1005" s="22"/>
+      <c r="C1005" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1005" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="E1005" s="22" t="s">
         <v>22</v>
       </c>
@@ -22894,12 +22903,13 @@
         <v>640</v>
       </c>
       <c r="G1005" s="23" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="H1005" s="23"/>
       <c r="I1005" s="23"/>
     </row>
     <row r="1006" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1006" s="9"/>
       <c r="B1006" s="22" t="s">
         <v>22</v>
       </c>
@@ -22912,7 +22922,7 @@
         <v>640</v>
       </c>
       <c r="G1006" s="23" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="H1006" s="23"/>
       <c r="I1006" s="23"/>
@@ -22930,7 +22940,7 @@
         <v>640</v>
       </c>
       <c r="G1007" s="23" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="H1007" s="23"/>
       <c r="I1007" s="23"/>
@@ -22939,12 +22949,8 @@
       <c r="B1008" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C1008" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1008" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C1008" s="25"/>
+      <c r="D1008" s="22"/>
       <c r="E1008" s="22" t="s">
         <v>22</v>
       </c>
@@ -22952,7 +22958,7 @@
         <v>640</v>
       </c>
       <c r="G1008" s="23" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="H1008" s="23"/>
       <c r="I1008" s="23"/>
@@ -22961,14 +22967,20 @@
       <c r="B1009" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C1009" s="25"/>
-      <c r="D1009" s="22"/>
-      <c r="E1009" s="25"/>
+      <c r="C1009" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1009" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1009" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="F1009" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G1009" s="23" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="H1009" s="23"/>
       <c r="I1009" s="23"/>
@@ -22977,20 +22989,14 @@
       <c r="B1010" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C1010" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1010" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1010" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="C1010" s="25"/>
+      <c r="D1010" s="22"/>
+      <c r="E1010" s="25"/>
       <c r="F1010" s="22" t="s">
         <v>640</v>
       </c>
       <c r="G1010" s="23" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="H1010" s="23"/>
       <c r="I1010" s="23"/>
@@ -23009,10 +23015,10 @@
         <v>22</v>
       </c>
       <c r="F1011" s="22" t="s">
-        <v>1028</v>
+        <v>640</v>
       </c>
       <c r="G1011" s="23" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="H1011" s="23"/>
       <c r="I1011" s="23"/>
@@ -23021,7 +23027,9 @@
       <c r="B1012" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C1012" s="25"/>
+      <c r="C1012" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D1012" s="22" t="s">
         <v>22</v>
       </c>
@@ -23029,79 +23037,98 @@
         <v>22</v>
       </c>
       <c r="F1012" s="22" t="s">
-        <v>1028</v>
+        <v>1031</v>
       </c>
       <c r="G1012" s="23" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="H1012" s="23"/>
-      <c r="I1012" s="23" t="s">
+      <c r="I1012" s="23"/>
+    </row>
+    <row r="1013" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1013" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1013" s="25"/>
+      <c r="D1013" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1013" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1013" s="22" t="s">
         <v>1031</v>
       </c>
-    </row>
-    <row r="1013" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1013" s="27" t="s">
+      <c r="G1013" s="23" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H1013" s="23"/>
+      <c r="I1013" s="23" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="1014" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1014" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="C1013" s="27"/>
-      <c r="D1013" s="27" t="s">
+      <c r="C1014" s="27"/>
+      <c r="D1014" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="E1013" s="27"/>
-      <c r="F1013" s="27" t="s">
+      <c r="E1014" s="27"/>
+      <c r="F1014" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="G1013" s="28" t="s">
-        <v>1032</v>
-      </c>
-      <c r="H1013" s="28"/>
-      <c r="I1013" s="28" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="1014" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1014" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1014" s="25"/>
-      <c r="D1014" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1014" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1014" s="22" t="s">
-        <v>1028</v>
-      </c>
-      <c r="G1014" s="23" t="s">
+      <c r="G1014" s="28" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H1014" s="28"/>
+      <c r="I1014" s="28" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="1015" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1015" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1015" s="25"/>
+      <c r="D1015" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1015" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1015" s="22" t="s">
+        <v>1031</v>
+      </c>
+      <c r="G1015" s="23" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H1015" s="23"/>
+      <c r="I1015" s="23" t="s">
         <v>1034</v>
       </c>
-      <c r="H1014" s="23"/>
-      <c r="I1014" s="23" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="1015" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1015" s="27" t="s">
+    </row>
+    <row r="1016" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1016" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="C1015" s="27"/>
-      <c r="D1015" s="27" t="s">
+      <c r="C1016" s="27"/>
+      <c r="D1016" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="E1015" s="27"/>
-      <c r="F1015" s="27" t="s">
+      <c r="E1016" s="27"/>
+      <c r="F1016" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="G1015" s="28" t="s">
-        <v>1035</v>
-      </c>
-      <c r="H1015" s="28"/>
-      <c r="I1015" s="28" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G1016" s="28" t="s">
+        <v>1038</v>
+      </c>
+      <c r="H1016" s="28"/>
+      <c r="I1016" s="28" t="s">
+        <v>1036</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
continued documentation --  Also added 1 new VI --  MathUtil_ApplyDeadband (this one can do joystick deadband...)
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4848" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4898" uniqueCount="1159">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -3016,6 +3016,9 @@
     <t xml:space="preserve">Matrix_ExtractFrom.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">Matrix_ExtractMatrix.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Matrix_ExtractRowVector.vi</t>
   </si>
   <si>
@@ -3040,6 +3043,9 @@
     <t xml:space="preserve">Matrix_SetRow.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">THERE ARE LOTS OF OTHER MATRIX FUNCTIONS THAT SHOULD BE INCLUDED HERE FOR ISOLATION.</t>
+  </si>
+  <si>
     <t xml:space="preserve">MATRIX HELPER</t>
   </si>
   <si>
@@ -3119,6 +3125,9 @@
   </si>
   <si>
     <t xml:space="preserve">MathUtil_Clamp.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MathUtil_ApplyDeadband.vi</t>
   </si>
   <si>
     <t xml:space="preserve">MathUtil_Clamp_Int.vi</t>
@@ -3937,10 +3946,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:Q1131"/>
+  <dimension ref="A1:Q1133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A908" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A927" activeCellId="0" sqref="A927"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4051,35 +4060,35 @@
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">B10+B11</f>
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C18:C1458,"X")</f>
-        <v>544</v>
+        <f aca="false">COUNTIF(C18:C1460,"X")</f>
+        <v>589</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D18:D1458,"X")</f>
+        <f aca="false">COUNTIF(D18:D1460,"X")</f>
         <v>217</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E18:E1458,"X")</f>
+        <f aca="false">COUNTIF(E18:E1460,"X")</f>
         <v>634</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F18:F1458,"S")+COUNTIF(F18:F1458,"I")+COUNTIF(F18:F1458,"X")+COUNTIF(F18:F1458,"SI")+COUNTIF(F18:F1458,"IS")+COUNTIF(F18:F1458,"N/A")</f>
+        <f aca="false">COUNTIF(F18:F1460,"S")+COUNTIF(F18:F1460,"I")+COUNTIF(F18:F1460,"X")+COUNTIF(F18:F1460,"SI")+COUNTIF(F18:F1460,"IS")+COUNTIF(F18:F1460,"N/A")</f>
         <v>231</v>
       </c>
       <c r="G9" s="13" t="n">
-        <f aca="false">COUNTIF(G18:G1458,"S")+COUNTIF(G18:G1458,"I")+COUNTIF(G18:G1458,"X")+COUNTIF(G18:G1458,"SI")+COUNTIF(G18:G1458,"IS")+COUNTIF(G18:G1458,"N/A")</f>
+        <f aca="false">COUNTIF(G18:G1460,"S")+COUNTIF(G18:G1460,"I")+COUNTIF(G18:G1460,"X")+COUNTIF(G18:G1460,"SI")+COUNTIF(G18:G1460,"IS")+COUNTIF(G18:G1460,"N/A")</f>
         <v>25</v>
       </c>
       <c r="H9" s="13" t="n">
-        <f aca="false">COUNTIF(H18:H1458,"S")+COUNTIF(H18:H1458,"I")+COUNTIF(H18:H1458,"X")+COUNTIF(H18:H1458,"SI")+COUNTIF(H18:H1458,"IS")+COUNTIF(H18:H1458,"N/A")</f>
+        <f aca="false">COUNTIF(H18:H1460,"S")+COUNTIF(H18:H1460,"I")+COUNTIF(H18:H1460,"X")+COUNTIF(H18:H1460,"SI")+COUNTIF(H18:H1460,"IS")+COUNTIF(H18:H1460,"N/A")</f>
         <v>12</v>
       </c>
       <c r="I9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.74931129476584</v>
+        <v>0.809065934065934</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4087,8 +4096,8 @@
         <v>14</v>
       </c>
       <c r="B10" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1458,"X")</f>
-        <v>651</v>
+        <f aca="false">COUNTIF(B18:B1460,"X")</f>
+        <v>653</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>15</v>
@@ -4099,12 +4108,12 @@
         <v>16</v>
       </c>
       <c r="B11" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1458,"Z")</f>
+        <f aca="false">COUNTIF(B18:B1460,"Z")</f>
         <v>75</v>
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.318181818181818</v>
+        <v>0.317307692307692</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4112,7 +4121,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1458,"/")</f>
+        <f aca="false">COUNTIF(B18:B1460,"/")</f>
         <v>11</v>
       </c>
       <c r="I12" s="4"/>
@@ -4122,7 +4131,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1458,"\")</f>
+        <f aca="false">COUNTIF(B18:B1460,"\")</f>
         <v>3</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -24627,7 +24636,9 @@
       <c r="B944" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C944" s="26"/>
+      <c r="C944" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D944" s="22"/>
       <c r="E944" s="22" t="s">
         <v>27</v>
@@ -24648,7 +24659,9 @@
       <c r="B945" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C945" s="26"/>
+      <c r="C945" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D945" s="22"/>
       <c r="E945" s="22" t="s">
         <v>27</v>
@@ -24669,7 +24682,9 @@
       <c r="B946" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C946" s="26"/>
+      <c r="C946" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D946" s="22"/>
       <c r="E946" s="22" t="s">
         <v>27</v>
@@ -24690,7 +24705,9 @@
       <c r="B947" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C947" s="26"/>
+      <c r="C947" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D947" s="22"/>
       <c r="E947" s="22" t="s">
         <v>27</v>
@@ -24711,7 +24728,9 @@
       <c r="B948" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C948" s="26"/>
+      <c r="C948" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D948" s="22"/>
       <c r="E948" s="22" t="s">
         <v>27</v>
@@ -24732,7 +24751,9 @@
       <c r="B949" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C949" s="26"/>
+      <c r="C949" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D949" s="22"/>
       <c r="E949" s="22" t="s">
         <v>27</v>
@@ -24753,7 +24774,9 @@
       <c r="B950" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C950" s="26"/>
+      <c r="C950" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D950" s="22"/>
       <c r="E950" s="22" t="s">
         <v>27</v>
@@ -24774,7 +24797,9 @@
       <c r="B951" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C951" s="26"/>
+      <c r="C951" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D951" s="22"/>
       <c r="E951" s="22" t="s">
         <v>27</v>
@@ -24797,9 +24822,7 @@
       </c>
       <c r="C952" s="26"/>
       <c r="D952" s="22"/>
-      <c r="E952" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E952" s="26"/>
       <c r="F952" s="26"/>
       <c r="G952" s="22"/>
       <c r="H952" s="22"/>
@@ -24816,7 +24839,9 @@
       <c r="B953" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C953" s="26"/>
+      <c r="C953" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D953" s="22"/>
       <c r="E953" s="22" t="s">
         <v>27</v>
@@ -24837,7 +24862,9 @@
       <c r="B954" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C954" s="26"/>
+      <c r="C954" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D954" s="22"/>
       <c r="E954" s="22" t="s">
         <v>27</v>
@@ -24858,7 +24885,9 @@
       <c r="B955" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C955" s="26"/>
+      <c r="C955" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D955" s="22"/>
       <c r="E955" s="22" t="s">
         <v>27</v>
@@ -24879,7 +24908,9 @@
       <c r="B956" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C956" s="26"/>
+      <c r="C956" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D956" s="22"/>
       <c r="E956" s="22" t="s">
         <v>27</v>
@@ -24900,7 +24931,9 @@
       <c r="B957" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C957" s="26"/>
+      <c r="C957" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D957" s="22"/>
       <c r="E957" s="22" t="s">
         <v>27</v>
@@ -24921,7 +24954,9 @@
       <c r="B958" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C958" s="26"/>
+      <c r="C958" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D958" s="22"/>
       <c r="E958" s="22" t="s">
         <v>27</v>
@@ -24942,7 +24977,9 @@
       <c r="B959" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C959" s="26"/>
+      <c r="C959" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D959" s="22"/>
       <c r="E959" s="22" t="s">
         <v>27</v>
@@ -24959,115 +24996,117 @@
       <c r="M959" s="22"/>
       <c r="N959" s="22"/>
     </row>
-    <row r="960" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B960" s="22"/>
-      <c r="C960" s="22"/>
+    <row r="960" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B960" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C960" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D960" s="22"/>
-      <c r="E960" s="22"/>
-      <c r="F960" s="22"/>
+      <c r="E960" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F960" s="26"/>
       <c r="G960" s="22"/>
       <c r="H960" s="22"/>
-      <c r="I960" s="23"/>
-      <c r="J960" s="23"/>
+      <c r="I960" s="23" t="s">
+        <v>1005</v>
+      </c>
+      <c r="J960" s="23" t="s">
+        <v>1006</v>
+      </c>
       <c r="K960" s="23"/>
       <c r="L960" s="22"/>
       <c r="M960" s="22"/>
       <c r="N960" s="22"/>
     </row>
     <row r="961" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A961" s="19"/>
-      <c r="B961" s="45"/>
-      <c r="C961" s="4"/>
-      <c r="D961" s="4"/>
-      <c r="E961" s="4"/>
-      <c r="F961" s="4"/>
-      <c r="G961" s="4"/>
-      <c r="H961" s="4"/>
+      <c r="B961" s="22"/>
+      <c r="C961" s="22"/>
+      <c r="D961" s="22"/>
+      <c r="E961" s="22"/>
+      <c r="F961" s="22"/>
+      <c r="G961" s="22"/>
+      <c r="H961" s="22"/>
+      <c r="I961" s="23"/>
+      <c r="J961" s="23"/>
+      <c r="K961" s="23"/>
+      <c r="L961" s="22"/>
+      <c r="M961" s="22"/>
+      <c r="N961" s="22"/>
     </row>
     <row r="962" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B962" s="47"/>
-      <c r="C962" s="1"/>
-      <c r="D962" s="1"/>
-      <c r="E962" s="1"/>
-      <c r="F962" s="1"/>
-      <c r="G962" s="1"/>
-      <c r="H962" s="1"/>
-      <c r="I962" s="1"/>
-      <c r="J962" s="1"/>
-      <c r="K962" s="1"/>
-      <c r="L962" s="1"/>
-      <c r="M962" s="1"/>
-      <c r="N962" s="1"/>
-    </row>
-    <row r="963" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A963" s="19"/>
-      <c r="B963" s="11" t="s">
+      <c r="A962" s="19"/>
+      <c r="B962" s="45"/>
+      <c r="C962" s="4"/>
+      <c r="D962" s="4"/>
+      <c r="E962" s="4"/>
+      <c r="F962" s="4"/>
+      <c r="G962" s="4"/>
+      <c r="H962" s="4"/>
+    </row>
+    <row r="963" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B963" s="47"/>
+      <c r="C963" s="1"/>
+      <c r="D963" s="1"/>
+      <c r="E963" s="1"/>
+      <c r="F963" s="1"/>
+      <c r="G963" s="1"/>
+      <c r="H963" s="1"/>
+      <c r="I963" s="1"/>
+      <c r="J963" s="1"/>
+      <c r="K963" s="1"/>
+      <c r="L963" s="1"/>
+      <c r="M963" s="1"/>
+      <c r="N963" s="1"/>
+    </row>
+    <row r="964" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A964" s="19"/>
+      <c r="B964" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C963" s="11" t="s">
+      <c r="C964" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D963" s="11" t="s">
+      <c r="D964" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E963" s="11" t="s">
+      <c r="E964" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F963" s="11" t="s">
+      <c r="F964" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G963" s="11" t="s">
+      <c r="G964" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H963" s="11" t="s">
+      <c r="H964" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I963" s="20" t="s">
+      <c r="I964" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J963" s="20" t="s">
+      <c r="J964" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K963" s="20" t="s">
+      <c r="K964" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L963" s="11" t="s">
+      <c r="L964" s="11" t="s">
         <v>702</v>
       </c>
-      <c r="M963" s="11" t="s">
+      <c r="M964" s="11" t="s">
         <v>703</v>
       </c>
-      <c r="N963" s="11" t="s">
+      <c r="N964" s="11" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="964" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A964" s="21" t="s">
-        <v>1005</v>
-      </c>
-      <c r="B964" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C964" s="26"/>
-      <c r="D964" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E964" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F964" s="26"/>
-      <c r="G964" s="22"/>
-      <c r="H964" s="22"/>
-      <c r="I964" s="23" t="s">
-        <v>1006</v>
-      </c>
-      <c r="J964" s="23"/>
-      <c r="K964" s="23"/>
-      <c r="L964" s="22"/>
-      <c r="M964" s="22"/>
-      <c r="N964" s="22"/>
-    </row>
     <row r="965" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A965" s="21" t="s">
+        <v>1007</v>
+      </c>
       <c r="B965" s="22" t="s">
         <v>27</v>
       </c>
@@ -25082,7 +25121,7 @@
       <c r="G965" s="22"/>
       <c r="H965" s="22"/>
       <c r="I965" s="23" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="J965" s="23"/>
       <c r="K965" s="23"/>
@@ -25105,7 +25144,7 @@
       <c r="G966" s="22"/>
       <c r="H966" s="22"/>
       <c r="I966" s="23" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="J966" s="23"/>
       <c r="K966" s="23"/>
@@ -25113,25 +25152,31 @@
       <c r="M966" s="22"/>
       <c r="N966" s="22"/>
     </row>
-    <row r="967" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B967" s="1"/>
-      <c r="C967" s="1"/>
-      <c r="D967" s="1"/>
-      <c r="E967" s="1"/>
-      <c r="F967" s="1"/>
-      <c r="G967" s="1"/>
-      <c r="H967" s="1"/>
-      <c r="I967" s="1"/>
-      <c r="J967" s="1"/>
-      <c r="K967" s="1"/>
-      <c r="L967" s="1"/>
-      <c r="M967" s="1"/>
-      <c r="N967" s="1"/>
-      <c r="O967" s="1"/>
-      <c r="P967" s="1"/>
+    <row r="967" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B967" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C967" s="26"/>
+      <c r="D967" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E967" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F967" s="26"/>
+      <c r="G967" s="22"/>
+      <c r="H967" s="22"/>
+      <c r="I967" s="23" t="s">
+        <v>1010</v>
+      </c>
+      <c r="J967" s="23"/>
+      <c r="K967" s="23"/>
+      <c r="L967" s="22"/>
+      <c r="M967" s="22"/>
+      <c r="N967" s="22"/>
     </row>
     <row r="968" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B968" s="47"/>
+      <c r="B968" s="1"/>
       <c r="C968" s="1"/>
       <c r="D968" s="1"/>
       <c r="E968" s="1"/>
@@ -25144,78 +25189,76 @@
       <c r="L968" s="1"/>
       <c r="M968" s="1"/>
       <c r="N968" s="1"/>
-    </row>
-    <row r="969" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A969" s="19"/>
-      <c r="B969" s="11" t="s">
+      <c r="O968" s="1"/>
+      <c r="P968" s="1"/>
+    </row>
+    <row r="969" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B969" s="47"/>
+      <c r="C969" s="1"/>
+      <c r="D969" s="1"/>
+      <c r="E969" s="1"/>
+      <c r="F969" s="1"/>
+      <c r="G969" s="1"/>
+      <c r="H969" s="1"/>
+      <c r="I969" s="1"/>
+      <c r="J969" s="1"/>
+      <c r="K969" s="1"/>
+      <c r="L969" s="1"/>
+      <c r="M969" s="1"/>
+      <c r="N969" s="1"/>
+    </row>
+    <row r="970" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A970" s="19"/>
+      <c r="B970" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C969" s="11" t="s">
+      <c r="C970" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D969" s="11" t="s">
+      <c r="D970" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E969" s="11" t="s">
+      <c r="E970" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F969" s="11" t="s">
+      <c r="F970" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G969" s="11" t="s">
+      <c r="G970" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H969" s="11" t="s">
+      <c r="H970" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I969" s="20" t="s">
+      <c r="I970" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J969" s="20" t="s">
+      <c r="J970" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K969" s="20" t="s">
+      <c r="K970" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L969" s="11" t="s">
+      <c r="L970" s="11" t="s">
         <v>702</v>
       </c>
-      <c r="M969" s="11" t="s">
+      <c r="M970" s="11" t="s">
         <v>703</v>
       </c>
-      <c r="N969" s="11" t="s">
+      <c r="N970" s="11" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="970" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A970" s="21" t="s">
-        <v>1009</v>
-      </c>
-      <c r="B970" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C970" s="26"/>
-      <c r="D970" s="22"/>
-      <c r="E970" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F970" s="26"/>
-      <c r="G970" s="22"/>
-      <c r="H970" s="22"/>
-      <c r="I970" s="23" t="s">
-        <v>1010</v>
-      </c>
-      <c r="J970" s="23"/>
-      <c r="K970" s="23"/>
-      <c r="L970" s="22"/>
-      <c r="M970" s="22"/>
-      <c r="N970" s="22"/>
-    </row>
     <row r="971" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A971" s="21" t="s">
+        <v>1011</v>
+      </c>
       <c r="B971" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C971" s="26"/>
+      <c r="C971" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D971" s="22"/>
       <c r="E971" s="22" t="s">
         <v>27</v>
@@ -25224,7 +25267,7 @@
       <c r="G971" s="22"/>
       <c r="H971" s="22"/>
       <c r="I971" s="23" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="J971" s="23"/>
       <c r="K971" s="23"/>
@@ -25236,7 +25279,9 @@
       <c r="B972" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C972" s="26"/>
+      <c r="C972" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D972" s="22"/>
       <c r="E972" s="22" t="s">
         <v>27</v>
@@ -25245,7 +25290,7 @@
       <c r="G972" s="22"/>
       <c r="H972" s="22"/>
       <c r="I972" s="23" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="J972" s="23"/>
       <c r="K972" s="23"/>
@@ -25257,7 +25302,9 @@
       <c r="B973" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C973" s="26"/>
+      <c r="C973" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D973" s="22"/>
       <c r="E973" s="22" t="s">
         <v>27</v>
@@ -25266,7 +25313,7 @@
       <c r="G973" s="22"/>
       <c r="H973" s="22"/>
       <c r="I973" s="23" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="J973" s="23"/>
       <c r="K973" s="23"/>
@@ -25278,14 +25325,18 @@
       <c r="B974" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C974" s="26"/>
+      <c r="C974" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D974" s="22"/>
-      <c r="E974" s="26"/>
+      <c r="E974" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F974" s="26"/>
       <c r="G974" s="22"/>
       <c r="H974" s="22"/>
       <c r="I974" s="23" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="J974" s="23"/>
       <c r="K974" s="23"/>
@@ -25297,14 +25348,16 @@
       <c r="B975" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C975" s="26"/>
+      <c r="C975" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D975" s="22"/>
       <c r="E975" s="26"/>
       <c r="F975" s="26"/>
       <c r="G975" s="22"/>
       <c r="H975" s="22"/>
       <c r="I975" s="23" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="J975" s="23"/>
       <c r="K975" s="23"/>
@@ -25316,14 +25369,16 @@
       <c r="B976" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C976" s="26"/>
+      <c r="C976" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D976" s="22"/>
       <c r="E976" s="26"/>
       <c r="F976" s="26"/>
       <c r="G976" s="22"/>
       <c r="H976" s="22"/>
       <c r="I976" s="23" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="J976" s="23"/>
       <c r="K976" s="23"/>
@@ -25335,14 +25390,16 @@
       <c r="B977" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C977" s="26"/>
+      <c r="C977" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D977" s="22"/>
       <c r="E977" s="26"/>
       <c r="F977" s="26"/>
       <c r="G977" s="22"/>
       <c r="H977" s="22"/>
       <c r="I977" s="23" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="J977" s="23"/>
       <c r="K977" s="23"/>
@@ -25351,15 +25408,19 @@
       <c r="N977" s="22"/>
     </row>
     <row r="978" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B978" s="26"/>
-      <c r="C978" s="26"/>
+      <c r="B978" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C978" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D978" s="22"/>
-      <c r="E978" s="22"/>
+      <c r="E978" s="26"/>
       <c r="F978" s="26"/>
       <c r="G978" s="22"/>
       <c r="H978" s="22"/>
       <c r="I978" s="23" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="J978" s="23"/>
       <c r="K978" s="23"/>
@@ -25376,7 +25437,7 @@
       <c r="G979" s="22"/>
       <c r="H979" s="22"/>
       <c r="I979" s="23" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="J979" s="23"/>
       <c r="K979" s="23"/>
@@ -25385,21 +25446,15 @@
       <c r="N979" s="22"/>
     </row>
     <row r="980" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B980" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="B980" s="26"/>
       <c r="C980" s="26"/>
-      <c r="D980" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E980" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="D980" s="22"/>
+      <c r="E980" s="22"/>
       <c r="F980" s="26"/>
       <c r="G980" s="22"/>
       <c r="H980" s="22"/>
       <c r="I980" s="23" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="J980" s="23"/>
       <c r="K980" s="23"/>
@@ -25407,15 +25462,25 @@
       <c r="M980" s="22"/>
       <c r="N980" s="22"/>
     </row>
-    <row r="981" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B981" s="22"/>
-      <c r="C981" s="22"/>
-      <c r="D981" s="22"/>
-      <c r="E981" s="22"/>
-      <c r="F981" s="22"/>
+    <row r="981" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B981" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C981" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D981" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E981" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F981" s="26"/>
       <c r="G981" s="22"/>
       <c r="H981" s="22"/>
-      <c r="I981" s="23"/>
+      <c r="I981" s="23" t="s">
+        <v>1022</v>
+      </c>
       <c r="J981" s="23"/>
       <c r="K981" s="23"/>
       <c r="L981" s="22"/>
@@ -25423,33 +25488,28 @@
       <c r="N981" s="22"/>
     </row>
     <row r="982" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B982" s="1"/>
-      <c r="C982" s="1"/>
-      <c r="D982" s="1"/>
-      <c r="E982" s="1"/>
-      <c r="F982" s="1"/>
-      <c r="G982" s="1"/>
-      <c r="H982" s="1"/>
-      <c r="I982" s="1"/>
-      <c r="J982" s="1"/>
-      <c r="K982" s="1"/>
-      <c r="L982" s="1"/>
-      <c r="M982" s="1"/>
-      <c r="N982" s="1"/>
-      <c r="O982" s="1"/>
-      <c r="P982" s="1"/>
+      <c r="B982" s="22"/>
+      <c r="C982" s="22"/>
+      <c r="D982" s="22"/>
+      <c r="E982" s="22"/>
+      <c r="F982" s="22"/>
+      <c r="G982" s="22"/>
+      <c r="H982" s="22"/>
+      <c r="I982" s="23"/>
+      <c r="J982" s="23"/>
+      <c r="K982" s="23"/>
+      <c r="L982" s="22"/>
+      <c r="M982" s="22"/>
+      <c r="N982" s="22"/>
     </row>
     <row r="983" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A983" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B983" s="17"/>
-      <c r="C983" s="18"/>
-      <c r="D983" s="18"/>
-      <c r="E983" s="18"/>
-      <c r="F983" s="18"/>
-      <c r="G983" s="18"/>
-      <c r="H983" s="18"/>
+      <c r="B983" s="1"/>
+      <c r="C983" s="1"/>
+      <c r="D983" s="1"/>
+      <c r="E983" s="1"/>
+      <c r="F983" s="1"/>
+      <c r="G983" s="1"/>
+      <c r="H983" s="1"/>
       <c r="I983" s="1"/>
       <c r="J983" s="1"/>
       <c r="K983" s="1"/>
@@ -25461,7 +25521,7 @@
     </row>
     <row r="984" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A984" s="16" t="s">
-        <v>1021</v>
+        <v>20</v>
       </c>
       <c r="B984" s="17"/>
       <c r="C984" s="18"/>
@@ -25481,7 +25541,7 @@
     </row>
     <row r="985" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A985" s="16" t="s">
-        <v>20</v>
+        <v>1023</v>
       </c>
       <c r="B985" s="17"/>
       <c r="C985" s="18"/>
@@ -25500,13 +25560,16 @@
       <c r="P985" s="1"/>
     </row>
     <row r="986" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B986" s="1"/>
-      <c r="C986" s="1"/>
-      <c r="D986" s="1"/>
-      <c r="E986" s="1"/>
-      <c r="F986" s="1"/>
-      <c r="G986" s="1"/>
-      <c r="H986" s="1"/>
+      <c r="A986" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B986" s="17"/>
+      <c r="C986" s="18"/>
+      <c r="D986" s="18"/>
+      <c r="E986" s="18"/>
+      <c r="F986" s="18"/>
+      <c r="G986" s="18"/>
+      <c r="H986" s="18"/>
       <c r="I986" s="1"/>
       <c r="J986" s="1"/>
       <c r="K986" s="1"/>
@@ -25516,94 +25579,88 @@
       <c r="O986" s="1"/>
       <c r="P986" s="1"/>
     </row>
-    <row r="987" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A987" s="19"/>
-      <c r="B987" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C987" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D987" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E987" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F987" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G987" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H987" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I987" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J987" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K987" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="L987" s="11" t="s">
-        <v>702</v>
-      </c>
-      <c r="M987" s="11" t="s">
-        <v>703</v>
-      </c>
-      <c r="N987" s="11" t="s">
-        <v>704</v>
-      </c>
+    <row r="987" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B987" s="1"/>
+      <c r="C987" s="1"/>
+      <c r="D987" s="1"/>
+      <c r="E987" s="1"/>
+      <c r="F987" s="1"/>
+      <c r="G987" s="1"/>
+      <c r="H987" s="1"/>
+      <c r="I987" s="1"/>
+      <c r="J987" s="1"/>
+      <c r="K987" s="1"/>
+      <c r="L987" s="1"/>
+      <c r="M987" s="1"/>
+      <c r="N987" s="1"/>
       <c r="O987" s="1"/>
       <c r="P987" s="1"/>
     </row>
-    <row r="988" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A988" s="21" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B988" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C988" s="26"/>
-      <c r="D988" s="22"/>
-      <c r="E988" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F988" s="26"/>
-      <c r="G988" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H988" s="22"/>
-      <c r="I988" s="23" t="s">
-        <v>1023</v>
-      </c>
-      <c r="J988" s="23"/>
-      <c r="K988" s="23"/>
-      <c r="L988" s="22"/>
-      <c r="M988" s="22"/>
-      <c r="N988" s="22"/>
+    <row r="988" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A988" s="19"/>
+      <c r="B988" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C988" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D988" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E988" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F988" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G988" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H988" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I988" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J988" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K988" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="L988" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="M988" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="N988" s="11" t="s">
+        <v>704</v>
+      </c>
       <c r="O988" s="1"/>
       <c r="P988" s="1"/>
     </row>
     <row r="989" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A989" s="21" t="s">
+        <v>1024</v>
+      </c>
       <c r="B989" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C989" s="26"/>
-      <c r="D989" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="C989" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D989" s="22"/>
       <c r="E989" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F989" s="26"/>
-      <c r="G989" s="22"/>
+      <c r="G989" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="H989" s="22"/>
       <c r="I989" s="23" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="J989" s="23"/>
       <c r="K989" s="23"/>
@@ -25617,18 +25674,20 @@
       <c r="B990" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C990" s="26"/>
-      <c r="D990" s="22"/>
+      <c r="C990" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D990" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="E990" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F990" s="26"/>
-      <c r="G990" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="G990" s="22"/>
       <c r="H990" s="22"/>
       <c r="I990" s="23" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="J990" s="23"/>
       <c r="K990" s="23"/>
@@ -25642,18 +25701,20 @@
       <c r="B991" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C991" s="26"/>
-      <c r="D991" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="C991" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D991" s="22"/>
       <c r="E991" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F991" s="26"/>
-      <c r="G991" s="22"/>
+      <c r="G991" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="H991" s="22"/>
       <c r="I991" s="23" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="J991" s="23"/>
       <c r="K991" s="23"/>
@@ -25667,18 +25728,20 @@
       <c r="B992" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C992" s="26"/>
-      <c r="D992" s="22"/>
+      <c r="C992" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D992" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="E992" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F992" s="26"/>
-      <c r="G992" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="G992" s="22"/>
       <c r="H992" s="22"/>
       <c r="I992" s="23" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="J992" s="23"/>
       <c r="K992" s="23"/>
@@ -25692,18 +25755,20 @@
       <c r="B993" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C993" s="26"/>
-      <c r="D993" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="C993" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D993" s="22"/>
       <c r="E993" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F993" s="26"/>
-      <c r="G993" s="22"/>
+      <c r="G993" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="H993" s="22"/>
       <c r="I993" s="23" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="J993" s="23"/>
       <c r="K993" s="23"/>
@@ -25713,15 +25778,25 @@
       <c r="O993" s="1"/>
       <c r="P993" s="1"/>
     </row>
-    <row r="994" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B994" s="22"/>
-      <c r="C994" s="22"/>
-      <c r="D994" s="22"/>
-      <c r="E994" s="22"/>
-      <c r="F994" s="22"/>
+    <row r="994" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B994" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C994" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D994" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E994" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F994" s="26"/>
       <c r="G994" s="22"/>
       <c r="H994" s="22"/>
-      <c r="I994" s="23"/>
+      <c r="I994" s="23" t="s">
+        <v>1030</v>
+      </c>
       <c r="J994" s="23"/>
       <c r="K994" s="23"/>
       <c r="L994" s="22"/>
@@ -25731,97 +25806,93 @@
       <c r="P994" s="1"/>
     </row>
     <row r="995" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B995" s="1"/>
-      <c r="C995" s="1"/>
-      <c r="D995" s="1"/>
-      <c r="E995" s="1"/>
-      <c r="F995" s="1"/>
-      <c r="G995" s="1"/>
-      <c r="H995" s="1"/>
-      <c r="I995" s="1"/>
-      <c r="J995" s="1"/>
-      <c r="K995" s="1"/>
-      <c r="L995" s="1"/>
-      <c r="M995" s="1"/>
-      <c r="N995" s="1"/>
+      <c r="B995" s="22"/>
+      <c r="C995" s="22"/>
+      <c r="D995" s="22"/>
+      <c r="E995" s="22"/>
+      <c r="F995" s="22"/>
+      <c r="G995" s="22"/>
+      <c r="H995" s="22"/>
+      <c r="I995" s="23"/>
+      <c r="J995" s="23"/>
+      <c r="K995" s="23"/>
+      <c r="L995" s="22"/>
+      <c r="M995" s="22"/>
+      <c r="N995" s="22"/>
       <c r="O995" s="1"/>
       <c r="P995" s="1"/>
     </row>
-    <row r="996" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A996" s="19"/>
-      <c r="B996" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C996" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D996" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E996" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F996" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G996" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H996" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I996" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J996" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K996" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="L996" s="11" t="s">
-        <v>702</v>
-      </c>
-      <c r="M996" s="11" t="s">
-        <v>703</v>
-      </c>
-      <c r="N996" s="11" t="s">
-        <v>704</v>
-      </c>
+    <row r="996" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B996" s="1"/>
+      <c r="C996" s="1"/>
+      <c r="D996" s="1"/>
+      <c r="E996" s="1"/>
+      <c r="F996" s="1"/>
+      <c r="G996" s="1"/>
+      <c r="H996" s="1"/>
+      <c r="I996" s="1"/>
+      <c r="J996" s="1"/>
+      <c r="K996" s="1"/>
+      <c r="L996" s="1"/>
+      <c r="M996" s="1"/>
+      <c r="N996" s="1"/>
       <c r="O996" s="1"/>
       <c r="P996" s="1"/>
     </row>
-    <row r="997" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A997" s="21" t="s">
-        <v>1029</v>
-      </c>
-      <c r="B997" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C997" s="26"/>
-      <c r="D997" s="22"/>
-      <c r="E997" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F997" s="26"/>
-      <c r="G997" s="22"/>
-      <c r="H997" s="22"/>
-      <c r="I997" s="23" t="s">
-        <v>1030</v>
-      </c>
-      <c r="J997" s="23"/>
-      <c r="K997" s="23"/>
-      <c r="L997" s="22"/>
-      <c r="M997" s="22"/>
-      <c r="N997" s="22"/>
+    <row r="997" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A997" s="19"/>
+      <c r="B997" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C997" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D997" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E997" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F997" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G997" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H997" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I997" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J997" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K997" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="L997" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="M997" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="N997" s="11" t="s">
+        <v>704</v>
+      </c>
       <c r="O997" s="1"/>
       <c r="P997" s="1"/>
     </row>
     <row r="998" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A998" s="21" t="s">
+        <v>1031</v>
+      </c>
       <c r="B998" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C998" s="26"/>
+      <c r="C998" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D998" s="22"/>
       <c r="E998" s="22" t="s">
         <v>27</v>
@@ -25830,7 +25901,7 @@
       <c r="G998" s="22"/>
       <c r="H998" s="22"/>
       <c r="I998" s="23" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="J998" s="23"/>
       <c r="K998" s="23"/>
@@ -25844,7 +25915,9 @@
       <c r="B999" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C999" s="26"/>
+      <c r="C999" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D999" s="22"/>
       <c r="E999" s="22" t="s">
         <v>27</v>
@@ -25853,7 +25926,7 @@
       <c r="G999" s="22"/>
       <c r="H999" s="22"/>
       <c r="I999" s="23" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="J999" s="23"/>
       <c r="K999" s="23"/>
@@ -25867,16 +25940,16 @@
       <c r="B1000" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1000" s="26"/>
+      <c r="C1000" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1000" s="22"/>
-      <c r="E1000" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1000" s="26"/>
       <c r="F1000" s="26"/>
       <c r="G1000" s="22"/>
       <c r="H1000" s="22"/>
       <c r="I1000" s="23" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="J1000" s="23"/>
       <c r="K1000" s="23"/>
@@ -25886,15 +25959,23 @@
       <c r="O1000" s="1"/>
       <c r="P1000" s="1"/>
     </row>
-    <row r="1001" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1001" s="22"/>
-      <c r="C1001" s="22"/>
+    <row r="1001" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1001" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1001" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1001" s="22"/>
-      <c r="E1001" s="22"/>
-      <c r="F1001" s="22"/>
+      <c r="E1001" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1001" s="26"/>
       <c r="G1001" s="22"/>
       <c r="H1001" s="22"/>
-      <c r="I1001" s="23"/>
+      <c r="I1001" s="23" t="s">
+        <v>1035</v>
+      </c>
       <c r="J1001" s="23"/>
       <c r="K1001" s="23"/>
       <c r="L1001" s="22"/>
@@ -25903,116 +25984,122 @@
       <c r="O1001" s="1"/>
       <c r="P1001" s="1"/>
     </row>
-    <row r="1002" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1002" s="47"/>
-      <c r="C1002" s="1"/>
-      <c r="D1002" s="1"/>
-      <c r="E1002" s="1"/>
-      <c r="F1002" s="1"/>
-      <c r="G1002" s="1"/>
-      <c r="H1002" s="1"/>
-      <c r="I1002" s="1"/>
-      <c r="J1002" s="1"/>
-      <c r="K1002" s="1"/>
-      <c r="L1002" s="1"/>
-      <c r="M1002" s="1"/>
-      <c r="N1002" s="1"/>
-    </row>
-    <row r="1003" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1003" s="19"/>
-      <c r="B1003" s="11" t="s">
+    <row r="1002" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1002" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1002" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1002" s="22"/>
+      <c r="E1002" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1002" s="26"/>
+      <c r="G1002" s="22"/>
+      <c r="H1002" s="22"/>
+      <c r="I1002" s="23" t="s">
+        <v>1036</v>
+      </c>
+      <c r="J1002" s="23"/>
+      <c r="K1002" s="23"/>
+      <c r="L1002" s="22"/>
+      <c r="M1002" s="22"/>
+      <c r="N1002" s="22"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+    </row>
+    <row r="1003" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1003" s="22"/>
+      <c r="C1003" s="22"/>
+      <c r="D1003" s="22"/>
+      <c r="E1003" s="22"/>
+      <c r="F1003" s="22"/>
+      <c r="G1003" s="22"/>
+      <c r="H1003" s="22"/>
+      <c r="I1003" s="23"/>
+      <c r="J1003" s="23"/>
+      <c r="K1003" s="23"/>
+      <c r="L1003" s="22"/>
+      <c r="M1003" s="22"/>
+      <c r="N1003" s="22"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+    </row>
+    <row r="1004" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1004" s="47"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="1"/>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1"/>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="1"/>
+      <c r="K1004" s="1"/>
+      <c r="L1004" s="1"/>
+      <c r="M1004" s="1"/>
+      <c r="N1004" s="1"/>
+    </row>
+    <row r="1005" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1005" s="19"/>
+      <c r="B1005" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1003" s="11" t="s">
+      <c r="C1005" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1003" s="11" t="s">
+      <c r="D1005" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1003" s="11" t="s">
+      <c r="E1005" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1003" s="11" t="s">
+      <c r="F1005" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G1003" s="11" t="s">
+      <c r="G1005" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1003" s="11" t="s">
+      <c r="H1005" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1003" s="20" t="s">
+      <c r="I1005" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1003" s="20" t="s">
+      <c r="J1005" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1003" s="20" t="s">
+      <c r="K1005" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L1003" s="11" t="s">
+      <c r="L1005" s="11" t="s">
         <v>702</v>
       </c>
-      <c r="M1003" s="11" t="s">
+      <c r="M1005" s="11" t="s">
         <v>703</v>
       </c>
-      <c r="N1003" s="11" t="s">
+      <c r="N1005" s="11" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="1004" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1004" s="21" t="s">
-        <v>1034</v>
-      </c>
-      <c r="B1004" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1004" s="26"/>
-      <c r="D1004" s="22"/>
-      <c r="E1004" s="26"/>
-      <c r="F1004" s="26"/>
-      <c r="G1004" s="22"/>
-      <c r="H1004" s="22"/>
-      <c r="I1004" s="23" t="s">
-        <v>1035</v>
-      </c>
-      <c r="J1004" s="23"/>
-      <c r="K1004" s="23"/>
-      <c r="L1004" s="22"/>
-      <c r="M1004" s="22"/>
-      <c r="N1004" s="22"/>
-    </row>
-    <row r="1005" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1005" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1005" s="26"/>
-      <c r="D1005" s="22"/>
-      <c r="E1005" s="26"/>
-      <c r="F1005" s="26"/>
-      <c r="G1005" s="22"/>
-      <c r="H1005" s="22"/>
-      <c r="I1005" s="23" t="s">
-        <v>1036</v>
-      </c>
-      <c r="J1005" s="23"/>
-      <c r="K1005" s="23"/>
-      <c r="L1005" s="22"/>
-      <c r="M1005" s="22"/>
-      <c r="N1005" s="22"/>
-    </row>
     <row r="1006" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1006" s="21" t="s">
+        <v>1037</v>
+      </c>
       <c r="B1006" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1006" s="26"/>
+      <c r="C1006" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1006" s="22"/>
       <c r="E1006" s="26"/>
       <c r="F1006" s="26"/>
       <c r="G1006" s="22"/>
       <c r="H1006" s="22"/>
       <c r="I1006" s="23" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="J1006" s="23"/>
       <c r="K1006" s="23"/>
@@ -26024,14 +26111,16 @@
       <c r="B1007" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1007" s="26"/>
+      <c r="C1007" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1007" s="22"/>
       <c r="E1007" s="26"/>
       <c r="F1007" s="26"/>
       <c r="G1007" s="22"/>
       <c r="H1007" s="22"/>
       <c r="I1007" s="23" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="J1007" s="23"/>
       <c r="K1007" s="23"/>
@@ -26043,14 +26132,16 @@
       <c r="B1008" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1008" s="26"/>
+      <c r="C1008" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1008" s="22"/>
       <c r="E1008" s="26"/>
       <c r="F1008" s="26"/>
       <c r="G1008" s="22"/>
       <c r="H1008" s="22"/>
       <c r="I1008" s="23" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="J1008" s="23"/>
       <c r="K1008" s="23"/>
@@ -26062,14 +26153,16 @@
       <c r="B1009" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1009" s="26"/>
+      <c r="C1009" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1009" s="22"/>
       <c r="E1009" s="26"/>
       <c r="F1009" s="26"/>
       <c r="G1009" s="22"/>
       <c r="H1009" s="22"/>
       <c r="I1009" s="23" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="J1009" s="23"/>
       <c r="K1009" s="23"/>
@@ -26081,14 +26174,16 @@
       <c r="B1010" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1010" s="26"/>
+      <c r="C1010" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1010" s="22"/>
       <c r="E1010" s="26"/>
       <c r="F1010" s="26"/>
       <c r="G1010" s="22"/>
       <c r="H1010" s="22"/>
       <c r="I1010" s="23" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="J1010" s="23"/>
       <c r="K1010" s="23"/>
@@ -26100,14 +26195,16 @@
       <c r="B1011" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1011" s="26"/>
+      <c r="C1011" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1011" s="22"/>
       <c r="E1011" s="26"/>
       <c r="F1011" s="26"/>
       <c r="G1011" s="22"/>
       <c r="H1011" s="22"/>
       <c r="I1011" s="23" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="J1011" s="23"/>
       <c r="K1011" s="23"/>
@@ -26119,14 +26216,16 @@
       <c r="B1012" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1012" s="26"/>
+      <c r="C1012" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1012" s="22"/>
       <c r="E1012" s="26"/>
       <c r="F1012" s="26"/>
       <c r="G1012" s="22"/>
       <c r="H1012" s="22"/>
       <c r="I1012" s="23" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="J1012" s="23"/>
       <c r="K1012" s="23"/>
@@ -26134,124 +26233,124 @@
       <c r="M1012" s="22"/>
       <c r="N1012" s="22"/>
     </row>
-    <row r="1013" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1013" s="22"/>
-      <c r="C1013" s="22"/>
+    <row r="1013" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1013" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1013" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1013" s="22"/>
-      <c r="E1013" s="22"/>
-      <c r="F1013" s="22"/>
+      <c r="E1013" s="26"/>
+      <c r="F1013" s="26"/>
       <c r="G1013" s="22"/>
       <c r="H1013" s="22"/>
-      <c r="I1013" s="23"/>
+      <c r="I1013" s="23" t="s">
+        <v>1045</v>
+      </c>
       <c r="J1013" s="23"/>
       <c r="K1013" s="23"/>
       <c r="L1013" s="22"/>
       <c r="M1013" s="22"/>
       <c r="N1013" s="22"/>
     </row>
-    <row r="1014" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1014" s="47"/>
-      <c r="C1014" s="1"/>
-      <c r="D1014" s="1"/>
-      <c r="E1014" s="1"/>
-      <c r="F1014" s="1"/>
-      <c r="G1014" s="1"/>
-      <c r="H1014" s="1"/>
-      <c r="I1014" s="1"/>
-      <c r="J1014" s="1"/>
-      <c r="K1014" s="1"/>
-      <c r="L1014" s="1"/>
-      <c r="M1014" s="1"/>
-      <c r="N1014" s="1"/>
-    </row>
-    <row r="1015" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1015" s="19"/>
-      <c r="B1015" s="11" t="s">
+    <row r="1014" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1014" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1014" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1014" s="22"/>
+      <c r="E1014" s="26"/>
+      <c r="F1014" s="26"/>
+      <c r="G1014" s="22"/>
+      <c r="H1014" s="22"/>
+      <c r="I1014" s="23" t="s">
+        <v>1046</v>
+      </c>
+      <c r="J1014" s="23"/>
+      <c r="K1014" s="23"/>
+      <c r="L1014" s="22"/>
+      <c r="M1014" s="22"/>
+      <c r="N1014" s="22"/>
+    </row>
+    <row r="1015" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1015" s="22"/>
+      <c r="C1015" s="22"/>
+      <c r="D1015" s="22"/>
+      <c r="E1015" s="22"/>
+      <c r="F1015" s="22"/>
+      <c r="G1015" s="22"/>
+      <c r="H1015" s="22"/>
+      <c r="I1015" s="23"/>
+      <c r="J1015" s="23"/>
+      <c r="K1015" s="23"/>
+      <c r="L1015" s="22"/>
+      <c r="M1015" s="22"/>
+      <c r="N1015" s="22"/>
+    </row>
+    <row r="1016" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1016" s="47"/>
+      <c r="C1016" s="1"/>
+      <c r="D1016" s="1"/>
+      <c r="E1016" s="1"/>
+      <c r="F1016" s="1"/>
+      <c r="G1016" s="1"/>
+      <c r="H1016" s="1"/>
+      <c r="I1016" s="1"/>
+      <c r="J1016" s="1"/>
+      <c r="K1016" s="1"/>
+      <c r="L1016" s="1"/>
+      <c r="M1016" s="1"/>
+      <c r="N1016" s="1"/>
+    </row>
+    <row r="1017" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1017" s="19"/>
+      <c r="B1017" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1015" s="11" t="s">
+      <c r="C1017" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1015" s="11" t="s">
+      <c r="D1017" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1015" s="11" t="s">
+      <c r="E1017" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1015" s="11" t="s">
+      <c r="F1017" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G1015" s="11" t="s">
+      <c r="G1017" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1015" s="11" t="s">
+      <c r="H1017" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1015" s="20" t="s">
+      <c r="I1017" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1015" s="20" t="s">
+      <c r="J1017" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1015" s="20" t="s">
+      <c r="K1017" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L1015" s="11" t="s">
+      <c r="L1017" s="11" t="s">
         <v>702</v>
       </c>
-      <c r="M1015" s="11" t="s">
+      <c r="M1017" s="11" t="s">
         <v>703</v>
       </c>
-      <c r="N1015" s="11" t="s">
+      <c r="N1017" s="11" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="1016" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1016" s="21" t="s">
-        <v>1044</v>
-      </c>
-      <c r="B1016" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1016" s="26"/>
-      <c r="D1016" s="22"/>
-      <c r="E1016" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1016" s="26"/>
-      <c r="G1016" s="22"/>
-      <c r="H1016" s="22"/>
-      <c r="I1016" s="23" t="s">
-        <v>1045</v>
-      </c>
-      <c r="J1016" s="23"/>
-      <c r="K1016" s="23"/>
-      <c r="L1016" s="22"/>
-      <c r="M1016" s="22"/>
-      <c r="N1016" s="22"/>
-    </row>
-    <row r="1017" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1017" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1017" s="26"/>
-      <c r="D1017" s="22"/>
-      <c r="E1017" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1017" s="26"/>
-      <c r="G1017" s="22"/>
-      <c r="H1017" s="22"/>
-      <c r="I1017" s="23" t="s">
-        <v>1046</v>
-      </c>
-      <c r="J1017" s="23"/>
-      <c r="K1017" s="23"/>
-      <c r="L1017" s="22"/>
-      <c r="M1017" s="22"/>
-      <c r="N1017" s="22"/>
-    </row>
     <row r="1018" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1018" s="21" t="s">
+        <v>1047</v>
+      </c>
       <c r="B1018" s="22" t="s">
         <v>27</v>
       </c>
@@ -26264,7 +26363,7 @@
       <c r="G1018" s="22"/>
       <c r="H1018" s="22"/>
       <c r="I1018" s="23" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="J1018" s="23"/>
       <c r="K1018" s="23"/>
@@ -26285,7 +26384,7 @@
       <c r="G1019" s="22"/>
       <c r="H1019" s="22"/>
       <c r="I1019" s="23" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="J1019" s="23"/>
       <c r="K1019" s="23"/>
@@ -26294,33 +26393,35 @@
       <c r="N1019" s="22"/>
     </row>
     <row r="1020" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1020" s="28" t="s">
-        <v>619</v>
+      <c r="B1020" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="C1020" s="26"/>
       <c r="D1020" s="22"/>
-      <c r="E1020" s="22"/>
+      <c r="E1020" s="22" t="s">
+        <v>65</v>
+      </c>
       <c r="F1020" s="26"/>
       <c r="G1020" s="22"/>
       <c r="H1020" s="22"/>
       <c r="I1020" s="23" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="J1020" s="23"/>
-      <c r="K1020" s="23" t="s">
-        <v>1050</v>
-      </c>
+      <c r="K1020" s="23"/>
       <c r="L1020" s="22"/>
       <c r="M1020" s="22"/>
       <c r="N1020" s="22"/>
     </row>
     <row r="1021" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1021" s="28" t="s">
-        <v>619</v>
+      <c r="B1021" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="C1021" s="26"/>
       <c r="D1021" s="22"/>
-      <c r="E1021" s="22"/>
+      <c r="E1021" s="22" t="s">
+        <v>65</v>
+      </c>
       <c r="F1021" s="26"/>
       <c r="G1021" s="22"/>
       <c r="H1021" s="22"/>
@@ -26328,22 +26429,18 @@
         <v>1051</v>
       </c>
       <c r="J1021" s="23"/>
-      <c r="K1021" s="23" t="s">
-        <v>1050</v>
-      </c>
+      <c r="K1021" s="23"/>
       <c r="L1021" s="22"/>
       <c r="M1021" s="22"/>
       <c r="N1021" s="22"/>
     </row>
     <row r="1022" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1022" s="22" t="s">
-        <v>27</v>
+      <c r="B1022" s="28" t="s">
+        <v>619</v>
       </c>
       <c r="C1022" s="26"/>
       <c r="D1022" s="22"/>
-      <c r="E1022" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1022" s="22"/>
       <c r="F1022" s="26"/>
       <c r="G1022" s="22"/>
       <c r="H1022" s="22"/>
@@ -26351,28 +26448,30 @@
         <v>1052</v>
       </c>
       <c r="J1022" s="23"/>
-      <c r="K1022" s="23"/>
+      <c r="K1022" s="23" t="s">
+        <v>1053</v>
+      </c>
       <c r="L1022" s="22"/>
       <c r="M1022" s="22"/>
       <c r="N1022" s="22"/>
     </row>
     <row r="1023" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1023" s="22" t="s">
-        <v>27</v>
+      <c r="B1023" s="28" t="s">
+        <v>619</v>
       </c>
       <c r="C1023" s="26"/>
       <c r="D1023" s="22"/>
-      <c r="E1023" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1023" s="22"/>
       <c r="F1023" s="26"/>
       <c r="G1023" s="22"/>
       <c r="H1023" s="22"/>
       <c r="I1023" s="23" t="s">
+        <v>1054</v>
+      </c>
+      <c r="J1023" s="23"/>
+      <c r="K1023" s="23" t="s">
         <v>1053</v>
       </c>
-      <c r="J1023" s="23"/>
-      <c r="K1023" s="23"/>
       <c r="L1023" s="22"/>
       <c r="M1023" s="22"/>
       <c r="N1023" s="22"/>
@@ -26390,7 +26489,7 @@
       <c r="G1024" s="22"/>
       <c r="H1024" s="22"/>
       <c r="I1024" s="23" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="J1024" s="23"/>
       <c r="K1024" s="23"/>
@@ -26405,13 +26504,13 @@
       <c r="C1025" s="26"/>
       <c r="D1025" s="22"/>
       <c r="E1025" s="22" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="F1025" s="26"/>
       <c r="G1025" s="22"/>
       <c r="H1025" s="22"/>
       <c r="I1025" s="23" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="J1025" s="23"/>
       <c r="K1025" s="23"/>
@@ -26432,7 +26531,7 @@
       <c r="G1026" s="22"/>
       <c r="H1026" s="22"/>
       <c r="I1026" s="23" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="J1026" s="23"/>
       <c r="K1026" s="23"/>
@@ -26447,13 +26546,13 @@
       <c r="C1027" s="26"/>
       <c r="D1027" s="22"/>
       <c r="E1027" s="22" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F1027" s="26"/>
       <c r="G1027" s="22"/>
       <c r="H1027" s="22"/>
       <c r="I1027" s="23" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="J1027" s="23"/>
       <c r="K1027" s="23"/>
@@ -26461,132 +26560,144 @@
       <c r="M1027" s="22"/>
       <c r="N1027" s="22"/>
     </row>
-    <row r="1028" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1028" s="22"/>
-      <c r="C1028" s="22"/>
+    <row r="1028" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1028" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1028" s="26"/>
       <c r="D1028" s="22"/>
-      <c r="E1028" s="22"/>
-      <c r="F1028" s="22"/>
+      <c r="E1028" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1028" s="26"/>
       <c r="G1028" s="22"/>
       <c r="H1028" s="22"/>
-      <c r="I1028" s="23"/>
+      <c r="I1028" s="23" t="s">
+        <v>1059</v>
+      </c>
       <c r="J1028" s="23"/>
       <c r="K1028" s="23"/>
       <c r="L1028" s="22"/>
       <c r="M1028" s="22"/>
       <c r="N1028" s="22"/>
     </row>
-    <row r="1029" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1029" s="47"/>
-      <c r="C1029" s="1"/>
-      <c r="D1029" s="1"/>
-      <c r="E1029" s="1"/>
-      <c r="F1029" s="1"/>
-      <c r="G1029" s="1"/>
-      <c r="H1029" s="1"/>
-      <c r="I1029" s="1"/>
-      <c r="J1029" s="1"/>
-      <c r="K1029" s="1"/>
-      <c r="L1029" s="1"/>
-      <c r="M1029" s="1"/>
-      <c r="N1029" s="1"/>
-    </row>
-    <row r="1030" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1030" s="19"/>
-      <c r="B1030" s="11" t="s">
+    <row r="1029" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1029" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1029" s="26"/>
+      <c r="D1029" s="22"/>
+      <c r="E1029" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1029" s="26"/>
+      <c r="G1029" s="22"/>
+      <c r="H1029" s="22"/>
+      <c r="I1029" s="23" t="s">
+        <v>1060</v>
+      </c>
+      <c r="J1029" s="23"/>
+      <c r="K1029" s="23"/>
+      <c r="L1029" s="22"/>
+      <c r="M1029" s="22"/>
+      <c r="N1029" s="22"/>
+    </row>
+    <row r="1030" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1030" s="22"/>
+      <c r="C1030" s="22"/>
+      <c r="D1030" s="22"/>
+      <c r="E1030" s="22"/>
+      <c r="F1030" s="22"/>
+      <c r="G1030" s="22"/>
+      <c r="H1030" s="22"/>
+      <c r="I1030" s="23"/>
+      <c r="J1030" s="23"/>
+      <c r="K1030" s="23"/>
+      <c r="L1030" s="22"/>
+      <c r="M1030" s="22"/>
+      <c r="N1030" s="22"/>
+    </row>
+    <row r="1031" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1031" s="47"/>
+      <c r="C1031" s="1"/>
+      <c r="D1031" s="1"/>
+      <c r="E1031" s="1"/>
+      <c r="F1031" s="1"/>
+      <c r="G1031" s="1"/>
+      <c r="H1031" s="1"/>
+      <c r="I1031" s="1"/>
+      <c r="J1031" s="1"/>
+      <c r="K1031" s="1"/>
+      <c r="L1031" s="1"/>
+      <c r="M1031" s="1"/>
+      <c r="N1031" s="1"/>
+    </row>
+    <row r="1032" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1032" s="19"/>
+      <c r="B1032" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1030" s="11" t="s">
+      <c r="C1032" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1030" s="11" t="s">
+      <c r="D1032" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1030" s="11" t="s">
+      <c r="E1032" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1030" s="11" t="s">
+      <c r="F1032" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G1030" s="11" t="s">
+      <c r="G1032" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1030" s="11" t="s">
+      <c r="H1032" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1030" s="20" t="s">
+      <c r="I1032" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1030" s="20" t="s">
+      <c r="J1032" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1030" s="20" t="s">
+      <c r="K1032" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L1030" s="11" t="s">
+      <c r="L1032" s="11" t="s">
         <v>702</v>
       </c>
-      <c r="M1030" s="11" t="s">
+      <c r="M1032" s="11" t="s">
         <v>703</v>
       </c>
-      <c r="N1030" s="11" t="s">
+      <c r="N1032" s="11" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="1031" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1031" s="21" t="s">
-        <v>1058</v>
-      </c>
-      <c r="B1031" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1031" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1031" s="22"/>
-      <c r="E1031" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1031" s="26"/>
-      <c r="G1031" s="22"/>
-      <c r="H1031" s="22"/>
-      <c r="I1031" s="23" t="s">
-        <v>1059</v>
-      </c>
-      <c r="J1031" s="23"/>
-      <c r="K1031" s="23" t="s">
-        <v>1060</v>
-      </c>
-      <c r="L1031" s="22"/>
-      <c r="M1031" s="22"/>
-      <c r="N1031" s="22"/>
-    </row>
-    <row r="1032" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1032" s="22"/>
-      <c r="C1032" s="22"/>
-      <c r="D1032" s="22"/>
-      <c r="E1032" s="22"/>
-      <c r="F1032" s="22"/>
-      <c r="G1032" s="22"/>
-      <c r="H1032" s="22"/>
-      <c r="I1032" s="23"/>
-      <c r="J1032" s="23"/>
-      <c r="K1032" s="23"/>
-      <c r="L1032" s="22"/>
-      <c r="M1032" s="22"/>
-      <c r="N1032" s="22"/>
-    </row>
-    <row r="1033" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1033" s="22"/>
-      <c r="C1033" s="22"/>
+    <row r="1033" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1033" s="21" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B1033" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1033" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1033" s="22"/>
-      <c r="E1033" s="22"/>
-      <c r="F1033" s="22"/>
+      <c r="E1033" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1033" s="26"/>
       <c r="G1033" s="22"/>
       <c r="H1033" s="22"/>
-      <c r="I1033" s="23"/>
+      <c r="I1033" s="23" t="s">
+        <v>1062</v>
+      </c>
       <c r="J1033" s="23"/>
-      <c r="K1033" s="23"/>
+      <c r="K1033" s="23" t="s">
+        <v>1063</v>
+      </c>
       <c r="L1033" s="22"/>
       <c r="M1033" s="22"/>
       <c r="N1033" s="22"/>
@@ -26637,141 +26748,123 @@
       <c r="N1036" s="22"/>
     </row>
     <row r="1037" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1037" s="1"/>
-      <c r="C1037" s="1"/>
-      <c r="D1037" s="1"/>
-      <c r="E1037" s="1"/>
-      <c r="F1037" s="1"/>
-      <c r="G1037" s="1"/>
-      <c r="H1037" s="1"/>
-      <c r="I1037" s="1"/>
-      <c r="J1037" s="1"/>
-      <c r="K1037" s="1"/>
-      <c r="L1037" s="1"/>
-      <c r="M1037" s="1"/>
-      <c r="N1037" s="1"/>
-      <c r="O1037" s="1"/>
-      <c r="P1037" s="1"/>
-    </row>
-    <row r="1038" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1038" s="19"/>
-      <c r="B1038" s="11" t="s">
+      <c r="B1037" s="22"/>
+      <c r="C1037" s="22"/>
+      <c r="D1037" s="22"/>
+      <c r="E1037" s="22"/>
+      <c r="F1037" s="22"/>
+      <c r="G1037" s="22"/>
+      <c r="H1037" s="22"/>
+      <c r="I1037" s="23"/>
+      <c r="J1037" s="23"/>
+      <c r="K1037" s="23"/>
+      <c r="L1037" s="22"/>
+      <c r="M1037" s="22"/>
+      <c r="N1037" s="22"/>
+    </row>
+    <row r="1038" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1038" s="22"/>
+      <c r="C1038" s="22"/>
+      <c r="D1038" s="22"/>
+      <c r="E1038" s="22"/>
+      <c r="F1038" s="22"/>
+      <c r="G1038" s="22"/>
+      <c r="H1038" s="22"/>
+      <c r="I1038" s="23"/>
+      <c r="J1038" s="23"/>
+      <c r="K1038" s="23"/>
+      <c r="L1038" s="22"/>
+      <c r="M1038" s="22"/>
+      <c r="N1038" s="22"/>
+    </row>
+    <row r="1039" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1039" s="1"/>
+      <c r="C1039" s="1"/>
+      <c r="D1039" s="1"/>
+      <c r="E1039" s="1"/>
+      <c r="F1039" s="1"/>
+      <c r="G1039" s="1"/>
+      <c r="H1039" s="1"/>
+      <c r="I1039" s="1"/>
+      <c r="J1039" s="1"/>
+      <c r="K1039" s="1"/>
+      <c r="L1039" s="1"/>
+      <c r="M1039" s="1"/>
+      <c r="N1039" s="1"/>
+      <c r="O1039" s="1"/>
+      <c r="P1039" s="1"/>
+    </row>
+    <row r="1040" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1040" s="19"/>
+      <c r="B1040" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1038" s="11" t="s">
+      <c r="C1040" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1038" s="11" t="s">
+      <c r="D1040" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1038" s="11" t="s">
+      <c r="E1040" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1038" s="11" t="s">
+      <c r="F1040" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G1038" s="11" t="s">
+      <c r="G1040" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1038" s="11" t="s">
+      <c r="H1040" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1038" s="20" t="s">
+      <c r="I1040" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1038" s="20" t="s">
+      <c r="J1040" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1038" s="20" t="s">
+      <c r="K1040" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L1038" s="11" t="s">
+      <c r="L1040" s="11" t="s">
         <v>702</v>
       </c>
-      <c r="M1038" s="11" t="s">
+      <c r="M1040" s="11" t="s">
         <v>703</v>
       </c>
-      <c r="N1038" s="11" t="s">
+      <c r="N1040" s="11" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="1039" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1039" s="21" t="s">
-        <v>1061</v>
-      </c>
-      <c r="B1039" s="28" t="s">
+    <row r="1041" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1041" s="21" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B1041" s="28" t="s">
         <v>619</v>
       </c>
-      <c r="C1039" s="26"/>
-      <c r="D1039" s="22"/>
-      <c r="E1039" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1039" s="26"/>
-      <c r="G1039" s="22"/>
-      <c r="H1039" s="22"/>
-      <c r="I1039" s="23" t="s">
-        <v>1062</v>
-      </c>
-      <c r="J1039" s="23"/>
-      <c r="K1039" s="23" t="s">
-        <v>621</v>
-      </c>
-      <c r="L1039" s="22"/>
-      <c r="M1039" s="22"/>
-      <c r="N1039" s="22"/>
-    </row>
-    <row r="1040" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1040" s="28" t="s">
-        <v>619</v>
-      </c>
-      <c r="C1040" s="26"/>
-      <c r="D1040" s="22"/>
-      <c r="E1040" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1040" s="26"/>
-      <c r="G1040" s="22"/>
-      <c r="H1040" s="22"/>
-      <c r="I1040" s="23" t="s">
-        <v>1063</v>
-      </c>
-      <c r="J1040" s="23"/>
-      <c r="K1040" s="23" t="s">
-        <v>1064</v>
-      </c>
-      <c r="L1040" s="22"/>
-      <c r="M1040" s="22"/>
-      <c r="N1040" s="22"/>
-    </row>
-    <row r="1041" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1041" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1041" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="C1041" s="26"/>
       <c r="D1041" s="22"/>
       <c r="E1041" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F1041" s="26"/>
-      <c r="G1041" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="G1041" s="22"/>
       <c r="H1041" s="22"/>
       <c r="I1041" s="23" t="s">
         <v>1065</v>
       </c>
       <c r="J1041" s="23"/>
-      <c r="K1041" s="23"/>
+      <c r="K1041" s="23" t="s">
+        <v>621</v>
+      </c>
       <c r="L1041" s="22"/>
       <c r="M1041" s="22"/>
       <c r="N1041" s="22"/>
     </row>
     <row r="1042" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1042" s="22" t="s">
-        <v>27</v>
+      <c r="B1042" s="28" t="s">
+        <v>619</v>
       </c>
       <c r="C1042" s="26"/>
       <c r="D1042" s="22"/>
@@ -26779,15 +26872,15 @@
         <v>27</v>
       </c>
       <c r="F1042" s="26"/>
-      <c r="G1042" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="G1042" s="22"/>
       <c r="H1042" s="22"/>
       <c r="I1042" s="23" t="s">
         <v>1066</v>
       </c>
       <c r="J1042" s="23"/>
-      <c r="K1042" s="23"/>
+      <c r="K1042" s="23" t="s">
+        <v>1067</v>
+      </c>
       <c r="L1042" s="22"/>
       <c r="M1042" s="22"/>
       <c r="N1042" s="22"/>
@@ -26800,12 +26893,16 @@
         <v>27</v>
       </c>
       <c r="D1043" s="22"/>
-      <c r="E1043" s="26"/>
+      <c r="E1043" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1043" s="26"/>
-      <c r="G1043" s="22"/>
+      <c r="G1043" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="H1043" s="22"/>
       <c r="I1043" s="23" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="J1043" s="23"/>
       <c r="K1043" s="23"/>
@@ -26823,10 +26920,12 @@
         <v>27</v>
       </c>
       <c r="F1044" s="26"/>
-      <c r="G1044" s="22"/>
+      <c r="G1044" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="H1044" s="22"/>
       <c r="I1044" s="23" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="J1044" s="23"/>
       <c r="K1044" s="23"/>
@@ -26834,62 +26933,80 @@
       <c r="M1044" s="22"/>
       <c r="N1044" s="22"/>
     </row>
-    <row r="1045" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1045" s="22"/>
-      <c r="C1045" s="22"/>
+    <row r="1045" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1045" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1045" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1045" s="22"/>
-      <c r="E1045" s="22"/>
-      <c r="F1045" s="22"/>
+      <c r="E1045" s="26"/>
+      <c r="F1045" s="26"/>
       <c r="G1045" s="22"/>
       <c r="H1045" s="22"/>
-      <c r="I1045" s="23"/>
+      <c r="I1045" s="23" t="s">
+        <v>1070</v>
+      </c>
       <c r="J1045" s="23"/>
       <c r="K1045" s="23"/>
       <c r="L1045" s="22"/>
       <c r="M1045" s="22"/>
       <c r="N1045" s="22"/>
     </row>
-    <row r="1046" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1046" s="47"/>
-      <c r="C1046" s="1"/>
-      <c r="D1046" s="1"/>
-      <c r="E1046" s="1"/>
-      <c r="F1046" s="1"/>
-      <c r="G1046" s="1"/>
-      <c r="H1046" s="1"/>
-      <c r="I1046" s="1"/>
-      <c r="J1046" s="1"/>
-      <c r="K1046" s="1"/>
-      <c r="L1046" s="1"/>
-      <c r="M1046" s="1"/>
-      <c r="N1046" s="1"/>
+    <row r="1046" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1046" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1046" s="26"/>
+      <c r="D1046" s="22"/>
+      <c r="E1046" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1046" s="26"/>
+      <c r="G1046" s="22"/>
+      <c r="H1046" s="22"/>
+      <c r="I1046" s="23" t="s">
+        <v>1071</v>
+      </c>
+      <c r="J1046" s="23"/>
+      <c r="K1046" s="23"/>
+      <c r="L1046" s="22"/>
+      <c r="M1046" s="22"/>
+      <c r="N1046" s="22"/>
     </row>
     <row r="1047" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1047" s="9"/>
+      <c r="B1047" s="22"/>
+      <c r="C1047" s="22"/>
+      <c r="D1047" s="22"/>
+      <c r="E1047" s="22"/>
+      <c r="F1047" s="22"/>
+      <c r="G1047" s="22"/>
+      <c r="H1047" s="22"/>
+      <c r="I1047" s="23"/>
+      <c r="J1047" s="23"/>
+      <c r="K1047" s="23"/>
+      <c r="L1047" s="22"/>
+      <c r="M1047" s="22"/>
+      <c r="N1047" s="22"/>
     </row>
     <row r="1048" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1048" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1048" s="17"/>
-      <c r="C1048" s="18"/>
-      <c r="D1048" s="18"/>
-      <c r="E1048" s="18"/>
-      <c r="F1048" s="18"/>
-      <c r="G1048" s="18"/>
-      <c r="H1048" s="18"/>
+      <c r="B1048" s="47"/>
+      <c r="C1048" s="1"/>
+      <c r="D1048" s="1"/>
+      <c r="E1048" s="1"/>
+      <c r="F1048" s="1"/>
+      <c r="G1048" s="1"/>
+      <c r="H1048" s="1"/>
+      <c r="I1048" s="1"/>
+      <c r="J1048" s="1"/>
+      <c r="K1048" s="1"/>
+      <c r="L1048" s="1"/>
+      <c r="M1048" s="1"/>
+      <c r="N1048" s="1"/>
     </row>
     <row r="1049" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1049" s="16" t="s">
-        <v>1069</v>
-      </c>
-      <c r="B1049" s="17"/>
-      <c r="C1049" s="18"/>
-      <c r="D1049" s="18"/>
-      <c r="E1049" s="18"/>
-      <c r="F1049" s="18"/>
-      <c r="G1049" s="18"/>
-      <c r="H1049" s="18"/>
+      <c r="A1049" s="9"/>
     </row>
     <row r="1050" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1050" s="16" t="s">
@@ -26903,91 +27020,69 @@
       <c r="G1050" s="18"/>
       <c r="H1050" s="18"/>
     </row>
-    <row r="1051" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1051" s="9"/>
-      <c r="B1051" s="11" t="s">
+    <row r="1051" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1051" s="16" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1051" s="17"/>
+      <c r="C1051" s="18"/>
+      <c r="D1051" s="18"/>
+      <c r="E1051" s="18"/>
+      <c r="F1051" s="18"/>
+      <c r="G1051" s="18"/>
+      <c r="H1051" s="18"/>
+    </row>
+    <row r="1052" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1052" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1052" s="17"/>
+      <c r="C1052" s="18"/>
+      <c r="D1052" s="18"/>
+      <c r="E1052" s="18"/>
+      <c r="F1052" s="18"/>
+      <c r="G1052" s="18"/>
+      <c r="H1052" s="18"/>
+    </row>
+    <row r="1053" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1053" s="9"/>
+      <c r="B1053" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1051" s="11" t="s">
+      <c r="C1053" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1051" s="11" t="s">
+      <c r="D1053" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1051" s="11" t="s">
+      <c r="E1053" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1051" s="11" t="s">
+      <c r="F1053" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G1051" s="11" t="s">
+      <c r="G1053" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1051" s="11" t="s">
+      <c r="H1053" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1051" s="20" t="s">
+      <c r="I1053" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1051" s="20" t="s">
+      <c r="J1053" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1051" s="20" t="s">
+      <c r="K1053" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="1052" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1052" s="21" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B1052" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1052" s="26"/>
-      <c r="D1052" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1052" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1052" s="22" t="s">
-        <v>648</v>
-      </c>
-      <c r="G1052" s="22"/>
-      <c r="H1052" s="22"/>
-      <c r="I1052" s="23" t="s">
-        <v>1072</v>
-      </c>
-      <c r="J1052" s="23"/>
-      <c r="K1052" s="23"/>
-    </row>
-    <row r="1053" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1053" s="21"/>
-      <c r="B1053" s="28" t="s">
+    <row r="1054" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1054" s="21" t="s">
         <v>1073</v>
       </c>
-      <c r="C1053" s="26"/>
-      <c r="D1053" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1053" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1053" s="22" t="s">
-        <v>648</v>
-      </c>
-      <c r="G1053" s="22"/>
-      <c r="H1053" s="22"/>
-      <c r="I1053" s="23" t="s">
+      <c r="B1054" s="22" t="s">
         <v>1074</v>
-      </c>
-      <c r="J1053" s="23"/>
-      <c r="K1053" s="23"/>
-    </row>
-    <row r="1054" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1054" s="21"/>
-      <c r="B1054" s="22" t="s">
-        <v>1071</v>
       </c>
       <c r="C1054" s="26"/>
       <c r="D1054" s="22" t="s">
@@ -27009,12 +27104,10 @@
     </row>
     <row r="1055" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1055" s="21"/>
-      <c r="B1055" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1055" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="B1055" s="28" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C1055" s="26"/>
       <c r="D1055" s="22" t="s">
         <v>27</v>
       </c>
@@ -27027,19 +27120,17 @@
       <c r="G1055" s="22"/>
       <c r="H1055" s="22"/>
       <c r="I1055" s="23" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="J1055" s="23"/>
       <c r="K1055" s="23"/>
     </row>
     <row r="1056" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1056" s="9"/>
+      <c r="A1056" s="21"/>
       <c r="B1056" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1056" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1056" s="26"/>
       <c r="D1056" s="22" t="s">
         <v>27</v>
       </c>
@@ -27052,17 +27143,19 @@
       <c r="G1056" s="22"/>
       <c r="H1056" s="22"/>
       <c r="I1056" s="23" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="J1056" s="23"/>
       <c r="K1056" s="23"/>
     </row>
     <row r="1057" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1057" s="9"/>
+      <c r="A1057" s="21"/>
       <c r="B1057" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1057" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1057" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1057" s="22" t="s">
         <v>27</v>
       </c>
@@ -27074,8 +27167,8 @@
       </c>
       <c r="G1057" s="22"/>
       <c r="H1057" s="22"/>
-      <c r="I1057" s="46" t="s">
-        <v>1078</v>
+      <c r="I1057" s="23" t="s">
+        <v>1079</v>
       </c>
       <c r="J1057" s="23"/>
       <c r="K1057" s="23"/>
@@ -27083,7 +27176,7 @@
     <row r="1058" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1058" s="9"/>
       <c r="B1058" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1058" s="22" t="s">
         <v>27</v>
@@ -27100,7 +27193,7 @@
       <c r="G1058" s="22"/>
       <c r="H1058" s="22"/>
       <c r="I1058" s="23" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="J1058" s="23"/>
       <c r="K1058" s="23"/>
@@ -27108,20 +27201,22 @@
     <row r="1059" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1059" s="9"/>
       <c r="B1059" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1059" s="26"/>
       <c r="D1059" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1059" s="26"/>
+      <c r="E1059" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1059" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1059" s="22"/>
       <c r="H1059" s="22"/>
-      <c r="I1059" s="23" t="s">
-        <v>1080</v>
+      <c r="I1059" s="46" t="s">
+        <v>1081</v>
       </c>
       <c r="J1059" s="23"/>
       <c r="K1059" s="23"/>
@@ -27129,20 +27224,24 @@
     <row r="1060" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1060" s="9"/>
       <c r="B1060" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1060" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1060" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1060" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1060" s="26"/>
+      <c r="E1060" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1060" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1060" s="22"/>
       <c r="H1060" s="22"/>
       <c r="I1060" s="23" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="J1060" s="23"/>
       <c r="K1060" s="23"/>
@@ -27150,7 +27249,7 @@
     <row r="1061" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1061" s="9"/>
       <c r="B1061" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1061" s="26"/>
       <c r="D1061" s="22" t="s">
@@ -27163,7 +27262,7 @@
       <c r="G1061" s="22"/>
       <c r="H1061" s="22"/>
       <c r="I1061" s="23" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="J1061" s="23"/>
       <c r="K1061" s="23"/>
@@ -27171,7 +27270,7 @@
     <row r="1062" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1062" s="9"/>
       <c r="B1062" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1062" s="26"/>
       <c r="D1062" s="22" t="s">
@@ -27184,7 +27283,7 @@
       <c r="G1062" s="22"/>
       <c r="H1062" s="22"/>
       <c r="I1062" s="23" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="J1062" s="23"/>
       <c r="K1062" s="23"/>
@@ -27192,7 +27291,7 @@
     <row r="1063" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1063" s="9"/>
       <c r="B1063" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1063" s="26"/>
       <c r="D1063" s="22" t="s">
@@ -27205,7 +27304,7 @@
       <c r="G1063" s="22"/>
       <c r="H1063" s="22"/>
       <c r="I1063" s="23" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="J1063" s="23"/>
       <c r="K1063" s="23"/>
@@ -27213,22 +27312,20 @@
     <row r="1064" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1064" s="9"/>
       <c r="B1064" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1064" s="26"/>
       <c r="D1064" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1064" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1064" s="26"/>
       <c r="F1064" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1064" s="22"/>
       <c r="H1064" s="22"/>
       <c r="I1064" s="23" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="J1064" s="23"/>
       <c r="K1064" s="23"/>
@@ -27236,22 +27333,20 @@
     <row r="1065" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1065" s="9"/>
       <c r="B1065" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1065" s="26"/>
       <c r="D1065" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1065" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1065" s="26"/>
       <c r="F1065" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1065" s="22"/>
       <c r="H1065" s="22"/>
       <c r="I1065" s="23" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="J1065" s="23"/>
       <c r="K1065" s="23"/>
@@ -27259,7 +27354,7 @@
     <row r="1066" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1066" s="9"/>
       <c r="B1066" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1066" s="26"/>
       <c r="D1066" s="22" t="s">
@@ -27274,7 +27369,7 @@
       <c r="G1066" s="22"/>
       <c r="H1066" s="22"/>
       <c r="I1066" s="23" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="J1066" s="23"/>
       <c r="K1066" s="23"/>
@@ -27282,7 +27377,7 @@
     <row r="1067" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1067" s="9"/>
       <c r="B1067" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1067" s="26"/>
       <c r="D1067" s="22" t="s">
@@ -27297,7 +27392,7 @@
       <c r="G1067" s="22"/>
       <c r="H1067" s="22"/>
       <c r="I1067" s="23" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="J1067" s="23"/>
       <c r="K1067" s="23"/>
@@ -27305,7 +27400,7 @@
     <row r="1068" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1068" s="9"/>
       <c r="B1068" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1068" s="26"/>
       <c r="D1068" s="22" t="s">
@@ -27320,7 +27415,7 @@
       <c r="G1068" s="22"/>
       <c r="H1068" s="22"/>
       <c r="I1068" s="23" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="J1068" s="23"/>
       <c r="K1068" s="23"/>
@@ -27328,7 +27423,7 @@
     <row r="1069" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1069" s="9"/>
       <c r="B1069" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1069" s="26"/>
       <c r="D1069" s="22" t="s">
@@ -27343,17 +27438,15 @@
       <c r="G1069" s="22"/>
       <c r="H1069" s="22"/>
       <c r="I1069" s="23" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="J1069" s="23"/>
-      <c r="K1069" s="23" t="s">
-        <v>274</v>
-      </c>
+      <c r="K1069" s="23"/>
     </row>
     <row r="1070" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1070" s="9"/>
       <c r="B1070" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1070" s="26"/>
       <c r="D1070" s="22" t="s">
@@ -27368,15 +27461,15 @@
       <c r="G1070" s="22"/>
       <c r="H1070" s="22"/>
       <c r="I1070" s="23" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="J1070" s="23"/>
       <c r="K1070" s="23"/>
     </row>
     <row r="1071" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1071" s="9"/>
-      <c r="B1071" s="28" t="s">
-        <v>1073</v>
+      <c r="B1071" s="22" t="s">
+        <v>1074</v>
       </c>
       <c r="C1071" s="26"/>
       <c r="D1071" s="22" t="s">
@@ -27391,19 +27484,19 @@
       <c r="G1071" s="22"/>
       <c r="H1071" s="22"/>
       <c r="I1071" s="23" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="J1071" s="23"/>
-      <c r="K1071" s="23"/>
+      <c r="K1071" s="23" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="1072" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1072" s="9"/>
       <c r="B1072" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1072" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1072" s="26"/>
       <c r="D1072" s="22" t="s">
         <v>27</v>
       </c>
@@ -27416,15 +27509,15 @@
       <c r="G1072" s="22"/>
       <c r="H1072" s="22"/>
       <c r="I1072" s="23" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="J1072" s="23"/>
       <c r="K1072" s="23"/>
     </row>
     <row r="1073" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1073" s="9"/>
-      <c r="B1073" s="22" t="s">
-        <v>1071</v>
+      <c r="B1073" s="28" t="s">
+        <v>1076</v>
       </c>
       <c r="C1073" s="26"/>
       <c r="D1073" s="22" t="s">
@@ -27439,7 +27532,7 @@
       <c r="G1073" s="22"/>
       <c r="H1073" s="22"/>
       <c r="I1073" s="23" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="J1073" s="23"/>
       <c r="K1073" s="23"/>
@@ -27447,9 +27540,11 @@
     <row r="1074" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1074" s="9"/>
       <c r="B1074" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1074" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1074" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1074" s="22" t="s">
         <v>27</v>
       </c>
@@ -27462,7 +27557,7 @@
       <c r="G1074" s="22"/>
       <c r="H1074" s="22"/>
       <c r="I1074" s="23" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="J1074" s="23"/>
       <c r="K1074" s="23"/>
@@ -27470,7 +27565,7 @@
     <row r="1075" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1075" s="9"/>
       <c r="B1075" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1075" s="26"/>
       <c r="D1075" s="22" t="s">
@@ -27485,7 +27580,7 @@
       <c r="G1075" s="22"/>
       <c r="H1075" s="22"/>
       <c r="I1075" s="23" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="J1075" s="23"/>
       <c r="K1075" s="23"/>
@@ -27493,7 +27588,7 @@
     <row r="1076" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1076" s="9"/>
       <c r="B1076" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1076" s="26"/>
       <c r="D1076" s="22" t="s">
@@ -27508,7 +27603,7 @@
       <c r="G1076" s="22"/>
       <c r="H1076" s="22"/>
       <c r="I1076" s="23" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="J1076" s="23"/>
       <c r="K1076" s="23"/>
@@ -27516,7 +27611,7 @@
     <row r="1077" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1077" s="9"/>
       <c r="B1077" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1077" s="26"/>
       <c r="D1077" s="22" t="s">
@@ -27531,7 +27626,7 @@
       <c r="G1077" s="22"/>
       <c r="H1077" s="22"/>
       <c r="I1077" s="23" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="J1077" s="23"/>
       <c r="K1077" s="23"/>
@@ -27539,11 +27634,9 @@
     <row r="1078" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1078" s="9"/>
       <c r="B1078" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1078" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1078" s="26"/>
       <c r="D1078" s="22" t="s">
         <v>27</v>
       </c>
@@ -27556,7 +27649,7 @@
       <c r="G1078" s="22"/>
       <c r="H1078" s="22"/>
       <c r="I1078" s="23" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="J1078" s="23"/>
       <c r="K1078" s="23"/>
@@ -27564,11 +27657,9 @@
     <row r="1079" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1079" s="9"/>
       <c r="B1079" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1079" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1079" s="26"/>
       <c r="D1079" s="22" t="s">
         <v>27</v>
       </c>
@@ -27581,7 +27672,7 @@
       <c r="G1079" s="22"/>
       <c r="H1079" s="22"/>
       <c r="I1079" s="23" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="J1079" s="23"/>
       <c r="K1079" s="23"/>
@@ -27589,7 +27680,7 @@
     <row r="1080" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1080" s="9"/>
       <c r="B1080" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1080" s="22" t="s">
         <v>27</v>
@@ -27606,7 +27697,7 @@
       <c r="G1080" s="22"/>
       <c r="H1080" s="22"/>
       <c r="I1080" s="23" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="J1080" s="23"/>
       <c r="K1080" s="23"/>
@@ -27614,9 +27705,11 @@
     <row r="1081" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1081" s="9"/>
       <c r="B1081" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1081" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1081" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1081" s="22" t="s">
         <v>27</v>
       </c>
@@ -27629,7 +27722,7 @@
       <c r="G1081" s="22"/>
       <c r="H1081" s="22"/>
       <c r="I1081" s="23" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="J1081" s="23"/>
       <c r="K1081" s="23"/>
@@ -27637,20 +27730,24 @@
     <row r="1082" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1082" s="9"/>
       <c r="B1082" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1082" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1082" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1082" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1082" s="26"/>
+      <c r="E1082" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1082" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1082" s="22"/>
       <c r="H1082" s="22"/>
       <c r="I1082" s="23" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="J1082" s="23"/>
       <c r="K1082" s="23"/>
@@ -27658,20 +27755,22 @@
     <row r="1083" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1083" s="9"/>
       <c r="B1083" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1083" s="26"/>
       <c r="D1083" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1083" s="26"/>
+      <c r="E1083" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1083" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1083" s="22"/>
       <c r="H1083" s="22"/>
       <c r="I1083" s="23" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="J1083" s="23"/>
       <c r="K1083" s="23"/>
@@ -27679,7 +27778,7 @@
     <row r="1084" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1084" s="9"/>
       <c r="B1084" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1084" s="26"/>
       <c r="D1084" s="22" t="s">
@@ -27692,7 +27791,7 @@
       <c r="G1084" s="22"/>
       <c r="H1084" s="22"/>
       <c r="I1084" s="23" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="J1084" s="23"/>
       <c r="K1084" s="23"/>
@@ -27700,24 +27799,20 @@
     <row r="1085" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1085" s="9"/>
       <c r="B1085" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1085" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1085" s="26"/>
       <c r="D1085" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1085" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1085" s="26"/>
       <c r="F1085" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1085" s="22"/>
       <c r="H1085" s="22"/>
       <c r="I1085" s="23" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="J1085" s="23"/>
       <c r="K1085" s="23"/>
@@ -27725,24 +27820,20 @@
     <row r="1086" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1086" s="9"/>
       <c r="B1086" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1086" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1086" s="26"/>
       <c r="D1086" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1086" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1086" s="26"/>
       <c r="F1086" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1086" s="22"/>
       <c r="H1086" s="22"/>
       <c r="I1086" s="23" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="J1086" s="23"/>
       <c r="K1086" s="23"/>
@@ -27750,9 +27841,11 @@
     <row r="1087" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1087" s="9"/>
       <c r="B1087" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1087" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1087" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1087" s="22" t="s">
         <v>27</v>
       </c>
@@ -27765,7 +27858,7 @@
       <c r="G1087" s="22"/>
       <c r="H1087" s="22"/>
       <c r="I1087" s="23" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="J1087" s="23"/>
       <c r="K1087" s="23"/>
@@ -27773,9 +27866,11 @@
     <row r="1088" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1088" s="9"/>
       <c r="B1088" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1088" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1088" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1088" s="22" t="s">
         <v>27</v>
       </c>
@@ -27788,7 +27883,7 @@
       <c r="G1088" s="22"/>
       <c r="H1088" s="22"/>
       <c r="I1088" s="23" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="J1088" s="23"/>
       <c r="K1088" s="23"/>
@@ -27796,7 +27891,7 @@
     <row r="1089" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1089" s="9"/>
       <c r="B1089" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1089" s="26"/>
       <c r="D1089" s="22" t="s">
@@ -27811,7 +27906,7 @@
       <c r="G1089" s="22"/>
       <c r="H1089" s="22"/>
       <c r="I1089" s="23" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="J1089" s="23"/>
       <c r="K1089" s="23"/>
@@ -27819,7 +27914,7 @@
     <row r="1090" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1090" s="9"/>
       <c r="B1090" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1090" s="26"/>
       <c r="D1090" s="22" t="s">
@@ -27834,7 +27929,7 @@
       <c r="G1090" s="22"/>
       <c r="H1090" s="22"/>
       <c r="I1090" s="23" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="J1090" s="23"/>
       <c r="K1090" s="23"/>
@@ -27842,7 +27937,7 @@
     <row r="1091" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1091" s="9"/>
       <c r="B1091" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1091" s="26"/>
       <c r="D1091" s="22" t="s">
@@ -27857,7 +27952,7 @@
       <c r="G1091" s="22"/>
       <c r="H1091" s="22"/>
       <c r="I1091" s="23" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="J1091" s="23"/>
       <c r="K1091" s="23"/>
@@ -27865,7 +27960,7 @@
     <row r="1092" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1092" s="9"/>
       <c r="B1092" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1092" s="26"/>
       <c r="D1092" s="22" t="s">
@@ -27880,7 +27975,7 @@
       <c r="G1092" s="22"/>
       <c r="H1092" s="22"/>
       <c r="I1092" s="23" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="J1092" s="23"/>
       <c r="K1092" s="23"/>
@@ -27888,11 +27983,9 @@
     <row r="1093" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1093" s="9"/>
       <c r="B1093" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1093" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1093" s="26"/>
       <c r="D1093" s="22" t="s">
         <v>27</v>
       </c>
@@ -27905,7 +27998,7 @@
       <c r="G1093" s="22"/>
       <c r="H1093" s="22"/>
       <c r="I1093" s="23" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="J1093" s="23"/>
       <c r="K1093" s="23"/>
@@ -27913,11 +28006,9 @@
     <row r="1094" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1094" s="9"/>
       <c r="B1094" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1094" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1094" s="26"/>
       <c r="D1094" s="22" t="s">
         <v>27</v>
       </c>
@@ -27930,7 +28021,7 @@
       <c r="G1094" s="22"/>
       <c r="H1094" s="22"/>
       <c r="I1094" s="23" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="J1094" s="23"/>
       <c r="K1094" s="23"/>
@@ -27938,9 +28029,11 @@
     <row r="1095" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1095" s="9"/>
       <c r="B1095" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1095" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1095" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1095" s="22" t="s">
         <v>27</v>
       </c>
@@ -27953,7 +28046,7 @@
       <c r="G1095" s="22"/>
       <c r="H1095" s="22"/>
       <c r="I1095" s="23" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="J1095" s="23"/>
       <c r="K1095" s="23"/>
@@ -27961,7 +28054,7 @@
     <row r="1096" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1096" s="9"/>
       <c r="B1096" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1096" s="22" t="s">
         <v>27</v>
@@ -27978,7 +28071,7 @@
       <c r="G1096" s="22"/>
       <c r="H1096" s="22"/>
       <c r="I1096" s="23" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="J1096" s="23"/>
       <c r="K1096" s="23"/>
@@ -27986,11 +28079,9 @@
     <row r="1097" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1097" s="9"/>
       <c r="B1097" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1097" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1097" s="26"/>
       <c r="D1097" s="22" t="s">
         <v>27</v>
       </c>
@@ -28003,7 +28094,7 @@
       <c r="G1097" s="22"/>
       <c r="H1097" s="22"/>
       <c r="I1097" s="23" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="J1097" s="23"/>
       <c r="K1097" s="23"/>
@@ -28011,9 +28102,11 @@
     <row r="1098" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1098" s="9"/>
       <c r="B1098" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1098" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1098" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1098" s="22" t="s">
         <v>27</v>
       </c>
@@ -28026,7 +28119,7 @@
       <c r="G1098" s="22"/>
       <c r="H1098" s="22"/>
       <c r="I1098" s="23" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="J1098" s="23"/>
       <c r="K1098" s="23"/>
@@ -28034,7 +28127,7 @@
     <row r="1099" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1099" s="9"/>
       <c r="B1099" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1099" s="22" t="s">
         <v>27</v>
@@ -28051,7 +28144,7 @@
       <c r="G1099" s="22"/>
       <c r="H1099" s="22"/>
       <c r="I1099" s="23" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="J1099" s="23"/>
       <c r="K1099" s="23"/>
@@ -28059,7 +28152,7 @@
     <row r="1100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1100" s="9"/>
       <c r="B1100" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1100" s="26"/>
       <c r="D1100" s="22" t="s">
@@ -28074,7 +28167,7 @@
       <c r="G1100" s="22"/>
       <c r="H1100" s="22"/>
       <c r="I1100" s="23" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="J1100" s="23"/>
       <c r="K1100" s="23"/>
@@ -28082,7 +28175,7 @@
     <row r="1101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1101" s="9"/>
       <c r="B1101" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1101" s="22" t="s">
         <v>27</v>
@@ -28099,7 +28192,7 @@
       <c r="G1101" s="22"/>
       <c r="H1101" s="22"/>
       <c r="I1101" s="23" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="J1101" s="23"/>
       <c r="K1101" s="23"/>
@@ -28107,11 +28200,9 @@
     <row r="1102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1102" s="9"/>
       <c r="B1102" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1102" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1102" s="26"/>
       <c r="D1102" s="22" t="s">
         <v>27</v>
       </c>
@@ -28124,7 +28215,7 @@
       <c r="G1102" s="22"/>
       <c r="H1102" s="22"/>
       <c r="I1102" s="23" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="J1102" s="23"/>
       <c r="K1102" s="23"/>
@@ -28132,7 +28223,7 @@
     <row r="1103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1103" s="9"/>
       <c r="B1103" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1103" s="22" t="s">
         <v>27</v>
@@ -28149,7 +28240,7 @@
       <c r="G1103" s="22"/>
       <c r="H1103" s="22"/>
       <c r="I1103" s="23" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="J1103" s="23"/>
       <c r="K1103" s="23"/>
@@ -28157,7 +28248,7 @@
     <row r="1104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1104" s="9"/>
       <c r="B1104" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1104" s="22" t="s">
         <v>27</v>
@@ -28174,7 +28265,7 @@
       <c r="G1104" s="22"/>
       <c r="H1104" s="22"/>
       <c r="I1104" s="23" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="J1104" s="23"/>
       <c r="K1104" s="23"/>
@@ -28182,7 +28273,7 @@
     <row r="1105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1105" s="9"/>
       <c r="B1105" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1105" s="22" t="s">
         <v>27</v>
@@ -28199,7 +28290,7 @@
       <c r="G1105" s="22"/>
       <c r="H1105" s="22"/>
       <c r="I1105" s="23" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="J1105" s="23"/>
       <c r="K1105" s="23"/>
@@ -28207,9 +28298,11 @@
     <row r="1106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1106" s="9"/>
       <c r="B1106" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1106" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1106" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1106" s="22" t="s">
         <v>27</v>
       </c>
@@ -28222,7 +28315,7 @@
       <c r="G1106" s="22"/>
       <c r="H1106" s="22"/>
       <c r="I1106" s="23" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="J1106" s="23"/>
       <c r="K1106" s="23"/>
@@ -28230,7 +28323,7 @@
     <row r="1107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1107" s="9"/>
       <c r="B1107" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1107" s="22" t="s">
         <v>27</v>
@@ -28247,7 +28340,7 @@
       <c r="G1107" s="22"/>
       <c r="H1107" s="22"/>
       <c r="I1107" s="23" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="J1107" s="23"/>
       <c r="K1107" s="23"/>
@@ -28255,11 +28348,9 @@
     <row r="1108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1108" s="9"/>
       <c r="B1108" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1108" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1108" s="26"/>
       <c r="D1108" s="22" t="s">
         <v>27</v>
       </c>
@@ -28272,7 +28363,7 @@
       <c r="G1108" s="22"/>
       <c r="H1108" s="22"/>
       <c r="I1108" s="23" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="J1108" s="23"/>
       <c r="K1108" s="23"/>
@@ -28280,7 +28371,7 @@
     <row r="1109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1109" s="9"/>
       <c r="B1109" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1109" s="22" t="s">
         <v>27</v>
@@ -28297,7 +28388,7 @@
       <c r="G1109" s="22"/>
       <c r="H1109" s="22"/>
       <c r="I1109" s="23" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="J1109" s="23"/>
       <c r="K1109" s="23"/>
@@ -28305,7 +28396,7 @@
     <row r="1110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1110" s="9"/>
       <c r="B1110" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1110" s="22" t="s">
         <v>27</v>
@@ -28322,38 +28413,40 @@
       <c r="G1110" s="22"/>
       <c r="H1110" s="22"/>
       <c r="I1110" s="23" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="J1110" s="23"/>
       <c r="K1110" s="23"/>
     </row>
     <row r="1111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1111" s="9"/>
-      <c r="B1111" s="28" t="s">
-        <v>1073</v>
-      </c>
-      <c r="C1111" s="26"/>
+      <c r="B1111" s="22" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C1111" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1111" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1111" s="26"/>
+      <c r="E1111" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1111" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1111" s="22"/>
       <c r="H1111" s="22"/>
       <c r="I1111" s="23" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="J1111" s="23"/>
-      <c r="K1111" s="23" t="s">
-        <v>621</v>
-      </c>
+      <c r="K1111" s="23"/>
     </row>
     <row r="1112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1112" s="9"/>
       <c r="B1112" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1112" s="22" t="s">
         <v>27</v>
@@ -28370,40 +28463,38 @@
       <c r="G1112" s="22"/>
       <c r="H1112" s="22"/>
       <c r="I1112" s="23" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="J1112" s="23"/>
       <c r="K1112" s="23"/>
     </row>
     <row r="1113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1113" s="9"/>
-      <c r="B1113" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1113" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="B1113" s="28" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C1113" s="26"/>
       <c r="D1113" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1113" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1113" s="26"/>
       <c r="F1113" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1113" s="22"/>
       <c r="H1113" s="22"/>
       <c r="I1113" s="23" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="J1113" s="23"/>
-      <c r="K1113" s="23"/>
+      <c r="K1113" s="23" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="1114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1114" s="9"/>
       <c r="B1114" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1114" s="22" t="s">
         <v>27</v>
@@ -28420,7 +28511,7 @@
       <c r="G1114" s="22"/>
       <c r="H1114" s="22"/>
       <c r="I1114" s="23" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="J1114" s="23"/>
       <c r="K1114" s="23"/>
@@ -28428,7 +28519,7 @@
     <row r="1115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1115" s="9"/>
       <c r="B1115" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1115" s="22" t="s">
         <v>27</v>
@@ -28445,7 +28536,7 @@
       <c r="G1115" s="22"/>
       <c r="H1115" s="22"/>
       <c r="I1115" s="23" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="J1115" s="23"/>
       <c r="K1115" s="23"/>
@@ -28453,7 +28544,7 @@
     <row r="1116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1116" s="9"/>
       <c r="B1116" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1116" s="22" t="s">
         <v>27</v>
@@ -28470,7 +28561,7 @@
       <c r="G1116" s="22"/>
       <c r="H1116" s="22"/>
       <c r="I1116" s="23" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="J1116" s="23"/>
       <c r="K1116" s="23"/>
@@ -28478,7 +28569,7 @@
     <row r="1117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1117" s="9"/>
       <c r="B1117" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1117" s="22" t="s">
         <v>27</v>
@@ -28495,7 +28586,7 @@
       <c r="G1117" s="22"/>
       <c r="H1117" s="22"/>
       <c r="I1117" s="23" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="J1117" s="23"/>
       <c r="K1117" s="23"/>
@@ -28503,7 +28594,7 @@
     <row r="1118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1118" s="9"/>
       <c r="B1118" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1118" s="22" t="s">
         <v>27</v>
@@ -28520,7 +28611,7 @@
       <c r="G1118" s="22"/>
       <c r="H1118" s="22"/>
       <c r="I1118" s="23" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="J1118" s="23"/>
       <c r="K1118" s="23"/>
@@ -28528,9 +28619,11 @@
     <row r="1119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1119" s="9"/>
       <c r="B1119" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1119" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1119" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1119" s="22" t="s">
         <v>27</v>
       </c>
@@ -28543,16 +28636,19 @@
       <c r="G1119" s="22"/>
       <c r="H1119" s="22"/>
       <c r="I1119" s="23" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="J1119" s="23"/>
       <c r="K1119" s="23"/>
     </row>
     <row r="1120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1120" s="9"/>
       <c r="B1120" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1120" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1120" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1120" s="22" t="s">
         <v>27</v>
       </c>
@@ -28565,14 +28661,15 @@
       <c r="G1120" s="22"/>
       <c r="H1120" s="22"/>
       <c r="I1120" s="23" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="J1120" s="23"/>
       <c r="K1120" s="23"/>
     </row>
     <row r="1121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1121" s="9"/>
       <c r="B1121" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1121" s="26"/>
       <c r="D1121" s="22" t="s">
@@ -28587,18 +28684,16 @@
       <c r="G1121" s="22"/>
       <c r="H1121" s="22"/>
       <c r="I1121" s="23" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="J1121" s="23"/>
       <c r="K1121" s="23"/>
     </row>
     <row r="1122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1122" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1122" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1122" s="26"/>
       <c r="D1122" s="22" t="s">
         <v>27</v>
       </c>
@@ -28611,54 +28706,60 @@
       <c r="G1122" s="22"/>
       <c r="H1122" s="22"/>
       <c r="I1122" s="23" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="J1122" s="23"/>
       <c r="K1122" s="23"/>
     </row>
     <row r="1123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1123" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1123" s="26"/>
       <c r="D1123" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1123" s="26"/>
+      <c r="E1123" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1123" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1123" s="22"/>
       <c r="H1123" s="22"/>
       <c r="I1123" s="23" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="J1123" s="23"/>
       <c r="K1123" s="23"/>
     </row>
     <row r="1124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1124" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1124" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1124" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1124" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1124" s="26"/>
+      <c r="E1124" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1124" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1124" s="22"/>
       <c r="H1124" s="22"/>
       <c r="I1124" s="23" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="J1124" s="23"/>
       <c r="K1124" s="23"/>
     </row>
     <row r="1125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1125" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1125" s="26"/>
       <c r="D1125" s="22" t="s">
@@ -28671,50 +28772,42 @@
       <c r="G1125" s="22"/>
       <c r="H1125" s="22"/>
       <c r="I1125" s="23" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="J1125" s="23"/>
       <c r="K1125" s="23"/>
     </row>
     <row r="1126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1126" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1126" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1126" s="26"/>
       <c r="D1126" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1126" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1126" s="26"/>
       <c r="F1126" s="22" t="s">
         <v>648</v>
       </c>
       <c r="G1126" s="22"/>
       <c r="H1126" s="22"/>
       <c r="I1126" s="23" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="J1126" s="23"/>
       <c r="K1126" s="23"/>
     </row>
     <row r="1127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1127" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1127" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1074</v>
+      </c>
+      <c r="C1127" s="26"/>
       <c r="D1127" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1127" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1127" s="26"/>
       <c r="F1127" s="22" t="s">
-        <v>1148</v>
+        <v>648</v>
       </c>
       <c r="G1127" s="22"/>
       <c r="H1127" s="22"/>
@@ -28726,9 +28819,11 @@
     </row>
     <row r="1128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1128" s="22" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C1128" s="26"/>
+        <v>1074</v>
+      </c>
+      <c r="C1128" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1128" s="22" t="s">
         <v>27</v>
       </c>
@@ -28736,7 +28831,7 @@
         <v>27</v>
       </c>
       <c r="F1128" s="22" t="s">
-        <v>1148</v>
+        <v>648</v>
       </c>
       <c r="G1128" s="22"/>
       <c r="H1128" s="22"/>
@@ -28744,35 +28839,35 @@
         <v>1150</v>
       </c>
       <c r="J1128" s="23"/>
-      <c r="K1128" s="23" t="s">
+      <c r="K1128" s="23"/>
+    </row>
+    <row r="1129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1129" s="22" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C1129" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1129" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1129" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1129" s="22" t="s">
         <v>1151</v>
       </c>
-    </row>
-    <row r="1129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1129" s="28" t="s">
-        <v>648</v>
-      </c>
-      <c r="C1129" s="28"/>
-      <c r="D1129" s="28" t="s">
-        <v>648</v>
-      </c>
-      <c r="E1129" s="28"/>
-      <c r="F1129" s="28" t="s">
-        <v>648</v>
-      </c>
-      <c r="G1129" s="28"/>
-      <c r="H1129" s="28"/>
-      <c r="I1129" s="29" t="s">
+      <c r="G1129" s="22"/>
+      <c r="H1129" s="22"/>
+      <c r="I1129" s="23" t="s">
         <v>1152</v>
       </c>
-      <c r="J1129" s="29"/>
-      <c r="K1129" s="29" t="s">
-        <v>1153</v>
-      </c>
+      <c r="J1129" s="23"/>
+      <c r="K1129" s="23"/>
     </row>
     <row r="1130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1130" s="22" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C1130" s="26"/>
       <c r="D1130" s="22" t="s">
@@ -28782,16 +28877,16 @@
         <v>27</v>
       </c>
       <c r="F1130" s="22" t="s">
-        <v>1148</v>
+        <v>1151</v>
       </c>
       <c r="G1130" s="22"/>
       <c r="H1130" s="22"/>
       <c r="I1130" s="23" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="J1130" s="23"/>
       <c r="K1130" s="23" t="s">
-        <v>1151</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="1131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28813,7 +28908,53 @@
       </c>
       <c r="J1131" s="29"/>
       <c r="K1131" s="29" t="s">
-        <v>1153</v>
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="1132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1132" s="22" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C1132" s="26"/>
+      <c r="D1132" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1132" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1132" s="22" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G1132" s="22"/>
+      <c r="H1132" s="22"/>
+      <c r="I1132" s="23" t="s">
+        <v>1157</v>
+      </c>
+      <c r="J1132" s="23"/>
+      <c r="K1132" s="23" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="1133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1133" s="28" t="s">
+        <v>648</v>
+      </c>
+      <c r="C1133" s="28"/>
+      <c r="D1133" s="28" t="s">
+        <v>648</v>
+      </c>
+      <c r="E1133" s="28"/>
+      <c r="F1133" s="28" t="s">
+        <v>648</v>
+      </c>
+      <c r="G1133" s="28"/>
+      <c r="H1133" s="28"/>
+      <c r="I1133" s="29" t="s">
+        <v>1158</v>
+      </c>
+      <c r="J1133" s="29"/>
+      <c r="K1133" s="29" t="s">
+        <v>1156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated bookmarks in vi -- no code changes
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4917" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4907" uniqueCount="1165">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -3966,8 +3966,8 @@
   </sheetPr>
   <dimension ref="A1:Q1139"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A577" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B577" activeCellId="0" sqref="B577"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">B10+B11</f>
-        <v>738</v>
+        <v>743</v>
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">COUNTIF(C18:C1466,"X")</f>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="E9" s="13" t="n">
         <f aca="false">COUNTIF(E18:E1466,"X")</f>
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="F9" s="13" t="n">
         <f aca="false">COUNTIF(F18:F1466,"S")+COUNTIF(F18:F1466,"I")+COUNTIF(F18:F1466,"X")+COUNTIF(F18:F1466,"SI")+COUNTIF(F18:F1466,"IS")+COUNTIF(F18:F1466,"N/A")</f>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="I9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.79810298102981</v>
+        <v>0.792732166890982</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4115,7 +4115,7 @@
       </c>
       <c r="B10" s="13" t="n">
         <f aca="false">COUNTIF(B18:B1466,"X")</f>
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>15</v>
@@ -4131,7 +4131,7 @@
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.313008130081301</v>
+        <v>0.310901749663526</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4140,7 +4140,7 @@
       </c>
       <c r="B12" s="13" t="n">
         <f aca="false">COUNTIF(B18:B1466,"/")</f>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -17582,8 +17582,8 @@
       <c r="A640" s="21" t="s">
         <v>731</v>
       </c>
-      <c r="B640" s="28" t="s">
-        <v>620</v>
+      <c r="B640" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="C640" s="22" t="s">
         <v>27</v>
@@ -17606,9 +17606,9 @@
       <c r="M640" s="22"/>
       <c r="N640" s="22"/>
     </row>
-    <row r="641" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B641" s="28" t="s">
-        <v>620</v>
+    <row r="641" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B641" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="C641" s="26"/>
       <c r="D641" s="22"/>
@@ -17625,15 +17625,13 @@
       <c r="M641" s="22"/>
       <c r="N641" s="22"/>
     </row>
-    <row r="642" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="642" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B642" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C642" s="26"/>
       <c r="D642" s="22"/>
-      <c r="E642" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E642" s="26"/>
       <c r="F642" s="26"/>
       <c r="G642" s="22"/>
       <c r="H642" s="22"/>
@@ -17646,15 +17644,13 @@
       <c r="M642" s="22"/>
       <c r="N642" s="22"/>
     </row>
-    <row r="643" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="643" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B643" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C643" s="26"/>
       <c r="D643" s="22"/>
-      <c r="E643" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E643" s="26"/>
       <c r="F643" s="26"/>
       <c r="G643" s="22"/>
       <c r="H643" s="22"/>
@@ -18568,7 +18564,7 @@
       </c>
       <c r="C681" s="26"/>
       <c r="D681" s="22"/>
-      <c r="E681" s="22"/>
+      <c r="E681" s="26"/>
       <c r="F681" s="26"/>
       <c r="G681" s="22"/>
       <c r="H681" s="22"/>
@@ -18583,14 +18579,14 @@
       <c r="M681" s="22"/>
       <c r="N681" s="22"/>
     </row>
-    <row r="682" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="682" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="21"/>
       <c r="B682" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C682" s="26"/>
       <c r="D682" s="22"/>
-      <c r="E682" s="22"/>
+      <c r="E682" s="26"/>
       <c r="F682" s="26"/>
       <c r="G682" s="22"/>
       <c r="H682" s="22"/>
@@ -18604,12 +18600,12 @@
       <c r="N682" s="22"/>
     </row>
     <row r="683" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B683" s="28" t="s">
-        <v>620</v>
+      <c r="B683" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="C683" s="26"/>
       <c r="D683" s="22"/>
-      <c r="E683" s="22"/>
+      <c r="E683" s="26"/>
       <c r="F683" s="26"/>
       <c r="G683" s="22"/>
       <c r="H683" s="22"/>
@@ -18630,7 +18626,7 @@
       </c>
       <c r="C684" s="26"/>
       <c r="D684" s="22"/>
-      <c r="E684" s="22"/>
+      <c r="E684" s="26"/>
       <c r="F684" s="26"/>
       <c r="G684" s="22"/>
       <c r="H684" s="22"/>
@@ -18645,13 +18641,13 @@
       <c r="M684" s="22"/>
       <c r="N684" s="22"/>
     </row>
-    <row r="685" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="685" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B685" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C685" s="26"/>
       <c r="D685" s="22"/>
-      <c r="E685" s="22"/>
+      <c r="E685" s="26"/>
       <c r="F685" s="26"/>
       <c r="G685" s="22"/>
       <c r="H685" s="22"/>
@@ -18670,7 +18666,7 @@
       </c>
       <c r="C686" s="26"/>
       <c r="D686" s="22"/>
-      <c r="E686" s="22"/>
+      <c r="E686" s="26"/>
       <c r="F686" s="26"/>
       <c r="G686" s="22"/>
       <c r="H686" s="22"/>
@@ -18691,7 +18687,7 @@
       </c>
       <c r="C687" s="26"/>
       <c r="D687" s="22"/>
-      <c r="E687" s="22"/>
+      <c r="E687" s="26"/>
       <c r="F687" s="26"/>
       <c r="G687" s="22"/>
       <c r="H687" s="22"/>
@@ -18801,13 +18797,13 @@
       <c r="N691" s="22"/>
     </row>
     <row r="692" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B692" s="28" t="s">
-        <v>620</v>
+      <c r="B692" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="C692" s="22"/>
       <c r="D692" s="22"/>
-      <c r="E692" s="22"/>
-      <c r="F692" s="22"/>
+      <c r="E692" s="26"/>
+      <c r="F692" s="26"/>
       <c r="G692" s="22"/>
       <c r="H692" s="22"/>
       <c r="I692" s="23" t="s">
@@ -18821,14 +18817,14 @@
       <c r="M692" s="22"/>
       <c r="N692" s="22"/>
     </row>
-    <row r="693" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B693" s="28" t="s">
-        <v>620</v>
+    <row r="693" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B693" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="C693" s="22"/>
       <c r="D693" s="22"/>
-      <c r="E693" s="22"/>
-      <c r="F693" s="22"/>
+      <c r="E693" s="26"/>
+      <c r="F693" s="26"/>
       <c r="G693" s="22"/>
       <c r="H693" s="22"/>
       <c r="I693" s="23" t="s">
@@ -18840,14 +18836,14 @@
       <c r="M693" s="22"/>
       <c r="N693" s="22"/>
     </row>
-    <row r="694" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="694" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B694" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C694" s="22"/>
       <c r="D694" s="22"/>
-      <c r="E694" s="22"/>
-      <c r="F694" s="22"/>
+      <c r="E694" s="26"/>
+      <c r="F694" s="26"/>
       <c r="G694" s="22"/>
       <c r="H694" s="22"/>
       <c r="I694" s="23" t="s">
@@ -18859,14 +18855,14 @@
       <c r="M694" s="22"/>
       <c r="N694" s="22"/>
     </row>
-    <row r="695" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="695" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B695" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C695" s="22"/>
       <c r="D695" s="22"/>
-      <c r="E695" s="22"/>
-      <c r="F695" s="22"/>
+      <c r="E695" s="26"/>
+      <c r="F695" s="26"/>
       <c r="G695" s="22"/>
       <c r="H695" s="22"/>
       <c r="I695" s="23" t="s">
@@ -18884,8 +18880,8 @@
       </c>
       <c r="C696" s="22"/>
       <c r="D696" s="22"/>
-      <c r="E696" s="22"/>
-      <c r="F696" s="22"/>
+      <c r="E696" s="26"/>
+      <c r="F696" s="26"/>
       <c r="G696" s="22"/>
       <c r="H696" s="22"/>
       <c r="I696" s="23" t="s">
@@ -18905,8 +18901,8 @@
       </c>
       <c r="C697" s="22"/>
       <c r="D697" s="22"/>
-      <c r="E697" s="22"/>
-      <c r="F697" s="22"/>
+      <c r="E697" s="26"/>
+      <c r="F697" s="26"/>
       <c r="G697" s="22"/>
       <c r="H697" s="22"/>
       <c r="I697" s="23" t="s">
@@ -18926,8 +18922,8 @@
       </c>
       <c r="C698" s="22"/>
       <c r="D698" s="22"/>
-      <c r="E698" s="22"/>
-      <c r="F698" s="22"/>
+      <c r="E698" s="26"/>
+      <c r="F698" s="26"/>
       <c r="G698" s="22"/>
       <c r="H698" s="22"/>
       <c r="I698" s="23" t="s">
@@ -18947,8 +18943,8 @@
       </c>
       <c r="C699" s="22"/>
       <c r="D699" s="22"/>
-      <c r="E699" s="22"/>
-      <c r="F699" s="22"/>
+      <c r="E699" s="26"/>
+      <c r="F699" s="26"/>
       <c r="G699" s="22"/>
       <c r="H699" s="22"/>
       <c r="I699" s="23" t="s">
@@ -18968,8 +18964,8 @@
       </c>
       <c r="C700" s="22"/>
       <c r="D700" s="22"/>
-      <c r="E700" s="22"/>
-      <c r="F700" s="22"/>
+      <c r="E700" s="26"/>
+      <c r="F700" s="26"/>
       <c r="G700" s="22"/>
       <c r="H700" s="22"/>
       <c r="I700" s="23" t="s">
@@ -18989,8 +18985,8 @@
       </c>
       <c r="C701" s="22"/>
       <c r="D701" s="22"/>
-      <c r="E701" s="22"/>
-      <c r="F701" s="22"/>
+      <c r="E701" s="26"/>
+      <c r="F701" s="26"/>
       <c r="G701" s="22"/>
       <c r="H701" s="22"/>
       <c r="I701" s="23" t="s">
@@ -21473,9 +21469,7 @@
       <c r="D813" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E813" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E813" s="26"/>
       <c r="F813" s="26"/>
       <c r="G813" s="22"/>
       <c r="H813" s="22"/>
@@ -21496,9 +21490,7 @@
       <c r="D814" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E814" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E814" s="26"/>
       <c r="F814" s="26"/>
       <c r="G814" s="22"/>
       <c r="H814" s="22"/>
@@ -21519,9 +21511,7 @@
       <c r="D815" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E815" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E815" s="26"/>
       <c r="F815" s="26"/>
       <c r="G815" s="22"/>
       <c r="H815" s="22"/>
@@ -21542,9 +21532,7 @@
       <c r="D816" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E816" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E816" s="26"/>
       <c r="F816" s="26"/>
       <c r="G816" s="22"/>
       <c r="H816" s="22"/>
@@ -25825,9 +25813,7 @@
       <c r="D996" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E996" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E996" s="26"/>
       <c r="F996" s="26"/>
       <c r="G996" s="22"/>
       <c r="H996" s="22"/>
@@ -25879,9 +25865,7 @@
       <c r="D998" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E998" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E998" s="26"/>
       <c r="F998" s="26"/>
       <c r="G998" s="22"/>
       <c r="H998" s="22"/>
@@ -25933,9 +25917,7 @@
       <c r="D1000" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1000" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1000" s="26"/>
       <c r="F1000" s="26"/>
       <c r="G1000" s="22"/>
       <c r="H1000" s="22"/>
@@ -27270,7 +27252,7 @@
       <c r="J1061" s="23"/>
       <c r="K1061" s="23"/>
     </row>
-    <row r="1062" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1062" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1062" s="21"/>
       <c r="B1062" s="22" t="s">
         <v>1080</v>
@@ -27279,9 +27261,7 @@
       <c r="D1062" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1062" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1062" s="26"/>
       <c r="F1062" s="22" t="s">
         <v>649</v>
       </c>

</xml_diff>

<commit_message>
implemented JacobianU -- needed for testing
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4907" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4909" uniqueCount="1166">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -3229,10 +3229,13 @@
     <t xml:space="preserve">NUMERICAL JACOBIAN</t>
   </si>
   <si>
-    <t xml:space="preserve">NumJacobianX.vi</t>
+    <t xml:space="preserve">NumJacobian_X.vi</t>
   </si>
   <si>
     <t xml:space="preserve">There are others that may need implemented.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumJacobian_U.vi</t>
   </si>
   <si>
     <t xml:space="preserve">RICCATI</t>
@@ -3966,8 +3969,8 @@
   </sheetPr>
   <dimension ref="A1:Q1139"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1030" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1040" activeCellId="0" sqref="C1040"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4078,7 +4081,7 @@
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">B10+B11</f>
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">COUNTIF(C18:C1466,"X")</f>
@@ -4106,7 +4109,7 @@
       </c>
       <c r="I9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.792732166890982</v>
+        <v>0.791666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4115,7 +4118,7 @@
       </c>
       <c r="B10" s="13" t="n">
         <f aca="false">COUNTIF(B18:B1466,"X")</f>
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>15</v>
@@ -4131,7 +4134,7 @@
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.310901749663526</v>
+        <v>0.310483870967742</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26801,7 +26804,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="1039" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1039" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1039" s="21" t="s">
         <v>1067</v>
       </c>
@@ -26829,15 +26832,19 @@
       <c r="M1039" s="22"/>
       <c r="N1039" s="22"/>
     </row>
-    <row r="1040" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1040" s="22"/>
-      <c r="C1040" s="22"/>
+    <row r="1040" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1040" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1040" s="26"/>
       <c r="D1040" s="22"/>
-      <c r="E1040" s="22"/>
-      <c r="F1040" s="22"/>
+      <c r="E1040" s="26"/>
+      <c r="F1040" s="26"/>
       <c r="G1040" s="22"/>
       <c r="H1040" s="22"/>
-      <c r="I1040" s="23"/>
+      <c r="I1040" s="23" t="s">
+        <v>1070</v>
+      </c>
       <c r="J1040" s="23"/>
       <c r="K1040" s="23"/>
       <c r="L1040" s="22"/>
@@ -26965,7 +26972,7 @@
     </row>
     <row r="1047" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1047" s="21" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B1047" s="28" t="s">
         <v>620</v>
@@ -26979,7 +26986,7 @@
       <c r="G1047" s="22"/>
       <c r="H1047" s="22"/>
       <c r="I1047" s="23" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="J1047" s="23"/>
       <c r="K1047" s="23" t="s">
@@ -27002,11 +27009,11 @@
       <c r="G1048" s="22"/>
       <c r="H1048" s="22"/>
       <c r="I1048" s="23" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="J1048" s="23"/>
       <c r="K1048" s="23" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="L1048" s="22"/>
       <c r="M1048" s="22"/>
@@ -27029,7 +27036,7 @@
       </c>
       <c r="H1049" s="22"/>
       <c r="I1049" s="23" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="J1049" s="23"/>
       <c r="K1049" s="23"/>
@@ -27052,7 +27059,7 @@
       </c>
       <c r="H1050" s="22"/>
       <c r="I1050" s="23" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="J1050" s="23"/>
       <c r="K1050" s="23"/>
@@ -27073,7 +27080,7 @@
       <c r="G1051" s="22"/>
       <c r="H1051" s="22"/>
       <c r="I1051" s="23" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="J1051" s="23"/>
       <c r="K1051" s="23"/>
@@ -27094,7 +27101,7 @@
       <c r="G1052" s="22"/>
       <c r="H1052" s="22"/>
       <c r="I1052" s="23" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="J1052" s="23"/>
       <c r="K1052" s="23"/>
@@ -27149,7 +27156,7 @@
     </row>
     <row r="1057" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1057" s="16" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B1057" s="17"/>
       <c r="C1057" s="18"/>
@@ -27206,10 +27213,10 @@
     </row>
     <row r="1060" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1060" s="21" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B1060" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1060" s="26"/>
       <c r="D1060" s="22" t="s">
@@ -27224,7 +27231,7 @@
       <c r="G1060" s="22"/>
       <c r="H1060" s="22"/>
       <c r="I1060" s="23" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="J1060" s="23"/>
       <c r="K1060" s="23"/>
@@ -27232,7 +27239,7 @@
     <row r="1061" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1061" s="21"/>
       <c r="B1061" s="28" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C1061" s="26"/>
       <c r="D1061" s="22" t="s">
@@ -27247,7 +27254,7 @@
       <c r="G1061" s="22"/>
       <c r="H1061" s="22"/>
       <c r="I1061" s="23" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="J1061" s="23"/>
       <c r="K1061" s="23"/>
@@ -27255,7 +27262,7 @@
     <row r="1062" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1062" s="21"/>
       <c r="B1062" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1062" s="26"/>
       <c r="D1062" s="22" t="s">
@@ -27268,7 +27275,7 @@
       <c r="G1062" s="22"/>
       <c r="H1062" s="22"/>
       <c r="I1062" s="23" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="J1062" s="23"/>
       <c r="K1062" s="23"/>
@@ -27276,7 +27283,7 @@
     <row r="1063" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1063" s="21"/>
       <c r="B1063" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1063" s="22" t="s">
         <v>27</v>
@@ -27293,7 +27300,7 @@
       <c r="G1063" s="22"/>
       <c r="H1063" s="22"/>
       <c r="I1063" s="23" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="J1063" s="23"/>
       <c r="K1063" s="23"/>
@@ -27301,7 +27308,7 @@
     <row r="1064" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1064" s="9"/>
       <c r="B1064" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1064" s="22" t="s">
         <v>27</v>
@@ -27318,7 +27325,7 @@
       <c r="G1064" s="22"/>
       <c r="H1064" s="22"/>
       <c r="I1064" s="23" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="J1064" s="23"/>
       <c r="K1064" s="23"/>
@@ -27326,7 +27333,7 @@
     <row r="1065" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1065" s="9"/>
       <c r="B1065" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1065" s="26"/>
       <c r="D1065" s="22" t="s">
@@ -27341,7 +27348,7 @@
       <c r="G1065" s="22"/>
       <c r="H1065" s="22"/>
       <c r="I1065" s="46" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="J1065" s="23"/>
       <c r="K1065" s="23"/>
@@ -27349,7 +27356,7 @@
     <row r="1066" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1066" s="9"/>
       <c r="B1066" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1066" s="22" t="s">
         <v>27</v>
@@ -27366,7 +27373,7 @@
       <c r="G1066" s="22"/>
       <c r="H1066" s="22"/>
       <c r="I1066" s="23" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="J1066" s="23"/>
       <c r="K1066" s="23"/>
@@ -27374,7 +27381,7 @@
     <row r="1067" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1067" s="9"/>
       <c r="B1067" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1067" s="26"/>
       <c r="D1067" s="22" t="s">
@@ -27387,7 +27394,7 @@
       <c r="G1067" s="22"/>
       <c r="H1067" s="22"/>
       <c r="I1067" s="23" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="J1067" s="23"/>
       <c r="K1067" s="23"/>
@@ -27395,7 +27402,7 @@
     <row r="1068" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1068" s="9"/>
       <c r="B1068" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1068" s="26"/>
       <c r="D1068" s="22" t="s">
@@ -27408,7 +27415,7 @@
       <c r="G1068" s="22"/>
       <c r="H1068" s="22"/>
       <c r="I1068" s="23" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="J1068" s="23"/>
       <c r="K1068" s="23"/>
@@ -27416,7 +27423,7 @@
     <row r="1069" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1069" s="9"/>
       <c r="B1069" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1069" s="26"/>
       <c r="D1069" s="22" t="s">
@@ -27429,7 +27436,7 @@
       <c r="G1069" s="22"/>
       <c r="H1069" s="22"/>
       <c r="I1069" s="23" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="J1069" s="23"/>
       <c r="K1069" s="23"/>
@@ -27437,7 +27444,7 @@
     <row r="1070" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1070" s="9"/>
       <c r="B1070" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1070" s="26"/>
       <c r="D1070" s="22" t="s">
@@ -27450,7 +27457,7 @@
       <c r="G1070" s="22"/>
       <c r="H1070" s="22"/>
       <c r="I1070" s="23" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="J1070" s="23"/>
       <c r="K1070" s="23"/>
@@ -27458,7 +27465,7 @@
     <row r="1071" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1071" s="9"/>
       <c r="B1071" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1071" s="26"/>
       <c r="D1071" s="22" t="s">
@@ -27471,7 +27478,7 @@
       <c r="G1071" s="22"/>
       <c r="H1071" s="22"/>
       <c r="I1071" s="23" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="J1071" s="23"/>
       <c r="K1071" s="23"/>
@@ -27479,7 +27486,7 @@
     <row r="1072" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1072" s="9"/>
       <c r="B1072" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1072" s="26"/>
       <c r="D1072" s="22" t="s">
@@ -27494,7 +27501,7 @@
       <c r="G1072" s="22"/>
       <c r="H1072" s="22"/>
       <c r="I1072" s="23" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="J1072" s="23"/>
       <c r="K1072" s="23"/>
@@ -27502,7 +27509,7 @@
     <row r="1073" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1073" s="9"/>
       <c r="B1073" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1073" s="26"/>
       <c r="D1073" s="22" t="s">
@@ -27517,7 +27524,7 @@
       <c r="G1073" s="22"/>
       <c r="H1073" s="22"/>
       <c r="I1073" s="23" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="J1073" s="23"/>
       <c r="K1073" s="23"/>
@@ -27525,7 +27532,7 @@
     <row r="1074" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1074" s="9"/>
       <c r="B1074" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1074" s="26"/>
       <c r="D1074" s="22" t="s">
@@ -27540,7 +27547,7 @@
       <c r="G1074" s="22"/>
       <c r="H1074" s="22"/>
       <c r="I1074" s="23" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="J1074" s="23"/>
       <c r="K1074" s="23"/>
@@ -27548,7 +27555,7 @@
     <row r="1075" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1075" s="9"/>
       <c r="B1075" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1075" s="26"/>
       <c r="D1075" s="22" t="s">
@@ -27563,7 +27570,7 @@
       <c r="G1075" s="22"/>
       <c r="H1075" s="22"/>
       <c r="I1075" s="23" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="J1075" s="23"/>
       <c r="K1075" s="23"/>
@@ -27571,7 +27578,7 @@
     <row r="1076" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1076" s="9"/>
       <c r="B1076" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1076" s="26"/>
       <c r="D1076" s="22" t="s">
@@ -27586,7 +27593,7 @@
       <c r="G1076" s="22"/>
       <c r="H1076" s="22"/>
       <c r="I1076" s="23" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="J1076" s="23"/>
       <c r="K1076" s="23"/>
@@ -27594,7 +27601,7 @@
     <row r="1077" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1077" s="9"/>
       <c r="B1077" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1077" s="26"/>
       <c r="D1077" s="22" t="s">
@@ -27609,7 +27616,7 @@
       <c r="G1077" s="22"/>
       <c r="H1077" s="22"/>
       <c r="I1077" s="23" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="J1077" s="23"/>
       <c r="K1077" s="23" t="s">
@@ -27619,7 +27626,7 @@
     <row r="1078" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1078" s="9"/>
       <c r="B1078" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1078" s="26"/>
       <c r="D1078" s="22" t="s">
@@ -27634,7 +27641,7 @@
       <c r="G1078" s="22"/>
       <c r="H1078" s="22"/>
       <c r="I1078" s="23" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="J1078" s="23"/>
       <c r="K1078" s="23"/>
@@ -27642,7 +27649,7 @@
     <row r="1079" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1079" s="9"/>
       <c r="B1079" s="28" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C1079" s="26"/>
       <c r="D1079" s="22" t="s">
@@ -27657,7 +27664,7 @@
       <c r="G1079" s="22"/>
       <c r="H1079" s="22"/>
       <c r="I1079" s="23" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="J1079" s="23"/>
       <c r="K1079" s="23"/>
@@ -27665,7 +27672,7 @@
     <row r="1080" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1080" s="9"/>
       <c r="B1080" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1080" s="22" t="s">
         <v>27</v>
@@ -27682,7 +27689,7 @@
       <c r="G1080" s="22"/>
       <c r="H1080" s="22"/>
       <c r="I1080" s="23" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="J1080" s="23"/>
       <c r="K1080" s="23"/>
@@ -27690,7 +27697,7 @@
     <row r="1081" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1081" s="9"/>
       <c r="B1081" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1081" s="26"/>
       <c r="D1081" s="22" t="s">
@@ -27705,7 +27712,7 @@
       <c r="G1081" s="22"/>
       <c r="H1081" s="22"/>
       <c r="I1081" s="23" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="J1081" s="23"/>
       <c r="K1081" s="23"/>
@@ -27713,7 +27720,7 @@
     <row r="1082" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1082" s="9"/>
       <c r="B1082" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1082" s="26"/>
       <c r="D1082" s="22" t="s">
@@ -27728,7 +27735,7 @@
       <c r="G1082" s="22"/>
       <c r="H1082" s="22"/>
       <c r="I1082" s="23" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="J1082" s="23"/>
       <c r="K1082" s="23"/>
@@ -27736,7 +27743,7 @@
     <row r="1083" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1083" s="9"/>
       <c r="B1083" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1083" s="26"/>
       <c r="D1083" s="22" t="s">
@@ -27751,7 +27758,7 @@
       <c r="G1083" s="22"/>
       <c r="H1083" s="22"/>
       <c r="I1083" s="23" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="J1083" s="23"/>
       <c r="K1083" s="23"/>
@@ -27759,7 +27766,7 @@
     <row r="1084" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1084" s="9"/>
       <c r="B1084" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1084" s="26"/>
       <c r="D1084" s="22" t="s">
@@ -27774,7 +27781,7 @@
       <c r="G1084" s="22"/>
       <c r="H1084" s="22"/>
       <c r="I1084" s="23" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="J1084" s="23"/>
       <c r="K1084" s="23"/>
@@ -27782,7 +27789,7 @@
     <row r="1085" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1085" s="9"/>
       <c r="B1085" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1085" s="26"/>
       <c r="D1085" s="22" t="s">
@@ -27797,7 +27804,7 @@
       <c r="G1085" s="22"/>
       <c r="H1085" s="22"/>
       <c r="I1085" s="23" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="J1085" s="23"/>
       <c r="K1085" s="23"/>
@@ -27805,7 +27812,7 @@
     <row r="1086" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1086" s="9"/>
       <c r="B1086" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1086" s="22" t="s">
         <v>27</v>
@@ -27822,7 +27829,7 @@
       <c r="G1086" s="22"/>
       <c r="H1086" s="22"/>
       <c r="I1086" s="23" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="J1086" s="23"/>
       <c r="K1086" s="23"/>
@@ -27830,7 +27837,7 @@
     <row r="1087" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1087" s="9"/>
       <c r="B1087" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1087" s="22" t="s">
         <v>27</v>
@@ -27847,7 +27854,7 @@
       <c r="G1087" s="22"/>
       <c r="H1087" s="22"/>
       <c r="I1087" s="23" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="J1087" s="23"/>
       <c r="K1087" s="23"/>
@@ -27855,7 +27862,7 @@
     <row r="1088" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1088" s="9"/>
       <c r="B1088" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1088" s="22" t="s">
         <v>27</v>
@@ -27872,7 +27879,7 @@
       <c r="G1088" s="22"/>
       <c r="H1088" s="22"/>
       <c r="I1088" s="23" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="J1088" s="23"/>
       <c r="K1088" s="23"/>
@@ -27880,7 +27887,7 @@
     <row r="1089" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1089" s="9"/>
       <c r="B1089" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1089" s="26"/>
       <c r="D1089" s="22" t="s">
@@ -27895,7 +27902,7 @@
       <c r="G1089" s="22"/>
       <c r="H1089" s="22"/>
       <c r="I1089" s="23" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="J1089" s="23"/>
       <c r="K1089" s="23"/>
@@ -27903,7 +27910,7 @@
     <row r="1090" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1090" s="9"/>
       <c r="B1090" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1090" s="26"/>
       <c r="D1090" s="22" t="s">
@@ -27916,7 +27923,7 @@
       <c r="G1090" s="22"/>
       <c r="H1090" s="22"/>
       <c r="I1090" s="23" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="J1090" s="23"/>
       <c r="K1090" s="23"/>
@@ -27924,7 +27931,7 @@
     <row r="1091" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1091" s="9"/>
       <c r="B1091" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1091" s="26"/>
       <c r="D1091" s="22" t="s">
@@ -27937,7 +27944,7 @@
       <c r="G1091" s="22"/>
       <c r="H1091" s="22"/>
       <c r="I1091" s="23" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="J1091" s="23"/>
       <c r="K1091" s="23"/>
@@ -27945,7 +27952,7 @@
     <row r="1092" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1092" s="9"/>
       <c r="B1092" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1092" s="26"/>
       <c r="D1092" s="22" t="s">
@@ -27958,7 +27965,7 @@
       <c r="G1092" s="22"/>
       <c r="H1092" s="22"/>
       <c r="I1092" s="23" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="J1092" s="23"/>
       <c r="K1092" s="23"/>
@@ -27966,7 +27973,7 @@
     <row r="1093" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1093" s="9"/>
       <c r="B1093" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1093" s="22" t="s">
         <v>27</v>
@@ -27983,7 +27990,7 @@
       <c r="G1093" s="22"/>
       <c r="H1093" s="22"/>
       <c r="I1093" s="23" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="J1093" s="23"/>
       <c r="K1093" s="23"/>
@@ -27991,7 +27998,7 @@
     <row r="1094" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1094" s="9"/>
       <c r="B1094" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1094" s="22" t="s">
         <v>27</v>
@@ -28008,7 +28015,7 @@
       <c r="G1094" s="22"/>
       <c r="H1094" s="22"/>
       <c r="I1094" s="23" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="J1094" s="23"/>
       <c r="K1094" s="23"/>
@@ -28016,7 +28023,7 @@
     <row r="1095" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1095" s="9"/>
       <c r="B1095" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1095" s="26"/>
       <c r="D1095" s="22" t="s">
@@ -28031,7 +28038,7 @@
       <c r="G1095" s="22"/>
       <c r="H1095" s="22"/>
       <c r="I1095" s="23" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="J1095" s="23"/>
       <c r="K1095" s="23"/>
@@ -28039,7 +28046,7 @@
     <row r="1096" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1096" s="9"/>
       <c r="B1096" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1096" s="26"/>
       <c r="D1096" s="22" t="s">
@@ -28054,7 +28061,7 @@
       <c r="G1096" s="22"/>
       <c r="H1096" s="22"/>
       <c r="I1096" s="23" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="J1096" s="23"/>
       <c r="K1096" s="23"/>
@@ -28062,7 +28069,7 @@
     <row r="1097" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1097" s="9"/>
       <c r="B1097" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1097" s="26"/>
       <c r="D1097" s="22" t="s">
@@ -28077,7 +28084,7 @@
       <c r="G1097" s="22"/>
       <c r="H1097" s="22"/>
       <c r="I1097" s="23" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="J1097" s="23"/>
       <c r="K1097" s="23"/>
@@ -28085,7 +28092,7 @@
     <row r="1098" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1098" s="9"/>
       <c r="B1098" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1098" s="26"/>
       <c r="D1098" s="22" t="s">
@@ -28100,7 +28107,7 @@
       <c r="G1098" s="22"/>
       <c r="H1098" s="22"/>
       <c r="I1098" s="23" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="J1098" s="23"/>
       <c r="K1098" s="23"/>
@@ -28108,7 +28115,7 @@
     <row r="1099" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1099" s="9"/>
       <c r="B1099" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1099" s="26"/>
       <c r="D1099" s="22" t="s">
@@ -28123,7 +28130,7 @@
       <c r="G1099" s="22"/>
       <c r="H1099" s="22"/>
       <c r="I1099" s="23" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="J1099" s="23"/>
       <c r="K1099" s="23"/>
@@ -28131,7 +28138,7 @@
     <row r="1100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1100" s="9"/>
       <c r="B1100" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1100" s="26"/>
       <c r="D1100" s="22" t="s">
@@ -28146,7 +28153,7 @@
       <c r="G1100" s="22"/>
       <c r="H1100" s="22"/>
       <c r="I1100" s="23" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="J1100" s="23"/>
       <c r="K1100" s="23"/>
@@ -28154,7 +28161,7 @@
     <row r="1101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1101" s="9"/>
       <c r="B1101" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1101" s="22" t="s">
         <v>27</v>
@@ -28171,7 +28178,7 @@
       <c r="G1101" s="22"/>
       <c r="H1101" s="22"/>
       <c r="I1101" s="23" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="J1101" s="23"/>
       <c r="K1101" s="23"/>
@@ -28179,7 +28186,7 @@
     <row r="1102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1102" s="9"/>
       <c r="B1102" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1102" s="22" t="s">
         <v>27</v>
@@ -28196,7 +28203,7 @@
       <c r="G1102" s="22"/>
       <c r="H1102" s="22"/>
       <c r="I1102" s="23" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="J1102" s="23"/>
       <c r="K1102" s="23"/>
@@ -28204,7 +28211,7 @@
     <row r="1103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1103" s="9"/>
       <c r="B1103" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1103" s="26"/>
       <c r="D1103" s="22" t="s">
@@ -28219,7 +28226,7 @@
       <c r="G1103" s="22"/>
       <c r="H1103" s="22"/>
       <c r="I1103" s="23" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="J1103" s="23"/>
       <c r="K1103" s="23"/>
@@ -28227,7 +28234,7 @@
     <row r="1104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1104" s="9"/>
       <c r="B1104" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1104" s="22" t="s">
         <v>27</v>
@@ -28244,7 +28251,7 @@
       <c r="G1104" s="22"/>
       <c r="H1104" s="22"/>
       <c r="I1104" s="23" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="J1104" s="23"/>
       <c r="K1104" s="23"/>
@@ -28252,7 +28259,7 @@
     <row r="1105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1105" s="9"/>
       <c r="B1105" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1105" s="22" t="s">
         <v>27</v>
@@ -28269,7 +28276,7 @@
       <c r="G1105" s="22"/>
       <c r="H1105" s="22"/>
       <c r="I1105" s="23" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="J1105" s="23"/>
       <c r="K1105" s="23"/>
@@ -28277,7 +28284,7 @@
     <row r="1106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1106" s="9"/>
       <c r="B1106" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1106" s="26"/>
       <c r="D1106" s="22" t="s">
@@ -28292,7 +28299,7 @@
       <c r="G1106" s="22"/>
       <c r="H1106" s="22"/>
       <c r="I1106" s="23" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="J1106" s="23"/>
       <c r="K1106" s="23"/>
@@ -28300,7 +28307,7 @@
     <row r="1107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1107" s="9"/>
       <c r="B1107" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1107" s="22" t="s">
         <v>27</v>
@@ -28317,7 +28324,7 @@
       <c r="G1107" s="22"/>
       <c r="H1107" s="22"/>
       <c r="I1107" s="23" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="J1107" s="23"/>
       <c r="K1107" s="23"/>
@@ -28325,7 +28332,7 @@
     <row r="1108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1108" s="9"/>
       <c r="B1108" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1108" s="26"/>
       <c r="D1108" s="22" t="s">
@@ -28340,7 +28347,7 @@
       <c r="G1108" s="22"/>
       <c r="H1108" s="22"/>
       <c r="I1108" s="23" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="J1108" s="23"/>
       <c r="K1108" s="23"/>
@@ -28348,7 +28355,7 @@
     <row r="1109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1109" s="9"/>
       <c r="B1109" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1109" s="22" t="s">
         <v>27</v>
@@ -28365,7 +28372,7 @@
       <c r="G1109" s="22"/>
       <c r="H1109" s="22"/>
       <c r="I1109" s="23" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="J1109" s="23"/>
       <c r="K1109" s="23"/>
@@ -28373,7 +28380,7 @@
     <row r="1110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1110" s="9"/>
       <c r="B1110" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1110" s="22" t="s">
         <v>27</v>
@@ -28390,7 +28397,7 @@
       <c r="G1110" s="22"/>
       <c r="H1110" s="22"/>
       <c r="I1110" s="23" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="J1110" s="23"/>
       <c r="K1110" s="23"/>
@@ -28398,7 +28405,7 @@
     <row r="1111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1111" s="9"/>
       <c r="B1111" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1111" s="22" t="s">
         <v>27</v>
@@ -28415,7 +28422,7 @@
       <c r="G1111" s="22"/>
       <c r="H1111" s="22"/>
       <c r="I1111" s="23" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="J1111" s="23"/>
       <c r="K1111" s="23"/>
@@ -28423,7 +28430,7 @@
     <row r="1112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1112" s="9"/>
       <c r="B1112" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1112" s="22" t="s">
         <v>27</v>
@@ -28440,7 +28447,7 @@
       <c r="G1112" s="22"/>
       <c r="H1112" s="22"/>
       <c r="I1112" s="23" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="J1112" s="23"/>
       <c r="K1112" s="23"/>
@@ -28448,7 +28455,7 @@
     <row r="1113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1113" s="9"/>
       <c r="B1113" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1113" s="22" t="s">
         <v>27</v>
@@ -28465,7 +28472,7 @@
       <c r="G1113" s="22"/>
       <c r="H1113" s="22"/>
       <c r="I1113" s="23" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="J1113" s="23"/>
       <c r="K1113" s="23"/>
@@ -28473,7 +28480,7 @@
     <row r="1114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1114" s="9"/>
       <c r="B1114" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1114" s="26"/>
       <c r="D1114" s="22" t="s">
@@ -28488,7 +28495,7 @@
       <c r="G1114" s="22"/>
       <c r="H1114" s="22"/>
       <c r="I1114" s="23" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="J1114" s="23"/>
       <c r="K1114" s="23"/>
@@ -28496,7 +28503,7 @@
     <row r="1115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1115" s="9"/>
       <c r="B1115" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1115" s="22" t="s">
         <v>27</v>
@@ -28513,7 +28520,7 @@
       <c r="G1115" s="22"/>
       <c r="H1115" s="22"/>
       <c r="I1115" s="23" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="J1115" s="23"/>
       <c r="K1115" s="23"/>
@@ -28521,7 +28528,7 @@
     <row r="1116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1116" s="9"/>
       <c r="B1116" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1116" s="22" t="s">
         <v>27</v>
@@ -28538,7 +28545,7 @@
       <c r="G1116" s="22"/>
       <c r="H1116" s="22"/>
       <c r="I1116" s="23" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="J1116" s="23"/>
       <c r="K1116" s="23"/>
@@ -28546,7 +28553,7 @@
     <row r="1117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1117" s="9"/>
       <c r="B1117" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1117" s="22" t="s">
         <v>27</v>
@@ -28563,7 +28570,7 @@
       <c r="G1117" s="22"/>
       <c r="H1117" s="22"/>
       <c r="I1117" s="23" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="J1117" s="23"/>
       <c r="K1117" s="23"/>
@@ -28571,7 +28578,7 @@
     <row r="1118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1118" s="9"/>
       <c r="B1118" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1118" s="22" t="s">
         <v>27</v>
@@ -28588,7 +28595,7 @@
       <c r="G1118" s="22"/>
       <c r="H1118" s="22"/>
       <c r="I1118" s="23" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="J1118" s="23"/>
       <c r="K1118" s="23"/>
@@ -28596,7 +28603,7 @@
     <row r="1119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1119" s="9"/>
       <c r="B1119" s="28" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C1119" s="26"/>
       <c r="D1119" s="22" t="s">
@@ -28609,7 +28616,7 @@
       <c r="G1119" s="22"/>
       <c r="H1119" s="22"/>
       <c r="I1119" s="23" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="J1119" s="23"/>
       <c r="K1119" s="23" t="s">
@@ -28619,7 +28626,7 @@
     <row r="1120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1120" s="9"/>
       <c r="B1120" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1120" s="22" t="s">
         <v>27</v>
@@ -28636,7 +28643,7 @@
       <c r="G1120" s="22"/>
       <c r="H1120" s="22"/>
       <c r="I1120" s="23" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="J1120" s="23"/>
       <c r="K1120" s="23"/>
@@ -28644,7 +28651,7 @@
     <row r="1121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1121" s="9"/>
       <c r="B1121" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1121" s="22" t="s">
         <v>27</v>
@@ -28661,7 +28668,7 @@
       <c r="G1121" s="22"/>
       <c r="H1121" s="22"/>
       <c r="I1121" s="23" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="J1121" s="23"/>
       <c r="K1121" s="23"/>
@@ -28669,7 +28676,7 @@
     <row r="1122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1122" s="9"/>
       <c r="B1122" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1122" s="22" t="s">
         <v>27</v>
@@ -28686,7 +28693,7 @@
       <c r="G1122" s="22"/>
       <c r="H1122" s="22"/>
       <c r="I1122" s="23" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="J1122" s="23"/>
       <c r="K1122" s="23"/>
@@ -28694,7 +28701,7 @@
     <row r="1123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1123" s="9"/>
       <c r="B1123" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1123" s="22" t="s">
         <v>27</v>
@@ -28711,7 +28718,7 @@
       <c r="G1123" s="22"/>
       <c r="H1123" s="22"/>
       <c r="I1123" s="23" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="J1123" s="23"/>
       <c r="K1123" s="23"/>
@@ -28719,7 +28726,7 @@
     <row r="1124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1124" s="9"/>
       <c r="B1124" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1124" s="22" t="s">
         <v>27</v>
@@ -28736,7 +28743,7 @@
       <c r="G1124" s="22"/>
       <c r="H1124" s="22"/>
       <c r="I1124" s="23" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="J1124" s="23"/>
       <c r="K1124" s="23"/>
@@ -28744,7 +28751,7 @@
     <row r="1125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1125" s="9"/>
       <c r="B1125" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1125" s="22" t="s">
         <v>27</v>
@@ -28761,7 +28768,7 @@
       <c r="G1125" s="22"/>
       <c r="H1125" s="22"/>
       <c r="I1125" s="23" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="J1125" s="23"/>
       <c r="K1125" s="23"/>
@@ -28769,7 +28776,7 @@
     <row r="1126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1126" s="9"/>
       <c r="B1126" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1126" s="22" t="s">
         <v>27</v>
@@ -28786,7 +28793,7 @@
       <c r="G1126" s="22"/>
       <c r="H1126" s="22"/>
       <c r="I1126" s="23" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="J1126" s="23"/>
       <c r="K1126" s="23"/>
@@ -28794,7 +28801,7 @@
     <row r="1127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1127" s="9"/>
       <c r="B1127" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1127" s="26"/>
       <c r="D1127" s="22" t="s">
@@ -28809,14 +28816,14 @@
       <c r="G1127" s="22"/>
       <c r="H1127" s="22"/>
       <c r="I1127" s="23" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="J1127" s="23"/>
       <c r="K1127" s="23"/>
     </row>
     <row r="1128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1128" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1128" s="26"/>
       <c r="D1128" s="22" t="s">
@@ -28831,14 +28838,14 @@
       <c r="G1128" s="22"/>
       <c r="H1128" s="22"/>
       <c r="I1128" s="23" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="J1128" s="23"/>
       <c r="K1128" s="23"/>
     </row>
     <row r="1129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1129" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1129" s="26"/>
       <c r="D1129" s="22" t="s">
@@ -28853,14 +28860,14 @@
       <c r="G1129" s="22"/>
       <c r="H1129" s="22"/>
       <c r="I1129" s="23" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="J1129" s="23"/>
       <c r="K1129" s="23"/>
     </row>
     <row r="1130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1130" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1130" s="22" t="s">
         <v>27</v>
@@ -28877,14 +28884,14 @@
       <c r="G1130" s="22"/>
       <c r="H1130" s="22"/>
       <c r="I1130" s="23" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="J1130" s="23"/>
       <c r="K1130" s="23"/>
     </row>
     <row r="1131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1131" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1131" s="26"/>
       <c r="D1131" s="22" t="s">
@@ -28897,14 +28904,14 @@
       <c r="G1131" s="22"/>
       <c r="H1131" s="22"/>
       <c r="I1131" s="23" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="J1131" s="23"/>
       <c r="K1131" s="23"/>
     </row>
     <row r="1132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1132" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1132" s="26"/>
       <c r="D1132" s="22" t="s">
@@ -28917,14 +28924,14 @@
       <c r="G1132" s="22"/>
       <c r="H1132" s="22"/>
       <c r="I1132" s="23" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="J1132" s="23"/>
       <c r="K1132" s="23"/>
     </row>
     <row r="1133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1133" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1133" s="26"/>
       <c r="D1133" s="22" t="s">
@@ -28937,14 +28944,14 @@
       <c r="G1133" s="22"/>
       <c r="H1133" s="22"/>
       <c r="I1133" s="23" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="J1133" s="23"/>
       <c r="K1133" s="23"/>
     </row>
     <row r="1134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1134" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1134" s="22" t="s">
         <v>27</v>
@@ -28961,14 +28968,14 @@
       <c r="G1134" s="22"/>
       <c r="H1134" s="22"/>
       <c r="I1134" s="23" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="J1134" s="23"/>
       <c r="K1134" s="23"/>
     </row>
     <row r="1135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1135" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1135" s="22" t="s">
         <v>27</v>
@@ -28980,19 +28987,19 @@
         <v>27</v>
       </c>
       <c r="F1135" s="22" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="G1135" s="22"/>
       <c r="H1135" s="22"/>
       <c r="I1135" s="23" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="J1135" s="23"/>
       <c r="K1135" s="23"/>
     </row>
     <row r="1136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1136" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1136" s="26"/>
       <c r="D1136" s="22" t="s">
@@ -29002,16 +29009,16 @@
         <v>27</v>
       </c>
       <c r="F1136" s="22" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="G1136" s="22"/>
       <c r="H1136" s="22"/>
       <c r="I1136" s="23" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="J1136" s="23"/>
       <c r="K1136" s="23" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29029,16 +29036,16 @@
       <c r="G1137" s="28"/>
       <c r="H1137" s="28"/>
       <c r="I1137" s="29" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="J1137" s="29"/>
       <c r="K1137" s="29" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="1138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1138" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C1138" s="26"/>
       <c r="D1138" s="22" t="s">
@@ -29048,16 +29055,16 @@
         <v>27</v>
       </c>
       <c r="F1138" s="22" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="G1138" s="22"/>
       <c r="H1138" s="22"/>
       <c r="I1138" s="23" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="J1138" s="23"/>
       <c r="K1138" s="23" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29075,11 +29082,11 @@
       <c r="G1139" s="28"/>
       <c r="H1139" s="28"/>
       <c r="I1139" s="29" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="J1139" s="29"/>
       <c r="K1139" s="29" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added macros for enhanced menu items.  Optimized a few VI
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5006" uniqueCount="1169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5043" uniqueCount="1169">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -3978,8 +3978,8 @@
   </sheetPr>
   <dimension ref="A1:Q1142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A423" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B435" activeCellId="0" sqref="B435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="F9" s="13" t="n">
         <f aca="false">COUNTIF(F18:F1469,"S")+COUNTIF(F18:F1469,"I")+COUNTIF(F18:F1469,"X")+COUNTIF(F18:F1469,"SI")+COUNTIF(F18:F1469,"IS")+COUNTIF(F18:F1469,"N/A")</f>
-        <v>232</v>
+        <v>269</v>
       </c>
       <c r="G9" s="13" t="n">
         <f aca="false">COUNTIF(G18:G1469,"S")+COUNTIF(G18:G1469,"I")+COUNTIF(G18:G1469,"X")+COUNTIF(G18:G1469,"SI")+COUNTIF(G18:G1469,"IS")+COUNTIF(G18:G1469,"N/A")</f>
@@ -4143,7 +4143,7 @@
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.310160427807487</v>
+        <v>0.359625668449198</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4664,7 +4664,9 @@
       <c r="E37" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="22"/>
+      <c r="F37" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G37" s="22"/>
       <c r="H37" s="25" t="s">
         <v>27</v>
@@ -4794,7 +4796,9 @@
       <c r="E43" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F43" s="22"/>
+      <c r="F43" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G43" s="22"/>
       <c r="H43" s="22"/>
       <c r="I43" s="23" t="s">
@@ -4817,7 +4821,9 @@
       <c r="E44" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F44" s="22"/>
+      <c r="F44" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G44" s="22"/>
       <c r="H44" s="22"/>
       <c r="I44" s="23" t="s">
@@ -4840,7 +4846,9 @@
       <c r="E45" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="22"/>
+      <c r="F45" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G45" s="22"/>
       <c r="H45" s="25" t="s">
         <v>27</v>
@@ -4890,7 +4898,9 @@
       <c r="E47" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F47" s="22"/>
+      <c r="F47" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G47" s="22"/>
       <c r="H47" s="22"/>
       <c r="I47" s="23" t="s">
@@ -4911,7 +4921,9 @@
       <c r="E48" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F48" s="22"/>
+      <c r="F48" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G48" s="22"/>
       <c r="H48" s="22"/>
       <c r="I48" s="23" t="s">
@@ -4932,7 +4944,9 @@
       <c r="E49" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F49" s="22"/>
+      <c r="F49" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G49" s="22"/>
       <c r="H49" s="22"/>
       <c r="I49" s="23" t="s">
@@ -5629,7 +5643,9 @@
       <c r="E84" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F84" s="22"/>
+      <c r="F84" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G84" s="22"/>
       <c r="H84" s="22"/>
       <c r="I84" s="23" t="s">
@@ -10006,7 +10022,9 @@
       <c r="E278" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F278" s="26"/>
+      <c r="F278" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G278" s="22"/>
       <c r="H278" s="22"/>
       <c r="I278" s="23" t="s">
@@ -16879,7 +16897,9 @@
       <c r="E609" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F609" s="26"/>
+      <c r="F609" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G609" s="22"/>
       <c r="H609" s="22"/>
       <c r="I609" s="46" t="s">
@@ -16903,7 +16923,9 @@
       <c r="E610" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F610" s="26"/>
+      <c r="F610" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G610" s="22"/>
       <c r="H610" s="22"/>
       <c r="I610" s="46" t="s">
@@ -16927,7 +16949,9 @@
       <c r="E611" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F611" s="26"/>
+      <c r="F611" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G611" s="22"/>
       <c r="H611" s="22"/>
       <c r="I611" s="46" t="s">
@@ -16951,7 +16975,9 @@
       <c r="E612" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F612" s="26"/>
+      <c r="F612" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G612" s="22"/>
       <c r="H612" s="22"/>
       <c r="I612" s="46" t="s">
@@ -16975,7 +17001,9 @@
       <c r="E613" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F613" s="26"/>
+      <c r="F613" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G613" s="22"/>
       <c r="H613" s="22"/>
       <c r="I613" s="46" t="s">
@@ -16999,7 +17027,9 @@
       <c r="E614" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F614" s="26"/>
+      <c r="F614" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G614" s="22"/>
       <c r="H614" s="22"/>
       <c r="I614" s="46" t="s">
@@ -17023,7 +17053,9 @@
       <c r="E615" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F615" s="26"/>
+      <c r="F615" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G615" s="22"/>
       <c r="H615" s="22"/>
       <c r="I615" s="46" t="s">
@@ -17047,7 +17079,9 @@
       <c r="E616" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F616" s="26"/>
+      <c r="F616" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G616" s="22"/>
       <c r="H616" s="22"/>
       <c r="I616" s="46" t="s">
@@ -17071,7 +17105,9 @@
       <c r="E617" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F617" s="26"/>
+      <c r="F617" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G617" s="22"/>
       <c r="H617" s="22"/>
       <c r="I617" s="46" t="s">
@@ -17095,7 +17131,9 @@
       <c r="E618" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F618" s="26"/>
+      <c r="F618" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G618" s="22"/>
       <c r="H618" s="22"/>
       <c r="I618" s="46" t="s">
@@ -17119,7 +17157,9 @@
       <c r="E619" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F619" s="26"/>
+      <c r="F619" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G619" s="22"/>
       <c r="H619" s="22"/>
       <c r="I619" s="46" t="s">
@@ -17143,7 +17183,9 @@
       <c r="E620" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F620" s="26"/>
+      <c r="F620" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G620" s="22"/>
       <c r="H620" s="22"/>
       <c r="I620" s="46" t="s">
@@ -17165,7 +17207,9 @@
       </c>
       <c r="D621" s="22"/>
       <c r="E621" s="26"/>
-      <c r="F621" s="26"/>
+      <c r="F621" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G621" s="22"/>
       <c r="H621" s="22"/>
       <c r="I621" s="46" t="s">
@@ -17189,7 +17233,9 @@
       <c r="E622" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F622" s="26"/>
+      <c r="F622" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G622" s="22"/>
       <c r="H622" s="22"/>
       <c r="I622" s="46" t="s">
@@ -24837,7 +24883,9 @@
       <c r="E948" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F948" s="26"/>
+      <c r="F948" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G948" s="22"/>
       <c r="H948" s="22"/>
       <c r="I948" s="23" t="s">
@@ -24858,7 +24906,9 @@
       <c r="E949" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F949" s="26"/>
+      <c r="F949" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G949" s="22"/>
       <c r="H949" s="22"/>
       <c r="I949" s="23" t="s">
@@ -25412,7 +25462,9 @@
       <c r="E973" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F973" s="26"/>
+      <c r="F973" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G973" s="22"/>
       <c r="H973" s="22"/>
       <c r="I973" s="23" t="s">
@@ -25435,7 +25487,9 @@
       <c r="E974" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F974" s="26"/>
+      <c r="F974" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G974" s="22"/>
       <c r="H974" s="22"/>
       <c r="I974" s="23" t="s">
@@ -25458,7 +25512,9 @@
       <c r="E975" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F975" s="26"/>
+      <c r="F975" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G975" s="22"/>
       <c r="H975" s="22"/>
       <c r="I975" s="23" t="s">
@@ -25558,7 +25614,9 @@
       <c r="E979" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F979" s="26"/>
+      <c r="F979" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G979" s="22"/>
       <c r="H979" s="22"/>
       <c r="I979" s="23" t="s">
@@ -25581,7 +25639,9 @@
       <c r="E980" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F980" s="26"/>
+      <c r="F980" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G980" s="22"/>
       <c r="H980" s="22"/>
       <c r="I980" s="23" t="s">
@@ -25604,7 +25664,9 @@
       <c r="E981" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F981" s="26"/>
+      <c r="F981" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G981" s="22"/>
       <c r="H981" s="22"/>
       <c r="I981" s="23" t="s">
@@ -25627,7 +25689,9 @@
       <c r="E982" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F982" s="26"/>
+      <c r="F982" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G982" s="22"/>
       <c r="H982" s="22"/>
       <c r="I982" s="23" t="s">
@@ -25650,7 +25714,9 @@
       <c r="E983" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F983" s="26"/>
+      <c r="F983" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G983" s="22"/>
       <c r="H983" s="22"/>
       <c r="I983" s="23" t="s">
@@ -25673,7 +25739,9 @@
       <c r="E984" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F984" s="26"/>
+      <c r="F984" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G984" s="22"/>
       <c r="H984" s="22"/>
       <c r="I984" s="23" t="s">
@@ -25696,7 +25764,9 @@
       <c r="E985" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F985" s="26"/>
+      <c r="F985" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G985" s="22"/>
       <c r="H985" s="22"/>
       <c r="I985" s="23" t="s">
@@ -25719,7 +25789,9 @@
       <c r="E986" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F986" s="26"/>
+      <c r="F986" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G986" s="22"/>
       <c r="H986" s="22"/>
       <c r="I986" s="23" t="s">
@@ -25733,10 +25805,10 @@
     </row>
     <row r="987" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B987" s="26"/>
-      <c r="C987" s="26"/>
+      <c r="C987" s="22"/>
       <c r="D987" s="22"/>
       <c r="E987" s="22"/>
-      <c r="F987" s="26"/>
+      <c r="F987" s="22"/>
       <c r="G987" s="22"/>
       <c r="H987" s="22"/>
       <c r="I987" s="23" t="s">
@@ -25750,10 +25822,10 @@
     </row>
     <row r="988" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B988" s="26"/>
-      <c r="C988" s="26"/>
+      <c r="C988" s="22"/>
       <c r="D988" s="22"/>
       <c r="E988" s="22"/>
-      <c r="F988" s="26"/>
+      <c r="F988" s="22"/>
       <c r="G988" s="22"/>
       <c r="H988" s="22"/>
       <c r="I988" s="23" t="s">
@@ -25778,7 +25850,9 @@
       <c r="E989" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F989" s="26"/>
+      <c r="F989" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G989" s="22"/>
       <c r="H989" s="22"/>
       <c r="I989" s="23" t="s">

</xml_diff>

<commit_message>
Continued work on menus.   Also optimized some VI.
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5043" uniqueCount="1169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5082" uniqueCount="1169">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -3978,8 +3978,8 @@
   </sheetPr>
   <dimension ref="A1:Q1142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A423" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B435" activeCellId="0" sqref="B435"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="F9" s="13" t="n">
         <f aca="false">COUNTIF(F18:F1469,"S")+COUNTIF(F18:F1469,"I")+COUNTIF(F18:F1469,"X")+COUNTIF(F18:F1469,"SI")+COUNTIF(F18:F1469,"IS")+COUNTIF(F18:F1469,"N/A")</f>
-        <v>269</v>
+        <v>308</v>
       </c>
       <c r="G9" s="13" t="n">
         <f aca="false">COUNTIF(G18:G1469,"S")+COUNTIF(G18:G1469,"I")+COUNTIF(G18:G1469,"X")+COUNTIF(G18:G1469,"SI")+COUNTIF(G18:G1469,"IS")+COUNTIF(G18:G1469,"N/A")</f>
@@ -4143,7 +4143,7 @@
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.359625668449198</v>
+        <v>0.411764705882353</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22368,7 +22368,9 @@
       <c r="E847" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F847" s="26"/>
+      <c r="F847" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G847" s="22"/>
       <c r="H847" s="22"/>
       <c r="I847" s="23" t="s">
@@ -22395,7 +22397,9 @@
       <c r="E848" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F848" s="26"/>
+      <c r="F848" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G848" s="22"/>
       <c r="H848" s="22"/>
       <c r="I848" s="23" t="s">
@@ -24986,7 +24990,9 @@
       <c r="E952" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F952" s="26"/>
+      <c r="F952" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G952" s="22"/>
       <c r="H952" s="22"/>
       <c r="I952" s="23" t="s">
@@ -25009,7 +25015,9 @@
       <c r="E953" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F953" s="26"/>
+      <c r="F953" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G953" s="22"/>
       <c r="H953" s="22"/>
       <c r="I953" s="23" t="s">
@@ -25032,7 +25040,9 @@
       <c r="E954" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F954" s="26"/>
+      <c r="F954" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G954" s="22"/>
       <c r="H954" s="22"/>
       <c r="I954" s="23" t="s">
@@ -25055,7 +25065,9 @@
       <c r="E955" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F955" s="26"/>
+      <c r="F955" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G955" s="22"/>
       <c r="H955" s="22"/>
       <c r="I955" s="23" t="s">
@@ -25078,7 +25090,9 @@
       <c r="E956" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F956" s="26"/>
+      <c r="F956" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G956" s="22"/>
       <c r="H956" s="22"/>
       <c r="I956" s="23" t="s">
@@ -25101,7 +25115,9 @@
       <c r="E957" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F957" s="26"/>
+      <c r="F957" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G957" s="22"/>
       <c r="H957" s="22"/>
       <c r="I957" s="23" t="s">
@@ -25124,7 +25140,9 @@
       <c r="E958" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F958" s="26"/>
+      <c r="F958" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G958" s="22"/>
       <c r="H958" s="22"/>
       <c r="I958" s="23" t="s">
@@ -25147,7 +25165,9 @@
       <c r="E959" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F959" s="26"/>
+      <c r="F959" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G959" s="22"/>
       <c r="H959" s="22"/>
       <c r="I959" s="23" t="s">
@@ -25168,7 +25188,9 @@
       <c r="E960" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F960" s="26"/>
+      <c r="F960" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G960" s="22"/>
       <c r="H960" s="22"/>
       <c r="I960" s="23" t="s">
@@ -25191,7 +25213,9 @@
       <c r="E961" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F961" s="26"/>
+      <c r="F961" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G961" s="22"/>
       <c r="H961" s="22"/>
       <c r="I961" s="23" t="s">
@@ -25214,7 +25238,9 @@
       <c r="E962" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F962" s="26"/>
+      <c r="F962" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G962" s="22"/>
       <c r="H962" s="22"/>
       <c r="I962" s="23" t="s">
@@ -25237,7 +25263,9 @@
       <c r="E963" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F963" s="26"/>
+      <c r="F963" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G963" s="22"/>
       <c r="H963" s="22"/>
       <c r="I963" s="23" t="s">
@@ -25260,7 +25288,9 @@
       <c r="E964" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F964" s="26"/>
+      <c r="F964" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G964" s="22"/>
       <c r="H964" s="22"/>
       <c r="I964" s="23" t="s">
@@ -25283,7 +25313,9 @@
       <c r="E965" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F965" s="26"/>
+      <c r="F965" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G965" s="22"/>
       <c r="H965" s="22"/>
       <c r="I965" s="23" t="s">
@@ -25306,7 +25338,9 @@
       <c r="E966" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F966" s="26"/>
+      <c r="F966" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G966" s="22"/>
       <c r="H966" s="22"/>
       <c r="I966" s="23" t="s">
@@ -25329,7 +25363,9 @@
       <c r="E967" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F967" s="26"/>
+      <c r="F967" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G967" s="22"/>
       <c r="H967" s="22"/>
       <c r="I967" s="23" t="s">
@@ -25352,7 +25388,9 @@
       <c r="E968" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F968" s="26"/>
+      <c r="F968" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G968" s="22"/>
       <c r="H968" s="22"/>
       <c r="I968" s="23" t="s">
@@ -26031,7 +26069,9 @@
       <c r="E997" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F997" s="26"/>
+      <c r="F997" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G997" s="22" t="s">
         <v>27</v>
       </c>
@@ -26060,7 +26100,9 @@
       <c r="E998" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F998" s="26"/>
+      <c r="F998" s="24" t="s">
+        <v>27</v>
+      </c>
       <c r="G998" s="22"/>
       <c r="H998" s="22"/>
       <c r="I998" s="23" t="s">
@@ -26085,7 +26127,9 @@
       <c r="E999" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F999" s="26"/>
+      <c r="F999" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G999" s="22" t="s">
         <v>27</v>
       </c>
@@ -26114,7 +26158,9 @@
       <c r="E1000" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1000" s="26"/>
+      <c r="F1000" s="24" t="s">
+        <v>27</v>
+      </c>
       <c r="G1000" s="22"/>
       <c r="H1000" s="22"/>
       <c r="I1000" s="23" t="s">
@@ -26139,7 +26185,9 @@
       <c r="E1001" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1001" s="26"/>
+      <c r="F1001" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G1001" s="22" t="s">
         <v>27</v>
       </c>
@@ -26168,7 +26216,9 @@
       <c r="E1002" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1002" s="26"/>
+      <c r="F1002" s="24" t="s">
+        <v>27</v>
+      </c>
       <c r="G1002" s="22"/>
       <c r="H1002" s="22"/>
       <c r="I1002" s="23" t="s">
@@ -26274,7 +26324,9 @@
       <c r="E1006" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1006" s="26"/>
+      <c r="F1006" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1006" s="22"/>
       <c r="H1006" s="22"/>
       <c r="I1006" s="23" t="s">
@@ -26299,7 +26351,9 @@
       <c r="E1007" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1007" s="26"/>
+      <c r="F1007" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1007" s="22"/>
       <c r="H1007" s="22"/>
       <c r="I1007" s="23" t="s">
@@ -26324,7 +26378,9 @@
       <c r="E1008" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1008" s="26"/>
+      <c r="F1008" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1008" s="22"/>
       <c r="H1008" s="22"/>
       <c r="I1008" s="23" t="s">
@@ -26349,7 +26405,9 @@
       <c r="E1009" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1009" s="26"/>
+      <c r="F1009" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1009" s="22"/>
       <c r="H1009" s="22"/>
       <c r="I1009" s="23" t="s">
@@ -26374,7 +26432,9 @@
       <c r="E1010" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1010" s="26"/>
+      <c r="F1010" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1010" s="22"/>
       <c r="H1010" s="22"/>
       <c r="I1010" s="23" t="s">
@@ -26476,7 +26536,9 @@
       <c r="E1014" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1014" s="26"/>
+      <c r="F1014" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G1014" s="22"/>
       <c r="H1014" s="22"/>
       <c r="I1014" s="23" t="s">
@@ -26499,7 +26561,9 @@
       <c r="E1015" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1015" s="26"/>
+      <c r="F1015" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1015" s="22"/>
       <c r="H1015" s="22"/>
       <c r="I1015" s="23" t="s">
@@ -26522,7 +26586,9 @@
       <c r="E1016" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1016" s="26"/>
+      <c r="F1016" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1016" s="22"/>
       <c r="H1016" s="22"/>
       <c r="I1016" s="23" t="s">
@@ -26545,7 +26611,9 @@
       <c r="E1017" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1017" s="26"/>
+      <c r="F1017" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1017" s="22"/>
       <c r="H1017" s="22"/>
       <c r="I1017" s="23" t="s">
@@ -26568,7 +26636,9 @@
       <c r="E1018" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1018" s="26"/>
+      <c r="F1018" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1018" s="22"/>
       <c r="H1018" s="22"/>
       <c r="I1018" s="23" t="s">
@@ -26591,7 +26661,9 @@
       <c r="E1019" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1019" s="26"/>
+      <c r="F1019" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1019" s="22"/>
       <c r="H1019" s="22"/>
       <c r="I1019" s="23" t="s">
@@ -26614,7 +26686,9 @@
       <c r="E1020" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1020" s="26"/>
+      <c r="F1020" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G1020" s="22"/>
       <c r="H1020" s="22"/>
       <c r="I1020" s="23" t="s">
@@ -26637,7 +26711,9 @@
       <c r="E1021" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1021" s="26"/>
+      <c r="F1021" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G1021" s="22"/>
       <c r="H1021" s="22"/>
       <c r="I1021" s="23" t="s">
@@ -26660,7 +26736,9 @@
       <c r="E1022" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1022" s="26"/>
+      <c r="F1022" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G1022" s="22"/>
       <c r="H1022" s="22"/>
       <c r="I1022" s="23" t="s">

</xml_diff>

<commit_message>
Continued work on documentation
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5206" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5216" uniqueCount="1190">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -4041,8 +4041,8 @@
   </sheetPr>
   <dimension ref="A1:Q1160"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A409" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I418" activeCellId="0" sqref="I418"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">COUNTIF(C18:C1487,"X")</f>
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="D9" s="13" t="n">
         <f aca="false">COUNTIF(D18:D1487,"X")</f>
@@ -4181,7 +4181,7 @@
       </c>
       <c r="I9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.843832020997375</v>
+        <v>0.856955380577428</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23747,7 +23747,9 @@
       <c r="B897" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C897" s="26"/>
+      <c r="C897" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D897" s="22"/>
       <c r="E897" s="22" t="s">
         <v>27</v>
@@ -23772,7 +23774,9 @@
       <c r="B898" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C898" s="26"/>
+      <c r="C898" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D898" s="22"/>
       <c r="E898" s="22" t="s">
         <v>27</v>
@@ -23796,7 +23800,9 @@
       <c r="B899" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C899" s="26"/>
+      <c r="C899" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D899" s="22"/>
       <c r="E899" s="22" t="s">
         <v>27</v>
@@ -23820,7 +23826,9 @@
       <c r="B900" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C900" s="26"/>
+      <c r="C900" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D900" s="22"/>
       <c r="E900" s="22" t="s">
         <v>27</v>
@@ -23868,7 +23876,9 @@
       <c r="B902" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C902" s="26"/>
+      <c r="C902" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D902" s="22"/>
       <c r="E902" s="22" t="s">
         <v>27</v>
@@ -23892,7 +23902,9 @@
       <c r="B903" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C903" s="26"/>
+      <c r="C903" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D903" s="22"/>
       <c r="E903" s="22" t="s">
         <v>27</v>
@@ -23916,7 +23928,9 @@
       <c r="B904" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C904" s="26"/>
+      <c r="C904" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D904" s="22"/>
       <c r="E904" s="22" t="s">
         <v>27</v>
@@ -23940,7 +23954,9 @@
       <c r="B905" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C905" s="26"/>
+      <c r="C905" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D905" s="22"/>
       <c r="E905" s="22" t="s">
         <v>27</v>
@@ -23992,7 +24008,9 @@
       <c r="B907" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C907" s="26"/>
+      <c r="C907" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D907" s="22"/>
       <c r="E907" s="22" t="s">
         <v>27</v>
@@ -24016,7 +24034,9 @@
       <c r="B908" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C908" s="26"/>
+      <c r="C908" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D908" s="22"/>
       <c r="E908" s="22" t="s">
         <v>27</v>
@@ -24064,10 +24084,10 @@
     </row>
     <row r="910" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B910" s="26"/>
-      <c r="C910" s="26"/>
+      <c r="C910" s="22"/>
       <c r="D910" s="22"/>
-      <c r="E910" s="26"/>
-      <c r="F910" s="26"/>
+      <c r="E910" s="22"/>
+      <c r="F910" s="22"/>
       <c r="G910" s="22"/>
       <c r="H910" s="22"/>
       <c r="I910" s="23" t="s">
@@ -24084,10 +24104,10 @@
     </row>
     <row r="911" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B911" s="26"/>
-      <c r="C911" s="26"/>
+      <c r="C911" s="22"/>
       <c r="D911" s="22"/>
-      <c r="E911" s="26"/>
-      <c r="F911" s="26"/>
+      <c r="E911" s="22"/>
+      <c r="F911" s="22"/>
       <c r="G911" s="22"/>
       <c r="H911" s="22"/>
       <c r="I911" s="23" t="s">
@@ -24104,10 +24124,10 @@
     </row>
     <row r="912" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B912" s="26"/>
-      <c r="C912" s="26"/>
+      <c r="C912" s="22"/>
       <c r="D912" s="22"/>
-      <c r="E912" s="26"/>
-      <c r="F912" s="26"/>
+      <c r="E912" s="22"/>
+      <c r="F912" s="22"/>
       <c r="G912" s="22"/>
       <c r="H912" s="22"/>
       <c r="I912" s="23" t="s">

</xml_diff>

<commit_message>
Documentation udpates.   Added Arm FF and Elev FF macro and menu
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5501" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5514" uniqueCount="1220">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -4135,8 +4135,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1094" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1123" activeCellId="0" sqref="C1123"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A191" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C218" activeCellId="0" sqref="C218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">COUNTIF(C18:C1513,"X")</f>
-        <v>738</v>
+        <v>751</v>
       </c>
       <c r="D9" s="13" t="n">
         <f aca="false">COUNTIF(D18:D1513,"X")</f>
@@ -4275,7 +4275,7 @@
       </c>
       <c r="I9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.938931297709924</v>
+        <v>0.955470737913486</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29002,14 +29002,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1100" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1100" s="21" t="s">
         <v>1125</v>
       </c>
       <c r="B1100" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1100" s="26"/>
+      <c r="C1100" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1100" s="22" t="s">
         <v>27</v>
       </c>
@@ -29153,7 +29155,9 @@
       <c r="B1106" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1106" s="26"/>
+      <c r="C1106" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1106" s="22" t="s">
         <v>27</v>
       </c>
@@ -29242,12 +29246,14 @@
       <c r="J1109" s="23"/>
       <c r="K1109" s="23"/>
     </row>
-    <row r="1110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1110" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1110" s="9"/>
       <c r="B1110" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1110" s="26"/>
+      <c r="C1110" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1110" s="22" t="s">
         <v>27</v>
       </c>
@@ -30305,12 +30311,14 @@
       <c r="J1154" s="23"/>
       <c r="K1154" s="23"/>
     </row>
-    <row r="1155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1155" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1155" s="9"/>
       <c r="B1155" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1155" s="26"/>
+      <c r="C1155" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1155" s="22" t="s">
         <v>27</v>
       </c>
@@ -30453,12 +30461,14 @@
       <c r="J1160" s="23"/>
       <c r="K1160" s="23"/>
     </row>
-    <row r="1161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1161" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1161" s="9"/>
       <c r="B1161" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1161" s="26"/>
+      <c r="C1161" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1161" s="26"/>
       <c r="E1161" s="22" t="s">
         <v>27</v>
@@ -30474,12 +30484,14 @@
       <c r="J1161" s="23"/>
       <c r="K1161" s="23"/>
     </row>
-    <row r="1162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1162" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1162" s="9"/>
       <c r="B1162" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1162" s="26"/>
+      <c r="C1162" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1162" s="22" t="s">
         <v>27</v>
       </c>
@@ -30720,12 +30732,14 @@
       <c r="J1171" s="23"/>
       <c r="K1171" s="23"/>
     </row>
-    <row r="1172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1172" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1172" s="9"/>
       <c r="B1172" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1172" s="26"/>
+      <c r="C1172" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1172" s="22" t="s">
         <v>27</v>
       </c>
@@ -30817,11 +30831,13 @@
       <c r="J1175" s="23"/>
       <c r="K1175" s="23"/>
     </row>
-    <row r="1176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1176" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1176" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1176" s="26"/>
+      <c r="C1176" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1176" s="22" t="s">
         <v>27</v>
       </c>
@@ -30839,11 +30855,13 @@
       <c r="J1176" s="23"/>
       <c r="K1176" s="23"/>
     </row>
-    <row r="1177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1177" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1177" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1177" s="26"/>
+      <c r="C1177" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1177" s="22" t="s">
         <v>27</v>
       </c>
@@ -30861,11 +30879,13 @@
       <c r="J1177" s="23"/>
       <c r="K1177" s="23"/>
     </row>
-    <row r="1178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1178" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1178" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1178" s="26"/>
+      <c r="C1178" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1178" s="22" t="s">
         <v>27</v>
       </c>
@@ -30907,11 +30927,13 @@
       <c r="J1179" s="23"/>
       <c r="K1179" s="23"/>
     </row>
-    <row r="1180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1180" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1180" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1180" s="26"/>
+      <c r="C1180" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1180" s="22" t="s">
         <v>27</v>
       </c>
@@ -30929,11 +30951,13 @@
       <c r="J1180" s="23"/>
       <c r="K1180" s="23"/>
     </row>
-    <row r="1181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1181" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1181" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1181" s="26"/>
+      <c r="C1181" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1181" s="22" t="s">
         <v>27</v>
       </c>
@@ -30951,11 +30975,13 @@
       <c r="J1181" s="23"/>
       <c r="K1181" s="23"/>
     </row>
-    <row r="1182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1182" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1182" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="C1182" s="26"/>
+      <c r="C1182" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1182" s="22" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
update numerical integration functions
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5528" uniqueCount="1221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5525" uniqueCount="1220">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -3325,22 +3325,10 @@
     <t xml:space="preserve">NOT USED</t>
   </si>
   <si>
-    <t xml:space="preserve">NumIntegrate_Func_Bs.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NumIntegrate_Func_Ch.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NumIntegrate_Func_Ct.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NumIntegrate_Rk4_Dbl.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOT DONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NumIntegrate_Rk4_K_Dbl.vi</t>
+    <t xml:space="preserve">NumIntegrate_Rk4_Dbl_X_U.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Rk4_Dbl_X.vi</t>
   </si>
   <si>
     <t xml:space="preserve">NumIntegrate_Rk4_Mat_X_U.vi</t>
@@ -3349,16 +3337,25 @@
     <t xml:space="preserve">NumIntegrate_Rk4_Mat_X.vi</t>
   </si>
   <si>
-    <t xml:space="preserve">IS THIS DONE??</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NumIntegrate_Rkf45.vi</t>
+    <t xml:space="preserve">NumIntegrate_RKDP_Mat_X_U.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_RKf45_Func_Bs.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_RKf45_Func_Ch.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_RKf45_Func_Ct.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Rkf45_Impl.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Rkf45_Mat_X_U.vi</t>
   </si>
   <si>
     <t xml:space="preserve">Note that this Feinberg method has been changed and a Dormand Price method has been implemented…. TODO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NumIntegrate_Rkf45_Impl.vi</t>
   </si>
   <si>
     <t xml:space="preserve">NumIntegrate_Trap_Dbl.vi</t>
@@ -4136,10 +4133,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:Q1187"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1121" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1146" activeCellId="0" sqref="C1146"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1058" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1065" activeCellId="0" sqref="A1065"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4250,35 +4247,35 @@
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">B10+B11</f>
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C18:C1514,"X")</f>
+        <f aca="false">COUNTIF(C18:C1512,"X")</f>
         <v>760</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D18:D1514,"X")</f>
+        <f aca="false">COUNTIF(D18:D1512,"X")</f>
         <v>238</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E18:E1514,"X")</f>
-        <v>760</v>
+        <f aca="false">COUNTIF(E18:E1512,"X")</f>
+        <v>758</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F18:F1514,"S")+COUNTIF(F18:F1514,"I")+COUNTIF(F18:F1514,"X")+COUNTIF(F18:F1514,"SI")+COUNTIF(F18:F1514,"IS")+COUNTIF(F18:F1514,"N/A")</f>
+        <f aca="false">COUNTIF(F18:F1512,"S")+COUNTIF(F18:F1512,"I")+COUNTIF(F18:F1512,"X")+COUNTIF(F18:F1512,"SI")+COUNTIF(F18:F1512,"IS")+COUNTIF(F18:F1512,"N/A")</f>
         <v>421</v>
       </c>
       <c r="G9" s="13" t="n">
-        <f aca="false">COUNTIF(G18:G1514,"S")+COUNTIF(G18:G1514,"I")+COUNTIF(G18:G1514,"X")+COUNTIF(G18:G1514,"SI")+COUNTIF(G18:G1514,"IS")+COUNTIF(G18:G1514,"N/A")</f>
+        <f aca="false">COUNTIF(G18:G1512,"S")+COUNTIF(G18:G1512,"I")+COUNTIF(G18:G1512,"X")+COUNTIF(G18:G1512,"SI")+COUNTIF(G18:G1512,"IS")+COUNTIF(G18:G1512,"N/A")</f>
         <v>25</v>
       </c>
       <c r="H9" s="13" t="n">
-        <f aca="false">COUNTIF(H18:H1514,"S")+COUNTIF(H18:H1514,"I")+COUNTIF(H18:H1514,"X")+COUNTIF(H18:H1514,"SI")+COUNTIF(H18:H1514,"IS")+COUNTIF(H18:H1514,"N/A")</f>
+        <f aca="false">COUNTIF(H18:H1512,"S")+COUNTIF(H18:H1512,"I")+COUNTIF(H18:H1512,"X")+COUNTIF(H18:H1512,"SI")+COUNTIF(H18:H1512,"IS")+COUNTIF(H18:H1512,"N/A")</f>
         <v>12</v>
       </c>
       <c r="I9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.96569250317662</v>
+        <v>0.962025316455696</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4286,8 +4283,8 @@
         <v>14</v>
       </c>
       <c r="B10" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1514,"X")</f>
-        <v>704</v>
+        <f aca="false">COUNTIF(B18:B1512,"X")</f>
+        <v>707</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>15</v>
@@ -4298,12 +4295,12 @@
         <v>16</v>
       </c>
       <c r="B11" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1514,"Z")</f>
+        <f aca="false">COUNTIF(B18:B1512,"Z")</f>
         <v>83</v>
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.534942820838628</v>
+        <v>0.532911392405063</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4311,8 +4308,8 @@
         <v>17</v>
       </c>
       <c r="B12" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1514,"/")</f>
-        <v>10</v>
+        <f aca="false">COUNTIF(B18:B1512,"/")</f>
+        <v>8</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -4321,7 +4318,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1514,"\")</f>
+        <f aca="false">COUNTIF(B18:B1512,"\")</f>
         <v>2</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -28246,7 +28243,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="1065" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1065" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1065" s="21" t="s">
         <v>1097</v>
       </c>
@@ -28276,20 +28273,14 @@
       <c r="M1065" s="22"/>
       <c r="N1065" s="22"/>
     </row>
-    <row r="1066" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1066" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1066" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1066" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="C1066" s="26"/>
       <c r="D1066" s="22"/>
-      <c r="E1066" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1066" s="22" t="s">
-        <v>28</v>
-      </c>
+      <c r="E1066" s="26"/>
+      <c r="F1066" s="26"/>
       <c r="G1066" s="22"/>
       <c r="H1066" s="22"/>
       <c r="I1066" s="23" t="s">
@@ -28301,20 +28292,14 @@
       <c r="M1066" s="22"/>
       <c r="N1066" s="22"/>
     </row>
-    <row r="1067" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1067" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1067" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1067" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="C1067" s="26"/>
       <c r="D1067" s="22"/>
-      <c r="E1067" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1067" s="22" t="s">
-        <v>28</v>
-      </c>
+      <c r="E1067" s="26"/>
+      <c r="F1067" s="26"/>
       <c r="G1067" s="22"/>
       <c r="H1067" s="22"/>
       <c r="I1067" s="23" t="s">
@@ -28326,7 +28311,7 @@
       <c r="M1067" s="22"/>
       <c r="N1067" s="22"/>
     </row>
-    <row r="1068" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1068" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1068" s="22" t="s">
         <v>27</v>
       </c>
@@ -28335,11 +28320,9 @@
       </c>
       <c r="D1068" s="22"/>
       <c r="E1068" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1068" s="22" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F1068" s="26"/>
       <c r="G1068" s="22"/>
       <c r="H1068" s="22"/>
       <c r="I1068" s="23" t="s">
@@ -28351,11 +28334,11 @@
       <c r="M1068" s="22"/>
       <c r="N1068" s="22"/>
     </row>
-    <row r="1069" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1069" s="28" t="s">
-        <v>653</v>
-      </c>
-      <c r="C1069" s="22"/>
+    <row r="1069" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1069" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1069" s="26"/>
       <c r="D1069" s="22"/>
       <c r="E1069" s="22" t="s">
         <v>27</v>
@@ -28367,37 +28350,31 @@
         <v>1103</v>
       </c>
       <c r="J1069" s="23"/>
-      <c r="K1069" s="23" t="s">
-        <v>1104</v>
-      </c>
+      <c r="K1069" s="23"/>
       <c r="L1069" s="22"/>
       <c r="M1069" s="22"/>
       <c r="N1069" s="22"/>
     </row>
-    <row r="1070" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1070" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1070" s="28" t="s">
         <v>653</v>
       </c>
       <c r="C1070" s="22"/>
       <c r="D1070" s="22"/>
-      <c r="E1070" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1070" s="26"/>
+      <c r="E1070" s="22"/>
+      <c r="F1070" s="22"/>
       <c r="G1070" s="22"/>
       <c r="H1070" s="22"/>
       <c r="I1070" s="23" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="J1070" s="23"/>
-      <c r="K1070" s="23" t="s">
-        <v>1104</v>
-      </c>
+      <c r="K1070" s="23"/>
       <c r="L1070" s="22"/>
       <c r="M1070" s="22"/>
       <c r="N1070" s="22"/>
     </row>
-    <row r="1071" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1071" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1071" s="22" t="s">
         <v>27</v>
       </c>
@@ -28406,13 +28383,15 @@
       </c>
       <c r="D1071" s="22"/>
       <c r="E1071" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1071" s="26"/>
+        <v>65</v>
+      </c>
+      <c r="F1071" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1071" s="22"/>
       <c r="H1071" s="22"/>
       <c r="I1071" s="23" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="J1071" s="23"/>
       <c r="K1071" s="23"/>
@@ -28420,30 +28399,32 @@
       <c r="M1071" s="22"/>
       <c r="N1071" s="22"/>
     </row>
-    <row r="1072" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1072" s="28" t="s">
-        <v>653</v>
-      </c>
-      <c r="C1072" s="22"/>
+    <row r="1072" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1072" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1072" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1072" s="22"/>
       <c r="E1072" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1072" s="26"/>
+        <v>65</v>
+      </c>
+      <c r="F1072" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1072" s="22"/>
       <c r="H1072" s="22"/>
       <c r="I1072" s="23" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="J1072" s="23"/>
-      <c r="K1072" s="23" t="s">
-        <v>1108</v>
-      </c>
+      <c r="K1072" s="23"/>
       <c r="L1072" s="22"/>
       <c r="M1072" s="22"/>
       <c r="N1072" s="22"/>
     </row>
-    <row r="1073" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1073" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1073" s="22" t="s">
         <v>27</v>
       </c>
@@ -28452,23 +28433,23 @@
       </c>
       <c r="D1073" s="22"/>
       <c r="E1073" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1073" s="26"/>
+        <v>65</v>
+      </c>
+      <c r="F1073" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1073" s="22"/>
       <c r="H1073" s="22"/>
       <c r="I1073" s="23" t="s">
-        <v>1109</v>
-      </c>
-      <c r="J1073" s="23" t="s">
-        <v>1110</v>
-      </c>
+        <v>1107</v>
+      </c>
+      <c r="J1073" s="23"/>
       <c r="K1073" s="23"/>
       <c r="L1073" s="22"/>
       <c r="M1073" s="22"/>
       <c r="N1073" s="22"/>
     </row>
-    <row r="1074" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1074" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1074" s="22" t="s">
         <v>27</v>
       </c>
@@ -28485,7 +28466,7 @@
       <c r="G1074" s="22"/>
       <c r="H1074" s="22"/>
       <c r="I1074" s="23" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="J1074" s="23"/>
       <c r="K1074" s="23"/>
@@ -28493,34 +28474,32 @@
       <c r="M1074" s="22"/>
       <c r="N1074" s="22"/>
     </row>
-    <row r="1075" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1075" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1075" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C1075" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1075" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="D1075" s="22"/>
       <c r="E1075" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1075" s="22" t="s">
-        <v>28</v>
-      </c>
+      <c r="F1075" s="26"/>
       <c r="G1075" s="22"/>
       <c r="H1075" s="22"/>
       <c r="I1075" s="23" t="s">
-        <v>1112</v>
-      </c>
-      <c r="J1075" s="23"/>
+        <v>1109</v>
+      </c>
+      <c r="J1075" s="23" t="s">
+        <v>1110</v>
+      </c>
       <c r="K1075" s="23"/>
       <c r="L1075" s="22"/>
       <c r="M1075" s="22"/>
       <c r="N1075" s="22"/>
     </row>
-    <row r="1076" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1076" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1076" s="22" t="s">
         <v>27</v>
       </c>
@@ -28534,12 +28513,12 @@
         <v>27</v>
       </c>
       <c r="F1076" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G1076" s="22"/>
       <c r="H1076" s="22"/>
       <c r="I1076" s="23" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="J1076" s="23"/>
       <c r="K1076" s="23"/>
@@ -28548,14 +28527,26 @@
       <c r="N1076" s="22"/>
     </row>
     <row r="1077" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1077" s="22"/>
-      <c r="C1077" s="22"/>
-      <c r="D1077" s="22"/>
-      <c r="E1077" s="22"/>
-      <c r="F1077" s="22"/>
+      <c r="B1077" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1077" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1077" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1077" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1077" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G1077" s="22"/>
       <c r="H1077" s="22"/>
-      <c r="I1077" s="23"/>
+      <c r="I1077" s="23" t="s">
+        <v>1112</v>
+      </c>
       <c r="J1077" s="23"/>
       <c r="K1077" s="23"/>
       <c r="L1077" s="22"/>
@@ -28563,89 +28554,81 @@
       <c r="N1077" s="22"/>
     </row>
     <row r="1078" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1078" s="47"/>
-      <c r="C1078" s="1"/>
-      <c r="D1078" s="1"/>
-      <c r="E1078" s="1"/>
-      <c r="F1078" s="1"/>
-      <c r="G1078" s="1"/>
-      <c r="H1078" s="1"/>
-      <c r="I1078" s="1"/>
-      <c r="J1078" s="1"/>
-      <c r="K1078" s="1"/>
-      <c r="L1078" s="1"/>
-      <c r="M1078" s="1"/>
-      <c r="N1078" s="1"/>
-    </row>
-    <row r="1079" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1079" s="19"/>
-      <c r="B1079" s="11" t="s">
+      <c r="B1078" s="22"/>
+      <c r="C1078" s="22"/>
+      <c r="D1078" s="22"/>
+      <c r="E1078" s="22"/>
+      <c r="F1078" s="22"/>
+      <c r="G1078" s="22"/>
+      <c r="H1078" s="22"/>
+      <c r="I1078" s="23"/>
+      <c r="J1078" s="23"/>
+      <c r="K1078" s="23"/>
+      <c r="L1078" s="22"/>
+      <c r="M1078" s="22"/>
+      <c r="N1078" s="22"/>
+    </row>
+    <row r="1079" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1079" s="47"/>
+      <c r="C1079" s="1"/>
+      <c r="D1079" s="1"/>
+      <c r="E1079" s="1"/>
+      <c r="F1079" s="1"/>
+      <c r="G1079" s="1"/>
+      <c r="H1079" s="1"/>
+      <c r="I1079" s="1"/>
+      <c r="J1079" s="1"/>
+      <c r="K1079" s="1"/>
+      <c r="L1079" s="1"/>
+      <c r="M1079" s="1"/>
+      <c r="N1079" s="1"/>
+    </row>
+    <row r="1080" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1080" s="19"/>
+      <c r="B1080" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1079" s="11" t="s">
+      <c r="C1080" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1079" s="11" t="s">
+      <c r="D1080" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1079" s="11" t="s">
+      <c r="E1080" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1079" s="11" t="s">
+      <c r="F1080" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G1079" s="11" t="s">
+      <c r="G1080" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1079" s="11" t="s">
+      <c r="H1080" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1079" s="20" t="s">
+      <c r="I1080" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1079" s="20" t="s">
+      <c r="J1080" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1079" s="20" t="s">
+      <c r="K1080" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L1079" s="11" t="s">
+      <c r="L1080" s="11" t="s">
         <v>740</v>
       </c>
-      <c r="M1079" s="11" t="s">
+      <c r="M1080" s="11" t="s">
         <v>741</v>
       </c>
-      <c r="N1079" s="11" t="s">
+      <c r="N1080" s="11" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="1080" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1080" s="21" t="s">
-        <v>1114</v>
-      </c>
-      <c r="B1080" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1080" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1080" s="22"/>
-      <c r="E1080" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1080" s="26"/>
-      <c r="G1080" s="22"/>
-      <c r="H1080" s="22"/>
-      <c r="I1080" s="23" t="s">
-        <v>1115</v>
-      </c>
-      <c r="J1080" s="23"/>
-      <c r="K1080" s="23"/>
-      <c r="L1080" s="22"/>
-      <c r="M1080" s="22"/>
-      <c r="N1080" s="22"/>
-    </row>
-    <row r="1081" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1081" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1081" s="21" t="s">
+        <v>1113</v>
+      </c>
       <c r="B1081" s="22" t="s">
         <v>27</v>
       </c>
@@ -28660,7 +28643,7 @@
       <c r="G1081" s="22"/>
       <c r="H1081" s="22"/>
       <c r="I1081" s="23" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="J1081" s="23"/>
       <c r="K1081" s="23"/>
@@ -28669,14 +28652,22 @@
       <c r="N1081" s="22"/>
     </row>
     <row r="1082" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1082" s="22"/>
-      <c r="C1082" s="22"/>
+      <c r="B1082" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1082" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1082" s="22"/>
-      <c r="E1082" s="22"/>
-      <c r="F1082" s="22"/>
+      <c r="E1082" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1082" s="26"/>
       <c r="G1082" s="22"/>
       <c r="H1082" s="22"/>
-      <c r="I1082" s="23"/>
+      <c r="I1082" s="23" t="s">
+        <v>1115</v>
+      </c>
       <c r="J1082" s="23"/>
       <c r="K1082" s="23"/>
       <c r="L1082" s="22"/>
@@ -28699,100 +28690,116 @@
       <c r="N1083" s="22"/>
     </row>
     <row r="1084" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1084" s="22"/>
-      <c r="C1084" s="22"/>
-      <c r="D1084" s="22"/>
-      <c r="E1084" s="22"/>
-      <c r="F1084" s="22"/>
-      <c r="G1084" s="22"/>
-      <c r="H1084" s="22"/>
-      <c r="I1084" s="23"/>
-      <c r="J1084" s="23"/>
-      <c r="K1084" s="23"/>
-      <c r="L1084" s="22"/>
-      <c r="M1084" s="22"/>
-      <c r="N1084" s="22"/>
-    </row>
-    <row r="1085" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1085" s="22"/>
-      <c r="C1085" s="22"/>
-      <c r="D1085" s="22"/>
-      <c r="E1085" s="22"/>
-      <c r="F1085" s="22"/>
-      <c r="G1085" s="22"/>
-      <c r="H1085" s="22"/>
-      <c r="I1085" s="23"/>
-      <c r="J1085" s="23"/>
-      <c r="K1085" s="23"/>
-      <c r="L1085" s="22"/>
-      <c r="M1085" s="22"/>
-      <c r="N1085" s="22"/>
-    </row>
-    <row r="1086" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1086" s="1"/>
-      <c r="C1086" s="1"/>
-      <c r="D1086" s="1"/>
-      <c r="E1086" s="1"/>
-      <c r="F1086" s="1"/>
-      <c r="G1086" s="1"/>
-      <c r="H1086" s="1"/>
-      <c r="I1086" s="1"/>
-      <c r="J1086" s="1"/>
-      <c r="K1086" s="1"/>
-      <c r="L1086" s="1"/>
-      <c r="M1086" s="1"/>
-      <c r="N1086" s="1"/>
-      <c r="O1086" s="1"/>
-      <c r="P1086" s="1"/>
-    </row>
-    <row r="1087" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1087" s="19"/>
-      <c r="B1087" s="11" t="s">
+      <c r="B1084" s="1"/>
+      <c r="C1084" s="1"/>
+      <c r="D1084" s="1"/>
+      <c r="E1084" s="1"/>
+      <c r="F1084" s="1"/>
+      <c r="G1084" s="1"/>
+      <c r="H1084" s="1"/>
+      <c r="I1084" s="1"/>
+      <c r="J1084" s="1"/>
+      <c r="K1084" s="1"/>
+      <c r="L1084" s="1"/>
+      <c r="M1084" s="1"/>
+      <c r="N1084" s="1"/>
+      <c r="O1084" s="1"/>
+      <c r="P1084" s="1"/>
+    </row>
+    <row r="1085" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1085" s="19"/>
+      <c r="B1085" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1087" s="11" t="s">
+      <c r="C1085" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1087" s="11" t="s">
+      <c r="D1085" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1087" s="11" t="s">
+      <c r="E1085" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1087" s="11" t="s">
+      <c r="F1085" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G1087" s="11" t="s">
+      <c r="G1085" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1087" s="11" t="s">
+      <c r="H1085" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1087" s="20" t="s">
+      <c r="I1085" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1087" s="20" t="s">
+      <c r="J1085" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1087" s="20" t="s">
+      <c r="K1085" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L1087" s="11" t="s">
+      <c r="L1085" s="11" t="s">
         <v>740</v>
       </c>
-      <c r="M1087" s="11" t="s">
+      <c r="M1085" s="11" t="s">
         <v>741</v>
       </c>
-      <c r="N1087" s="11" t="s">
+      <c r="N1085" s="11" t="s">
         <v>742</v>
       </c>
     </row>
+    <row r="1086" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1086" s="21" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B1086" s="28" t="s">
+        <v>653</v>
+      </c>
+      <c r="C1086" s="26"/>
+      <c r="D1086" s="22"/>
+      <c r="E1086" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1086" s="26"/>
+      <c r="G1086" s="22"/>
+      <c r="H1086" s="22"/>
+      <c r="I1086" s="23" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J1086" s="23"/>
+      <c r="K1086" s="23" t="s">
+        <v>655</v>
+      </c>
+      <c r="L1086" s="22"/>
+      <c r="M1086" s="22"/>
+      <c r="N1086" s="22"/>
+    </row>
+    <row r="1087" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1087" s="28" t="s">
+        <v>653</v>
+      </c>
+      <c r="C1087" s="26"/>
+      <c r="D1087" s="22"/>
+      <c r="E1087" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1087" s="26"/>
+      <c r="G1087" s="22"/>
+      <c r="H1087" s="22"/>
+      <c r="I1087" s="23" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J1087" s="23"/>
+      <c r="K1087" s="23" t="s">
+        <v>1119</v>
+      </c>
+      <c r="L1087" s="22"/>
+      <c r="M1087" s="22"/>
+      <c r="N1087" s="22"/>
+    </row>
     <row r="1088" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1088" s="21" t="s">
-        <v>1117</v>
-      </c>
-      <c r="B1088" s="28" t="s">
-        <v>653</v>
+      <c r="B1088" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="C1088" s="26"/>
       <c r="D1088" s="22"/>
@@ -28800,24 +28807,26 @@
         <v>27</v>
       </c>
       <c r="F1088" s="26"/>
-      <c r="G1088" s="22"/>
+      <c r="G1088" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="H1088" s="22"/>
       <c r="I1088" s="23" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="J1088" s="23"/>
-      <c r="K1088" s="23" t="s">
-        <v>655</v>
-      </c>
+      <c r="K1088" s="23"/>
       <c r="L1088" s="22"/>
       <c r="M1088" s="22"/>
       <c r="N1088" s="22"/>
     </row>
     <row r="1089" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1089" s="28" t="s">
-        <v>653</v>
-      </c>
-      <c r="C1089" s="26"/>
+      <c r="B1089" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1089" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1089" s="22"/>
       <c r="E1089" s="22" t="s">
         <v>27</v>
@@ -28826,12 +28835,10 @@
       <c r="G1089" s="22"/>
       <c r="H1089" s="22"/>
       <c r="I1089" s="23" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="J1089" s="23"/>
-      <c r="K1089" s="23" t="s">
-        <v>1120</v>
-      </c>
+      <c r="K1089" s="23"/>
       <c r="L1089" s="22"/>
       <c r="M1089" s="22"/>
       <c r="N1089" s="22"/>
@@ -28840,7 +28847,9 @@
       <c r="B1090" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1090" s="26"/>
+      <c r="C1090" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1090" s="22"/>
       <c r="E1090" s="22" t="s">
         <v>27</v>
@@ -28851,7 +28860,7 @@
       </c>
       <c r="H1090" s="22"/>
       <c r="I1090" s="23" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="J1090" s="23"/>
       <c r="K1090" s="23"/>
@@ -28863,9 +28872,7 @@
       <c r="B1091" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1091" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="C1091" s="26"/>
       <c r="D1091" s="22"/>
       <c r="E1091" s="22" t="s">
         <v>27</v>
@@ -28874,7 +28881,7 @@
       <c r="G1091" s="22"/>
       <c r="H1091" s="22"/>
       <c r="I1091" s="23" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="J1091" s="23"/>
       <c r="K1091" s="23"/>
@@ -28882,84 +28889,62 @@
       <c r="M1091" s="22"/>
       <c r="N1091" s="22"/>
     </row>
-    <row r="1092" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1092" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1092" s="22" t="s">
-        <v>27</v>
-      </c>
+    <row r="1092" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1092" s="22"/>
+      <c r="C1092" s="22"/>
       <c r="D1092" s="22"/>
-      <c r="E1092" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1092" s="26"/>
-      <c r="G1092" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1092" s="22"/>
+      <c r="F1092" s="22"/>
+      <c r="G1092" s="22"/>
       <c r="H1092" s="22"/>
-      <c r="I1092" s="23" t="s">
-        <v>1123</v>
-      </c>
+      <c r="I1092" s="23"/>
       <c r="J1092" s="23"/>
       <c r="K1092" s="23"/>
       <c r="L1092" s="22"/>
       <c r="M1092" s="22"/>
       <c r="N1092" s="22"/>
     </row>
-    <row r="1093" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1093" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1093" s="26"/>
-      <c r="D1093" s="22"/>
-      <c r="E1093" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1093" s="26"/>
-      <c r="G1093" s="22"/>
-      <c r="H1093" s="22"/>
-      <c r="I1093" s="23" t="s">
+    <row r="1093" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1093" s="47"/>
+      <c r="C1093" s="1"/>
+      <c r="D1093" s="1"/>
+      <c r="E1093" s="1"/>
+      <c r="F1093" s="1"/>
+      <c r="G1093" s="1"/>
+      <c r="H1093" s="1"/>
+      <c r="I1093" s="1"/>
+      <c r="J1093" s="1"/>
+      <c r="K1093" s="1"/>
+      <c r="L1093" s="1"/>
+      <c r="M1093" s="1"/>
+      <c r="N1093" s="1"/>
+    </row>
+    <row r="1094" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1094" s="9"/>
+    </row>
+    <row r="1095" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1095" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1095" s="17"/>
+      <c r="C1095" s="18"/>
+      <c r="D1095" s="18"/>
+      <c r="E1095" s="18"/>
+      <c r="F1095" s="18"/>
+      <c r="G1095" s="18"/>
+      <c r="H1095" s="18"/>
+    </row>
+    <row r="1096" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1096" s="16" t="s">
         <v>1124</v>
       </c>
-      <c r="J1093" s="23"/>
-      <c r="K1093" s="23"/>
-      <c r="L1093" s="22"/>
-      <c r="M1093" s="22"/>
-      <c r="N1093" s="22"/>
-    </row>
-    <row r="1094" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1094" s="22"/>
-      <c r="C1094" s="22"/>
-      <c r="D1094" s="22"/>
-      <c r="E1094" s="22"/>
-      <c r="F1094" s="22"/>
-      <c r="G1094" s="22"/>
-      <c r="H1094" s="22"/>
-      <c r="I1094" s="23"/>
-      <c r="J1094" s="23"/>
-      <c r="K1094" s="23"/>
-      <c r="L1094" s="22"/>
-      <c r="M1094" s="22"/>
-      <c r="N1094" s="22"/>
-    </row>
-    <row r="1095" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1095" s="47"/>
-      <c r="C1095" s="1"/>
-      <c r="D1095" s="1"/>
-      <c r="E1095" s="1"/>
-      <c r="F1095" s="1"/>
-      <c r="G1095" s="1"/>
-      <c r="H1095" s="1"/>
-      <c r="I1095" s="1"/>
-      <c r="J1095" s="1"/>
-      <c r="K1095" s="1"/>
-      <c r="L1095" s="1"/>
-      <c r="M1095" s="1"/>
-      <c r="N1095" s="1"/>
-    </row>
-    <row r="1096" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1096" s="9"/>
+      <c r="B1096" s="17"/>
+      <c r="C1096" s="18"/>
+      <c r="D1096" s="18"/>
+      <c r="E1096" s="18"/>
+      <c r="F1096" s="18"/>
+      <c r="G1096" s="18"/>
+      <c r="H1096" s="18"/>
     </row>
     <row r="1097" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1097" s="16" t="s">
@@ -28973,73 +28958,97 @@
       <c r="G1097" s="18"/>
       <c r="H1097" s="18"/>
     </row>
-    <row r="1098" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1098" s="16" t="s">
+    <row r="1098" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1098" s="9"/>
+      <c r="B1098" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1098" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1098" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1098" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1098" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1098" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1098" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1098" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1098" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1098" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1099" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1099" s="21" t="s">
         <v>1125</v>
       </c>
-      <c r="B1098" s="17"/>
-      <c r="C1098" s="18"/>
-      <c r="D1098" s="18"/>
-      <c r="E1098" s="18"/>
-      <c r="F1098" s="18"/>
-      <c r="G1098" s="18"/>
-      <c r="H1098" s="18"/>
-    </row>
-    <row r="1099" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1099" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1099" s="17"/>
-      <c r="C1099" s="18"/>
-      <c r="D1099" s="18"/>
-      <c r="E1099" s="18"/>
-      <c r="F1099" s="18"/>
-      <c r="G1099" s="18"/>
-      <c r="H1099" s="18"/>
-    </row>
-    <row r="1100" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1100" s="9"/>
-      <c r="B1100" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1100" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1100" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1100" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1100" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1100" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1100" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1100" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1100" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1100" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="1101" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1101" s="21" t="s">
+      <c r="B1099" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="B1101" s="22" t="s">
+      <c r="C1099" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1099" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1099" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1099" s="22" t="s">
+        <v>683</v>
+      </c>
+      <c r="G1099" s="22"/>
+      <c r="H1099" s="22"/>
+      <c r="I1099" s="23" t="s">
         <v>1127</v>
       </c>
-      <c r="C1101" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="J1099" s="23"/>
+      <c r="K1099" s="23"/>
+    </row>
+    <row r="1100" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1100" s="21"/>
+      <c r="B1100" s="22" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C1100" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1100" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1100" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1100" s="22" t="s">
+        <v>683</v>
+      </c>
+      <c r="G1100" s="22"/>
+      <c r="H1100" s="22"/>
+      <c r="I1100" s="23" t="s">
+        <v>1128</v>
+      </c>
+      <c r="J1100" s="23"/>
+      <c r="K1100" s="23"/>
+    </row>
+    <row r="1101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1101" s="21"/>
+      <c r="B1101" s="28" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C1101" s="26"/>
       <c r="D1101" s="22" t="s">
         <v>27</v>
       </c>
@@ -29052,19 +29061,17 @@
       <c r="G1101" s="22"/>
       <c r="H1101" s="22"/>
       <c r="I1101" s="23" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="J1101" s="23"/>
       <c r="K1101" s="23"/>
     </row>
-    <row r="1102" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1102" s="21"/>
       <c r="B1102" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1102" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1102" s="26"/>
       <c r="D1102" s="22" t="s">
         <v>27</v>
       </c>
@@ -29077,17 +29084,19 @@
       <c r="G1102" s="22"/>
       <c r="H1102" s="22"/>
       <c r="I1102" s="23" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="J1102" s="23"/>
       <c r="K1102" s="23"/>
     </row>
     <row r="1103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1103" s="21"/>
-      <c r="B1103" s="28" t="s">
-        <v>1130</v>
-      </c>
-      <c r="C1103" s="26"/>
+      <c r="B1103" s="22" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C1103" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1103" s="22" t="s">
         <v>27</v>
       </c>
@@ -29100,17 +29109,19 @@
       <c r="G1103" s="22"/>
       <c r="H1103" s="22"/>
       <c r="I1103" s="23" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="J1103" s="23"/>
       <c r="K1103" s="23"/>
     </row>
     <row r="1104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1104" s="21"/>
+      <c r="A1104" s="9"/>
       <c r="B1104" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1104" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1104" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1104" s="22" t="s">
         <v>27</v>
       </c>
@@ -29123,15 +29134,15 @@
       <c r="G1104" s="22"/>
       <c r="H1104" s="22"/>
       <c r="I1104" s="23" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="J1104" s="23"/>
       <c r="K1104" s="23"/>
     </row>
     <row r="1105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1105" s="21"/>
+      <c r="A1105" s="9"/>
       <c r="B1105" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1105" s="22" t="s">
         <v>27</v>
@@ -29147,8 +29158,8 @@
       </c>
       <c r="G1105" s="22"/>
       <c r="H1105" s="22"/>
-      <c r="I1105" s="23" t="s">
-        <v>1133</v>
+      <c r="I1105" s="46" t="s">
+        <v>1134</v>
       </c>
       <c r="J1105" s="23"/>
       <c r="K1105" s="23"/>
@@ -29156,7 +29167,7 @@
     <row r="1106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1106" s="9"/>
       <c r="B1106" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1106" s="22" t="s">
         <v>27</v>
@@ -29172,8 +29183,8 @@
       </c>
       <c r="G1106" s="22"/>
       <c r="H1106" s="22"/>
-      <c r="I1106" s="23" t="s">
-        <v>1134</v>
+      <c r="I1106" s="46" t="s">
+        <v>1135</v>
       </c>
       <c r="J1106" s="23"/>
       <c r="K1106" s="23"/>
@@ -29181,7 +29192,7 @@
     <row r="1107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1107" s="9"/>
       <c r="B1107" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1107" s="22" t="s">
         <v>27</v>
@@ -29197,16 +29208,16 @@
       </c>
       <c r="G1107" s="22"/>
       <c r="H1107" s="22"/>
-      <c r="I1107" s="46" t="s">
-        <v>1135</v>
+      <c r="I1107" s="23" t="s">
+        <v>1136</v>
       </c>
       <c r="J1107" s="23"/>
       <c r="K1107" s="23"/>
     </row>
-    <row r="1108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1108" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1108" s="9"/>
       <c r="B1108" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1108" s="22" t="s">
         <v>27</v>
@@ -29222,16 +29233,16 @@
       </c>
       <c r="G1108" s="22"/>
       <c r="H1108" s="22"/>
-      <c r="I1108" s="46" t="s">
-        <v>1136</v>
+      <c r="I1108" s="23" t="s">
+        <v>1137</v>
       </c>
       <c r="J1108" s="23"/>
       <c r="K1108" s="23"/>
     </row>
-    <row r="1109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1109" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1109" s="9"/>
       <c r="B1109" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1109" s="22" t="s">
         <v>27</v>
@@ -29248,7 +29259,7 @@
       <c r="G1109" s="22"/>
       <c r="H1109" s="22"/>
       <c r="I1109" s="23" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="J1109" s="23"/>
       <c r="K1109" s="23"/>
@@ -29256,7 +29267,7 @@
     <row r="1110" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1110" s="9"/>
       <c r="B1110" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1110" s="22" t="s">
         <v>27</v>
@@ -29273,7 +29284,7 @@
       <c r="G1110" s="22"/>
       <c r="H1110" s="22"/>
       <c r="I1110" s="23" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="J1110" s="23"/>
       <c r="K1110" s="23"/>
@@ -29281,7 +29292,7 @@
     <row r="1111" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1111" s="9"/>
       <c r="B1111" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1111" s="22" t="s">
         <v>27</v>
@@ -29298,7 +29309,7 @@
       <c r="G1111" s="22"/>
       <c r="H1111" s="22"/>
       <c r="I1111" s="23" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="J1111" s="23"/>
       <c r="K1111" s="23"/>
@@ -29306,14 +29317,12 @@
     <row r="1112" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1112" s="9"/>
       <c r="B1112" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1112" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1112" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="D1112" s="22"/>
       <c r="E1112" s="22" t="s">
         <v>27</v>
       </c>
@@ -29323,7 +29332,7 @@
       <c r="G1112" s="22"/>
       <c r="H1112" s="22"/>
       <c r="I1112" s="23" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="J1112" s="23"/>
       <c r="K1112" s="23"/>
@@ -29331,7 +29340,7 @@
     <row r="1113" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1113" s="9"/>
       <c r="B1113" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1113" s="22" t="s">
         <v>27</v>
@@ -29348,38 +29357,42 @@
       <c r="G1113" s="22"/>
       <c r="H1113" s="22"/>
       <c r="I1113" s="23" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="J1113" s="23"/>
       <c r="K1113" s="23"/>
     </row>
-    <row r="1114" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1114" s="9"/>
       <c r="B1114" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1114" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1114" s="22"/>
+      <c r="D1114" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="E1114" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F1114" s="22" t="s">
-        <v>683</v>
+        <v>1143</v>
       </c>
       <c r="G1114" s="22"/>
       <c r="H1114" s="22"/>
       <c r="I1114" s="23" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="J1114" s="23"/>
-      <c r="K1114" s="23"/>
-    </row>
-    <row r="1115" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1114" s="23" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="1115" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1115" s="9"/>
       <c r="B1115" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1115" s="22" t="s">
         <v>27</v>
@@ -29391,20 +29404,22 @@
         <v>27</v>
       </c>
       <c r="F1115" s="22" t="s">
-        <v>683</v>
+        <v>1143</v>
       </c>
       <c r="G1115" s="22"/>
       <c r="H1115" s="22"/>
       <c r="I1115" s="23" t="s">
-        <v>1143</v>
+        <v>1146</v>
       </c>
       <c r="J1115" s="23"/>
-      <c r="K1115" s="23"/>
-    </row>
-    <row r="1116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1115" s="23" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="1116" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1116" s="9"/>
       <c r="B1116" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1116" s="22" t="s">
         <v>27</v>
@@ -29416,26 +29431,22 @@
         <v>27</v>
       </c>
       <c r="F1116" s="22" t="s">
-        <v>1144</v>
+        <v>683</v>
       </c>
       <c r="G1116" s="22"/>
       <c r="H1116" s="22"/>
       <c r="I1116" s="23" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="J1116" s="23"/>
-      <c r="K1116" s="23" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="1117" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1116" s="23"/>
+    </row>
+    <row r="1117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1117" s="9"/>
       <c r="B1117" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1117" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1117" s="26"/>
       <c r="D1117" s="22" t="s">
         <v>27</v>
       </c>
@@ -29443,26 +29454,22 @@
         <v>27</v>
       </c>
       <c r="F1117" s="22" t="s">
-        <v>1144</v>
+        <v>683</v>
       </c>
       <c r="G1117" s="22"/>
       <c r="H1117" s="22"/>
       <c r="I1117" s="23" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="J1117" s="23"/>
-      <c r="K1117" s="23" t="s">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="1118" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1117" s="23"/>
+    </row>
+    <row r="1118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1118" s="9"/>
       <c r="B1118" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1118" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1118" s="26"/>
       <c r="D1118" s="22" t="s">
         <v>27</v>
       </c>
@@ -29475,7 +29482,7 @@
       <c r="G1118" s="22"/>
       <c r="H1118" s="22"/>
       <c r="I1118" s="23" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="J1118" s="23"/>
       <c r="K1118" s="23"/>
@@ -29483,7 +29490,7 @@
     <row r="1119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1119" s="9"/>
       <c r="B1119" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1119" s="26"/>
       <c r="D1119" s="22" t="s">
@@ -29498,7 +29505,7 @@
       <c r="G1119" s="22"/>
       <c r="H1119" s="22"/>
       <c r="I1119" s="23" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="J1119" s="23"/>
       <c r="K1119" s="23"/>
@@ -29506,7 +29513,7 @@
     <row r="1120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1120" s="9"/>
       <c r="B1120" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1120" s="26"/>
       <c r="D1120" s="22" t="s">
@@ -29521,7 +29528,7 @@
       <c r="G1120" s="22"/>
       <c r="H1120" s="22"/>
       <c r="I1120" s="23" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="J1120" s="23"/>
       <c r="K1120" s="23"/>
@@ -29529,7 +29536,7 @@
     <row r="1121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1121" s="9"/>
       <c r="B1121" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1121" s="26"/>
       <c r="D1121" s="22" t="s">
@@ -29544,15 +29551,17 @@
       <c r="G1121" s="22"/>
       <c r="H1121" s="22"/>
       <c r="I1121" s="23" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="J1121" s="23"/>
-      <c r="K1121" s="23"/>
+      <c r="K1121" s="23" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="1122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1122" s="9"/>
       <c r="B1122" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1122" s="26"/>
       <c r="D1122" s="22" t="s">
@@ -29567,7 +29576,7 @@
       <c r="G1122" s="22"/>
       <c r="H1122" s="22"/>
       <c r="I1122" s="23" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="J1122" s="23"/>
       <c r="K1122" s="23"/>
@@ -29575,7 +29584,7 @@
     <row r="1123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1123" s="9"/>
       <c r="B1123" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1123" s="26"/>
       <c r="D1123" s="22" t="s">
@@ -29590,17 +29599,15 @@
       <c r="G1123" s="22"/>
       <c r="H1123" s="22"/>
       <c r="I1123" s="23" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="J1123" s="23"/>
-      <c r="K1123" s="23" t="s">
-        <v>280</v>
-      </c>
+      <c r="K1123" s="23"/>
     </row>
     <row r="1124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1124" s="9"/>
       <c r="B1124" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1124" s="26"/>
       <c r="D1124" s="22" t="s">
@@ -29615,7 +29622,7 @@
       <c r="G1124" s="22"/>
       <c r="H1124" s="22"/>
       <c r="I1124" s="23" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="J1124" s="23"/>
       <c r="K1124" s="23"/>
@@ -29623,9 +29630,11 @@
     <row r="1125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1125" s="9"/>
       <c r="B1125" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1125" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1125" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1125" s="22" t="s">
         <v>27</v>
       </c>
@@ -29638,7 +29647,7 @@
       <c r="G1125" s="22"/>
       <c r="H1125" s="22"/>
       <c r="I1125" s="23" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="J1125" s="23"/>
       <c r="K1125" s="23"/>
@@ -29646,7 +29655,7 @@
     <row r="1126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1126" s="9"/>
       <c r="B1126" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1126" s="26"/>
       <c r="D1126" s="22" t="s">
@@ -29661,7 +29670,7 @@
       <c r="G1126" s="22"/>
       <c r="H1126" s="22"/>
       <c r="I1126" s="23" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="J1126" s="23"/>
       <c r="K1126" s="23"/>
@@ -29669,11 +29678,9 @@
     <row r="1127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1127" s="9"/>
       <c r="B1127" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1127" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1127" s="26"/>
       <c r="D1127" s="22" t="s">
         <v>27</v>
       </c>
@@ -29686,7 +29693,7 @@
       <c r="G1127" s="22"/>
       <c r="H1127" s="22"/>
       <c r="I1127" s="23" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="J1127" s="23"/>
       <c r="K1127" s="23"/>
@@ -29694,7 +29701,7 @@
     <row r="1128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1128" s="9"/>
       <c r="B1128" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1128" s="26"/>
       <c r="D1128" s="22" t="s">
@@ -29709,7 +29716,7 @@
       <c r="G1128" s="22"/>
       <c r="H1128" s="22"/>
       <c r="I1128" s="23" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="J1128" s="23"/>
       <c r="K1128" s="23"/>
@@ -29717,7 +29724,7 @@
     <row r="1129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1129" s="9"/>
       <c r="B1129" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1129" s="26"/>
       <c r="D1129" s="22" t="s">
@@ -29732,7 +29739,7 @@
       <c r="G1129" s="22"/>
       <c r="H1129" s="22"/>
       <c r="I1129" s="23" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="J1129" s="23"/>
       <c r="K1129" s="23"/>
@@ -29740,7 +29747,7 @@
     <row r="1130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1130" s="9"/>
       <c r="B1130" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1130" s="26"/>
       <c r="D1130" s="22" t="s">
@@ -29755,7 +29762,7 @@
       <c r="G1130" s="22"/>
       <c r="H1130" s="22"/>
       <c r="I1130" s="23" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="J1130" s="23"/>
       <c r="K1130" s="23"/>
@@ -29763,9 +29770,11 @@
     <row r="1131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1131" s="9"/>
       <c r="B1131" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1131" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1131" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1131" s="22" t="s">
         <v>27</v>
       </c>
@@ -29778,7 +29787,7 @@
       <c r="G1131" s="22"/>
       <c r="H1131" s="22"/>
       <c r="I1131" s="23" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="J1131" s="23"/>
       <c r="K1131" s="23"/>
@@ -29786,9 +29795,11 @@
     <row r="1132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1132" s="9"/>
       <c r="B1132" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1132" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1132" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1132" s="22" t="s">
         <v>27</v>
       </c>
@@ -29801,7 +29812,7 @@
       <c r="G1132" s="22"/>
       <c r="H1132" s="22"/>
       <c r="I1132" s="23" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="J1132" s="23"/>
       <c r="K1132" s="23"/>
@@ -29809,7 +29820,7 @@
     <row r="1133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1133" s="9"/>
       <c r="B1133" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1133" s="22" t="s">
         <v>27</v>
@@ -29826,7 +29837,7 @@
       <c r="G1133" s="22"/>
       <c r="H1133" s="22"/>
       <c r="I1133" s="23" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="J1133" s="23"/>
       <c r="K1133" s="23"/>
@@ -29834,11 +29845,9 @@
     <row r="1134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1134" s="9"/>
       <c r="B1134" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1134" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1134" s="26"/>
       <c r="D1134" s="22" t="s">
         <v>27</v>
       </c>
@@ -29851,7 +29860,7 @@
       <c r="G1134" s="22"/>
       <c r="H1134" s="22"/>
       <c r="I1134" s="23" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="J1134" s="23"/>
       <c r="K1134" s="23"/>
@@ -29859,11 +29868,9 @@
     <row r="1135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1135" s="9"/>
       <c r="B1135" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1135" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1135" s="26"/>
       <c r="D1135" s="22" t="s">
         <v>27</v>
       </c>
@@ -29876,7 +29883,7 @@
       <c r="G1135" s="22"/>
       <c r="H1135" s="22"/>
       <c r="I1135" s="23" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="J1135" s="23"/>
       <c r="K1135" s="23"/>
@@ -29884,7 +29891,7 @@
     <row r="1136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1136" s="9"/>
       <c r="B1136" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1136" s="26"/>
       <c r="D1136" s="22" t="s">
@@ -29899,7 +29906,7 @@
       <c r="G1136" s="22"/>
       <c r="H1136" s="22"/>
       <c r="I1136" s="23" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="J1136" s="23"/>
       <c r="K1136" s="23"/>
@@ -29907,7 +29914,7 @@
     <row r="1137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1137" s="9"/>
       <c r="B1137" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1137" s="26"/>
       <c r="D1137" s="22" t="s">
@@ -29922,7 +29929,7 @@
       <c r="G1137" s="22"/>
       <c r="H1137" s="22"/>
       <c r="I1137" s="23" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="J1137" s="23"/>
       <c r="K1137" s="23"/>
@@ -29930,9 +29937,11 @@
     <row r="1138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1138" s="9"/>
       <c r="B1138" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1138" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1138" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1138" s="22" t="s">
         <v>27</v>
       </c>
@@ -29945,7 +29954,7 @@
       <c r="G1138" s="22"/>
       <c r="H1138" s="22"/>
       <c r="I1138" s="23" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="J1138" s="23"/>
       <c r="K1138" s="23"/>
@@ -29953,9 +29962,11 @@
     <row r="1139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1139" s="9"/>
       <c r="B1139" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1139" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1139" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1139" s="22" t="s">
         <v>27</v>
       </c>
@@ -29968,7 +29979,7 @@
       <c r="G1139" s="22"/>
       <c r="H1139" s="22"/>
       <c r="I1139" s="23" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="J1139" s="23"/>
       <c r="K1139" s="23"/>
@@ -29976,11 +29987,9 @@
     <row r="1140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1140" s="9"/>
       <c r="B1140" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1140" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1140" s="26"/>
       <c r="D1140" s="22" t="s">
         <v>27</v>
       </c>
@@ -29993,7 +30002,7 @@
       <c r="G1140" s="22"/>
       <c r="H1140" s="22"/>
       <c r="I1140" s="23" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="J1140" s="23"/>
       <c r="K1140" s="23"/>
@@ -30001,11 +30010,9 @@
     <row r="1141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1141" s="9"/>
       <c r="B1141" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1141" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1141" s="26"/>
       <c r="D1141" s="22" t="s">
         <v>27</v>
       </c>
@@ -30018,7 +30025,7 @@
       <c r="G1141" s="22"/>
       <c r="H1141" s="22"/>
       <c r="I1141" s="23" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="J1141" s="23"/>
       <c r="K1141" s="23"/>
@@ -30026,7 +30033,7 @@
     <row r="1142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1142" s="9"/>
       <c r="B1142" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1142" s="26"/>
       <c r="D1142" s="22" t="s">
@@ -30041,7 +30048,7 @@
       <c r="G1142" s="22"/>
       <c r="H1142" s="22"/>
       <c r="I1142" s="23" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="J1142" s="23"/>
       <c r="K1142" s="23"/>
@@ -30049,7 +30056,7 @@
     <row r="1143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1143" s="9"/>
       <c r="B1143" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1143" s="26"/>
       <c r="D1143" s="22" t="s">
@@ -30064,7 +30071,7 @@
       <c r="G1143" s="22"/>
       <c r="H1143" s="22"/>
       <c r="I1143" s="23" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="J1143" s="23"/>
       <c r="K1143" s="23"/>
@@ -30072,7 +30079,7 @@
     <row r="1144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1144" s="9"/>
       <c r="B1144" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1144" s="26"/>
       <c r="D1144" s="22" t="s">
@@ -30087,7 +30094,7 @@
       <c r="G1144" s="22"/>
       <c r="H1144" s="22"/>
       <c r="I1144" s="23" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="J1144" s="23"/>
       <c r="K1144" s="23"/>
@@ -30095,7 +30102,7 @@
     <row r="1145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1145" s="9"/>
       <c r="B1145" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1145" s="26"/>
       <c r="D1145" s="22" t="s">
@@ -30110,7 +30117,7 @@
       <c r="G1145" s="22"/>
       <c r="H1145" s="22"/>
       <c r="I1145" s="23" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="J1145" s="23"/>
       <c r="K1145" s="23"/>
@@ -30118,9 +30125,11 @@
     <row r="1146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1146" s="9"/>
       <c r="B1146" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1146" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1146" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1146" s="22" t="s">
         <v>27</v>
       </c>
@@ -30133,7 +30142,7 @@
       <c r="G1146" s="22"/>
       <c r="H1146" s="22"/>
       <c r="I1146" s="23" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="J1146" s="23"/>
       <c r="K1146" s="23"/>
@@ -30141,9 +30150,11 @@
     <row r="1147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1147" s="9"/>
       <c r="B1147" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1147" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1147" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1147" s="22" t="s">
         <v>27</v>
       </c>
@@ -30156,7 +30167,7 @@
       <c r="G1147" s="22"/>
       <c r="H1147" s="22"/>
       <c r="I1147" s="23" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="J1147" s="23"/>
       <c r="K1147" s="23"/>
@@ -30164,11 +30175,9 @@
     <row r="1148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1148" s="9"/>
       <c r="B1148" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1148" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1148" s="26"/>
       <c r="D1148" s="22" t="s">
         <v>27</v>
       </c>
@@ -30181,7 +30190,7 @@
       <c r="G1148" s="22"/>
       <c r="H1148" s="22"/>
       <c r="I1148" s="23" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="J1148" s="23"/>
       <c r="K1148" s="23"/>
@@ -30189,11 +30198,9 @@
     <row r="1149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1149" s="9"/>
       <c r="B1149" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1149" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1149" s="26"/>
       <c r="D1149" s="22" t="s">
         <v>27</v>
       </c>
@@ -30206,7 +30213,7 @@
       <c r="G1149" s="22"/>
       <c r="H1149" s="22"/>
       <c r="I1149" s="23" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="J1149" s="23"/>
       <c r="K1149" s="23"/>
@@ -30214,9 +30221,11 @@
     <row r="1150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1150" s="9"/>
       <c r="B1150" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1150" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1150" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1150" s="22" t="s">
         <v>27</v>
       </c>
@@ -30229,7 +30238,7 @@
       <c r="G1150" s="22"/>
       <c r="H1150" s="22"/>
       <c r="I1150" s="23" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="J1150" s="23"/>
       <c r="K1150" s="23"/>
@@ -30237,9 +30246,11 @@
     <row r="1151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1151" s="9"/>
       <c r="B1151" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1151" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1151" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1151" s="22" t="s">
         <v>27</v>
       </c>
@@ -30252,7 +30263,7 @@
       <c r="G1151" s="22"/>
       <c r="H1151" s="22"/>
       <c r="I1151" s="23" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="J1151" s="23"/>
       <c r="K1151" s="23"/>
@@ -30260,7 +30271,7 @@
     <row r="1152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1152" s="9"/>
       <c r="B1152" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1152" s="22" t="s">
         <v>27</v>
@@ -30277,7 +30288,7 @@
       <c r="G1152" s="22"/>
       <c r="H1152" s="22"/>
       <c r="I1152" s="23" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="J1152" s="23"/>
       <c r="K1152" s="23"/>
@@ -30285,11 +30296,9 @@
     <row r="1153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1153" s="9"/>
       <c r="B1153" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1153" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="C1153" s="26"/>
       <c r="D1153" s="22" t="s">
         <v>27</v>
       </c>
@@ -30302,15 +30311,15 @@
       <c r="G1153" s="22"/>
       <c r="H1153" s="22"/>
       <c r="I1153" s="23" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="J1153" s="23"/>
       <c r="K1153" s="23"/>
     </row>
-    <row r="1154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1154" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1154" s="9"/>
       <c r="B1154" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1154" s="22" t="s">
         <v>27</v>
@@ -30327,7 +30336,7 @@
       <c r="G1154" s="22"/>
       <c r="H1154" s="22"/>
       <c r="I1154" s="23" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="J1154" s="23"/>
       <c r="K1154" s="23"/>
@@ -30335,9 +30344,11 @@
     <row r="1155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1155" s="9"/>
       <c r="B1155" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1155" s="26"/>
+        <v>1126</v>
+      </c>
+      <c r="C1155" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1155" s="22" t="s">
         <v>27</v>
       </c>
@@ -30350,15 +30361,15 @@
       <c r="G1155" s="22"/>
       <c r="H1155" s="22"/>
       <c r="I1155" s="23" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="J1155" s="23"/>
       <c r="K1155" s="23"/>
     </row>
-    <row r="1156" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1156" s="9"/>
       <c r="B1156" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1156" s="22" t="s">
         <v>27</v>
@@ -30375,7 +30386,7 @@
       <c r="G1156" s="22"/>
       <c r="H1156" s="22"/>
       <c r="I1156" s="23" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="J1156" s="23"/>
       <c r="K1156" s="23"/>
@@ -30383,7 +30394,7 @@
     <row r="1157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1157" s="9"/>
       <c r="B1157" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1157" s="22" t="s">
         <v>27</v>
@@ -30400,7 +30411,7 @@
       <c r="G1157" s="22"/>
       <c r="H1157" s="22"/>
       <c r="I1157" s="23" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="J1157" s="23"/>
       <c r="K1157" s="23"/>
@@ -30408,7 +30419,7 @@
     <row r="1158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1158" s="9"/>
       <c r="B1158" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1158" s="22" t="s">
         <v>27</v>
@@ -30425,7 +30436,7 @@
       <c r="G1158" s="22"/>
       <c r="H1158" s="22"/>
       <c r="I1158" s="23" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="J1158" s="23"/>
       <c r="K1158" s="23"/>
@@ -30433,7 +30444,7 @@
     <row r="1159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1159" s="9"/>
       <c r="B1159" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1159" s="22" t="s">
         <v>27</v>
@@ -30450,22 +30461,20 @@
       <c r="G1159" s="22"/>
       <c r="H1159" s="22"/>
       <c r="I1159" s="23" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="J1159" s="23"/>
       <c r="K1159" s="23"/>
     </row>
-    <row r="1160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1160" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1160" s="9"/>
       <c r="B1160" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1160" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1160" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="D1160" s="26"/>
       <c r="E1160" s="22" t="s">
         <v>27</v>
       </c>
@@ -30475,15 +30484,15 @@
       <c r="G1160" s="22"/>
       <c r="H1160" s="22"/>
       <c r="I1160" s="23" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="J1160" s="23"/>
       <c r="K1160" s="23"/>
     </row>
-    <row r="1161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1161" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1161" s="9"/>
       <c r="B1161" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1161" s="22" t="s">
         <v>27</v>
@@ -30500,20 +30509,22 @@
       <c r="G1161" s="22"/>
       <c r="H1161" s="22"/>
       <c r="I1161" s="23" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="J1161" s="23"/>
       <c r="K1161" s="23"/>
     </row>
-    <row r="1162" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1162" s="9"/>
       <c r="B1162" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1162" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1162" s="26"/>
+      <c r="D1162" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="E1162" s="22" t="s">
         <v>27</v>
       </c>
@@ -30523,15 +30534,15 @@
       <c r="G1162" s="22"/>
       <c r="H1162" s="22"/>
       <c r="I1162" s="23" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="J1162" s="23"/>
       <c r="K1162" s="23"/>
     </row>
-    <row r="1163" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1163" s="9"/>
       <c r="B1163" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1163" s="22" t="s">
         <v>27</v>
@@ -30548,7 +30559,7 @@
       <c r="G1163" s="22"/>
       <c r="H1163" s="22"/>
       <c r="I1163" s="23" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="J1163" s="23"/>
       <c r="K1163" s="23"/>
@@ -30556,7 +30567,7 @@
     <row r="1164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1164" s="9"/>
       <c r="B1164" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1164" s="22" t="s">
         <v>27</v>
@@ -30573,7 +30584,7 @@
       <c r="G1164" s="22"/>
       <c r="H1164" s="22"/>
       <c r="I1164" s="23" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="J1164" s="23"/>
       <c r="K1164" s="23"/>
@@ -30581,7 +30592,7 @@
     <row r="1165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1165" s="9"/>
       <c r="B1165" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1165" s="22" t="s">
         <v>27</v>
@@ -30598,40 +30609,38 @@
       <c r="G1165" s="22"/>
       <c r="H1165" s="22"/>
       <c r="I1165" s="23" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="J1165" s="23"/>
       <c r="K1165" s="23"/>
     </row>
     <row r="1166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1166" s="9"/>
-      <c r="B1166" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1166" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="B1166" s="28" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C1166" s="26"/>
       <c r="D1166" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1166" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1166" s="26"/>
       <c r="F1166" s="22" t="s">
         <v>683</v>
       </c>
       <c r="G1166" s="22"/>
       <c r="H1166" s="22"/>
       <c r="I1166" s="23" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="J1166" s="23"/>
-      <c r="K1166" s="23"/>
+      <c r="K1166" s="23" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="1167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1167" s="9"/>
       <c r="B1167" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1167" s="22" t="s">
         <v>27</v>
@@ -30648,38 +30657,40 @@
       <c r="G1167" s="22"/>
       <c r="H1167" s="22"/>
       <c r="I1167" s="23" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="J1167" s="23"/>
       <c r="K1167" s="23"/>
     </row>
     <row r="1168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1168" s="9"/>
-      <c r="B1168" s="28" t="s">
-        <v>1130</v>
-      </c>
-      <c r="C1168" s="26"/>
+      <c r="B1168" s="22" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C1168" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1168" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1168" s="26"/>
+      <c r="E1168" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1168" s="22" t="s">
         <v>683</v>
       </c>
       <c r="G1168" s="22"/>
       <c r="H1168" s="22"/>
       <c r="I1168" s="23" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="J1168" s="23"/>
-      <c r="K1168" s="23" t="s">
-        <v>655</v>
-      </c>
+      <c r="K1168" s="23"/>
     </row>
     <row r="1169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1169" s="9"/>
       <c r="B1169" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1169" s="22" t="s">
         <v>27</v>
@@ -30696,7 +30707,7 @@
       <c r="G1169" s="22"/>
       <c r="H1169" s="22"/>
       <c r="I1169" s="23" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="J1169" s="23"/>
       <c r="K1169" s="23"/>
@@ -30704,7 +30715,7 @@
     <row r="1170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1170" s="9"/>
       <c r="B1170" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1170" s="22" t="s">
         <v>27</v>
@@ -30721,15 +30732,15 @@
       <c r="G1170" s="22"/>
       <c r="H1170" s="22"/>
       <c r="I1170" s="23" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="J1170" s="23"/>
       <c r="K1170" s="23"/>
     </row>
-    <row r="1171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1171" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1171" s="9"/>
       <c r="B1171" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1171" s="22" t="s">
         <v>27</v>
@@ -30746,7 +30757,7 @@
       <c r="G1171" s="22"/>
       <c r="H1171" s="22"/>
       <c r="I1171" s="23" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="J1171" s="23"/>
       <c r="K1171" s="23"/>
@@ -30754,7 +30765,7 @@
     <row r="1172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1172" s="9"/>
       <c r="B1172" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1172" s="22" t="s">
         <v>27</v>
@@ -30771,15 +30782,15 @@
       <c r="G1172" s="22"/>
       <c r="H1172" s="22"/>
       <c r="I1172" s="23" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="J1172" s="23"/>
       <c r="K1172" s="23"/>
     </row>
-    <row r="1173" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1173" s="9"/>
       <c r="B1173" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1173" s="22" t="s">
         <v>27</v>
@@ -30796,15 +30807,14 @@
       <c r="G1173" s="22"/>
       <c r="H1173" s="22"/>
       <c r="I1173" s="23" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="J1173" s="23"/>
       <c r="K1173" s="23"/>
     </row>
     <row r="1174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1174" s="9"/>
       <c r="B1174" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1174" s="22" t="s">
         <v>27</v>
@@ -30821,15 +30831,14 @@
       <c r="G1174" s="22"/>
       <c r="H1174" s="22"/>
       <c r="I1174" s="23" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="J1174" s="23"/>
       <c r="K1174" s="23"/>
     </row>
-    <row r="1175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1175" s="9"/>
+    <row r="1175" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1175" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1175" s="22" t="s">
         <v>27</v>
@@ -30846,14 +30855,14 @@
       <c r="G1175" s="22"/>
       <c r="H1175" s="22"/>
       <c r="I1175" s="23" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="J1175" s="23"/>
       <c r="K1175" s="23"/>
     </row>
-    <row r="1176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1176" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1176" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1176" s="22" t="s">
         <v>27</v>
@@ -30870,14 +30879,14 @@
       <c r="G1176" s="22"/>
       <c r="H1176" s="22"/>
       <c r="I1176" s="23" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="J1176" s="23"/>
       <c r="K1176" s="23"/>
     </row>
     <row r="1177" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1177" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1177" s="22" t="s">
         <v>27</v>
@@ -30894,14 +30903,14 @@
       <c r="G1177" s="22"/>
       <c r="H1177" s="22"/>
       <c r="I1177" s="23" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="J1177" s="23"/>
       <c r="K1177" s="23"/>
     </row>
-    <row r="1178" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1178" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1178" s="22" t="s">
         <v>27</v>
@@ -30918,14 +30927,14 @@
       <c r="G1178" s="22"/>
       <c r="H1178" s="22"/>
       <c r="I1178" s="23" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="J1178" s="23"/>
       <c r="K1178" s="23"/>
     </row>
     <row r="1179" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1179" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1179" s="22" t="s">
         <v>27</v>
@@ -30942,14 +30951,14 @@
       <c r="G1179" s="22"/>
       <c r="H1179" s="22"/>
       <c r="I1179" s="23" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="J1179" s="23"/>
       <c r="K1179" s="23"/>
     </row>
-    <row r="1180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1180" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1180" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1180" s="22" t="s">
         <v>27</v>
@@ -30966,14 +30975,14 @@
       <c r="G1180" s="22"/>
       <c r="H1180" s="22"/>
       <c r="I1180" s="23" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="J1180" s="23"/>
       <c r="K1180" s="23"/>
     </row>
     <row r="1181" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1181" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1181" s="22" t="s">
         <v>27</v>
@@ -30990,14 +30999,14 @@
       <c r="G1181" s="22"/>
       <c r="H1181" s="22"/>
       <c r="I1181" s="23" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="J1181" s="23"/>
       <c r="K1181" s="23"/>
     </row>
-    <row r="1182" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1182" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1182" s="22" t="s">
         <v>27</v>
@@ -31014,38 +31023,36 @@
       <c r="G1182" s="22"/>
       <c r="H1182" s="22"/>
       <c r="I1182" s="23" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="J1182" s="23"/>
       <c r="K1182" s="23"/>
     </row>
-    <row r="1183" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1183" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1183" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1183" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1183" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1183" s="22" t="s">
+    <row r="1183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1183" s="28" t="s">
         <v>683</v>
       </c>
-      <c r="G1183" s="22"/>
-      <c r="H1183" s="22"/>
-      <c r="I1183" s="23" t="s">
-        <v>1214</v>
-      </c>
-      <c r="J1183" s="23"/>
-      <c r="K1183" s="23"/>
-    </row>
-    <row r="1184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1183" s="28"/>
+      <c r="D1183" s="28" t="s">
+        <v>683</v>
+      </c>
+      <c r="E1183" s="28"/>
+      <c r="F1183" s="28" t="s">
+        <v>683</v>
+      </c>
+      <c r="G1183" s="28"/>
+      <c r="H1183" s="28"/>
+      <c r="I1183" s="29" t="s">
+        <v>1215</v>
+      </c>
+      <c r="J1183" s="29"/>
+      <c r="K1183" s="29" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="1184" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1184" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C1184" s="22" t="s">
         <v>27</v>
@@ -31057,15 +31064,17 @@
         <v>27</v>
       </c>
       <c r="F1184" s="22" t="s">
-        <v>683</v>
+        <v>1143</v>
       </c>
       <c r="G1184" s="22"/>
       <c r="H1184" s="22"/>
       <c r="I1184" s="23" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
       <c r="J1184" s="23"/>
-      <c r="K1184" s="23"/>
+      <c r="K1184" s="23" t="s">
+        <v>1218</v>
+      </c>
     </row>
     <row r="1185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1185" s="28" t="s">
@@ -31082,61 +31091,16 @@
       <c r="G1185" s="28"/>
       <c r="H1185" s="28"/>
       <c r="I1185" s="29" t="s">
-        <v>1216</v>
+        <v>1219</v>
       </c>
       <c r="J1185" s="29"/>
       <c r="K1185" s="29" t="s">
-        <v>1217</v>
-      </c>
-    </row>
-    <row r="1186" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1186" s="22" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C1186" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1186" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1186" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1186" s="22" t="s">
-        <v>1144</v>
-      </c>
-      <c r="G1186" s="22"/>
-      <c r="H1186" s="22"/>
-      <c r="I1186" s="23" t="s">
-        <v>1218</v>
-      </c>
-      <c r="J1186" s="23"/>
-      <c r="K1186" s="23" t="s">
-        <v>1219</v>
-      </c>
-    </row>
-    <row r="1187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1187" s="28" t="s">
-        <v>683</v>
-      </c>
-      <c r="C1187" s="28"/>
-      <c r="D1187" s="28" t="s">
-        <v>683</v>
-      </c>
-      <c r="E1187" s="28"/>
-      <c r="F1187" s="28" t="s">
-        <v>683</v>
-      </c>
-      <c r="G1187" s="28"/>
-      <c r="H1187" s="28"/>
-      <c r="I1187" s="29" t="s">
-        <v>1220</v>
-      </c>
-      <c r="J1187" s="29"/>
-      <c r="K1187" s="29" t="s">
-        <v>1217</v>
-      </c>
-    </row>
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.766666666666667" header="0.511805555555555" footer="0.5"/>

</xml_diff>

<commit_message>
update menu with LQR_NEW_N
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5674" uniqueCount="1265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5675" uniqueCount="1265">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -4271,7 +4271,7 @@
   <dimension ref="A1:Q1226"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A785" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A801" activeCellId="0" sqref="A801"/>
+      <selection pane="topLeft" activeCell="E802" activeCellId="0" sqref="E802"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="E9" s="13" t="n">
         <f aca="false">COUNTIF(E18:E1553,"X")</f>
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F9" s="13" t="n">
         <f aca="false">COUNTIF(F18:F1553,"S")+COUNTIF(F18:F1553,"I")+COUNTIF(F18:F1553,"X")+COUNTIF(F18:F1553,"SI")+COUNTIF(F18:F1553,"IS")+COUNTIF(F18:F1553,"N/A")</f>
@@ -21843,7 +21843,9 @@
         <v>27</v>
       </c>
       <c r="D803" s="22"/>
-      <c r="E803" s="26"/>
+      <c r="E803" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F803" s="26"/>
       <c r="G803" s="22"/>
       <c r="H803" s="22"/>

</xml_diff>

<commit_message>
Add Kn (overall normalizing gain) to PID and advPID tuning
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5720" uniqueCount="1275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5725" uniqueCount="1275">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -4300,8 +4300,8 @@
   </sheetPr>
   <dimension ref="A1:Q1237"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="E9" s="13" t="n">
         <f aca="false">COUNTIF(E18:E1564,"X")</f>
-        <v>771</v>
+        <v>776</v>
       </c>
       <c r="F9" s="13" t="n">
         <f aca="false">COUNTIF(F18:F1564,"S")+COUNTIF(F18:F1564,"I")+COUNTIF(F18:F1564,"X")+COUNTIF(F18:F1564,"SI")+COUNTIF(F18:F1564,"IS")+COUNTIF(F18:F1564,"N/A")</f>
@@ -5854,7 +5854,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="21" t="s">
         <v>84</v>
       </c>
@@ -5865,7 +5865,9 @@
         <v>27</v>
       </c>
       <c r="D77" s="22"/>
-      <c r="E77" s="26"/>
+      <c r="E77" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F77" s="26"/>
       <c r="G77" s="22"/>
       <c r="H77" s="22"/>
@@ -5875,7 +5877,7 @@
       <c r="J77" s="23"/>
       <c r="K77" s="23"/>
     </row>
-    <row r="78" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="21"/>
       <c r="B78" s="22" t="s">
         <v>27</v>
@@ -5884,7 +5886,9 @@
         <v>27</v>
       </c>
       <c r="D78" s="22"/>
-      <c r="E78" s="26"/>
+      <c r="E78" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F78" s="26"/>
       <c r="G78" s="22"/>
       <c r="H78" s="22"/>
@@ -5894,7 +5898,7 @@
       <c r="J78" s="23"/>
       <c r="K78" s="23"/>
     </row>
-    <row r="79" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="19"/>
       <c r="B79" s="22" t="s">
         <v>27</v>
@@ -5905,7 +5909,9 @@
       <c r="D79" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E79" s="26"/>
+      <c r="E79" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F79" s="26"/>
       <c r="G79" s="22"/>
       <c r="H79" s="22"/>
@@ -30374,7 +30380,9 @@
       <c r="D1157" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1157" s="26"/>
+      <c r="E1157" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1157" s="22" t="s">
         <v>700</v>
       </c>
@@ -30397,7 +30405,9 @@
       <c r="D1158" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1158" s="26"/>
+      <c r="E1158" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1158" s="22" t="s">
         <v>700</v>
       </c>

</xml_diff>

<commit_message>
Update menus for new interpolate functions.
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5741" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5747" uniqueCount="1279">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -4312,8 +4312,8 @@
   </sheetPr>
   <dimension ref="A1:Q1241"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A282" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C296" activeCellId="0" sqref="C296"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1147" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1155" activeCellId="0" sqref="A1155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4432,15 +4432,15 @@
       </c>
       <c r="D9" s="13" t="n">
         <f aca="false">COUNTIF(D18:D1568,"X")</f>
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E9" s="13" t="n">
         <f aca="false">COUNTIF(E18:E1568,"X")</f>
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="F9" s="13" t="n">
         <f aca="false">COUNTIF(F18:F1568,"S")+COUNTIF(F18:F1568,"I")+COUNTIF(F18:F1568,"X")+COUNTIF(F18:F1568,"SI")+COUNTIF(F18:F1568,"IS")+COUNTIF(F18:F1568,"N/A")</f>
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G9" s="13" t="n">
         <f aca="false">COUNTIF(G18:G1568,"S")+COUNTIF(G18:G1568,"I")+COUNTIF(G18:G1568,"X")+COUNTIF(G18:G1568,"SI")+COUNTIF(G18:G1568,"IS")+COUNTIF(G18:G1568,"N/A")</f>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.526315789473684</v>
+        <v>0.527539779681763</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8263,7 +8263,7 @@
       <c r="J186" s="23"/>
       <c r="K186" s="23"/>
     </row>
-    <row r="187" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="19"/>
       <c r="B187" s="22" t="s">
         <v>27</v>
@@ -8277,7 +8277,9 @@
       <c r="E187" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F187" s="26"/>
+      <c r="F187" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G187" s="22"/>
       <c r="H187" s="22"/>
       <c r="I187" s="23" t="s">
@@ -9622,7 +9624,9 @@
         <v>27</v>
       </c>
       <c r="D245" s="22"/>
-      <c r="E245" s="26"/>
+      <c r="E245" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F245" s="22" t="s">
         <v>28</v>
       </c>
@@ -10144,7 +10148,9 @@
         <v>27</v>
       </c>
       <c r="D266" s="22"/>
-      <c r="E266" s="26"/>
+      <c r="E266" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F266" s="22" t="s">
         <v>30</v>
       </c>
@@ -10872,7 +10878,9 @@
         <v>27</v>
       </c>
       <c r="D296" s="22"/>
-      <c r="E296" s="26"/>
+      <c r="E296" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F296" s="22" t="s">
         <v>30</v>
       </c>
@@ -28989,7 +28997,9 @@
         <v>27</v>
       </c>
       <c r="D1098" s="22"/>
-      <c r="E1098" s="26"/>
+      <c r="E1098" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1098" s="22" t="s">
         <v>338</v>
       </c>
@@ -31846,7 +31856,7 @@
       <c r="J1215" s="23"/>
       <c r="K1215" s="23"/>
     </row>
-    <row r="1216" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1216" s="9"/>
       <c r="B1216" s="22" t="s">
         <v>1182</v>
@@ -31854,7 +31864,9 @@
       <c r="C1216" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1216" s="26"/>
+      <c r="D1216" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="E1216" s="22" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Complete update of numerical integration #29
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5774" uniqueCount="1284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5784" uniqueCount="1289">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -3496,12 +3496,12 @@
     <t xml:space="preserve">NumIntegrate_Rkdp_Func_B1.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">NumIntegrate_Rkdp_Func_B1B2.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">NumIntegrate_Rkdp_Func_B2.vi</t>
   </si>
   <si>
-    <t xml:space="preserve">NumIntegrate_Rkdp_Func_B1B2.vi</t>
-  </si>
-  <si>
     <t xml:space="preserve">Numintegrate_Rkdp_Impl.vi</t>
   </si>
   <si>
@@ -3511,9 +3511,24 @@
     <t xml:space="preserve">New replacement for RKF45</t>
   </si>
   <si>
+    <t xml:space="preserve">NumIntegrate_Rkf45_Func_A.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Rkf45_Func_B1.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Rkf45_Func_B1B2.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumIntegrate_Rkf45_Func_B2.vi</t>
+  </si>
+  <si>
     <t xml:space="preserve">NumIntegrate_RKf45_Func_Bs.vi</t>
   </si>
   <si>
+    <t xml:space="preserve">Removed.  Replaced with newer functions.</t>
+  </si>
+  <si>
     <t xml:space="preserve">NumIntegrate_RKf45_Func_Ch.vi</t>
   </si>
   <si>
@@ -3532,7 +3547,7 @@
     <t xml:space="preserve">NumIntegrate_RKf45_New.vi</t>
   </si>
   <si>
-    <t xml:space="preserve">New for using new refactored values.  Work In Progress…</t>
+    <t xml:space="preserve">Removed.  Never used.</t>
   </si>
   <si>
     <t xml:space="preserve">NumIntegrate_Trap_Dbl.vi</t>
@@ -3935,7 +3950,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4002,6 +4017,12 @@
         <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
@@ -4051,7 +4072,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4248,6 +4269,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4273,7 +4298,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -4325,10 +4350,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:Q1246"/>
+  <dimension ref="A1:Q1250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1107" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1118" activeCellId="0" sqref="F1118"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1127" activeCellId="0" sqref="A1127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4439,30 +4464,30 @@
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">B10+B11</f>
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C18:C1573,"X")</f>
-        <v>823</v>
+        <f aca="false">COUNTIF(C18:C1577,"X")</f>
+        <v>824</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D18:D1573,"X")</f>
+        <f aca="false">COUNTIF(D18:D1577,"X")</f>
         <v>248</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E18:E1573,"X")</f>
+        <f aca="false">COUNTIF(E18:E1577,"X")</f>
         <v>781</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F18:F1573,"S")+COUNTIF(F18:F1573,"I")+COUNTIF(F18:F1573,"X")+COUNTIF(F18:F1573,"SI")+COUNTIF(F18:F1573,"IS")+COUNTIF(F18:F1573,"N/A")</f>
-        <v>436</v>
+        <f aca="false">COUNTIF(F18:F1577,"S")+COUNTIF(F18:F1577,"I")+COUNTIF(F18:F1577,"X")+COUNTIF(F18:F1577,"SI")+COUNTIF(F18:F1577,"IS")+COUNTIF(F18:F1577,"N/A")</f>
+        <v>437</v>
       </c>
       <c r="G9" s="13" t="n">
-        <f aca="false">COUNTIF(G18:G1573,"S")+COUNTIF(G18:G1573,"I")+COUNTIF(G18:G1573,"X")+COUNTIF(G18:G1573,"SI")+COUNTIF(G18:G1573,"IS")+COUNTIF(G18:G1573,"N/A")</f>
+        <f aca="false">COUNTIF(G18:G1577,"S")+COUNTIF(G18:G1577,"I")+COUNTIF(G18:G1577,"X")+COUNTIF(G18:G1577,"SI")+COUNTIF(G18:G1577,"IS")+COUNTIF(G18:G1577,"N/A")</f>
         <v>26</v>
       </c>
       <c r="H9" s="13" t="n">
-        <f aca="false">COUNTIF(H18:H1573,"S")+COUNTIF(H18:H1573,"I")+COUNTIF(H18:H1573,"X")+COUNTIF(H18:H1573,"SI")+COUNTIF(H18:H1573,"IS")+COUNTIF(H18:H1573,"N/A")</f>
+        <f aca="false">COUNTIF(H18:H1577,"S")+COUNTIF(H18:H1577,"I")+COUNTIF(H18:H1577,"X")+COUNTIF(H18:H1577,"SI")+COUNTIF(H18:H1577,"IS")+COUNTIF(H18:H1577,"N/A")</f>
         <v>12</v>
       </c>
       <c r="I9" s="14" t="n">
@@ -4475,8 +4500,8 @@
         <v>14</v>
       </c>
       <c r="B10" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1573,"X")</f>
-        <v>738</v>
+        <f aca="false">COUNTIF(B18:B1577,"X")</f>
+        <v>739</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>15</v>
@@ -4487,12 +4512,12 @@
         <v>16</v>
       </c>
       <c r="B11" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1573,"Z")</f>
+        <f aca="false">COUNTIF(B18:B1577,"Z")</f>
         <v>85</v>
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.529769137302552</v>
+        <v>0.530339805825243</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4500,8 +4525,8 @@
         <v>17</v>
       </c>
       <c r="B12" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1573,"/")</f>
-        <v>5</v>
+        <f aca="false">COUNTIF(B18:B1577,"/")</f>
+        <v>4</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -4510,7 +4535,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1573,"\")</f>
+        <f aca="false">COUNTIF(B18:B1577,"\")</f>
         <v>2</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -29405,7 +29430,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="1114" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1114" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1114" s="21" t="s">
         <v>1148</v>
       </c>
@@ -29435,7 +29460,7 @@
       <c r="M1114" s="22"/>
       <c r="N1114" s="22"/>
     </row>
-    <row r="1115" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1115" s="22" t="s">
         <v>27</v>
       </c>
@@ -29458,7 +29483,7 @@
       <c r="M1115" s="22"/>
       <c r="N1115" s="22"/>
     </row>
-    <row r="1116" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1116" s="22" t="s">
         <v>27</v>
       </c>
@@ -29504,7 +29529,7 @@
       <c r="M1117" s="22"/>
       <c r="N1117" s="22"/>
     </row>
-    <row r="1118" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1118" s="22" t="s">
         <v>27</v>
       </c>
@@ -29764,7 +29789,7 @@
         <v>35</v>
       </c>
       <c r="F1128" s="22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G1128" s="22"/>
       <c r="H1128" s="22"/>
@@ -29777,24 +29802,18 @@
       <c r="M1128" s="22"/>
       <c r="N1128" s="22"/>
     </row>
-    <row r="1129" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1129" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1129" s="22" t="s">
-        <v>27</v>
-      </c>
+    <row r="1129" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1129" s="49"/>
+      <c r="C1129" s="49"/>
       <c r="D1129" s="22"/>
-      <c r="E1129" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1129" s="26"/>
+      <c r="E1129" s="49"/>
+      <c r="F1129" s="49"/>
       <c r="G1129" s="22"/>
       <c r="H1129" s="22"/>
       <c r="I1129" s="23" t="s">
         <v>1166</v>
       </c>
-      <c r="J1129" s="0"/>
+      <c r="J1129" s="23"/>
       <c r="K1129" s="23" t="s">
         <v>1167</v>
       </c>
@@ -29803,13 +29822,11 @@
       <c r="N1129" s="22"/>
     </row>
     <row r="1130" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1130" s="28" t="s">
-        <v>673</v>
-      </c>
-      <c r="C1130" s="22"/>
+      <c r="B1130" s="49"/>
+      <c r="C1130" s="49"/>
       <c r="D1130" s="22"/>
-      <c r="E1130" s="22"/>
-      <c r="F1130" s="22"/>
+      <c r="E1130" s="49"/>
+      <c r="F1130" s="49"/>
       <c r="G1130" s="22"/>
       <c r="H1130" s="22"/>
       <c r="I1130" s="23" t="s">
@@ -29817,35 +29834,27 @@
       </c>
       <c r="J1130" s="23"/>
       <c r="K1130" s="23" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="L1130" s="22"/>
       <c r="M1130" s="22"/>
       <c r="N1130" s="22"/>
     </row>
-    <row r="1131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1131" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1131" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1131" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1131" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1131" s="22" t="s">
-        <v>30</v>
-      </c>
+    <row r="1131" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1131" s="49"/>
+      <c r="C1131" s="49"/>
+      <c r="D1131" s="22"/>
+      <c r="E1131" s="49"/>
+      <c r="F1131" s="49"/>
       <c r="G1131" s="22"/>
       <c r="H1131" s="22"/>
       <c r="I1131" s="23" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="J1131" s="23"/>
-      <c r="K1131" s="23"/>
+      <c r="K1131" s="23" t="s">
+        <v>1167</v>
+      </c>
       <c r="L1131" s="22"/>
       <c r="M1131" s="22"/>
       <c r="N1131" s="22"/>
@@ -29857,11 +29866,9 @@
       <c r="C1132" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1132" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="D1132" s="22"/>
       <c r="E1132" s="22" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F1132" s="22" t="s">
         <v>28</v>
@@ -29869,7 +29876,7 @@
       <c r="G1132" s="22"/>
       <c r="H1132" s="22"/>
       <c r="I1132" s="23" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="J1132" s="23"/>
       <c r="K1132" s="23"/>
@@ -29877,97 +29884,97 @@
       <c r="M1132" s="22"/>
       <c r="N1132" s="22"/>
     </row>
-    <row r="1133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1133" s="22"/>
-      <c r="C1133" s="22"/>
+    <row r="1133" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1133" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1133" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1133" s="22"/>
-      <c r="E1133" s="22"/>
-      <c r="F1133" s="22"/>
+      <c r="E1133" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1133" s="26"/>
       <c r="G1133" s="22"/>
       <c r="H1133" s="22"/>
-      <c r="I1133" s="23"/>
-      <c r="J1133" s="23"/>
-      <c r="K1133" s="23"/>
+      <c r="I1133" s="23" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J1133" s="0"/>
+      <c r="K1133" s="23" t="s">
+        <v>1172</v>
+      </c>
       <c r="L1133" s="22"/>
       <c r="M1133" s="22"/>
       <c r="N1133" s="22"/>
     </row>
     <row r="1134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1134" s="47"/>
-      <c r="C1134" s="1"/>
-      <c r="D1134" s="1"/>
-      <c r="E1134" s="1"/>
-      <c r="F1134" s="1"/>
-      <c r="G1134" s="1"/>
-      <c r="H1134" s="1"/>
-      <c r="I1134" s="1"/>
-      <c r="J1134" s="1"/>
-      <c r="K1134" s="1"/>
-      <c r="L1134" s="1"/>
-      <c r="M1134" s="1"/>
-      <c r="N1134" s="1"/>
-    </row>
-    <row r="1135" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1135" s="19"/>
-      <c r="B1135" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1135" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1135" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1135" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1135" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1135" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1135" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1135" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1135" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1135" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1135" s="11" t="s">
-        <v>760</v>
-      </c>
-      <c r="M1135" s="11" t="s">
-        <v>761</v>
-      </c>
-      <c r="N1135" s="11" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="1136" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1136" s="21" t="s">
-        <v>1172</v>
-      </c>
+      <c r="B1134" s="49"/>
+      <c r="C1134" s="49"/>
+      <c r="D1134" s="22"/>
+      <c r="E1134" s="49"/>
+      <c r="F1134" s="49"/>
+      <c r="G1134" s="22"/>
+      <c r="H1134" s="22"/>
+      <c r="I1134" s="23" t="s">
+        <v>1173</v>
+      </c>
+      <c r="J1134" s="23"/>
+      <c r="K1134" s="23" t="s">
+        <v>1174</v>
+      </c>
+      <c r="L1134" s="22"/>
+      <c r="M1134" s="22"/>
+      <c r="N1134" s="22"/>
+    </row>
+    <row r="1135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1135" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1135" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1135" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1135" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1135" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1135" s="22"/>
+      <c r="H1135" s="22"/>
+      <c r="I1135" s="23" t="s">
+        <v>1175</v>
+      </c>
+      <c r="J1135" s="23"/>
+      <c r="K1135" s="23"/>
+      <c r="L1135" s="22"/>
+      <c r="M1135" s="22"/>
+      <c r="N1135" s="22"/>
+    </row>
+    <row r="1136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1136" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C1136" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1136" s="22"/>
+      <c r="D1136" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="E1136" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1136" s="26"/>
+        <v>27</v>
+      </c>
+      <c r="F1136" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="G1136" s="22"/>
       <c r="H1136" s="22"/>
       <c r="I1136" s="23" t="s">
-        <v>1173</v>
+        <v>1176</v>
       </c>
       <c r="J1136" s="23"/>
       <c r="K1136" s="23"/>
@@ -30049,7 +30056,7 @@
     </row>
     <row r="1140" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1140" s="21" t="s">
-        <v>1174</v>
+        <v>1177</v>
       </c>
       <c r="B1140" s="22" t="s">
         <v>27</v>
@@ -30059,13 +30066,13 @@
       </c>
       <c r="D1140" s="22"/>
       <c r="E1140" s="22" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F1140" s="26"/>
       <c r="G1140" s="22"/>
       <c r="H1140" s="22"/>
       <c r="I1140" s="23" t="s">
-        <v>1175</v>
+        <v>1178</v>
       </c>
       <c r="J1140" s="23"/>
       <c r="K1140" s="23"/>
@@ -30074,22 +30081,14 @@
       <c r="N1140" s="22"/>
     </row>
     <row r="1141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1141" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1141" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="B1141" s="22"/>
+      <c r="C1141" s="22"/>
       <c r="D1141" s="22"/>
-      <c r="E1141" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1141" s="26"/>
+      <c r="E1141" s="22"/>
+      <c r="F1141" s="22"/>
       <c r="G1141" s="22"/>
       <c r="H1141" s="22"/>
-      <c r="I1141" s="23" t="s">
-        <v>1176</v>
-      </c>
+      <c r="I1141" s="23"/>
       <c r="J1141" s="23"/>
       <c r="K1141" s="23"/>
       <c r="L1141" s="22"/>
@@ -30097,83 +30096,89 @@
       <c r="N1141" s="22"/>
     </row>
     <row r="1142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1142" s="22"/>
-      <c r="C1142" s="22"/>
-      <c r="D1142" s="22"/>
-      <c r="E1142" s="22"/>
-      <c r="F1142" s="22"/>
-      <c r="G1142" s="22"/>
-      <c r="H1142" s="22"/>
-      <c r="I1142" s="23"/>
-      <c r="J1142" s="23"/>
-      <c r="K1142" s="23"/>
-      <c r="L1142" s="22"/>
-      <c r="M1142" s="22"/>
-      <c r="N1142" s="22"/>
-    </row>
-    <row r="1143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1143" s="1"/>
-      <c r="C1143" s="1"/>
-      <c r="D1143" s="1"/>
-      <c r="E1143" s="1"/>
-      <c r="F1143" s="1"/>
-      <c r="G1143" s="1"/>
-      <c r="H1143" s="1"/>
-      <c r="I1143" s="1"/>
-      <c r="J1143" s="1"/>
-      <c r="K1143" s="1"/>
-      <c r="L1143" s="1"/>
-      <c r="M1143" s="1"/>
-      <c r="N1143" s="1"/>
-      <c r="O1143" s="1"/>
-      <c r="P1143" s="1"/>
-    </row>
-    <row r="1144" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1144" s="19"/>
-      <c r="B1144" s="11" t="s">
+      <c r="B1142" s="47"/>
+      <c r="C1142" s="1"/>
+      <c r="D1142" s="1"/>
+      <c r="E1142" s="1"/>
+      <c r="F1142" s="1"/>
+      <c r="G1142" s="1"/>
+      <c r="H1142" s="1"/>
+      <c r="I1142" s="1"/>
+      <c r="J1142" s="1"/>
+      <c r="K1142" s="1"/>
+      <c r="L1142" s="1"/>
+      <c r="M1142" s="1"/>
+      <c r="N1142" s="1"/>
+    </row>
+    <row r="1143" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1143" s="19"/>
+      <c r="B1143" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1144" s="11" t="s">
+      <c r="C1143" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1144" s="11" t="s">
+      <c r="D1143" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1144" s="11" t="s">
+      <c r="E1143" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1144" s="11" t="s">
+      <c r="F1143" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G1144" s="11" t="s">
+      <c r="G1143" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1144" s="11" t="s">
+      <c r="H1143" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1144" s="20" t="s">
+      <c r="I1143" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1144" s="20" t="s">
+      <c r="J1143" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1144" s="20" t="s">
+      <c r="K1143" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L1144" s="11" t="s">
+      <c r="L1143" s="11" t="s">
         <v>760</v>
       </c>
-      <c r="M1144" s="11" t="s">
+      <c r="M1143" s="11" t="s">
         <v>761</v>
       </c>
-      <c r="N1144" s="11" t="s">
+      <c r="N1143" s="11" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="1145" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1145" s="21" t="s">
-        <v>1177</v>
-      </c>
+    <row r="1144" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1144" s="21" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B1144" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1144" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1144" s="22"/>
+      <c r="E1144" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1144" s="26"/>
+      <c r="G1144" s="22"/>
+      <c r="H1144" s="22"/>
+      <c r="I1144" s="23" t="s">
+        <v>1180</v>
+      </c>
+      <c r="J1144" s="23"/>
+      <c r="K1144" s="23"/>
+      <c r="L1144" s="22"/>
+      <c r="M1144" s="22"/>
+      <c r="N1144" s="22"/>
+    </row>
+    <row r="1145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1145" s="22" t="s">
         <v>27</v>
       </c>
@@ -30188,90 +30193,92 @@
       <c r="G1145" s="22"/>
       <c r="H1145" s="22"/>
       <c r="I1145" s="23" t="s">
-        <v>1178</v>
+        <v>1181</v>
       </c>
       <c r="J1145" s="23"/>
-      <c r="K1145" s="23" t="s">
-        <v>675</v>
-      </c>
+      <c r="K1145" s="23"/>
       <c r="L1145" s="22"/>
       <c r="M1145" s="22"/>
       <c r="N1145" s="22"/>
     </row>
-    <row r="1146" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1146" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1146" s="22" t="s">
-        <v>27</v>
-      </c>
+    <row r="1146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1146" s="22"/>
+      <c r="C1146" s="22"/>
       <c r="D1146" s="22"/>
-      <c r="E1146" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1146" s="26"/>
+      <c r="E1146" s="22"/>
+      <c r="F1146" s="22"/>
       <c r="G1146" s="22"/>
       <c r="H1146" s="22"/>
-      <c r="I1146" s="23" t="s">
-        <v>1179</v>
-      </c>
+      <c r="I1146" s="23"/>
       <c r="J1146" s="23"/>
-      <c r="K1146" s="23" t="s">
-        <v>1180</v>
-      </c>
+      <c r="K1146" s="23"/>
       <c r="L1146" s="22"/>
       <c r="M1146" s="22"/>
       <c r="N1146" s="22"/>
     </row>
-    <row r="1147" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1147" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1147" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1147" s="22"/>
-      <c r="E1147" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1147" s="26"/>
-      <c r="G1147" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1147" s="22"/>
-      <c r="I1147" s="23" t="s">
-        <v>1181</v>
-      </c>
-      <c r="J1147" s="23"/>
-      <c r="K1147" s="23"/>
-      <c r="L1147" s="22"/>
-      <c r="M1147" s="22"/>
-      <c r="N1147" s="22"/>
-    </row>
-    <row r="1148" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1148" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1148" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1148" s="22"/>
-      <c r="E1148" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1148" s="26"/>
-      <c r="G1148" s="22"/>
-      <c r="H1148" s="22"/>
-      <c r="I1148" s="23" t="s">
+    <row r="1147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1147" s="1"/>
+      <c r="C1147" s="1"/>
+      <c r="D1147" s="1"/>
+      <c r="E1147" s="1"/>
+      <c r="F1147" s="1"/>
+      <c r="G1147" s="1"/>
+      <c r="H1147" s="1"/>
+      <c r="I1147" s="1"/>
+      <c r="J1147" s="1"/>
+      <c r="K1147" s="1"/>
+      <c r="L1147" s="1"/>
+      <c r="M1147" s="1"/>
+      <c r="N1147" s="1"/>
+      <c r="O1147" s="1"/>
+      <c r="P1147" s="1"/>
+    </row>
+    <row r="1148" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1148" s="19"/>
+      <c r="B1148" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1148" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1148" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1148" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1148" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1148" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1148" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1148" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1148" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1148" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1148" s="11" t="s">
+        <v>760</v>
+      </c>
+      <c r="M1148" s="11" t="s">
+        <v>761</v>
+      </c>
+      <c r="N1148" s="11" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="1149" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1149" s="21" t="s">
         <v>1182</v>
       </c>
-      <c r="J1148" s="23"/>
-      <c r="K1148" s="23"/>
-      <c r="L1148" s="22"/>
-      <c r="M1148" s="22"/>
-      <c r="N1148" s="22"/>
-    </row>
-    <row r="1149" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1149" s="22" t="s">
         <v>27</v>
       </c>
@@ -30283,15 +30290,15 @@
         <v>27</v>
       </c>
       <c r="F1149" s="26"/>
-      <c r="G1149" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="G1149" s="22"/>
       <c r="H1149" s="22"/>
       <c r="I1149" s="23" t="s">
         <v>1183</v>
       </c>
       <c r="J1149" s="23"/>
-      <c r="K1149" s="23"/>
+      <c r="K1149" s="23" t="s">
+        <v>675</v>
+      </c>
       <c r="L1149" s="22"/>
       <c r="M1149" s="22"/>
       <c r="N1149" s="22"/>
@@ -30314,219 +30321,217 @@
         <v>1184</v>
       </c>
       <c r="J1150" s="23"/>
-      <c r="K1150" s="23"/>
+      <c r="K1150" s="23" t="s">
+        <v>1185</v>
+      </c>
       <c r="L1150" s="22"/>
       <c r="M1150" s="22"/>
       <c r="N1150" s="22"/>
     </row>
-    <row r="1151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1151" s="22"/>
-      <c r="C1151" s="22"/>
+    <row r="1151" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1151" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1151" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1151" s="22"/>
-      <c r="E1151" s="22"/>
-      <c r="F1151" s="22"/>
-      <c r="G1151" s="22"/>
+      <c r="E1151" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1151" s="26"/>
+      <c r="G1151" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="H1151" s="22"/>
-      <c r="I1151" s="23"/>
+      <c r="I1151" s="23" t="s">
+        <v>1186</v>
+      </c>
       <c r="J1151" s="23"/>
       <c r="K1151" s="23"/>
       <c r="L1151" s="22"/>
       <c r="M1151" s="22"/>
       <c r="N1151" s="22"/>
     </row>
-    <row r="1152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1152" s="47"/>
-      <c r="C1152" s="1"/>
-      <c r="D1152" s="1"/>
-      <c r="E1152" s="1"/>
-      <c r="F1152" s="1"/>
-      <c r="G1152" s="1"/>
-      <c r="H1152" s="1"/>
-      <c r="I1152" s="1"/>
-      <c r="J1152" s="1"/>
-      <c r="K1152" s="1"/>
-      <c r="L1152" s="1"/>
-      <c r="M1152" s="1"/>
-      <c r="N1152" s="1"/>
-    </row>
-    <row r="1153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1153" s="9"/>
-    </row>
-    <row r="1154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1154" s="16" t="s">
+    <row r="1152" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1152" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1152" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1152" s="22"/>
+      <c r="E1152" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1152" s="26"/>
+      <c r="G1152" s="22"/>
+      <c r="H1152" s="22"/>
+      <c r="I1152" s="23" t="s">
+        <v>1187</v>
+      </c>
+      <c r="J1152" s="23"/>
+      <c r="K1152" s="23"/>
+      <c r="L1152" s="22"/>
+      <c r="M1152" s="22"/>
+      <c r="N1152" s="22"/>
+    </row>
+    <row r="1153" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1153" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1153" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1153" s="22"/>
+      <c r="E1153" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1153" s="26"/>
+      <c r="G1153" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1153" s="22"/>
+      <c r="I1153" s="23" t="s">
+        <v>1188</v>
+      </c>
+      <c r="J1153" s="23"/>
+      <c r="K1153" s="23"/>
+      <c r="L1153" s="22"/>
+      <c r="M1153" s="22"/>
+      <c r="N1153" s="22"/>
+    </row>
+    <row r="1154" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1154" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1154" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1154" s="22"/>
+      <c r="E1154" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1154" s="26"/>
+      <c r="G1154" s="22"/>
+      <c r="H1154" s="22"/>
+      <c r="I1154" s="23" t="s">
+        <v>1189</v>
+      </c>
+      <c r="J1154" s="23"/>
+      <c r="K1154" s="23"/>
+      <c r="L1154" s="22"/>
+      <c r="M1154" s="22"/>
+      <c r="N1154" s="22"/>
+    </row>
+    <row r="1155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1155" s="22"/>
+      <c r="C1155" s="22"/>
+      <c r="D1155" s="22"/>
+      <c r="E1155" s="22"/>
+      <c r="F1155" s="22"/>
+      <c r="G1155" s="22"/>
+      <c r="H1155" s="22"/>
+      <c r="I1155" s="23"/>
+      <c r="J1155" s="23"/>
+      <c r="K1155" s="23"/>
+      <c r="L1155" s="22"/>
+      <c r="M1155" s="22"/>
+      <c r="N1155" s="22"/>
+    </row>
+    <row r="1156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1156" s="47"/>
+      <c r="C1156" s="1"/>
+      <c r="D1156" s="1"/>
+      <c r="E1156" s="1"/>
+      <c r="F1156" s="1"/>
+      <c r="G1156" s="1"/>
+      <c r="H1156" s="1"/>
+      <c r="I1156" s="1"/>
+      <c r="J1156" s="1"/>
+      <c r="K1156" s="1"/>
+      <c r="L1156" s="1"/>
+      <c r="M1156" s="1"/>
+      <c r="N1156" s="1"/>
+    </row>
+    <row r="1157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1157" s="9"/>
+    </row>
+    <row r="1158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1158" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B1154" s="17"/>
-      <c r="C1154" s="18"/>
-      <c r="D1154" s="18"/>
-      <c r="E1154" s="18"/>
-      <c r="F1154" s="18"/>
-      <c r="G1154" s="18"/>
-      <c r="H1154" s="18"/>
-    </row>
-    <row r="1155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1155" s="16" t="s">
-        <v>1185</v>
-      </c>
-      <c r="B1155" s="17"/>
-      <c r="C1155" s="18"/>
-      <c r="D1155" s="18"/>
-      <c r="E1155" s="18"/>
-      <c r="F1155" s="18"/>
-      <c r="G1155" s="18"/>
-      <c r="H1155" s="18"/>
-    </row>
-    <row r="1156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1156" s="16" t="s">
+      <c r="B1158" s="17"/>
+      <c r="C1158" s="18"/>
+      <c r="D1158" s="18"/>
+      <c r="E1158" s="18"/>
+      <c r="F1158" s="18"/>
+      <c r="G1158" s="18"/>
+      <c r="H1158" s="18"/>
+    </row>
+    <row r="1159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1159" s="16" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B1159" s="17"/>
+      <c r="C1159" s="18"/>
+      <c r="D1159" s="18"/>
+      <c r="E1159" s="18"/>
+      <c r="F1159" s="18"/>
+      <c r="G1159" s="18"/>
+      <c r="H1159" s="18"/>
+    </row>
+    <row r="1160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1160" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B1156" s="17"/>
-      <c r="C1156" s="18"/>
-      <c r="D1156" s="18"/>
-      <c r="E1156" s="18"/>
-      <c r="F1156" s="18"/>
-      <c r="G1156" s="18"/>
-      <c r="H1156" s="18"/>
-    </row>
-    <row r="1157" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1157" s="9"/>
-      <c r="B1157" s="11" t="s">
+      <c r="B1160" s="17"/>
+      <c r="C1160" s="18"/>
+      <c r="D1160" s="18"/>
+      <c r="E1160" s="18"/>
+      <c r="F1160" s="18"/>
+      <c r="G1160" s="18"/>
+      <c r="H1160" s="18"/>
+    </row>
+    <row r="1161" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1161" s="9"/>
+      <c r="B1161" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1157" s="11" t="s">
+      <c r="C1161" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1157" s="11" t="s">
+      <c r="D1161" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1157" s="11" t="s">
+      <c r="E1161" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1157" s="11" t="s">
+      <c r="F1161" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G1157" s="11" t="s">
+      <c r="G1161" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1157" s="11" t="s">
+      <c r="H1161" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1157" s="20" t="s">
+      <c r="I1161" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1157" s="20" t="s">
+      <c r="J1161" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1157" s="20" t="s">
+      <c r="K1161" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="1158" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1158" s="21" t="s">
-        <v>1186</v>
-      </c>
-      <c r="B1158" s="22" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C1158" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1158" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1158" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1158" s="22" t="s">
-        <v>703</v>
-      </c>
-      <c r="G1158" s="22"/>
-      <c r="H1158" s="22"/>
-      <c r="I1158" s="23" t="s">
-        <v>1188</v>
-      </c>
-      <c r="J1158" s="23"/>
-      <c r="K1158" s="23"/>
-    </row>
-    <row r="1159" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1159" s="21"/>
-      <c r="B1159" s="22" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C1159" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1159" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1159" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1159" s="22" t="s">
-        <v>703</v>
-      </c>
-      <c r="G1159" s="22"/>
-      <c r="H1159" s="22"/>
-      <c r="I1159" s="23" t="s">
-        <v>1189</v>
-      </c>
-      <c r="J1159" s="23"/>
-      <c r="K1159" s="23"/>
-    </row>
-    <row r="1160" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1160" s="21"/>
-      <c r="B1160" s="28" t="s">
-        <v>1190</v>
-      </c>
-      <c r="C1160" s="26"/>
-      <c r="D1160" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1160" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1160" s="22" t="s">
-        <v>703</v>
-      </c>
-      <c r="G1160" s="22"/>
-      <c r="H1160" s="22"/>
-      <c r="I1160" s="23" t="s">
+    <row r="1162" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1162" s="21" t="s">
         <v>1191</v>
       </c>
-      <c r="J1160" s="23"/>
-      <c r="K1160" s="23" t="s">
+      <c r="B1162" s="22" t="s">
         <v>1192</v>
-      </c>
-    </row>
-    <row r="1161" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1161" s="21"/>
-      <c r="B1161" s="22" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C1161" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1161" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1161" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1161" s="22" t="s">
-        <v>703</v>
-      </c>
-      <c r="G1161" s="22"/>
-      <c r="H1161" s="22"/>
-      <c r="I1161" s="23" t="s">
-        <v>1193</v>
-      </c>
-      <c r="J1161" s="23"/>
-      <c r="K1161" s="23"/>
-    </row>
-    <row r="1162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1162" s="21"/>
-      <c r="B1162" s="22" t="s">
-        <v>1187</v>
       </c>
       <c r="C1162" s="22" t="s">
         <v>27</v>
@@ -30543,15 +30548,15 @@
       <c r="G1162" s="22"/>
       <c r="H1162" s="22"/>
       <c r="I1162" s="23" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="J1162" s="23"/>
       <c r="K1162" s="23"/>
     </row>
-    <row r="1163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1163" s="9"/>
+    <row r="1163" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1163" s="21"/>
       <c r="B1163" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1163" s="22" t="s">
         <v>27</v>
@@ -30568,19 +30573,17 @@
       <c r="G1163" s="22"/>
       <c r="H1163" s="22"/>
       <c r="I1163" s="23" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="J1163" s="23"/>
       <c r="K1163" s="23"/>
     </row>
-    <row r="1164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1164" s="9"/>
-      <c r="B1164" s="22" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C1164" s="22" t="s">
-        <v>27</v>
-      </c>
+    <row r="1164" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1164" s="21"/>
+      <c r="B1164" s="28" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C1164" s="26"/>
       <c r="D1164" s="22" t="s">
         <v>27</v>
       </c>
@@ -30592,16 +30595,18 @@
       </c>
       <c r="G1164" s="22"/>
       <c r="H1164" s="22"/>
-      <c r="I1164" s="46" t="s">
+      <c r="I1164" s="23" t="s">
         <v>1196</v>
       </c>
       <c r="J1164" s="23"/>
-      <c r="K1164" s="23"/>
-    </row>
-    <row r="1165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1165" s="9"/>
+      <c r="K1164" s="23" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="1165" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1165" s="21"/>
       <c r="B1165" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1165" s="22" t="s">
         <v>27</v>
@@ -30617,16 +30622,16 @@
       </c>
       <c r="G1165" s="22"/>
       <c r="H1165" s="22"/>
-      <c r="I1165" s="46" t="s">
-        <v>1197</v>
+      <c r="I1165" s="23" t="s">
+        <v>1198</v>
       </c>
       <c r="J1165" s="23"/>
       <c r="K1165" s="23"/>
     </row>
     <row r="1166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1166" s="9"/>
+      <c r="A1166" s="21"/>
       <c r="B1166" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1166" s="22" t="s">
         <v>27</v>
@@ -30642,8 +30647,8 @@
       </c>
       <c r="G1166" s="22"/>
       <c r="H1166" s="22"/>
-      <c r="I1166" s="46" t="s">
-        <v>1198</v>
+      <c r="I1166" s="23" t="s">
+        <v>1199</v>
       </c>
       <c r="J1166" s="23"/>
       <c r="K1166" s="23"/>
@@ -30651,7 +30656,7 @@
     <row r="1167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1167" s="9"/>
       <c r="B1167" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1167" s="22" t="s">
         <v>27</v>
@@ -30667,8 +30672,8 @@
       </c>
       <c r="G1167" s="22"/>
       <c r="H1167" s="22"/>
-      <c r="I1167" s="46" t="s">
-        <v>1199</v>
+      <c r="I1167" s="23" t="s">
+        <v>1200</v>
       </c>
       <c r="J1167" s="23"/>
       <c r="K1167" s="23"/>
@@ -30676,7 +30681,7 @@
     <row r="1168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1168" s="9"/>
       <c r="B1168" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1168" s="22" t="s">
         <v>27</v>
@@ -30692,16 +30697,16 @@
       </c>
       <c r="G1168" s="22"/>
       <c r="H1168" s="22"/>
-      <c r="I1168" s="23" t="s">
-        <v>1200</v>
+      <c r="I1168" s="46" t="s">
+        <v>1201</v>
       </c>
       <c r="J1168" s="23"/>
       <c r="K1168" s="23"/>
     </row>
-    <row r="1169" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1169" s="9"/>
       <c r="B1169" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1169" s="22" t="s">
         <v>27</v>
@@ -30717,16 +30722,16 @@
       </c>
       <c r="G1169" s="22"/>
       <c r="H1169" s="22"/>
-      <c r="I1169" s="23" t="s">
-        <v>1201</v>
+      <c r="I1169" s="46" t="s">
+        <v>1202</v>
       </c>
       <c r="J1169" s="23"/>
       <c r="K1169" s="23"/>
     </row>
-    <row r="1170" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1170" s="9"/>
       <c r="B1170" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1170" s="22" t="s">
         <v>27</v>
@@ -30742,16 +30747,16 @@
       </c>
       <c r="G1170" s="22"/>
       <c r="H1170" s="22"/>
-      <c r="I1170" s="23" t="s">
-        <v>1202</v>
+      <c r="I1170" s="46" t="s">
+        <v>1203</v>
       </c>
       <c r="J1170" s="23"/>
       <c r="K1170" s="23"/>
     </row>
-    <row r="1171" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1171" s="9"/>
       <c r="B1171" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1171" s="22" t="s">
         <v>27</v>
@@ -30767,16 +30772,16 @@
       </c>
       <c r="G1171" s="22"/>
       <c r="H1171" s="22"/>
-      <c r="I1171" s="23" t="s">
-        <v>1203</v>
+      <c r="I1171" s="46" t="s">
+        <v>1204</v>
       </c>
       <c r="J1171" s="23"/>
       <c r="K1171" s="23"/>
     </row>
-    <row r="1172" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1172" s="9"/>
       <c r="B1172" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1172" s="22" t="s">
         <v>27</v>
@@ -30793,7 +30798,7 @@
       <c r="G1172" s="22"/>
       <c r="H1172" s="22"/>
       <c r="I1172" s="23" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="J1172" s="23"/>
       <c r="K1172" s="23"/>
@@ -30801,12 +30806,14 @@
     <row r="1173" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1173" s="9"/>
       <c r="B1173" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1173" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1173" s="22"/>
+      <c r="D1173" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="E1173" s="22" t="s">
         <v>27</v>
       </c>
@@ -30816,7 +30823,7 @@
       <c r="G1173" s="22"/>
       <c r="H1173" s="22"/>
       <c r="I1173" s="23" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="J1173" s="23"/>
       <c r="K1173" s="23"/>
@@ -30824,7 +30831,7 @@
     <row r="1174" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1174" s="9"/>
       <c r="B1174" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1174" s="22" t="s">
         <v>27</v>
@@ -30841,15 +30848,15 @@
       <c r="G1174" s="22"/>
       <c r="H1174" s="22"/>
       <c r="I1174" s="23" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="J1174" s="23"/>
       <c r="K1174" s="23"/>
     </row>
-    <row r="1175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1175" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1175" s="9"/>
       <c r="B1175" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1175" s="22" t="s">
         <v>27</v>
@@ -30861,7 +30868,7 @@
         <v>27</v>
       </c>
       <c r="F1175" s="22" t="s">
-        <v>1207</v>
+        <v>703</v>
       </c>
       <c r="G1175" s="22"/>
       <c r="H1175" s="22"/>
@@ -30869,14 +30876,12 @@
         <v>1208</v>
       </c>
       <c r="J1175" s="23"/>
-      <c r="K1175" s="23" t="s">
-        <v>1209</v>
-      </c>
-    </row>
-    <row r="1176" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1175" s="23"/>
+    </row>
+    <row r="1176" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1176" s="9"/>
       <c r="B1176" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1176" s="22" t="s">
         <v>27</v>
@@ -30888,29 +30893,25 @@
         <v>27</v>
       </c>
       <c r="F1176" s="22" t="s">
-        <v>1207</v>
+        <v>703</v>
       </c>
       <c r="G1176" s="22"/>
       <c r="H1176" s="22"/>
       <c r="I1176" s="23" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="J1176" s="23"/>
-      <c r="K1176" s="23" t="s">
-        <v>1211</v>
-      </c>
+      <c r="K1176" s="23"/>
     </row>
     <row r="1177" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1177" s="9"/>
       <c r="B1177" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1177" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1177" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="D1177" s="22"/>
       <c r="E1177" s="22" t="s">
         <v>27</v>
       </c>
@@ -30920,7 +30921,7 @@
       <c r="G1177" s="22"/>
       <c r="H1177" s="22"/>
       <c r="I1177" s="23" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="J1177" s="23"/>
       <c r="K1177" s="23"/>
@@ -30928,7 +30929,7 @@
     <row r="1178" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1178" s="9"/>
       <c r="B1178" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1178" s="22" t="s">
         <v>27</v>
@@ -30945,15 +30946,15 @@
       <c r="G1178" s="22"/>
       <c r="H1178" s="22"/>
       <c r="I1178" s="23" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="J1178" s="23"/>
       <c r="K1178" s="23"/>
     </row>
-    <row r="1179" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1179" s="9"/>
       <c r="B1179" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1179" s="22" t="s">
         <v>27</v>
@@ -30965,22 +30966,26 @@
         <v>27</v>
       </c>
       <c r="F1179" s="22" t="s">
-        <v>703</v>
+        <v>1212</v>
       </c>
       <c r="G1179" s="22"/>
       <c r="H1179" s="22"/>
       <c r="I1179" s="23" t="s">
+        <v>1213</v>
+      </c>
+      <c r="J1179" s="23"/>
+      <c r="K1179" s="23" t="s">
         <v>1214</v>
       </c>
-      <c r="J1179" s="23"/>
-      <c r="K1179" s="23"/>
-    </row>
-    <row r="1180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="1180" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1180" s="9"/>
       <c r="B1180" s="22" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C1180" s="26"/>
+        <v>1192</v>
+      </c>
+      <c r="C1180" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1180" s="22" t="s">
         <v>27</v>
       </c>
@@ -30988,7 +30993,7 @@
         <v>27</v>
       </c>
       <c r="F1180" s="22" t="s">
-        <v>703</v>
+        <v>1212</v>
       </c>
       <c r="G1180" s="22"/>
       <c r="H1180" s="22"/>
@@ -30996,12 +31001,14 @@
         <v>1215</v>
       </c>
       <c r="J1180" s="23"/>
-      <c r="K1180" s="23"/>
+      <c r="K1180" s="23" t="s">
+        <v>1216</v>
+      </c>
     </row>
     <row r="1181" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1181" s="9"/>
       <c r="B1181" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1181" s="22" t="s">
         <v>27</v>
@@ -31018,7 +31025,7 @@
       <c r="G1181" s="22"/>
       <c r="H1181" s="22"/>
       <c r="I1181" s="23" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="J1181" s="23"/>
       <c r="K1181" s="23"/>
@@ -31026,7 +31033,7 @@
     <row r="1182" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1182" s="9"/>
       <c r="B1182" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1182" s="22" t="s">
         <v>27</v>
@@ -31043,17 +31050,15 @@
       <c r="G1182" s="22"/>
       <c r="H1182" s="22"/>
       <c r="I1182" s="23" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="J1182" s="23"/>
-      <c r="K1182" s="23" t="s">
-        <v>297</v>
-      </c>
+      <c r="K1182" s="23"/>
     </row>
     <row r="1183" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1183" s="9"/>
       <c r="B1183" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1183" s="22" t="s">
         <v>27</v>
@@ -31070,19 +31075,17 @@
       <c r="G1183" s="22"/>
       <c r="H1183" s="22"/>
       <c r="I1183" s="23" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="J1183" s="23"/>
       <c r="K1183" s="23"/>
     </row>
-    <row r="1184" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1184" s="9"/>
       <c r="B1184" s="22" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C1184" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1192</v>
+      </c>
+      <c r="C1184" s="26"/>
       <c r="D1184" s="22" t="s">
         <v>27</v>
       </c>
@@ -31095,7 +31098,7 @@
       <c r="G1184" s="22"/>
       <c r="H1184" s="22"/>
       <c r="I1184" s="23" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="J1184" s="23"/>
       <c r="K1184" s="23"/>
@@ -31103,7 +31106,7 @@
     <row r="1185" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1185" s="9"/>
       <c r="B1185" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1185" s="22" t="s">
         <v>27</v>
@@ -31120,15 +31123,15 @@
       <c r="G1185" s="22"/>
       <c r="H1185" s="22"/>
       <c r="I1185" s="23" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="J1185" s="23"/>
       <c r="K1185" s="23"/>
     </row>
-    <row r="1186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1186" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1186" s="9"/>
       <c r="B1186" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1186" s="22" t="s">
         <v>27</v>
@@ -31145,15 +31148,17 @@
       <c r="G1186" s="22"/>
       <c r="H1186" s="22"/>
       <c r="I1186" s="23" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="J1186" s="23"/>
-      <c r="K1186" s="23"/>
+      <c r="K1186" s="23" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="1187" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1187" s="9"/>
       <c r="B1187" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1187" s="22" t="s">
         <v>27</v>
@@ -31170,7 +31175,7 @@
       <c r="G1187" s="22"/>
       <c r="H1187" s="22"/>
       <c r="I1187" s="23" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="J1187" s="23"/>
       <c r="K1187" s="23"/>
@@ -31178,7 +31183,7 @@
     <row r="1188" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1188" s="9"/>
       <c r="B1188" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1188" s="22" t="s">
         <v>27</v>
@@ -31195,7 +31200,7 @@
       <c r="G1188" s="22"/>
       <c r="H1188" s="22"/>
       <c r="I1188" s="23" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="J1188" s="23"/>
       <c r="K1188" s="23"/>
@@ -31203,7 +31208,7 @@
     <row r="1189" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1189" s="9"/>
       <c r="B1189" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1189" s="22" t="s">
         <v>27</v>
@@ -31220,15 +31225,15 @@
       <c r="G1189" s="22"/>
       <c r="H1189" s="22"/>
       <c r="I1189" s="23" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="J1189" s="23"/>
       <c r="K1189" s="23"/>
     </row>
-    <row r="1190" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1190" s="9"/>
       <c r="B1190" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1190" s="22" t="s">
         <v>27</v>
@@ -31245,7 +31250,7 @@
       <c r="G1190" s="22"/>
       <c r="H1190" s="22"/>
       <c r="I1190" s="23" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="J1190" s="23"/>
       <c r="K1190" s="23"/>
@@ -31253,7 +31258,7 @@
     <row r="1191" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1191" s="9"/>
       <c r="B1191" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1191" s="22" t="s">
         <v>27</v>
@@ -31270,15 +31275,15 @@
       <c r="G1191" s="22"/>
       <c r="H1191" s="22"/>
       <c r="I1191" s="23" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="J1191" s="23"/>
       <c r="K1191" s="23"/>
     </row>
-    <row r="1192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1192" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1192" s="9"/>
       <c r="B1192" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1192" s="22" t="s">
         <v>27</v>
@@ -31295,15 +31300,15 @@
       <c r="G1192" s="22"/>
       <c r="H1192" s="22"/>
       <c r="I1192" s="23" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="J1192" s="23"/>
       <c r="K1192" s="23"/>
     </row>
-    <row r="1193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1193" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1193" s="9"/>
       <c r="B1193" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1193" s="22" t="s">
         <v>27</v>
@@ -31320,15 +31325,15 @@
       <c r="G1193" s="22"/>
       <c r="H1193" s="22"/>
       <c r="I1193" s="23" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="J1193" s="23"/>
       <c r="K1193" s="23"/>
     </row>
-    <row r="1194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1194" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1194" s="9"/>
       <c r="B1194" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1194" s="22" t="s">
         <v>27</v>
@@ -31345,7 +31350,7 @@
       <c r="G1194" s="22"/>
       <c r="H1194" s="22"/>
       <c r="I1194" s="23" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="J1194" s="23"/>
       <c r="K1194" s="23"/>
@@ -31353,7 +31358,7 @@
     <row r="1195" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1195" s="9"/>
       <c r="B1195" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1195" s="22" t="s">
         <v>27</v>
@@ -31370,15 +31375,15 @@
       <c r="G1195" s="22"/>
       <c r="H1195" s="22"/>
       <c r="I1195" s="23" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="J1195" s="23"/>
       <c r="K1195" s="23"/>
     </row>
-    <row r="1196" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1196" s="9"/>
       <c r="B1196" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1196" s="22" t="s">
         <v>27</v>
@@ -31395,15 +31400,15 @@
       <c r="G1196" s="22"/>
       <c r="H1196" s="22"/>
       <c r="I1196" s="23" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="J1196" s="23"/>
       <c r="K1196" s="23"/>
     </row>
-    <row r="1197" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1197" s="9"/>
       <c r="B1197" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1197" s="22" t="s">
         <v>27</v>
@@ -31420,15 +31425,15 @@
       <c r="G1197" s="22"/>
       <c r="H1197" s="22"/>
       <c r="I1197" s="23" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="J1197" s="23"/>
       <c r="K1197" s="23"/>
     </row>
-    <row r="1198" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1198" s="9"/>
       <c r="B1198" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1198" s="22" t="s">
         <v>27</v>
@@ -31445,15 +31450,15 @@
       <c r="G1198" s="22"/>
       <c r="H1198" s="22"/>
       <c r="I1198" s="23" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="J1198" s="23"/>
       <c r="K1198" s="23"/>
     </row>
-    <row r="1199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1199" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1199" s="9"/>
       <c r="B1199" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1199" s="22" t="s">
         <v>27</v>
@@ -31470,15 +31475,15 @@
       <c r="G1199" s="22"/>
       <c r="H1199" s="22"/>
       <c r="I1199" s="23" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="J1199" s="23"/>
       <c r="K1199" s="23"/>
     </row>
-    <row r="1200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1200" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1200" s="9"/>
       <c r="B1200" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1200" s="22" t="s">
         <v>27</v>
@@ -31495,7 +31500,7 @@
       <c r="G1200" s="22"/>
       <c r="H1200" s="22"/>
       <c r="I1200" s="23" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="J1200" s="23"/>
       <c r="K1200" s="23"/>
@@ -31503,7 +31508,7 @@
     <row r="1201" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1201" s="9"/>
       <c r="B1201" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1201" s="22" t="s">
         <v>27</v>
@@ -31520,7 +31525,7 @@
       <c r="G1201" s="22"/>
       <c r="H1201" s="22"/>
       <c r="I1201" s="23" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="J1201" s="23"/>
       <c r="K1201" s="23"/>
@@ -31528,7 +31533,7 @@
     <row r="1202" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1202" s="9"/>
       <c r="B1202" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1202" s="22" t="s">
         <v>27</v>
@@ -31545,15 +31550,15 @@
       <c r="G1202" s="22"/>
       <c r="H1202" s="22"/>
       <c r="I1202" s="23" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="J1202" s="23"/>
       <c r="K1202" s="23"/>
     </row>
-    <row r="1203" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1203" s="9"/>
       <c r="B1203" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1203" s="22" t="s">
         <v>27</v>
@@ -31570,15 +31575,15 @@
       <c r="G1203" s="22"/>
       <c r="H1203" s="22"/>
       <c r="I1203" s="23" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="J1203" s="23"/>
       <c r="K1203" s="23"/>
     </row>
-    <row r="1204" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1204" s="9"/>
       <c r="B1204" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1204" s="22" t="s">
         <v>27</v>
@@ -31595,7 +31600,7 @@
       <c r="G1204" s="22"/>
       <c r="H1204" s="22"/>
       <c r="I1204" s="23" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="J1204" s="23"/>
       <c r="K1204" s="23"/>
@@ -31603,7 +31608,7 @@
     <row r="1205" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1205" s="9"/>
       <c r="B1205" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1205" s="22" t="s">
         <v>27</v>
@@ -31620,7 +31625,7 @@
       <c r="G1205" s="22"/>
       <c r="H1205" s="22"/>
       <c r="I1205" s="23" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="J1205" s="23"/>
       <c r="K1205" s="23"/>
@@ -31628,7 +31633,7 @@
     <row r="1206" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1206" s="9"/>
       <c r="B1206" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1206" s="22" t="s">
         <v>27</v>
@@ -31645,15 +31650,15 @@
       <c r="G1206" s="22"/>
       <c r="H1206" s="22"/>
       <c r="I1206" s="23" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="J1206" s="23"/>
       <c r="K1206" s="23"/>
     </row>
-    <row r="1207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1207" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1207" s="9"/>
       <c r="B1207" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1207" s="22" t="s">
         <v>27</v>
@@ -31670,15 +31675,15 @@
       <c r="G1207" s="22"/>
       <c r="H1207" s="22"/>
       <c r="I1207" s="23" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="J1207" s="23"/>
       <c r="K1207" s="23"/>
     </row>
-    <row r="1208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1208" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1208" s="9"/>
       <c r="B1208" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1208" s="22" t="s">
         <v>27</v>
@@ -31695,7 +31700,7 @@
       <c r="G1208" s="22"/>
       <c r="H1208" s="22"/>
       <c r="I1208" s="23" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="J1208" s="23"/>
       <c r="K1208" s="23"/>
@@ -31703,7 +31708,7 @@
     <row r="1209" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1209" s="9"/>
       <c r="B1209" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1209" s="22" t="s">
         <v>27</v>
@@ -31720,7 +31725,7 @@
       <c r="G1209" s="22"/>
       <c r="H1209" s="22"/>
       <c r="I1209" s="23" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="J1209" s="23"/>
       <c r="K1209" s="23"/>
@@ -31728,7 +31733,7 @@
     <row r="1210" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1210" s="9"/>
       <c r="B1210" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1210" s="22" t="s">
         <v>27</v>
@@ -31745,7 +31750,7 @@
       <c r="G1210" s="22"/>
       <c r="H1210" s="22"/>
       <c r="I1210" s="23" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="J1210" s="23"/>
       <c r="K1210" s="23"/>
@@ -31753,7 +31758,7 @@
     <row r="1211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1211" s="9"/>
       <c r="B1211" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1211" s="22" t="s">
         <v>27</v>
@@ -31770,7 +31775,7 @@
       <c r="G1211" s="22"/>
       <c r="H1211" s="22"/>
       <c r="I1211" s="23" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="J1211" s="23"/>
       <c r="K1211" s="23"/>
@@ -31778,7 +31783,7 @@
     <row r="1212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1212" s="9"/>
       <c r="B1212" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1212" s="22" t="s">
         <v>27</v>
@@ -31795,15 +31800,15 @@
       <c r="G1212" s="22"/>
       <c r="H1212" s="22"/>
       <c r="I1212" s="23" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="J1212" s="23"/>
       <c r="K1212" s="23"/>
     </row>
-    <row r="1213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1213" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1213" s="9"/>
       <c r="B1213" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1213" s="22" t="s">
         <v>27</v>
@@ -31820,7 +31825,7 @@
       <c r="G1213" s="22"/>
       <c r="H1213" s="22"/>
       <c r="I1213" s="23" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="J1213" s="23"/>
       <c r="K1213" s="23"/>
@@ -31828,7 +31833,7 @@
     <row r="1214" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1214" s="9"/>
       <c r="B1214" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1214" s="22" t="s">
         <v>27</v>
@@ -31845,15 +31850,15 @@
       <c r="G1214" s="22"/>
       <c r="H1214" s="22"/>
       <c r="I1214" s="23" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="J1214" s="23"/>
       <c r="K1214" s="23"/>
     </row>
-    <row r="1215" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1215" s="9"/>
       <c r="B1215" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1215" s="22" t="s">
         <v>27</v>
@@ -31870,7 +31875,7 @@
       <c r="G1215" s="22"/>
       <c r="H1215" s="22"/>
       <c r="I1215" s="23" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="J1215" s="23"/>
       <c r="K1215" s="23"/>
@@ -31878,7 +31883,7 @@
     <row r="1216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1216" s="9"/>
       <c r="B1216" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1216" s="22" t="s">
         <v>27</v>
@@ -31895,7 +31900,7 @@
       <c r="G1216" s="22"/>
       <c r="H1216" s="22"/>
       <c r="I1216" s="23" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="J1216" s="23"/>
       <c r="K1216" s="23"/>
@@ -31903,7 +31908,7 @@
     <row r="1217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1217" s="9"/>
       <c r="B1217" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1217" s="22" t="s">
         <v>27</v>
@@ -31920,15 +31925,15 @@
       <c r="G1217" s="22"/>
       <c r="H1217" s="22"/>
       <c r="I1217" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J1217" s="23"/>
       <c r="K1217" s="23"/>
     </row>
-    <row r="1218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1218" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1218" s="9"/>
       <c r="B1218" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1218" s="22" t="s">
         <v>27</v>
@@ -31945,15 +31950,15 @@
       <c r="G1218" s="22"/>
       <c r="H1218" s="22"/>
       <c r="I1218" s="23" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="J1218" s="23"/>
       <c r="K1218" s="23"/>
     </row>
-    <row r="1219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1219" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1219" s="9"/>
       <c r="B1219" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1219" s="22" t="s">
         <v>27</v>
@@ -31970,7 +31975,7 @@
       <c r="G1219" s="22"/>
       <c r="H1219" s="22"/>
       <c r="I1219" s="23" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="J1219" s="23"/>
       <c r="K1219" s="23"/>
@@ -31978,7 +31983,7 @@
     <row r="1220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1220" s="9"/>
       <c r="B1220" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1220" s="22" t="s">
         <v>27</v>
@@ -31995,7 +32000,7 @@
       <c r="G1220" s="22"/>
       <c r="H1220" s="22"/>
       <c r="I1220" s="23" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="J1220" s="23"/>
       <c r="K1220" s="23"/>
@@ -32003,7 +32008,7 @@
     <row r="1221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1221" s="9"/>
       <c r="B1221" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1221" s="22" t="s">
         <v>27</v>
@@ -32020,15 +32025,15 @@
       <c r="G1221" s="22"/>
       <c r="H1221" s="22"/>
       <c r="I1221" s="23" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="J1221" s="23"/>
       <c r="K1221" s="23"/>
     </row>
-    <row r="1222" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1222" s="9"/>
       <c r="B1222" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1222" s="22" t="s">
         <v>27</v>
@@ -32045,7 +32050,7 @@
       <c r="G1222" s="22"/>
       <c r="H1222" s="22"/>
       <c r="I1222" s="23" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="J1222" s="23"/>
       <c r="K1222" s="23"/>
@@ -32053,7 +32058,7 @@
     <row r="1223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1223" s="9"/>
       <c r="B1223" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1223" s="22" t="s">
         <v>27</v>
@@ -32070,7 +32075,7 @@
       <c r="G1223" s="22"/>
       <c r="H1223" s="22"/>
       <c r="I1223" s="23" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="J1223" s="23"/>
       <c r="K1223" s="23"/>
@@ -32078,7 +32083,7 @@
     <row r="1224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1224" s="9"/>
       <c r="B1224" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1224" s="22" t="s">
         <v>27</v>
@@ -32095,7 +32100,7 @@
       <c r="G1224" s="22"/>
       <c r="H1224" s="22"/>
       <c r="I1224" s="23" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="J1224" s="23"/>
       <c r="K1224" s="23"/>
@@ -32103,7 +32108,7 @@
     <row r="1225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1225" s="9"/>
       <c r="B1225" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1225" s="22" t="s">
         <v>27</v>
@@ -32120,15 +32125,15 @@
       <c r="G1225" s="22"/>
       <c r="H1225" s="22"/>
       <c r="I1225" s="23" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="J1225" s="23"/>
       <c r="K1225" s="23"/>
     </row>
-    <row r="1226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1226" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1226" s="9"/>
       <c r="B1226" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1226" s="22" t="s">
         <v>27</v>
@@ -32145,38 +32150,40 @@
       <c r="G1226" s="22"/>
       <c r="H1226" s="22"/>
       <c r="I1226" s="23" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="J1226" s="23"/>
       <c r="K1226" s="23"/>
     </row>
     <row r="1227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1227" s="9"/>
-      <c r="B1227" s="28" t="s">
-        <v>1190</v>
-      </c>
-      <c r="C1227" s="26"/>
+      <c r="B1227" s="22" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C1227" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1227" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1227" s="26"/>
+      <c r="E1227" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1227" s="22" t="s">
         <v>703</v>
       </c>
       <c r="G1227" s="22"/>
       <c r="H1227" s="22"/>
       <c r="I1227" s="23" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="J1227" s="23"/>
-      <c r="K1227" s="23" t="s">
-        <v>675</v>
-      </c>
+      <c r="K1227" s="23"/>
     </row>
     <row r="1228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1228" s="9"/>
       <c r="B1228" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1228" s="22" t="s">
         <v>27</v>
@@ -32193,7 +32200,7 @@
       <c r="G1228" s="22"/>
       <c r="H1228" s="22"/>
       <c r="I1228" s="23" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="J1228" s="23"/>
       <c r="K1228" s="23"/>
@@ -32201,7 +32208,7 @@
     <row r="1229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1229" s="9"/>
       <c r="B1229" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1229" s="22" t="s">
         <v>27</v>
@@ -32218,7 +32225,7 @@
       <c r="G1229" s="22"/>
       <c r="H1229" s="22"/>
       <c r="I1229" s="23" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="J1229" s="23"/>
       <c r="K1229" s="23"/>
@@ -32226,7 +32233,7 @@
     <row r="1230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1230" s="9"/>
       <c r="B1230" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1230" s="22" t="s">
         <v>27</v>
@@ -32243,40 +32250,38 @@
       <c r="G1230" s="22"/>
       <c r="H1230" s="22"/>
       <c r="I1230" s="23" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="J1230" s="23"/>
       <c r="K1230" s="23"/>
     </row>
     <row r="1231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1231" s="9"/>
-      <c r="B1231" s="22" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C1231" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="B1231" s="28" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C1231" s="26"/>
       <c r="D1231" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1231" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1231" s="26"/>
       <c r="F1231" s="22" t="s">
         <v>703</v>
       </c>
       <c r="G1231" s="22"/>
       <c r="H1231" s="22"/>
       <c r="I1231" s="23" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="J1231" s="23"/>
-      <c r="K1231" s="23"/>
-    </row>
-    <row r="1232" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1231" s="23" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="1232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1232" s="9"/>
       <c r="B1232" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1232" s="22" t="s">
         <v>27</v>
@@ -32293,7 +32298,7 @@
       <c r="G1232" s="22"/>
       <c r="H1232" s="22"/>
       <c r="I1232" s="23" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="J1232" s="23"/>
       <c r="K1232" s="23"/>
@@ -32301,7 +32306,7 @@
     <row r="1233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1233" s="9"/>
       <c r="B1233" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1233" s="22" t="s">
         <v>27</v>
@@ -32318,7 +32323,7 @@
       <c r="G1233" s="22"/>
       <c r="H1233" s="22"/>
       <c r="I1233" s="23" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="J1233" s="23"/>
       <c r="K1233" s="23"/>
@@ -32326,7 +32331,7 @@
     <row r="1234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1234" s="9"/>
       <c r="B1234" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1234" s="22" t="s">
         <v>27</v>
@@ -32343,14 +32348,15 @@
       <c r="G1234" s="22"/>
       <c r="H1234" s="22"/>
       <c r="I1234" s="23" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="J1234" s="23"/>
       <c r="K1234" s="23"/>
     </row>
     <row r="1235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1235" s="9"/>
       <c r="B1235" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1235" s="22" t="s">
         <v>27</v>
@@ -32367,14 +32373,15 @@
       <c r="G1235" s="22"/>
       <c r="H1235" s="22"/>
       <c r="I1235" s="23" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="J1235" s="23"/>
       <c r="K1235" s="23"/>
     </row>
     <row r="1236" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1236" s="9"/>
       <c r="B1236" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1236" s="22" t="s">
         <v>27</v>
@@ -32391,14 +32398,15 @@
       <c r="G1236" s="22"/>
       <c r="H1236" s="22"/>
       <c r="I1236" s="23" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="J1236" s="23"/>
       <c r="K1236" s="23"/>
     </row>
-    <row r="1237" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1237" s="9"/>
       <c r="B1237" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1237" s="22" t="s">
         <v>27</v>
@@ -32415,14 +32423,15 @@
       <c r="G1237" s="22"/>
       <c r="H1237" s="22"/>
       <c r="I1237" s="23" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="J1237" s="23"/>
       <c r="K1237" s="23"/>
     </row>
-    <row r="1238" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1238" s="9"/>
       <c r="B1238" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1238" s="22" t="s">
         <v>27</v>
@@ -32439,14 +32448,14 @@
       <c r="G1238" s="22"/>
       <c r="H1238" s="22"/>
       <c r="I1238" s="23" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="J1238" s="23"/>
       <c r="K1238" s="23"/>
     </row>
     <row r="1239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1239" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1239" s="22" t="s">
         <v>27</v>
@@ -32463,14 +32472,14 @@
       <c r="G1239" s="22"/>
       <c r="H1239" s="22"/>
       <c r="I1239" s="23" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="J1239" s="23"/>
       <c r="K1239" s="23"/>
     </row>
     <row r="1240" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1240" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1240" s="22" t="s">
         <v>27</v>
@@ -32487,14 +32496,14 @@
       <c r="G1240" s="22"/>
       <c r="H1240" s="22"/>
       <c r="I1240" s="23" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="J1240" s="23"/>
       <c r="K1240" s="23"/>
     </row>
     <row r="1241" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1241" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1241" s="22" t="s">
         <v>27</v>
@@ -32511,14 +32520,14 @@
       <c r="G1241" s="22"/>
       <c r="H1241" s="22"/>
       <c r="I1241" s="23" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="J1241" s="23"/>
       <c r="K1241" s="23"/>
     </row>
     <row r="1242" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1242" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1242" s="22" t="s">
         <v>27</v>
@@ -32535,14 +32544,14 @@
       <c r="G1242" s="22"/>
       <c r="H1242" s="22"/>
       <c r="I1242" s="23" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="J1242" s="23"/>
       <c r="K1242" s="23"/>
     </row>
     <row r="1243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1243" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1243" s="22" t="s">
         <v>27</v>
@@ -32559,36 +32568,38 @@
       <c r="G1243" s="22"/>
       <c r="H1243" s="22"/>
       <c r="I1243" s="23" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="J1243" s="23"/>
       <c r="K1243" s="23"/>
     </row>
-    <row r="1244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1244" s="28" t="s">
+    <row r="1244" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1244" s="22" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C1244" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1244" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1244" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1244" s="22" t="s">
         <v>703</v>
       </c>
-      <c r="C1244" s="28"/>
-      <c r="D1244" s="28" t="s">
-        <v>703</v>
-      </c>
-      <c r="E1244" s="28"/>
-      <c r="F1244" s="28" t="s">
-        <v>703</v>
-      </c>
-      <c r="G1244" s="28"/>
-      <c r="H1244" s="28"/>
-      <c r="I1244" s="29" t="s">
-        <v>1279</v>
-      </c>
-      <c r="J1244" s="29"/>
-      <c r="K1244" s="29" t="s">
+      <c r="G1244" s="22"/>
+      <c r="H1244" s="22"/>
+      <c r="I1244" s="23" t="s">
         <v>1280</v>
       </c>
+      <c r="J1244" s="23"/>
+      <c r="K1244" s="23"/>
     </row>
     <row r="1245" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1245" s="22" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="C1245" s="22" t="s">
         <v>27</v>
@@ -32600,7 +32611,7 @@
         <v>27</v>
       </c>
       <c r="F1245" s="22" t="s">
-        <v>1207</v>
+        <v>703</v>
       </c>
       <c r="G1245" s="22"/>
       <c r="H1245" s="22"/>
@@ -32608,30 +32619,124 @@
         <v>1281</v>
       </c>
       <c r="J1245" s="23"/>
-      <c r="K1245" s="23" t="s">
+      <c r="K1245" s="23"/>
+    </row>
+    <row r="1246" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1246" s="22" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C1246" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1246" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1246" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1246" s="22" t="s">
+        <v>703</v>
+      </c>
+      <c r="G1246" s="22"/>
+      <c r="H1246" s="22"/>
+      <c r="I1246" s="23" t="s">
         <v>1282</v>
       </c>
-    </row>
-    <row r="1246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1246" s="28" t="s">
+      <c r="J1246" s="23"/>
+      <c r="K1246" s="23"/>
+    </row>
+    <row r="1247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1247" s="22" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C1247" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1247" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1247" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1247" s="22" t="s">
         <v>703</v>
       </c>
-      <c r="C1246" s="28"/>
-      <c r="D1246" s="28" t="s">
+      <c r="G1247" s="22"/>
+      <c r="H1247" s="22"/>
+      <c r="I1247" s="23" t="s">
+        <v>1283</v>
+      </c>
+      <c r="J1247" s="23"/>
+      <c r="K1247" s="23"/>
+    </row>
+    <row r="1248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1248" s="28" t="s">
         <v>703</v>
       </c>
-      <c r="E1246" s="28"/>
-      <c r="F1246" s="28" t="s">
+      <c r="C1248" s="28"/>
+      <c r="D1248" s="28" t="s">
         <v>703</v>
       </c>
-      <c r="G1246" s="28"/>
-      <c r="H1246" s="28"/>
-      <c r="I1246" s="29" t="s">
-        <v>1283</v>
-      </c>
-      <c r="J1246" s="29"/>
-      <c r="K1246" s="29" t="s">
-        <v>1280</v>
+      <c r="E1248" s="28"/>
+      <c r="F1248" s="28" t="s">
+        <v>703</v>
+      </c>
+      <c r="G1248" s="28"/>
+      <c r="H1248" s="28"/>
+      <c r="I1248" s="29" t="s">
+        <v>1284</v>
+      </c>
+      <c r="J1248" s="29"/>
+      <c r="K1248" s="29" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="1249" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1249" s="22" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C1249" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1249" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1249" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1249" s="22" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G1249" s="22"/>
+      <c r="H1249" s="22"/>
+      <c r="I1249" s="23" t="s">
+        <v>1286</v>
+      </c>
+      <c r="J1249" s="23"/>
+      <c r="K1249" s="23" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="1250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1250" s="28" t="s">
+        <v>703</v>
+      </c>
+      <c r="C1250" s="28"/>
+      <c r="D1250" s="28" t="s">
+        <v>703</v>
+      </c>
+      <c r="E1250" s="28"/>
+      <c r="F1250" s="28" t="s">
+        <v>703</v>
+      </c>
+      <c r="G1250" s="28"/>
+      <c r="H1250" s="28"/>
+      <c r="I1250" s="29" t="s">
+        <v>1288</v>
+      </c>
+      <c r="J1250" s="29"/>
+      <c r="K1250" s="29" t="s">
+        <v>1285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Menu items for computer vision utilities   Issue #53
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,12 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5888" uniqueCount="1311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5920" uniqueCount="1318">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
   <si>
-    <t xml:space="preserve">Revision 2.X    04/25/2022 – Added DC Motor Sim</t>
+    <t xml:space="preserve">Revision 2.X    04/27/2022 – Added computer vision utility</t>
   </si>
   <si>
     <t xml:space="preserve">This documents which Java/C++ WPILIB routines have been </t>
@@ -3656,6 +3656,27 @@
   </si>
   <si>
     <t xml:space="preserve">Riccati_Input_Check.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VISION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPUTER VISION UTILITIES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CompVisionUtil_CalculateDistanceToTarget.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CompVisionUtil_EstimateCameraToTarget.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CompVisionUtil_EstimateFieldToCamera.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CompVisionUtil_EstimateFieldToRobot.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CompVisionUtil_EstimateFieldToRobot_Alt.vi</t>
   </si>
   <si>
     <t xml:space="preserve">TYPE DEFINITIONS</t>
@@ -4426,10 +4447,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:Q1271"/>
+  <dimension ref="A1:AMI1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4540,30 +4561,30 @@
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">B10+B11</f>
-        <v>842</v>
+        <v>847</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C18:C1598,"X")</f>
-        <v>842</v>
+        <f aca="false">COUNTIF(C18:C1609,"X")</f>
+        <v>847</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D18:D1598,"X")</f>
+        <f aca="false">COUNTIF(D18:D1609,"X")</f>
         <v>255</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E18:E1598,"X")</f>
+        <f aca="false">COUNTIF(E18:E1609,"X")</f>
         <v>799</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F18:F1598,"S")+COUNTIF(F18:F1598,"I")+COUNTIF(F18:F1598,"X")+COUNTIF(F18:F1598,"SI")+COUNTIF(F18:F1598,"IS")+COUNTIF(F18:F1598,"N/A")</f>
+        <f aca="false">COUNTIF(F18:F1609,"S")+COUNTIF(F18:F1609,"I")+COUNTIF(F18:F1609,"X")+COUNTIF(F18:F1609,"SI")+COUNTIF(F18:F1609,"IS")+COUNTIF(F18:F1609,"N/A")</f>
         <v>439</v>
       </c>
       <c r="G9" s="13" t="n">
-        <f aca="false">COUNTIF(G18:G1598,"S")+COUNTIF(G18:G1598,"I")+COUNTIF(G18:G1598,"X")+COUNTIF(G18:G1598,"SI")+COUNTIF(G18:G1598,"IS")+COUNTIF(G18:G1598,"N/A")</f>
+        <f aca="false">COUNTIF(G18:G1609,"S")+COUNTIF(G18:G1609,"I")+COUNTIF(G18:G1609,"X")+COUNTIF(G18:G1609,"SI")+COUNTIF(G18:G1609,"IS")+COUNTIF(G18:G1609,"N/A")</f>
         <v>26</v>
       </c>
       <c r="H9" s="13" t="n">
-        <f aca="false">COUNTIF(H18:H1598,"S")+COUNTIF(H18:H1598,"I")+COUNTIF(H18:H1598,"X")+COUNTIF(H18:H1598,"SI")+COUNTIF(H18:H1598,"IS")+COUNTIF(H18:H1598,"N/A")</f>
+        <f aca="false">COUNTIF(H18:H1609,"S")+COUNTIF(H18:H1609,"I")+COUNTIF(H18:H1609,"X")+COUNTIF(H18:H1609,"SI")+COUNTIF(H18:H1609,"IS")+COUNTIF(H18:H1609,"N/A")</f>
         <v>12</v>
       </c>
       <c r="I9" s="14" t="n">
@@ -4576,8 +4597,8 @@
         <v>14</v>
       </c>
       <c r="B10" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1598,"X")</f>
-        <v>756</v>
+        <f aca="false">COUNTIF(B18:B1609,"X")</f>
+        <v>761</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>15</v>
@@ -4588,12 +4609,12 @@
         <v>16</v>
       </c>
       <c r="B11" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1598,"Z")</f>
+        <f aca="false">COUNTIF(B18:B1609,"Z")</f>
         <v>86</v>
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.521377672209026</v>
+        <v>0.518299881936246</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4601,7 +4622,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1598,"/")</f>
+        <f aca="false">COUNTIF(B18:B1609,"/")</f>
         <v>4</v>
       </c>
       <c r="I12" s="4"/>
@@ -4611,7 +4632,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="13" t="n">
-        <f aca="false">COUNTIF(B18:B1598,"\")</f>
+        <f aca="false">COUNTIF(B18:B1609,"\")</f>
         <v>2</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -31023,37 +31044,31 @@
       <c r="N1174" s="22"/>
     </row>
     <row r="1175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1175" s="22"/>
-      <c r="C1175" s="22"/>
-      <c r="D1175" s="22"/>
-      <c r="E1175" s="22"/>
-      <c r="F1175" s="22"/>
-      <c r="G1175" s="22"/>
-      <c r="H1175" s="22"/>
-      <c r="I1175" s="23"/>
-      <c r="J1175" s="23"/>
-      <c r="K1175" s="23"/>
-      <c r="L1175" s="22"/>
-      <c r="M1175" s="22"/>
-      <c r="N1175" s="22"/>
+      <c r="A1175" s="9"/>
     </row>
     <row r="1176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1176" s="48"/>
-      <c r="C1176" s="1"/>
-      <c r="D1176" s="1"/>
-      <c r="E1176" s="1"/>
-      <c r="F1176" s="1"/>
-      <c r="G1176" s="1"/>
-      <c r="H1176" s="1"/>
-      <c r="I1176" s="1"/>
-      <c r="J1176" s="1"/>
-      <c r="K1176" s="1"/>
-      <c r="L1176" s="1"/>
-      <c r="M1176" s="1"/>
-      <c r="N1176" s="1"/>
+      <c r="A1176" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1176" s="17"/>
+      <c r="C1176" s="18"/>
+      <c r="D1176" s="18"/>
+      <c r="E1176" s="18"/>
+      <c r="F1176" s="18"/>
+      <c r="G1176" s="18"/>
+      <c r="H1176" s="18"/>
     </row>
     <row r="1177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1177" s="9"/>
+      <c r="A1177" s="16" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B1177" s="17"/>
+      <c r="C1177" s="18"/>
+      <c r="D1177" s="18"/>
+      <c r="E1177" s="18"/>
+      <c r="F1177" s="18"/>
+      <c r="G1177" s="18"/>
+      <c r="H1177" s="18"/>
     </row>
     <row r="1178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1178" s="16" t="s">
@@ -31068,81 +31083,1095 @@
       <c r="H1178" s="18"/>
     </row>
     <row r="1179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1179" s="16" t="s">
-        <v>1211</v>
-      </c>
-      <c r="B1179" s="17"/>
-      <c r="C1179" s="18"/>
-      <c r="D1179" s="18"/>
-      <c r="E1179" s="18"/>
-      <c r="F1179" s="18"/>
-      <c r="G1179" s="18"/>
-      <c r="H1179" s="18"/>
-    </row>
-    <row r="1180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1180" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1180" s="17"/>
-      <c r="C1180" s="18"/>
-      <c r="D1180" s="18"/>
-      <c r="E1180" s="18"/>
-      <c r="F1180" s="18"/>
-      <c r="G1180" s="18"/>
-      <c r="H1180" s="18"/>
-    </row>
-    <row r="1181" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1181" s="9"/>
-      <c r="B1181" s="11" t="s">
+      <c r="B1179" s="48"/>
+      <c r="C1179" s="1"/>
+      <c r="D1179" s="1"/>
+      <c r="E1179" s="1"/>
+      <c r="F1179" s="1"/>
+      <c r="G1179" s="1"/>
+      <c r="H1179" s="1"/>
+      <c r="I1179" s="1"/>
+      <c r="J1179" s="1"/>
+      <c r="K1179" s="1"/>
+      <c r="L1179" s="1"/>
+      <c r="M1179" s="1"/>
+      <c r="N1179" s="1"/>
+      <c r="Y1179" s="0"/>
+      <c r="Z1179" s="0"/>
+      <c r="AA1179" s="0"/>
+      <c r="AB1179" s="0"/>
+      <c r="AC1179" s="0"/>
+      <c r="AD1179" s="0"/>
+      <c r="AE1179" s="0"/>
+      <c r="AF1179" s="0"/>
+      <c r="AG1179" s="0"/>
+      <c r="AH1179" s="0"/>
+      <c r="AI1179" s="0"/>
+      <c r="AJ1179" s="0"/>
+      <c r="AK1179" s="0"/>
+      <c r="AL1179" s="0"/>
+      <c r="AM1179" s="0"/>
+      <c r="AN1179" s="0"/>
+      <c r="AO1179" s="0"/>
+      <c r="AP1179" s="0"/>
+      <c r="AQ1179" s="0"/>
+      <c r="AR1179" s="0"/>
+      <c r="AS1179" s="0"/>
+      <c r="AT1179" s="0"/>
+      <c r="AU1179" s="0"/>
+      <c r="AV1179" s="0"/>
+      <c r="AW1179" s="0"/>
+      <c r="AX1179" s="0"/>
+      <c r="AY1179" s="0"/>
+      <c r="AZ1179" s="0"/>
+      <c r="BA1179" s="0"/>
+      <c r="BB1179" s="0"/>
+      <c r="BC1179" s="0"/>
+      <c r="BD1179" s="0"/>
+      <c r="BE1179" s="0"/>
+      <c r="BF1179" s="0"/>
+      <c r="BG1179" s="0"/>
+      <c r="BH1179" s="0"/>
+      <c r="BI1179" s="0"/>
+      <c r="BJ1179" s="0"/>
+      <c r="BK1179" s="0"/>
+      <c r="BL1179" s="0"/>
+      <c r="BM1179" s="0"/>
+      <c r="BN1179" s="0"/>
+      <c r="BO1179" s="0"/>
+      <c r="BP1179" s="0"/>
+      <c r="BQ1179" s="0"/>
+      <c r="BR1179" s="0"/>
+      <c r="BS1179" s="0"/>
+      <c r="BT1179" s="0"/>
+      <c r="BU1179" s="0"/>
+      <c r="BV1179" s="0"/>
+      <c r="BW1179" s="0"/>
+      <c r="BX1179" s="0"/>
+      <c r="BY1179" s="0"/>
+      <c r="BZ1179" s="0"/>
+      <c r="CA1179" s="0"/>
+      <c r="CB1179" s="0"/>
+      <c r="CC1179" s="0"/>
+      <c r="CD1179" s="0"/>
+      <c r="CE1179" s="0"/>
+      <c r="CF1179" s="0"/>
+      <c r="CG1179" s="0"/>
+      <c r="CH1179" s="0"/>
+      <c r="CI1179" s="0"/>
+      <c r="CJ1179" s="0"/>
+      <c r="CK1179" s="0"/>
+      <c r="CL1179" s="0"/>
+      <c r="CM1179" s="0"/>
+      <c r="CN1179" s="0"/>
+      <c r="CO1179" s="0"/>
+      <c r="CP1179" s="0"/>
+      <c r="CQ1179" s="0"/>
+      <c r="CR1179" s="0"/>
+      <c r="CS1179" s="0"/>
+      <c r="CT1179" s="0"/>
+      <c r="CU1179" s="0"/>
+      <c r="CV1179" s="0"/>
+      <c r="CW1179" s="0"/>
+      <c r="CX1179" s="0"/>
+      <c r="CY1179" s="0"/>
+      <c r="CZ1179" s="0"/>
+      <c r="DA1179" s="0"/>
+      <c r="DB1179" s="0"/>
+      <c r="DC1179" s="0"/>
+      <c r="DD1179" s="0"/>
+      <c r="DE1179" s="0"/>
+      <c r="DF1179" s="0"/>
+      <c r="DG1179" s="0"/>
+      <c r="DH1179" s="0"/>
+      <c r="DI1179" s="0"/>
+      <c r="DJ1179" s="0"/>
+      <c r="DK1179" s="0"/>
+      <c r="DL1179" s="0"/>
+      <c r="DM1179" s="0"/>
+      <c r="DN1179" s="0"/>
+      <c r="DO1179" s="0"/>
+      <c r="DP1179" s="0"/>
+      <c r="DQ1179" s="0"/>
+      <c r="DR1179" s="0"/>
+      <c r="DS1179" s="0"/>
+      <c r="DT1179" s="0"/>
+      <c r="DU1179" s="0"/>
+      <c r="DV1179" s="0"/>
+      <c r="DW1179" s="0"/>
+      <c r="DX1179" s="0"/>
+      <c r="DY1179" s="0"/>
+      <c r="DZ1179" s="0"/>
+      <c r="EA1179" s="0"/>
+      <c r="EB1179" s="0"/>
+      <c r="EC1179" s="0"/>
+      <c r="ED1179" s="0"/>
+      <c r="EE1179" s="0"/>
+      <c r="EF1179" s="0"/>
+      <c r="EG1179" s="0"/>
+      <c r="EH1179" s="0"/>
+      <c r="EI1179" s="0"/>
+      <c r="EJ1179" s="0"/>
+      <c r="EK1179" s="0"/>
+      <c r="EL1179" s="0"/>
+      <c r="EM1179" s="0"/>
+      <c r="EN1179" s="0"/>
+      <c r="EO1179" s="0"/>
+      <c r="EP1179" s="0"/>
+      <c r="EQ1179" s="0"/>
+      <c r="ER1179" s="0"/>
+      <c r="ES1179" s="0"/>
+      <c r="ET1179" s="0"/>
+      <c r="EU1179" s="0"/>
+      <c r="EV1179" s="0"/>
+      <c r="EW1179" s="0"/>
+      <c r="EX1179" s="0"/>
+      <c r="EY1179" s="0"/>
+      <c r="EZ1179" s="0"/>
+      <c r="FA1179" s="0"/>
+      <c r="FB1179" s="0"/>
+      <c r="FC1179" s="0"/>
+      <c r="FD1179" s="0"/>
+      <c r="FE1179" s="0"/>
+      <c r="FF1179" s="0"/>
+      <c r="FG1179" s="0"/>
+      <c r="FH1179" s="0"/>
+      <c r="FI1179" s="0"/>
+      <c r="FJ1179" s="0"/>
+      <c r="FK1179" s="0"/>
+      <c r="FL1179" s="0"/>
+      <c r="FM1179" s="0"/>
+      <c r="FN1179" s="0"/>
+      <c r="FO1179" s="0"/>
+      <c r="FP1179" s="0"/>
+      <c r="FQ1179" s="0"/>
+      <c r="FR1179" s="0"/>
+      <c r="FS1179" s="0"/>
+      <c r="FT1179" s="0"/>
+      <c r="FU1179" s="0"/>
+      <c r="FV1179" s="0"/>
+      <c r="FW1179" s="0"/>
+      <c r="FX1179" s="0"/>
+      <c r="FY1179" s="0"/>
+      <c r="FZ1179" s="0"/>
+      <c r="GA1179" s="0"/>
+      <c r="GB1179" s="0"/>
+      <c r="GC1179" s="0"/>
+      <c r="GD1179" s="0"/>
+      <c r="GE1179" s="0"/>
+      <c r="GF1179" s="0"/>
+      <c r="GG1179" s="0"/>
+      <c r="GH1179" s="0"/>
+      <c r="GI1179" s="0"/>
+      <c r="GJ1179" s="0"/>
+      <c r="GK1179" s="0"/>
+      <c r="GL1179" s="0"/>
+      <c r="GM1179" s="0"/>
+      <c r="GN1179" s="0"/>
+      <c r="GO1179" s="0"/>
+      <c r="GP1179" s="0"/>
+      <c r="GQ1179" s="0"/>
+      <c r="GR1179" s="0"/>
+      <c r="GS1179" s="0"/>
+      <c r="GT1179" s="0"/>
+      <c r="GU1179" s="0"/>
+      <c r="GV1179" s="0"/>
+      <c r="GW1179" s="0"/>
+      <c r="GX1179" s="0"/>
+      <c r="GY1179" s="0"/>
+      <c r="GZ1179" s="0"/>
+      <c r="HA1179" s="0"/>
+      <c r="HB1179" s="0"/>
+      <c r="HC1179" s="0"/>
+      <c r="HD1179" s="0"/>
+      <c r="HE1179" s="0"/>
+      <c r="HF1179" s="0"/>
+      <c r="HG1179" s="0"/>
+      <c r="HH1179" s="0"/>
+      <c r="HI1179" s="0"/>
+      <c r="HJ1179" s="0"/>
+      <c r="HK1179" s="0"/>
+      <c r="HL1179" s="0"/>
+      <c r="HM1179" s="0"/>
+      <c r="HN1179" s="0"/>
+      <c r="HO1179" s="0"/>
+      <c r="HP1179" s="0"/>
+      <c r="HQ1179" s="0"/>
+      <c r="HR1179" s="0"/>
+      <c r="HS1179" s="0"/>
+      <c r="HT1179" s="0"/>
+      <c r="HU1179" s="0"/>
+      <c r="HV1179" s="0"/>
+      <c r="HW1179" s="0"/>
+      <c r="HX1179" s="0"/>
+      <c r="HY1179" s="0"/>
+      <c r="HZ1179" s="0"/>
+      <c r="IA1179" s="0"/>
+      <c r="IB1179" s="0"/>
+      <c r="IC1179" s="0"/>
+      <c r="ID1179" s="0"/>
+      <c r="IE1179" s="0"/>
+      <c r="IF1179" s="0"/>
+      <c r="IG1179" s="0"/>
+      <c r="IH1179" s="0"/>
+      <c r="II1179" s="0"/>
+      <c r="IJ1179" s="0"/>
+      <c r="IK1179" s="0"/>
+      <c r="IL1179" s="0"/>
+      <c r="IM1179" s="0"/>
+      <c r="IN1179" s="0"/>
+      <c r="IO1179" s="0"/>
+      <c r="IP1179" s="0"/>
+      <c r="IQ1179" s="0"/>
+      <c r="IR1179" s="0"/>
+      <c r="IS1179" s="0"/>
+      <c r="IT1179" s="0"/>
+      <c r="IU1179" s="0"/>
+      <c r="IV1179" s="0"/>
+      <c r="IW1179" s="0"/>
+      <c r="IX1179" s="0"/>
+      <c r="IY1179" s="0"/>
+      <c r="IZ1179" s="0"/>
+      <c r="JA1179" s="0"/>
+      <c r="JB1179" s="0"/>
+      <c r="JC1179" s="0"/>
+      <c r="JD1179" s="0"/>
+      <c r="JE1179" s="0"/>
+      <c r="JF1179" s="0"/>
+      <c r="JG1179" s="0"/>
+      <c r="JH1179" s="0"/>
+      <c r="JI1179" s="0"/>
+      <c r="JJ1179" s="0"/>
+      <c r="JK1179" s="0"/>
+      <c r="JL1179" s="0"/>
+      <c r="JM1179" s="0"/>
+      <c r="JN1179" s="0"/>
+      <c r="JO1179" s="0"/>
+      <c r="JP1179" s="0"/>
+      <c r="JQ1179" s="0"/>
+      <c r="JR1179" s="0"/>
+      <c r="JS1179" s="0"/>
+      <c r="JT1179" s="0"/>
+      <c r="JU1179" s="0"/>
+      <c r="JV1179" s="0"/>
+      <c r="JW1179" s="0"/>
+      <c r="JX1179" s="0"/>
+      <c r="JY1179" s="0"/>
+      <c r="JZ1179" s="0"/>
+      <c r="KA1179" s="0"/>
+      <c r="KB1179" s="0"/>
+      <c r="KC1179" s="0"/>
+      <c r="KD1179" s="0"/>
+      <c r="KE1179" s="0"/>
+      <c r="KF1179" s="0"/>
+      <c r="KG1179" s="0"/>
+      <c r="KH1179" s="0"/>
+      <c r="KI1179" s="0"/>
+      <c r="KJ1179" s="0"/>
+      <c r="KK1179" s="0"/>
+      <c r="KL1179" s="0"/>
+      <c r="KM1179" s="0"/>
+      <c r="KN1179" s="0"/>
+      <c r="KO1179" s="0"/>
+      <c r="KP1179" s="0"/>
+      <c r="KQ1179" s="0"/>
+      <c r="KR1179" s="0"/>
+      <c r="KS1179" s="0"/>
+      <c r="KT1179" s="0"/>
+      <c r="KU1179" s="0"/>
+      <c r="KV1179" s="0"/>
+      <c r="KW1179" s="0"/>
+      <c r="KX1179" s="0"/>
+      <c r="KY1179" s="0"/>
+      <c r="KZ1179" s="0"/>
+      <c r="LA1179" s="0"/>
+      <c r="LB1179" s="0"/>
+      <c r="LC1179" s="0"/>
+      <c r="LD1179" s="0"/>
+      <c r="LE1179" s="0"/>
+      <c r="LF1179" s="0"/>
+      <c r="LG1179" s="0"/>
+      <c r="LH1179" s="0"/>
+      <c r="LI1179" s="0"/>
+      <c r="LJ1179" s="0"/>
+      <c r="LK1179" s="0"/>
+      <c r="LL1179" s="0"/>
+      <c r="LM1179" s="0"/>
+      <c r="LN1179" s="0"/>
+      <c r="LO1179" s="0"/>
+      <c r="LP1179" s="0"/>
+      <c r="LQ1179" s="0"/>
+      <c r="LR1179" s="0"/>
+      <c r="LS1179" s="0"/>
+      <c r="LT1179" s="0"/>
+      <c r="LU1179" s="0"/>
+      <c r="LV1179" s="0"/>
+      <c r="LW1179" s="0"/>
+      <c r="LX1179" s="0"/>
+      <c r="LY1179" s="0"/>
+      <c r="LZ1179" s="0"/>
+      <c r="MA1179" s="0"/>
+      <c r="MB1179" s="0"/>
+      <c r="MC1179" s="0"/>
+      <c r="MD1179" s="0"/>
+      <c r="ME1179" s="0"/>
+      <c r="MF1179" s="0"/>
+      <c r="MG1179" s="0"/>
+      <c r="MH1179" s="0"/>
+      <c r="MI1179" s="0"/>
+      <c r="MJ1179" s="0"/>
+      <c r="MK1179" s="0"/>
+      <c r="ML1179" s="0"/>
+      <c r="MM1179" s="0"/>
+      <c r="MN1179" s="0"/>
+      <c r="MO1179" s="0"/>
+      <c r="MP1179" s="0"/>
+      <c r="MQ1179" s="0"/>
+      <c r="MR1179" s="0"/>
+      <c r="MS1179" s="0"/>
+      <c r="MT1179" s="0"/>
+      <c r="MU1179" s="0"/>
+      <c r="MV1179" s="0"/>
+      <c r="MW1179" s="0"/>
+      <c r="MX1179" s="0"/>
+      <c r="MY1179" s="0"/>
+      <c r="MZ1179" s="0"/>
+      <c r="NA1179" s="0"/>
+      <c r="NB1179" s="0"/>
+      <c r="NC1179" s="0"/>
+      <c r="ND1179" s="0"/>
+      <c r="NE1179" s="0"/>
+      <c r="NF1179" s="0"/>
+      <c r="NG1179" s="0"/>
+      <c r="NH1179" s="0"/>
+      <c r="NI1179" s="0"/>
+      <c r="NJ1179" s="0"/>
+      <c r="NK1179" s="0"/>
+      <c r="NL1179" s="0"/>
+      <c r="NM1179" s="0"/>
+      <c r="NN1179" s="0"/>
+      <c r="NO1179" s="0"/>
+      <c r="NP1179" s="0"/>
+      <c r="NQ1179" s="0"/>
+      <c r="NR1179" s="0"/>
+      <c r="NS1179" s="0"/>
+      <c r="NT1179" s="0"/>
+      <c r="NU1179" s="0"/>
+      <c r="NV1179" s="0"/>
+      <c r="NW1179" s="0"/>
+      <c r="NX1179" s="0"/>
+      <c r="NY1179" s="0"/>
+      <c r="NZ1179" s="0"/>
+      <c r="OA1179" s="0"/>
+      <c r="OB1179" s="0"/>
+      <c r="OC1179" s="0"/>
+      <c r="OD1179" s="0"/>
+      <c r="OE1179" s="0"/>
+      <c r="OF1179" s="0"/>
+      <c r="OG1179" s="0"/>
+      <c r="OH1179" s="0"/>
+      <c r="OI1179" s="0"/>
+      <c r="OJ1179" s="0"/>
+      <c r="OK1179" s="0"/>
+      <c r="OL1179" s="0"/>
+      <c r="OM1179" s="0"/>
+      <c r="ON1179" s="0"/>
+      <c r="OO1179" s="0"/>
+      <c r="OP1179" s="0"/>
+      <c r="OQ1179" s="0"/>
+      <c r="OR1179" s="0"/>
+      <c r="OS1179" s="0"/>
+      <c r="OT1179" s="0"/>
+      <c r="OU1179" s="0"/>
+      <c r="OV1179" s="0"/>
+      <c r="OW1179" s="0"/>
+      <c r="OX1179" s="0"/>
+      <c r="OY1179" s="0"/>
+      <c r="OZ1179" s="0"/>
+      <c r="PA1179" s="0"/>
+      <c r="PB1179" s="0"/>
+      <c r="PC1179" s="0"/>
+      <c r="PD1179" s="0"/>
+      <c r="PE1179" s="0"/>
+      <c r="PF1179" s="0"/>
+      <c r="PG1179" s="0"/>
+      <c r="PH1179" s="0"/>
+      <c r="PI1179" s="0"/>
+      <c r="PJ1179" s="0"/>
+      <c r="PK1179" s="0"/>
+      <c r="PL1179" s="0"/>
+      <c r="PM1179" s="0"/>
+      <c r="PN1179" s="0"/>
+      <c r="PO1179" s="0"/>
+      <c r="PP1179" s="0"/>
+      <c r="PQ1179" s="0"/>
+      <c r="PR1179" s="0"/>
+      <c r="PS1179" s="0"/>
+      <c r="PT1179" s="0"/>
+      <c r="PU1179" s="0"/>
+      <c r="PV1179" s="0"/>
+      <c r="PW1179" s="0"/>
+      <c r="PX1179" s="0"/>
+      <c r="PY1179" s="0"/>
+      <c r="PZ1179" s="0"/>
+      <c r="QA1179" s="0"/>
+      <c r="QB1179" s="0"/>
+      <c r="QC1179" s="0"/>
+      <c r="QD1179" s="0"/>
+      <c r="QE1179" s="0"/>
+      <c r="QF1179" s="0"/>
+      <c r="QG1179" s="0"/>
+      <c r="QH1179" s="0"/>
+      <c r="QI1179" s="0"/>
+      <c r="QJ1179" s="0"/>
+      <c r="QK1179" s="0"/>
+      <c r="QL1179" s="0"/>
+      <c r="QM1179" s="0"/>
+      <c r="QN1179" s="0"/>
+      <c r="QO1179" s="0"/>
+      <c r="QP1179" s="0"/>
+      <c r="QQ1179" s="0"/>
+      <c r="QR1179" s="0"/>
+      <c r="QS1179" s="0"/>
+      <c r="QT1179" s="0"/>
+      <c r="QU1179" s="0"/>
+      <c r="QV1179" s="0"/>
+      <c r="QW1179" s="0"/>
+      <c r="QX1179" s="0"/>
+      <c r="QY1179" s="0"/>
+      <c r="QZ1179" s="0"/>
+      <c r="RA1179" s="0"/>
+      <c r="RB1179" s="0"/>
+      <c r="RC1179" s="0"/>
+      <c r="RD1179" s="0"/>
+      <c r="RE1179" s="0"/>
+      <c r="RF1179" s="0"/>
+      <c r="RG1179" s="0"/>
+      <c r="RH1179" s="0"/>
+      <c r="RI1179" s="0"/>
+      <c r="RJ1179" s="0"/>
+      <c r="RK1179" s="0"/>
+      <c r="RL1179" s="0"/>
+      <c r="RM1179" s="0"/>
+      <c r="RN1179" s="0"/>
+      <c r="RO1179" s="0"/>
+      <c r="RP1179" s="0"/>
+      <c r="RQ1179" s="0"/>
+      <c r="RR1179" s="0"/>
+      <c r="RS1179" s="0"/>
+      <c r="RT1179" s="0"/>
+      <c r="RU1179" s="0"/>
+      <c r="RV1179" s="0"/>
+      <c r="RW1179" s="0"/>
+      <c r="RX1179" s="0"/>
+      <c r="RY1179" s="0"/>
+      <c r="RZ1179" s="0"/>
+      <c r="SA1179" s="0"/>
+      <c r="SB1179" s="0"/>
+      <c r="SC1179" s="0"/>
+      <c r="SD1179" s="0"/>
+      <c r="SE1179" s="0"/>
+      <c r="SF1179" s="0"/>
+      <c r="SG1179" s="0"/>
+      <c r="SH1179" s="0"/>
+      <c r="SI1179" s="0"/>
+      <c r="SJ1179" s="0"/>
+      <c r="SK1179" s="0"/>
+      <c r="SL1179" s="0"/>
+      <c r="SM1179" s="0"/>
+      <c r="SN1179" s="0"/>
+      <c r="SO1179" s="0"/>
+      <c r="SP1179" s="0"/>
+      <c r="SQ1179" s="0"/>
+      <c r="SR1179" s="0"/>
+      <c r="SS1179" s="0"/>
+      <c r="ST1179" s="0"/>
+      <c r="SU1179" s="0"/>
+      <c r="SV1179" s="0"/>
+      <c r="SW1179" s="0"/>
+      <c r="SX1179" s="0"/>
+      <c r="SY1179" s="0"/>
+      <c r="SZ1179" s="0"/>
+      <c r="TA1179" s="0"/>
+      <c r="TB1179" s="0"/>
+      <c r="TC1179" s="0"/>
+      <c r="TD1179" s="0"/>
+      <c r="TE1179" s="0"/>
+      <c r="TF1179" s="0"/>
+      <c r="TG1179" s="0"/>
+      <c r="TH1179" s="0"/>
+      <c r="TI1179" s="0"/>
+      <c r="TJ1179" s="0"/>
+      <c r="TK1179" s="0"/>
+      <c r="TL1179" s="0"/>
+      <c r="TM1179" s="0"/>
+      <c r="TN1179" s="0"/>
+      <c r="TO1179" s="0"/>
+      <c r="TP1179" s="0"/>
+      <c r="TQ1179" s="0"/>
+      <c r="TR1179" s="0"/>
+      <c r="TS1179" s="0"/>
+      <c r="TT1179" s="0"/>
+      <c r="TU1179" s="0"/>
+      <c r="TV1179" s="0"/>
+      <c r="TW1179" s="0"/>
+      <c r="TX1179" s="0"/>
+      <c r="TY1179" s="0"/>
+      <c r="TZ1179" s="0"/>
+      <c r="UA1179" s="0"/>
+      <c r="UB1179" s="0"/>
+      <c r="UC1179" s="0"/>
+      <c r="UD1179" s="0"/>
+      <c r="UE1179" s="0"/>
+      <c r="UF1179" s="0"/>
+      <c r="UG1179" s="0"/>
+      <c r="UH1179" s="0"/>
+      <c r="UI1179" s="0"/>
+      <c r="UJ1179" s="0"/>
+      <c r="UK1179" s="0"/>
+      <c r="UL1179" s="0"/>
+      <c r="UM1179" s="0"/>
+      <c r="UN1179" s="0"/>
+      <c r="UO1179" s="0"/>
+      <c r="UP1179" s="0"/>
+      <c r="UQ1179" s="0"/>
+      <c r="UR1179" s="0"/>
+      <c r="US1179" s="0"/>
+      <c r="UT1179" s="0"/>
+      <c r="UU1179" s="0"/>
+      <c r="UV1179" s="0"/>
+      <c r="UW1179" s="0"/>
+      <c r="UX1179" s="0"/>
+      <c r="UY1179" s="0"/>
+      <c r="UZ1179" s="0"/>
+      <c r="VA1179" s="0"/>
+      <c r="VB1179" s="0"/>
+      <c r="VC1179" s="0"/>
+      <c r="VD1179" s="0"/>
+      <c r="VE1179" s="0"/>
+      <c r="VF1179" s="0"/>
+      <c r="VG1179" s="0"/>
+      <c r="VH1179" s="0"/>
+      <c r="VI1179" s="0"/>
+      <c r="VJ1179" s="0"/>
+      <c r="VK1179" s="0"/>
+      <c r="VL1179" s="0"/>
+      <c r="VM1179" s="0"/>
+      <c r="VN1179" s="0"/>
+      <c r="VO1179" s="0"/>
+      <c r="VP1179" s="0"/>
+      <c r="VQ1179" s="0"/>
+      <c r="VR1179" s="0"/>
+      <c r="VS1179" s="0"/>
+      <c r="VT1179" s="0"/>
+      <c r="VU1179" s="0"/>
+      <c r="VV1179" s="0"/>
+      <c r="VW1179" s="0"/>
+      <c r="VX1179" s="0"/>
+      <c r="VY1179" s="0"/>
+      <c r="VZ1179" s="0"/>
+      <c r="WA1179" s="0"/>
+      <c r="WB1179" s="0"/>
+      <c r="WC1179" s="0"/>
+      <c r="WD1179" s="0"/>
+      <c r="WE1179" s="0"/>
+      <c r="WF1179" s="0"/>
+      <c r="WG1179" s="0"/>
+      <c r="WH1179" s="0"/>
+      <c r="WI1179" s="0"/>
+      <c r="WJ1179" s="0"/>
+      <c r="WK1179" s="0"/>
+      <c r="WL1179" s="0"/>
+      <c r="WM1179" s="0"/>
+      <c r="WN1179" s="0"/>
+      <c r="WO1179" s="0"/>
+      <c r="WP1179" s="0"/>
+      <c r="WQ1179" s="0"/>
+      <c r="WR1179" s="0"/>
+      <c r="WS1179" s="0"/>
+      <c r="WT1179" s="0"/>
+      <c r="WU1179" s="0"/>
+      <c r="WV1179" s="0"/>
+      <c r="WW1179" s="0"/>
+      <c r="WX1179" s="0"/>
+      <c r="WY1179" s="0"/>
+      <c r="WZ1179" s="0"/>
+      <c r="XA1179" s="0"/>
+      <c r="XB1179" s="0"/>
+      <c r="XC1179" s="0"/>
+      <c r="XD1179" s="0"/>
+      <c r="XE1179" s="0"/>
+      <c r="XF1179" s="0"/>
+      <c r="XG1179" s="0"/>
+      <c r="XH1179" s="0"/>
+      <c r="XI1179" s="0"/>
+      <c r="XJ1179" s="0"/>
+      <c r="XK1179" s="0"/>
+      <c r="XL1179" s="0"/>
+      <c r="XM1179" s="0"/>
+      <c r="XN1179" s="0"/>
+      <c r="XO1179" s="0"/>
+      <c r="XP1179" s="0"/>
+      <c r="XQ1179" s="0"/>
+      <c r="XR1179" s="0"/>
+      <c r="XS1179" s="0"/>
+      <c r="XT1179" s="0"/>
+      <c r="XU1179" s="0"/>
+      <c r="XV1179" s="0"/>
+      <c r="XW1179" s="0"/>
+      <c r="XX1179" s="0"/>
+      <c r="XY1179" s="0"/>
+      <c r="XZ1179" s="0"/>
+      <c r="YA1179" s="0"/>
+      <c r="YB1179" s="0"/>
+      <c r="YC1179" s="0"/>
+      <c r="YD1179" s="0"/>
+      <c r="YE1179" s="0"/>
+      <c r="YF1179" s="0"/>
+      <c r="YG1179" s="0"/>
+      <c r="YH1179" s="0"/>
+      <c r="YI1179" s="0"/>
+      <c r="YJ1179" s="0"/>
+      <c r="YK1179" s="0"/>
+      <c r="YL1179" s="0"/>
+      <c r="YM1179" s="0"/>
+      <c r="YN1179" s="0"/>
+      <c r="YO1179" s="0"/>
+      <c r="YP1179" s="0"/>
+      <c r="YQ1179" s="0"/>
+      <c r="YR1179" s="0"/>
+      <c r="YS1179" s="0"/>
+      <c r="YT1179" s="0"/>
+      <c r="YU1179" s="0"/>
+      <c r="YV1179" s="0"/>
+      <c r="YW1179" s="0"/>
+      <c r="YX1179" s="0"/>
+      <c r="YY1179" s="0"/>
+      <c r="YZ1179" s="0"/>
+      <c r="ZA1179" s="0"/>
+      <c r="ZB1179" s="0"/>
+      <c r="ZC1179" s="0"/>
+      <c r="ZD1179" s="0"/>
+      <c r="ZE1179" s="0"/>
+      <c r="ZF1179" s="0"/>
+      <c r="ZG1179" s="0"/>
+      <c r="ZH1179" s="0"/>
+      <c r="ZI1179" s="0"/>
+      <c r="ZJ1179" s="0"/>
+      <c r="ZK1179" s="0"/>
+      <c r="ZL1179" s="0"/>
+      <c r="ZM1179" s="0"/>
+      <c r="ZN1179" s="0"/>
+      <c r="ZO1179" s="0"/>
+      <c r="ZP1179" s="0"/>
+      <c r="ZQ1179" s="0"/>
+      <c r="ZR1179" s="0"/>
+      <c r="ZS1179" s="0"/>
+      <c r="ZT1179" s="0"/>
+      <c r="ZU1179" s="0"/>
+      <c r="ZV1179" s="0"/>
+      <c r="ZW1179" s="0"/>
+      <c r="ZX1179" s="0"/>
+      <c r="ZY1179" s="0"/>
+      <c r="ZZ1179" s="0"/>
+      <c r="AAA1179" s="0"/>
+      <c r="AAB1179" s="0"/>
+      <c r="AAC1179" s="0"/>
+      <c r="AAD1179" s="0"/>
+      <c r="AAE1179" s="0"/>
+      <c r="AAF1179" s="0"/>
+      <c r="AAG1179" s="0"/>
+      <c r="AAH1179" s="0"/>
+      <c r="AAI1179" s="0"/>
+      <c r="AAJ1179" s="0"/>
+      <c r="AAK1179" s="0"/>
+      <c r="AAL1179" s="0"/>
+      <c r="AAM1179" s="0"/>
+      <c r="AAN1179" s="0"/>
+      <c r="AAO1179" s="0"/>
+      <c r="AAP1179" s="0"/>
+      <c r="AAQ1179" s="0"/>
+      <c r="AAR1179" s="0"/>
+      <c r="AAS1179" s="0"/>
+      <c r="AAT1179" s="0"/>
+      <c r="AAU1179" s="0"/>
+      <c r="AAV1179" s="0"/>
+      <c r="AAW1179" s="0"/>
+      <c r="AAX1179" s="0"/>
+      <c r="AAY1179" s="0"/>
+      <c r="AAZ1179" s="0"/>
+      <c r="ABA1179" s="0"/>
+      <c r="ABB1179" s="0"/>
+      <c r="ABC1179" s="0"/>
+      <c r="ABD1179" s="0"/>
+      <c r="ABE1179" s="0"/>
+      <c r="ABF1179" s="0"/>
+      <c r="ABG1179" s="0"/>
+      <c r="ABH1179" s="0"/>
+      <c r="ABI1179" s="0"/>
+      <c r="ABJ1179" s="0"/>
+      <c r="ABK1179" s="0"/>
+      <c r="ABL1179" s="0"/>
+      <c r="ABM1179" s="0"/>
+      <c r="ABN1179" s="0"/>
+      <c r="ABO1179" s="0"/>
+      <c r="ABP1179" s="0"/>
+      <c r="ABQ1179" s="0"/>
+      <c r="ABR1179" s="0"/>
+      <c r="ABS1179" s="0"/>
+      <c r="ABT1179" s="0"/>
+      <c r="ABU1179" s="0"/>
+      <c r="ABV1179" s="0"/>
+      <c r="ABW1179" s="0"/>
+      <c r="ABX1179" s="0"/>
+      <c r="ABY1179" s="0"/>
+      <c r="ABZ1179" s="0"/>
+      <c r="ACA1179" s="0"/>
+      <c r="ACB1179" s="0"/>
+      <c r="ACC1179" s="0"/>
+      <c r="ACD1179" s="0"/>
+      <c r="ACE1179" s="0"/>
+      <c r="ACF1179" s="0"/>
+      <c r="ACG1179" s="0"/>
+      <c r="ACH1179" s="0"/>
+      <c r="ACI1179" s="0"/>
+      <c r="ACJ1179" s="0"/>
+      <c r="ACK1179" s="0"/>
+      <c r="ACL1179" s="0"/>
+      <c r="ACM1179" s="0"/>
+      <c r="ACN1179" s="0"/>
+      <c r="ACO1179" s="0"/>
+      <c r="ACP1179" s="0"/>
+      <c r="ACQ1179" s="0"/>
+      <c r="ACR1179" s="0"/>
+      <c r="ACS1179" s="0"/>
+      <c r="ACT1179" s="0"/>
+      <c r="ACU1179" s="0"/>
+      <c r="ACV1179" s="0"/>
+      <c r="ACW1179" s="0"/>
+      <c r="ACX1179" s="0"/>
+      <c r="ACY1179" s="0"/>
+      <c r="ACZ1179" s="0"/>
+      <c r="ADA1179" s="0"/>
+      <c r="ADB1179" s="0"/>
+      <c r="ADC1179" s="0"/>
+      <c r="ADD1179" s="0"/>
+      <c r="ADE1179" s="0"/>
+      <c r="ADF1179" s="0"/>
+      <c r="ADG1179" s="0"/>
+      <c r="ADH1179" s="0"/>
+      <c r="ADI1179" s="0"/>
+      <c r="ADJ1179" s="0"/>
+      <c r="ADK1179" s="0"/>
+      <c r="ADL1179" s="0"/>
+      <c r="ADM1179" s="0"/>
+      <c r="ADN1179" s="0"/>
+      <c r="ADO1179" s="0"/>
+      <c r="ADP1179" s="0"/>
+      <c r="ADQ1179" s="0"/>
+      <c r="ADR1179" s="0"/>
+      <c r="ADS1179" s="0"/>
+      <c r="ADT1179" s="0"/>
+      <c r="ADU1179" s="0"/>
+      <c r="ADV1179" s="0"/>
+      <c r="ADW1179" s="0"/>
+      <c r="ADX1179" s="0"/>
+      <c r="ADY1179" s="0"/>
+      <c r="ADZ1179" s="0"/>
+      <c r="AEA1179" s="0"/>
+      <c r="AEB1179" s="0"/>
+      <c r="AEC1179" s="0"/>
+      <c r="AED1179" s="0"/>
+      <c r="AEE1179" s="0"/>
+      <c r="AEF1179" s="0"/>
+      <c r="AEG1179" s="0"/>
+      <c r="AEH1179" s="0"/>
+      <c r="AEI1179" s="0"/>
+      <c r="AEJ1179" s="0"/>
+      <c r="AEK1179" s="0"/>
+      <c r="AEL1179" s="0"/>
+      <c r="AEM1179" s="0"/>
+      <c r="AEN1179" s="0"/>
+      <c r="AEO1179" s="0"/>
+      <c r="AEP1179" s="0"/>
+      <c r="AEQ1179" s="0"/>
+      <c r="AER1179" s="0"/>
+      <c r="AES1179" s="0"/>
+      <c r="AET1179" s="0"/>
+      <c r="AEU1179" s="0"/>
+      <c r="AEV1179" s="0"/>
+      <c r="AEW1179" s="0"/>
+      <c r="AEX1179" s="0"/>
+      <c r="AEY1179" s="0"/>
+      <c r="AEZ1179" s="0"/>
+      <c r="AFA1179" s="0"/>
+      <c r="AFB1179" s="0"/>
+      <c r="AFC1179" s="0"/>
+      <c r="AFD1179" s="0"/>
+      <c r="AFE1179" s="0"/>
+      <c r="AFF1179" s="0"/>
+      <c r="AFG1179" s="0"/>
+      <c r="AFH1179" s="0"/>
+      <c r="AFI1179" s="0"/>
+      <c r="AFJ1179" s="0"/>
+      <c r="AFK1179" s="0"/>
+      <c r="AFL1179" s="0"/>
+      <c r="AFM1179" s="0"/>
+      <c r="AFN1179" s="0"/>
+      <c r="AFO1179" s="0"/>
+      <c r="AFP1179" s="0"/>
+      <c r="AFQ1179" s="0"/>
+      <c r="AFR1179" s="0"/>
+      <c r="AFS1179" s="0"/>
+      <c r="AFT1179" s="0"/>
+      <c r="AFU1179" s="0"/>
+      <c r="AFV1179" s="0"/>
+      <c r="AFW1179" s="0"/>
+      <c r="AFX1179" s="0"/>
+      <c r="AFY1179" s="0"/>
+      <c r="AFZ1179" s="0"/>
+      <c r="AGA1179" s="0"/>
+      <c r="AGB1179" s="0"/>
+      <c r="AGC1179" s="0"/>
+      <c r="AGD1179" s="0"/>
+      <c r="AGE1179" s="0"/>
+      <c r="AGF1179" s="0"/>
+      <c r="AGG1179" s="0"/>
+      <c r="AGH1179" s="0"/>
+      <c r="AGI1179" s="0"/>
+      <c r="AGJ1179" s="0"/>
+      <c r="AGK1179" s="0"/>
+      <c r="AGL1179" s="0"/>
+      <c r="AGM1179" s="0"/>
+      <c r="AGN1179" s="0"/>
+      <c r="AGO1179" s="0"/>
+      <c r="AGP1179" s="0"/>
+      <c r="AGQ1179" s="0"/>
+      <c r="AGR1179" s="0"/>
+      <c r="AGS1179" s="0"/>
+      <c r="AGT1179" s="0"/>
+      <c r="AGU1179" s="0"/>
+      <c r="AGV1179" s="0"/>
+      <c r="AGW1179" s="0"/>
+      <c r="AGX1179" s="0"/>
+      <c r="AGY1179" s="0"/>
+      <c r="AGZ1179" s="0"/>
+      <c r="AHA1179" s="0"/>
+      <c r="AHB1179" s="0"/>
+      <c r="AHC1179" s="0"/>
+      <c r="AHD1179" s="0"/>
+      <c r="AHE1179" s="0"/>
+      <c r="AHF1179" s="0"/>
+      <c r="AHG1179" s="0"/>
+      <c r="AHH1179" s="0"/>
+      <c r="AHI1179" s="0"/>
+      <c r="AHJ1179" s="0"/>
+      <c r="AHK1179" s="0"/>
+      <c r="AHL1179" s="0"/>
+      <c r="AHM1179" s="0"/>
+      <c r="AHN1179" s="0"/>
+      <c r="AHO1179" s="0"/>
+      <c r="AHP1179" s="0"/>
+      <c r="AHQ1179" s="0"/>
+      <c r="AHR1179" s="0"/>
+      <c r="AHS1179" s="0"/>
+      <c r="AHT1179" s="0"/>
+      <c r="AHU1179" s="0"/>
+      <c r="AHV1179" s="0"/>
+      <c r="AHW1179" s="0"/>
+      <c r="AHX1179" s="0"/>
+      <c r="AHY1179" s="0"/>
+      <c r="AHZ1179" s="0"/>
+      <c r="AIA1179" s="0"/>
+      <c r="AIB1179" s="0"/>
+      <c r="AIC1179" s="0"/>
+      <c r="AID1179" s="0"/>
+      <c r="AIE1179" s="0"/>
+      <c r="AIF1179" s="0"/>
+      <c r="AIG1179" s="0"/>
+      <c r="AIH1179" s="0"/>
+      <c r="AII1179" s="0"/>
+      <c r="AIJ1179" s="0"/>
+      <c r="AIK1179" s="0"/>
+      <c r="AIL1179" s="0"/>
+      <c r="AIM1179" s="0"/>
+      <c r="AIN1179" s="0"/>
+      <c r="AIO1179" s="0"/>
+      <c r="AIP1179" s="0"/>
+      <c r="AIQ1179" s="0"/>
+      <c r="AIR1179" s="0"/>
+      <c r="AIS1179" s="0"/>
+      <c r="AIT1179" s="0"/>
+      <c r="AIU1179" s="0"/>
+      <c r="AIV1179" s="0"/>
+      <c r="AIW1179" s="0"/>
+      <c r="AIX1179" s="0"/>
+      <c r="AIY1179" s="0"/>
+      <c r="AIZ1179" s="0"/>
+      <c r="AJA1179" s="0"/>
+      <c r="AJB1179" s="0"/>
+      <c r="AJC1179" s="0"/>
+      <c r="AJD1179" s="0"/>
+      <c r="AJE1179" s="0"/>
+      <c r="AJF1179" s="0"/>
+      <c r="AJG1179" s="0"/>
+      <c r="AJH1179" s="0"/>
+      <c r="AJI1179" s="0"/>
+      <c r="AJJ1179" s="0"/>
+      <c r="AJK1179" s="0"/>
+      <c r="AJL1179" s="0"/>
+      <c r="AJM1179" s="0"/>
+      <c r="AJN1179" s="0"/>
+      <c r="AJO1179" s="0"/>
+      <c r="AJP1179" s="0"/>
+      <c r="AJQ1179" s="0"/>
+      <c r="AJR1179" s="0"/>
+      <c r="AJS1179" s="0"/>
+      <c r="AJT1179" s="0"/>
+      <c r="AJU1179" s="0"/>
+      <c r="AJV1179" s="0"/>
+      <c r="AJW1179" s="0"/>
+      <c r="AJX1179" s="0"/>
+      <c r="AJY1179" s="0"/>
+      <c r="AJZ1179" s="0"/>
+      <c r="AKA1179" s="0"/>
+      <c r="AKB1179" s="0"/>
+      <c r="AKC1179" s="0"/>
+      <c r="AKD1179" s="0"/>
+      <c r="AKE1179" s="0"/>
+      <c r="AKF1179" s="0"/>
+      <c r="AKG1179" s="0"/>
+      <c r="AKH1179" s="0"/>
+      <c r="AKI1179" s="0"/>
+      <c r="AKJ1179" s="0"/>
+      <c r="AKK1179" s="0"/>
+      <c r="AKL1179" s="0"/>
+      <c r="AKM1179" s="0"/>
+      <c r="AKN1179" s="0"/>
+      <c r="AKO1179" s="0"/>
+      <c r="AKP1179" s="0"/>
+      <c r="AKQ1179" s="0"/>
+      <c r="AKR1179" s="0"/>
+      <c r="AKS1179" s="0"/>
+      <c r="AKT1179" s="0"/>
+      <c r="AKU1179" s="0"/>
+      <c r="AKV1179" s="0"/>
+      <c r="AKW1179" s="0"/>
+      <c r="AKX1179" s="0"/>
+      <c r="AKY1179" s="0"/>
+      <c r="AKZ1179" s="0"/>
+      <c r="ALA1179" s="0"/>
+      <c r="ALB1179" s="0"/>
+      <c r="ALC1179" s="0"/>
+      <c r="ALD1179" s="0"/>
+      <c r="ALE1179" s="0"/>
+      <c r="ALF1179" s="0"/>
+      <c r="ALG1179" s="0"/>
+      <c r="ALH1179" s="0"/>
+      <c r="ALI1179" s="0"/>
+      <c r="ALJ1179" s="0"/>
+      <c r="ALK1179" s="0"/>
+      <c r="ALL1179" s="0"/>
+      <c r="ALM1179" s="0"/>
+      <c r="ALN1179" s="0"/>
+      <c r="ALO1179" s="0"/>
+      <c r="ALP1179" s="0"/>
+      <c r="ALQ1179" s="0"/>
+      <c r="ALR1179" s="0"/>
+      <c r="ALS1179" s="0"/>
+      <c r="ALT1179" s="0"/>
+      <c r="ALU1179" s="0"/>
+      <c r="ALV1179" s="0"/>
+      <c r="ALW1179" s="0"/>
+      <c r="ALX1179" s="0"/>
+      <c r="ALY1179" s="0"/>
+      <c r="ALZ1179" s="0"/>
+      <c r="AMA1179" s="0"/>
+      <c r="AMB1179" s="0"/>
+      <c r="AMC1179" s="0"/>
+      <c r="AMD1179" s="0"/>
+      <c r="AME1179" s="0"/>
+      <c r="AMF1179" s="0"/>
+      <c r="AMG1179" s="0"/>
+      <c r="AMH1179" s="0"/>
+      <c r="AMI1179" s="0"/>
+    </row>
+    <row r="1180" customFormat="false" ht="111.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1180" s="19"/>
+      <c r="B1180" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1181" s="11" t="s">
+      <c r="C1180" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1181" s="11" t="s">
+      <c r="D1180" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1181" s="11" t="s">
+      <c r="E1180" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1181" s="11" t="s">
+      <c r="F1180" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G1181" s="11" t="s">
+      <c r="G1180" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1181" s="11" t="s">
+      <c r="H1180" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I1181" s="20" t="s">
+      <c r="I1180" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1181" s="20" t="s">
+      <c r="J1180" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1181" s="20" t="s">
+      <c r="K1180" s="20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="1182" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1182" s="21" t="s">
+      <c r="L1180" s="11" t="s">
+        <v>771</v>
+      </c>
+      <c r="M1180" s="11" t="s">
+        <v>772</v>
+      </c>
+      <c r="N1180" s="11" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="1181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1181" s="21" t="s">
         <v>1212</v>
       </c>
+      <c r="B1181" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1181" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1181" s="22"/>
+      <c r="E1181" s="22"/>
+      <c r="F1181" s="26"/>
+      <c r="G1181" s="22"/>
+      <c r="H1181" s="22"/>
+      <c r="I1181" s="23" t="s">
+        <v>1213</v>
+      </c>
+      <c r="J1181" s="23"/>
+      <c r="K1181" s="23"/>
+      <c r="L1181" s="22"/>
+      <c r="M1181" s="22"/>
+      <c r="N1181" s="22"/>
+    </row>
+    <row r="1182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1182" s="22" t="s">
-        <v>1213</v>
+        <v>27</v>
       </c>
       <c r="C1182" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1182" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1182" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1182" s="22" t="s">
-        <v>714</v>
-      </c>
+      <c r="D1182" s="22"/>
+      <c r="E1182" s="22"/>
+      <c r="F1182" s="26"/>
       <c r="G1182" s="22"/>
       <c r="H1182" s="22"/>
       <c r="I1182" s="23" t="s">
@@ -31150,24 +32179,20 @@
       </c>
       <c r="J1182" s="23"/>
       <c r="K1182" s="23"/>
-    </row>
-    <row r="1183" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1183" s="21"/>
+      <c r="L1182" s="22"/>
+      <c r="M1182" s="22"/>
+      <c r="N1182" s="22"/>
+    </row>
+    <row r="1183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1183" s="22" t="s">
-        <v>1213</v>
+        <v>27</v>
       </c>
       <c r="C1183" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1183" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1183" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1183" s="22" t="s">
-        <v>714</v>
-      </c>
+      <c r="D1183" s="22"/>
+      <c r="E1183" s="22"/>
+      <c r="F1183" s="26"/>
       <c r="G1183" s="22"/>
       <c r="H1183" s="22"/>
       <c r="I1183" s="23" t="s">
@@ -31175,236 +32200,160 @@
       </c>
       <c r="J1183" s="23"/>
       <c r="K1183" s="23"/>
-    </row>
-    <row r="1184" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1184" s="21"/>
-      <c r="B1184" s="28" t="s">
-        <v>1216</v>
-      </c>
-      <c r="C1184" s="26"/>
-      <c r="D1184" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1184" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1184" s="22" t="s">
-        <v>714</v>
-      </c>
+      <c r="L1183" s="22"/>
+      <c r="M1183" s="22"/>
+      <c r="N1183" s="22"/>
+    </row>
+    <row r="1184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1184" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1184" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1184" s="22"/>
+      <c r="E1184" s="22"/>
+      <c r="F1184" s="26"/>
       <c r="G1184" s="22"/>
       <c r="H1184" s="22"/>
       <c r="I1184" s="23" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="J1184" s="23"/>
-      <c r="K1184" s="23" t="s">
-        <v>1218</v>
-      </c>
-    </row>
-    <row r="1185" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1185" s="21"/>
+      <c r="K1184" s="23"/>
+      <c r="L1184" s="22"/>
+      <c r="M1184" s="22"/>
+      <c r="N1184" s="22"/>
+    </row>
+    <row r="1185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1185" s="22" t="s">
-        <v>1213</v>
+        <v>27</v>
       </c>
       <c r="C1185" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1185" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1185" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1185" s="22" t="s">
-        <v>714</v>
-      </c>
+      <c r="D1185" s="22"/>
+      <c r="E1185" s="22"/>
+      <c r="F1185" s="26"/>
       <c r="G1185" s="22"/>
       <c r="H1185" s="22"/>
       <c r="I1185" s="23" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="J1185" s="23"/>
       <c r="K1185" s="23"/>
+      <c r="L1185" s="22"/>
+      <c r="M1185" s="22"/>
+      <c r="N1185" s="22"/>
     </row>
     <row r="1186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1186" s="21"/>
-      <c r="B1186" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1186" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1186" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1186" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1186" s="22" t="s">
-        <v>714</v>
-      </c>
+      <c r="B1186" s="22"/>
+      <c r="C1186" s="22"/>
+      <c r="D1186" s="22"/>
+      <c r="E1186" s="22"/>
+      <c r="F1186" s="22"/>
       <c r="G1186" s="22"/>
       <c r="H1186" s="22"/>
-      <c r="I1186" s="23" t="s">
-        <v>1220</v>
-      </c>
+      <c r="I1186" s="23"/>
       <c r="J1186" s="23"/>
       <c r="K1186" s="23"/>
+      <c r="L1186" s="22"/>
+      <c r="M1186" s="22"/>
+      <c r="N1186" s="22"/>
     </row>
     <row r="1187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1187" s="9"/>
-      <c r="B1187" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1187" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1187" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1187" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1187" s="22" t="s">
-        <v>714</v>
-      </c>
-      <c r="G1187" s="22"/>
-      <c r="H1187" s="22"/>
-      <c r="I1187" s="23" t="s">
-        <v>1221</v>
-      </c>
-      <c r="J1187" s="23"/>
-      <c r="K1187" s="23"/>
+      <c r="B1187" s="48"/>
+      <c r="C1187" s="1"/>
+      <c r="D1187" s="1"/>
+      <c r="E1187" s="1"/>
+      <c r="F1187" s="1"/>
+      <c r="G1187" s="1"/>
+      <c r="H1187" s="1"/>
+      <c r="I1187" s="1"/>
+      <c r="J1187" s="1"/>
+      <c r="K1187" s="1"/>
+      <c r="L1187" s="1"/>
+      <c r="M1187" s="1"/>
+      <c r="N1187" s="1"/>
     </row>
     <row r="1188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1188" s="9"/>
-      <c r="B1188" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1188" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1188" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1188" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1188" s="22" t="s">
-        <v>714</v>
-      </c>
-      <c r="G1188" s="22"/>
-      <c r="H1188" s="22"/>
-      <c r="I1188" s="47" t="s">
-        <v>1222</v>
-      </c>
-      <c r="J1188" s="23"/>
-      <c r="K1188" s="23"/>
     </row>
     <row r="1189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1189" s="9"/>
-      <c r="B1189" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1189" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1189" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1189" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1189" s="22" t="s">
-        <v>714</v>
-      </c>
-      <c r="G1189" s="22"/>
-      <c r="H1189" s="22"/>
-      <c r="I1189" s="47" t="s">
-        <v>1223</v>
-      </c>
-      <c r="J1189" s="23"/>
-      <c r="K1189" s="23"/>
+      <c r="A1189" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1189" s="17"/>
+      <c r="C1189" s="18"/>
+      <c r="D1189" s="18"/>
+      <c r="E1189" s="18"/>
+      <c r="F1189" s="18"/>
+      <c r="G1189" s="18"/>
+      <c r="H1189" s="18"/>
     </row>
     <row r="1190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1190" s="9"/>
-      <c r="B1190" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1190" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1190" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1190" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1190" s="22" t="s">
-        <v>714</v>
-      </c>
-      <c r="G1190" s="22"/>
-      <c r="H1190" s="22"/>
-      <c r="I1190" s="47" t="s">
-        <v>1224</v>
-      </c>
-      <c r="J1190" s="23"/>
-      <c r="K1190" s="23"/>
+      <c r="A1190" s="16" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1190" s="17"/>
+      <c r="C1190" s="18"/>
+      <c r="D1190" s="18"/>
+      <c r="E1190" s="18"/>
+      <c r="F1190" s="18"/>
+      <c r="G1190" s="18"/>
+      <c r="H1190" s="18"/>
     </row>
     <row r="1191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1191" s="9"/>
-      <c r="B1191" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1191" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1191" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1191" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1191" s="22" t="s">
-        <v>714</v>
-      </c>
-      <c r="G1191" s="22"/>
-      <c r="H1191" s="22"/>
-      <c r="I1191" s="47" t="s">
-        <v>1225</v>
-      </c>
-      <c r="J1191" s="23"/>
-      <c r="K1191" s="23"/>
-    </row>
-    <row r="1192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1191" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1191" s="17"/>
+      <c r="C1191" s="18"/>
+      <c r="D1191" s="18"/>
+      <c r="E1191" s="18"/>
+      <c r="F1191" s="18"/>
+      <c r="G1191" s="18"/>
+      <c r="H1191" s="18"/>
+    </row>
+    <row r="1192" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1192" s="9"/>
-      <c r="B1192" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1192" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1192" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1192" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1192" s="22" t="s">
-        <v>714</v>
-      </c>
-      <c r="G1192" s="22"/>
-      <c r="H1192" s="22"/>
-      <c r="I1192" s="47" t="s">
-        <v>1226</v>
-      </c>
-      <c r="J1192" s="23"/>
-      <c r="K1192" s="23"/>
-    </row>
-    <row r="1193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1193" s="9"/>
+      <c r="B1192" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1192" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1192" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1192" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1192" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1192" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1192" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1192" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1192" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1192" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1193" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1193" s="21" t="s">
+        <v>1219</v>
+      </c>
       <c r="B1193" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1193" s="22" t="s">
         <v>27</v>
@@ -31421,15 +32370,15 @@
       <c r="G1193" s="22"/>
       <c r="H1193" s="22"/>
       <c r="I1193" s="23" t="s">
-        <v>1227</v>
+        <v>1221</v>
       </c>
       <c r="J1193" s="23"/>
       <c r="K1193" s="23"/>
     </row>
     <row r="1194" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1194" s="9"/>
+      <c r="A1194" s="21"/>
       <c r="B1194" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1194" s="22" t="s">
         <v>27</v>
@@ -31446,19 +32395,17 @@
       <c r="G1194" s="22"/>
       <c r="H1194" s="22"/>
       <c r="I1194" s="23" t="s">
-        <v>1228</v>
+        <v>1222</v>
       </c>
       <c r="J1194" s="23"/>
       <c r="K1194" s="23"/>
     </row>
-    <row r="1195" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1195" s="9"/>
-      <c r="B1195" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1195" s="22" t="s">
-        <v>27</v>
-      </c>
+    <row r="1195" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1195" s="21"/>
+      <c r="B1195" s="28" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C1195" s="26"/>
       <c r="D1195" s="22" t="s">
         <v>27</v>
       </c>
@@ -31471,15 +32418,17 @@
       <c r="G1195" s="22"/>
       <c r="H1195" s="22"/>
       <c r="I1195" s="23" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="J1195" s="23"/>
-      <c r="K1195" s="23"/>
+      <c r="K1195" s="23" t="s">
+        <v>1225</v>
+      </c>
     </row>
     <row r="1196" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1196" s="9"/>
+      <c r="A1196" s="21"/>
       <c r="B1196" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1196" s="22" t="s">
         <v>27</v>
@@ -31496,15 +32445,15 @@
       <c r="G1196" s="22"/>
       <c r="H1196" s="22"/>
       <c r="I1196" s="23" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="J1196" s="23"/>
       <c r="K1196" s="23"/>
     </row>
-    <row r="1197" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1197" s="9"/>
+    <row r="1197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1197" s="21"/>
       <c r="B1197" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1197" s="22" t="s">
         <v>27</v>
@@ -31521,20 +32470,22 @@
       <c r="G1197" s="22"/>
       <c r="H1197" s="22"/>
       <c r="I1197" s="23" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="J1197" s="23"/>
       <c r="K1197" s="23"/>
     </row>
-    <row r="1198" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1198" s="9"/>
       <c r="B1198" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1198" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1198" s="22"/>
+      <c r="D1198" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="E1198" s="22" t="s">
         <v>27</v>
       </c>
@@ -31544,15 +32495,15 @@
       <c r="G1198" s="22"/>
       <c r="H1198" s="22"/>
       <c r="I1198" s="23" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="J1198" s="23"/>
       <c r="K1198" s="23"/>
     </row>
-    <row r="1199" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1199" s="9"/>
       <c r="B1199" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1199" s="22" t="s">
         <v>27</v>
@@ -31568,8 +32519,8 @@
       </c>
       <c r="G1199" s="22"/>
       <c r="H1199" s="22"/>
-      <c r="I1199" s="23" t="s">
-        <v>1233</v>
+      <c r="I1199" s="47" t="s">
+        <v>1229</v>
       </c>
       <c r="J1199" s="23"/>
       <c r="K1199" s="23"/>
@@ -31577,7 +32528,7 @@
     <row r="1200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1200" s="9"/>
       <c r="B1200" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1200" s="22" t="s">
         <v>27</v>
@@ -31589,22 +32540,20 @@
         <v>27</v>
       </c>
       <c r="F1200" s="22" t="s">
-        <v>1234</v>
+        <v>714</v>
       </c>
       <c r="G1200" s="22"/>
       <c r="H1200" s="22"/>
-      <c r="I1200" s="23" t="s">
-        <v>1235</v>
+      <c r="I1200" s="47" t="s">
+        <v>1230</v>
       </c>
       <c r="J1200" s="23"/>
-      <c r="K1200" s="23" t="s">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="1201" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1200" s="23"/>
+    </row>
+    <row r="1201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1201" s="9"/>
       <c r="B1201" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1201" s="22" t="s">
         <v>27</v>
@@ -31616,22 +32565,20 @@
         <v>27</v>
       </c>
       <c r="F1201" s="22" t="s">
-        <v>1234</v>
+        <v>714</v>
       </c>
       <c r="G1201" s="22"/>
       <c r="H1201" s="22"/>
-      <c r="I1201" s="23" t="s">
-        <v>1237</v>
+      <c r="I1201" s="47" t="s">
+        <v>1231</v>
       </c>
       <c r="J1201" s="23"/>
-      <c r="K1201" s="23" t="s">
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="1202" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1201" s="23"/>
+    </row>
+    <row r="1202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1202" s="9"/>
       <c r="B1202" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1202" s="22" t="s">
         <v>27</v>
@@ -31647,16 +32594,16 @@
       </c>
       <c r="G1202" s="22"/>
       <c r="H1202" s="22"/>
-      <c r="I1202" s="23" t="s">
-        <v>1239</v>
+      <c r="I1202" s="47" t="s">
+        <v>1232</v>
       </c>
       <c r="J1202" s="23"/>
       <c r="K1202" s="23"/>
     </row>
-    <row r="1203" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1203" s="9"/>
       <c r="B1203" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1203" s="22" t="s">
         <v>27</v>
@@ -31672,16 +32619,16 @@
       </c>
       <c r="G1203" s="22"/>
       <c r="H1203" s="22"/>
-      <c r="I1203" s="23" t="s">
-        <v>1240</v>
+      <c r="I1203" s="47" t="s">
+        <v>1233</v>
       </c>
       <c r="J1203" s="23"/>
       <c r="K1203" s="23"/>
     </row>
-    <row r="1204" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1204" s="9"/>
       <c r="B1204" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1204" s="22" t="s">
         <v>27</v>
@@ -31698,17 +32645,19 @@
       <c r="G1204" s="22"/>
       <c r="H1204" s="22"/>
       <c r="I1204" s="23" t="s">
-        <v>1241</v>
+        <v>1234</v>
       </c>
       <c r="J1204" s="23"/>
       <c r="K1204" s="23"/>
     </row>
-    <row r="1205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1205" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1205" s="9"/>
       <c r="B1205" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1205" s="26"/>
+        <v>1220</v>
+      </c>
+      <c r="C1205" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1205" s="22" t="s">
         <v>27</v>
       </c>
@@ -31721,7 +32670,7 @@
       <c r="G1205" s="22"/>
       <c r="H1205" s="22"/>
       <c r="I1205" s="23" t="s">
-        <v>1242</v>
+        <v>1235</v>
       </c>
       <c r="J1205" s="23"/>
       <c r="K1205" s="23"/>
@@ -31729,7 +32678,7 @@
     <row r="1206" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1206" s="9"/>
       <c r="B1206" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1206" s="22" t="s">
         <v>27</v>
@@ -31746,7 +32695,7 @@
       <c r="G1206" s="22"/>
       <c r="H1206" s="22"/>
       <c r="I1206" s="23" t="s">
-        <v>1243</v>
+        <v>1236</v>
       </c>
       <c r="J1206" s="23"/>
       <c r="K1206" s="23"/>
@@ -31754,7 +32703,7 @@
     <row r="1207" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1207" s="9"/>
       <c r="B1207" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1207" s="22" t="s">
         <v>27</v>
@@ -31771,17 +32720,15 @@
       <c r="G1207" s="22"/>
       <c r="H1207" s="22"/>
       <c r="I1207" s="23" t="s">
-        <v>1244</v>
+        <v>1237</v>
       </c>
       <c r="J1207" s="23"/>
-      <c r="K1207" s="23" t="s">
-        <v>303</v>
-      </c>
+      <c r="K1207" s="23"/>
     </row>
     <row r="1208" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1208" s="9"/>
       <c r="B1208" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1208" s="22" t="s">
         <v>27</v>
@@ -31798,7 +32745,7 @@
       <c r="G1208" s="22"/>
       <c r="H1208" s="22"/>
       <c r="I1208" s="23" t="s">
-        <v>1245</v>
+        <v>1238</v>
       </c>
       <c r="J1208" s="23"/>
       <c r="K1208" s="23"/>
@@ -31806,14 +32753,12 @@
     <row r="1209" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1209" s="9"/>
       <c r="B1209" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1209" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1209" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="D1209" s="22"/>
       <c r="E1209" s="22" t="s">
         <v>27</v>
       </c>
@@ -31823,7 +32768,7 @@
       <c r="G1209" s="22"/>
       <c r="H1209" s="22"/>
       <c r="I1209" s="23" t="s">
-        <v>1246</v>
+        <v>1239</v>
       </c>
       <c r="J1209" s="23"/>
       <c r="K1209" s="23"/>
@@ -31831,7 +32776,7 @@
     <row r="1210" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1210" s="9"/>
       <c r="B1210" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1210" s="22" t="s">
         <v>27</v>
@@ -31848,7 +32793,7 @@
       <c r="G1210" s="22"/>
       <c r="H1210" s="22"/>
       <c r="I1210" s="23" t="s">
-        <v>1247</v>
+        <v>1240</v>
       </c>
       <c r="J1210" s="23"/>
       <c r="K1210" s="23"/>
@@ -31856,7 +32801,7 @@
     <row r="1211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1211" s="9"/>
       <c r="B1211" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1211" s="22" t="s">
         <v>27</v>
@@ -31868,20 +32813,22 @@
         <v>27</v>
       </c>
       <c r="F1211" s="22" t="s">
-        <v>714</v>
+        <v>1241</v>
       </c>
       <c r="G1211" s="22"/>
       <c r="H1211" s="22"/>
       <c r="I1211" s="23" t="s">
-        <v>1248</v>
+        <v>1242</v>
       </c>
       <c r="J1211" s="23"/>
-      <c r="K1211" s="23"/>
-    </row>
-    <row r="1212" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1211" s="23" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="1212" customFormat="false" ht="42.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1212" s="9"/>
       <c r="B1212" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1212" s="22" t="s">
         <v>27</v>
@@ -31893,20 +32840,22 @@
         <v>27</v>
       </c>
       <c r="F1212" s="22" t="s">
-        <v>714</v>
+        <v>1241</v>
       </c>
       <c r="G1212" s="22"/>
       <c r="H1212" s="22"/>
       <c r="I1212" s="23" t="s">
-        <v>1249</v>
+        <v>1244</v>
       </c>
       <c r="J1212" s="23"/>
-      <c r="K1212" s="23"/>
+      <c r="K1212" s="23" t="s">
+        <v>1245</v>
+      </c>
     </row>
     <row r="1213" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1213" s="9"/>
       <c r="B1213" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1213" s="22" t="s">
         <v>27</v>
@@ -31923,7 +32872,7 @@
       <c r="G1213" s="22"/>
       <c r="H1213" s="22"/>
       <c r="I1213" s="23" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
       <c r="J1213" s="23"/>
       <c r="K1213" s="23"/>
@@ -31931,7 +32880,7 @@
     <row r="1214" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1214" s="9"/>
       <c r="B1214" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1214" s="22" t="s">
         <v>27</v>
@@ -31948,7 +32897,7 @@
       <c r="G1214" s="22"/>
       <c r="H1214" s="22"/>
       <c r="I1214" s="23" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="J1214" s="23"/>
       <c r="K1214" s="23"/>
@@ -31956,7 +32905,7 @@
     <row r="1215" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1215" s="9"/>
       <c r="B1215" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1215" s="22" t="s">
         <v>27</v>
@@ -31973,19 +32922,17 @@
       <c r="G1215" s="22"/>
       <c r="H1215" s="22"/>
       <c r="I1215" s="23" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="J1215" s="23"/>
       <c r="K1215" s="23"/>
     </row>
-    <row r="1216" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1216" s="9"/>
       <c r="B1216" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1216" s="22" t="s">
-        <v>27</v>
-      </c>
+        <v>1220</v>
+      </c>
+      <c r="C1216" s="26"/>
       <c r="D1216" s="22" t="s">
         <v>27</v>
       </c>
@@ -31998,15 +32945,15 @@
       <c r="G1216" s="22"/>
       <c r="H1216" s="22"/>
       <c r="I1216" s="23" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="J1216" s="23"/>
       <c r="K1216" s="23"/>
     </row>
-    <row r="1217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1217" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1217" s="9"/>
       <c r="B1217" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1217" s="22" t="s">
         <v>27</v>
@@ -32023,15 +32970,15 @@
       <c r="G1217" s="22"/>
       <c r="H1217" s="22"/>
       <c r="I1217" s="23" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="J1217" s="23"/>
       <c r="K1217" s="23"/>
     </row>
-    <row r="1218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1218" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1218" s="9"/>
       <c r="B1218" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1218" s="22" t="s">
         <v>27</v>
@@ -32048,15 +32995,17 @@
       <c r="G1218" s="22"/>
       <c r="H1218" s="22"/>
       <c r="I1218" s="23" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="J1218" s="23"/>
-      <c r="K1218" s="23"/>
-    </row>
-    <row r="1219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1218" s="23" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="1219" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1219" s="9"/>
       <c r="B1219" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1219" s="22" t="s">
         <v>27</v>
@@ -32073,7 +33022,7 @@
       <c r="G1219" s="22"/>
       <c r="H1219" s="22"/>
       <c r="I1219" s="23" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="J1219" s="23"/>
       <c r="K1219" s="23"/>
@@ -32081,7 +33030,7 @@
     <row r="1220" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1220" s="9"/>
       <c r="B1220" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1220" s="22" t="s">
         <v>27</v>
@@ -32098,7 +33047,7 @@
       <c r="G1220" s="22"/>
       <c r="H1220" s="22"/>
       <c r="I1220" s="23" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="J1220" s="23"/>
       <c r="K1220" s="23"/>
@@ -32106,7 +33055,7 @@
     <row r="1221" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1221" s="9"/>
       <c r="B1221" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1221" s="22" t="s">
         <v>27</v>
@@ -32123,15 +33072,15 @@
       <c r="G1221" s="22"/>
       <c r="H1221" s="22"/>
       <c r="I1221" s="23" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="J1221" s="23"/>
       <c r="K1221" s="23"/>
     </row>
-    <row r="1222" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1222" s="9"/>
       <c r="B1222" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1222" s="22" t="s">
         <v>27</v>
@@ -32148,7 +33097,7 @@
       <c r="G1222" s="22"/>
       <c r="H1222" s="22"/>
       <c r="I1222" s="23" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="J1222" s="23"/>
       <c r="K1222" s="23"/>
@@ -32156,7 +33105,7 @@
     <row r="1223" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1223" s="9"/>
       <c r="B1223" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1223" s="22" t="s">
         <v>27</v>
@@ -32173,15 +33122,15 @@
       <c r="G1223" s="22"/>
       <c r="H1223" s="22"/>
       <c r="I1223" s="23" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="J1223" s="23"/>
       <c r="K1223" s="23"/>
     </row>
-    <row r="1224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1224" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1224" s="9"/>
       <c r="B1224" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1224" s="22" t="s">
         <v>27</v>
@@ -32198,15 +33147,15 @@
       <c r="G1224" s="22"/>
       <c r="H1224" s="22"/>
       <c r="I1224" s="23" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="J1224" s="23"/>
       <c r="K1224" s="23"/>
     </row>
-    <row r="1225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1225" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1225" s="9"/>
       <c r="B1225" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1225" s="22" t="s">
         <v>27</v>
@@ -32223,7 +33172,7 @@
       <c r="G1225" s="22"/>
       <c r="H1225" s="22"/>
       <c r="I1225" s="23" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="J1225" s="23"/>
       <c r="K1225" s="23"/>
@@ -32231,7 +33180,7 @@
     <row r="1226" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1226" s="9"/>
       <c r="B1226" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1226" s="22" t="s">
         <v>27</v>
@@ -32248,7 +33197,7 @@
       <c r="G1226" s="22"/>
       <c r="H1226" s="22"/>
       <c r="I1226" s="23" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
       <c r="J1226" s="23"/>
       <c r="K1226" s="23"/>
@@ -32256,7 +33205,7 @@
     <row r="1227" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1227" s="9"/>
       <c r="B1227" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1227" s="22" t="s">
         <v>27</v>
@@ -32273,15 +33222,15 @@
       <c r="G1227" s="22"/>
       <c r="H1227" s="22"/>
       <c r="I1227" s="23" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="J1227" s="23"/>
       <c r="K1227" s="23"/>
     </row>
-    <row r="1228" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1228" s="9"/>
       <c r="B1228" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1228" s="22" t="s">
         <v>27</v>
@@ -32298,15 +33247,15 @@
       <c r="G1228" s="22"/>
       <c r="H1228" s="22"/>
       <c r="I1228" s="23" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="J1228" s="23"/>
       <c r="K1228" s="23"/>
     </row>
-    <row r="1229" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1229" s="9"/>
       <c r="B1229" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1229" s="22" t="s">
         <v>27</v>
@@ -32323,15 +33272,15 @@
       <c r="G1229" s="22"/>
       <c r="H1229" s="22"/>
       <c r="I1229" s="23" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
       <c r="J1229" s="23"/>
       <c r="K1229" s="23"/>
     </row>
-    <row r="1230" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1230" s="9"/>
       <c r="B1230" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1230" s="22" t="s">
         <v>27</v>
@@ -32348,7 +33297,7 @@
       <c r="G1230" s="22"/>
       <c r="H1230" s="22"/>
       <c r="I1230" s="23" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
       <c r="J1230" s="23"/>
       <c r="K1230" s="23"/>
@@ -32356,7 +33305,7 @@
     <row r="1231" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1231" s="9"/>
       <c r="B1231" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1231" s="22" t="s">
         <v>27</v>
@@ -32373,15 +33322,15 @@
       <c r="G1231" s="22"/>
       <c r="H1231" s="22"/>
       <c r="I1231" s="23" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="J1231" s="23"/>
       <c r="K1231" s="23"/>
     </row>
-    <row r="1232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1232" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1232" s="9"/>
       <c r="B1232" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1232" s="22" t="s">
         <v>27</v>
@@ -32398,15 +33347,15 @@
       <c r="G1232" s="22"/>
       <c r="H1232" s="22"/>
       <c r="I1232" s="23" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="J1232" s="23"/>
       <c r="K1232" s="23"/>
     </row>
-    <row r="1233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1233" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1233" s="9"/>
       <c r="B1233" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1233" s="22" t="s">
         <v>27</v>
@@ -32423,7 +33372,7 @@
       <c r="G1233" s="22"/>
       <c r="H1233" s="22"/>
       <c r="I1233" s="23" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="J1233" s="23"/>
       <c r="K1233" s="23"/>
@@ -32431,7 +33380,7 @@
     <row r="1234" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1234" s="9"/>
       <c r="B1234" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1234" s="22" t="s">
         <v>27</v>
@@ -32448,15 +33397,15 @@
       <c r="G1234" s="22"/>
       <c r="H1234" s="22"/>
       <c r="I1234" s="23" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="J1234" s="23"/>
       <c r="K1234" s="23"/>
     </row>
-    <row r="1235" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1235" s="9"/>
       <c r="B1235" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1235" s="22" t="s">
         <v>27</v>
@@ -32473,7 +33422,7 @@
       <c r="G1235" s="22"/>
       <c r="H1235" s="22"/>
       <c r="I1235" s="23" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="J1235" s="23"/>
       <c r="K1235" s="23"/>
@@ -32481,7 +33430,7 @@
     <row r="1236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1236" s="9"/>
       <c r="B1236" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1236" s="22" t="s">
         <v>27</v>
@@ -32498,15 +33447,15 @@
       <c r="G1236" s="22"/>
       <c r="H1236" s="22"/>
       <c r="I1236" s="23" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="J1236" s="23"/>
       <c r="K1236" s="23"/>
     </row>
-    <row r="1237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1237" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1237" s="9"/>
       <c r="B1237" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1237" s="22" t="s">
         <v>27</v>
@@ -32523,15 +33472,15 @@
       <c r="G1237" s="22"/>
       <c r="H1237" s="22"/>
       <c r="I1237" s="23" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="J1237" s="23"/>
       <c r="K1237" s="23"/>
     </row>
-    <row r="1238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1238" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1238" s="9"/>
       <c r="B1238" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1238" s="22" t="s">
         <v>27</v>
@@ -32548,7 +33497,7 @@
       <c r="G1238" s="22"/>
       <c r="H1238" s="22"/>
       <c r="I1238" s="23" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="J1238" s="23"/>
       <c r="K1238" s="23"/>
@@ -32556,7 +33505,7 @@
     <row r="1239" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1239" s="9"/>
       <c r="B1239" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1239" s="22" t="s">
         <v>27</v>
@@ -32573,7 +33522,7 @@
       <c r="G1239" s="22"/>
       <c r="H1239" s="22"/>
       <c r="I1239" s="23" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="J1239" s="23"/>
       <c r="K1239" s="23"/>
@@ -32581,7 +33530,7 @@
     <row r="1240" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1240" s="9"/>
       <c r="B1240" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1240" s="22" t="s">
         <v>27</v>
@@ -32598,15 +33547,15 @@
       <c r="G1240" s="22"/>
       <c r="H1240" s="22"/>
       <c r="I1240" s="23" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="J1240" s="23"/>
       <c r="K1240" s="23"/>
     </row>
-    <row r="1241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1241" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1241" s="9"/>
       <c r="B1241" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1241" s="22" t="s">
         <v>27</v>
@@ -32623,15 +33572,15 @@
       <c r="G1241" s="22"/>
       <c r="H1241" s="22"/>
       <c r="I1241" s="23" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="J1241" s="23"/>
       <c r="K1241" s="23"/>
     </row>
-    <row r="1242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1242" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1242" s="9"/>
       <c r="B1242" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1242" s="22" t="s">
         <v>27</v>
@@ -32648,7 +33597,7 @@
       <c r="G1242" s="22"/>
       <c r="H1242" s="22"/>
       <c r="I1242" s="23" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="J1242" s="23"/>
       <c r="K1242" s="23"/>
@@ -32656,7 +33605,7 @@
     <row r="1243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1243" s="9"/>
       <c r="B1243" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1243" s="22" t="s">
         <v>27</v>
@@ -32673,7 +33622,7 @@
       <c r="G1243" s="22"/>
       <c r="H1243" s="22"/>
       <c r="I1243" s="23" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="J1243" s="23"/>
       <c r="K1243" s="23"/>
@@ -32681,7 +33630,7 @@
     <row r="1244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1244" s="9"/>
       <c r="B1244" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1244" s="22" t="s">
         <v>27</v>
@@ -32698,15 +33647,15 @@
       <c r="G1244" s="22"/>
       <c r="H1244" s="22"/>
       <c r="I1244" s="23" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="J1244" s="23"/>
       <c r="K1244" s="23"/>
     </row>
-    <row r="1245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1245" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1245" s="9"/>
       <c r="B1245" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1245" s="22" t="s">
         <v>27</v>
@@ -32723,15 +33672,15 @@
       <c r="G1245" s="22"/>
       <c r="H1245" s="22"/>
       <c r="I1245" s="23" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="J1245" s="23"/>
       <c r="K1245" s="23"/>
     </row>
-    <row r="1246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1246" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1246" s="9"/>
       <c r="B1246" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1246" s="22" t="s">
         <v>27</v>
@@ -32748,15 +33697,15 @@
       <c r="G1246" s="22"/>
       <c r="H1246" s="22"/>
       <c r="I1246" s="23" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="J1246" s="23"/>
       <c r="K1246" s="23"/>
     </row>
-    <row r="1247" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1247" s="9"/>
       <c r="B1247" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1247" s="22" t="s">
         <v>27</v>
@@ -32773,7 +33722,7 @@
       <c r="G1247" s="22"/>
       <c r="H1247" s="22"/>
       <c r="I1247" s="23" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="J1247" s="23"/>
       <c r="K1247" s="23"/>
@@ -32781,7 +33730,7 @@
     <row r="1248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1248" s="9"/>
       <c r="B1248" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1248" s="22" t="s">
         <v>27</v>
@@ -32798,7 +33747,7 @@
       <c r="G1248" s="22"/>
       <c r="H1248" s="22"/>
       <c r="I1248" s="23" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="J1248" s="23"/>
       <c r="K1248" s="23"/>
@@ -32806,7 +33755,7 @@
     <row r="1249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1249" s="9"/>
       <c r="B1249" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1249" s="22" t="s">
         <v>27</v>
@@ -32823,15 +33772,15 @@
       <c r="G1249" s="22"/>
       <c r="H1249" s="22"/>
       <c r="I1249" s="23" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="J1249" s="23"/>
       <c r="K1249" s="23"/>
     </row>
-    <row r="1250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1250" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1250" s="9"/>
       <c r="B1250" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1250" s="22" t="s">
         <v>27</v>
@@ -32848,15 +33797,15 @@
       <c r="G1250" s="22"/>
       <c r="H1250" s="22"/>
       <c r="I1250" s="23" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="J1250" s="23"/>
       <c r="K1250" s="23"/>
     </row>
-    <row r="1251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1251" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1251" s="9"/>
       <c r="B1251" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1251" s="22" t="s">
         <v>27</v>
@@ -32873,38 +33822,40 @@
       <c r="G1251" s="22"/>
       <c r="H1251" s="22"/>
       <c r="I1251" s="23" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="J1251" s="23"/>
       <c r="K1251" s="23"/>
     </row>
     <row r="1252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1252" s="9"/>
-      <c r="B1252" s="28" t="s">
-        <v>1216</v>
-      </c>
-      <c r="C1252" s="26"/>
+      <c r="B1252" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1252" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D1252" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1252" s="26"/>
+      <c r="E1252" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="F1252" s="22" t="s">
         <v>714</v>
       </c>
       <c r="G1252" s="22"/>
       <c r="H1252" s="22"/>
       <c r="I1252" s="23" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="J1252" s="23"/>
-      <c r="K1252" s="23" t="s">
-        <v>686</v>
-      </c>
+      <c r="K1252" s="23"/>
     </row>
     <row r="1253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1253" s="9"/>
       <c r="B1253" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1253" s="22" t="s">
         <v>27</v>
@@ -32921,7 +33872,7 @@
       <c r="G1253" s="22"/>
       <c r="H1253" s="22"/>
       <c r="I1253" s="23" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="J1253" s="23"/>
       <c r="K1253" s="23"/>
@@ -32929,7 +33880,7 @@
     <row r="1254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1254" s="9"/>
       <c r="B1254" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1254" s="22" t="s">
         <v>27</v>
@@ -32946,7 +33897,7 @@
       <c r="G1254" s="22"/>
       <c r="H1254" s="22"/>
       <c r="I1254" s="23" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="J1254" s="23"/>
       <c r="K1254" s="23"/>
@@ -32954,7 +33905,7 @@
     <row r="1255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1255" s="9"/>
       <c r="B1255" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1255" s="22" t="s">
         <v>27</v>
@@ -32971,7 +33922,7 @@
       <c r="G1255" s="22"/>
       <c r="H1255" s="22"/>
       <c r="I1255" s="23" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="J1255" s="23"/>
       <c r="K1255" s="23"/>
@@ -32979,7 +33930,7 @@
     <row r="1256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1256" s="9"/>
       <c r="B1256" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1256" s="22" t="s">
         <v>27</v>
@@ -32996,15 +33947,15 @@
       <c r="G1256" s="22"/>
       <c r="H1256" s="22"/>
       <c r="I1256" s="23" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="J1256" s="23"/>
       <c r="K1256" s="23"/>
     </row>
-    <row r="1257" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1257" s="9"/>
       <c r="B1257" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1257" s="22" t="s">
         <v>27</v>
@@ -33021,15 +33972,15 @@
       <c r="G1257" s="22"/>
       <c r="H1257" s="22"/>
       <c r="I1257" s="23" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="J1257" s="23"/>
       <c r="K1257" s="23"/>
     </row>
-    <row r="1258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1258" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1258" s="9"/>
       <c r="B1258" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1258" s="22" t="s">
         <v>27</v>
@@ -33046,7 +33997,7 @@
       <c r="G1258" s="22"/>
       <c r="H1258" s="22"/>
       <c r="I1258" s="23" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="J1258" s="23"/>
       <c r="K1258" s="23"/>
@@ -33054,7 +34005,7 @@
     <row r="1259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1259" s="9"/>
       <c r="B1259" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1259" s="22" t="s">
         <v>27</v>
@@ -33071,14 +34022,15 @@
       <c r="G1259" s="22"/>
       <c r="H1259" s="22"/>
       <c r="I1259" s="23" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="J1259" s="23"/>
       <c r="K1259" s="23"/>
     </row>
     <row r="1260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1260" s="9"/>
       <c r="B1260" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1260" s="22" t="s">
         <v>27</v>
@@ -33095,14 +34047,15 @@
       <c r="G1260" s="22"/>
       <c r="H1260" s="22"/>
       <c r="I1260" s="23" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="J1260" s="23"/>
       <c r="K1260" s="23"/>
     </row>
-    <row r="1261" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1261" s="9"/>
       <c r="B1261" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1261" s="22" t="s">
         <v>27</v>
@@ -33119,14 +34072,15 @@
       <c r="G1261" s="22"/>
       <c r="H1261" s="22"/>
       <c r="I1261" s="23" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="J1261" s="23"/>
       <c r="K1261" s="23"/>
     </row>
-    <row r="1262" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1262" s="9"/>
       <c r="B1262" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1262" s="22" t="s">
         <v>27</v>
@@ -33143,38 +34097,38 @@
       <c r="G1262" s="22"/>
       <c r="H1262" s="22"/>
       <c r="I1262" s="23" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="J1262" s="23"/>
       <c r="K1262" s="23"/>
     </row>
-    <row r="1263" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1263" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1263" s="22" t="s">
-        <v>27</v>
-      </c>
+    <row r="1263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1263" s="9"/>
+      <c r="B1263" s="28" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C1263" s="26"/>
       <c r="D1263" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1263" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="E1263" s="26"/>
       <c r="F1263" s="22" t="s">
         <v>714</v>
       </c>
       <c r="G1263" s="22"/>
       <c r="H1263" s="22"/>
       <c r="I1263" s="23" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="J1263" s="23"/>
-      <c r="K1263" s="23"/>
+      <c r="K1263" s="23" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="1264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1264" s="9"/>
       <c r="B1264" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1264" s="22" t="s">
         <v>27</v>
@@ -33191,14 +34145,15 @@
       <c r="G1264" s="22"/>
       <c r="H1264" s="22"/>
       <c r="I1264" s="23" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="J1264" s="23"/>
       <c r="K1264" s="23"/>
     </row>
-    <row r="1265" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1265" s="9"/>
       <c r="B1265" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1265" s="22" t="s">
         <v>27</v>
@@ -33215,14 +34170,15 @@
       <c r="G1265" s="22"/>
       <c r="H1265" s="22"/>
       <c r="I1265" s="23" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="J1265" s="23"/>
       <c r="K1265" s="23"/>
     </row>
-    <row r="1266" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1266" s="9"/>
       <c r="B1266" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1266" s="22" t="s">
         <v>27</v>
@@ -33239,14 +34195,15 @@
       <c r="G1266" s="22"/>
       <c r="H1266" s="22"/>
       <c r="I1266" s="23" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="J1266" s="23"/>
       <c r="K1266" s="23"/>
     </row>
-    <row r="1267" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1267" s="9"/>
       <c r="B1267" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1267" s="22" t="s">
         <v>27</v>
@@ -33263,14 +34220,15 @@
       <c r="G1267" s="22"/>
       <c r="H1267" s="22"/>
       <c r="I1267" s="23" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="J1267" s="23"/>
       <c r="K1267" s="23"/>
     </row>
-    <row r="1268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1268" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1268" s="9"/>
       <c r="B1268" s="22" t="s">
-        <v>1213</v>
+        <v>1220</v>
       </c>
       <c r="C1268" s="22" t="s">
         <v>27</v>
@@ -33287,81 +34245,354 @@
       <c r="G1268" s="22"/>
       <c r="H1268" s="22"/>
       <c r="I1268" s="23" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="J1268" s="23"/>
       <c r="K1268" s="23"/>
     </row>
     <row r="1269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1269" s="28" t="s">
+      <c r="A1269" s="9"/>
+      <c r="B1269" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1269" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1269" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1269" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1269" s="22" t="s">
         <v>714</v>
       </c>
-      <c r="C1269" s="28"/>
-      <c r="D1269" s="28" t="s">
+      <c r="G1269" s="22"/>
+      <c r="H1269" s="22"/>
+      <c r="I1269" s="23" t="s">
+        <v>1302</v>
+      </c>
+      <c r="J1269" s="23"/>
+      <c r="K1269" s="23"/>
+    </row>
+    <row r="1270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1270" s="9"/>
+      <c r="B1270" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1270" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1270" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1270" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1270" s="22" t="s">
         <v>714</v>
-      </c>
-      <c r="E1269" s="28"/>
-      <c r="F1269" s="28" t="s">
-        <v>714</v>
-      </c>
-      <c r="G1269" s="28"/>
-      <c r="H1269" s="28"/>
-      <c r="I1269" s="29" t="s">
-        <v>1306</v>
-      </c>
-      <c r="J1269" s="29"/>
-      <c r="K1269" s="29" t="s">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="1270" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1270" s="22" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C1270" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1270" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1270" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1270" s="22" t="s">
-        <v>1234</v>
       </c>
       <c r="G1270" s="22"/>
       <c r="H1270" s="22"/>
       <c r="I1270" s="23" t="s">
+        <v>1303</v>
+      </c>
+      <c r="J1270" s="23"/>
+      <c r="K1270" s="23"/>
+    </row>
+    <row r="1271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1271" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1271" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1271" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1271" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1271" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1271" s="22"/>
+      <c r="H1271" s="22"/>
+      <c r="I1271" s="23" t="s">
+        <v>1304</v>
+      </c>
+      <c r="J1271" s="23"/>
+      <c r="K1271" s="23"/>
+    </row>
+    <row r="1272" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1272" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1272" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1272" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1272" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1272" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1272" s="22"/>
+      <c r="H1272" s="22"/>
+      <c r="I1272" s="23" t="s">
+        <v>1305</v>
+      </c>
+      <c r="J1272" s="23"/>
+      <c r="K1272" s="23"/>
+    </row>
+    <row r="1273" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1273" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1273" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1273" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1273" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1273" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1273" s="22"/>
+      <c r="H1273" s="22"/>
+      <c r="I1273" s="23" t="s">
+        <v>1306</v>
+      </c>
+      <c r="J1273" s="23"/>
+      <c r="K1273" s="23"/>
+    </row>
+    <row r="1274" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1274" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1274" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1274" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1274" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1274" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1274" s="22"/>
+      <c r="H1274" s="22"/>
+      <c r="I1274" s="23" t="s">
+        <v>1307</v>
+      </c>
+      <c r="J1274" s="23"/>
+      <c r="K1274" s="23"/>
+    </row>
+    <row r="1275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1275" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1275" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1275" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1275" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1275" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1275" s="22"/>
+      <c r="H1275" s="22"/>
+      <c r="I1275" s="23" t="s">
         <v>1308</v>
       </c>
-      <c r="J1270" s="23"/>
-      <c r="K1270" s="23" t="s">
+      <c r="J1275" s="23"/>
+      <c r="K1275" s="23"/>
+    </row>
+    <row r="1276" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1276" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1276" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1276" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1276" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1276" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1276" s="22"/>
+      <c r="H1276" s="22"/>
+      <c r="I1276" s="23" t="s">
         <v>1309</v>
       </c>
-    </row>
-    <row r="1271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1271" s="28" t="s">
+      <c r="J1276" s="23"/>
+      <c r="K1276" s="23"/>
+    </row>
+    <row r="1277" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1277" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1277" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1277" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1277" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1277" s="22" t="s">
         <v>714</v>
       </c>
-      <c r="C1271" s="28"/>
-      <c r="D1271" s="28" t="s">
+      <c r="G1277" s="22"/>
+      <c r="H1277" s="22"/>
+      <c r="I1277" s="23" t="s">
+        <v>1310</v>
+      </c>
+      <c r="J1277" s="23"/>
+      <c r="K1277" s="23"/>
+    </row>
+    <row r="1278" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1278" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1278" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1278" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1278" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1278" s="22" t="s">
         <v>714</v>
       </c>
-      <c r="E1271" s="28"/>
-      <c r="F1271" s="28" t="s">
+      <c r="G1278" s="22"/>
+      <c r="H1278" s="22"/>
+      <c r="I1278" s="23" t="s">
+        <v>1311</v>
+      </c>
+      <c r="J1278" s="23"/>
+      <c r="K1278" s="23"/>
+    </row>
+    <row r="1279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1279" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1279" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1279" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1279" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1279" s="22" t="s">
         <v>714</v>
       </c>
-      <c r="G1271" s="28"/>
-      <c r="H1271" s="28"/>
-      <c r="I1271" s="29" t="s">
-        <v>1310</v>
-      </c>
-      <c r="J1271" s="29"/>
-      <c r="K1271" s="29" t="s">
-        <v>1307</v>
-      </c>
-    </row>
+      <c r="G1279" s="22"/>
+      <c r="H1279" s="22"/>
+      <c r="I1279" s="23" t="s">
+        <v>1312</v>
+      </c>
+      <c r="J1279" s="23"/>
+      <c r="K1279" s="23"/>
+    </row>
+    <row r="1280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1280" s="28" t="s">
+        <v>714</v>
+      </c>
+      <c r="C1280" s="28"/>
+      <c r="D1280" s="28" t="s">
+        <v>714</v>
+      </c>
+      <c r="E1280" s="28"/>
+      <c r="F1280" s="28" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1280" s="28"/>
+      <c r="H1280" s="28"/>
+      <c r="I1280" s="29" t="s">
+        <v>1313</v>
+      </c>
+      <c r="J1280" s="29"/>
+      <c r="K1280" s="29" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="1281" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1281" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1281" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1281" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1281" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1281" s="22" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G1281" s="22"/>
+      <c r="H1281" s="22"/>
+      <c r="I1281" s="23" t="s">
+        <v>1315</v>
+      </c>
+      <c r="J1281" s="23"/>
+      <c r="K1281" s="23" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="1282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1282" s="28" t="s">
+        <v>714</v>
+      </c>
+      <c r="C1282" s="28"/>
+      <c r="D1282" s="28" t="s">
+        <v>714</v>
+      </c>
+      <c r="E1282" s="28"/>
+      <c r="F1282" s="28" t="s">
+        <v>714</v>
+      </c>
+      <c r="G1282" s="28"/>
+      <c r="H1282" s="28"/>
+      <c r="I1282" s="29" t="s">
+        <v>1317</v>
+      </c>
+      <c r="J1282" s="29"/>
+      <c r="K1282" s="29" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.766666666666667" header="0.511811023622047" footer="0.5"/>

</xml_diff>

<commit_message>
renamed geometry routines in preparation for 3D routines.
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -337,37 +337,37 @@
     <t xml:space="preserve">TIME INTERPOLATABLE POSE</t>
   </si>
   <si>
-    <t xml:space="preserve">TimeInterpPose_AddSample.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeInterpPose_CleanUp.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeInterpPose_Clear.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeInterpPose_GetSample.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeInterpPose_New.vi</t>
+    <t xml:space="preserve">TimeInterpPose2d_AddSample.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeInterpPose2d_CleanUp.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeInterpPose2d_Clear.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeInterpPose2d_GetSample.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeInterpPose2d_New.vi</t>
   </si>
   <si>
     <t xml:space="preserve">TIME INTERPOLATABLE ROTATION</t>
   </si>
   <si>
-    <t xml:space="preserve">TimeInterpRotation_AddSample.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeInterpRotation_CleanUp.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeInterpRotation_Clear.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeInterpRotation_GetSample.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeInterpRotation_New.vi</t>
+    <t xml:space="preserve">TimeInterpRotation2d_AddSample.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeInterpRotation2d_CleanUp.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeInterpRotation2d_Clear.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeInterpRotation2d_GetSample.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeInterpRotation2d_New.vi</t>
   </si>
   <si>
     <t xml:space="preserve">DIG SEQ LOGIC </t>
@@ -922,22 +922,22 @@
     <t xml:space="preserve">GEOMETRY</t>
   </si>
   <si>
-    <t xml:space="preserve">POSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pose_Equals.VI</t>
+    <t xml:space="preserve">POSE2D  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pose2d_Equals.VI</t>
   </si>
   <si>
     <t xml:space="preserve">boolean equals( other obj )</t>
   </si>
   <si>
-    <t xml:space="preserve">Pose_Exp.vi</t>
+    <t xml:space="preserve">Pose2d_Exp.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> pose2d exp( twist2d twist )</t>
   </si>
   <si>
-    <t xml:space="preserve">Pose_getRotation.vi</t>
+    <t xml:space="preserve">Pose2d_getRotation.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> rotation2d getRotation()    </t>
@@ -946,58 +946,58 @@
     <t xml:space="preserve">can also use cluster unpack</t>
   </si>
   <si>
-    <t xml:space="preserve">Pose_getTranslation.vi</t>
+    <t xml:space="preserve">Pose2d_getTranslation.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> translation2d getTranslation()   </t>
   </si>
   <si>
-    <t xml:space="preserve">Pose_getXY.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pose_getXYAngle.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pose_Interpolate.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pose_Log.vi</t>
+    <t xml:space="preserve">Pose2d_getXY.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pose2d_getXYAngle.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pose2d_Interpolate.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pose2d_Log.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> twist2d log( pose2d end )</t>
   </si>
   <si>
-    <t xml:space="preserve">Pose_Minus.vi</t>
+    <t xml:space="preserve">Pose2d_Minus.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> transform2d minus( pose2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Pose_New_TRRO.vi</t>
+    <t xml:space="preserve">Pose2d_New_TRRO.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> pose2d new( translation2d, rotation2d )</t>
   </si>
   <si>
-    <t xml:space="preserve">Pose_New.vi</t>
+    <t xml:space="preserve">Pose2d_New.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> pose2d new( double x, double y, rotation2d )</t>
   </si>
   <si>
-    <t xml:space="preserve">Pose_Plus.vi</t>
+    <t xml:space="preserve">Pose2d_Plus.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> pose2d plus( transform2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Pose_RelativeTo.vi</t>
+    <t xml:space="preserve">Pose2d_RelativeTo.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> pose2d relativeto( pose2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Pose_TransformBy.vi</t>
+    <t xml:space="preserve">Pose2d_TransformBy.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> pose2d transformby( transform2d other )</t>
@@ -1009,16 +1009,16 @@
     <t xml:space="preserve">can use cluster constant</t>
   </si>
   <si>
-    <t xml:space="preserve">ROTATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation_CreateAngle.vi</t>
+    <t xml:space="preserve">ROTATION2D  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation2d_CreateAngle.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> rotation2d new( double value )</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_CreateAngleDegrees.vi</t>
+    <t xml:space="preserve">Rotation2d_CreateAngleDegrees.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> rotation2d fromDegrees( double degrees )</t>
@@ -1027,28 +1027,28 @@
     <t xml:space="preserve">convert to radians then create</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_CreateAngleRotations.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation_CreateXY.vi</t>
+    <t xml:space="preserve">Rotation2d_CreateAngleRotations.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation2d_CreateXY.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> rotation2d new( double x, double y )</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_Equals.vi</t>
+    <t xml:space="preserve">Rotation2d_Equals.vi</t>
   </si>
   <si>
     <t xml:space="preserve">boolean equals( rotation2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_GetAngleCosSin.vi</t>
+    <t xml:space="preserve">Rotation2d_GetAngleCosSin.vi</t>
   </si>
   <si>
     <t xml:space="preserve">New 1/26/21</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_GetCos.VI</t>
+    <t xml:space="preserve">Rotation2d_GetCos.VI</t>
   </si>
   <si>
     <t xml:space="preserve"> double getCos()  </t>
@@ -1057,7 +1057,7 @@
     <t xml:space="preserve">use cluster unpack</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_GetDegrees.VI</t>
+    <t xml:space="preserve">Rotation2d_GetDegrees.VI</t>
   </si>
   <si>
     <t xml:space="preserve"> double getDegrees()</t>
@@ -1066,22 +1066,22 @@
     <t xml:space="preserve">use cluster unpack, then convert to degree</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_GetRadians.VI</t>
+    <t xml:space="preserve">Rotation2d_GetRadians.VI</t>
   </si>
   <si>
     <t xml:space="preserve"> double getRadians()  </t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_GetRotations.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation_GetSin.VI</t>
+    <t xml:space="preserve">Rotation2d_GetRotations.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation2d_GetSin.VI</t>
   </si>
   <si>
     <t xml:space="preserve"> double getSin()  </t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_GetTan.VI</t>
+    <t xml:space="preserve">Rotation2d_GetTan.VI</t>
   </si>
   <si>
     <t xml:space="preserve"> double getTan()  </t>
@@ -1090,34 +1090,34 @@
     <t xml:space="preserve">can calculate</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_Interpolate.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation_Minus.vi</t>
+    <t xml:space="preserve">Rotation2d_Interpolate.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation2d_Minus.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> rotation2d minus( rotation2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_Plus.vi</t>
+    <t xml:space="preserve">Rotation2d_Plus.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> rotation2d plus( rotation2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_RotateBy.vi</t>
+    <t xml:space="preserve">Rotation2d_RotateBy.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> rotation2d rotateby( rotation2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_Times.vi</t>
+    <t xml:space="preserve">Rotation2d_Times.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> rotation2d times( double scalar )</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation_UnaryMinus.vi</t>
+    <t xml:space="preserve">Rotation2d_UnaryMinus.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> rotation2d unaryminus( )</t>
@@ -1126,43 +1126,43 @@
     <t xml:space="preserve"> rotation2d new()</t>
   </si>
   <si>
-    <t xml:space="preserve">TRANSFORM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transform_Create_PosePose.vi</t>
+    <t xml:space="preserve">TRANSFORM2D </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform2d_Create_PosePose.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> transform2d new( pose2d, pose2d )</t>
   </si>
   <si>
-    <t xml:space="preserve">Transform_Create_TransRot.vi</t>
+    <t xml:space="preserve">Transform2d_Create_TransRot.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> transform2d new( translation2d, rotation2d )</t>
   </si>
   <si>
-    <t xml:space="preserve">Transform_Equals.VI</t>
+    <t xml:space="preserve">Transform2d_Equals.VI</t>
   </si>
   <si>
     <t xml:space="preserve">boolean equals( other transform2d )</t>
   </si>
   <si>
-    <t xml:space="preserve">Transform_GetRotation.VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transform_GetTranslation.VI</t>
+    <t xml:space="preserve">Transform2d_GetRotation.VI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform2d_GetTranslation.VI</t>
   </si>
   <si>
     <t xml:space="preserve"> translation2d getTranslation()    </t>
   </si>
   <si>
-    <t xml:space="preserve">Transform_GetXY.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transform_GetXYAngle.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transform_Inverse.vi</t>
+    <t xml:space="preserve">Transform2d_GetXY.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform2d_GetXYAngle.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform2d_Inverse.vi</t>
   </si>
   <si>
     <t xml:space="preserve">transform inverse()</t>
@@ -1174,10 +1174,10 @@
     <t xml:space="preserve">Si</t>
   </si>
   <si>
-    <t xml:space="preserve">Transform_Plus.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transform_Times.vi</t>
+    <t xml:space="preserve">Transform2d_Plus.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform2d_Times.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> transform2d times( double scalar )</t>
@@ -1186,31 +1186,31 @@
     <t xml:space="preserve"> transform2d new( )</t>
   </si>
   <si>
-    <t xml:space="preserve">TRANSLATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Translation_Create_DistAng.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Translation_Create.vi</t>
+    <t xml:space="preserve">TRANSLATION2D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Translation2d_Create_DistAng.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Translation2d_Create.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> translation2d new( double x, double y )</t>
   </si>
   <si>
-    <t xml:space="preserve">Translation_Equals.vi</t>
+    <t xml:space="preserve">Translation2d_Equals.vi</t>
   </si>
   <si>
     <t xml:space="preserve">boolean equals( translation other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Translation_GetDistance.vi</t>
+    <t xml:space="preserve">Translation2d_GetDistance.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> double getDistance( translation2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Translation_GetNorm.VI</t>
+    <t xml:space="preserve">Translation2d_GetNorm.VI</t>
   </si>
   <si>
     <t xml:space="preserve"> double getNorm()</t>
@@ -1219,49 +1219,49 @@
     <t xml:space="preserve">can use cluster unpack</t>
   </si>
   <si>
-    <t xml:space="preserve">Translation_GetX.VI</t>
+    <t xml:space="preserve">Translation2d_GetX.VI</t>
   </si>
   <si>
     <t xml:space="preserve"> double getX() </t>
   </si>
   <si>
-    <t xml:space="preserve">Translation_GetXY.VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Translation_GetY.VI</t>
+    <t xml:space="preserve">Translation2d_GetXY.VI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Translation2d_GetY.VI</t>
   </si>
   <si>
     <t xml:space="preserve"> double getY()</t>
   </si>
   <si>
-    <t xml:space="preserve">Translation_Interpolate.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Translation_Minus.vi</t>
+    <t xml:space="preserve">Translation2d_Interpolate.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Translation2d_Minus.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> translation2d minus( translation2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Translation_Plus.vi</t>
+    <t xml:space="preserve">Translation2d_Plus.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> translation2d plus( translation2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Translation_RotateBy.vi</t>
+    <t xml:space="preserve">Translation2d_RotateBy.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> translation2d rotateBy( rotation2d other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Translation_Times.vi</t>
+    <t xml:space="preserve">Translation2d_Times.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> translation2d times( double scalar )</t>
   </si>
   <si>
-    <t xml:space="preserve">Translation_UnaryMinus.vi</t>
+    <t xml:space="preserve">Translation2d_UnaryMinus.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> translation2d unaryminus( )</t>
@@ -1276,22 +1276,22 @@
     <t xml:space="preserve">can multiply by 1/scalar</t>
   </si>
   <si>
-    <t xml:space="preserve">TWIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twist_Create.vi</t>
+    <t xml:space="preserve">TWIST2D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twist2d_Create.vi</t>
   </si>
   <si>
     <t xml:space="preserve"> twist new( x, y, theta )</t>
   </si>
   <si>
-    <t xml:space="preserve">Twist_Equals.VI</t>
+    <t xml:space="preserve">Twist2d_Equals.VI</t>
   </si>
   <si>
     <t xml:space="preserve"> boolean equals( obj other )</t>
   </si>
   <si>
-    <t xml:space="preserve">Twist_GetAll.VI</t>
+    <t xml:space="preserve">Twist2d_GetAll.VI</t>
   </si>
   <si>
     <t xml:space="preserve">KINEMATICS</t>
@@ -2329,19 +2329,19 @@
     <t xml:space="preserve">Util_TrajState_to_DiffDrive_WheelPos.vi</t>
   </si>
   <si>
-    <t xml:space="preserve">Util_Waypoint_Eng_To_SI.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Util_Waypoint_To_CubicInput.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Util_Waypoint_To_QuinticInput.vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Util_WeightedWaypiont_Eng_To_WeightedWaypoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Util_WeightedWayPoint_To_WeightedWayPoint.vi</t>
+    <t xml:space="preserve">Util_DispWaypoint_Eng_To_SI.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Util_DispWaypoint_To_CubicInput.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Util_DispWaypoint_To_QuinticInput.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Util_DispWeightedWaypiont_Eng_To_WeightedWaypoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Util_DispWeightedWayPoint_To_WeightedWayPoint.vi</t>
   </si>
   <si>
     <t xml:space="preserve">Sorry about the confusing name..</t>
@@ -2389,7 +2389,7 @@
     <t xml:space="preserve">Conv_Meters_Inches.vi</t>
   </si>
   <si>
-    <t xml:space="preserve">Conv_POSE_SI_Eng.vi</t>
+    <t xml:space="preserve">Conv_Pose2d_SI_Eng.vi</t>
   </si>
   <si>
     <t xml:space="preserve">Conv_Pounds_Kilograms.vi</t>
@@ -3943,7 +3943,7 @@
     <t xml:space="preserve">DIFF_DRIVE_Kitbot_WheelSize_ENUM.ctl</t>
   </si>
   <si>
-    <t xml:space="preserve">DiFF_DRIVE_POSE_EST.ctl</t>
+    <t xml:space="preserve">DiFF_DRIVE_Pose_EST.ctl</t>
   </si>
   <si>
     <t xml:space="preserve">DIFF_DRIVE_ToughBoxMini_GearChoice_ENUM.ctl</t>
@@ -4000,10 +4000,10 @@
     <t xml:space="preserve">TIME_INTERPOLATABLE_DOUBLE.CTL</t>
   </si>
   <si>
-    <t xml:space="preserve">TIME_INTERPOLATABLE_POSE.CTL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIME_INTERPOLATABLE_ROTATION.CTL</t>
+    <t xml:space="preserve">TIME_INTERPOLATABLE_POSE2D.CTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME_INTERPOLATABLE_ROTATION2D.CTL</t>
   </si>
   <si>
     <t xml:space="preserve">KALMAN_FILTER_LATENCY_COMP_FUNC_GROUP.CTL</t>
@@ -4135,7 +4135,7 @@
     <t xml:space="preserve">SWERVE_DRIVE_ODOMETRY.CTL</t>
   </si>
   <si>
-    <t xml:space="preserve">SWERVE_DRIVE_POSE_EST.CTL</t>
+    <t xml:space="preserve">SWERVE_DRIVE_Pose_EST.CTL</t>
   </si>
   <si>
     <t xml:space="preserve">TIMER.CTL</t>
@@ -4622,15 +4622,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -4701,8 +4692,8 @@
   </sheetPr>
   <dimension ref="A1:AMI1373"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B563" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I656" activeCellId="0" sqref="I656"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>